<commit_message>
Balance patch: extra spread when holding
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D79553-0E6E-43F6-A504-C927D673A0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD118C1C-4BD3-439E-83C1-92A923EFBE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-190" yWindow="10" windowWidth="20010" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2011,7 +2011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2329,79 +2329,76 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3512,29 +3509,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="5.08203125" customWidth="1"/>
-    <col min="2" max="2" width="20.9140625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.08203125" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" customWidth="1"/>
-    <col min="38" max="38" width="20.08203125" customWidth="1"/>
+    <col min="1" max="1" width="5.0625" customWidth="1"/>
+    <col min="2" max="2" width="20.9375" customWidth="1"/>
+    <col min="10" max="10" width="10.6875" customWidth="1"/>
+    <col min="12" max="12" width="10.0625" customWidth="1"/>
+    <col min="15" max="15" width="9.3125" customWidth="1"/>
+    <col min="38" max="38" width="20.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:38" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="82"/>
       <c r="B1" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="123" t="s">
+      <c r="C1" s="131" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="123"/>
+      <c r="D1" s="131"/>
       <c r="G1" s="56" t="s">
         <v>162</v>
       </c>
@@ -3560,7 +3557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="35"/>
       <c r="B2" s="77" t="s">
         <v>177</v>
@@ -3630,20 +3627,20 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="128" t="s">
+      <c r="Z2" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="128"/>
+      <c r="AA2" s="123"/>
       <c r="AG2" s="43" t="s">
         <v>85</v>
       </c>
       <c r="AH2" s="39"/>
       <c r="AI2" s="39"/>
-      <c r="AL2" s="137" t="s">
+      <c r="AL2" s="114" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="59"/>
       <c r="B3" s="18" t="s">
         <v>66</v>
@@ -3732,11 +3729,11 @@
       <c r="AH3" s="53"/>
       <c r="AI3" s="53"/>
       <c r="AJ3" s="53"/>
-      <c r="AL3" s="136">
+      <c r="AL3" s="113">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -3819,9 +3816,9 @@
       <c r="Z4" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="AL4" s="135"/>
-    </row>
-    <row r="5" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL4" s="36"/>
+    </row>
+    <row r="5" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="22" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3906,9 +3903,9 @@
       <c r="Z5" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="AL5" s="135"/>
-    </row>
-    <row r="6" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL5" s="36"/>
+    </row>
+    <row r="6" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="22" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -3991,9 +3988,9 @@
       <c r="Z6" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="AL6" s="135"/>
-    </row>
-    <row r="7" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL6" s="36"/>
+    </row>
+    <row r="7" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="22" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -4052,9 +4049,9 @@
       <c r="Z7" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="AL7" s="135"/>
-    </row>
-    <row r="8" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL7" s="36"/>
+    </row>
+    <row r="8" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="76"/>
@@ -4081,9 +4078,9 @@
       <c r="X8" s="74"/>
       <c r="Y8" s="74"/>
       <c r="Z8" s="57"/>
-      <c r="AL8" s="135"/>
-    </row>
-    <row r="9" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL8" s="36"/>
+    </row>
+    <row r="9" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="76"/>
@@ -4110,9 +4107,9 @@
       <c r="X9" s="57"/>
       <c r="Y9" s="57"/>
       <c r="Z9" s="57"/>
-      <c r="AL9" s="135"/>
-    </row>
-    <row r="10" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL9" s="36"/>
+    </row>
+    <row r="10" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="18" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -4197,7 +4194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="18" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -4282,7 +4279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="18" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -4367,7 +4364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="18" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -4454,7 +4451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="76"/>
@@ -4481,9 +4478,9 @@
       <c r="X14" s="74"/>
       <c r="Y14" s="74"/>
       <c r="Z14" s="57"/>
-      <c r="AL14" s="135"/>
-    </row>
-    <row r="15" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL14" s="36"/>
+    </row>
+    <row r="15" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="76"/>
@@ -4510,9 +4507,9 @@
       <c r="X15" s="74"/>
       <c r="Y15" s="74"/>
       <c r="Z15" s="57"/>
-      <c r="AL15" s="135"/>
-    </row>
-    <row r="16" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL15" s="36"/>
+    </row>
+    <row r="16" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="18" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -4593,11 +4590,11 @@
       </c>
       <c r="Y16" s="19"/>
       <c r="Z16" s="57"/>
-      <c r="AL16" s="136">
+      <c r="AL16" s="113">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="18" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -4690,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="18" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -4777,7 +4774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="18" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -4862,7 +4859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="18" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -4953,7 +4950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="42"/>
@@ -4980,9 +4977,9 @@
       <c r="X21" s="20"/>
       <c r="Y21" s="19"/>
       <c r="Z21" s="57"/>
-      <c r="AL21" s="135"/>
-    </row>
-    <row r="22" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL21" s="36"/>
+    </row>
+    <row r="22" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="76"/>
@@ -5009,9 +5006,9 @@
       <c r="X22" s="74"/>
       <c r="Y22" s="74"/>
       <c r="Z22" s="57"/>
-      <c r="AL22" s="135"/>
-    </row>
-    <row r="23" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL22" s="36"/>
+    </row>
+    <row r="23" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="18" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -5022,7 +5019,7 @@
         <v>320</v>
       </c>
       <c r="D23" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" s="19">
         <v>5</v>
@@ -5068,7 +5065,7 @@
       </c>
       <c r="R23" s="19">
         <f>ROUND(D23/H23,3)</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S23" s="28" t="s">
         <v>29</v>
@@ -5098,7 +5095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="18" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -5109,7 +5106,7 @@
         <v>448</v>
       </c>
       <c r="D24" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="23">
         <v>3</v>
@@ -5155,7 +5152,7 @@
       </c>
       <c r="R24" s="19">
         <f>ROUND(D24/H24,3)</f>
-        <v>0.23100000000000001</v>
+        <v>0.154</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>28</v>
@@ -5183,7 +5180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="18" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
@@ -5194,7 +5191,7 @@
         <v>448</v>
       </c>
       <c r="D25" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="19">
         <v>2</v>
@@ -5240,7 +5237,7 @@
       </c>
       <c r="R25" s="19">
         <f>ROUND(D25/H25,3)</f>
-        <v>0.214</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="S25" s="28" t="s">
         <v>29</v>
@@ -5268,7 +5265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="42"/>
@@ -5295,9 +5292,9 @@
       <c r="X26" s="20"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="57"/>
-      <c r="AL26" s="135"/>
-    </row>
-    <row r="27" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL26" s="36"/>
+    </row>
+    <row r="27" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="76"/>
@@ -5324,9 +5321,9 @@
       <c r="X27" s="74"/>
       <c r="Y27" s="74"/>
       <c r="Z27" s="57"/>
-      <c r="AL27" s="135"/>
-    </row>
-    <row r="28" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL27" s="36"/>
+    </row>
+    <row r="28" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -5411,7 +5408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="18" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -5496,7 +5493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="18" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
@@ -5581,7 +5578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="42"/>
@@ -5608,9 +5605,9 @@
       <c r="X31" s="34"/>
       <c r="Y31" s="19"/>
       <c r="Z31" s="57"/>
-      <c r="AL31" s="135"/>
-    </row>
-    <row r="32" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL31" s="36"/>
+    </row>
+    <row r="32" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="35"/>
       <c r="B32" s="77" t="s">
         <v>50</v>
@@ -5639,9 +5636,9 @@
       <c r="X32" s="34"/>
       <c r="Y32" s="19"/>
       <c r="Z32" s="57"/>
-      <c r="AL32" s="135"/>
-    </row>
-    <row r="33" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL32" s="36"/>
+    </row>
+    <row r="33" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="18" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
@@ -5708,9 +5705,9 @@
       <c r="Z33" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="AL33" s="135"/>
-    </row>
-    <row r="34" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL33" s="36"/>
+    </row>
+    <row r="34" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="18" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
@@ -5778,9 +5775,9 @@
       </c>
       <c r="Y34" s="19"/>
       <c r="Z34" s="57"/>
-      <c r="AL34" s="135"/>
-    </row>
-    <row r="35" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL34" s="36"/>
+    </row>
+    <row r="35" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="18" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
@@ -5848,9 +5845,9 @@
       </c>
       <c r="Y35" s="19"/>
       <c r="Z35" s="57"/>
-      <c r="AL35" s="135"/>
-    </row>
-    <row r="36" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL35" s="36"/>
+    </row>
+    <row r="36" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="76"/>
@@ -5876,9 +5873,9 @@
       <c r="W36" s="74"/>
       <c r="X36" s="74"/>
       <c r="Y36" s="74"/>
-      <c r="AL36" s="135"/>
-    </row>
-    <row r="37" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL36" s="36"/>
+    </row>
+    <row r="37" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="76"/>
@@ -5904,10 +5901,10 @@
       <c r="W37" s="74"/>
       <c r="X37" s="74"/>
       <c r="Y37" s="74"/>
-      <c r="AL37" s="135"/>
-    </row>
-    <row r="38" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AL37" s="36"/>
+    </row>
+    <row r="38" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="39" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="36"/>
       <c r="B39" s="36"/>
       <c r="C39" s="37"/>
@@ -5918,138 +5915,138 @@
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
     </row>
-    <row r="40" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="35"/>
       <c r="B40" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="116" t="s">
+      <c r="C40" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="116"/>
-      <c r="E40" s="116"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="116"/>
-      <c r="H40" s="116"/>
-      <c r="I40" s="116" t="s">
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="129"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="116"/>
-      <c r="K40" s="116"/>
-      <c r="L40" s="116"/>
+      <c r="J40" s="129"/>
+      <c r="K40" s="129"/>
+      <c r="L40" s="129"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="129" t="s">
+      <c r="S40" s="128" t="s">
         <v>78</v>
       </c>
-      <c r="T40" s="129"/>
+      <c r="T40" s="128"/>
       <c r="U40" s="57"/>
     </row>
-    <row r="41" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="38" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="117" t="s">
+      <c r="C41" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="117"/>
-      <c r="E41" s="117"/>
-      <c r="F41" s="117" t="s">
+      <c r="D41" s="130"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="117"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="117" t="s">
+      <c r="G41" s="130"/>
+      <c r="H41" s="130"/>
+      <c r="I41" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="J41" s="117"/>
-      <c r="K41" s="117"/>
-      <c r="L41" s="117"/>
+      <c r="J41" s="130"/>
+      <c r="K41" s="130"/>
+      <c r="L41" s="130"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="129" t="s">
+      <c r="S41" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="T41" s="129"/>
+      <c r="T41" s="128"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
       <c r="V41" s="57"/>
     </row>
-    <row r="42" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="38" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="117" t="s">
+      <c r="C42" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="117"/>
-      <c r="E42" s="117"/>
-      <c r="F42" s="117" t="s">
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="130" t="s">
         <v>203</v>
       </c>
-      <c r="G42" s="117"/>
-      <c r="H42" s="117"/>
-      <c r="I42" s="117" t="s">
+      <c r="G42" s="130"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="J42" s="117"/>
-      <c r="K42" s="117"/>
-      <c r="L42" s="117"/>
+      <c r="J42" s="130"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="130"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="129" t="s">
+      <c r="S42" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="T42" s="129"/>
+      <c r="T42" s="128"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
       <c r="V42" s="57"/>
     </row>
-    <row r="43" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="18" t="s">
         <v>205</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C43" s="118" t="s">
+      <c r="C43" s="126" t="s">
         <v>210</v>
       </c>
-      <c r="D43" s="118"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118" t="s">
+      <c r="D43" s="126"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="126" t="s">
         <v>211</v>
       </c>
-      <c r="G43" s="118"/>
-      <c r="H43" s="118"/>
-      <c r="I43" s="118" t="s">
+      <c r="G43" s="126"/>
+      <c r="H43" s="126"/>
+      <c r="I43" s="126" t="s">
         <v>208</v>
       </c>
-      <c r="J43" s="118"/>
-      <c r="K43" s="118"/>
-      <c r="L43" s="118"/>
+      <c r="J43" s="126"/>
+      <c r="K43" s="126"/>
+      <c r="L43" s="126"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="129" t="s">
+      <c r="S43" s="128" t="s">
         <v>99</v>
       </c>
-      <c r="T43" s="129"/>
+      <c r="T43" s="128"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6057,27 +6054,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="18" t="s">
         <v>205</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="118" t="s">
+      <c r="C44" s="126" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118" t="s">
+      <c r="D44" s="126"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="126"/>
+      <c r="G44" s="126"/>
+      <c r="H44" s="126"/>
+      <c r="I44" s="126" t="s">
         <v>209</v>
       </c>
-      <c r="J44" s="118"/>
-      <c r="K44" s="118"/>
-      <c r="L44" s="118"/>
+      <c r="J44" s="126"/>
+      <c r="K44" s="126"/>
+      <c r="L44" s="126"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6086,102 +6083,102 @@
       <c r="T44" s="57"/>
       <c r="U44" s="57"/>
     </row>
-    <row r="45" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="46" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="35"/>
       <c r="B47" s="77" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="116" t="s">
+      <c r="C47" s="129" t="s">
         <v>195</v>
       </c>
-      <c r="D47" s="116"/>
-      <c r="E47" s="116" t="s">
+      <c r="D47" s="129"/>
+      <c r="E47" s="129" t="s">
         <v>194</v>
       </c>
-      <c r="F47" s="116"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="116"/>
+      <c r="F47" s="129"/>
+      <c r="G47" s="129"/>
+      <c r="H47" s="129"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
-    <row r="48" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A48" s="38" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="C48" s="117">
+      <c r="C48" s="130">
         <v>2</v>
       </c>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117" t="s">
+      <c r="D48" s="130"/>
+      <c r="E48" s="130" t="s">
         <v>199</v>
       </c>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
+      <c r="F48" s="130"/>
+      <c r="G48" s="130"/>
+      <c r="H48" s="130"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
-    <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="38" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="117" t="s">
+      <c r="C49" s="130" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="117"/>
-      <c r="E49" s="117" t="s">
+      <c r="D49" s="130"/>
+      <c r="E49" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="117"/>
-      <c r="G49" s="117"/>
-      <c r="H49" s="117"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="130"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
-    <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="118"/>
-      <c r="H50" s="118"/>
+      <c r="C50" s="126"/>
+      <c r="D50" s="126"/>
+      <c r="E50" s="126"/>
+      <c r="F50" s="126"/>
+      <c r="G50" s="126"/>
+      <c r="H50" s="126"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
-    <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A53" s="58" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C54" s="63" t="s">
         <v>167</v>
       </c>
       <c r="D54" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="H54" s="121" t="s">
+      <c r="H54" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="I54" s="121"/>
-      <c r="J54" s="121"/>
-      <c r="K54" s="121"/>
-      <c r="L54" s="121"/>
-      <c r="M54" s="121"/>
-    </row>
-    <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I54" s="135"/>
+      <c r="J54" s="135"/>
+      <c r="K54" s="135"/>
+      <c r="L54" s="135"/>
+      <c r="M54" s="135"/>
+    </row>
+    <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
       <c r="B55" s="87" t="s">
         <v>174</v>
@@ -6220,7 +6217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A56" s="90"/>
       <c r="B56" s="59" t="s">
         <v>70</v>
@@ -6270,7 +6267,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
       <c r="B57" s="59" t="s">
         <v>71</v>
@@ -6320,7 +6317,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C58" s="64" t="s">
         <v>168</v>
       </c>
@@ -6330,17 +6327,17 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="122" t="s">
+      <c r="H58" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="I58" s="122"/>
-      <c r="J58" s="122"/>
-      <c r="K58" s="122"/>
-      <c r="L58" s="122"/>
-      <c r="M58" s="122"/>
-    </row>
-    <row r="59" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I58" s="136"/>
+      <c r="J58" s="136"/>
+      <c r="K58" s="136"/>
+      <c r="L58" s="136"/>
+      <c r="M58" s="136"/>
+    </row>
+    <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O60" t="s">
         <v>110</v>
       </c>
@@ -6361,7 +6358,7 @@
       <c r="AI60" s="80"/>
       <c r="AJ60" s="80"/>
     </row>
-    <row r="61" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O61">
         <v>200</v>
       </c>
@@ -6382,14 +6379,14 @@
       <c r="AI61" s="81"/>
       <c r="AJ61" s="81"/>
     </row>
-    <row r="62" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="I62" t="s">
         <v>97</v>
       </c>
-      <c r="J62" s="125" t="s">
+      <c r="J62" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="K62" s="125"/>
+      <c r="K62" s="133"/>
       <c r="L62" t="s">
         <v>102</v>
       </c>
@@ -6397,19 +6394,19 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="O62" s="124" t="s">
+      <c r="O62" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="P62" s="124"/>
-      <c r="Q62" s="124"/>
-      <c r="R62" s="124"/>
-      <c r="S62" s="124"/>
+      <c r="P62" s="132"/>
+      <c r="Q62" s="132"/>
+      <c r="R62" s="132"/>
+      <c r="S62" s="132"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
       <c r="AJ62" s="81"/>
     </row>
-    <row r="63" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A63" s="91" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -6425,20 +6422,20 @@
       <c r="E63" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="F63" s="130" t="s">
+      <c r="F63" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="G63" s="130"/>
+      <c r="G63" s="118"/>
       <c r="H63" s="86" t="s">
         <v>191</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="130" t="s">
+      <c r="J63" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="K63" s="130"/>
+      <c r="K63" s="118"/>
       <c r="L63" s="86" t="s">
         <v>103</v>
       </c>
@@ -6462,10 +6459,10 @@
         <v>114</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="130" t="s">
+      <c r="U63" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="V63" s="130"/>
+      <c r="V63" s="118"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6479,7 +6476,7 @@
       <c r="AI63" s="81"/>
       <c r="AJ63" s="81"/>
     </row>
-    <row r="64" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A64" s="38"/>
       <c r="B64" s="38" t="s">
         <v>86</v>
@@ -6493,21 +6490,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="131" t="s">
+      <c r="F64" s="134" t="s">
         <v>96</v>
       </c>
-      <c r="G64" s="131"/>
+      <c r="G64" s="134"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="120">
+      <c r="J64" s="121">
         <f t="shared" ref="J64:J69" si="17">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="120"/>
+      <c r="K64" s="121"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>11</v>
@@ -6538,11 +6535,11 @@
         <v>10.100000000000001</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="133">
+      <c r="U64" s="119">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="133"/>
+      <c r="V64" s="119"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6556,7 +6553,7 @@
       <c r="AI64" s="81"/>
       <c r="AJ64" s="81"/>
     </row>
-    <row r="65" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
         <v>87</v>
@@ -6570,21 +6567,21 @@
       <c r="E65" s="54">
         <v>3</v>
       </c>
-      <c r="F65" s="113" t="s">
+      <c r="F65" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="G65" s="113"/>
+      <c r="G65" s="116"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="120">
+      <c r="J65" s="121">
         <f t="shared" si="17"/>
         <v>32</v>
       </c>
-      <c r="K65" s="120"/>
+      <c r="K65" s="121"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6615,11 +6612,11 @@
         <v>12.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="134">
+      <c r="U65" s="120">
         <f t="shared" ref="U65:U70" si="24">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="134"/>
+      <c r="V65" s="120"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6633,7 +6630,7 @@
       <c r="AI65" s="81"/>
       <c r="AJ65" s="81"/>
     </row>
-    <row r="66" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
         <v>88</v>
@@ -6647,21 +6644,21 @@
       <c r="E66" s="54">
         <v>4</v>
       </c>
-      <c r="F66" s="113" t="s">
+      <c r="F66" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="113"/>
+      <c r="G66" s="116"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="120">
+      <c r="J66" s="121">
         <f t="shared" si="17"/>
         <v>28</v>
       </c>
-      <c r="K66" s="120"/>
+      <c r="K66" s="121"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6692,11 +6689,11 @@
         <v>14.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="134">
+      <c r="U66" s="120">
         <f t="shared" si="24"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="134"/>
+      <c r="V66" s="120"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6710,7 +6707,7 @@
       <c r="AI66" s="81"/>
       <c r="AJ66" s="81"/>
     </row>
-    <row r="67" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A67" s="18"/>
       <c r="B67" s="18" t="s">
         <v>89</v>
@@ -6724,21 +6721,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="113" t="s">
+      <c r="F67" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="113"/>
+      <c r="G67" s="116"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="120">
+      <c r="J67" s="121">
         <f t="shared" si="17"/>
         <v>48</v>
       </c>
-      <c r="K67" s="120"/>
+      <c r="K67" s="121"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6769,11 +6766,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="134">
+      <c r="U67" s="120">
         <f t="shared" si="24"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="134"/>
+      <c r="V67" s="120"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6783,7 +6780,7 @@
       <c r="Y67" s="57"/>
       <c r="Z67" s="57"/>
     </row>
-    <row r="68" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A68" s="18"/>
       <c r="B68" s="18" t="s">
         <v>94</v>
@@ -6797,21 +6794,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="113" t="s">
+      <c r="F68" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="113"/>
+      <c r="G68" s="116"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="120">
+      <c r="J68" s="121">
         <f t="shared" si="17"/>
         <v>72</v>
       </c>
-      <c r="K68" s="120"/>
+      <c r="K68" s="121"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -6842,11 +6839,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="134">
+      <c r="U68" s="120">
         <f t="shared" si="24"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="134"/>
+      <c r="V68" s="120"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6856,7 +6853,7 @@
       <c r="Y68" s="57"/>
       <c r="Z68" s="57"/>
     </row>
-    <row r="69" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A69" s="18"/>
       <c r="B69" s="18" t="s">
         <v>105</v>
@@ -6870,21 +6867,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="113" t="s">
+      <c r="F69" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="113"/>
+      <c r="G69" s="116"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="120">
+      <c r="J69" s="121">
         <f t="shared" si="17"/>
         <v>20</v>
       </c>
-      <c r="K69" s="120"/>
+      <c r="K69" s="121"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6915,11 +6912,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="134">
+      <c r="U69" s="120">
         <f t="shared" si="24"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="134"/>
+      <c r="V69" s="120"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6929,7 +6926,7 @@
       <c r="Y69" s="57"/>
       <c r="Z69" s="57"/>
     </row>
-    <row r="70" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A70" s="18"/>
       <c r="B70" s="18" t="s">
         <v>116</v>
@@ -6943,21 +6940,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="G70" s="113"/>
+      <c r="G70" s="116"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="120">
+      <c r="J70" s="121">
         <f t="shared" ref="J70" si="25">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="120"/>
+      <c r="K70" s="121"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -6988,11 +6985,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="134">
+      <c r="U70" s="120">
         <f t="shared" si="24"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="134"/>
+      <c r="V70" s="120"/>
       <c r="W70" s="25" t="s">
         <v>75</v>
       </c>
@@ -7002,17 +6999,17 @@
       <c r="Y70" s="57"/>
       <c r="Z70" s="57"/>
     </row>
-    <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="O73" s="128" t="s">
+    <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="O73" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="P73" s="128"/>
-      <c r="Q73" s="128"/>
-      <c r="R73" s="128"/>
-    </row>
-    <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="P73" s="123"/>
+      <c r="Q73" s="123"/>
+      <c r="R73" s="123"/>
+    </row>
+    <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
       <c r="B74" s="77" t="s">
         <v>130</v>
@@ -7026,33 +7023,33 @@
       <c r="E74" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="F74" s="119" t="s">
+      <c r="F74" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119" t="s">
+      <c r="G74" s="122"/>
+      <c r="H74" s="122" t="s">
         <v>138</v>
       </c>
-      <c r="I74" s="119"/>
-      <c r="J74" s="119" t="s">
+      <c r="I74" s="122"/>
+      <c r="J74" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="K74" s="119"/>
-      <c r="L74" s="119"/>
-      <c r="M74" s="119"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="122"/>
+      <c r="M74" s="122"/>
       <c r="N74" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="O74" s="119" t="s">
+      <c r="O74" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="P74" s="119"/>
-      <c r="Q74" s="119" t="s">
+      <c r="P74" s="122"/>
+      <c r="Q74" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="R74" s="119"/>
-    </row>
-    <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R74" s="122"/>
+    </row>
+    <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
@@ -7068,21 +7065,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="120" t="s">
+      <c r="F75" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="G75" s="120"/>
-      <c r="H75" s="120">
+      <c r="G75" s="121"/>
+      <c r="H75" s="121">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="120"/>
-      <c r="J75" s="120" t="s">
+      <c r="I75" s="121"/>
+      <c r="J75" s="121" t="s">
         <v>134</v>
       </c>
-      <c r="K75" s="120"/>
-      <c r="L75" s="120"/>
-      <c r="M75" s="120"/>
+      <c r="K75" s="121"/>
+      <c r="L75" s="121"/>
+      <c r="M75" s="121"/>
       <c r="N75" s="78" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -7095,7 +7092,7 @@
       <c r="Q75" s="79"/>
       <c r="R75" s="95"/>
     </row>
-    <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A76" s="38" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
@@ -7111,21 +7108,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="120" t="s">
+      <c r="F76" s="121" t="s">
         <v>127</v>
       </c>
-      <c r="G76" s="120"/>
-      <c r="H76" s="120">
+      <c r="G76" s="121"/>
+      <c r="H76" s="121">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="120"/>
-      <c r="J76" s="120" t="s">
+      <c r="I76" s="121"/>
+      <c r="J76" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="K76" s="120"/>
-      <c r="L76" s="120"/>
-      <c r="M76" s="120"/>
+      <c r="K76" s="121"/>
+      <c r="L76" s="121"/>
+      <c r="M76" s="121"/>
       <c r="N76" s="78" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -7138,27 +7135,27 @@
       <c r="Q76" s="79"/>
       <c r="R76" s="95"/>
     </row>
-    <row r="77" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A77" s="18"/>
       <c r="B77" s="18"/>
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="118"/>
-      <c r="G77" s="118"/>
-      <c r="H77" s="118"/>
-      <c r="I77" s="118"/>
-      <c r="J77" s="118"/>
-      <c r="K77" s="118"/>
-      <c r="L77" s="118"/>
-      <c r="M77" s="118"/>
+      <c r="F77" s="126"/>
+      <c r="G77" s="126"/>
+      <c r="H77" s="126"/>
+      <c r="I77" s="126"/>
+      <c r="J77" s="126"/>
+      <c r="K77" s="126"/>
+      <c r="L77" s="126"/>
+      <c r="M77" s="126"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="126"/>
-      <c r="P77" s="126"/>
-      <c r="Q77" s="126"/>
-      <c r="R77" s="126"/>
-    </row>
-    <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O77" s="124"/>
+      <c r="P77" s="124"/>
+      <c r="Q77" s="124"/>
+      <c r="R77" s="124"/>
+    </row>
+    <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
         <v>202</v>
       </c>
@@ -7166,9 +7163,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="81" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A81" s="35" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
@@ -7184,34 +7181,34 @@
       <c r="E81" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="F81" s="119" t="s">
+      <c r="F81" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="G81" s="119"/>
-      <c r="H81" s="119"/>
-      <c r="I81" s="119"/>
-      <c r="J81" s="119"/>
-      <c r="K81" s="119"/>
-      <c r="L81" s="119"/>
-      <c r="M81" s="119"/>
-      <c r="N81" s="119"/>
-      <c r="O81" s="119"/>
-      <c r="P81" s="119"/>
-      <c r="Q81" s="119" t="s">
+      <c r="G81" s="122"/>
+      <c r="H81" s="122"/>
+      <c r="I81" s="122"/>
+      <c r="J81" s="122"/>
+      <c r="K81" s="122"/>
+      <c r="L81" s="122"/>
+      <c r="M81" s="122"/>
+      <c r="N81" s="122"/>
+      <c r="O81" s="122"/>
+      <c r="P81" s="122"/>
+      <c r="Q81" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="R81" s="119"/>
-      <c r="S81" s="119"/>
-      <c r="T81" s="119"/>
-      <c r="U81" s="119"/>
-      <c r="V81" s="119"/>
-      <c r="W81" s="119"/>
-      <c r="X81" s="119"/>
-      <c r="Y81" s="119"/>
-      <c r="Z81" s="119"/>
-      <c r="AA81" s="119"/>
-    </row>
-    <row r="82" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R81" s="122"/>
+      <c r="S81" s="122"/>
+      <c r="T81" s="122"/>
+      <c r="U81" s="122"/>
+      <c r="V81" s="122"/>
+      <c r="W81" s="122"/>
+      <c r="X81" s="122"/>
+      <c r="Y81" s="122"/>
+      <c r="Z81" s="122"/>
+      <c r="AA81" s="122"/>
+    </row>
+    <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
       <c r="B82" s="38" t="s">
         <v>147</v>
@@ -7225,34 +7222,34 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="132" t="s">
+      <c r="F82" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="G82" s="132"/>
-      <c r="H82" s="132"/>
-      <c r="I82" s="132"/>
-      <c r="J82" s="132"/>
-      <c r="K82" s="132"/>
-      <c r="L82" s="132"/>
-      <c r="M82" s="132"/>
-      <c r="N82" s="132"/>
-      <c r="O82" s="132"/>
-      <c r="P82" s="132"/>
-      <c r="Q82" s="132" t="s">
+      <c r="G82" s="127"/>
+      <c r="H82" s="127"/>
+      <c r="I82" s="127"/>
+      <c r="J82" s="127"/>
+      <c r="K82" s="127"/>
+      <c r="L82" s="127"/>
+      <c r="M82" s="127"/>
+      <c r="N82" s="127"/>
+      <c r="O82" s="127"/>
+      <c r="P82" s="127"/>
+      <c r="Q82" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="R82" s="132"/>
-      <c r="S82" s="132"/>
-      <c r="T82" s="132"/>
-      <c r="U82" s="132"/>
-      <c r="V82" s="132"/>
-      <c r="W82" s="132"/>
-      <c r="X82" s="132"/>
-      <c r="Y82" s="132"/>
-      <c r="Z82" s="132"/>
-      <c r="AA82" s="132"/>
-    </row>
-    <row r="83" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R82" s="127"/>
+      <c r="S82" s="127"/>
+      <c r="T82" s="127"/>
+      <c r="U82" s="127"/>
+      <c r="V82" s="127"/>
+      <c r="W82" s="127"/>
+      <c r="X82" s="127"/>
+      <c r="Y82" s="127"/>
+      <c r="Z82" s="127"/>
+      <c r="AA82" s="127"/>
+    </row>
+    <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
       <c r="B83" s="38" t="s">
         <v>148</v>
@@ -7266,32 +7263,32 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="115" t="s">
+      <c r="F83" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="G83" s="115"/>
-      <c r="H83" s="115"/>
-      <c r="I83" s="115"/>
-      <c r="J83" s="115"/>
-      <c r="K83" s="115"/>
-      <c r="L83" s="115"/>
-      <c r="M83" s="115"/>
-      <c r="N83" s="115"/>
-      <c r="O83" s="115"/>
-      <c r="P83" s="115"/>
-      <c r="Q83" s="115"/>
-      <c r="R83" s="115"/>
-      <c r="S83" s="115"/>
-      <c r="T83" s="115"/>
-      <c r="U83" s="115"/>
-      <c r="V83" s="115"/>
-      <c r="W83" s="115"/>
-      <c r="X83" s="115"/>
-      <c r="Y83" s="115"/>
-      <c r="Z83" s="115"/>
-      <c r="AA83" s="115"/>
-    </row>
-    <row r="84" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G83" s="117"/>
+      <c r="H83" s="117"/>
+      <c r="I83" s="117"/>
+      <c r="J83" s="117"/>
+      <c r="K83" s="117"/>
+      <c r="L83" s="117"/>
+      <c r="M83" s="117"/>
+      <c r="N83" s="117"/>
+      <c r="O83" s="117"/>
+      <c r="P83" s="117"/>
+      <c r="Q83" s="117"/>
+      <c r="R83" s="117"/>
+      <c r="S83" s="117"/>
+      <c r="T83" s="117"/>
+      <c r="U83" s="117"/>
+      <c r="V83" s="117"/>
+      <c r="W83" s="117"/>
+      <c r="X83" s="117"/>
+      <c r="Y83" s="117"/>
+      <c r="Z83" s="117"/>
+      <c r="AA83" s="117"/>
+    </row>
+    <row r="84" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A84" s="38"/>
       <c r="B84" s="38" t="s">
         <v>149</v>
@@ -7305,32 +7302,32 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="115" t="s">
+      <c r="F84" s="117" t="s">
         <v>153</v>
       </c>
-      <c r="G84" s="115"/>
-      <c r="H84" s="115"/>
-      <c r="I84" s="115"/>
-      <c r="J84" s="115"/>
-      <c r="K84" s="115"/>
-      <c r="L84" s="115"/>
-      <c r="M84" s="115"/>
-      <c r="N84" s="115"/>
-      <c r="O84" s="115"/>
-      <c r="P84" s="115"/>
-      <c r="Q84" s="115"/>
-      <c r="R84" s="115"/>
-      <c r="S84" s="115"/>
-      <c r="T84" s="115"/>
-      <c r="U84" s="115"/>
-      <c r="V84" s="115"/>
-      <c r="W84" s="115"/>
-      <c r="X84" s="115"/>
-      <c r="Y84" s="115"/>
-      <c r="Z84" s="115"/>
-      <c r="AA84" s="115"/>
-    </row>
-    <row r="85" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G84" s="117"/>
+      <c r="H84" s="117"/>
+      <c r="I84" s="117"/>
+      <c r="J84" s="117"/>
+      <c r="K84" s="117"/>
+      <c r="L84" s="117"/>
+      <c r="M84" s="117"/>
+      <c r="N84" s="117"/>
+      <c r="O84" s="117"/>
+      <c r="P84" s="117"/>
+      <c r="Q84" s="117"/>
+      <c r="R84" s="117"/>
+      <c r="S84" s="117"/>
+      <c r="T84" s="117"/>
+      <c r="U84" s="117"/>
+      <c r="V84" s="117"/>
+      <c r="W84" s="117"/>
+      <c r="X84" s="117"/>
+      <c r="Y84" s="117"/>
+      <c r="Z84" s="117"/>
+      <c r="AA84" s="117"/>
+    </row>
+    <row r="85" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A85" s="38"/>
       <c r="B85" s="38" t="s">
         <v>150</v>
@@ -7344,34 +7341,34 @@
       <c r="E85" s="54">
         <v>1</v>
       </c>
-      <c r="F85" s="115" t="s">
+      <c r="F85" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="G85" s="115"/>
-      <c r="H85" s="115"/>
-      <c r="I85" s="115"/>
-      <c r="J85" s="115"/>
-      <c r="K85" s="115"/>
-      <c r="L85" s="115"/>
-      <c r="M85" s="115"/>
-      <c r="N85" s="115"/>
-      <c r="O85" s="115"/>
-      <c r="P85" s="115"/>
-      <c r="Q85" s="115" t="s">
+      <c r="G85" s="117"/>
+      <c r="H85" s="117"/>
+      <c r="I85" s="117"/>
+      <c r="J85" s="117"/>
+      <c r="K85" s="117"/>
+      <c r="L85" s="117"/>
+      <c r="M85" s="117"/>
+      <c r="N85" s="117"/>
+      <c r="O85" s="117"/>
+      <c r="P85" s="117"/>
+      <c r="Q85" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="R85" s="115"/>
-      <c r="S85" s="115"/>
-      <c r="T85" s="115"/>
-      <c r="U85" s="115"/>
-      <c r="V85" s="115"/>
-      <c r="W85" s="115"/>
-      <c r="X85" s="115"/>
-      <c r="Y85" s="115"/>
-      <c r="Z85" s="115"/>
-      <c r="AA85" s="115"/>
-    </row>
-    <row r="86" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R85" s="117"/>
+      <c r="S85" s="117"/>
+      <c r="T85" s="117"/>
+      <c r="U85" s="117"/>
+      <c r="V85" s="117"/>
+      <c r="W85" s="117"/>
+      <c r="X85" s="117"/>
+      <c r="Y85" s="117"/>
+      <c r="Z85" s="117"/>
+      <c r="AA85" s="117"/>
+    </row>
+    <row r="86" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="38" t="s">
         <v>205</v>
       </c>
@@ -7381,743 +7378,728 @@
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="115"/>
-      <c r="G86" s="115"/>
-      <c r="H86" s="115"/>
-      <c r="I86" s="115"/>
-      <c r="J86" s="115"/>
-      <c r="K86" s="115"/>
-      <c r="L86" s="115"/>
-      <c r="M86" s="115"/>
-      <c r="N86" s="115"/>
-      <c r="O86" s="115"/>
-      <c r="P86" s="115"/>
-      <c r="Q86" s="115"/>
-      <c r="R86" s="115"/>
-      <c r="S86" s="115"/>
-      <c r="T86" s="115"/>
-      <c r="U86" s="115"/>
-      <c r="V86" s="115"/>
-      <c r="W86" s="115"/>
-      <c r="X86" s="115"/>
-      <c r="Y86" s="115"/>
-      <c r="Z86" s="115"/>
-      <c r="AA86" s="115"/>
-    </row>
-    <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F86" s="117"/>
+      <c r="G86" s="117"/>
+      <c r="H86" s="117"/>
+      <c r="I86" s="117"/>
+      <c r="J86" s="117"/>
+      <c r="K86" s="117"/>
+      <c r="L86" s="117"/>
+      <c r="M86" s="117"/>
+      <c r="N86" s="117"/>
+      <c r="O86" s="117"/>
+      <c r="P86" s="117"/>
+      <c r="Q86" s="117"/>
+      <c r="R86" s="117"/>
+      <c r="S86" s="117"/>
+      <c r="T86" s="117"/>
+      <c r="U86" s="117"/>
+      <c r="V86" s="117"/>
+      <c r="W86" s="117"/>
+      <c r="X86" s="117"/>
+      <c r="Y86" s="117"/>
+      <c r="Z86" s="117"/>
+      <c r="AA86" s="117"/>
+    </row>
+    <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="38"/>
       <c r="B87" s="38"/>
       <c r="C87" s="65"/>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
-      <c r="F87" s="115"/>
-      <c r="G87" s="115"/>
-      <c r="H87" s="115"/>
-      <c r="I87" s="115"/>
-      <c r="J87" s="115"/>
-      <c r="K87" s="115"/>
-      <c r="L87" s="115"/>
-      <c r="M87" s="115"/>
-      <c r="N87" s="115"/>
-      <c r="O87" s="115"/>
-      <c r="P87" s="115"/>
-      <c r="Q87" s="115"/>
-      <c r="R87" s="115"/>
-      <c r="S87" s="115"/>
-      <c r="T87" s="115"/>
-      <c r="U87" s="115"/>
-      <c r="V87" s="115"/>
-      <c r="W87" s="115"/>
-      <c r="X87" s="115"/>
-      <c r="Y87" s="115"/>
-      <c r="Z87" s="115"/>
-      <c r="AA87" s="115"/>
-    </row>
-    <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F87" s="117"/>
+      <c r="G87" s="117"/>
+      <c r="H87" s="117"/>
+      <c r="I87" s="117"/>
+      <c r="J87" s="117"/>
+      <c r="K87" s="117"/>
+      <c r="L87" s="117"/>
+      <c r="M87" s="117"/>
+      <c r="N87" s="117"/>
+      <c r="O87" s="117"/>
+      <c r="P87" s="117"/>
+      <c r="Q87" s="117"/>
+      <c r="R87" s="117"/>
+      <c r="S87" s="117"/>
+      <c r="T87" s="117"/>
+      <c r="U87" s="117"/>
+      <c r="V87" s="117"/>
+      <c r="W87" s="117"/>
+      <c r="X87" s="117"/>
+      <c r="Y87" s="117"/>
+      <c r="Z87" s="117"/>
+      <c r="AA87" s="117"/>
+    </row>
+    <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="89" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="35"/>
       <c r="B90" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C90" s="127" t="s">
+      <c r="C90" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="D90" s="127"/>
-      <c r="E90" s="127"/>
-      <c r="F90" s="127"/>
-      <c r="G90" s="127"/>
-      <c r="H90" s="127" t="s">
+      <c r="D90" s="125"/>
+      <c r="E90" s="125"/>
+      <c r="F90" s="125"/>
+      <c r="G90" s="125"/>
+      <c r="H90" s="125" t="s">
         <v>141</v>
       </c>
-      <c r="I90" s="127"/>
-      <c r="J90" s="127"/>
-      <c r="K90" s="127"/>
-      <c r="L90" s="127"/>
-      <c r="M90" s="119" t="s">
+      <c r="I90" s="125"/>
+      <c r="J90" s="125"/>
+      <c r="K90" s="125"/>
+      <c r="L90" s="125"/>
+      <c r="M90" s="122" t="s">
         <v>189</v>
       </c>
-      <c r="N90" s="119"/>
+      <c r="N90" s="122"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A91" s="38" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="114" t="s">
+      <c r="C91" s="115" t="s">
         <v>184</v>
       </c>
-      <c r="D91" s="114"/>
-      <c r="E91" s="114"/>
-      <c r="F91" s="114"/>
-      <c r="G91" s="114"/>
-      <c r="H91" s="114" t="s">
+      <c r="D91" s="115"/>
+      <c r="E91" s="115"/>
+      <c r="F91" s="115"/>
+      <c r="G91" s="115"/>
+      <c r="H91" s="115" t="s">
         <v>186</v>
       </c>
-      <c r="I91" s="114"/>
-      <c r="J91" s="114"/>
-      <c r="K91" s="114"/>
-      <c r="L91" s="114"/>
-      <c r="M91" s="113" t="s">
+      <c r="I91" s="115"/>
+      <c r="J91" s="115"/>
+      <c r="K91" s="115"/>
+      <c r="L91" s="115"/>
+      <c r="M91" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N91" s="113"/>
+      <c r="N91" s="116"/>
       <c r="O91" s="65"/>
     </row>
-    <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A92" s="38" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C92" s="114" t="s">
+      <c r="C92" s="115" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="114"/>
-      <c r="E92" s="114"/>
-      <c r="F92" s="114"/>
-      <c r="G92" s="114"/>
-      <c r="H92" s="114" t="s">
+      <c r="D92" s="115"/>
+      <c r="E92" s="115"/>
+      <c r="F92" s="115"/>
+      <c r="G92" s="115"/>
+      <c r="H92" s="115" t="s">
         <v>188</v>
       </c>
-      <c r="I92" s="114"/>
-      <c r="J92" s="114"/>
-      <c r="K92" s="114"/>
-      <c r="L92" s="114"/>
-      <c r="M92" s="113" t="s">
+      <c r="I92" s="115"/>
+      <c r="J92" s="115"/>
+      <c r="K92" s="115"/>
+      <c r="L92" s="115"/>
+      <c r="M92" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N92" s="113"/>
+      <c r="N92" s="116"/>
       <c r="O92" s="65"/>
     </row>
-    <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A93" s="38" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="C93" s="114" t="s">
+      <c r="C93" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D93" s="114"/>
-      <c r="E93" s="114"/>
-      <c r="F93" s="114"/>
-      <c r="G93" s="114"/>
-      <c r="H93" s="114" t="s">
+      <c r="D93" s="115"/>
+      <c r="E93" s="115"/>
+      <c r="F93" s="115"/>
+      <c r="G93" s="115"/>
+      <c r="H93" s="115" t="s">
         <v>185</v>
       </c>
-      <c r="I93" s="114"/>
-      <c r="J93" s="114"/>
-      <c r="K93" s="114"/>
-      <c r="L93" s="114"/>
-      <c r="M93" s="113" t="s">
+      <c r="I93" s="115"/>
+      <c r="J93" s="115"/>
+      <c r="K93" s="115"/>
+      <c r="L93" s="115"/>
+      <c r="M93" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N93" s="113"/>
+      <c r="N93" s="116"/>
       <c r="O93" s="65"/>
     </row>
-    <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A94" s="38" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C94" s="114" t="s">
+      <c r="C94" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D94" s="114"/>
-      <c r="E94" s="114"/>
-      <c r="F94" s="114"/>
-      <c r="G94" s="114"/>
-      <c r="H94" s="114" t="s">
+      <c r="D94" s="115"/>
+      <c r="E94" s="115"/>
+      <c r="F94" s="115"/>
+      <c r="G94" s="115"/>
+      <c r="H94" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="I94" s="114"/>
-      <c r="J94" s="114"/>
-      <c r="K94" s="114"/>
-      <c r="L94" s="114"/>
-      <c r="M94" s="113" t="s">
+      <c r="I94" s="115"/>
+      <c r="J94" s="115"/>
+      <c r="K94" s="115"/>
+      <c r="L94" s="115"/>
+      <c r="M94" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N94" s="113"/>
+      <c r="N94" s="116"/>
       <c r="O94" s="65"/>
     </row>
-    <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A95" s="38" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C95" s="114" t="s">
+      <c r="C95" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D95" s="114"/>
-      <c r="E95" s="114"/>
-      <c r="F95" s="114"/>
-      <c r="G95" s="114"/>
-      <c r="H95" s="114" t="s">
+      <c r="D95" s="115"/>
+      <c r="E95" s="115"/>
+      <c r="F95" s="115"/>
+      <c r="G95" s="115"/>
+      <c r="H95" s="115" t="s">
         <v>222</v>
       </c>
-      <c r="I95" s="114"/>
-      <c r="J95" s="114"/>
-      <c r="K95" s="114"/>
-      <c r="L95" s="114"/>
-      <c r="M95" s="113" t="s">
+      <c r="I95" s="115"/>
+      <c r="J95" s="115"/>
+      <c r="K95" s="115"/>
+      <c r="L95" s="115"/>
+      <c r="M95" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N95" s="113"/>
+      <c r="N95" s="116"/>
       <c r="O95" s="65"/>
     </row>
-    <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A96" s="38" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C96" s="114" t="s">
+      <c r="C96" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D96" s="114"/>
-      <c r="E96" s="114"/>
-      <c r="F96" s="114"/>
-      <c r="G96" s="114"/>
-      <c r="H96" s="114" t="s">
+      <c r="D96" s="115"/>
+      <c r="E96" s="115"/>
+      <c r="F96" s="115"/>
+      <c r="G96" s="115"/>
+      <c r="H96" s="115" t="s">
         <v>223</v>
       </c>
-      <c r="I96" s="114"/>
-      <c r="J96" s="114"/>
-      <c r="K96" s="114"/>
-      <c r="L96" s="114"/>
-      <c r="M96" s="113" t="s">
+      <c r="I96" s="115"/>
+      <c r="J96" s="115"/>
+      <c r="K96" s="115"/>
+      <c r="L96" s="115"/>
+      <c r="M96" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N96" s="113"/>
+      <c r="N96" s="116"/>
       <c r="O96" s="65"/>
     </row>
-    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A97" s="38" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C97" s="114" t="s">
+      <c r="C97" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D97" s="114"/>
-      <c r="E97" s="114"/>
-      <c r="F97" s="114"/>
-      <c r="G97" s="114"/>
-      <c r="H97" s="114" t="s">
+      <c r="D97" s="115"/>
+      <c r="E97" s="115"/>
+      <c r="F97" s="115"/>
+      <c r="G97" s="115"/>
+      <c r="H97" s="115" t="s">
         <v>224</v>
       </c>
-      <c r="I97" s="114"/>
-      <c r="J97" s="114"/>
-      <c r="K97" s="114"/>
-      <c r="L97" s="114"/>
-      <c r="M97" s="113" t="s">
+      <c r="I97" s="115"/>
+      <c r="J97" s="115"/>
+      <c r="K97" s="115"/>
+      <c r="L97" s="115"/>
+      <c r="M97" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N97" s="113"/>
+      <c r="N97" s="116"/>
       <c r="O97" s="65"/>
     </row>
-    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A98" s="38" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="114" t="s">
+      <c r="C98" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D98" s="114"/>
-      <c r="E98" s="114"/>
-      <c r="F98" s="114"/>
-      <c r="G98" s="114"/>
-      <c r="H98" s="114" t="s">
+      <c r="D98" s="115"/>
+      <c r="E98" s="115"/>
+      <c r="F98" s="115"/>
+      <c r="G98" s="115"/>
+      <c r="H98" s="115" t="s">
         <v>225</v>
       </c>
-      <c r="I98" s="114"/>
-      <c r="J98" s="114"/>
-      <c r="K98" s="114"/>
-      <c r="L98" s="114"/>
-      <c r="M98" s="113" t="s">
+      <c r="I98" s="115"/>
+      <c r="J98" s="115"/>
+      <c r="K98" s="115"/>
+      <c r="L98" s="115"/>
+      <c r="M98" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N98" s="113"/>
+      <c r="N98" s="116"/>
       <c r="O98" s="65"/>
     </row>
-    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A99" s="38" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C99" s="114" t="s">
+      <c r="C99" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D99" s="114"/>
-      <c r="E99" s="114"/>
-      <c r="F99" s="114"/>
-      <c r="G99" s="114"/>
-      <c r="H99" s="114" t="s">
+      <c r="D99" s="115"/>
+      <c r="E99" s="115"/>
+      <c r="F99" s="115"/>
+      <c r="G99" s="115"/>
+      <c r="H99" s="115" t="s">
         <v>226</v>
       </c>
-      <c r="I99" s="114"/>
-      <c r="J99" s="114"/>
-      <c r="K99" s="114"/>
-      <c r="L99" s="114"/>
-      <c r="M99" s="113" t="s">
+      <c r="I99" s="115"/>
+      <c r="J99" s="115"/>
+      <c r="K99" s="115"/>
+      <c r="L99" s="115"/>
+      <c r="M99" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N99" s="113"/>
+      <c r="N99" s="116"/>
       <c r="O99" s="65"/>
     </row>
-    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A100" s="38" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="114" t="s">
+      <c r="C100" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="D100" s="114"/>
-      <c r="E100" s="114"/>
-      <c r="F100" s="114"/>
-      <c r="G100" s="114"/>
-      <c r="H100" s="114" t="s">
+      <c r="D100" s="115"/>
+      <c r="E100" s="115"/>
+      <c r="F100" s="115"/>
+      <c r="G100" s="115"/>
+      <c r="H100" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="I100" s="114"/>
-      <c r="J100" s="114"/>
-      <c r="K100" s="114"/>
-      <c r="L100" s="114"/>
-      <c r="M100" s="113" t="s">
+      <c r="I100" s="115"/>
+      <c r="J100" s="115"/>
+      <c r="K100" s="115"/>
+      <c r="L100" s="115"/>
+      <c r="M100" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="N100" s="113"/>
+      <c r="N100" s="116"/>
       <c r="O100" s="65"/>
     </row>
-    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="114"/>
-      <c r="D101" s="114"/>
-      <c r="E101" s="114"/>
-      <c r="F101" s="114"/>
-      <c r="G101" s="114"/>
-      <c r="H101" s="114"/>
-      <c r="I101" s="114"/>
-      <c r="J101" s="114"/>
-      <c r="K101" s="114"/>
-      <c r="L101" s="114"/>
-      <c r="M101" s="113"/>
-      <c r="N101" s="113"/>
+      <c r="C101" s="115"/>
+      <c r="D101" s="115"/>
+      <c r="E101" s="115"/>
+      <c r="F101" s="115"/>
+      <c r="G101" s="115"/>
+      <c r="H101" s="115"/>
+      <c r="I101" s="115"/>
+      <c r="J101" s="115"/>
+      <c r="K101" s="115"/>
+      <c r="L101" s="115"/>
+      <c r="M101" s="116"/>
+      <c r="N101" s="116"/>
       <c r="O101" s="65"/>
     </row>
-    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="114"/>
-      <c r="I102" s="114"/>
-      <c r="J102" s="114"/>
-      <c r="K102" s="114"/>
-      <c r="L102" s="114"/>
-      <c r="M102" s="113"/>
-      <c r="N102" s="113"/>
+      <c r="H102" s="115"/>
+      <c r="I102" s="115"/>
+      <c r="J102" s="115"/>
+      <c r="K102" s="115"/>
+      <c r="L102" s="115"/>
+      <c r="M102" s="116"/>
+      <c r="N102" s="116"/>
       <c r="O102" s="65"/>
     </row>
-    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="114"/>
-      <c r="D103" s="114"/>
-      <c r="E103" s="114"/>
-      <c r="F103" s="114"/>
-      <c r="G103" s="114"/>
-      <c r="H103" s="114"/>
-      <c r="I103" s="114"/>
-      <c r="J103" s="114"/>
-      <c r="K103" s="114"/>
-      <c r="L103" s="114"/>
-      <c r="M103" s="113"/>
-      <c r="N103" s="113"/>
+      <c r="C103" s="115"/>
+      <c r="D103" s="115"/>
+      <c r="E103" s="115"/>
+      <c r="F103" s="115"/>
+      <c r="G103" s="115"/>
+      <c r="H103" s="115"/>
+      <c r="I103" s="115"/>
+      <c r="J103" s="115"/>
+      <c r="K103" s="115"/>
+      <c r="L103" s="115"/>
+      <c r="M103" s="116"/>
+      <c r="N103" s="116"/>
       <c r="O103" s="65"/>
     </row>
-    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="114"/>
-      <c r="D104" s="114"/>
-      <c r="E104" s="114"/>
-      <c r="F104" s="114"/>
-      <c r="G104" s="114"/>
-      <c r="H104" s="114"/>
-      <c r="I104" s="114"/>
-      <c r="J104" s="114"/>
-      <c r="K104" s="114"/>
-      <c r="L104" s="114"/>
-      <c r="M104" s="113"/>
-      <c r="N104" s="113"/>
+      <c r="C104" s="115"/>
+      <c r="D104" s="115"/>
+      <c r="E104" s="115"/>
+      <c r="F104" s="115"/>
+      <c r="G104" s="115"/>
+      <c r="H104" s="115"/>
+      <c r="I104" s="115"/>
+      <c r="J104" s="115"/>
+      <c r="K104" s="115"/>
+      <c r="L104" s="115"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
       <c r="O104" s="65"/>
     </row>
-    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="114"/>
-      <c r="D105" s="114"/>
-      <c r="E105" s="114"/>
-      <c r="F105" s="114"/>
-      <c r="G105" s="114"/>
-      <c r="H105" s="114"/>
-      <c r="I105" s="114"/>
-      <c r="J105" s="114"/>
-      <c r="K105" s="114"/>
-      <c r="L105" s="114"/>
-      <c r="M105" s="113"/>
-      <c r="N105" s="113"/>
+      <c r="C105" s="115"/>
+      <c r="D105" s="115"/>
+      <c r="E105" s="115"/>
+      <c r="F105" s="115"/>
+      <c r="G105" s="115"/>
+      <c r="H105" s="115"/>
+      <c r="I105" s="115"/>
+      <c r="J105" s="115"/>
+      <c r="K105" s="115"/>
+      <c r="L105" s="115"/>
+      <c r="M105" s="116"/>
+      <c r="N105" s="116"/>
       <c r="O105" s="65"/>
     </row>
-    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="114"/>
-      <c r="D106" s="114"/>
-      <c r="E106" s="114"/>
-      <c r="F106" s="114"/>
-      <c r="G106" s="114"/>
-      <c r="H106" s="114"/>
-      <c r="I106" s="114"/>
-      <c r="J106" s="114"/>
-      <c r="K106" s="114"/>
-      <c r="L106" s="114"/>
-      <c r="M106" s="113"/>
-      <c r="N106" s="113"/>
+      <c r="C106" s="115"/>
+      <c r="D106" s="115"/>
+      <c r="E106" s="115"/>
+      <c r="F106" s="115"/>
+      <c r="G106" s="115"/>
+      <c r="H106" s="115"/>
+      <c r="I106" s="115"/>
+      <c r="J106" s="115"/>
+      <c r="K106" s="115"/>
+      <c r="L106" s="115"/>
+      <c r="M106" s="116"/>
+      <c r="N106" s="116"/>
       <c r="O106" s="65"/>
     </row>
-    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="114"/>
-      <c r="D107" s="114"/>
-      <c r="E107" s="114"/>
-      <c r="F107" s="114"/>
-      <c r="G107" s="114"/>
-      <c r="H107" s="114"/>
-      <c r="I107" s="114"/>
-      <c r="J107" s="114"/>
-      <c r="K107" s="114"/>
-      <c r="L107" s="114"/>
-      <c r="M107" s="113"/>
-      <c r="N107" s="113"/>
+      <c r="C107" s="115"/>
+      <c r="D107" s="115"/>
+      <c r="E107" s="115"/>
+      <c r="F107" s="115"/>
+      <c r="G107" s="115"/>
+      <c r="H107" s="115"/>
+      <c r="I107" s="115"/>
+      <c r="J107" s="115"/>
+      <c r="K107" s="115"/>
+      <c r="L107" s="115"/>
+      <c r="M107" s="116"/>
+      <c r="N107" s="116"/>
       <c r="O107" s="65"/>
     </row>
-    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="114"/>
-      <c r="D108" s="114"/>
-      <c r="E108" s="114"/>
-      <c r="F108" s="114"/>
-      <c r="G108" s="114"/>
-      <c r="H108" s="114"/>
-      <c r="I108" s="114"/>
-      <c r="J108" s="114"/>
-      <c r="K108" s="114"/>
-      <c r="L108" s="114"/>
-      <c r="M108" s="113"/>
-      <c r="N108" s="113"/>
+      <c r="C108" s="115"/>
+      <c r="D108" s="115"/>
+      <c r="E108" s="115"/>
+      <c r="F108" s="115"/>
+      <c r="G108" s="115"/>
+      <c r="H108" s="115"/>
+      <c r="I108" s="115"/>
+      <c r="J108" s="115"/>
+      <c r="K108" s="115"/>
+      <c r="L108" s="115"/>
+      <c r="M108" s="116"/>
+      <c r="N108" s="116"/>
       <c r="O108" s="65"/>
     </row>
-    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="114"/>
-      <c r="D109" s="114"/>
-      <c r="E109" s="114"/>
-      <c r="F109" s="114"/>
-      <c r="G109" s="114"/>
-      <c r="H109" s="114"/>
-      <c r="I109" s="114"/>
-      <c r="J109" s="114"/>
-      <c r="K109" s="114"/>
-      <c r="L109" s="114"/>
-      <c r="M109" s="113"/>
-      <c r="N109" s="113"/>
+      <c r="C109" s="115"/>
+      <c r="D109" s="115"/>
+      <c r="E109" s="115"/>
+      <c r="F109" s="115"/>
+      <c r="G109" s="115"/>
+      <c r="H109" s="115"/>
+      <c r="I109" s="115"/>
+      <c r="J109" s="115"/>
+      <c r="K109" s="115"/>
+      <c r="L109" s="115"/>
+      <c r="M109" s="116"/>
+      <c r="N109" s="116"/>
       <c r="O109" s="65"/>
     </row>
-    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="114"/>
-      <c r="D110" s="114"/>
-      <c r="E110" s="114"/>
-      <c r="F110" s="114"/>
-      <c r="G110" s="114"/>
-      <c r="H110" s="114"/>
-      <c r="I110" s="114"/>
-      <c r="J110" s="114"/>
-      <c r="K110" s="114"/>
-      <c r="L110" s="114"/>
-      <c r="M110" s="113"/>
-      <c r="N110" s="113"/>
+      <c r="C110" s="115"/>
+      <c r="D110" s="115"/>
+      <c r="E110" s="115"/>
+      <c r="F110" s="115"/>
+      <c r="G110" s="115"/>
+      <c r="H110" s="115"/>
+      <c r="I110" s="115"/>
+      <c r="J110" s="115"/>
+      <c r="K110" s="115"/>
+      <c r="L110" s="115"/>
+      <c r="M110" s="116"/>
+      <c r="N110" s="116"/>
       <c r="O110" s="65"/>
     </row>
-    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="114"/>
-      <c r="D111" s="114"/>
-      <c r="E111" s="114"/>
-      <c r="F111" s="114"/>
-      <c r="G111" s="114"/>
-      <c r="H111" s="114"/>
-      <c r="I111" s="114"/>
-      <c r="J111" s="114"/>
-      <c r="K111" s="114"/>
-      <c r="L111" s="114"/>
-      <c r="M111" s="113"/>
-      <c r="N111" s="113"/>
+      <c r="C111" s="115"/>
+      <c r="D111" s="115"/>
+      <c r="E111" s="115"/>
+      <c r="F111" s="115"/>
+      <c r="G111" s="115"/>
+      <c r="H111" s="115"/>
+      <c r="I111" s="115"/>
+      <c r="J111" s="115"/>
+      <c r="K111" s="115"/>
+      <c r="L111" s="115"/>
+      <c r="M111" s="116"/>
+      <c r="N111" s="116"/>
       <c r="O111" s="65"/>
     </row>
-    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="114"/>
-      <c r="D112" s="114"/>
-      <c r="E112" s="114"/>
-      <c r="F112" s="114"/>
-      <c r="G112" s="114"/>
-      <c r="H112" s="114"/>
-      <c r="I112" s="114"/>
-      <c r="J112" s="114"/>
-      <c r="K112" s="114"/>
-      <c r="L112" s="114"/>
-      <c r="M112" s="113"/>
-      <c r="N112" s="113"/>
+      <c r="C112" s="115"/>
+      <c r="D112" s="115"/>
+      <c r="E112" s="115"/>
+      <c r="F112" s="115"/>
+      <c r="G112" s="115"/>
+      <c r="H112" s="115"/>
+      <c r="I112" s="115"/>
+      <c r="J112" s="115"/>
+      <c r="K112" s="115"/>
+      <c r="L112" s="115"/>
+      <c r="M112" s="116"/>
+      <c r="N112" s="116"/>
       <c r="O112" s="65"/>
     </row>
-    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="114"/>
-      <c r="D113" s="114"/>
-      <c r="E113" s="114"/>
-      <c r="F113" s="114"/>
-      <c r="G113" s="114"/>
-      <c r="H113" s="114"/>
-      <c r="I113" s="114"/>
-      <c r="J113" s="114"/>
-      <c r="K113" s="114"/>
-      <c r="L113" s="114"/>
-      <c r="M113" s="113"/>
-      <c r="N113" s="113"/>
+      <c r="C113" s="115"/>
+      <c r="D113" s="115"/>
+      <c r="E113" s="115"/>
+      <c r="F113" s="115"/>
+      <c r="G113" s="115"/>
+      <c r="H113" s="115"/>
+      <c r="I113" s="115"/>
+      <c r="J113" s="115"/>
+      <c r="K113" s="115"/>
+      <c r="L113" s="115"/>
+      <c r="M113" s="116"/>
+      <c r="N113" s="116"/>
       <c r="O113" s="65"/>
     </row>
-    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="114"/>
-      <c r="D114" s="114"/>
-      <c r="E114" s="114"/>
-      <c r="F114" s="114"/>
-      <c r="G114" s="114"/>
-      <c r="H114" s="114"/>
-      <c r="I114" s="114"/>
-      <c r="J114" s="114"/>
-      <c r="K114" s="114"/>
-      <c r="L114" s="114"/>
-      <c r="M114" s="113"/>
-      <c r="N114" s="113"/>
+      <c r="C114" s="115"/>
+      <c r="D114" s="115"/>
+      <c r="E114" s="115"/>
+      <c r="F114" s="115"/>
+      <c r="G114" s="115"/>
+      <c r="H114" s="115"/>
+      <c r="I114" s="115"/>
+      <c r="J114" s="115"/>
+      <c r="K114" s="115"/>
+      <c r="L114" s="115"/>
+      <c r="M114" s="116"/>
+      <c r="N114" s="116"/>
       <c r="O114" s="65"/>
     </row>
-    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="114"/>
-      <c r="D115" s="114"/>
-      <c r="E115" s="114"/>
-      <c r="F115" s="114"/>
-      <c r="G115" s="114"/>
-      <c r="H115" s="114"/>
-      <c r="I115" s="114"/>
-      <c r="J115" s="114"/>
-      <c r="K115" s="114"/>
-      <c r="L115" s="114"/>
-      <c r="M115" s="113"/>
-      <c r="N115" s="113"/>
+      <c r="C115" s="115"/>
+      <c r="D115" s="115"/>
+      <c r="E115" s="115"/>
+      <c r="F115" s="115"/>
+      <c r="G115" s="115"/>
+      <c r="H115" s="115"/>
+      <c r="I115" s="115"/>
+      <c r="J115" s="115"/>
+      <c r="K115" s="115"/>
+      <c r="L115" s="115"/>
+      <c r="M115" s="116"/>
+      <c r="N115" s="116"/>
       <c r="O115" s="65"/>
     </row>
-    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="114"/>
-      <c r="D116" s="114"/>
-      <c r="E116" s="114"/>
-      <c r="F116" s="114"/>
-      <c r="G116" s="114"/>
-      <c r="H116" s="114"/>
-      <c r="I116" s="114"/>
-      <c r="J116" s="114"/>
-      <c r="K116" s="114"/>
-      <c r="L116" s="114"/>
-      <c r="M116" s="113"/>
-      <c r="N116" s="113"/>
+      <c r="C116" s="115"/>
+      <c r="D116" s="115"/>
+      <c r="E116" s="115"/>
+      <c r="F116" s="115"/>
+      <c r="G116" s="115"/>
+      <c r="H116" s="115"/>
+      <c r="I116" s="115"/>
+      <c r="J116" s="115"/>
+      <c r="K116" s="115"/>
+      <c r="L116" s="115"/>
+      <c r="M116" s="116"/>
+      <c r="N116" s="116"/>
       <c r="O116" s="65"/>
     </row>
-    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="114"/>
-      <c r="D117" s="114"/>
-      <c r="E117" s="114"/>
-      <c r="F117" s="114"/>
-      <c r="G117" s="114"/>
-      <c r="H117" s="114"/>
-      <c r="I117" s="114"/>
-      <c r="J117" s="114"/>
-      <c r="K117" s="114"/>
-      <c r="L117" s="114"/>
-      <c r="M117" s="113"/>
-      <c r="N117" s="113"/>
+      <c r="C117" s="115"/>
+      <c r="D117" s="115"/>
+      <c r="E117" s="115"/>
+      <c r="F117" s="115"/>
+      <c r="G117" s="115"/>
+      <c r="H117" s="115"/>
+      <c r="I117" s="115"/>
+      <c r="J117" s="115"/>
+      <c r="K117" s="115"/>
+      <c r="L117" s="115"/>
+      <c r="M117" s="116"/>
+      <c r="N117" s="116"/>
       <c r="O117" s="65"/>
     </row>
-    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="114"/>
-      <c r="D118" s="114"/>
-      <c r="E118" s="114"/>
-      <c r="F118" s="114"/>
-      <c r="G118" s="114"/>
-      <c r="H118" s="114"/>
-      <c r="I118" s="114"/>
-      <c r="J118" s="114"/>
-      <c r="K118" s="114"/>
-      <c r="L118" s="114"/>
-      <c r="M118" s="113"/>
-      <c r="N118" s="113"/>
+      <c r="C118" s="115"/>
+      <c r="D118" s="115"/>
+      <c r="E118" s="115"/>
+      <c r="F118" s="115"/>
+      <c r="G118" s="115"/>
+      <c r="H118" s="115"/>
+      <c r="I118" s="115"/>
+      <c r="J118" s="115"/>
+      <c r="K118" s="115"/>
+      <c r="L118" s="115"/>
+      <c r="M118" s="116"/>
+      <c r="N118" s="116"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="H54:M54"/>
+    <mergeCell ref="H58:M58"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
     <mergeCell ref="C92:G92"/>
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="Q77:R77"/>
@@ -8142,73 +8124,88 @@
     <mergeCell ref="M93:N93"/>
     <mergeCell ref="Q81:AA81"/>
     <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="H54:M54"/>
-    <mergeCell ref="H58:M58"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pistol buffed (shake 3 => 2) Fennek and APC speed is changed
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD118C1C-4BD3-439E-83C1-92A923EFBE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FFAA6-B1BF-45DF-981E-B4078C4F281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2336,69 +2336,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3509,8 +3509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3528,10 +3528,10 @@
       <c r="B1" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="131"/>
+      <c r="D1" s="125"/>
       <c r="G1" s="56" t="s">
         <v>162</v>
       </c>
@@ -3627,10 +3627,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="123" t="s">
+      <c r="Z2" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="123"/>
+      <c r="AA2" s="130"/>
       <c r="AG2" s="43" t="s">
         <v>85</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>576</v>
       </c>
       <c r="D16" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="19">
         <v>1</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="R16" s="19">
         <f>ROUND(D16/H16,3)</f>
-        <v>0.2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="S16" s="28" t="s">
         <v>29</v>
@@ -5920,28 +5920,28 @@
       <c r="B40" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="129" t="s">
+      <c r="C40" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="129"/>
-      <c r="E40" s="129"/>
-      <c r="F40" s="129"/>
-      <c r="G40" s="129"/>
-      <c r="H40" s="129"/>
-      <c r="I40" s="129" t="s">
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="129"/>
-      <c r="K40" s="129"/>
-      <c r="L40" s="129"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="118"/>
+      <c r="L40" s="118"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="128" t="s">
+      <c r="S40" s="131" t="s">
         <v>78</v>
       </c>
-      <c r="T40" s="128"/>
+      <c r="T40" s="131"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -5951,30 +5951,30 @@
       <c r="B41" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="130" t="s">
+      <c r="C41" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="130" t="s">
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="130"/>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130" t="s">
+      <c r="G41" s="119"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="J41" s="130"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="130"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="119"/>
+      <c r="L41" s="119"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="128" t="s">
+      <c r="S41" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="T41" s="128"/>
+      <c r="T41" s="131"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -5987,30 +5987,30 @@
       <c r="B42" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="130" t="s">
+      <c r="C42" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="130"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="130" t="s">
+      <c r="D42" s="119"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119" t="s">
         <v>203</v>
       </c>
-      <c r="G42" s="130"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130" t="s">
+      <c r="G42" s="119"/>
+      <c r="H42" s="119"/>
+      <c r="I42" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="J42" s="130"/>
-      <c r="K42" s="130"/>
-      <c r="L42" s="130"/>
+      <c r="J42" s="119"/>
+      <c r="K42" s="119"/>
+      <c r="L42" s="119"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="128" t="s">
+      <c r="S42" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="T42" s="128"/>
+      <c r="T42" s="131"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6023,30 +6023,30 @@
       <c r="B43" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C43" s="126" t="s">
+      <c r="C43" s="120" t="s">
         <v>210</v>
       </c>
-      <c r="D43" s="126"/>
-      <c r="E43" s="126"/>
-      <c r="F43" s="126" t="s">
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120" t="s">
         <v>211</v>
       </c>
-      <c r="G43" s="126"/>
-      <c r="H43" s="126"/>
-      <c r="I43" s="126" t="s">
+      <c r="G43" s="120"/>
+      <c r="H43" s="120"/>
+      <c r="I43" s="120" t="s">
         <v>208</v>
       </c>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="126"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="128" t="s">
+      <c r="S43" s="131" t="s">
         <v>99</v>
       </c>
-      <c r="T43" s="128"/>
+      <c r="T43" s="131"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6061,20 +6061,20 @@
       <c r="B44" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="126" t="s">
+      <c r="C44" s="120" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="126"/>
-      <c r="E44" s="126"/>
-      <c r="F44" s="126"/>
-      <c r="G44" s="126"/>
-      <c r="H44" s="126"/>
-      <c r="I44" s="126" t="s">
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="120"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="120"/>
+      <c r="I44" s="120" t="s">
         <v>209</v>
       </c>
-      <c r="J44" s="126"/>
-      <c r="K44" s="126"/>
-      <c r="L44" s="126"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6090,16 +6090,16 @@
       <c r="B47" s="77" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="129" t="s">
+      <c r="C47" s="118" t="s">
         <v>195</v>
       </c>
-      <c r="D47" s="129"/>
-      <c r="E47" s="129" t="s">
+      <c r="D47" s="118"/>
+      <c r="E47" s="118" t="s">
         <v>194</v>
       </c>
-      <c r="F47" s="129"/>
-      <c r="G47" s="129"/>
-      <c r="H47" s="129"/>
+      <c r="F47" s="118"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="118"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -6110,16 +6110,16 @@
       <c r="B48" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="C48" s="130">
+      <c r="C48" s="119">
         <v>2</v>
       </c>
-      <c r="D48" s="130"/>
-      <c r="E48" s="130" t="s">
+      <c r="D48" s="119"/>
+      <c r="E48" s="119" t="s">
         <v>199</v>
       </c>
-      <c r="F48" s="130"/>
-      <c r="G48" s="130"/>
-      <c r="H48" s="130"/>
+      <c r="F48" s="119"/>
+      <c r="G48" s="119"/>
+      <c r="H48" s="119"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
@@ -6130,28 +6130,28 @@
       <c r="B49" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="130" t="s">
+      <c r="C49" s="119" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="130"/>
-      <c r="E49" s="130" t="s">
+      <c r="D49" s="119"/>
+      <c r="E49" s="119" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="130"/>
-      <c r="G49" s="130"/>
-      <c r="H49" s="130"/>
+      <c r="F49" s="119"/>
+      <c r="G49" s="119"/>
+      <c r="H49" s="119"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="126"/>
-      <c r="D50" s="126"/>
-      <c r="E50" s="126"/>
-      <c r="F50" s="126"/>
-      <c r="G50" s="126"/>
-      <c r="H50" s="126"/>
+      <c r="C50" s="120"/>
+      <c r="D50" s="120"/>
+      <c r="E50" s="120"/>
+      <c r="F50" s="120"/>
+      <c r="G50" s="120"/>
+      <c r="H50" s="120"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6169,14 +6169,14 @@
       <c r="D54" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="H54" s="135" t="s">
+      <c r="H54" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="I54" s="135"/>
-      <c r="J54" s="135"/>
-      <c r="K54" s="135"/>
-      <c r="L54" s="135"/>
-      <c r="M54" s="135"/>
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6327,14 +6327,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="136" t="s">
+      <c r="H58" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="I58" s="136"/>
-      <c r="J58" s="136"/>
-      <c r="K58" s="136"/>
-      <c r="L58" s="136"/>
-      <c r="M58" s="136"/>
+      <c r="I58" s="124"/>
+      <c r="J58" s="124"/>
+      <c r="K58" s="124"/>
+      <c r="L58" s="124"/>
+      <c r="M58" s="124"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6383,10 +6383,10 @@
       <c r="I62" t="s">
         <v>97</v>
       </c>
-      <c r="J62" s="133" t="s">
+      <c r="J62" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="K62" s="133"/>
+      <c r="K62" s="127"/>
       <c r="L62" t="s">
         <v>102</v>
       </c>
@@ -6394,13 +6394,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="O62" s="132" t="s">
+      <c r="O62" s="126" t="s">
         <v>107</v>
       </c>
-      <c r="P62" s="132"/>
-      <c r="Q62" s="132"/>
-      <c r="R62" s="132"/>
-      <c r="S62" s="132"/>
+      <c r="P62" s="126"/>
+      <c r="Q62" s="126"/>
+      <c r="R62" s="126"/>
+      <c r="S62" s="126"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6422,20 +6422,20 @@
       <c r="E63" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="F63" s="118" t="s">
+      <c r="F63" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="G63" s="118"/>
+      <c r="G63" s="132"/>
       <c r="H63" s="86" t="s">
         <v>191</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="118" t="s">
+      <c r="J63" s="132" t="s">
         <v>98</v>
       </c>
-      <c r="K63" s="118"/>
+      <c r="K63" s="132"/>
       <c r="L63" s="86" t="s">
         <v>103</v>
       </c>
@@ -6459,10 +6459,10 @@
         <v>114</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="118" t="s">
+      <c r="U63" s="132" t="s">
         <v>118</v>
       </c>
-      <c r="V63" s="118"/>
+      <c r="V63" s="132"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6490,21 +6490,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="134" t="s">
+      <c r="F64" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="G64" s="134"/>
+      <c r="G64" s="133"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="121">
+      <c r="J64" s="122">
         <f t="shared" ref="J64:J69" si="17">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="121"/>
+      <c r="K64" s="122"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>11</v>
@@ -6535,11 +6535,11 @@
         <v>10.100000000000001</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="119">
+      <c r="U64" s="135">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="119"/>
+      <c r="V64" s="135"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6565,23 +6565,23 @@
         <v>60</v>
       </c>
       <c r="E65" s="54">
-        <v>3</v>
-      </c>
-      <c r="F65" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="G65" s="116"/>
+      <c r="G65" s="115"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="121">
+      <c r="J65" s="122">
         <f t="shared" si="17"/>
         <v>32</v>
       </c>
-      <c r="K65" s="121"/>
+      <c r="K65" s="122"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6601,7 +6601,7 @@
       </c>
       <c r="Q65" s="68">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R65" s="69">
         <f t="shared" si="21"/>
@@ -6609,14 +6609,14 @@
       </c>
       <c r="S65" s="70">
         <f t="shared" ref="S65:S69" si="23">SUM(O65:R65)</f>
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="120">
+      <c r="U65" s="136">
         <f t="shared" ref="U65:U70" si="24">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="120"/>
+      <c r="V65" s="136"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6642,23 +6642,23 @@
         <v>50</v>
       </c>
       <c r="E66" s="54">
-        <v>4</v>
-      </c>
-      <c r="F66" s="116" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="116"/>
+      <c r="G66" s="115"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="121">
+      <c r="J66" s="122">
         <f t="shared" si="17"/>
         <v>28</v>
       </c>
-      <c r="K66" s="121"/>
+      <c r="K66" s="122"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="Q66" s="68">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R66" s="69">
         <f t="shared" si="21"/>
@@ -6686,14 +6686,14 @@
       </c>
       <c r="S66" s="70">
         <f t="shared" si="23"/>
-        <v>14.399999999999999</v>
+        <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="120">
+      <c r="U66" s="136">
         <f t="shared" si="24"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="120"/>
+      <c r="V66" s="136"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6721,21 +6721,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="116" t="s">
+      <c r="F67" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="116"/>
+      <c r="G67" s="115"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="121">
+      <c r="J67" s="122">
         <f t="shared" si="17"/>
         <v>48</v>
       </c>
-      <c r="K67" s="121"/>
+      <c r="K67" s="122"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6766,11 +6766,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="120">
+      <c r="U67" s="136">
         <f t="shared" si="24"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="120"/>
+      <c r="V67" s="136"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6794,21 +6794,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="116" t="s">
+      <c r="F68" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="116"/>
+      <c r="G68" s="115"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="121">
+      <c r="J68" s="122">
         <f t="shared" si="17"/>
         <v>72</v>
       </c>
-      <c r="K68" s="121"/>
+      <c r="K68" s="122"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -6839,11 +6839,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="120">
+      <c r="U68" s="136">
         <f t="shared" si="24"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="120"/>
+      <c r="V68" s="136"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6867,21 +6867,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="116" t="s">
+      <c r="F69" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="116"/>
+      <c r="G69" s="115"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="121">
+      <c r="J69" s="122">
         <f t="shared" si="17"/>
         <v>20</v>
       </c>
-      <c r="K69" s="121"/>
+      <c r="K69" s="122"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6912,11 +6912,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="120">
+      <c r="U69" s="136">
         <f t="shared" si="24"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="120"/>
+      <c r="V69" s="136"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6940,21 +6940,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="116" t="s">
+      <c r="F70" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="G70" s="116"/>
+      <c r="G70" s="115"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="121">
+      <c r="J70" s="122">
         <f t="shared" ref="J70" si="25">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="121"/>
+      <c r="K70" s="122"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -6985,11 +6985,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="120">
+      <c r="U70" s="136">
         <f t="shared" si="24"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="120"/>
+      <c r="V70" s="136"/>
       <c r="W70" s="25" t="s">
         <v>75</v>
       </c>
@@ -7002,12 +7002,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="123" t="s">
+      <c r="O73" s="130" t="s">
         <v>169</v>
       </c>
-      <c r="P73" s="123"/>
-      <c r="Q73" s="123"/>
-      <c r="R73" s="123"/>
+      <c r="P73" s="130"/>
+      <c r="Q73" s="130"/>
+      <c r="R73" s="130"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7023,31 +7023,31 @@
       <c r="E74" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="F74" s="122" t="s">
+      <c r="F74" s="121" t="s">
         <v>137</v>
       </c>
-      <c r="G74" s="122"/>
-      <c r="H74" s="122" t="s">
+      <c r="G74" s="121"/>
+      <c r="H74" s="121" t="s">
         <v>138</v>
       </c>
-      <c r="I74" s="122"/>
-      <c r="J74" s="122" t="s">
+      <c r="I74" s="121"/>
+      <c r="J74" s="121" t="s">
         <v>135</v>
       </c>
-      <c r="K74" s="122"/>
-      <c r="L74" s="122"/>
-      <c r="M74" s="122"/>
+      <c r="K74" s="121"/>
+      <c r="L74" s="121"/>
+      <c r="M74" s="121"/>
       <c r="N74" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="O74" s="122" t="s">
+      <c r="O74" s="121" t="s">
         <v>171</v>
       </c>
-      <c r="P74" s="122"/>
-      <c r="Q74" s="122" t="s">
+      <c r="P74" s="121"/>
+      <c r="Q74" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="R74" s="122"/>
+      <c r="R74" s="121"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="28">
@@ -7065,21 +7065,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="121" t="s">
+      <c r="F75" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="G75" s="121"/>
-      <c r="H75" s="121">
+      <c r="G75" s="122"/>
+      <c r="H75" s="122">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="121"/>
-      <c r="J75" s="121" t="s">
+      <c r="I75" s="122"/>
+      <c r="J75" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="K75" s="121"/>
-      <c r="L75" s="121"/>
-      <c r="M75" s="121"/>
+      <c r="K75" s="122"/>
+      <c r="L75" s="122"/>
+      <c r="M75" s="122"/>
       <c r="N75" s="78" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -7108,21 +7108,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="121" t="s">
+      <c r="F76" s="122" t="s">
         <v>127</v>
       </c>
-      <c r="G76" s="121"/>
-      <c r="H76" s="121">
+      <c r="G76" s="122"/>
+      <c r="H76" s="122">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="121"/>
-      <c r="J76" s="121" t="s">
+      <c r="I76" s="122"/>
+      <c r="J76" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="K76" s="121"/>
-      <c r="L76" s="121"/>
-      <c r="M76" s="121"/>
+      <c r="K76" s="122"/>
+      <c r="L76" s="122"/>
+      <c r="M76" s="122"/>
       <c r="N76" s="78" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -7141,19 +7141,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="126"/>
-      <c r="G77" s="126"/>
-      <c r="H77" s="126"/>
-      <c r="I77" s="126"/>
-      <c r="J77" s="126"/>
-      <c r="K77" s="126"/>
-      <c r="L77" s="126"/>
-      <c r="M77" s="126"/>
+      <c r="F77" s="120"/>
+      <c r="G77" s="120"/>
+      <c r="H77" s="120"/>
+      <c r="I77" s="120"/>
+      <c r="J77" s="120"/>
+      <c r="K77" s="120"/>
+      <c r="L77" s="120"/>
+      <c r="M77" s="120"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="124"/>
-      <c r="P77" s="124"/>
-      <c r="Q77" s="124"/>
-      <c r="R77" s="124"/>
+      <c r="O77" s="128"/>
+      <c r="P77" s="128"/>
+      <c r="Q77" s="128"/>
+      <c r="R77" s="128"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7181,32 +7181,32 @@
       <c r="E81" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="F81" s="122" t="s">
+      <c r="F81" s="121" t="s">
         <v>141</v>
       </c>
-      <c r="G81" s="122"/>
-      <c r="H81" s="122"/>
-      <c r="I81" s="122"/>
-      <c r="J81" s="122"/>
-      <c r="K81" s="122"/>
-      <c r="L81" s="122"/>
-      <c r="M81" s="122"/>
-      <c r="N81" s="122"/>
-      <c r="O81" s="122"/>
-      <c r="P81" s="122"/>
-      <c r="Q81" s="122" t="s">
+      <c r="G81" s="121"/>
+      <c r="H81" s="121"/>
+      <c r="I81" s="121"/>
+      <c r="J81" s="121"/>
+      <c r="K81" s="121"/>
+      <c r="L81" s="121"/>
+      <c r="M81" s="121"/>
+      <c r="N81" s="121"/>
+      <c r="O81" s="121"/>
+      <c r="P81" s="121"/>
+      <c r="Q81" s="121" t="s">
         <v>156</v>
       </c>
-      <c r="R81" s="122"/>
-      <c r="S81" s="122"/>
-      <c r="T81" s="122"/>
-      <c r="U81" s="122"/>
-      <c r="V81" s="122"/>
-      <c r="W81" s="122"/>
-      <c r="X81" s="122"/>
-      <c r="Y81" s="122"/>
-      <c r="Z81" s="122"/>
-      <c r="AA81" s="122"/>
+      <c r="R81" s="121"/>
+      <c r="S81" s="121"/>
+      <c r="T81" s="121"/>
+      <c r="U81" s="121"/>
+      <c r="V81" s="121"/>
+      <c r="W81" s="121"/>
+      <c r="X81" s="121"/>
+      <c r="Y81" s="121"/>
+      <c r="Z81" s="121"/>
+      <c r="AA81" s="121"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7222,32 +7222,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="127" t="s">
+      <c r="F82" s="134" t="s">
         <v>152</v>
       </c>
-      <c r="G82" s="127"/>
-      <c r="H82" s="127"/>
-      <c r="I82" s="127"/>
-      <c r="J82" s="127"/>
-      <c r="K82" s="127"/>
-      <c r="L82" s="127"/>
-      <c r="M82" s="127"/>
-      <c r="N82" s="127"/>
-      <c r="O82" s="127"/>
-      <c r="P82" s="127"/>
-      <c r="Q82" s="127" t="s">
+      <c r="G82" s="134"/>
+      <c r="H82" s="134"/>
+      <c r="I82" s="134"/>
+      <c r="J82" s="134"/>
+      <c r="K82" s="134"/>
+      <c r="L82" s="134"/>
+      <c r="M82" s="134"/>
+      <c r="N82" s="134"/>
+      <c r="O82" s="134"/>
+      <c r="P82" s="134"/>
+      <c r="Q82" s="134" t="s">
         <v>157</v>
       </c>
-      <c r="R82" s="127"/>
-      <c r="S82" s="127"/>
-      <c r="T82" s="127"/>
-      <c r="U82" s="127"/>
-      <c r="V82" s="127"/>
-      <c r="W82" s="127"/>
-      <c r="X82" s="127"/>
-      <c r="Y82" s="127"/>
-      <c r="Z82" s="127"/>
-      <c r="AA82" s="127"/>
+      <c r="R82" s="134"/>
+      <c r="S82" s="134"/>
+      <c r="T82" s="134"/>
+      <c r="U82" s="134"/>
+      <c r="V82" s="134"/>
+      <c r="W82" s="134"/>
+      <c r="X82" s="134"/>
+      <c r="Y82" s="134"/>
+      <c r="Z82" s="134"/>
+      <c r="AA82" s="134"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7437,24 +7437,24 @@
       <c r="B90" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C90" s="125" t="s">
+      <c r="C90" s="129" t="s">
         <v>181</v>
       </c>
-      <c r="D90" s="125"/>
-      <c r="E90" s="125"/>
-      <c r="F90" s="125"/>
-      <c r="G90" s="125"/>
-      <c r="H90" s="125" t="s">
+      <c r="D90" s="129"/>
+      <c r="E90" s="129"/>
+      <c r="F90" s="129"/>
+      <c r="G90" s="129"/>
+      <c r="H90" s="129" t="s">
         <v>141</v>
       </c>
-      <c r="I90" s="125"/>
-      <c r="J90" s="125"/>
-      <c r="K90" s="125"/>
-      <c r="L90" s="125"/>
-      <c r="M90" s="122" t="s">
+      <c r="I90" s="129"/>
+      <c r="J90" s="129"/>
+      <c r="K90" s="129"/>
+      <c r="L90" s="129"/>
+      <c r="M90" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="N90" s="122"/>
+      <c r="N90" s="121"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>200</v>
@@ -7467,24 +7467,24 @@
       <c r="B91" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="115" t="s">
+      <c r="C91" s="116" t="s">
         <v>184</v>
       </c>
-      <c r="D91" s="115"/>
-      <c r="E91" s="115"/>
-      <c r="F91" s="115"/>
-      <c r="G91" s="115"/>
-      <c r="H91" s="115" t="s">
+      <c r="D91" s="116"/>
+      <c r="E91" s="116"/>
+      <c r="F91" s="116"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="116" t="s">
         <v>186</v>
       </c>
-      <c r="I91" s="115"/>
-      <c r="J91" s="115"/>
-      <c r="K91" s="115"/>
-      <c r="L91" s="115"/>
-      <c r="M91" s="116" t="s">
+      <c r="I91" s="116"/>
+      <c r="J91" s="116"/>
+      <c r="K91" s="116"/>
+      <c r="L91" s="116"/>
+      <c r="M91" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N91" s="116"/>
+      <c r="N91" s="115"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7494,24 +7494,24 @@
       <c r="B92" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C92" s="115" t="s">
+      <c r="C92" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="115"/>
-      <c r="E92" s="115"/>
-      <c r="F92" s="115"/>
-      <c r="G92" s="115"/>
-      <c r="H92" s="115" t="s">
+      <c r="D92" s="116"/>
+      <c r="E92" s="116"/>
+      <c r="F92" s="116"/>
+      <c r="G92" s="116"/>
+      <c r="H92" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="I92" s="115"/>
-      <c r="J92" s="115"/>
-      <c r="K92" s="115"/>
-      <c r="L92" s="115"/>
-      <c r="M92" s="116" t="s">
+      <c r="I92" s="116"/>
+      <c r="J92" s="116"/>
+      <c r="K92" s="116"/>
+      <c r="L92" s="116"/>
+      <c r="M92" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N92" s="116"/>
+      <c r="N92" s="115"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7521,24 +7521,24 @@
       <c r="B93" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="C93" s="115" t="s">
+      <c r="C93" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D93" s="115"/>
-      <c r="E93" s="115"/>
-      <c r="F93" s="115"/>
-      <c r="G93" s="115"/>
-      <c r="H93" s="115" t="s">
+      <c r="D93" s="116"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="116"/>
+      <c r="G93" s="116"/>
+      <c r="H93" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="I93" s="115"/>
-      <c r="J93" s="115"/>
-      <c r="K93" s="115"/>
-      <c r="L93" s="115"/>
-      <c r="M93" s="116" t="s">
+      <c r="I93" s="116"/>
+      <c r="J93" s="116"/>
+      <c r="K93" s="116"/>
+      <c r="L93" s="116"/>
+      <c r="M93" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N93" s="116"/>
+      <c r="N93" s="115"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7548,24 +7548,24 @@
       <c r="B94" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C94" s="115" t="s">
+      <c r="C94" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D94" s="115"/>
-      <c r="E94" s="115"/>
-      <c r="F94" s="115"/>
-      <c r="G94" s="115"/>
-      <c r="H94" s="115" t="s">
+      <c r="D94" s="116"/>
+      <c r="E94" s="116"/>
+      <c r="F94" s="116"/>
+      <c r="G94" s="116"/>
+      <c r="H94" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="I94" s="115"/>
-      <c r="J94" s="115"/>
-      <c r="K94" s="115"/>
-      <c r="L94" s="115"/>
-      <c r="M94" s="116" t="s">
+      <c r="I94" s="116"/>
+      <c r="J94" s="116"/>
+      <c r="K94" s="116"/>
+      <c r="L94" s="116"/>
+      <c r="M94" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N94" s="116"/>
+      <c r="N94" s="115"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7575,24 +7575,24 @@
       <c r="B95" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C95" s="115" t="s">
+      <c r="C95" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D95" s="115"/>
-      <c r="E95" s="115"/>
-      <c r="F95" s="115"/>
-      <c r="G95" s="115"/>
-      <c r="H95" s="115" t="s">
+      <c r="D95" s="116"/>
+      <c r="E95" s="116"/>
+      <c r="F95" s="116"/>
+      <c r="G95" s="116"/>
+      <c r="H95" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="I95" s="115"/>
-      <c r="J95" s="115"/>
-      <c r="K95" s="115"/>
-      <c r="L95" s="115"/>
-      <c r="M95" s="116" t="s">
+      <c r="I95" s="116"/>
+      <c r="J95" s="116"/>
+      <c r="K95" s="116"/>
+      <c r="L95" s="116"/>
+      <c r="M95" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N95" s="116"/>
+      <c r="N95" s="115"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7602,24 +7602,24 @@
       <c r="B96" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C96" s="115" t="s">
+      <c r="C96" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D96" s="115"/>
-      <c r="E96" s="115"/>
-      <c r="F96" s="115"/>
-      <c r="G96" s="115"/>
-      <c r="H96" s="115" t="s">
+      <c r="D96" s="116"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="116"/>
+      <c r="G96" s="116"/>
+      <c r="H96" s="116" t="s">
         <v>223</v>
       </c>
-      <c r="I96" s="115"/>
-      <c r="J96" s="115"/>
-      <c r="K96" s="115"/>
-      <c r="L96" s="115"/>
-      <c r="M96" s="116" t="s">
+      <c r="I96" s="116"/>
+      <c r="J96" s="116"/>
+      <c r="K96" s="116"/>
+      <c r="L96" s="116"/>
+      <c r="M96" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N96" s="116"/>
+      <c r="N96" s="115"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7629,24 +7629,24 @@
       <c r="B97" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C97" s="115" t="s">
+      <c r="C97" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D97" s="115"/>
-      <c r="E97" s="115"/>
-      <c r="F97" s="115"/>
-      <c r="G97" s="115"/>
-      <c r="H97" s="115" t="s">
+      <c r="D97" s="116"/>
+      <c r="E97" s="116"/>
+      <c r="F97" s="116"/>
+      <c r="G97" s="116"/>
+      <c r="H97" s="116" t="s">
         <v>224</v>
       </c>
-      <c r="I97" s="115"/>
-      <c r="J97" s="115"/>
-      <c r="K97" s="115"/>
-      <c r="L97" s="115"/>
-      <c r="M97" s="116" t="s">
+      <c r="I97" s="116"/>
+      <c r="J97" s="116"/>
+      <c r="K97" s="116"/>
+      <c r="L97" s="116"/>
+      <c r="M97" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N97" s="116"/>
+      <c r="N97" s="115"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7656,24 +7656,24 @@
       <c r="B98" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="115" t="s">
+      <c r="C98" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D98" s="115"/>
-      <c r="E98" s="115"/>
-      <c r="F98" s="115"/>
-      <c r="G98" s="115"/>
-      <c r="H98" s="115" t="s">
+      <c r="D98" s="116"/>
+      <c r="E98" s="116"/>
+      <c r="F98" s="116"/>
+      <c r="G98" s="116"/>
+      <c r="H98" s="116" t="s">
         <v>225</v>
       </c>
-      <c r="I98" s="115"/>
-      <c r="J98" s="115"/>
-      <c r="K98" s="115"/>
-      <c r="L98" s="115"/>
-      <c r="M98" s="116" t="s">
+      <c r="I98" s="116"/>
+      <c r="J98" s="116"/>
+      <c r="K98" s="116"/>
+      <c r="L98" s="116"/>
+      <c r="M98" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N98" s="116"/>
+      <c r="N98" s="115"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7683,24 +7683,24 @@
       <c r="B99" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C99" s="115" t="s">
+      <c r="C99" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D99" s="115"/>
-      <c r="E99" s="115"/>
-      <c r="F99" s="115"/>
-      <c r="G99" s="115"/>
-      <c r="H99" s="115" t="s">
+      <c r="D99" s="116"/>
+      <c r="E99" s="116"/>
+      <c r="F99" s="116"/>
+      <c r="G99" s="116"/>
+      <c r="H99" s="116" t="s">
         <v>226</v>
       </c>
-      <c r="I99" s="115"/>
-      <c r="J99" s="115"/>
-      <c r="K99" s="115"/>
-      <c r="L99" s="115"/>
-      <c r="M99" s="116" t="s">
+      <c r="I99" s="116"/>
+      <c r="J99" s="116"/>
+      <c r="K99" s="116"/>
+      <c r="L99" s="116"/>
+      <c r="M99" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N99" s="116"/>
+      <c r="N99" s="115"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7710,329 +7710,478 @@
       <c r="B100" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="115" t="s">
+      <c r="C100" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="D100" s="115"/>
-      <c r="E100" s="115"/>
-      <c r="F100" s="115"/>
-      <c r="G100" s="115"/>
-      <c r="H100" s="115" t="s">
+      <c r="D100" s="116"/>
+      <c r="E100" s="116"/>
+      <c r="F100" s="116"/>
+      <c r="G100" s="116"/>
+      <c r="H100" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="I100" s="115"/>
-      <c r="J100" s="115"/>
-      <c r="K100" s="115"/>
-      <c r="L100" s="115"/>
-      <c r="M100" s="116" t="s">
+      <c r="I100" s="116"/>
+      <c r="J100" s="116"/>
+      <c r="K100" s="116"/>
+      <c r="L100" s="116"/>
+      <c r="M100" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="N100" s="116"/>
+      <c r="N100" s="115"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="115"/>
-      <c r="D101" s="115"/>
-      <c r="E101" s="115"/>
-      <c r="F101" s="115"/>
-      <c r="G101" s="115"/>
-      <c r="H101" s="115"/>
-      <c r="I101" s="115"/>
-      <c r="J101" s="115"/>
-      <c r="K101" s="115"/>
-      <c r="L101" s="115"/>
-      <c r="M101" s="116"/>
-      <c r="N101" s="116"/>
+      <c r="C101" s="116"/>
+      <c r="D101" s="116"/>
+      <c r="E101" s="116"/>
+      <c r="F101" s="116"/>
+      <c r="G101" s="116"/>
+      <c r="H101" s="116"/>
+      <c r="I101" s="116"/>
+      <c r="J101" s="116"/>
+      <c r="K101" s="116"/>
+      <c r="L101" s="116"/>
+      <c r="M101" s="115"/>
+      <c r="N101" s="115"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="115"/>
-      <c r="I102" s="115"/>
-      <c r="J102" s="115"/>
-      <c r="K102" s="115"/>
-      <c r="L102" s="115"/>
-      <c r="M102" s="116"/>
-      <c r="N102" s="116"/>
+      <c r="H102" s="116"/>
+      <c r="I102" s="116"/>
+      <c r="J102" s="116"/>
+      <c r="K102" s="116"/>
+      <c r="L102" s="116"/>
+      <c r="M102" s="115"/>
+      <c r="N102" s="115"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="115"/>
-      <c r="D103" s="115"/>
-      <c r="E103" s="115"/>
-      <c r="F103" s="115"/>
-      <c r="G103" s="115"/>
-      <c r="H103" s="115"/>
-      <c r="I103" s="115"/>
-      <c r="J103" s="115"/>
-      <c r="K103" s="115"/>
-      <c r="L103" s="115"/>
-      <c r="M103" s="116"/>
-      <c r="N103" s="116"/>
+      <c r="C103" s="116"/>
+      <c r="D103" s="116"/>
+      <c r="E103" s="116"/>
+      <c r="F103" s="116"/>
+      <c r="G103" s="116"/>
+      <c r="H103" s="116"/>
+      <c r="I103" s="116"/>
+      <c r="J103" s="116"/>
+      <c r="K103" s="116"/>
+      <c r="L103" s="116"/>
+      <c r="M103" s="115"/>
+      <c r="N103" s="115"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="115"/>
-      <c r="D104" s="115"/>
-      <c r="E104" s="115"/>
-      <c r="F104" s="115"/>
-      <c r="G104" s="115"/>
-      <c r="H104" s="115"/>
-      <c r="I104" s="115"/>
-      <c r="J104" s="115"/>
-      <c r="K104" s="115"/>
-      <c r="L104" s="115"/>
-      <c r="M104" s="116"/>
-      <c r="N104" s="116"/>
+      <c r="C104" s="116"/>
+      <c r="D104" s="116"/>
+      <c r="E104" s="116"/>
+      <c r="F104" s="116"/>
+      <c r="G104" s="116"/>
+      <c r="H104" s="116"/>
+      <c r="I104" s="116"/>
+      <c r="J104" s="116"/>
+      <c r="K104" s="116"/>
+      <c r="L104" s="116"/>
+      <c r="M104" s="115"/>
+      <c r="N104" s="115"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="115"/>
-      <c r="D105" s="115"/>
-      <c r="E105" s="115"/>
-      <c r="F105" s="115"/>
-      <c r="G105" s="115"/>
-      <c r="H105" s="115"/>
-      <c r="I105" s="115"/>
-      <c r="J105" s="115"/>
-      <c r="K105" s="115"/>
-      <c r="L105" s="115"/>
-      <c r="M105" s="116"/>
-      <c r="N105" s="116"/>
+      <c r="C105" s="116"/>
+      <c r="D105" s="116"/>
+      <c r="E105" s="116"/>
+      <c r="F105" s="116"/>
+      <c r="G105" s="116"/>
+      <c r="H105" s="116"/>
+      <c r="I105" s="116"/>
+      <c r="J105" s="116"/>
+      <c r="K105" s="116"/>
+      <c r="L105" s="116"/>
+      <c r="M105" s="115"/>
+      <c r="N105" s="115"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="115"/>
-      <c r="D106" s="115"/>
-      <c r="E106" s="115"/>
-      <c r="F106" s="115"/>
-      <c r="G106" s="115"/>
-      <c r="H106" s="115"/>
-      <c r="I106" s="115"/>
-      <c r="J106" s="115"/>
-      <c r="K106" s="115"/>
-      <c r="L106" s="115"/>
-      <c r="M106" s="116"/>
-      <c r="N106" s="116"/>
+      <c r="C106" s="116"/>
+      <c r="D106" s="116"/>
+      <c r="E106" s="116"/>
+      <c r="F106" s="116"/>
+      <c r="G106" s="116"/>
+      <c r="H106" s="116"/>
+      <c r="I106" s="116"/>
+      <c r="J106" s="116"/>
+      <c r="K106" s="116"/>
+      <c r="L106" s="116"/>
+      <c r="M106" s="115"/>
+      <c r="N106" s="115"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="115"/>
-      <c r="D107" s="115"/>
-      <c r="E107" s="115"/>
-      <c r="F107" s="115"/>
-      <c r="G107" s="115"/>
-      <c r="H107" s="115"/>
-      <c r="I107" s="115"/>
-      <c r="J107" s="115"/>
-      <c r="K107" s="115"/>
-      <c r="L107" s="115"/>
-      <c r="M107" s="116"/>
-      <c r="N107" s="116"/>
+      <c r="C107" s="116"/>
+      <c r="D107" s="116"/>
+      <c r="E107" s="116"/>
+      <c r="F107" s="116"/>
+      <c r="G107" s="116"/>
+      <c r="H107" s="116"/>
+      <c r="I107" s="116"/>
+      <c r="J107" s="116"/>
+      <c r="K107" s="116"/>
+      <c r="L107" s="116"/>
+      <c r="M107" s="115"/>
+      <c r="N107" s="115"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="115"/>
-      <c r="D108" s="115"/>
-      <c r="E108" s="115"/>
-      <c r="F108" s="115"/>
-      <c r="G108" s="115"/>
-      <c r="H108" s="115"/>
-      <c r="I108" s="115"/>
-      <c r="J108" s="115"/>
-      <c r="K108" s="115"/>
-      <c r="L108" s="115"/>
-      <c r="M108" s="116"/>
-      <c r="N108" s="116"/>
+      <c r="C108" s="116"/>
+      <c r="D108" s="116"/>
+      <c r="E108" s="116"/>
+      <c r="F108" s="116"/>
+      <c r="G108" s="116"/>
+      <c r="H108" s="116"/>
+      <c r="I108" s="116"/>
+      <c r="J108" s="116"/>
+      <c r="K108" s="116"/>
+      <c r="L108" s="116"/>
+      <c r="M108" s="115"/>
+      <c r="N108" s="115"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="115"/>
-      <c r="D109" s="115"/>
-      <c r="E109" s="115"/>
-      <c r="F109" s="115"/>
-      <c r="G109" s="115"/>
-      <c r="H109" s="115"/>
-      <c r="I109" s="115"/>
-      <c r="J109" s="115"/>
-      <c r="K109" s="115"/>
-      <c r="L109" s="115"/>
-      <c r="M109" s="116"/>
-      <c r="N109" s="116"/>
+      <c r="C109" s="116"/>
+      <c r="D109" s="116"/>
+      <c r="E109" s="116"/>
+      <c r="F109" s="116"/>
+      <c r="G109" s="116"/>
+      <c r="H109" s="116"/>
+      <c r="I109" s="116"/>
+      <c r="J109" s="116"/>
+      <c r="K109" s="116"/>
+      <c r="L109" s="116"/>
+      <c r="M109" s="115"/>
+      <c r="N109" s="115"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="115"/>
-      <c r="D110" s="115"/>
-      <c r="E110" s="115"/>
-      <c r="F110" s="115"/>
-      <c r="G110" s="115"/>
-      <c r="H110" s="115"/>
-      <c r="I110" s="115"/>
-      <c r="J110" s="115"/>
-      <c r="K110" s="115"/>
-      <c r="L110" s="115"/>
-      <c r="M110" s="116"/>
-      <c r="N110" s="116"/>
+      <c r="C110" s="116"/>
+      <c r="D110" s="116"/>
+      <c r="E110" s="116"/>
+      <c r="F110" s="116"/>
+      <c r="G110" s="116"/>
+      <c r="H110" s="116"/>
+      <c r="I110" s="116"/>
+      <c r="J110" s="116"/>
+      <c r="K110" s="116"/>
+      <c r="L110" s="116"/>
+      <c r="M110" s="115"/>
+      <c r="N110" s="115"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="115"/>
-      <c r="D111" s="115"/>
-      <c r="E111" s="115"/>
-      <c r="F111" s="115"/>
-      <c r="G111" s="115"/>
-      <c r="H111" s="115"/>
-      <c r="I111" s="115"/>
-      <c r="J111" s="115"/>
-      <c r="K111" s="115"/>
-      <c r="L111" s="115"/>
-      <c r="M111" s="116"/>
-      <c r="N111" s="116"/>
+      <c r="C111" s="116"/>
+      <c r="D111" s="116"/>
+      <c r="E111" s="116"/>
+      <c r="F111" s="116"/>
+      <c r="G111" s="116"/>
+      <c r="H111" s="116"/>
+      <c r="I111" s="116"/>
+      <c r="J111" s="116"/>
+      <c r="K111" s="116"/>
+      <c r="L111" s="116"/>
+      <c r="M111" s="115"/>
+      <c r="N111" s="115"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="115"/>
-      <c r="D112" s="115"/>
-      <c r="E112" s="115"/>
-      <c r="F112" s="115"/>
-      <c r="G112" s="115"/>
-      <c r="H112" s="115"/>
-      <c r="I112" s="115"/>
-      <c r="J112" s="115"/>
-      <c r="K112" s="115"/>
-      <c r="L112" s="115"/>
-      <c r="M112" s="116"/>
-      <c r="N112" s="116"/>
+      <c r="C112" s="116"/>
+      <c r="D112" s="116"/>
+      <c r="E112" s="116"/>
+      <c r="F112" s="116"/>
+      <c r="G112" s="116"/>
+      <c r="H112" s="116"/>
+      <c r="I112" s="116"/>
+      <c r="J112" s="116"/>
+      <c r="K112" s="116"/>
+      <c r="L112" s="116"/>
+      <c r="M112" s="115"/>
+      <c r="N112" s="115"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="115"/>
-      <c r="D113" s="115"/>
-      <c r="E113" s="115"/>
-      <c r="F113" s="115"/>
-      <c r="G113" s="115"/>
-      <c r="H113" s="115"/>
-      <c r="I113" s="115"/>
-      <c r="J113" s="115"/>
-      <c r="K113" s="115"/>
-      <c r="L113" s="115"/>
-      <c r="M113" s="116"/>
-      <c r="N113" s="116"/>
+      <c r="C113" s="116"/>
+      <c r="D113" s="116"/>
+      <c r="E113" s="116"/>
+      <c r="F113" s="116"/>
+      <c r="G113" s="116"/>
+      <c r="H113" s="116"/>
+      <c r="I113" s="116"/>
+      <c r="J113" s="116"/>
+      <c r="K113" s="116"/>
+      <c r="L113" s="116"/>
+      <c r="M113" s="115"/>
+      <c r="N113" s="115"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="115"/>
-      <c r="D114" s="115"/>
-      <c r="E114" s="115"/>
-      <c r="F114" s="115"/>
-      <c r="G114" s="115"/>
-      <c r="H114" s="115"/>
-      <c r="I114" s="115"/>
-      <c r="J114" s="115"/>
-      <c r="K114" s="115"/>
-      <c r="L114" s="115"/>
-      <c r="M114" s="116"/>
-      <c r="N114" s="116"/>
+      <c r="C114" s="116"/>
+      <c r="D114" s="116"/>
+      <c r="E114" s="116"/>
+      <c r="F114" s="116"/>
+      <c r="G114" s="116"/>
+      <c r="H114" s="116"/>
+      <c r="I114" s="116"/>
+      <c r="J114" s="116"/>
+      <c r="K114" s="116"/>
+      <c r="L114" s="116"/>
+      <c r="M114" s="115"/>
+      <c r="N114" s="115"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="115"/>
-      <c r="D115" s="115"/>
-      <c r="E115" s="115"/>
-      <c r="F115" s="115"/>
-      <c r="G115" s="115"/>
-      <c r="H115" s="115"/>
-      <c r="I115" s="115"/>
-      <c r="J115" s="115"/>
-      <c r="K115" s="115"/>
-      <c r="L115" s="115"/>
-      <c r="M115" s="116"/>
-      <c r="N115" s="116"/>
+      <c r="C115" s="116"/>
+      <c r="D115" s="116"/>
+      <c r="E115" s="116"/>
+      <c r="F115" s="116"/>
+      <c r="G115" s="116"/>
+      <c r="H115" s="116"/>
+      <c r="I115" s="116"/>
+      <c r="J115" s="116"/>
+      <c r="K115" s="116"/>
+      <c r="L115" s="116"/>
+      <c r="M115" s="115"/>
+      <c r="N115" s="115"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="115"/>
-      <c r="D116" s="115"/>
-      <c r="E116" s="115"/>
-      <c r="F116" s="115"/>
-      <c r="G116" s="115"/>
-      <c r="H116" s="115"/>
-      <c r="I116" s="115"/>
-      <c r="J116" s="115"/>
-      <c r="K116" s="115"/>
-      <c r="L116" s="115"/>
-      <c r="M116" s="116"/>
-      <c r="N116" s="116"/>
+      <c r="C116" s="116"/>
+      <c r="D116" s="116"/>
+      <c r="E116" s="116"/>
+      <c r="F116" s="116"/>
+      <c r="G116" s="116"/>
+      <c r="H116" s="116"/>
+      <c r="I116" s="116"/>
+      <c r="J116" s="116"/>
+      <c r="K116" s="116"/>
+      <c r="L116" s="116"/>
+      <c r="M116" s="115"/>
+      <c r="N116" s="115"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="115"/>
-      <c r="D117" s="115"/>
-      <c r="E117" s="115"/>
-      <c r="F117" s="115"/>
-      <c r="G117" s="115"/>
-      <c r="H117" s="115"/>
-      <c r="I117" s="115"/>
-      <c r="J117" s="115"/>
-      <c r="K117" s="115"/>
-      <c r="L117" s="115"/>
-      <c r="M117" s="116"/>
-      <c r="N117" s="116"/>
+      <c r="C117" s="116"/>
+      <c r="D117" s="116"/>
+      <c r="E117" s="116"/>
+      <c r="F117" s="116"/>
+      <c r="G117" s="116"/>
+      <c r="H117" s="116"/>
+      <c r="I117" s="116"/>
+      <c r="J117" s="116"/>
+      <c r="K117" s="116"/>
+      <c r="L117" s="116"/>
+      <c r="M117" s="115"/>
+      <c r="N117" s="115"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="115"/>
-      <c r="D118" s="115"/>
-      <c r="E118" s="115"/>
-      <c r="F118" s="115"/>
-      <c r="G118" s="115"/>
-      <c r="H118" s="115"/>
-      <c r="I118" s="115"/>
-      <c r="J118" s="115"/>
-      <c r="K118" s="115"/>
-      <c r="L118" s="115"/>
-      <c r="M118" s="116"/>
-      <c r="N118" s="116"/>
+      <c r="C118" s="116"/>
+      <c r="D118" s="116"/>
+      <c r="E118" s="116"/>
+      <c r="F118" s="116"/>
+      <c r="G118" s="116"/>
+      <c r="H118" s="116"/>
+      <c r="I118" s="116"/>
+      <c r="J118" s="116"/>
+      <c r="K118" s="116"/>
+      <c r="L118" s="116"/>
+      <c r="M118" s="115"/>
+      <c r="N118" s="115"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
     <mergeCell ref="M96:N96"/>
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="Q83:AA83"/>
@@ -8057,155 +8206,6 @@
     <mergeCell ref="J65:K65"/>
     <mergeCell ref="J66:K66"/>
     <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nerfed shotgun: shotgun range reduced
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FFAA6-B1BF-45DF-981E-B4078C4F281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BBA59-F43E-47D1-BBCD-8FB448CAF4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1147,14 +1147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Drop a tank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Drop one of these guns [grenade launcer, AWM, tank buster], and a scope(+2), and an armor (reduce)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Can transport the caller player when able to pickup. Player then can get off the plane on its route.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1449,6 +1441,14 @@
   </si>
   <si>
     <t>priority in deathmatch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drop a medkit, a scope(+2), and an armor (reduce)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drop a Fennek</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3509,8 +3509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3526,14 +3526,14 @@
     <row r="1" spans="1:38" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="82"/>
       <c r="B1" s="83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" s="125" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D1" s="125"/>
       <c r="G1" s="56" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>0</v>
@@ -3560,7 +3560,7 @@
     <row r="2" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="35"/>
       <c r="B2" s="77" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C2" s="84" t="s">
         <v>7</v>
@@ -3637,7 +3637,7 @@
       <c r="AH2" s="39"/>
       <c r="AI2" s="39"/>
       <c r="AL2" s="114" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -3995,10 +3995,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="74">
         <v>0</v>
@@ -4022,7 +4022,7 @@
         <v>1000</v>
       </c>
       <c r="K7" s="75" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L7" s="74"/>
       <c r="M7" s="19"/>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T7" s="74"/>
       <c r="U7" s="19"/>
@@ -4047,7 +4047,7 @@
       <c r="X7" s="26"/>
       <c r="Y7" s="74"/>
       <c r="Z7" s="57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AL7" s="36"/>
     </row>
@@ -5016,7 +5016,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="51">
-        <v>320</v>
+        <v>180</v>
       </c>
       <c r="D23" s="19">
         <v>4</v>
@@ -5103,7 +5103,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="52">
-        <v>448</v>
+        <v>320</v>
       </c>
       <c r="D24" s="19">
         <v>2</v>
@@ -5188,7 +5188,7 @@
         <v>45</v>
       </c>
       <c r="C25" s="52">
-        <v>448</v>
+        <v>320</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
@@ -5918,7 +5918,7 @@
     <row r="40" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="35"/>
       <c r="B40" s="77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C40" s="118" t="s">
         <v>57</v>
@@ -5993,7 +5993,7 @@
       <c r="D42" s="119"/>
       <c r="E42" s="119"/>
       <c r="F42" s="119" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G42" s="119"/>
       <c r="H42" s="119"/>
@@ -6018,23 +6018,23 @@
     </row>
     <row r="43" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C43" s="120" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D43" s="120"/>
       <c r="E43" s="120"/>
       <c r="F43" s="120" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G43" s="120"/>
       <c r="H43" s="120"/>
       <c r="I43" s="120" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J43" s="120"/>
       <c r="K43" s="120"/>
@@ -6056,13 +6056,13 @@
     </row>
     <row r="44" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>207</v>
-      </c>
       <c r="C44" s="120" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D44" s="120"/>
       <c r="E44" s="120"/>
@@ -6070,7 +6070,7 @@
       <c r="G44" s="120"/>
       <c r="H44" s="120"/>
       <c r="I44" s="120" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J44" s="120"/>
       <c r="K44" s="120"/>
@@ -6088,14 +6088,14 @@
     <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="35"/>
       <c r="B47" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="118" t="s">
         <v>193</v>
-      </c>
-      <c r="C47" s="118" t="s">
-        <v>195</v>
       </c>
       <c r="D47" s="118"/>
       <c r="E47" s="118" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F47" s="118"/>
       <c r="G47" s="118"/>
@@ -6108,14 +6108,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C48" s="119">
         <v>2</v>
       </c>
       <c r="D48" s="119"/>
       <c r="E48" s="119" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F48" s="119"/>
       <c r="G48" s="119"/>
@@ -6128,10 +6128,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="119" t="s">
         <v>196</v>
-      </c>
-      <c r="C49" s="119" t="s">
-        <v>198</v>
       </c>
       <c r="D49" s="119"/>
       <c r="E49" s="119" t="s">
@@ -6159,15 +6159,15 @@
     <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A53" s="58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C54" s="63" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H54" s="123" t="s">
         <v>69</v>
@@ -6181,7 +6181,7 @@
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
       <c r="B55" s="87" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C55" s="88">
         <v>-1</v>
@@ -6319,7 +6319,7 @@
     </row>
     <row r="58" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C58" s="64" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D58" s="60" t="s">
         <v>77</v>
@@ -6328,7 +6328,7 @@
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
       <c r="H58" s="124" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I58" s="124"/>
       <c r="J58" s="124"/>
@@ -6411,7 +6411,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="85" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C63" s="86" t="s">
         <v>90</v>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="G63" s="132"/>
       <c r="H63" s="86" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
@@ -7003,7 +7003,7 @@
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O73" s="130" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P73" s="130"/>
       <c r="Q73" s="130"/>
@@ -7038,14 +7038,14 @@
       <c r="L74" s="121"/>
       <c r="M74" s="121"/>
       <c r="N74" s="107" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O74" s="121" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P74" s="121"/>
       <c r="Q74" s="121" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="R74" s="121"/>
     </row>
@@ -7157,10 +7157,10 @@
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B78" s="112" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -7195,7 +7195,7 @@
       <c r="O81" s="121"/>
       <c r="P81" s="121"/>
       <c r="Q81" s="121" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="R81" s="121"/>
       <c r="S81" s="121"/>
@@ -7236,7 +7236,7 @@
       <c r="O82" s="134"/>
       <c r="P82" s="134"/>
       <c r="Q82" s="134" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R82" s="134"/>
       <c r="S82" s="134"/>
@@ -7264,7 +7264,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="117" t="s">
-        <v>154</v>
+        <v>227</v>
       </c>
       <c r="G83" s="117"/>
       <c r="H83" s="117"/>
@@ -7303,7 +7303,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="117" t="s">
-        <v>153</v>
+        <v>228</v>
       </c>
       <c r="G84" s="117"/>
       <c r="H84" s="117"/>
@@ -7342,7 +7342,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="117" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G85" s="117"/>
       <c r="H85" s="117"/>
@@ -7355,7 +7355,7 @@
       <c r="O85" s="117"/>
       <c r="P85" s="117"/>
       <c r="Q85" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R85" s="117"/>
       <c r="S85" s="117"/>
@@ -7370,10 +7370,10 @@
     </row>
     <row r="86" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
@@ -7435,10 +7435,10 @@
     <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="35"/>
       <c r="B90" s="77" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C90" s="129" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D90" s="129"/>
       <c r="E90" s="129"/>
@@ -7452,12 +7452,12 @@
       <c r="K90" s="129"/>
       <c r="L90" s="129"/>
       <c r="M90" s="121" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N90" s="121"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7465,24 +7465,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="116" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="116"/>
       <c r="F91" s="116"/>
       <c r="G91" s="116"/>
       <c r="H91" s="116" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I91" s="116"/>
       <c r="J91" s="116"/>
       <c r="K91" s="116"/>
       <c r="L91" s="116"/>
       <c r="M91" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N91" s="115"/>
       <c r="O91" s="65"/>
@@ -7492,24 +7492,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C92" s="116" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D92" s="116"/>
       <c r="E92" s="116"/>
       <c r="F92" s="116"/>
       <c r="G92" s="116"/>
       <c r="H92" s="116" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I92" s="116"/>
       <c r="J92" s="116"/>
       <c r="K92" s="116"/>
       <c r="L92" s="116"/>
       <c r="M92" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N92" s="115"/>
       <c r="O92" s="65"/>
@@ -7519,24 +7519,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C93" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D93" s="116"/>
       <c r="E93" s="116"/>
       <c r="F93" s="116"/>
       <c r="G93" s="116"/>
       <c r="H93" s="116" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I93" s="116"/>
       <c r="J93" s="116"/>
       <c r="K93" s="116"/>
       <c r="L93" s="116"/>
       <c r="M93" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N93" s="115"/>
       <c r="O93" s="65"/>
@@ -7546,24 +7546,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C94" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="116"/>
       <c r="F94" s="116"/>
       <c r="G94" s="116"/>
       <c r="H94" s="116" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I94" s="116"/>
       <c r="J94" s="116"/>
       <c r="K94" s="116"/>
       <c r="L94" s="116"/>
       <c r="M94" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N94" s="115"/>
       <c r="O94" s="65"/>
@@ -7573,24 +7573,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C95" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D95" s="116"/>
       <c r="E95" s="116"/>
       <c r="F95" s="116"/>
       <c r="G95" s="116"/>
       <c r="H95" s="116" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I95" s="116"/>
       <c r="J95" s="116"/>
       <c r="K95" s="116"/>
       <c r="L95" s="116"/>
       <c r="M95" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N95" s="115"/>
       <c r="O95" s="65"/>
@@ -7600,24 +7600,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C96" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D96" s="116"/>
       <c r="E96" s="116"/>
       <c r="F96" s="116"/>
       <c r="G96" s="116"/>
       <c r="H96" s="116" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I96" s="116"/>
       <c r="J96" s="116"/>
       <c r="K96" s="116"/>
       <c r="L96" s="116"/>
       <c r="M96" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N96" s="115"/>
       <c r="O96" s="65"/>
@@ -7627,24 +7627,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C97" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D97" s="116"/>
       <c r="E97" s="116"/>
       <c r="F97" s="116"/>
       <c r="G97" s="116"/>
       <c r="H97" s="116" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I97" s="116"/>
       <c r="J97" s="116"/>
       <c r="K97" s="116"/>
       <c r="L97" s="116"/>
       <c r="M97" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N97" s="115"/>
       <c r="O97" s="65"/>
@@ -7654,24 +7654,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C98" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D98" s="116"/>
       <c r="E98" s="116"/>
       <c r="F98" s="116"/>
       <c r="G98" s="116"/>
       <c r="H98" s="116" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I98" s="116"/>
       <c r="J98" s="116"/>
       <c r="K98" s="116"/>
       <c r="L98" s="116"/>
       <c r="M98" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N98" s="115"/>
       <c r="O98" s="65"/>
@@ -7681,24 +7681,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="C99" s="116" t="s">
         <v>218</v>
-      </c>
-      <c r="C99" s="116" t="s">
-        <v>220</v>
       </c>
       <c r="D99" s="116"/>
       <c r="E99" s="116"/>
       <c r="F99" s="116"/>
       <c r="G99" s="116"/>
       <c r="H99" s="116" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I99" s="116"/>
       <c r="J99" s="116"/>
       <c r="K99" s="116"/>
       <c r="L99" s="116"/>
       <c r="M99" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N99" s="115"/>
       <c r="O99" s="65"/>
@@ -7708,24 +7708,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C100" s="116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D100" s="116"/>
       <c r="E100" s="116"/>
       <c r="F100" s="116"/>
       <c r="G100" s="116"/>
       <c r="H100" s="116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I100" s="116"/>
       <c r="J100" s="116"/>
       <c r="K100" s="116"/>
       <c r="L100" s="116"/>
       <c r="M100" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N100" s="115"/>
       <c r="O100" s="65"/>

</xml_diff>

<commit_message>
VSS sound range reduced significantly + mag size increased
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BBA59-F43E-47D1-BBCD-8FB448CAF4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF9790-5CFA-4C50-9A8C-2C639CFFB4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,10 +692,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VSS: travel distance is unusually far compared to 5mm using guns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ak47</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1449,6 +1445,10 @@
   </si>
   <si>
     <t>Drop a Fennek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VSS: surpressed sound / travel distance is unusually far compared to 5mm using guns</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3509,8 +3509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3526,14 +3526,14 @@
     <row r="1" spans="1:38" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="82"/>
       <c r="B1" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C1" s="125" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="125"/>
       <c r="G1" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>0</v>
@@ -3560,7 +3560,7 @@
     <row r="2" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="35"/>
       <c r="B2" s="77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" s="84" t="s">
         <v>7</v>
@@ -3590,7 +3590,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>16</v>
@@ -3632,18 +3632,18 @@
       </c>
       <c r="AA2" s="130"/>
       <c r="AG2" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH2" s="39"/>
       <c r="AI2" s="39"/>
       <c r="AL2" s="114" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="59"/>
       <c r="B3" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="40">
         <v>576</v>
@@ -3670,7 +3670,7 @@
         <v>1800</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L3" s="19">
         <v>6</v>
@@ -3721,10 +3721,10 @@
       </c>
       <c r="Y3" s="19"/>
       <c r="Z3" s="57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG3" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH3" s="53"/>
       <c r="AI3" s="53"/>
@@ -3738,7 +3738,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="42">
         <v>192</v>
@@ -3765,7 +3765,7 @@
         <v>1400</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L4" s="23"/>
       <c r="M4" s="19">
@@ -3793,7 +3793,7 @@
         <v>0.375</v>
       </c>
       <c r="S4" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T4" s="23"/>
       <c r="U4" s="19">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="Y4" s="23"/>
       <c r="Z4" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL4" s="36"/>
     </row>
@@ -3823,7 +3823,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="41">
         <v>832</v>
@@ -3850,7 +3850,7 @@
         <v>6000</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L5" s="23">
         <v>6</v>
@@ -3880,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T5" s="19"/>
       <c r="U5" s="19">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="Y5" s="19"/>
       <c r="Z5" s="57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AL5" s="36"/>
     </row>
@@ -3910,7 +3910,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="42">
         <v>192</v>
@@ -3937,7 +3937,7 @@
         <v>1400</v>
       </c>
       <c r="K6" s="74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L6" s="74"/>
       <c r="M6" s="19">
@@ -3965,7 +3965,7 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="S6" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T6" s="74"/>
       <c r="U6" s="19">
@@ -3986,7 +3986,7 @@
       </c>
       <c r="Y6" s="74"/>
       <c r="Z6" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL6" s="36"/>
     </row>
@@ -3995,10 +3995,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B7" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="55" t="s">
         <v>157</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>158</v>
       </c>
       <c r="D7" s="74">
         <v>0</v>
@@ -4022,7 +4022,7 @@
         <v>1000</v>
       </c>
       <c r="K7" s="75" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L7" s="74"/>
       <c r="M7" s="19"/>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T7" s="74"/>
       <c r="U7" s="19"/>
@@ -4047,7 +4047,7 @@
       <c r="X7" s="26"/>
       <c r="Y7" s="74"/>
       <c r="Z7" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL7" s="36"/>
     </row>
@@ -4634,7 +4634,7 @@
         <v>13.33</v>
       </c>
       <c r="N17" s="19">
-        <f t="shared" si="10"/>
+        <f>ROUND(E17*F17/(G17+J17/I17)*1000,2)</f>
         <v>8.0399999999999991</v>
       </c>
       <c r="O17" s="19">
@@ -4678,7 +4678,7 @@
         <v>37</v>
       </c>
       <c r="AG17" s="53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH17" s="53"/>
       <c r="AI17" s="53"/>
@@ -4713,7 +4713,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J18" s="19">
         <v>2300</v>
@@ -4728,11 +4728,11 @@
       </c>
       <c r="N18" s="19">
         <f t="shared" si="10"/>
-        <v>3.03</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="O18" s="19">
         <f>E18*F18*I18</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P18" s="33">
         <f>ROUND(playerHealth/(E18*F18),1)</f>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="Y18" s="19"/>
       <c r="Z18" s="57" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="AL18" s="112">
         <v>12</v>
@@ -4779,7 +4779,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="50">
         <v>704</v>
@@ -4864,7 +4864,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="48">
         <v>576</v>
@@ -4941,7 +4941,7 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="57"/>
       <c r="AG20" s="53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH20" s="53"/>
       <c r="AI20" s="53"/>
@@ -5013,7 +5013,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="51">
         <v>180</v>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="Y23" s="19"/>
       <c r="Z23" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AL23" s="112">
         <v>4</v>
@@ -5100,7 +5100,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="52">
         <v>320</v>
@@ -5185,7 +5185,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="52">
         <v>320</v>
@@ -5328,7 +5328,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="42">
         <v>700</v>
@@ -5355,7 +5355,7 @@
         <v>2800</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19">
@@ -5413,7 +5413,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="42">
         <v>600</v>
@@ -5440,7 +5440,7 @@
         <v>2600</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29" s="19"/>
       <c r="M29" s="19">
@@ -5498,7 +5498,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="42">
         <v>650</v>
@@ -5525,7 +5525,7 @@
         <v>2100</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19">
@@ -5610,7 +5610,7 @@
     <row r="32" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="35"/>
       <c r="B32" s="77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="19"/>
@@ -5643,7 +5643,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="42">
         <v>24</v>
@@ -5664,7 +5664,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J33" s="19">
         <v>0</v>
@@ -5703,7 +5703,7 @@
       <c r="X33" s="34"/>
       <c r="Y33" s="19"/>
       <c r="Z33" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AL33" s="36"/>
     </row>
@@ -5712,7 +5712,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="42">
         <v>32</v>
@@ -5733,7 +5733,7 @@
         <v>8</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J34" s="19">
         <v>0</v>
@@ -5782,7 +5782,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="42">
         <v>48</v>
@@ -5803,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J35" s="19">
         <v>0</v>
@@ -5918,10 +5918,10 @@
     <row r="40" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="35"/>
       <c r="B40" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C40" s="118" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" s="118"/>
       <c r="E40" s="118"/>
@@ -5929,7 +5929,7 @@
       <c r="G40" s="118"/>
       <c r="H40" s="118"/>
       <c r="I40" s="118" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J40" s="118"/>
       <c r="K40" s="118"/>
@@ -5939,7 +5939,7 @@
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
       <c r="S40" s="131" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T40" s="131"/>
       <c r="U40" s="57"/>
@@ -5949,20 +5949,20 @@
         <v>#VALUE!</v>
       </c>
       <c r="B41" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="119" t="s">
         <v>59</v>
-      </c>
-      <c r="C41" s="119" t="s">
-        <v>60</v>
       </c>
       <c r="D41" s="119"/>
       <c r="E41" s="119"/>
       <c r="F41" s="119" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" s="119"/>
       <c r="H41" s="119"/>
       <c r="I41" s="119" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J41" s="119"/>
       <c r="K41" s="119"/>
@@ -5972,7 +5972,7 @@
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
       <c r="S41" s="131" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T41" s="131"/>
       <c r="U41" s="57">
@@ -5985,20 +5985,20 @@
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="119" t="s">
         <v>63</v>
-      </c>
-      <c r="C42" s="119" t="s">
-        <v>64</v>
       </c>
       <c r="D42" s="119"/>
       <c r="E42" s="119"/>
       <c r="F42" s="119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G42" s="119"/>
       <c r="H42" s="119"/>
       <c r="I42" s="119" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J42" s="119"/>
       <c r="K42" s="119"/>
@@ -6008,7 +6008,7 @@
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
       <c r="S42" s="131" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T42" s="131"/>
       <c r="U42" s="57">
@@ -6018,23 +6018,23 @@
     </row>
     <row r="43" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>204</v>
-      </c>
       <c r="C43" s="120" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D43" s="120"/>
       <c r="E43" s="120"/>
       <c r="F43" s="120" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G43" s="120"/>
       <c r="H43" s="120"/>
       <c r="I43" s="120" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J43" s="120"/>
       <c r="K43" s="120"/>
@@ -6044,25 +6044,25 @@
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
       <c r="S43" s="131" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T43" s="131"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
       <c r="V43" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C44" s="120" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D44" s="120"/>
       <c r="E44" s="120"/>
@@ -6070,7 +6070,7 @@
       <c r="G44" s="120"/>
       <c r="H44" s="120"/>
       <c r="I44" s="120" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J44" s="120"/>
       <c r="K44" s="120"/>
@@ -6088,14 +6088,14 @@
     <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="35"/>
       <c r="B47" s="77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C47" s="118" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D47" s="118"/>
       <c r="E47" s="118" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F47" s="118"/>
       <c r="G47" s="118"/>
@@ -6108,14 +6108,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C48" s="119">
         <v>2</v>
       </c>
       <c r="D48" s="119"/>
       <c r="E48" s="119" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F48" s="119"/>
       <c r="G48" s="119"/>
@@ -6128,14 +6128,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D49" s="119"/>
       <c r="E49" s="119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F49" s="119"/>
       <c r="G49" s="119"/>
@@ -6159,18 +6159,18 @@
     <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A53" s="58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C54" s="63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H54" s="123" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I54" s="123"/>
       <c r="J54" s="123"/>
@@ -6181,7 +6181,7 @@
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
       <c r="B55" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C55" s="88">
         <v>-1</v>
@@ -6220,7 +6220,7 @@
     <row r="56" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A56" s="90"/>
       <c r="B56" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="19">
         <f t="shared" ref="C56:M56" si="15">(2+C55)*tilesize</f>
@@ -6270,7 +6270,7 @@
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
       <c r="B57" s="59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="51">
         <f t="shared" ref="C57:M57" si="16">(2+C55+1)*tilesize+tilesize/2</f>
@@ -6319,16 +6319,16 @@
     </row>
     <row r="58" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C58" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D58" s="60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
       <c r="H58" s="124" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I58" s="124"/>
       <c r="J58" s="124"/>
@@ -6339,19 +6339,19 @@
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P60" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q60" t="s">
         <v>110</v>
       </c>
-      <c r="P60" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q60" t="s">
+      <c r="R60" t="s">
         <v>111</v>
       </c>
-      <c r="R60" t="s">
-        <v>112</v>
-      </c>
       <c r="S60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG60" s="80"/>
       <c r="AH60" s="80"/>
@@ -6381,21 +6381,21 @@
     </row>
     <row r="62" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="I62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J62" s="127" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K62" s="127"/>
       <c r="L62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M62" s="96">
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
       <c r="O62" s="126" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P62" s="126"/>
       <c r="Q62" s="126"/>
@@ -6411,63 +6411,63 @@
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="85" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="86" t="s">
+      <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="E63" s="86" t="s">
+      <c r="F63" s="132" t="s">
         <v>92</v>
-      </c>
-      <c r="F63" s="132" t="s">
-        <v>93</v>
       </c>
       <c r="G63" s="132"/>
       <c r="H63" s="86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
       <c r="J63" s="132" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K63" s="132"/>
       <c r="L63" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="M63" s="86" t="s">
         <v>103</v>
-      </c>
-      <c r="M63" s="86" t="s">
-        <v>104</v>
       </c>
       <c r="N63" s="86"/>
       <c r="O63" s="105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P63" s="86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q63" s="86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R63" s="86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S63" s="106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T63" s="86"/>
       <c r="U63" s="132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V63" s="132"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
       <c r="X63" s="86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y63" s="57"/>
       <c r="Z63" s="57"/>
@@ -6479,7 +6479,7 @@
     <row r="64" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A64" s="38"/>
       <c r="B64" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="97">
         <v>24</v>
@@ -6491,7 +6491,7 @@
         <v>6</v>
       </c>
       <c r="F64" s="133" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G64" s="133"/>
       <c r="H64" s="97">
@@ -6544,7 +6544,7 @@
         <v>29</v>
       </c>
       <c r="X64" s="58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y64" s="57"/>
       <c r="Z64" s="57"/>
@@ -6556,7 +6556,7 @@
     <row r="65" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="54">
         <v>32</v>
@@ -6568,7 +6568,7 @@
         <v>4</v>
       </c>
       <c r="F65" s="115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G65" s="115"/>
       <c r="H65" s="54">
@@ -6621,7 +6621,7 @@
         <v>29</v>
       </c>
       <c r="X65" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Y65" s="57"/>
       <c r="Z65" s="57"/>
@@ -6633,7 +6633,7 @@
     <row r="66" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" s="54">
         <v>30</v>
@@ -6645,7 +6645,7 @@
         <v>3</v>
       </c>
       <c r="F66" s="115" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G66" s="115"/>
       <c r="H66" s="54">
@@ -6698,7 +6698,7 @@
         <v>29</v>
       </c>
       <c r="X66" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Y66" s="57"/>
       <c r="Z66" s="57"/>
@@ -6710,7 +6710,7 @@
     <row r="67" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A67" s="18"/>
       <c r="B67" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C67" s="54">
         <v>40</v>
@@ -6722,7 +6722,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="115" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G67" s="115"/>
       <c r="H67" s="54">
@@ -6775,7 +6775,7 @@
         <v>28</v>
       </c>
       <c r="X67" s="58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y67" s="57"/>
       <c r="Z67" s="57"/>
@@ -6783,7 +6783,7 @@
     <row r="68" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A68" s="18"/>
       <c r="B68" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="54">
         <v>52</v>
@@ -6848,7 +6848,7 @@
         <v>29</v>
       </c>
       <c r="X68" s="58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y68" s="57"/>
       <c r="Z68" s="57"/>
@@ -6856,7 +6856,7 @@
     <row r="69" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A69" s="18"/>
       <c r="B69" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C69" s="54">
         <v>26</v>
@@ -6868,7 +6868,7 @@
         <v>10</v>
       </c>
       <c r="F69" s="115" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G69" s="115"/>
       <c r="H69" s="54">
@@ -6921,7 +6921,7 @@
         <v>28</v>
       </c>
       <c r="X69" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y69" s="57"/>
       <c r="Z69" s="57"/>
@@ -6929,7 +6929,7 @@
     <row r="70" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A70" s="18"/>
       <c r="B70" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C70" s="54">
         <v>28</v>
@@ -6941,7 +6941,7 @@
         <v>8</v>
       </c>
       <c r="F70" s="115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G70" s="115"/>
       <c r="H70" s="54">
@@ -6991,10 +6991,10 @@
       </c>
       <c r="V70" s="136"/>
       <c r="W70" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X70" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y70" s="57"/>
       <c r="Z70" s="57"/>
@@ -7003,7 +7003,7 @@
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O73" s="130" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P73" s="130"/>
       <c r="Q73" s="130"/>
@@ -7012,40 +7012,40 @@
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
       <c r="B74" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C74" s="107" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D74" s="107" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E74" s="107" t="s">
+        <v>135</v>
+      </c>
+      <c r="F74" s="121" t="s">
         <v>136</v>
-      </c>
-      <c r="F74" s="121" t="s">
-        <v>137</v>
       </c>
       <c r="G74" s="121"/>
       <c r="H74" s="121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I74" s="121"/>
       <c r="J74" s="121" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K74" s="121"/>
       <c r="L74" s="121"/>
       <c r="M74" s="121"/>
       <c r="N74" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="O74" s="121" t="s">
         <v>168</v>
-      </c>
-      <c r="O74" s="121" t="s">
-        <v>169</v>
       </c>
       <c r="P74" s="121"/>
       <c r="Q74" s="121" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R74" s="121"/>
     </row>
@@ -7054,7 +7054,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C75" s="65">
         <v>2</v>
@@ -7066,7 +7066,7 @@
         <v>18</v>
       </c>
       <c r="F75" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G75" s="122"/>
       <c r="H75" s="122">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="I75" s="122"/>
       <c r="J75" s="122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K75" s="122"/>
       <c r="L75" s="122"/>
@@ -7097,7 +7097,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C76" s="65">
         <v>30</v>
@@ -7109,7 +7109,7 @@
         <v>12</v>
       </c>
       <c r="F76" s="122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G76" s="122"/>
       <c r="H76" s="122">
@@ -7118,7 +7118,7 @@
       </c>
       <c r="I76" s="122"/>
       <c r="J76" s="122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K76" s="122"/>
       <c r="L76" s="122"/>
@@ -7157,10 +7157,10 @@
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B78" s="112" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -7170,19 +7170,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="B81" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="C81" s="107" t="s">
+      <c r="D81" s="107" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="F81" s="121" t="s">
         <v>140</v>
-      </c>
-      <c r="D81" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="E81" s="107" t="s">
-        <v>146</v>
-      </c>
-      <c r="F81" s="121" t="s">
-        <v>141</v>
       </c>
       <c r="G81" s="121"/>
       <c r="H81" s="121"/>
@@ -7195,7 +7195,7 @@
       <c r="O81" s="121"/>
       <c r="P81" s="121"/>
       <c r="Q81" s="121" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R81" s="121"/>
       <c r="S81" s="121"/>
@@ -7211,10 +7211,10 @@
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
       <c r="B82" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C82" s="98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D82" s="36">
         <v>7</v>
@@ -7223,7 +7223,7 @@
         <v>16</v>
       </c>
       <c r="F82" s="134" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G82" s="134"/>
       <c r="H82" s="134"/>
@@ -7236,7 +7236,7 @@
       <c r="O82" s="134"/>
       <c r="P82" s="134"/>
       <c r="Q82" s="134" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R82" s="134"/>
       <c r="S82" s="134"/>
@@ -7252,19 +7252,19 @@
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
       <c r="B83" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C83" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D83" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E83" s="54">
         <v>1</v>
       </c>
       <c r="F83" s="117" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G83" s="117"/>
       <c r="H83" s="117"/>
@@ -7291,19 +7291,19 @@
     <row r="84" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A84" s="38"/>
       <c r="B84" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C84" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D84" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E84" s="54">
         <v>1</v>
       </c>
       <c r="F84" s="117" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G84" s="117"/>
       <c r="H84" s="117"/>
@@ -7330,10 +7330,10 @@
     <row r="85" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A85" s="38"/>
       <c r="B85" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C85" s="65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D85" s="54">
         <v>6</v>
@@ -7342,7 +7342,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="117" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G85" s="117"/>
       <c r="H85" s="117"/>
@@ -7355,7 +7355,7 @@
       <c r="O85" s="117"/>
       <c r="P85" s="117"/>
       <c r="Q85" s="117" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R85" s="117"/>
       <c r="S85" s="117"/>
@@ -7370,10 +7370,10 @@
     </row>
     <row r="86" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
@@ -7435,29 +7435,29 @@
     <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="35"/>
       <c r="B90" s="77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C90" s="129" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D90" s="129"/>
       <c r="E90" s="129"/>
       <c r="F90" s="129"/>
       <c r="G90" s="129"/>
       <c r="H90" s="129" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I90" s="129"/>
       <c r="J90" s="129"/>
       <c r="K90" s="129"/>
       <c r="L90" s="129"/>
       <c r="M90" s="121" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N90" s="121"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7465,24 +7465,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C91" s="116" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="116"/>
       <c r="F91" s="116"/>
       <c r="G91" s="116"/>
       <c r="H91" s="116" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I91" s="116"/>
       <c r="J91" s="116"/>
       <c r="K91" s="116"/>
       <c r="L91" s="116"/>
       <c r="M91" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N91" s="115"/>
       <c r="O91" s="65"/>
@@ -7492,24 +7492,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C92" s="116" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D92" s="116"/>
       <c r="E92" s="116"/>
       <c r="F92" s="116"/>
       <c r="G92" s="116"/>
       <c r="H92" s="116" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I92" s="116"/>
       <c r="J92" s="116"/>
       <c r="K92" s="116"/>
       <c r="L92" s="116"/>
       <c r="M92" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N92" s="115"/>
       <c r="O92" s="65"/>
@@ -7519,24 +7519,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C93" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D93" s="116"/>
       <c r="E93" s="116"/>
       <c r="F93" s="116"/>
       <c r="G93" s="116"/>
       <c r="H93" s="116" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I93" s="116"/>
       <c r="J93" s="116"/>
       <c r="K93" s="116"/>
       <c r="L93" s="116"/>
       <c r="M93" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N93" s="115"/>
       <c r="O93" s="65"/>
@@ -7546,24 +7546,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C94" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="116"/>
       <c r="F94" s="116"/>
       <c r="G94" s="116"/>
       <c r="H94" s="116" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I94" s="116"/>
       <c r="J94" s="116"/>
       <c r="K94" s="116"/>
       <c r="L94" s="116"/>
       <c r="M94" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N94" s="115"/>
       <c r="O94" s="65"/>
@@ -7573,24 +7573,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C95" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D95" s="116"/>
       <c r="E95" s="116"/>
       <c r="F95" s="116"/>
       <c r="G95" s="116"/>
       <c r="H95" s="116" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I95" s="116"/>
       <c r="J95" s="116"/>
       <c r="K95" s="116"/>
       <c r="L95" s="116"/>
       <c r="M95" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N95" s="115"/>
       <c r="O95" s="65"/>
@@ -7600,24 +7600,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C96" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D96" s="116"/>
       <c r="E96" s="116"/>
       <c r="F96" s="116"/>
       <c r="G96" s="116"/>
       <c r="H96" s="116" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I96" s="116"/>
       <c r="J96" s="116"/>
       <c r="K96" s="116"/>
       <c r="L96" s="116"/>
       <c r="M96" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N96" s="115"/>
       <c r="O96" s="65"/>
@@ -7627,24 +7627,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C97" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D97" s="116"/>
       <c r="E97" s="116"/>
       <c r="F97" s="116"/>
       <c r="G97" s="116"/>
       <c r="H97" s="116" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I97" s="116"/>
       <c r="J97" s="116"/>
       <c r="K97" s="116"/>
       <c r="L97" s="116"/>
       <c r="M97" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N97" s="115"/>
       <c r="O97" s="65"/>
@@ -7654,24 +7654,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C98" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D98" s="116"/>
       <c r="E98" s="116"/>
       <c r="F98" s="116"/>
       <c r="G98" s="116"/>
       <c r="H98" s="116" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I98" s="116"/>
       <c r="J98" s="116"/>
       <c r="K98" s="116"/>
       <c r="L98" s="116"/>
       <c r="M98" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N98" s="115"/>
       <c r="O98" s="65"/>
@@ -7681,24 +7681,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C99" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D99" s="116"/>
       <c r="E99" s="116"/>
       <c r="F99" s="116"/>
       <c r="G99" s="116"/>
       <c r="H99" s="116" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I99" s="116"/>
       <c r="J99" s="116"/>
       <c r="K99" s="116"/>
       <c r="L99" s="116"/>
       <c r="M99" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N99" s="115"/>
       <c r="O99" s="65"/>
@@ -7708,24 +7708,24 @@
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" s="116" t="s">
         <v>217</v>
-      </c>
-      <c r="C100" s="116" t="s">
-        <v>218</v>
       </c>
       <c r="D100" s="116"/>
       <c r="E100" s="116"/>
       <c r="F100" s="116"/>
       <c r="G100" s="116"/>
       <c r="H100" s="116" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I100" s="116"/>
       <c r="J100" s="116"/>
       <c r="K100" s="116"/>
       <c r="L100" s="116"/>
       <c r="M100" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N100" s="115"/>
       <c r="O100" s="65"/>

</xml_diff>

<commit_message>
- Added Deagle - VSS sound range decreased - USAS12 explosive ammo
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF9790-5CFA-4C50-9A8C-2C639CFFB4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992C65B-7328-4014-84D4-78ED056906C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="frag_damage">Sheet1!$F$4</definedName>
     <definedName name="fragHitNum">Sheet1!$L$3</definedName>
     <definedName name="fraghitnum2">Sheet1!$L$5</definedName>
+    <definedName name="gun_bullet_explosion_damage">Sheet1!$F$35</definedName>
     <definedName name="guns_cap">Sheet1!$P$61</definedName>
     <definedName name="health_cap">Sheet1!$O$61</definedName>
     <definedName name="player_radius">Sheet1!$U$43</definedName>
@@ -53,7 +54,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="46">
+  <futureMetadata name="XLRICHVALUE" count="47">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -376,8 +377,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="46"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="46">
+  <valueMetadata count="47">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -515,13 +523,16 @@
     </bk>
     <bk>
       <rc t="1" v="45"/>
+    </bk>
+    <bk>
+      <rc t="1" v="46"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="233">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1449,6 +1460,22 @@
   </si>
   <si>
     <t>VSS: surpressed sound / travel distance is unusually far compared to 5mm using guns</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deagle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Better version of pistol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slow bullet speed, low range, low fireRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPLOSIVE AMMO : 3~5 fragments (average of 4 frags, but statistically 3 hits most frequent) / each frag deals 1 damage (same as a bat)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2011,7 +2038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2334,6 +2361,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2996,7 +3026,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="46">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="47">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -3181,6 +3211,10 @@
     <v>45</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>46</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -3241,6 +3275,7 @@
   <rel r:id="rId44"/>
   <rel r:id="rId45"/>
   <rel r:id="rId46"/>
+  <rel r:id="rId47"/>
 </richValueRels>
 </file>
 
@@ -3509,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3528,10 +3563,10 @@
       <c r="B1" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="125" t="s">
+      <c r="C1" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="125"/>
+      <c r="D1" s="126"/>
       <c r="G1" s="56" t="s">
         <v>159</v>
       </c>
@@ -3627,10 +3662,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="130" t="s">
+      <c r="Z2" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="130"/>
+      <c r="AA2" s="131"/>
       <c r="AG2" s="43" t="s">
         <v>84</v>
       </c>
@@ -4507,7 +4542,6 @@
       <c r="X15" s="74"/>
       <c r="Y15" s="74"/>
       <c r="Z15" s="57"/>
-      <c r="AL15" s="36"/>
     </row>
     <row r="16" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="18" t="e" vm="9">
@@ -4568,8 +4602,8 @@
         <f>ROUND(D16/H16,3)</f>
         <v>0.13300000000000001</v>
       </c>
-      <c r="S16" s="28" t="s">
-        <v>29</v>
+      <c r="S16" s="25" t="s">
+        <v>74</v>
       </c>
       <c r="T16" s="19"/>
       <c r="U16" s="19">
@@ -4589,9 +4623,8 @@
         <v>13.33</v>
       </c>
       <c r="Y16" s="19"/>
-      <c r="Z16" s="57"/>
-      <c r="AL16" s="113">
-        <v>16</v>
+      <c r="Z16" s="57" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -4746,8 +4779,8 @@
         <f>ROUND(D18/H18,3)</f>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="S18" s="21" t="s">
-        <v>28</v>
+      <c r="S18" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="T18" s="19"/>
       <c r="U18" s="19">
@@ -4951,33 +4984,91 @@
       </c>
     </row>
     <row r="21" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="A21" s="18" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" s="48">
+        <v>576</v>
+      </c>
+      <c r="D21" s="19">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+      <c r="F21" s="19">
+        <v>3</v>
+      </c>
+      <c r="G21" s="19">
+        <v>450</v>
+      </c>
+      <c r="H21" s="19">
+        <v>18</v>
+      </c>
+      <c r="I21" s="19">
+        <v>7</v>
+      </c>
+      <c r="J21" s="19">
+        <v>2300</v>
+      </c>
+      <c r="K21" s="19">
+        <v>7</v>
+      </c>
       <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="32"/>
+      <c r="M21" s="19">
+        <f>ROUND(E21*F21/G21*1000,2)</f>
+        <v>6.67</v>
+      </c>
+      <c r="N21" s="19">
+        <f t="shared" ref="N21" si="12">ROUND(E21*F21/(G21+J21/I21)*1000,2)</f>
+        <v>3.85</v>
+      </c>
+      <c r="O21" s="19">
+        <f>E21*F21*I21</f>
+        <v>21</v>
+      </c>
+      <c r="P21" s="20">
+        <f>ROUND(playerHealth/(E21*F21),1)</f>
+        <v>2.7</v>
+      </c>
+      <c r="Q21" s="19">
+        <f>-(FLOOR(H21/6,1)-1)</f>
+        <v>-2</v>
+      </c>
+      <c r="R21" s="19">
+        <f>ROUND(D21/H21,3)</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="S21" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="20"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="20"/>
+      <c r="U21" s="19">
+        <f xml:space="preserve"> E21*F21*9/10</f>
+        <v>2.7</v>
+      </c>
+      <c r="V21" s="29">
+        <f>ROUND(playerHealth/(U21),2)</f>
+        <v>2.96</v>
+      </c>
+      <c r="W21" s="19">
+        <f>E21*(F21-0.4)</f>
+        <v>2.6</v>
+      </c>
+      <c r="X21" s="115">
+        <f>ROUND(playerHealth/(W21),2)</f>
+        <v>3.08</v>
+      </c>
       <c r="Y21" s="19"/>
-      <c r="Z21" s="57"/>
-      <c r="AL21" s="36"/>
+      <c r="Z21" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL21" s="113">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="18"/>
@@ -5009,7 +5100,7 @@
       <c r="AL22" s="36"/>
     </row>
     <row r="23" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="18" t="e" vm="14">
+      <c r="A23" s="18" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -5037,7 +5128,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="19">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="K23" s="19">
         <v>12</v>
@@ -5049,7 +5140,7 @@
       </c>
       <c r="N23" s="19">
         <f t="shared" si="10"/>
-        <v>6.41</v>
+        <v>6.02</v>
       </c>
       <c r="O23" s="19">
         <f>E23*F23*I23</f>
@@ -5096,7 +5187,7 @@
       </c>
     </row>
     <row r="24" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="18" t="e" vm="15">
+      <c r="A24" s="18" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -5181,26 +5272,26 @@
       </c>
     </row>
     <row r="25" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="18" t="e" vm="16">
+      <c r="A25" s="18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="52">
-        <v>320</v>
+      <c r="C25" s="51">
+        <v>256</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
       </c>
       <c r="E25" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="19">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="H25" s="19">
         <v>14</v>
@@ -5209,34 +5300,36 @@
         <v>5</v>
       </c>
       <c r="J25" s="19">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="K25" s="19">
         <v>12</v>
       </c>
-      <c r="L25" s="19"/>
+      <c r="L25" s="19">
+        <v>4</v>
+      </c>
       <c r="M25" s="19">
-        <f>ROUND(E25*F25/G25*1000,2)</f>
-        <v>11.11</v>
+        <f>ROUND(E25*(F25+L25*gun_bullet_explosion_damage)/G25*1000,2)</f>
+        <v>20</v>
       </c>
       <c r="N25" s="19">
-        <f t="shared" si="10"/>
-        <v>3.13</v>
+        <f>ROUND(E25*(F25+L25*gun_bullet_explosion_damage)/(G25+J25/I25)*1000,2)</f>
+        <v>5.71</v>
       </c>
       <c r="O25" s="19">
-        <f>E25*F25*I25</f>
-        <v>10</v>
-      </c>
-      <c r="P25" s="33">
-        <f>ROUND(playerHealth/(E25*F25),1)</f>
-        <v>4</v>
+        <f>E25*(F25+L25*gun_bullet_explosion_damage)*I25</f>
+        <v>20</v>
+      </c>
+      <c r="P25" s="20">
+        <f>ROUND(playerHealth/(E25*(F25+L25*gun_bullet_explosion_damage)),1)</f>
+        <v>2</v>
       </c>
       <c r="Q25" s="19">
-        <f>-(FLOOR(H25/6,1)-1)</f>
+        <f t="shared" ref="Q25" si="13">-(FLOOR(H25/6,1)-1)</f>
         <v>-1</v>
       </c>
       <c r="R25" s="19">
-        <f>ROUND(D25/H25,3)</f>
+        <f t="shared" ref="R25" si="14">ROUND(D25/H25,3)</f>
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="S25" s="28" t="s">
@@ -5244,23 +5337,25 @@
       </c>
       <c r="T25" s="19"/>
       <c r="U25" s="19">
-        <f xml:space="preserve"> E25*F25*9/10</f>
-        <v>1.8</v>
-      </c>
-      <c r="V25" s="34">
+        <f xml:space="preserve"> E25*(F25+L25*gun_bullet_explosion_damage)*9/10</f>
+        <v>3.6</v>
+      </c>
+      <c r="V25" s="29">
         <f>ROUND(playerHealth/(U25),2)</f>
-        <v>4.4400000000000004</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="W25" s="19">
-        <f>E25*(F25-0.4)</f>
-        <v>1.2</v>
-      </c>
-      <c r="X25" s="34">
+        <f>E25*((F25+L25*gun_bullet_explosion_damage)-0.4)</f>
+        <v>3.6</v>
+      </c>
+      <c r="X25" s="29">
         <f>ROUND(playerHealth/(W25),2)</f>
-        <v>6.67</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="Y25" s="19"/>
-      <c r="Z25" s="57"/>
+      <c r="Z25" s="57" t="s">
+        <v>232</v>
+      </c>
       <c r="AL25" s="112">
         <v>8</v>
       </c>
@@ -5324,7 +5419,7 @@
       <c r="AL27" s="36"/>
     </row>
     <row r="28" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="18" t="e" vm="17">
+      <c r="A28" s="18" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -5409,7 +5504,7 @@
       </c>
     </row>
     <row r="29" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="18" t="e" vm="18">
+      <c r="A29" s="18" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -5494,7 +5589,7 @@
       </c>
     </row>
     <row r="30" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="18" t="e" vm="19">
+      <c r="A30" s="18" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -5639,7 +5734,7 @@
       <c r="AL32" s="36"/>
     </row>
     <row r="33" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A33" s="18" t="e" vm="20">
+      <c r="A33" s="18" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -5689,7 +5784,7 @@
       <c r="S33" s="32"/>
       <c r="T33" s="19"/>
       <c r="U33" s="19">
-        <f t="shared" ref="U33:U35" si="12" xml:space="preserve"> E33*F33*9/10</f>
+        <f t="shared" ref="U33:U35" si="15" xml:space="preserve"> E33*F33*9/10</f>
         <v>0.18</v>
       </c>
       <c r="V33" s="34">
@@ -5697,7 +5792,7 @@
         <v>44.44</v>
       </c>
       <c r="W33" s="19">
-        <f t="shared" ref="W33:W34" si="13">E33*(F33-0.2)</f>
+        <f t="shared" ref="W33:W34" si="16">E33*(F33-0.2)</f>
         <v>0</v>
       </c>
       <c r="X33" s="34"/>
@@ -5708,7 +5803,7 @@
       <c r="AL33" s="36"/>
     </row>
     <row r="34" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="18" t="e" vm="21">
+      <c r="A34" s="18" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
       <c r="B34" s="18" t="s">
@@ -5758,7 +5853,7 @@
       <c r="S34" s="32"/>
       <c r="T34" s="19"/>
       <c r="U34" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.36</v>
       </c>
       <c r="V34" s="34">
@@ -5766,7 +5861,7 @@
         <v>22.22</v>
       </c>
       <c r="W34" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.2</v>
       </c>
       <c r="X34" s="34">
@@ -5778,7 +5873,7 @@
       <c r="AL34" s="36"/>
     </row>
     <row r="35" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="18" t="e" vm="22">
+      <c r="A35" s="18" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="B35" s="18" t="s">
@@ -5811,7 +5906,7 @@
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
       <c r="M35" s="19">
-        <f t="shared" ref="M35" si="14">ROUND(E35*F35/G35*1000,3)</f>
+        <f t="shared" ref="M35" si="17">ROUND(E35*F35/G35*1000,3)</f>
         <v>2</v>
       </c>
       <c r="N35" s="19">
@@ -5828,7 +5923,7 @@
       <c r="S35" s="32"/>
       <c r="T35" s="19"/>
       <c r="U35" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.9</v>
       </c>
       <c r="V35" s="33">
@@ -5920,97 +6015,97 @@
       <c r="B40" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="118" t="s">
+      <c r="C40" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118" t="s">
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="118"/>
-      <c r="K40" s="118"/>
-      <c r="L40" s="118"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="131" t="s">
+      <c r="S40" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="131"/>
+      <c r="T40" s="132"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A41" s="38" t="e" vm="23">
+      <c r="A41" s="38" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="119" t="s">
+      <c r="C41" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="119"/>
-      <c r="E41" s="119"/>
-      <c r="F41" s="119" t="s">
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="119"/>
-      <c r="H41" s="119"/>
-      <c r="I41" s="119" t="s">
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="119"/>
-      <c r="K41" s="119"/>
-      <c r="L41" s="119"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="131" t="s">
+      <c r="S41" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="131"/>
+      <c r="T41" s="132"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
       <c r="V41" s="57"/>
     </row>
     <row r="42" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="38" t="e" vm="24">
+      <c r="A42" s="38" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="119" t="s">
+      <c r="C42" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="119"/>
-      <c r="E42" s="119"/>
-      <c r="F42" s="119" t="s">
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="119"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="119" t="s">
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="119"/>
-      <c r="K42" s="119"/>
-      <c r="L42" s="119"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="131" t="s">
+      <c r="S42" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="131"/>
+      <c r="T42" s="132"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6023,30 +6118,30 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="120" t="s">
+      <c r="C43" s="121" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="120" t="s">
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="120" t="s">
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="I43" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="120"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="121"/>
+      <c r="L43" s="121"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="131" t="s">
+      <c r="S43" s="132" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="131"/>
+      <c r="T43" s="132"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6061,20 +6156,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="120" t="s">
+      <c r="C44" s="121" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="120" t="s">
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="121" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="120"/>
-      <c r="K44" s="120"/>
-      <c r="L44" s="120"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="121"/>
+      <c r="L44" s="121"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6090,68 +6185,68 @@
       <c r="B47" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="118" t="s">
+      <c r="C47" s="119" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118" t="s">
+      <c r="D47" s="119"/>
+      <c r="E47" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
+      <c r="F47" s="119"/>
+      <c r="G47" s="119"/>
+      <c r="H47" s="119"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
     <row r="48" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="38" t="e" vm="25">
+      <c r="A48" s="38" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="119">
+      <c r="C48" s="120">
         <v>2</v>
       </c>
-      <c r="D48" s="119"/>
-      <c r="E48" s="119" t="s">
+      <c r="D48" s="120"/>
+      <c r="E48" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="119"/>
-      <c r="G48" s="119"/>
-      <c r="H48" s="119"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="38" t="e" vm="26">
+      <c r="A49" s="38" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="119" t="s">
+      <c r="C49" s="120" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="119"/>
-      <c r="E49" s="119" t="s">
+      <c r="D49" s="120"/>
+      <c r="E49" s="120" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="119"/>
-      <c r="G49" s="119"/>
-      <c r="H49" s="119"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="120"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="120"/>
-      <c r="F50" s="120"/>
-      <c r="G50" s="120"/>
-      <c r="H50" s="120"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="121"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6169,14 +6264,14 @@
       <c r="D54" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="123" t="s">
+      <c r="H54" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="123"/>
-      <c r="J54" s="123"/>
-      <c r="K54" s="123"/>
-      <c r="L54" s="123"/>
-      <c r="M54" s="123"/>
+      <c r="I54" s="124"/>
+      <c r="J54" s="124"/>
+      <c r="K54" s="124"/>
+      <c r="L54" s="124"/>
+      <c r="M54" s="124"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6223,47 +6318,47 @@
         <v>69</v>
       </c>
       <c r="C56" s="19">
-        <f t="shared" ref="C56:M56" si="15">(2+C55)*tilesize</f>
+        <f t="shared" ref="C56:M56" si="18">(2+C55)*tilesize</f>
         <v>128</v>
       </c>
       <c r="D56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>256</v>
       </c>
       <c r="E56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>384</v>
       </c>
       <c r="F56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>512</v>
       </c>
       <c r="G56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>640</v>
       </c>
       <c r="H56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>768</v>
       </c>
       <c r="I56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>896</v>
       </c>
       <c r="J56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1024</v>
       </c>
       <c r="K56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1152</v>
       </c>
       <c r="L56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1280</v>
       </c>
       <c r="M56" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1408</v>
       </c>
     </row>
@@ -6273,47 +6368,47 @@
         <v>70</v>
       </c>
       <c r="C57" s="51">
-        <f t="shared" ref="C57:M57" si="16">(2+C55+1)*tilesize+tilesize/2</f>
+        <f t="shared" ref="C57:M57" si="19">(2+C55+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
       <c r="D57" s="52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>448</v>
       </c>
       <c r="E57" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>576</v>
       </c>
       <c r="F57" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>704</v>
       </c>
       <c r="G57" s="49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>832</v>
       </c>
       <c r="H57" s="92">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>960</v>
       </c>
       <c r="I57" s="46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1088</v>
       </c>
       <c r="J57" s="47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1216</v>
       </c>
       <c r="K57" s="93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1344</v>
       </c>
       <c r="L57" s="45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1472</v>
       </c>
       <c r="M57" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1600</v>
       </c>
     </row>
@@ -6327,14 +6422,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="124" t="s">
+      <c r="H58" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="124"/>
-      <c r="J58" s="124"/>
-      <c r="K58" s="124"/>
-      <c r="L58" s="124"/>
-      <c r="M58" s="124"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="125"/>
+      <c r="L58" s="125"/>
+      <c r="M58" s="125"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6383,31 +6478,31 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="127" t="s">
+      <c r="J62" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="127"/>
+      <c r="K62" s="128"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
       <c r="M62" s="96">
         <f>COUNTIF(H3:H35,"&gt;0")</f>
-        <v>23</v>
-      </c>
-      <c r="O62" s="126" t="s">
+        <v>24</v>
+      </c>
+      <c r="O62" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="126"/>
-      <c r="Q62" s="126"/>
-      <c r="R62" s="126"/>
-      <c r="S62" s="126"/>
+      <c r="P62" s="127"/>
+      <c r="Q62" s="127"/>
+      <c r="R62" s="127"/>
+      <c r="S62" s="127"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
       <c r="AJ62" s="81"/>
     </row>
     <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="91" t="e" vm="27">
+      <c r="A63" s="91" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="85" t="s">
@@ -6422,20 +6517,20 @@
       <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="132" t="s">
+      <c r="F63" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="132"/>
+      <c r="G63" s="133"/>
       <c r="H63" s="86" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="132" t="s">
+      <c r="J63" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="132"/>
+      <c r="K63" s="133"/>
       <c r="L63" s="86" t="s">
         <v>102</v>
       </c>
@@ -6459,10 +6554,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="132" t="s">
+      <c r="U63" s="133" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="132"/>
+      <c r="V63" s="133"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6490,56 +6585,56 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="133" t="s">
+      <c r="F64" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="133"/>
+      <c r="G64" s="134"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="122">
-        <f t="shared" ref="J64:J69" si="17">(C64-player_radius)*2</f>
+      <c r="J64" s="123">
+        <f t="shared" ref="J64:J69" si="20">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="122"/>
+      <c r="K64" s="123"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M64" s="97">
         <f>21-L64</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N64" s="97"/>
       <c r="O64" s="99">
-        <f t="shared" ref="O64:O70" si="18">ROUND(D64/health_cap,2)*10</f>
+        <f t="shared" ref="O64:O70" si="21">ROUND(D64/health_cap,2)*10</f>
         <v>0.8</v>
       </c>
       <c r="P64" s="100">
-        <f t="shared" ref="P64:P70" si="19">ROUND(M64/guns_cap,2)*10</f>
-        <v>3.3000000000000003</v>
+        <f t="shared" ref="P64:P70" si="22">ROUND(M64/guns_cap,2)*10</f>
+        <v>3</v>
       </c>
       <c r="Q64" s="101">
-        <f t="shared" ref="Q64:Q70" si="20">ROUND(E64/speed_cap,2)*10</f>
+        <f t="shared" ref="Q64:Q70" si="23">ROUND(E64/speed_cap,2)*10</f>
         <v>6</v>
       </c>
       <c r="R64" s="102">
-        <f t="shared" ref="R64:R70" si="21">ROUND(I64/DPS_cap,2)*10</f>
+        <f t="shared" ref="R64:R70" si="24">ROUND(I64/DPS_cap,2)*10</f>
         <v>0</v>
       </c>
       <c r="S64" s="103">
         <f>SUM(O64:R64)</f>
-        <v>10.100000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="135">
+      <c r="U64" s="136">
         <f>R64+O64+P64</f>
-        <v>4.1000000000000005</v>
-      </c>
-      <c r="V64" s="135"/>
+        <v>3.8</v>
+      </c>
+      <c r="V64" s="136"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6567,56 +6662,56 @@
       <c r="E65" s="54">
         <v>4</v>
       </c>
-      <c r="F65" s="115" t="s">
+      <c r="F65" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="115"/>
+      <c r="G65" s="116"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="122">
-        <f t="shared" si="17"/>
+      <c r="J65" s="123">
+        <f t="shared" si="20"/>
         <v>32</v>
       </c>
-      <c r="K65" s="122"/>
+      <c r="K65" s="123"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
       </c>
       <c r="M65" s="54">
-        <f t="shared" ref="M65:M68" si="22">21-L65</f>
+        <f t="shared" ref="M65:M68" si="25">21-L65</f>
         <v>19</v>
       </c>
       <c r="N65" s="54"/>
       <c r="O65" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="P65" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>6.3</v>
       </c>
       <c r="Q65" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="R65" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S65" s="70">
-        <f t="shared" ref="S65:S69" si="23">SUM(O65:R65)</f>
+        <f t="shared" ref="S65:S69" si="26">SUM(O65:R65)</f>
         <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="136">
-        <f t="shared" ref="U65:U70" si="24">R65+O65+P65</f>
+      <c r="U65" s="137">
+        <f t="shared" ref="U65:U70" si="27">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="136"/>
+      <c r="V65" s="137"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6644,56 +6739,56 @@
       <c r="E66" s="54">
         <v>3</v>
       </c>
-      <c r="F66" s="115" t="s">
+      <c r="F66" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="115"/>
+      <c r="G66" s="116"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="122">
-        <f t="shared" si="17"/>
+      <c r="J66" s="123">
+        <f t="shared" si="20"/>
         <v>28</v>
       </c>
-      <c r="K66" s="122"/>
+      <c r="K66" s="123"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
       </c>
       <c r="M66" s="54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
       <c r="N66" s="54"/>
       <c r="O66" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2.5</v>
       </c>
       <c r="P66" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="Q66" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="R66" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="S66" s="70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="136">
-        <f t="shared" si="24"/>
+      <c r="U66" s="137">
+        <f t="shared" si="27"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="136"/>
+      <c r="V66" s="137"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6721,56 +6816,56 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="115" t="s">
+      <c r="F67" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="115"/>
+      <c r="G67" s="116"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="122">
-        <f t="shared" si="17"/>
+      <c r="J67" s="123">
+        <f t="shared" si="20"/>
         <v>48</v>
       </c>
-      <c r="K67" s="122"/>
+      <c r="K67" s="123"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
       </c>
       <c r="M67" s="54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>21</v>
       </c>
       <c r="N67" s="54"/>
       <c r="O67" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.6</v>
       </c>
       <c r="P67" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="Q67" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="R67" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="S67" s="70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="136">
-        <f t="shared" si="24"/>
+      <c r="U67" s="137">
+        <f t="shared" si="27"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="136"/>
+      <c r="V67" s="137"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6794,56 +6889,56 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="115" t="s">
+      <c r="F68" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="115"/>
+      <c r="G68" s="116"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="122">
-        <f t="shared" si="17"/>
+      <c r="J68" s="123">
+        <f t="shared" si="20"/>
         <v>72</v>
       </c>
-      <c r="K68" s="122"/>
+      <c r="K68" s="123"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
       </c>
       <c r="M68" s="54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>21</v>
       </c>
       <c r="N68" s="54"/>
       <c r="O68" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.4</v>
       </c>
       <c r="P68" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="Q68" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R68" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2.7</v>
       </c>
       <c r="S68" s="70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="136">
-        <f t="shared" si="24"/>
+      <c r="U68" s="137">
+        <f t="shared" si="27"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="136"/>
+      <c r="V68" s="137"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6867,21 +6962,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="115" t="s">
+      <c r="F69" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="115"/>
+      <c r="G69" s="116"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="122">
-        <f t="shared" si="17"/>
+      <c r="J69" s="123">
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
-      <c r="K69" s="122"/>
+      <c r="K69" s="123"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6892,31 +6987,31 @@
       </c>
       <c r="N69" s="54"/>
       <c r="O69" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="P69" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="Q69" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
       <c r="R69" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="S69" s="70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="136">
-        <f t="shared" si="24"/>
+      <c r="U69" s="137">
+        <f t="shared" si="27"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="136"/>
+      <c r="V69" s="137"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6940,21 +7035,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="115" t="s">
+      <c r="F70" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="115"/>
+      <c r="G70" s="116"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="122">
-        <f t="shared" ref="J70" si="25">(C70-player_radius)*2</f>
+      <c r="J70" s="123">
+        <f t="shared" ref="J70" si="28">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="122"/>
+      <c r="K70" s="123"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -6965,31 +7060,31 @@
       </c>
       <c r="N70" s="54"/>
       <c r="O70" s="66">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2.5</v>
       </c>
       <c r="P70" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="Q70" s="68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="R70" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>9.6</v>
       </c>
       <c r="S70" s="70">
-        <f t="shared" ref="S70" si="26">SUM(O70:R70)</f>
+        <f t="shared" ref="S70" si="29">SUM(O70:R70)</f>
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="136">
-        <f t="shared" si="24"/>
+      <c r="U70" s="137">
+        <f t="shared" si="27"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="136"/>
+      <c r="V70" s="137"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7002,12 +7097,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="130" t="s">
+      <c r="O73" s="131" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="130"/>
-      <c r="Q73" s="130"/>
-      <c r="R73" s="130"/>
+      <c r="P73" s="131"/>
+      <c r="Q73" s="131"/>
+      <c r="R73" s="131"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7023,34 +7118,34 @@
       <c r="E74" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="121" t="s">
+      <c r="F74" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="121"/>
-      <c r="H74" s="121" t="s">
+      <c r="G74" s="122"/>
+      <c r="H74" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="121"/>
-      <c r="J74" s="121" t="s">
+      <c r="I74" s="122"/>
+      <c r="J74" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="121"/>
-      <c r="L74" s="121"/>
-      <c r="M74" s="121"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="122"/>
+      <c r="M74" s="122"/>
       <c r="N74" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="121" t="s">
+      <c r="O74" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="121"/>
-      <c r="Q74" s="121" t="s">
+      <c r="P74" s="122"/>
+      <c r="Q74" s="122" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="121"/>
+      <c r="R74" s="122"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A75" s="38" t="e" vm="28">
+      <c r="A75" s="38" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
       <c r="B75" s="38" t="s">
@@ -7065,35 +7160,35 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="122" t="s">
+      <c r="F75" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122">
+      <c r="G75" s="123"/>
+      <c r="H75" s="123">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="122"/>
-      <c r="J75" s="122" t="s">
+      <c r="I75" s="123"/>
+      <c r="J75" s="123" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="122"/>
-      <c r="L75" s="122"/>
-      <c r="M75" s="122"/>
-      <c r="N75" s="78" t="e" vm="29">
+      <c r="K75" s="123"/>
+      <c r="L75" s="123"/>
+      <c r="M75" s="123"/>
+      <c r="N75" s="78" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
-      <c r="O75" s="70" t="e" vm="30">
+      <c r="O75" s="70" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
-      <c r="P75" s="70" t="e" vm="31">
+      <c r="P75" s="70" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
       <c r="Q75" s="79"/>
       <c r="R75" s="95"/>
     </row>
     <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A76" s="38" t="e" vm="32">
+      <c r="A76" s="38" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="38" t="s">
@@ -7108,28 +7203,28 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="122" t="s">
+      <c r="F76" s="123" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="122"/>
-      <c r="H76" s="122">
+      <c r="G76" s="123"/>
+      <c r="H76" s="123">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="122"/>
-      <c r="J76" s="122" t="s">
+      <c r="I76" s="123"/>
+      <c r="J76" s="123" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="122"/>
-      <c r="L76" s="122"/>
-      <c r="M76" s="122"/>
-      <c r="N76" s="78" t="e" vm="33">
+      <c r="K76" s="123"/>
+      <c r="L76" s="123"/>
+      <c r="M76" s="123"/>
+      <c r="N76" s="78" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
-      <c r="O76" s="70" t="e" vm="34">
+      <c r="O76" s="70" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
-      <c r="P76" s="70" t="e" vm="35">
+      <c r="P76" s="70" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
       <c r="Q76" s="79"/>
@@ -7141,19 +7236,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="120"/>
-      <c r="G77" s="120"/>
-      <c r="H77" s="120"/>
-      <c r="I77" s="120"/>
-      <c r="J77" s="120"/>
-      <c r="K77" s="120"/>
-      <c r="L77" s="120"/>
-      <c r="M77" s="120"/>
+      <c r="F77" s="121"/>
+      <c r="G77" s="121"/>
+      <c r="H77" s="121"/>
+      <c r="I77" s="121"/>
+      <c r="J77" s="121"/>
+      <c r="K77" s="121"/>
+      <c r="L77" s="121"/>
+      <c r="M77" s="121"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="128"/>
-      <c r="P77" s="128"/>
-      <c r="Q77" s="128"/>
-      <c r="R77" s="128"/>
+      <c r="O77" s="129"/>
+      <c r="P77" s="129"/>
+      <c r="Q77" s="129"/>
+      <c r="R77" s="129"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7166,7 +7261,7 @@
     <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="81" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A81" s="35" t="e" vm="36">
+      <c r="A81" s="35" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
       <c r="B81" s="77" t="s">
@@ -7181,32 +7276,32 @@
       <c r="E81" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="121" t="s">
+      <c r="F81" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="121"/>
-      <c r="H81" s="121"/>
-      <c r="I81" s="121"/>
-      <c r="J81" s="121"/>
-      <c r="K81" s="121"/>
-      <c r="L81" s="121"/>
-      <c r="M81" s="121"/>
-      <c r="N81" s="121"/>
-      <c r="O81" s="121"/>
-      <c r="P81" s="121"/>
-      <c r="Q81" s="121" t="s">
+      <c r="G81" s="122"/>
+      <c r="H81" s="122"/>
+      <c r="I81" s="122"/>
+      <c r="J81" s="122"/>
+      <c r="K81" s="122"/>
+      <c r="L81" s="122"/>
+      <c r="M81" s="122"/>
+      <c r="N81" s="122"/>
+      <c r="O81" s="122"/>
+      <c r="P81" s="122"/>
+      <c r="Q81" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="121"/>
-      <c r="S81" s="121"/>
-      <c r="T81" s="121"/>
-      <c r="U81" s="121"/>
-      <c r="V81" s="121"/>
-      <c r="W81" s="121"/>
-      <c r="X81" s="121"/>
-      <c r="Y81" s="121"/>
-      <c r="Z81" s="121"/>
-      <c r="AA81" s="121"/>
+      <c r="R81" s="122"/>
+      <c r="S81" s="122"/>
+      <c r="T81" s="122"/>
+      <c r="U81" s="122"/>
+      <c r="V81" s="122"/>
+      <c r="W81" s="122"/>
+      <c r="X81" s="122"/>
+      <c r="Y81" s="122"/>
+      <c r="Z81" s="122"/>
+      <c r="AA81" s="122"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7222,32 +7317,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="134" t="s">
+      <c r="F82" s="135" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="134"/>
-      <c r="H82" s="134"/>
-      <c r="I82" s="134"/>
-      <c r="J82" s="134"/>
-      <c r="K82" s="134"/>
-      <c r="L82" s="134"/>
-      <c r="M82" s="134"/>
-      <c r="N82" s="134"/>
-      <c r="O82" s="134"/>
-      <c r="P82" s="134"/>
-      <c r="Q82" s="134" t="s">
+      <c r="G82" s="135"/>
+      <c r="H82" s="135"/>
+      <c r="I82" s="135"/>
+      <c r="J82" s="135"/>
+      <c r="K82" s="135"/>
+      <c r="L82" s="135"/>
+      <c r="M82" s="135"/>
+      <c r="N82" s="135"/>
+      <c r="O82" s="135"/>
+      <c r="P82" s="135"/>
+      <c r="Q82" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="134"/>
-      <c r="S82" s="134"/>
-      <c r="T82" s="134"/>
-      <c r="U82" s="134"/>
-      <c r="V82" s="134"/>
-      <c r="W82" s="134"/>
-      <c r="X82" s="134"/>
-      <c r="Y82" s="134"/>
-      <c r="Z82" s="134"/>
-      <c r="AA82" s="134"/>
+      <c r="R82" s="135"/>
+      <c r="S82" s="135"/>
+      <c r="T82" s="135"/>
+      <c r="U82" s="135"/>
+      <c r="V82" s="135"/>
+      <c r="W82" s="135"/>
+      <c r="X82" s="135"/>
+      <c r="Y82" s="135"/>
+      <c r="Z82" s="135"/>
+      <c r="AA82" s="135"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7263,30 +7358,30 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="117" t="s">
+      <c r="F83" s="118" t="s">
         <v>226</v>
       </c>
-      <c r="G83" s="117"/>
-      <c r="H83" s="117"/>
-      <c r="I83" s="117"/>
-      <c r="J83" s="117"/>
-      <c r="K83" s="117"/>
-      <c r="L83" s="117"/>
-      <c r="M83" s="117"/>
-      <c r="N83" s="117"/>
-      <c r="O83" s="117"/>
-      <c r="P83" s="117"/>
-      <c r="Q83" s="117"/>
-      <c r="R83" s="117"/>
-      <c r="S83" s="117"/>
-      <c r="T83" s="117"/>
-      <c r="U83" s="117"/>
-      <c r="V83" s="117"/>
-      <c r="W83" s="117"/>
-      <c r="X83" s="117"/>
-      <c r="Y83" s="117"/>
-      <c r="Z83" s="117"/>
-      <c r="AA83" s="117"/>
+      <c r="G83" s="118"/>
+      <c r="H83" s="118"/>
+      <c r="I83" s="118"/>
+      <c r="J83" s="118"/>
+      <c r="K83" s="118"/>
+      <c r="L83" s="118"/>
+      <c r="M83" s="118"/>
+      <c r="N83" s="118"/>
+      <c r="O83" s="118"/>
+      <c r="P83" s="118"/>
+      <c r="Q83" s="118"/>
+      <c r="R83" s="118"/>
+      <c r="S83" s="118"/>
+      <c r="T83" s="118"/>
+      <c r="U83" s="118"/>
+      <c r="V83" s="118"/>
+      <c r="W83" s="118"/>
+      <c r="X83" s="118"/>
+      <c r="Y83" s="118"/>
+      <c r="Z83" s="118"/>
+      <c r="AA83" s="118"/>
     </row>
     <row r="84" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A84" s="38"/>
@@ -7302,30 +7397,30 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="117" t="s">
+      <c r="F84" s="118" t="s">
         <v>227</v>
       </c>
-      <c r="G84" s="117"/>
-      <c r="H84" s="117"/>
-      <c r="I84" s="117"/>
-      <c r="J84" s="117"/>
-      <c r="K84" s="117"/>
-      <c r="L84" s="117"/>
-      <c r="M84" s="117"/>
-      <c r="N84" s="117"/>
-      <c r="O84" s="117"/>
-      <c r="P84" s="117"/>
-      <c r="Q84" s="117"/>
-      <c r="R84" s="117"/>
-      <c r="S84" s="117"/>
-      <c r="T84" s="117"/>
-      <c r="U84" s="117"/>
-      <c r="V84" s="117"/>
-      <c r="W84" s="117"/>
-      <c r="X84" s="117"/>
-      <c r="Y84" s="117"/>
-      <c r="Z84" s="117"/>
-      <c r="AA84" s="117"/>
+      <c r="G84" s="118"/>
+      <c r="H84" s="118"/>
+      <c r="I84" s="118"/>
+      <c r="J84" s="118"/>
+      <c r="K84" s="118"/>
+      <c r="L84" s="118"/>
+      <c r="M84" s="118"/>
+      <c r="N84" s="118"/>
+      <c r="O84" s="118"/>
+      <c r="P84" s="118"/>
+      <c r="Q84" s="118"/>
+      <c r="R84" s="118"/>
+      <c r="S84" s="118"/>
+      <c r="T84" s="118"/>
+      <c r="U84" s="118"/>
+      <c r="V84" s="118"/>
+      <c r="W84" s="118"/>
+      <c r="X84" s="118"/>
+      <c r="Y84" s="118"/>
+      <c r="Z84" s="118"/>
+      <c r="AA84" s="118"/>
     </row>
     <row r="85" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A85" s="38"/>
@@ -7341,32 +7436,32 @@
       <c r="E85" s="54">
         <v>1</v>
       </c>
-      <c r="F85" s="117" t="s">
+      <c r="F85" s="118" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="117"/>
-      <c r="H85" s="117"/>
-      <c r="I85" s="117"/>
-      <c r="J85" s="117"/>
-      <c r="K85" s="117"/>
-      <c r="L85" s="117"/>
-      <c r="M85" s="117"/>
-      <c r="N85" s="117"/>
-      <c r="O85" s="117"/>
-      <c r="P85" s="117"/>
-      <c r="Q85" s="117" t="s">
+      <c r="G85" s="118"/>
+      <c r="H85" s="118"/>
+      <c r="I85" s="118"/>
+      <c r="J85" s="118"/>
+      <c r="K85" s="118"/>
+      <c r="L85" s="118"/>
+      <c r="M85" s="118"/>
+      <c r="N85" s="118"/>
+      <c r="O85" s="118"/>
+      <c r="P85" s="118"/>
+      <c r="Q85" s="118" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="117"/>
-      <c r="S85" s="117"/>
-      <c r="T85" s="117"/>
-      <c r="U85" s="117"/>
-      <c r="V85" s="117"/>
-      <c r="W85" s="117"/>
-      <c r="X85" s="117"/>
-      <c r="Y85" s="117"/>
-      <c r="Z85" s="117"/>
-      <c r="AA85" s="117"/>
+      <c r="R85" s="118"/>
+      <c r="S85" s="118"/>
+      <c r="T85" s="118"/>
+      <c r="U85" s="118"/>
+      <c r="V85" s="118"/>
+      <c r="W85" s="118"/>
+      <c r="X85" s="118"/>
+      <c r="Y85" s="118"/>
+      <c r="Z85" s="118"/>
+      <c r="AA85" s="118"/>
     </row>
     <row r="86" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="38" t="s">
@@ -7378,28 +7473,28 @@
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="117"/>
-      <c r="G86" s="117"/>
-      <c r="H86" s="117"/>
-      <c r="I86" s="117"/>
-      <c r="J86" s="117"/>
-      <c r="K86" s="117"/>
-      <c r="L86" s="117"/>
-      <c r="M86" s="117"/>
-      <c r="N86" s="117"/>
-      <c r="O86" s="117"/>
-      <c r="P86" s="117"/>
-      <c r="Q86" s="117"/>
-      <c r="R86" s="117"/>
-      <c r="S86" s="117"/>
-      <c r="T86" s="117"/>
-      <c r="U86" s="117"/>
-      <c r="V86" s="117"/>
-      <c r="W86" s="117"/>
-      <c r="X86" s="117"/>
-      <c r="Y86" s="117"/>
-      <c r="Z86" s="117"/>
-      <c r="AA86" s="117"/>
+      <c r="F86" s="118"/>
+      <c r="G86" s="118"/>
+      <c r="H86" s="118"/>
+      <c r="I86" s="118"/>
+      <c r="J86" s="118"/>
+      <c r="K86" s="118"/>
+      <c r="L86" s="118"/>
+      <c r="M86" s="118"/>
+      <c r="N86" s="118"/>
+      <c r="O86" s="118"/>
+      <c r="P86" s="118"/>
+      <c r="Q86" s="118"/>
+      <c r="R86" s="118"/>
+      <c r="S86" s="118"/>
+      <c r="T86" s="118"/>
+      <c r="U86" s="118"/>
+      <c r="V86" s="118"/>
+      <c r="W86" s="118"/>
+      <c r="X86" s="118"/>
+      <c r="Y86" s="118"/>
+      <c r="Z86" s="118"/>
+      <c r="AA86" s="118"/>
     </row>
     <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="38"/>
@@ -7407,28 +7502,28 @@
       <c r="C87" s="65"/>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
-      <c r="F87" s="117"/>
-      <c r="G87" s="117"/>
-      <c r="H87" s="117"/>
-      <c r="I87" s="117"/>
-      <c r="J87" s="117"/>
-      <c r="K87" s="117"/>
-      <c r="L87" s="117"/>
-      <c r="M87" s="117"/>
-      <c r="N87" s="117"/>
-      <c r="O87" s="117"/>
-      <c r="P87" s="117"/>
-      <c r="Q87" s="117"/>
-      <c r="R87" s="117"/>
-      <c r="S87" s="117"/>
-      <c r="T87" s="117"/>
-      <c r="U87" s="117"/>
-      <c r="V87" s="117"/>
-      <c r="W87" s="117"/>
-      <c r="X87" s="117"/>
-      <c r="Y87" s="117"/>
-      <c r="Z87" s="117"/>
-      <c r="AA87" s="117"/>
+      <c r="F87" s="118"/>
+      <c r="G87" s="118"/>
+      <c r="H87" s="118"/>
+      <c r="I87" s="118"/>
+      <c r="J87" s="118"/>
+      <c r="K87" s="118"/>
+      <c r="L87" s="118"/>
+      <c r="M87" s="118"/>
+      <c r="N87" s="118"/>
+      <c r="O87" s="118"/>
+      <c r="P87" s="118"/>
+      <c r="Q87" s="118"/>
+      <c r="R87" s="118"/>
+      <c r="S87" s="118"/>
+      <c r="T87" s="118"/>
+      <c r="U87" s="118"/>
+      <c r="V87" s="118"/>
+      <c r="W87" s="118"/>
+      <c r="X87" s="118"/>
+      <c r="Y87" s="118"/>
+      <c r="Z87" s="118"/>
+      <c r="AA87" s="118"/>
     </row>
     <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="89" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -7437,598 +7532,598 @@
       <c r="B90" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="129" t="s">
+      <c r="C90" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="129"/>
-      <c r="E90" s="129"/>
-      <c r="F90" s="129"/>
-      <c r="G90" s="129"/>
-      <c r="H90" s="129" t="s">
+      <c r="D90" s="130"/>
+      <c r="E90" s="130"/>
+      <c r="F90" s="130"/>
+      <c r="G90" s="130"/>
+      <c r="H90" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="129"/>
-      <c r="J90" s="129"/>
-      <c r="K90" s="129"/>
-      <c r="L90" s="129"/>
-      <c r="M90" s="121" t="s">
+      <c r="I90" s="130"/>
+      <c r="J90" s="130"/>
+      <c r="K90" s="130"/>
+      <c r="L90" s="130"/>
+      <c r="M90" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="121"/>
+      <c r="N90" s="122"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A91" s="38" t="e" vm="37">
+      <c r="A91" s="38" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="116" t="s">
+      <c r="C91" s="117" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="116"/>
-      <c r="E91" s="116"/>
-      <c r="F91" s="116"/>
-      <c r="G91" s="116"/>
-      <c r="H91" s="116" t="s">
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="117"/>
+      <c r="G91" s="117"/>
+      <c r="H91" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="116"/>
-      <c r="J91" s="116"/>
-      <c r="K91" s="116"/>
-      <c r="L91" s="116"/>
-      <c r="M91" s="115" t="s">
+      <c r="I91" s="117"/>
+      <c r="J91" s="117"/>
+      <c r="K91" s="117"/>
+      <c r="L91" s="117"/>
+      <c r="M91" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="115"/>
+      <c r="N91" s="116"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A92" s="38" t="e" vm="38">
+      <c r="A92" s="38" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="116" t="s">
+      <c r="C92" s="117" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="116"/>
-      <c r="E92" s="116"/>
-      <c r="F92" s="116"/>
-      <c r="G92" s="116"/>
-      <c r="H92" s="116" t="s">
+      <c r="D92" s="117"/>
+      <c r="E92" s="117"/>
+      <c r="F92" s="117"/>
+      <c r="G92" s="117"/>
+      <c r="H92" s="117" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="116"/>
-      <c r="J92" s="116"/>
-      <c r="K92" s="116"/>
-      <c r="L92" s="116"/>
-      <c r="M92" s="115" t="s">
+      <c r="I92" s="117"/>
+      <c r="J92" s="117"/>
+      <c r="K92" s="117"/>
+      <c r="L92" s="117"/>
+      <c r="M92" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="115"/>
+      <c r="N92" s="116"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A93" s="38" t="e" vm="39">
+      <c r="A93" s="38" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="116" t="s">
+      <c r="C93" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="116"/>
-      <c r="E93" s="116"/>
-      <c r="F93" s="116"/>
-      <c r="G93" s="116"/>
-      <c r="H93" s="116" t="s">
+      <c r="D93" s="117"/>
+      <c r="E93" s="117"/>
+      <c r="F93" s="117"/>
+      <c r="G93" s="117"/>
+      <c r="H93" s="117" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="116"/>
-      <c r="J93" s="116"/>
-      <c r="K93" s="116"/>
-      <c r="L93" s="116"/>
-      <c r="M93" s="115" t="s">
+      <c r="I93" s="117"/>
+      <c r="J93" s="117"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="117"/>
+      <c r="M93" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="115"/>
+      <c r="N93" s="116"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A94" s="38" t="e" vm="40">
+      <c r="A94" s="38" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="116" t="s">
+      <c r="C94" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="116"/>
-      <c r="E94" s="116"/>
-      <c r="F94" s="116"/>
-      <c r="G94" s="116"/>
-      <c r="H94" s="116" t="s">
+      <c r="D94" s="117"/>
+      <c r="E94" s="117"/>
+      <c r="F94" s="117"/>
+      <c r="G94" s="117"/>
+      <c r="H94" s="117" t="s">
         <v>218</v>
       </c>
-      <c r="I94" s="116"/>
-      <c r="J94" s="116"/>
-      <c r="K94" s="116"/>
-      <c r="L94" s="116"/>
-      <c r="M94" s="115" t="s">
+      <c r="I94" s="117"/>
+      <c r="J94" s="117"/>
+      <c r="K94" s="117"/>
+      <c r="L94" s="117"/>
+      <c r="M94" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="115"/>
+      <c r="N94" s="116"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A95" s="38" t="e" vm="41">
+      <c r="A95" s="38" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C95" s="116" t="s">
+      <c r="C95" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="116"/>
-      <c r="E95" s="116"/>
-      <c r="F95" s="116"/>
-      <c r="G95" s="116"/>
-      <c r="H95" s="116" t="s">
+      <c r="D95" s="117"/>
+      <c r="E95" s="117"/>
+      <c r="F95" s="117"/>
+      <c r="G95" s="117"/>
+      <c r="H95" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="I95" s="116"/>
-      <c r="J95" s="116"/>
-      <c r="K95" s="116"/>
-      <c r="L95" s="116"/>
-      <c r="M95" s="115" t="s">
+      <c r="I95" s="117"/>
+      <c r="J95" s="117"/>
+      <c r="K95" s="117"/>
+      <c r="L95" s="117"/>
+      <c r="M95" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="115"/>
+      <c r="N95" s="116"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A96" s="38" t="e" vm="42">
+      <c r="A96" s="38" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="116" t="s">
+      <c r="C96" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="116"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="116"/>
-      <c r="G96" s="116"/>
-      <c r="H96" s="116" t="s">
+      <c r="D96" s="117"/>
+      <c r="E96" s="117"/>
+      <c r="F96" s="117"/>
+      <c r="G96" s="117"/>
+      <c r="H96" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="I96" s="116"/>
-      <c r="J96" s="116"/>
-      <c r="K96" s="116"/>
-      <c r="L96" s="116"/>
-      <c r="M96" s="115" t="s">
+      <c r="I96" s="117"/>
+      <c r="J96" s="117"/>
+      <c r="K96" s="117"/>
+      <c r="L96" s="117"/>
+      <c r="M96" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="115"/>
+      <c r="N96" s="116"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A97" s="38" t="e" vm="43">
+      <c r="A97" s="38" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="116" t="s">
+      <c r="C97" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="116"/>
-      <c r="E97" s="116"/>
-      <c r="F97" s="116"/>
-      <c r="G97" s="116"/>
-      <c r="H97" s="116" t="s">
+      <c r="D97" s="117"/>
+      <c r="E97" s="117"/>
+      <c r="F97" s="117"/>
+      <c r="G97" s="117"/>
+      <c r="H97" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="I97" s="116"/>
-      <c r="J97" s="116"/>
-      <c r="K97" s="116"/>
-      <c r="L97" s="116"/>
-      <c r="M97" s="115" t="s">
+      <c r="I97" s="117"/>
+      <c r="J97" s="117"/>
+      <c r="K97" s="117"/>
+      <c r="L97" s="117"/>
+      <c r="M97" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="115"/>
+      <c r="N97" s="116"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A98" s="38" t="e" vm="44">
+      <c r="A98" s="38" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="116" t="s">
+      <c r="C98" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="116"/>
-      <c r="E98" s="116"/>
-      <c r="F98" s="116"/>
-      <c r="G98" s="116"/>
-      <c r="H98" s="116" t="s">
+      <c r="D98" s="117"/>
+      <c r="E98" s="117"/>
+      <c r="F98" s="117"/>
+      <c r="G98" s="117"/>
+      <c r="H98" s="117" t="s">
         <v>222</v>
       </c>
-      <c r="I98" s="116"/>
-      <c r="J98" s="116"/>
-      <c r="K98" s="116"/>
-      <c r="L98" s="116"/>
-      <c r="M98" s="115" t="s">
+      <c r="I98" s="117"/>
+      <c r="J98" s="117"/>
+      <c r="K98" s="117"/>
+      <c r="L98" s="117"/>
+      <c r="M98" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="115"/>
+      <c r="N98" s="116"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A99" s="38" t="e" vm="45">
+      <c r="A99" s="38" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C99" s="116" t="s">
+      <c r="C99" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="116"/>
-      <c r="E99" s="116"/>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116" t="s">
+      <c r="D99" s="117"/>
+      <c r="E99" s="117"/>
+      <c r="F99" s="117"/>
+      <c r="G99" s="117"/>
+      <c r="H99" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="I99" s="116"/>
-      <c r="J99" s="116"/>
-      <c r="K99" s="116"/>
-      <c r="L99" s="116"/>
-      <c r="M99" s="115" t="s">
+      <c r="I99" s="117"/>
+      <c r="J99" s="117"/>
+      <c r="K99" s="117"/>
+      <c r="L99" s="117"/>
+      <c r="M99" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="115"/>
+      <c r="N99" s="116"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A100" s="38" t="e" vm="46">
+      <c r="A100" s="38" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C100" s="116" t="s">
+      <c r="C100" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="116"/>
-      <c r="E100" s="116"/>
-      <c r="F100" s="116"/>
-      <c r="G100" s="116"/>
-      <c r="H100" s="116" t="s">
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="116"/>
-      <c r="J100" s="116"/>
-      <c r="K100" s="116"/>
-      <c r="L100" s="116"/>
-      <c r="M100" s="115" t="s">
+      <c r="I100" s="117"/>
+      <c r="J100" s="117"/>
+      <c r="K100" s="117"/>
+      <c r="L100" s="117"/>
+      <c r="M100" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="115"/>
+      <c r="N100" s="116"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="116"/>
-      <c r="D101" s="116"/>
-      <c r="E101" s="116"/>
-      <c r="F101" s="116"/>
-      <c r="G101" s="116"/>
-      <c r="H101" s="116"/>
-      <c r="I101" s="116"/>
-      <c r="J101" s="116"/>
-      <c r="K101" s="116"/>
-      <c r="L101" s="116"/>
-      <c r="M101" s="115"/>
-      <c r="N101" s="115"/>
+      <c r="C101" s="117"/>
+      <c r="D101" s="117"/>
+      <c r="E101" s="117"/>
+      <c r="F101" s="117"/>
+      <c r="G101" s="117"/>
+      <c r="H101" s="117"/>
+      <c r="I101" s="117"/>
+      <c r="J101" s="117"/>
+      <c r="K101" s="117"/>
+      <c r="L101" s="117"/>
+      <c r="M101" s="116"/>
+      <c r="N101" s="116"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="116"/>
-      <c r="I102" s="116"/>
-      <c r="J102" s="116"/>
-      <c r="K102" s="116"/>
-      <c r="L102" s="116"/>
-      <c r="M102" s="115"/>
-      <c r="N102" s="115"/>
+      <c r="H102" s="117"/>
+      <c r="I102" s="117"/>
+      <c r="J102" s="117"/>
+      <c r="K102" s="117"/>
+      <c r="L102" s="117"/>
+      <c r="M102" s="116"/>
+      <c r="N102" s="116"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="116"/>
-      <c r="D103" s="116"/>
-      <c r="E103" s="116"/>
-      <c r="F103" s="116"/>
-      <c r="G103" s="116"/>
-      <c r="H103" s="116"/>
-      <c r="I103" s="116"/>
-      <c r="J103" s="116"/>
-      <c r="K103" s="116"/>
-      <c r="L103" s="116"/>
-      <c r="M103" s="115"/>
-      <c r="N103" s="115"/>
+      <c r="C103" s="117"/>
+      <c r="D103" s="117"/>
+      <c r="E103" s="117"/>
+      <c r="F103" s="117"/>
+      <c r="G103" s="117"/>
+      <c r="H103" s="117"/>
+      <c r="I103" s="117"/>
+      <c r="J103" s="117"/>
+      <c r="K103" s="117"/>
+      <c r="L103" s="117"/>
+      <c r="M103" s="116"/>
+      <c r="N103" s="116"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="116"/>
-      <c r="D104" s="116"/>
-      <c r="E104" s="116"/>
-      <c r="F104" s="116"/>
-      <c r="G104" s="116"/>
-      <c r="H104" s="116"/>
-      <c r="I104" s="116"/>
-      <c r="J104" s="116"/>
-      <c r="K104" s="116"/>
-      <c r="L104" s="116"/>
-      <c r="M104" s="115"/>
-      <c r="N104" s="115"/>
+      <c r="C104" s="117"/>
+      <c r="D104" s="117"/>
+      <c r="E104" s="117"/>
+      <c r="F104" s="117"/>
+      <c r="G104" s="117"/>
+      <c r="H104" s="117"/>
+      <c r="I104" s="117"/>
+      <c r="J104" s="117"/>
+      <c r="K104" s="117"/>
+      <c r="L104" s="117"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="116"/>
-      <c r="D105" s="116"/>
-      <c r="E105" s="116"/>
-      <c r="F105" s="116"/>
-      <c r="G105" s="116"/>
-      <c r="H105" s="116"/>
-      <c r="I105" s="116"/>
-      <c r="J105" s="116"/>
-      <c r="K105" s="116"/>
-      <c r="L105" s="116"/>
-      <c r="M105" s="115"/>
-      <c r="N105" s="115"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
+      <c r="M105" s="116"/>
+      <c r="N105" s="116"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="116"/>
-      <c r="D106" s="116"/>
-      <c r="E106" s="116"/>
-      <c r="F106" s="116"/>
-      <c r="G106" s="116"/>
-      <c r="H106" s="116"/>
-      <c r="I106" s="116"/>
-      <c r="J106" s="116"/>
-      <c r="K106" s="116"/>
-      <c r="L106" s="116"/>
-      <c r="M106" s="115"/>
-      <c r="N106" s="115"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
+      <c r="M106" s="116"/>
+      <c r="N106" s="116"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="116"/>
-      <c r="D107" s="116"/>
-      <c r="E107" s="116"/>
-      <c r="F107" s="116"/>
-      <c r="G107" s="116"/>
-      <c r="H107" s="116"/>
-      <c r="I107" s="116"/>
-      <c r="J107" s="116"/>
-      <c r="K107" s="116"/>
-      <c r="L107" s="116"/>
-      <c r="M107" s="115"/>
-      <c r="N107" s="115"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="117"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="117"/>
+      <c r="J107" s="117"/>
+      <c r="K107" s="117"/>
+      <c r="L107" s="117"/>
+      <c r="M107" s="116"/>
+      <c r="N107" s="116"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="116"/>
-      <c r="D108" s="116"/>
-      <c r="E108" s="116"/>
-      <c r="F108" s="116"/>
-      <c r="G108" s="116"/>
-      <c r="H108" s="116"/>
-      <c r="I108" s="116"/>
-      <c r="J108" s="116"/>
-      <c r="K108" s="116"/>
-      <c r="L108" s="116"/>
-      <c r="M108" s="115"/>
-      <c r="N108" s="115"/>
+      <c r="C108" s="117"/>
+      <c r="D108" s="117"/>
+      <c r="E108" s="117"/>
+      <c r="F108" s="117"/>
+      <c r="G108" s="117"/>
+      <c r="H108" s="117"/>
+      <c r="I108" s="117"/>
+      <c r="J108" s="117"/>
+      <c r="K108" s="117"/>
+      <c r="L108" s="117"/>
+      <c r="M108" s="116"/>
+      <c r="N108" s="116"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="116"/>
-      <c r="D109" s="116"/>
-      <c r="E109" s="116"/>
-      <c r="F109" s="116"/>
-      <c r="G109" s="116"/>
-      <c r="H109" s="116"/>
-      <c r="I109" s="116"/>
-      <c r="J109" s="116"/>
-      <c r="K109" s="116"/>
-      <c r="L109" s="116"/>
-      <c r="M109" s="115"/>
-      <c r="N109" s="115"/>
+      <c r="C109" s="117"/>
+      <c r="D109" s="117"/>
+      <c r="E109" s="117"/>
+      <c r="F109" s="117"/>
+      <c r="G109" s="117"/>
+      <c r="H109" s="117"/>
+      <c r="I109" s="117"/>
+      <c r="J109" s="117"/>
+      <c r="K109" s="117"/>
+      <c r="L109" s="117"/>
+      <c r="M109" s="116"/>
+      <c r="N109" s="116"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="116"/>
-      <c r="D110" s="116"/>
-      <c r="E110" s="116"/>
-      <c r="F110" s="116"/>
-      <c r="G110" s="116"/>
-      <c r="H110" s="116"/>
-      <c r="I110" s="116"/>
-      <c r="J110" s="116"/>
-      <c r="K110" s="116"/>
-      <c r="L110" s="116"/>
-      <c r="M110" s="115"/>
-      <c r="N110" s="115"/>
+      <c r="C110" s="117"/>
+      <c r="D110" s="117"/>
+      <c r="E110" s="117"/>
+      <c r="F110" s="117"/>
+      <c r="G110" s="117"/>
+      <c r="H110" s="117"/>
+      <c r="I110" s="117"/>
+      <c r="J110" s="117"/>
+      <c r="K110" s="117"/>
+      <c r="L110" s="117"/>
+      <c r="M110" s="116"/>
+      <c r="N110" s="116"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="116"/>
-      <c r="E111" s="116"/>
-      <c r="F111" s="116"/>
-      <c r="G111" s="116"/>
-      <c r="H111" s="116"/>
-      <c r="I111" s="116"/>
-      <c r="J111" s="116"/>
-      <c r="K111" s="116"/>
-      <c r="L111" s="116"/>
-      <c r="M111" s="115"/>
-      <c r="N111" s="115"/>
+      <c r="C111" s="117"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="117"/>
+      <c r="F111" s="117"/>
+      <c r="G111" s="117"/>
+      <c r="H111" s="117"/>
+      <c r="I111" s="117"/>
+      <c r="J111" s="117"/>
+      <c r="K111" s="117"/>
+      <c r="L111" s="117"/>
+      <c r="M111" s="116"/>
+      <c r="N111" s="116"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="116"/>
-      <c r="D112" s="116"/>
-      <c r="E112" s="116"/>
-      <c r="F112" s="116"/>
-      <c r="G112" s="116"/>
-      <c r="H112" s="116"/>
-      <c r="I112" s="116"/>
-      <c r="J112" s="116"/>
-      <c r="K112" s="116"/>
-      <c r="L112" s="116"/>
-      <c r="M112" s="115"/>
-      <c r="N112" s="115"/>
+      <c r="C112" s="117"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="117"/>
+      <c r="F112" s="117"/>
+      <c r="G112" s="117"/>
+      <c r="H112" s="117"/>
+      <c r="I112" s="117"/>
+      <c r="J112" s="117"/>
+      <c r="K112" s="117"/>
+      <c r="L112" s="117"/>
+      <c r="M112" s="116"/>
+      <c r="N112" s="116"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="116"/>
-      <c r="D113" s="116"/>
-      <c r="E113" s="116"/>
-      <c r="F113" s="116"/>
-      <c r="G113" s="116"/>
-      <c r="H113" s="116"/>
-      <c r="I113" s="116"/>
-      <c r="J113" s="116"/>
-      <c r="K113" s="116"/>
-      <c r="L113" s="116"/>
-      <c r="M113" s="115"/>
-      <c r="N113" s="115"/>
+      <c r="C113" s="117"/>
+      <c r="D113" s="117"/>
+      <c r="E113" s="117"/>
+      <c r="F113" s="117"/>
+      <c r="G113" s="117"/>
+      <c r="H113" s="117"/>
+      <c r="I113" s="117"/>
+      <c r="J113" s="117"/>
+      <c r="K113" s="117"/>
+      <c r="L113" s="117"/>
+      <c r="M113" s="116"/>
+      <c r="N113" s="116"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="116"/>
-      <c r="D114" s="116"/>
-      <c r="E114" s="116"/>
-      <c r="F114" s="116"/>
-      <c r="G114" s="116"/>
-      <c r="H114" s="116"/>
-      <c r="I114" s="116"/>
-      <c r="J114" s="116"/>
-      <c r="K114" s="116"/>
-      <c r="L114" s="116"/>
-      <c r="M114" s="115"/>
-      <c r="N114" s="115"/>
+      <c r="C114" s="117"/>
+      <c r="D114" s="117"/>
+      <c r="E114" s="117"/>
+      <c r="F114" s="117"/>
+      <c r="G114" s="117"/>
+      <c r="H114" s="117"/>
+      <c r="I114" s="117"/>
+      <c r="J114" s="117"/>
+      <c r="K114" s="117"/>
+      <c r="L114" s="117"/>
+      <c r="M114" s="116"/>
+      <c r="N114" s="116"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="116"/>
-      <c r="D115" s="116"/>
-      <c r="E115" s="116"/>
-      <c r="F115" s="116"/>
-      <c r="G115" s="116"/>
-      <c r="H115" s="116"/>
-      <c r="I115" s="116"/>
-      <c r="J115" s="116"/>
-      <c r="K115" s="116"/>
-      <c r="L115" s="116"/>
-      <c r="M115" s="115"/>
-      <c r="N115" s="115"/>
+      <c r="C115" s="117"/>
+      <c r="D115" s="117"/>
+      <c r="E115" s="117"/>
+      <c r="F115" s="117"/>
+      <c r="G115" s="117"/>
+      <c r="H115" s="117"/>
+      <c r="I115" s="117"/>
+      <c r="J115" s="117"/>
+      <c r="K115" s="117"/>
+      <c r="L115" s="117"/>
+      <c r="M115" s="116"/>
+      <c r="N115" s="116"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="116"/>
-      <c r="D116" s="116"/>
-      <c r="E116" s="116"/>
-      <c r="F116" s="116"/>
-      <c r="G116" s="116"/>
-      <c r="H116" s="116"/>
-      <c r="I116" s="116"/>
-      <c r="J116" s="116"/>
-      <c r="K116" s="116"/>
-      <c r="L116" s="116"/>
-      <c r="M116" s="115"/>
-      <c r="N116" s="115"/>
+      <c r="C116" s="117"/>
+      <c r="D116" s="117"/>
+      <c r="E116" s="117"/>
+      <c r="F116" s="117"/>
+      <c r="G116" s="117"/>
+      <c r="H116" s="117"/>
+      <c r="I116" s="117"/>
+      <c r="J116" s="117"/>
+      <c r="K116" s="117"/>
+      <c r="L116" s="117"/>
+      <c r="M116" s="116"/>
+      <c r="N116" s="116"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="116"/>
-      <c r="D117" s="116"/>
-      <c r="E117" s="116"/>
-      <c r="F117" s="116"/>
-      <c r="G117" s="116"/>
-      <c r="H117" s="116"/>
-      <c r="I117" s="116"/>
-      <c r="J117" s="116"/>
-      <c r="K117" s="116"/>
-      <c r="L117" s="116"/>
-      <c r="M117" s="115"/>
-      <c r="N117" s="115"/>
+      <c r="C117" s="117"/>
+      <c r="D117" s="117"/>
+      <c r="E117" s="117"/>
+      <c r="F117" s="117"/>
+      <c r="G117" s="117"/>
+      <c r="H117" s="117"/>
+      <c r="I117" s="117"/>
+      <c r="J117" s="117"/>
+      <c r="K117" s="117"/>
+      <c r="L117" s="117"/>
+      <c r="M117" s="116"/>
+      <c r="N117" s="116"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="116"/>
-      <c r="D118" s="116"/>
-      <c r="E118" s="116"/>
-      <c r="F118" s="116"/>
-      <c r="G118" s="116"/>
-      <c r="H118" s="116"/>
-      <c r="I118" s="116"/>
-      <c r="J118" s="116"/>
-      <c r="K118" s="116"/>
-      <c r="L118" s="116"/>
-      <c r="M118" s="115"/>
-      <c r="N118" s="115"/>
+      <c r="C118" s="117"/>
+      <c r="D118" s="117"/>
+      <c r="E118" s="117"/>
+      <c r="F118" s="117"/>
+      <c r="G118" s="117"/>
+      <c r="H118" s="117"/>
+      <c r="I118" s="117"/>
+      <c r="J118" s="117"/>
+      <c r="K118" s="117"/>
+      <c r="L118" s="117"/>
+      <c r="M118" s="116"/>
+      <c r="N118" s="116"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Advanced kill log (includes server's kill message) - Zombie damage proportional to its health - Mines now counts as a kill - Airstrikes now counts as a kill
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992C65B-7328-4014-84D4-78ED056906C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B56ECE-D4A9-4C0B-9865-F771A5DDABA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="234">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1475,7 +1475,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EXPLOSIVE AMMO : 3~5 fragments (average of 4 frags, but statistically 3 hits most frequent) / each frag deals 1 damage (same as a bat)</t>
+    <t>explosion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPLOSIVE AMMO : 3~5 explosives (average of 4 frags, but statistically 3 hits most frequent) / each frag deals 1 damage (same as a bat)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2366,69 +2370,69 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2982,6 +2986,45 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304816" cy="298920"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C046836F-8785-4B25-BC2D-DB9ADCFB8881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="721179"/>
+          <a:ext cx="304816" cy="298920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3544,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3563,10 +3606,10 @@
       <c r="B1" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="132" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="126"/>
+      <c r="D1" s="132"/>
       <c r="G1" s="56" t="s">
         <v>159</v>
       </c>
@@ -3662,10 +3705,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="131" t="s">
+      <c r="Z2" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="131"/>
+      <c r="AA2" s="124"/>
       <c r="AG2" s="43" t="s">
         <v>84</v>
       </c>
@@ -4065,11 +4108,11 @@
       <c r="O7" s="19"/>
       <c r="P7" s="33"/>
       <c r="Q7" s="19">
-        <f t="shared" ref="Q7" si="8">-(FLOOR(H7/6,1)-1)</f>
+        <f t="shared" ref="Q7:Q8" si="8">-(FLOOR(H7/6,1)-1)</f>
         <v>1</v>
       </c>
       <c r="R7" s="19">
-        <f t="shared" ref="R7" si="9">ROUND(D7/H7,3)</f>
+        <f t="shared" ref="R7:R8" si="9">ROUND(D7/H7,3)</f>
         <v>0</v>
       </c>
       <c r="S7" s="32" t="s">
@@ -4087,30 +4130,82 @@
       <c r="AL7" s="36"/>
     </row>
     <row r="8" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
+      <c r="A8" s="22" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="42">
+        <v>32</v>
+      </c>
+      <c r="D8" s="19">
+        <v>3</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <v>500</v>
+      </c>
+      <c r="H8" s="19">
+        <v>6</v>
+      </c>
+      <c r="I8" s="19">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19">
+        <f>ROUND(E8*F8/G8*1000,2)</f>
+        <v>2</v>
+      </c>
+      <c r="N8" s="19">
+        <f>ROUND(E8*F8/(G8+J8/I8)*1000,2)</f>
+        <v>0.67</v>
+      </c>
+      <c r="O8" s="19">
+        <f>E8*F8*I8</f>
+        <v>1</v>
+      </c>
+      <c r="P8" s="33">
+        <f>ROUND(playerHealth/(E8*F8),1)</f>
+        <v>8</v>
+      </c>
+      <c r="Q8" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="19">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" s="23"/>
+      <c r="U8" s="19">
+        <f t="shared" ref="U8" si="10" xml:space="preserve"> E8*F8*7/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="V8" s="34">
+        <f>ROUND(playerHealth/(U8),2)</f>
+        <v>11.43</v>
+      </c>
+      <c r="W8" s="19">
+        <f t="shared" ref="W8" si="11">E8*(F8-0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="X8" s="34">
+        <f>ROUND(playerHealth/(W8),2)</f>
+        <v>13.33</v>
+      </c>
       <c r="Y8" s="74"/>
       <c r="Z8" s="57"/>
       <c r="AL8" s="36"/>
@@ -4269,7 +4364,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="19">
-        <f t="shared" ref="N11:N30" si="10">ROUND(E11*F11/(G11+J11/I11)*1000,2)</f>
+        <f t="shared" ref="N11:N30" si="12">ROUND(E11*F11/(G11+J11/I11)*1000,2)</f>
         <v>3.59</v>
       </c>
       <c r="O11" s="19">
@@ -4293,7 +4388,7 @@
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19">
-        <f t="shared" ref="U11" si="11" xml:space="preserve"> E11*F11*9/10</f>
+        <f t="shared" ref="U11" si="13" xml:space="preserve"> E11*F11*9/10</f>
         <v>2.7</v>
       </c>
       <c r="V11" s="29">
@@ -4354,7 +4449,7 @@
         <v>10</v>
       </c>
       <c r="N12" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.65</v>
       </c>
       <c r="O12" s="19">
@@ -4439,7 +4534,7 @@
         <v>4.5</v>
       </c>
       <c r="N13" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.5</v>
       </c>
       <c r="O13" s="19">
@@ -4579,27 +4674,27 @@
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="19">
-        <f>ROUND(E16*F16/G16*1000,2)</f>
+        <f t="shared" ref="M16:M21" si="14">ROUND(E16*F16/G16*1000,2)</f>
         <v>3.33</v>
       </c>
       <c r="N16" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.68</v>
       </c>
       <c r="O16" s="19">
-        <f>E16*F16*I16</f>
+        <f t="shared" ref="O16:O21" si="15">E16*F16*I16</f>
         <v>15</v>
       </c>
       <c r="P16" s="33">
-        <f>ROUND(playerHealth/(E16*F16),1)</f>
+        <f t="shared" ref="P16:P21" si="16">ROUND(playerHealth/(E16*F16),1)</f>
         <v>8</v>
       </c>
       <c r="Q16" s="19">
-        <f>-(FLOOR(H16/6,1)-1)</f>
+        <f t="shared" ref="Q16:Q21" si="17">-(FLOOR(H16/6,1)-1)</f>
         <v>-1</v>
       </c>
       <c r="R16" s="19">
-        <f>ROUND(D16/H16,3)</f>
+        <f t="shared" ref="R16:R21" si="18">ROUND(D16/H16,3)</f>
         <v>0.13300000000000001</v>
       </c>
       <c r="S16" s="25" t="s">
@@ -4607,19 +4702,19 @@
       </c>
       <c r="T16" s="19"/>
       <c r="U16" s="19">
-        <f xml:space="preserve"> E16*F16*9/10</f>
+        <f t="shared" ref="U16:U21" si="19" xml:space="preserve"> E16*F16*9/10</f>
         <v>0.9</v>
       </c>
       <c r="V16" s="34">
-        <f>ROUND(playerHealth/(U16),2)</f>
+        <f t="shared" ref="V16:V21" si="20">ROUND(playerHealth/(U16),2)</f>
         <v>8.89</v>
       </c>
       <c r="W16" s="19">
-        <f>E16*(F16-0.4)</f>
+        <f t="shared" ref="W16:W21" si="21">E16*(F16-0.4)</f>
         <v>0.6</v>
       </c>
       <c r="X16" s="34">
-        <f>ROUND(playerHealth/(W16),2)</f>
+        <f t="shared" ref="X16:X21" si="22">ROUND(playerHealth/(W16),2)</f>
         <v>13.33</v>
       </c>
       <c r="Y16" s="19"/>
@@ -4663,7 +4758,7 @@
       </c>
       <c r="L17" s="19"/>
       <c r="M17" s="19">
-        <f>ROUND(E17*F17/G17*1000,2)</f>
+        <f t="shared" si="14"/>
         <v>13.33</v>
       </c>
       <c r="N17" s="19">
@@ -4671,19 +4766,19 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="O17" s="19">
-        <f>E17*F17*I17</f>
+        <f t="shared" si="15"/>
         <v>150</v>
       </c>
       <c r="P17" s="33">
-        <f>ROUND(playerHealth/(E17*F17),1)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="Q17" s="19">
-        <f>-(FLOOR(H17/6,1)-1)</f>
+        <f t="shared" si="17"/>
         <v>-2</v>
       </c>
       <c r="R17" s="19">
-        <f>ROUND(D17/H17,3)</f>
+        <f t="shared" si="18"/>
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="S17" s="21" t="s">
@@ -4691,19 +4786,19 @@
       </c>
       <c r="T17" s="19"/>
       <c r="U17" s="19">
-        <f xml:space="preserve"> E17*F17*9/10</f>
+        <f t="shared" si="19"/>
         <v>0.9</v>
       </c>
       <c r="V17" s="34">
-        <f>ROUND(playerHealth/(U17),2)</f>
+        <f t="shared" si="20"/>
         <v>8.89</v>
       </c>
       <c r="W17" s="19">
-        <f>E17*(F17-0.4)</f>
+        <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
       <c r="X17" s="34">
-        <f>ROUND(playerHealth/(W17),2)</f>
+        <f t="shared" si="22"/>
         <v>13.33</v>
       </c>
       <c r="Y17" s="19"/>
@@ -4756,27 +4851,27 @@
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="19">
-        <f>ROUND(E18*F18/G18*1000,2)</f>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="N18" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.6500000000000004</v>
       </c>
       <c r="O18" s="19">
-        <f>E18*F18*I18</f>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="P18" s="33">
-        <f>ROUND(playerHealth/(E18*F18),1)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="Q18" s="19">
-        <f>-(FLOOR(H18/6,1)-1)</f>
+        <f t="shared" si="17"/>
         <v>-2</v>
       </c>
       <c r="R18" s="19">
-        <f>ROUND(D18/H18,3)</f>
+        <f t="shared" si="18"/>
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="S18" s="28" t="s">
@@ -4784,19 +4879,19 @@
       </c>
       <c r="T18" s="19"/>
       <c r="U18" s="19">
-        <f xml:space="preserve"> E18*F18*9/10</f>
+        <f t="shared" si="19"/>
         <v>0.9</v>
       </c>
       <c r="V18" s="34">
-        <f>ROUND(playerHealth/(U18),2)</f>
+        <f t="shared" si="20"/>
         <v>8.89</v>
       </c>
       <c r="W18" s="19">
-        <f>E18*(F18-0.4)</f>
+        <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
       <c r="X18" s="34">
-        <f>ROUND(playerHealth/(W18),2)</f>
+        <f t="shared" si="22"/>
         <v>13.33</v>
       </c>
       <c r="Y18" s="19"/>
@@ -4843,27 +4938,27 @@
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19">
-        <f>ROUND(E19*F19/G19*1000,2)</f>
+        <f t="shared" si="14"/>
         <v>9.09</v>
       </c>
       <c r="N19" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.66</v>
       </c>
       <c r="O19" s="19">
-        <f>E19*F19*I19</f>
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
       <c r="P19" s="33">
-        <f>ROUND(playerHealth/(E19*F19),1)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="Q19" s="19">
-        <f>-(FLOOR(H19/6,1)-1)</f>
+        <f t="shared" si="17"/>
         <v>-2</v>
       </c>
       <c r="R19" s="19">
-        <f>ROUND(D19/H19,3)</f>
+        <f t="shared" si="18"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="S19" s="28" t="s">
@@ -4871,19 +4966,19 @@
       </c>
       <c r="T19" s="19"/>
       <c r="U19" s="19">
-        <f xml:space="preserve"> E19*F19*9/10</f>
+        <f t="shared" si="19"/>
         <v>0.9</v>
       </c>
       <c r="V19" s="34">
-        <f>ROUND(playerHealth/(U19),2)</f>
+        <f t="shared" si="20"/>
         <v>8.89</v>
       </c>
       <c r="W19" s="19">
-        <f>E19*(F19-0.4)</f>
+        <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
       <c r="X19" s="34">
-        <f>ROUND(playerHealth/(W19),2)</f>
+        <f t="shared" si="22"/>
         <v>13.33</v>
       </c>
       <c r="Y19" s="19"/>
@@ -4928,27 +5023,27 @@
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="19">
-        <f>ROUND(E20*F20/G20*1000,2)</f>
+        <f t="shared" si="14"/>
         <v>11.11</v>
       </c>
       <c r="N20" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.08</v>
       </c>
       <c r="O20" s="19">
-        <f>E20*F20*I20</f>
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
       <c r="P20" s="33">
-        <f>ROUND(playerHealth/(E20*F20),1)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="Q20" s="19">
-        <f>-(FLOOR(H20/6,1)-1)</f>
+        <f t="shared" si="17"/>
         <v>-1</v>
       </c>
       <c r="R20" s="19">
-        <f>ROUND(D20/H20,3)</f>
+        <f t="shared" si="18"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="S20" s="28" t="s">
@@ -4956,19 +5051,19 @@
       </c>
       <c r="T20" s="19"/>
       <c r="U20" s="19">
-        <f xml:space="preserve"> E20*F20*9/10</f>
+        <f t="shared" si="19"/>
         <v>0.9</v>
       </c>
       <c r="V20" s="34">
-        <f>ROUND(playerHealth/(U20),2)</f>
+        <f t="shared" si="20"/>
         <v>8.89</v>
       </c>
       <c r="W20" s="19">
-        <f>E20*(F20-0.4)</f>
+        <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
       <c r="X20" s="34">
-        <f>ROUND(playerHealth/(W20),2)</f>
+        <f t="shared" si="22"/>
         <v>13.33</v>
       </c>
       <c r="Y20" s="19"/>
@@ -5019,27 +5114,27 @@
       </c>
       <c r="L21" s="19"/>
       <c r="M21" s="19">
-        <f>ROUND(E21*F21/G21*1000,2)</f>
+        <f t="shared" si="14"/>
         <v>6.67</v>
       </c>
       <c r="N21" s="19">
-        <f t="shared" ref="N21" si="12">ROUND(E21*F21/(G21+J21/I21)*1000,2)</f>
+        <f t="shared" ref="N21" si="23">ROUND(E21*F21/(G21+J21/I21)*1000,2)</f>
         <v>3.85</v>
       </c>
       <c r="O21" s="19">
-        <f>E21*F21*I21</f>
+        <f t="shared" si="15"/>
         <v>21</v>
       </c>
       <c r="P21" s="20">
-        <f>ROUND(playerHealth/(E21*F21),1)</f>
+        <f t="shared" si="16"/>
         <v>2.7</v>
       </c>
       <c r="Q21" s="19">
-        <f>-(FLOOR(H21/6,1)-1)</f>
+        <f t="shared" si="17"/>
         <v>-2</v>
       </c>
       <c r="R21" s="19">
-        <f>ROUND(D21/H21,3)</f>
+        <f t="shared" si="18"/>
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="S21" s="28" t="s">
@@ -5047,19 +5142,19 @@
       </c>
       <c r="T21" s="19"/>
       <c r="U21" s="19">
-        <f xml:space="preserve"> E21*F21*9/10</f>
+        <f t="shared" si="19"/>
         <v>2.7</v>
       </c>
       <c r="V21" s="29">
-        <f>ROUND(playerHealth/(U21),2)</f>
+        <f t="shared" si="20"/>
         <v>2.96</v>
       </c>
       <c r="W21" s="19">
-        <f>E21*(F21-0.4)</f>
+        <f t="shared" si="21"/>
         <v>2.6</v>
       </c>
       <c r="X21" s="115">
-        <f>ROUND(playerHealth/(W21),2)</f>
+        <f t="shared" si="22"/>
         <v>3.08</v>
       </c>
       <c r="Y21" s="19"/>
@@ -5139,7 +5234,7 @@
         <v>27.78</v>
       </c>
       <c r="N23" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.02</v>
       </c>
       <c r="O23" s="19">
@@ -5226,7 +5321,7 @@
         <v>7.5</v>
       </c>
       <c r="N24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.62</v>
       </c>
       <c r="O24" s="19">
@@ -5325,11 +5420,11 @@
         <v>2</v>
       </c>
       <c r="Q25" s="19">
-        <f t="shared" ref="Q25" si="13">-(FLOOR(H25/6,1)-1)</f>
+        <f t="shared" ref="Q25" si="24">-(FLOOR(H25/6,1)-1)</f>
         <v>-1</v>
       </c>
       <c r="R25" s="19">
-        <f t="shared" ref="R25" si="14">ROUND(D25/H25,3)</f>
+        <f t="shared" ref="R25" si="25">ROUND(D25/H25,3)</f>
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="S25" s="28" t="s">
@@ -5354,7 +5449,7 @@
       </c>
       <c r="Y25" s="19"/>
       <c r="Z25" s="57" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AL25" s="112">
         <v>8</v>
@@ -5458,7 +5553,7 @@
         <v>9.41</v>
       </c>
       <c r="N28" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.0599999999999996</v>
       </c>
       <c r="O28" s="19">
@@ -5543,7 +5638,7 @@
         <v>16</v>
       </c>
       <c r="N29" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.28</v>
       </c>
       <c r="O29" s="19">
@@ -5628,7 +5723,7 @@
         <v>11.43</v>
       </c>
       <c r="N30" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.71</v>
       </c>
       <c r="O30" s="19">
@@ -5784,7 +5879,7 @@
       <c r="S33" s="32"/>
       <c r="T33" s="19"/>
       <c r="U33" s="19">
-        <f t="shared" ref="U33:U35" si="15" xml:space="preserve"> E33*F33*9/10</f>
+        <f t="shared" ref="U33:U35" si="26" xml:space="preserve"> E33*F33*9/10</f>
         <v>0.18</v>
       </c>
       <c r="V33" s="34">
@@ -5792,7 +5887,7 @@
         <v>44.44</v>
       </c>
       <c r="W33" s="19">
-        <f t="shared" ref="W33:W34" si="16">E33*(F33-0.2)</f>
+        <f t="shared" ref="W33:W34" si="27">E33*(F33-0.2)</f>
         <v>0</v>
       </c>
       <c r="X33" s="34"/>
@@ -5853,7 +5948,7 @@
       <c r="S34" s="32"/>
       <c r="T34" s="19"/>
       <c r="U34" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="26"/>
         <v>0.36</v>
       </c>
       <c r="V34" s="34">
@@ -5861,7 +5956,7 @@
         <v>22.22</v>
       </c>
       <c r="W34" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="27"/>
         <v>0.2</v>
       </c>
       <c r="X34" s="34">
@@ -5883,7 +5978,7 @@
         <v>48</v>
       </c>
       <c r="D35" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="19">
         <v>1</v>
@@ -5906,7 +6001,7 @@
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
       <c r="M35" s="19">
-        <f t="shared" ref="M35" si="17">ROUND(E35*F35/G35*1000,3)</f>
+        <f t="shared" ref="M35" si="28">ROUND(E35*F35/G35*1000,3)</f>
         <v>2</v>
       </c>
       <c r="N35" s="19">
@@ -5923,7 +6018,7 @@
       <c r="S35" s="32"/>
       <c r="T35" s="19"/>
       <c r="U35" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="26"/>
         <v>0.9</v>
       </c>
       <c r="V35" s="33">
@@ -6015,28 +6110,28 @@
       <c r="B40" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="119" t="s">
+      <c r="C40" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119" t="s">
+      <c r="D40" s="130"/>
+      <c r="E40" s="130"/>
+      <c r="F40" s="130"/>
+      <c r="G40" s="130"/>
+      <c r="H40" s="130"/>
+      <c r="I40" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="119"/>
-      <c r="K40" s="119"/>
-      <c r="L40" s="119"/>
+      <c r="J40" s="130"/>
+      <c r="K40" s="130"/>
+      <c r="L40" s="130"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="132" t="s">
+      <c r="S40" s="129" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="132"/>
+      <c r="T40" s="129"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6046,30 +6141,30 @@
       <c r="B41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="120" t="s">
+      <c r="C41" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120" t="s">
+      <c r="D41" s="131"/>
+      <c r="E41" s="131"/>
+      <c r="F41" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120" t="s">
+      <c r="G41" s="131"/>
+      <c r="H41" s="131"/>
+      <c r="I41" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="120"/>
-      <c r="K41" s="120"/>
-      <c r="L41" s="120"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="131"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="132" t="s">
+      <c r="S41" s="129" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="132"/>
+      <c r="T41" s="129"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -6082,30 +6177,30 @@
       <c r="B42" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="120" t="s">
+      <c r="C42" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="120" t="s">
+      <c r="D42" s="131"/>
+      <c r="E42" s="131"/>
+      <c r="F42" s="131" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="120"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="120" t="s">
+      <c r="G42" s="131"/>
+      <c r="H42" s="131"/>
+      <c r="I42" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="120"/>
-      <c r="K42" s="120"/>
-      <c r="L42" s="120"/>
+      <c r="J42" s="131"/>
+      <c r="K42" s="131"/>
+      <c r="L42" s="131"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="132" t="s">
+      <c r="S42" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="132"/>
+      <c r="T42" s="129"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6118,30 +6213,30 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="121" t="s">
+      <c r="C43" s="127" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
-      <c r="F43" s="121" t="s">
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="121"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="121" t="s">
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
+      <c r="I43" s="127" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="121"/>
-      <c r="K43" s="121"/>
-      <c r="L43" s="121"/>
+      <c r="J43" s="127"/>
+      <c r="K43" s="127"/>
+      <c r="L43" s="127"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="132" t="s">
+      <c r="S43" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="132"/>
+      <c r="T43" s="129"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6156,20 +6251,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="121" t="s">
+      <c r="C44" s="127" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121" t="s">
+      <c r="D44" s="127"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="127"/>
+      <c r="I44" s="127" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="121"/>
+      <c r="J44" s="127"/>
+      <c r="K44" s="127"/>
+      <c r="L44" s="127"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6185,16 +6280,16 @@
       <c r="B47" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="119" t="s">
+      <c r="C47" s="130" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="119"/>
-      <c r="E47" s="119" t="s">
+      <c r="D47" s="130"/>
+      <c r="E47" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
+      <c r="F47" s="130"/>
+      <c r="G47" s="130"/>
+      <c r="H47" s="130"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -6205,16 +6300,16 @@
       <c r="B48" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="120">
+      <c r="C48" s="131">
         <v>2</v>
       </c>
-      <c r="D48" s="120"/>
-      <c r="E48" s="120" t="s">
+      <c r="D48" s="131"/>
+      <c r="E48" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="120"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="120"/>
+      <c r="F48" s="131"/>
+      <c r="G48" s="131"/>
+      <c r="H48" s="131"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
@@ -6225,28 +6320,28 @@
       <c r="B49" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="120" t="s">
+      <c r="C49" s="131" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="120" t="s">
+      <c r="D49" s="131"/>
+      <c r="E49" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="120"/>
-      <c r="G49" s="120"/>
-      <c r="H49" s="120"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="121"/>
-      <c r="D50" s="121"/>
-      <c r="E50" s="121"/>
-      <c r="F50" s="121"/>
-      <c r="G50" s="121"/>
-      <c r="H50" s="121"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="127"/>
+      <c r="E50" s="127"/>
+      <c r="F50" s="127"/>
+      <c r="G50" s="127"/>
+      <c r="H50" s="127"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6264,14 +6359,14 @@
       <c r="D54" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="124" t="s">
+      <c r="H54" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="124"/>
-      <c r="J54" s="124"/>
-      <c r="K54" s="124"/>
-      <c r="L54" s="124"/>
-      <c r="M54" s="124"/>
+      <c r="I54" s="136"/>
+      <c r="J54" s="136"/>
+      <c r="K54" s="136"/>
+      <c r="L54" s="136"/>
+      <c r="M54" s="136"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6318,47 +6413,47 @@
         <v>69</v>
       </c>
       <c r="C56" s="19">
-        <f t="shared" ref="C56:M56" si="18">(2+C55)*tilesize</f>
+        <f t="shared" ref="C56:M56" si="29">(2+C55)*tilesize</f>
         <v>128</v>
       </c>
       <c r="D56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>256</v>
       </c>
       <c r="E56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>384</v>
       </c>
       <c r="F56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>512</v>
       </c>
       <c r="G56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>640</v>
       </c>
       <c r="H56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>768</v>
       </c>
       <c r="I56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>896</v>
       </c>
       <c r="J56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>1024</v>
       </c>
       <c r="K56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>1152</v>
       </c>
       <c r="L56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>1280</v>
       </c>
       <c r="M56" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="29"/>
         <v>1408</v>
       </c>
     </row>
@@ -6368,47 +6463,47 @@
         <v>70</v>
       </c>
       <c r="C57" s="51">
-        <f t="shared" ref="C57:M57" si="19">(2+C55+1)*tilesize+tilesize/2</f>
+        <f t="shared" ref="C57:M57" si="30">(2+C55+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
       <c r="D57" s="52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>448</v>
       </c>
       <c r="E57" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>576</v>
       </c>
       <c r="F57" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>704</v>
       </c>
       <c r="G57" s="49">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>832</v>
       </c>
       <c r="H57" s="92">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>960</v>
       </c>
       <c r="I57" s="46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>1088</v>
       </c>
       <c r="J57" s="47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>1216</v>
       </c>
       <c r="K57" s="93">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>1344</v>
       </c>
       <c r="L57" s="45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>1472</v>
       </c>
       <c r="M57" s="42">
-        <f t="shared" si="19"/>
+        <f t="shared" si="30"/>
         <v>1600</v>
       </c>
     </row>
@@ -6422,14 +6517,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="125" t="s">
+      <c r="H58" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="125"/>
-      <c r="J58" s="125"/>
-      <c r="K58" s="125"/>
-      <c r="L58" s="125"/>
-      <c r="M58" s="125"/>
+      <c r="I58" s="137"/>
+      <c r="J58" s="137"/>
+      <c r="K58" s="137"/>
+      <c r="L58" s="137"/>
+      <c r="M58" s="137"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6478,24 +6573,24 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="128" t="s">
+      <c r="J62" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="128"/>
+      <c r="K62" s="134"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
       <c r="M62" s="96">
         <f>COUNTIF(H3:H35,"&gt;0")</f>
-        <v>24</v>
-      </c>
-      <c r="O62" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="O62" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="127"/>
-      <c r="Q62" s="127"/>
-      <c r="R62" s="127"/>
-      <c r="S62" s="127"/>
+      <c r="P62" s="133"/>
+      <c r="Q62" s="133"/>
+      <c r="R62" s="133"/>
+      <c r="S62" s="133"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6517,20 +6612,20 @@
       <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="133" t="s">
+      <c r="F63" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="133"/>
+      <c r="G63" s="119"/>
       <c r="H63" s="86" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="133" t="s">
+      <c r="J63" s="119" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="133"/>
+      <c r="K63" s="119"/>
       <c r="L63" s="86" t="s">
         <v>102</v>
       </c>
@@ -6554,10 +6649,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="133" t="s">
+      <c r="U63" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="133"/>
+      <c r="V63" s="119"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6585,21 +6680,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="134" t="s">
+      <c r="F64" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="134"/>
+      <c r="G64" s="135"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="123">
-        <f t="shared" ref="J64:J69" si="20">(C64-player_radius)*2</f>
+      <c r="J64" s="122">
+        <f t="shared" ref="J64:J69" si="31">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="123"/>
+      <c r="K64" s="122"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -6610,19 +6705,19 @@
       </c>
       <c r="N64" s="97"/>
       <c r="O64" s="99">
-        <f t="shared" ref="O64:O70" si="21">ROUND(D64/health_cap,2)*10</f>
+        <f t="shared" ref="O64:O70" si="32">ROUND(D64/health_cap,2)*10</f>
         <v>0.8</v>
       </c>
       <c r="P64" s="100">
-        <f t="shared" ref="P64:P70" si="22">ROUND(M64/guns_cap,2)*10</f>
+        <f t="shared" ref="P64:P70" si="33">ROUND(M64/guns_cap,2)*10</f>
         <v>3</v>
       </c>
       <c r="Q64" s="101">
-        <f t="shared" ref="Q64:Q70" si="23">ROUND(E64/speed_cap,2)*10</f>
+        <f t="shared" ref="Q64:Q70" si="34">ROUND(E64/speed_cap,2)*10</f>
         <v>6</v>
       </c>
       <c r="R64" s="102">
-        <f t="shared" ref="R64:R70" si="24">ROUND(I64/DPS_cap,2)*10</f>
+        <f t="shared" ref="R64:R70" si="35">ROUND(I64/DPS_cap,2)*10</f>
         <v>0</v>
       </c>
       <c r="S64" s="103">
@@ -6630,11 +6725,11 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="136">
+      <c r="U64" s="120">
         <f>R64+O64+P64</f>
         <v>3.8</v>
       </c>
-      <c r="V64" s="136"/>
+      <c r="V64" s="120"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6662,56 +6757,56 @@
       <c r="E65" s="54">
         <v>4</v>
       </c>
-      <c r="F65" s="116" t="s">
+      <c r="F65" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="116"/>
+      <c r="G65" s="117"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="123">
-        <f t="shared" si="20"/>
+      <c r="J65" s="122">
+        <f t="shared" si="31"/>
         <v>32</v>
       </c>
-      <c r="K65" s="123"/>
+      <c r="K65" s="122"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
       </c>
       <c r="M65" s="54">
-        <f t="shared" ref="M65:M68" si="25">21-L65</f>
+        <f t="shared" ref="M65:M68" si="36">21-L65</f>
         <v>19</v>
       </c>
       <c r="N65" s="54"/>
       <c r="O65" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="P65" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>6.3</v>
       </c>
       <c r="Q65" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="R65" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="S65" s="70">
-        <f t="shared" ref="S65:S69" si="26">SUM(O65:R65)</f>
+        <f t="shared" ref="S65:S69" si="37">SUM(O65:R65)</f>
         <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="137">
-        <f t="shared" ref="U65:U70" si="27">R65+O65+P65</f>
+      <c r="U65" s="121">
+        <f t="shared" ref="U65:U70" si="38">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="137"/>
+      <c r="V65" s="121"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6739,56 +6834,56 @@
       <c r="E66" s="54">
         <v>3</v>
       </c>
-      <c r="F66" s="116" t="s">
+      <c r="F66" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="116"/>
+      <c r="G66" s="117"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="123">
-        <f t="shared" si="20"/>
+      <c r="J66" s="122">
+        <f t="shared" si="31"/>
         <v>28</v>
       </c>
-      <c r="K66" s="123"/>
+      <c r="K66" s="122"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
       </c>
       <c r="M66" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>17</v>
       </c>
       <c r="N66" s="54"/>
       <c r="O66" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>2.5</v>
       </c>
       <c r="P66" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="Q66" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>3</v>
       </c>
       <c r="R66" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="S66" s="70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="137">
-        <f t="shared" si="27"/>
+      <c r="U66" s="121">
+        <f t="shared" si="38"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="137"/>
+      <c r="V66" s="121"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6816,56 +6911,56 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="116" t="s">
+      <c r="F67" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="116"/>
+      <c r="G67" s="117"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="123">
-        <f t="shared" si="20"/>
+      <c r="J67" s="122">
+        <f t="shared" si="31"/>
         <v>48</v>
       </c>
-      <c r="K67" s="123"/>
+      <c r="K67" s="122"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
       </c>
       <c r="M67" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>21</v>
       </c>
       <c r="N67" s="54"/>
       <c r="O67" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>9.6</v>
       </c>
       <c r="P67" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>7</v>
       </c>
       <c r="Q67" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="R67" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="S67" s="70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="137">
-        <f t="shared" si="27"/>
+      <c r="U67" s="121">
+        <f t="shared" si="38"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="137"/>
+      <c r="V67" s="121"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6889,56 +6984,56 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="116" t="s">
+      <c r="F68" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="116"/>
+      <c r="G68" s="117"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="123">
-        <f t="shared" si="20"/>
+      <c r="J68" s="122">
+        <f t="shared" si="31"/>
         <v>72</v>
       </c>
-      <c r="K68" s="123"/>
+      <c r="K68" s="122"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
       </c>
       <c r="M68" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>21</v>
       </c>
       <c r="N68" s="54"/>
       <c r="O68" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>7.4</v>
       </c>
       <c r="P68" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>7</v>
       </c>
       <c r="Q68" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="R68" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>2.7</v>
       </c>
       <c r="S68" s="70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="137">
-        <f t="shared" si="27"/>
+      <c r="U68" s="121">
+        <f t="shared" si="38"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="137"/>
+      <c r="V68" s="121"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6962,21 +7057,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="116" t="s">
+      <c r="F69" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="116"/>
+      <c r="G69" s="117"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="123">
-        <f t="shared" si="20"/>
+      <c r="J69" s="122">
+        <f t="shared" si="31"/>
         <v>20</v>
       </c>
-      <c r="K69" s="123"/>
+      <c r="K69" s="122"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6987,31 +7082,31 @@
       </c>
       <c r="N69" s="54"/>
       <c r="O69" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="P69" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="Q69" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>10</v>
       </c>
       <c r="R69" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="S69" s="70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="137">
-        <f t="shared" si="27"/>
+      <c r="U69" s="121">
+        <f t="shared" si="38"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="137"/>
+      <c r="V69" s="121"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7035,21 +7130,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="116" t="s">
+      <c r="F70" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="116"/>
+      <c r="G70" s="117"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="123">
-        <f t="shared" ref="J70" si="28">(C70-player_radius)*2</f>
+      <c r="J70" s="122">
+        <f t="shared" ref="J70" si="39">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="123"/>
+      <c r="K70" s="122"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7060,31 +7155,31 @@
       </c>
       <c r="N70" s="54"/>
       <c r="O70" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="32"/>
         <v>2.5</v>
       </c>
       <c r="P70" s="67">
-        <f t="shared" si="22"/>
+        <f t="shared" si="33"/>
         <v>5.6999999999999993</v>
       </c>
       <c r="Q70" s="68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="34"/>
         <v>8</v>
       </c>
       <c r="R70" s="69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>9.6</v>
       </c>
       <c r="S70" s="70">
-        <f t="shared" ref="S70" si="29">SUM(O70:R70)</f>
+        <f t="shared" ref="S70" si="40">SUM(O70:R70)</f>
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="137">
-        <f t="shared" si="27"/>
+      <c r="U70" s="121">
+        <f t="shared" si="38"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="137"/>
+      <c r="V70" s="121"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7097,12 +7192,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="131" t="s">
+      <c r="O73" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="131"/>
-      <c r="Q73" s="131"/>
-      <c r="R73" s="131"/>
+      <c r="P73" s="124"/>
+      <c r="Q73" s="124"/>
+      <c r="R73" s="124"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7118,31 +7213,31 @@
       <c r="E74" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="122" t="s">
+      <c r="F74" s="123" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="122"/>
-      <c r="H74" s="122" t="s">
+      <c r="G74" s="123"/>
+      <c r="H74" s="123" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="122"/>
-      <c r="J74" s="122" t="s">
+      <c r="I74" s="123"/>
+      <c r="J74" s="123" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="122"/>
-      <c r="L74" s="122"/>
-      <c r="M74" s="122"/>
+      <c r="K74" s="123"/>
+      <c r="L74" s="123"/>
+      <c r="M74" s="123"/>
       <c r="N74" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="122" t="s">
+      <c r="O74" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="122"/>
-      <c r="Q74" s="122" t="s">
+      <c r="P74" s="123"/>
+      <c r="Q74" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="122"/>
+      <c r="R74" s="123"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="29">
@@ -7160,21 +7255,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="123" t="s">
+      <c r="F75" s="122" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="123"/>
-      <c r="H75" s="123">
+      <c r="G75" s="122"/>
+      <c r="H75" s="122">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="123"/>
-      <c r="J75" s="123" t="s">
+      <c r="I75" s="122"/>
+      <c r="J75" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="123"/>
-      <c r="L75" s="123"/>
-      <c r="M75" s="123"/>
+      <c r="K75" s="122"/>
+      <c r="L75" s="122"/>
+      <c r="M75" s="122"/>
       <c r="N75" s="78" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7203,21 +7298,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="123" t="s">
+      <c r="F76" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="123"/>
-      <c r="H76" s="123">
+      <c r="G76" s="122"/>
+      <c r="H76" s="122">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="123"/>
-      <c r="J76" s="123" t="s">
+      <c r="I76" s="122"/>
+      <c r="J76" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="123"/>
-      <c r="L76" s="123"/>
-      <c r="M76" s="123"/>
+      <c r="K76" s="122"/>
+      <c r="L76" s="122"/>
+      <c r="M76" s="122"/>
       <c r="N76" s="78" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7236,19 +7331,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="121"/>
-      <c r="G77" s="121"/>
-      <c r="H77" s="121"/>
-      <c r="I77" s="121"/>
-      <c r="J77" s="121"/>
-      <c r="K77" s="121"/>
-      <c r="L77" s="121"/>
-      <c r="M77" s="121"/>
+      <c r="F77" s="127"/>
+      <c r="G77" s="127"/>
+      <c r="H77" s="127"/>
+      <c r="I77" s="127"/>
+      <c r="J77" s="127"/>
+      <c r="K77" s="127"/>
+      <c r="L77" s="127"/>
+      <c r="M77" s="127"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="129"/>
-      <c r="P77" s="129"/>
-      <c r="Q77" s="129"/>
-      <c r="R77" s="129"/>
+      <c r="O77" s="125"/>
+      <c r="P77" s="125"/>
+      <c r="Q77" s="125"/>
+      <c r="R77" s="125"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7276,32 +7371,32 @@
       <c r="E81" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="122" t="s">
+      <c r="F81" s="123" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="122"/>
-      <c r="H81" s="122"/>
-      <c r="I81" s="122"/>
-      <c r="J81" s="122"/>
-      <c r="K81" s="122"/>
-      <c r="L81" s="122"/>
-      <c r="M81" s="122"/>
-      <c r="N81" s="122"/>
-      <c r="O81" s="122"/>
-      <c r="P81" s="122"/>
-      <c r="Q81" s="122" t="s">
+      <c r="G81" s="123"/>
+      <c r="H81" s="123"/>
+      <c r="I81" s="123"/>
+      <c r="J81" s="123"/>
+      <c r="K81" s="123"/>
+      <c r="L81" s="123"/>
+      <c r="M81" s="123"/>
+      <c r="N81" s="123"/>
+      <c r="O81" s="123"/>
+      <c r="P81" s="123"/>
+      <c r="Q81" s="123" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="122"/>
-      <c r="S81" s="122"/>
-      <c r="T81" s="122"/>
-      <c r="U81" s="122"/>
-      <c r="V81" s="122"/>
-      <c r="W81" s="122"/>
-      <c r="X81" s="122"/>
-      <c r="Y81" s="122"/>
-      <c r="Z81" s="122"/>
-      <c r="AA81" s="122"/>
+      <c r="R81" s="123"/>
+      <c r="S81" s="123"/>
+      <c r="T81" s="123"/>
+      <c r="U81" s="123"/>
+      <c r="V81" s="123"/>
+      <c r="W81" s="123"/>
+      <c r="X81" s="123"/>
+      <c r="Y81" s="123"/>
+      <c r="Z81" s="123"/>
+      <c r="AA81" s="123"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7317,32 +7412,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="135" t="s">
+      <c r="F82" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="135"/>
-      <c r="H82" s="135"/>
-      <c r="I82" s="135"/>
-      <c r="J82" s="135"/>
-      <c r="K82" s="135"/>
-      <c r="L82" s="135"/>
-      <c r="M82" s="135"/>
-      <c r="N82" s="135"/>
-      <c r="O82" s="135"/>
-      <c r="P82" s="135"/>
-      <c r="Q82" s="135" t="s">
+      <c r="G82" s="128"/>
+      <c r="H82" s="128"/>
+      <c r="I82" s="128"/>
+      <c r="J82" s="128"/>
+      <c r="K82" s="128"/>
+      <c r="L82" s="128"/>
+      <c r="M82" s="128"/>
+      <c r="N82" s="128"/>
+      <c r="O82" s="128"/>
+      <c r="P82" s="128"/>
+      <c r="Q82" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="135"/>
-      <c r="S82" s="135"/>
-      <c r="T82" s="135"/>
-      <c r="U82" s="135"/>
-      <c r="V82" s="135"/>
-      <c r="W82" s="135"/>
-      <c r="X82" s="135"/>
-      <c r="Y82" s="135"/>
-      <c r="Z82" s="135"/>
-      <c r="AA82" s="135"/>
+      <c r="R82" s="128"/>
+      <c r="S82" s="128"/>
+      <c r="T82" s="128"/>
+      <c r="U82" s="128"/>
+      <c r="V82" s="128"/>
+      <c r="W82" s="128"/>
+      <c r="X82" s="128"/>
+      <c r="Y82" s="128"/>
+      <c r="Z82" s="128"/>
+      <c r="AA82" s="128"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7532,24 +7627,24 @@
       <c r="B90" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="130" t="s">
+      <c r="C90" s="126" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="130"/>
-      <c r="E90" s="130"/>
-      <c r="F90" s="130"/>
-      <c r="G90" s="130"/>
-      <c r="H90" s="130" t="s">
+      <c r="D90" s="126"/>
+      <c r="E90" s="126"/>
+      <c r="F90" s="126"/>
+      <c r="G90" s="126"/>
+      <c r="H90" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="130"/>
-      <c r="J90" s="130"/>
-      <c r="K90" s="130"/>
-      <c r="L90" s="130"/>
-      <c r="M90" s="122" t="s">
+      <c r="I90" s="126"/>
+      <c r="J90" s="126"/>
+      <c r="K90" s="126"/>
+      <c r="L90" s="126"/>
+      <c r="M90" s="123" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="122"/>
+      <c r="N90" s="123"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>197</v>
@@ -7562,24 +7657,24 @@
       <c r="B91" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="117" t="s">
+      <c r="C91" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="117"/>
-      <c r="E91" s="117"/>
-      <c r="F91" s="117"/>
-      <c r="G91" s="117"/>
-      <c r="H91" s="117" t="s">
+      <c r="D91" s="116"/>
+      <c r="E91" s="116"/>
+      <c r="F91" s="116"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="117"/>
-      <c r="J91" s="117"/>
-      <c r="K91" s="117"/>
-      <c r="L91" s="117"/>
-      <c r="M91" s="116" t="s">
+      <c r="I91" s="116"/>
+      <c r="J91" s="116"/>
+      <c r="K91" s="116"/>
+      <c r="L91" s="116"/>
+      <c r="M91" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="116"/>
+      <c r="N91" s="117"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7589,24 +7684,24 @@
       <c r="B92" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="117" t="s">
+      <c r="C92" s="116" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="117"/>
-      <c r="E92" s="117"/>
-      <c r="F92" s="117"/>
-      <c r="G92" s="117"/>
-      <c r="H92" s="117" t="s">
+      <c r="D92" s="116"/>
+      <c r="E92" s="116"/>
+      <c r="F92" s="116"/>
+      <c r="G92" s="116"/>
+      <c r="H92" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="117"/>
-      <c r="J92" s="117"/>
-      <c r="K92" s="117"/>
-      <c r="L92" s="117"/>
-      <c r="M92" s="116" t="s">
+      <c r="I92" s="116"/>
+      <c r="J92" s="116"/>
+      <c r="K92" s="116"/>
+      <c r="L92" s="116"/>
+      <c r="M92" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="116"/>
+      <c r="N92" s="117"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7616,24 +7711,24 @@
       <c r="B93" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="117" t="s">
+      <c r="C93" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="117"/>
-      <c r="E93" s="117"/>
-      <c r="F93" s="117"/>
-      <c r="G93" s="117"/>
-      <c r="H93" s="117" t="s">
+      <c r="D93" s="116"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="116"/>
+      <c r="G93" s="116"/>
+      <c r="H93" s="116" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="117"/>
-      <c r="J93" s="117"/>
-      <c r="K93" s="117"/>
-      <c r="L93" s="117"/>
-      <c r="M93" s="116" t="s">
+      <c r="I93" s="116"/>
+      <c r="J93" s="116"/>
+      <c r="K93" s="116"/>
+      <c r="L93" s="116"/>
+      <c r="M93" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="116"/>
+      <c r="N93" s="117"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7643,24 +7738,24 @@
       <c r="B94" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="117" t="s">
+      <c r="C94" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="117"/>
-      <c r="E94" s="117"/>
-      <c r="F94" s="117"/>
-      <c r="G94" s="117"/>
-      <c r="H94" s="117" t="s">
+      <c r="D94" s="116"/>
+      <c r="E94" s="116"/>
+      <c r="F94" s="116"/>
+      <c r="G94" s="116"/>
+      <c r="H94" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="I94" s="117"/>
-      <c r="J94" s="117"/>
-      <c r="K94" s="117"/>
-      <c r="L94" s="117"/>
-      <c r="M94" s="116" t="s">
+      <c r="I94" s="116"/>
+      <c r="J94" s="116"/>
+      <c r="K94" s="116"/>
+      <c r="L94" s="116"/>
+      <c r="M94" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="116"/>
+      <c r="N94" s="117"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7670,24 +7765,24 @@
       <c r="B95" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C95" s="117" t="s">
+      <c r="C95" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="117"/>
-      <c r="E95" s="117"/>
-      <c r="F95" s="117"/>
-      <c r="G95" s="117"/>
-      <c r="H95" s="117" t="s">
+      <c r="D95" s="116"/>
+      <c r="E95" s="116"/>
+      <c r="F95" s="116"/>
+      <c r="G95" s="116"/>
+      <c r="H95" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="I95" s="117"/>
-      <c r="J95" s="117"/>
-      <c r="K95" s="117"/>
-      <c r="L95" s="117"/>
-      <c r="M95" s="116" t="s">
+      <c r="I95" s="116"/>
+      <c r="J95" s="116"/>
+      <c r="K95" s="116"/>
+      <c r="L95" s="116"/>
+      <c r="M95" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="116"/>
+      <c r="N95" s="117"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7697,24 +7792,24 @@
       <c r="B96" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="117" t="s">
+      <c r="C96" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="117"/>
-      <c r="E96" s="117"/>
-      <c r="F96" s="117"/>
-      <c r="G96" s="117"/>
-      <c r="H96" s="117" t="s">
+      <c r="D96" s="116"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="116"/>
+      <c r="G96" s="116"/>
+      <c r="H96" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="I96" s="117"/>
-      <c r="J96" s="117"/>
-      <c r="K96" s="117"/>
-      <c r="L96" s="117"/>
-      <c r="M96" s="116" t="s">
+      <c r="I96" s="116"/>
+      <c r="J96" s="116"/>
+      <c r="K96" s="116"/>
+      <c r="L96" s="116"/>
+      <c r="M96" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="116"/>
+      <c r="N96" s="117"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7724,24 +7819,24 @@
       <c r="B97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="117" t="s">
+      <c r="C97" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="117"/>
-      <c r="E97" s="117"/>
-      <c r="F97" s="117"/>
-      <c r="G97" s="117"/>
-      <c r="H97" s="117" t="s">
+      <c r="D97" s="116"/>
+      <c r="E97" s="116"/>
+      <c r="F97" s="116"/>
+      <c r="G97" s="116"/>
+      <c r="H97" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="I97" s="117"/>
-      <c r="J97" s="117"/>
-      <c r="K97" s="117"/>
-      <c r="L97" s="117"/>
-      <c r="M97" s="116" t="s">
+      <c r="I97" s="116"/>
+      <c r="J97" s="116"/>
+      <c r="K97" s="116"/>
+      <c r="L97" s="116"/>
+      <c r="M97" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="116"/>
+      <c r="N97" s="117"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7751,24 +7846,24 @@
       <c r="B98" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="117" t="s">
+      <c r="C98" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="117"/>
-      <c r="E98" s="117"/>
-      <c r="F98" s="117"/>
-      <c r="G98" s="117"/>
-      <c r="H98" s="117" t="s">
+      <c r="D98" s="116"/>
+      <c r="E98" s="116"/>
+      <c r="F98" s="116"/>
+      <c r="G98" s="116"/>
+      <c r="H98" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="I98" s="117"/>
-      <c r="J98" s="117"/>
-      <c r="K98" s="117"/>
-      <c r="L98" s="117"/>
-      <c r="M98" s="116" t="s">
+      <c r="I98" s="116"/>
+      <c r="J98" s="116"/>
+      <c r="K98" s="116"/>
+      <c r="L98" s="116"/>
+      <c r="M98" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="116"/>
+      <c r="N98" s="117"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7778,24 +7873,24 @@
       <c r="B99" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C99" s="117" t="s">
+      <c r="C99" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="117"/>
-      <c r="E99" s="117"/>
-      <c r="F99" s="117"/>
-      <c r="G99" s="117"/>
-      <c r="H99" s="117" t="s">
+      <c r="D99" s="116"/>
+      <c r="E99" s="116"/>
+      <c r="F99" s="116"/>
+      <c r="G99" s="116"/>
+      <c r="H99" s="116" t="s">
         <v>223</v>
       </c>
-      <c r="I99" s="117"/>
-      <c r="J99" s="117"/>
-      <c r="K99" s="117"/>
-      <c r="L99" s="117"/>
-      <c r="M99" s="116" t="s">
+      <c r="I99" s="116"/>
+      <c r="J99" s="116"/>
+      <c r="K99" s="116"/>
+      <c r="L99" s="116"/>
+      <c r="M99" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="116"/>
+      <c r="N99" s="117"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7805,411 +7900,396 @@
       <c r="B100" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C100" s="117" t="s">
+      <c r="C100" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="117"/>
-      <c r="E100" s="117"/>
-      <c r="F100" s="117"/>
-      <c r="G100" s="117"/>
-      <c r="H100" s="117" t="s">
+      <c r="D100" s="116"/>
+      <c r="E100" s="116"/>
+      <c r="F100" s="116"/>
+      <c r="G100" s="116"/>
+      <c r="H100" s="116" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="117"/>
-      <c r="J100" s="117"/>
-      <c r="K100" s="117"/>
-      <c r="L100" s="117"/>
-      <c r="M100" s="116" t="s">
+      <c r="I100" s="116"/>
+      <c r="J100" s="116"/>
+      <c r="K100" s="116"/>
+      <c r="L100" s="116"/>
+      <c r="M100" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="116"/>
+      <c r="N100" s="117"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="117"/>
-      <c r="D101" s="117"/>
-      <c r="E101" s="117"/>
-      <c r="F101" s="117"/>
-      <c r="G101" s="117"/>
-      <c r="H101" s="117"/>
-      <c r="I101" s="117"/>
-      <c r="J101" s="117"/>
-      <c r="K101" s="117"/>
-      <c r="L101" s="117"/>
-      <c r="M101" s="116"/>
-      <c r="N101" s="116"/>
+      <c r="C101" s="116"/>
+      <c r="D101" s="116"/>
+      <c r="E101" s="116"/>
+      <c r="F101" s="116"/>
+      <c r="G101" s="116"/>
+      <c r="H101" s="116"/>
+      <c r="I101" s="116"/>
+      <c r="J101" s="116"/>
+      <c r="K101" s="116"/>
+      <c r="L101" s="116"/>
+      <c r="M101" s="117"/>
+      <c r="N101" s="117"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="117"/>
-      <c r="I102" s="117"/>
-      <c r="J102" s="117"/>
-      <c r="K102" s="117"/>
-      <c r="L102" s="117"/>
-      <c r="M102" s="116"/>
-      <c r="N102" s="116"/>
+      <c r="H102" s="116"/>
+      <c r="I102" s="116"/>
+      <c r="J102" s="116"/>
+      <c r="K102" s="116"/>
+      <c r="L102" s="116"/>
+      <c r="M102" s="117"/>
+      <c r="N102" s="117"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="117"/>
-      <c r="D103" s="117"/>
-      <c r="E103" s="117"/>
-      <c r="F103" s="117"/>
-      <c r="G103" s="117"/>
-      <c r="H103" s="117"/>
-      <c r="I103" s="117"/>
-      <c r="J103" s="117"/>
-      <c r="K103" s="117"/>
-      <c r="L103" s="117"/>
-      <c r="M103" s="116"/>
-      <c r="N103" s="116"/>
+      <c r="C103" s="116"/>
+      <c r="D103" s="116"/>
+      <c r="E103" s="116"/>
+      <c r="F103" s="116"/>
+      <c r="G103" s="116"/>
+      <c r="H103" s="116"/>
+      <c r="I103" s="116"/>
+      <c r="J103" s="116"/>
+      <c r="K103" s="116"/>
+      <c r="L103" s="116"/>
+      <c r="M103" s="117"/>
+      <c r="N103" s="117"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="117"/>
-      <c r="D104" s="117"/>
-      <c r="E104" s="117"/>
-      <c r="F104" s="117"/>
-      <c r="G104" s="117"/>
-      <c r="H104" s="117"/>
-      <c r="I104" s="117"/>
-      <c r="J104" s="117"/>
-      <c r="K104" s="117"/>
-      <c r="L104" s="117"/>
-      <c r="M104" s="116"/>
-      <c r="N104" s="116"/>
+      <c r="C104" s="116"/>
+      <c r="D104" s="116"/>
+      <c r="E104" s="116"/>
+      <c r="F104" s="116"/>
+      <c r="G104" s="116"/>
+      <c r="H104" s="116"/>
+      <c r="I104" s="116"/>
+      <c r="J104" s="116"/>
+      <c r="K104" s="116"/>
+      <c r="L104" s="116"/>
+      <c r="M104" s="117"/>
+      <c r="N104" s="117"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="117"/>
-      <c r="D105" s="117"/>
-      <c r="E105" s="117"/>
-      <c r="F105" s="117"/>
-      <c r="G105" s="117"/>
-      <c r="H105" s="117"/>
-      <c r="I105" s="117"/>
-      <c r="J105" s="117"/>
-      <c r="K105" s="117"/>
-      <c r="L105" s="117"/>
-      <c r="M105" s="116"/>
-      <c r="N105" s="116"/>
+      <c r="C105" s="116"/>
+      <c r="D105" s="116"/>
+      <c r="E105" s="116"/>
+      <c r="F105" s="116"/>
+      <c r="G105" s="116"/>
+      <c r="H105" s="116"/>
+      <c r="I105" s="116"/>
+      <c r="J105" s="116"/>
+      <c r="K105" s="116"/>
+      <c r="L105" s="116"/>
+      <c r="M105" s="117"/>
+      <c r="N105" s="117"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="117"/>
-      <c r="D106" s="117"/>
-      <c r="E106" s="117"/>
-      <c r="F106" s="117"/>
-      <c r="G106" s="117"/>
-      <c r="H106" s="117"/>
-      <c r="I106" s="117"/>
-      <c r="J106" s="117"/>
-      <c r="K106" s="117"/>
-      <c r="L106" s="117"/>
-      <c r="M106" s="116"/>
-      <c r="N106" s="116"/>
+      <c r="C106" s="116"/>
+      <c r="D106" s="116"/>
+      <c r="E106" s="116"/>
+      <c r="F106" s="116"/>
+      <c r="G106" s="116"/>
+      <c r="H106" s="116"/>
+      <c r="I106" s="116"/>
+      <c r="J106" s="116"/>
+      <c r="K106" s="116"/>
+      <c r="L106" s="116"/>
+      <c r="M106" s="117"/>
+      <c r="N106" s="117"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="117"/>
-      <c r="D107" s="117"/>
-      <c r="E107" s="117"/>
-      <c r="F107" s="117"/>
-      <c r="G107" s="117"/>
-      <c r="H107" s="117"/>
-      <c r="I107" s="117"/>
-      <c r="J107" s="117"/>
-      <c r="K107" s="117"/>
-      <c r="L107" s="117"/>
-      <c r="M107" s="116"/>
-      <c r="N107" s="116"/>
+      <c r="C107" s="116"/>
+      <c r="D107" s="116"/>
+      <c r="E107" s="116"/>
+      <c r="F107" s="116"/>
+      <c r="G107" s="116"/>
+      <c r="H107" s="116"/>
+      <c r="I107" s="116"/>
+      <c r="J107" s="116"/>
+      <c r="K107" s="116"/>
+      <c r="L107" s="116"/>
+      <c r="M107" s="117"/>
+      <c r="N107" s="117"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="117"/>
-      <c r="D108" s="117"/>
-      <c r="E108" s="117"/>
-      <c r="F108" s="117"/>
-      <c r="G108" s="117"/>
-      <c r="H108" s="117"/>
-      <c r="I108" s="117"/>
-      <c r="J108" s="117"/>
-      <c r="K108" s="117"/>
-      <c r="L108" s="117"/>
-      <c r="M108" s="116"/>
-      <c r="N108" s="116"/>
+      <c r="C108" s="116"/>
+      <c r="D108" s="116"/>
+      <c r="E108" s="116"/>
+      <c r="F108" s="116"/>
+      <c r="G108" s="116"/>
+      <c r="H108" s="116"/>
+      <c r="I108" s="116"/>
+      <c r="J108" s="116"/>
+      <c r="K108" s="116"/>
+      <c r="L108" s="116"/>
+      <c r="M108" s="117"/>
+      <c r="N108" s="117"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="117"/>
-      <c r="D109" s="117"/>
-      <c r="E109" s="117"/>
-      <c r="F109" s="117"/>
-      <c r="G109" s="117"/>
-      <c r="H109" s="117"/>
-      <c r="I109" s="117"/>
-      <c r="J109" s="117"/>
-      <c r="K109" s="117"/>
-      <c r="L109" s="117"/>
-      <c r="M109" s="116"/>
-      <c r="N109" s="116"/>
+      <c r="C109" s="116"/>
+      <c r="D109" s="116"/>
+      <c r="E109" s="116"/>
+      <c r="F109" s="116"/>
+      <c r="G109" s="116"/>
+      <c r="H109" s="116"/>
+      <c r="I109" s="116"/>
+      <c r="J109" s="116"/>
+      <c r="K109" s="116"/>
+      <c r="L109" s="116"/>
+      <c r="M109" s="117"/>
+      <c r="N109" s="117"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="117"/>
-      <c r="D110" s="117"/>
-      <c r="E110" s="117"/>
-      <c r="F110" s="117"/>
-      <c r="G110" s="117"/>
-      <c r="H110" s="117"/>
-      <c r="I110" s="117"/>
-      <c r="J110" s="117"/>
-      <c r="K110" s="117"/>
-      <c r="L110" s="117"/>
-      <c r="M110" s="116"/>
-      <c r="N110" s="116"/>
+      <c r="C110" s="116"/>
+      <c r="D110" s="116"/>
+      <c r="E110" s="116"/>
+      <c r="F110" s="116"/>
+      <c r="G110" s="116"/>
+      <c r="H110" s="116"/>
+      <c r="I110" s="116"/>
+      <c r="J110" s="116"/>
+      <c r="K110" s="116"/>
+      <c r="L110" s="116"/>
+      <c r="M110" s="117"/>
+      <c r="N110" s="117"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="117"/>
-      <c r="D111" s="117"/>
-      <c r="E111" s="117"/>
-      <c r="F111" s="117"/>
-      <c r="G111" s="117"/>
-      <c r="H111" s="117"/>
-      <c r="I111" s="117"/>
-      <c r="J111" s="117"/>
-      <c r="K111" s="117"/>
-      <c r="L111" s="117"/>
-      <c r="M111" s="116"/>
-      <c r="N111" s="116"/>
+      <c r="C111" s="116"/>
+      <c r="D111" s="116"/>
+      <c r="E111" s="116"/>
+      <c r="F111" s="116"/>
+      <c r="G111" s="116"/>
+      <c r="H111" s="116"/>
+      <c r="I111" s="116"/>
+      <c r="J111" s="116"/>
+      <c r="K111" s="116"/>
+      <c r="L111" s="116"/>
+      <c r="M111" s="117"/>
+      <c r="N111" s="117"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="117"/>
-      <c r="D112" s="117"/>
-      <c r="E112" s="117"/>
-      <c r="F112" s="117"/>
-      <c r="G112" s="117"/>
-      <c r="H112" s="117"/>
-      <c r="I112" s="117"/>
-      <c r="J112" s="117"/>
-      <c r="K112" s="117"/>
-      <c r="L112" s="117"/>
-      <c r="M112" s="116"/>
-      <c r="N112" s="116"/>
+      <c r="C112" s="116"/>
+      <c r="D112" s="116"/>
+      <c r="E112" s="116"/>
+      <c r="F112" s="116"/>
+      <c r="G112" s="116"/>
+      <c r="H112" s="116"/>
+      <c r="I112" s="116"/>
+      <c r="J112" s="116"/>
+      <c r="K112" s="116"/>
+      <c r="L112" s="116"/>
+      <c r="M112" s="117"/>
+      <c r="N112" s="117"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="117"/>
-      <c r="D113" s="117"/>
-      <c r="E113" s="117"/>
-      <c r="F113" s="117"/>
-      <c r="G113" s="117"/>
-      <c r="H113" s="117"/>
-      <c r="I113" s="117"/>
-      <c r="J113" s="117"/>
-      <c r="K113" s="117"/>
-      <c r="L113" s="117"/>
-      <c r="M113" s="116"/>
-      <c r="N113" s="116"/>
+      <c r="C113" s="116"/>
+      <c r="D113" s="116"/>
+      <c r="E113" s="116"/>
+      <c r="F113" s="116"/>
+      <c r="G113" s="116"/>
+      <c r="H113" s="116"/>
+      <c r="I113" s="116"/>
+      <c r="J113" s="116"/>
+      <c r="K113" s="116"/>
+      <c r="L113" s="116"/>
+      <c r="M113" s="117"/>
+      <c r="N113" s="117"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="117"/>
-      <c r="D114" s="117"/>
-      <c r="E114" s="117"/>
-      <c r="F114" s="117"/>
-      <c r="G114" s="117"/>
-      <c r="H114" s="117"/>
-      <c r="I114" s="117"/>
-      <c r="J114" s="117"/>
-      <c r="K114" s="117"/>
-      <c r="L114" s="117"/>
-      <c r="M114" s="116"/>
-      <c r="N114" s="116"/>
+      <c r="C114" s="116"/>
+      <c r="D114" s="116"/>
+      <c r="E114" s="116"/>
+      <c r="F114" s="116"/>
+      <c r="G114" s="116"/>
+      <c r="H114" s="116"/>
+      <c r="I114" s="116"/>
+      <c r="J114" s="116"/>
+      <c r="K114" s="116"/>
+      <c r="L114" s="116"/>
+      <c r="M114" s="117"/>
+      <c r="N114" s="117"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="117"/>
-      <c r="D115" s="117"/>
-      <c r="E115" s="117"/>
-      <c r="F115" s="117"/>
-      <c r="G115" s="117"/>
-      <c r="H115" s="117"/>
-      <c r="I115" s="117"/>
-      <c r="J115" s="117"/>
-      <c r="K115" s="117"/>
-      <c r="L115" s="117"/>
-      <c r="M115" s="116"/>
-      <c r="N115" s="116"/>
+      <c r="C115" s="116"/>
+      <c r="D115" s="116"/>
+      <c r="E115" s="116"/>
+      <c r="F115" s="116"/>
+      <c r="G115" s="116"/>
+      <c r="H115" s="116"/>
+      <c r="I115" s="116"/>
+      <c r="J115" s="116"/>
+      <c r="K115" s="116"/>
+      <c r="L115" s="116"/>
+      <c r="M115" s="117"/>
+      <c r="N115" s="117"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="117"/>
-      <c r="D116" s="117"/>
-      <c r="E116" s="117"/>
-      <c r="F116" s="117"/>
-      <c r="G116" s="117"/>
-      <c r="H116" s="117"/>
-      <c r="I116" s="117"/>
-      <c r="J116" s="117"/>
-      <c r="K116" s="117"/>
-      <c r="L116" s="117"/>
-      <c r="M116" s="116"/>
-      <c r="N116" s="116"/>
+      <c r="C116" s="116"/>
+      <c r="D116" s="116"/>
+      <c r="E116" s="116"/>
+      <c r="F116" s="116"/>
+      <c r="G116" s="116"/>
+      <c r="H116" s="116"/>
+      <c r="I116" s="116"/>
+      <c r="J116" s="116"/>
+      <c r="K116" s="116"/>
+      <c r="L116" s="116"/>
+      <c r="M116" s="117"/>
+      <c r="N116" s="117"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="117"/>
-      <c r="D117" s="117"/>
-      <c r="E117" s="117"/>
-      <c r="F117" s="117"/>
-      <c r="G117" s="117"/>
-      <c r="H117" s="117"/>
-      <c r="I117" s="117"/>
-      <c r="J117" s="117"/>
-      <c r="K117" s="117"/>
-      <c r="L117" s="117"/>
-      <c r="M117" s="116"/>
-      <c r="N117" s="116"/>
+      <c r="C117" s="116"/>
+      <c r="D117" s="116"/>
+      <c r="E117" s="116"/>
+      <c r="F117" s="116"/>
+      <c r="G117" s="116"/>
+      <c r="H117" s="116"/>
+      <c r="I117" s="116"/>
+      <c r="J117" s="116"/>
+      <c r="K117" s="116"/>
+      <c r="L117" s="116"/>
+      <c r="M117" s="117"/>
+      <c r="N117" s="117"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="117"/>
-      <c r="D118" s="117"/>
-      <c r="E118" s="117"/>
-      <c r="F118" s="117"/>
-      <c r="G118" s="117"/>
-      <c r="H118" s="117"/>
-      <c r="I118" s="117"/>
-      <c r="J118" s="117"/>
-      <c r="K118" s="117"/>
-      <c r="L118" s="117"/>
-      <c r="M118" s="116"/>
-      <c r="N118" s="116"/>
+      <c r="C118" s="116"/>
+      <c r="D118" s="116"/>
+      <c r="E118" s="116"/>
+      <c r="F118" s="116"/>
+      <c r="G118" s="116"/>
+      <c r="H118" s="116"/>
+      <c r="I118" s="116"/>
+      <c r="J118" s="116"/>
+      <c r="K118" s="116"/>
+      <c r="L118" s="116"/>
+      <c r="M118" s="117"/>
+      <c r="N118" s="117"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="H54:M54"/>
+    <mergeCell ref="H58:M58"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
     <mergeCell ref="C92:G92"/>
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="Q77:R77"/>
@@ -8234,73 +8314,88 @@
     <mergeCell ref="M93:N93"/>
     <mergeCell ref="Q81:AA81"/>
     <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="H54:M54"/>
-    <mergeCell ref="H58:M58"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deagle sound effect added
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B56ECE-D4A9-4C0B-9865-F771A5DDABA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFB0ED7-6E21-4724-AD85-7FF2E3061D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="14243" windowHeight="12112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2370,69 +2370,69 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3587,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3606,10 +3606,10 @@
       <c r="B1" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="132"/>
+      <c r="D1" s="126"/>
       <c r="G1" s="56" t="s">
         <v>159</v>
       </c>
@@ -3705,10 +3705,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="124" t="s">
+      <c r="Z2" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="124"/>
+      <c r="AA2" s="131"/>
       <c r="AG2" s="43" t="s">
         <v>84</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="19">
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="H21" s="19">
         <v>18</v>
@@ -5107,7 +5107,7 @@
         <v>7</v>
       </c>
       <c r="J21" s="19">
-        <v>2300</v>
+        <v>3300</v>
       </c>
       <c r="K21" s="19">
         <v>7</v>
@@ -5115,11 +5115,11 @@
       <c r="L21" s="19"/>
       <c r="M21" s="19">
         <f t="shared" si="14"/>
-        <v>6.67</v>
+        <v>8.57</v>
       </c>
       <c r="N21" s="19">
         <f t="shared" ref="N21" si="23">ROUND(E21*F21/(G21+J21/I21)*1000,2)</f>
-        <v>3.85</v>
+        <v>3.65</v>
       </c>
       <c r="O21" s="19">
         <f t="shared" si="15"/>
@@ -6110,28 +6110,28 @@
       <c r="B40" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="130" t="s">
+      <c r="C40" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="130"/>
-      <c r="E40" s="130"/>
-      <c r="F40" s="130"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="130"/>
-      <c r="I40" s="130" t="s">
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="130"/>
-      <c r="K40" s="130"/>
-      <c r="L40" s="130"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="129" t="s">
+      <c r="S40" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="129"/>
+      <c r="T40" s="132"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6141,30 +6141,30 @@
       <c r="B41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="131" t="s">
+      <c r="C41" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="131"/>
-      <c r="E41" s="131"/>
-      <c r="F41" s="131" t="s">
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="131"/>
-      <c r="H41" s="131"/>
-      <c r="I41" s="131" t="s">
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="131"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="131"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="129" t="s">
+      <c r="S41" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="129"/>
+      <c r="T41" s="132"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -6177,30 +6177,30 @@
       <c r="B42" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="131" t="s">
+      <c r="C42" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131"/>
-      <c r="F42" s="131" t="s">
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="131"/>
-      <c r="H42" s="131"/>
-      <c r="I42" s="131" t="s">
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="131"/>
-      <c r="K42" s="131"/>
-      <c r="L42" s="131"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="129" t="s">
+      <c r="S42" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="129"/>
+      <c r="T42" s="132"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6213,30 +6213,30 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="127" t="s">
+      <c r="C43" s="121" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="127"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127" t="s">
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="127"/>
-      <c r="H43" s="127"/>
-      <c r="I43" s="127" t="s">
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="I43" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="127"/>
-      <c r="K43" s="127"/>
-      <c r="L43" s="127"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="121"/>
+      <c r="L43" s="121"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="129" t="s">
+      <c r="S43" s="132" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="129"/>
+      <c r="T43" s="132"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6251,20 +6251,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="127" t="s">
+      <c r="C44" s="121" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="127"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="127" t="s">
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="121" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="127"/>
-      <c r="K44" s="127"/>
-      <c r="L44" s="127"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="121"/>
+      <c r="L44" s="121"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6280,16 +6280,16 @@
       <c r="B47" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="130" t="s">
+      <c r="C47" s="119" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="130"/>
-      <c r="E47" s="130" t="s">
+      <c r="D47" s="119"/>
+      <c r="E47" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="130"/>
-      <c r="G47" s="130"/>
-      <c r="H47" s="130"/>
+      <c r="F47" s="119"/>
+      <c r="G47" s="119"/>
+      <c r="H47" s="119"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -6300,16 +6300,16 @@
       <c r="B48" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="131">
+      <c r="C48" s="120">
         <v>2</v>
       </c>
-      <c r="D48" s="131"/>
-      <c r="E48" s="131" t="s">
+      <c r="D48" s="120"/>
+      <c r="E48" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
@@ -6320,28 +6320,28 @@
       <c r="B49" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="131" t="s">
+      <c r="C49" s="120" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="131"/>
-      <c r="E49" s="131" t="s">
+      <c r="D49" s="120"/>
+      <c r="E49" s="120" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="131"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="120"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="127"/>
-      <c r="D50" s="127"/>
-      <c r="E50" s="127"/>
-      <c r="F50" s="127"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="127"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="121"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6359,14 +6359,14 @@
       <c r="D54" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="136" t="s">
+      <c r="H54" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="136"/>
-      <c r="J54" s="136"/>
-      <c r="K54" s="136"/>
-      <c r="L54" s="136"/>
-      <c r="M54" s="136"/>
+      <c r="I54" s="124"/>
+      <c r="J54" s="124"/>
+      <c r="K54" s="124"/>
+      <c r="L54" s="124"/>
+      <c r="M54" s="124"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6517,14 +6517,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="137" t="s">
+      <c r="H58" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="137"/>
-      <c r="J58" s="137"/>
-      <c r="K58" s="137"/>
-      <c r="L58" s="137"/>
-      <c r="M58" s="137"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="125"/>
+      <c r="L58" s="125"/>
+      <c r="M58" s="125"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6573,10 +6573,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="134" t="s">
+      <c r="J62" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="134"/>
+      <c r="K62" s="128"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -6584,13 +6584,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="133" t="s">
+      <c r="O62" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="133"/>
-      <c r="Q62" s="133"/>
-      <c r="R62" s="133"/>
-      <c r="S62" s="133"/>
+      <c r="P62" s="127"/>
+      <c r="Q62" s="127"/>
+      <c r="R62" s="127"/>
+      <c r="S62" s="127"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6612,20 +6612,20 @@
       <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="119" t="s">
+      <c r="F63" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="119"/>
+      <c r="G63" s="133"/>
       <c r="H63" s="86" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="119" t="s">
+      <c r="J63" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="119"/>
+      <c r="K63" s="133"/>
       <c r="L63" s="86" t="s">
         <v>102</v>
       </c>
@@ -6649,10 +6649,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="119" t="s">
+      <c r="U63" s="133" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="119"/>
+      <c r="V63" s="133"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6680,21 +6680,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="135" t="s">
+      <c r="F64" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="135"/>
+      <c r="G64" s="134"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="122">
+      <c r="J64" s="123">
         <f t="shared" ref="J64:J69" si="31">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="122"/>
+      <c r="K64" s="123"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -6725,11 +6725,11 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="120">
+      <c r="U64" s="136">
         <f>R64+O64+P64</f>
         <v>3.8</v>
       </c>
-      <c r="V64" s="120"/>
+      <c r="V64" s="136"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6757,21 +6757,21 @@
       <c r="E65" s="54">
         <v>4</v>
       </c>
-      <c r="F65" s="117" t="s">
+      <c r="F65" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="117"/>
+      <c r="G65" s="116"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="122">
+      <c r="J65" s="123">
         <f t="shared" si="31"/>
         <v>32</v>
       </c>
-      <c r="K65" s="122"/>
+      <c r="K65" s="123"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6802,11 +6802,11 @@
         <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="121">
+      <c r="U65" s="137">
         <f t="shared" ref="U65:U70" si="38">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="121"/>
+      <c r="V65" s="137"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6834,21 +6834,21 @@
       <c r="E66" s="54">
         <v>3</v>
       </c>
-      <c r="F66" s="117" t="s">
+      <c r="F66" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="117"/>
+      <c r="G66" s="116"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="122">
+      <c r="J66" s="123">
         <f t="shared" si="31"/>
         <v>28</v>
       </c>
-      <c r="K66" s="122"/>
+      <c r="K66" s="123"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6879,11 +6879,11 @@
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="121">
+      <c r="U66" s="137">
         <f t="shared" si="38"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="121"/>
+      <c r="V66" s="137"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6911,21 +6911,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="117" t="s">
+      <c r="F67" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="117"/>
+      <c r="G67" s="116"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="122">
+      <c r="J67" s="123">
         <f t="shared" si="31"/>
         <v>48</v>
       </c>
-      <c r="K67" s="122"/>
+      <c r="K67" s="123"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6956,11 +6956,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="121">
+      <c r="U67" s="137">
         <f t="shared" si="38"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="121"/>
+      <c r="V67" s="137"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6984,21 +6984,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="117" t="s">
+      <c r="F68" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="117"/>
+      <c r="G68" s="116"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="122">
+      <c r="J68" s="123">
         <f t="shared" si="31"/>
         <v>72</v>
       </c>
-      <c r="K68" s="122"/>
+      <c r="K68" s="123"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7029,11 +7029,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="121">
+      <c r="U68" s="137">
         <f t="shared" si="38"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="121"/>
+      <c r="V68" s="137"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7057,21 +7057,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="117" t="s">
+      <c r="F69" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="117"/>
+      <c r="G69" s="116"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="122">
+      <c r="J69" s="123">
         <f t="shared" si="31"/>
         <v>20</v>
       </c>
-      <c r="K69" s="122"/>
+      <c r="K69" s="123"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7102,11 +7102,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="121">
+      <c r="U69" s="137">
         <f t="shared" si="38"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="121"/>
+      <c r="V69" s="137"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7130,21 +7130,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="117"/>
+      <c r="G70" s="116"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="122">
+      <c r="J70" s="123">
         <f t="shared" ref="J70" si="39">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="122"/>
+      <c r="K70" s="123"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7175,11 +7175,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="121">
+      <c r="U70" s="137">
         <f t="shared" si="38"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="121"/>
+      <c r="V70" s="137"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7192,12 +7192,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="124" t="s">
+      <c r="O73" s="131" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="124"/>
-      <c r="Q73" s="124"/>
-      <c r="R73" s="124"/>
+      <c r="P73" s="131"/>
+      <c r="Q73" s="131"/>
+      <c r="R73" s="131"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7213,31 +7213,31 @@
       <c r="E74" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="123" t="s">
+      <c r="F74" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="123"/>
-      <c r="H74" s="123" t="s">
+      <c r="G74" s="122"/>
+      <c r="H74" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="123"/>
-      <c r="J74" s="123" t="s">
+      <c r="I74" s="122"/>
+      <c r="J74" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="123"/>
-      <c r="L74" s="123"/>
-      <c r="M74" s="123"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="122"/>
+      <c r="M74" s="122"/>
       <c r="N74" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="123" t="s">
+      <c r="O74" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="123"/>
-      <c r="Q74" s="123" t="s">
+      <c r="P74" s="122"/>
+      <c r="Q74" s="122" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="123"/>
+      <c r="R74" s="122"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="29">
@@ -7255,21 +7255,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="122" t="s">
+      <c r="F75" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122">
+      <c r="G75" s="123"/>
+      <c r="H75" s="123">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="122"/>
-      <c r="J75" s="122" t="s">
+      <c r="I75" s="123"/>
+      <c r="J75" s="123" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="122"/>
-      <c r="L75" s="122"/>
-      <c r="M75" s="122"/>
+      <c r="K75" s="123"/>
+      <c r="L75" s="123"/>
+      <c r="M75" s="123"/>
       <c r="N75" s="78" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7298,21 +7298,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="122" t="s">
+      <c r="F76" s="123" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="122"/>
-      <c r="H76" s="122">
+      <c r="G76" s="123"/>
+      <c r="H76" s="123">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="122"/>
-      <c r="J76" s="122" t="s">
+      <c r="I76" s="123"/>
+      <c r="J76" s="123" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="122"/>
-      <c r="L76" s="122"/>
-      <c r="M76" s="122"/>
+      <c r="K76" s="123"/>
+      <c r="L76" s="123"/>
+      <c r="M76" s="123"/>
       <c r="N76" s="78" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7331,19 +7331,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="127"/>
-      <c r="G77" s="127"/>
-      <c r="H77" s="127"/>
-      <c r="I77" s="127"/>
-      <c r="J77" s="127"/>
-      <c r="K77" s="127"/>
-      <c r="L77" s="127"/>
-      <c r="M77" s="127"/>
+      <c r="F77" s="121"/>
+      <c r="G77" s="121"/>
+      <c r="H77" s="121"/>
+      <c r="I77" s="121"/>
+      <c r="J77" s="121"/>
+      <c r="K77" s="121"/>
+      <c r="L77" s="121"/>
+      <c r="M77" s="121"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="125"/>
-      <c r="P77" s="125"/>
-      <c r="Q77" s="125"/>
-      <c r="R77" s="125"/>
+      <c r="O77" s="129"/>
+      <c r="P77" s="129"/>
+      <c r="Q77" s="129"/>
+      <c r="R77" s="129"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7371,32 +7371,32 @@
       <c r="E81" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="123" t="s">
+      <c r="F81" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="123"/>
-      <c r="H81" s="123"/>
-      <c r="I81" s="123"/>
-      <c r="J81" s="123"/>
-      <c r="K81" s="123"/>
-      <c r="L81" s="123"/>
-      <c r="M81" s="123"/>
-      <c r="N81" s="123"/>
-      <c r="O81" s="123"/>
-      <c r="P81" s="123"/>
-      <c r="Q81" s="123" t="s">
+      <c r="G81" s="122"/>
+      <c r="H81" s="122"/>
+      <c r="I81" s="122"/>
+      <c r="J81" s="122"/>
+      <c r="K81" s="122"/>
+      <c r="L81" s="122"/>
+      <c r="M81" s="122"/>
+      <c r="N81" s="122"/>
+      <c r="O81" s="122"/>
+      <c r="P81" s="122"/>
+      <c r="Q81" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="123"/>
-      <c r="S81" s="123"/>
-      <c r="T81" s="123"/>
-      <c r="U81" s="123"/>
-      <c r="V81" s="123"/>
-      <c r="W81" s="123"/>
-      <c r="X81" s="123"/>
-      <c r="Y81" s="123"/>
-      <c r="Z81" s="123"/>
-      <c r="AA81" s="123"/>
+      <c r="R81" s="122"/>
+      <c r="S81" s="122"/>
+      <c r="T81" s="122"/>
+      <c r="U81" s="122"/>
+      <c r="V81" s="122"/>
+      <c r="W81" s="122"/>
+      <c r="X81" s="122"/>
+      <c r="Y81" s="122"/>
+      <c r="Z81" s="122"/>
+      <c r="AA81" s="122"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7412,32 +7412,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="128" t="s">
+      <c r="F82" s="135" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="128"/>
-      <c r="H82" s="128"/>
-      <c r="I82" s="128"/>
-      <c r="J82" s="128"/>
-      <c r="K82" s="128"/>
-      <c r="L82" s="128"/>
-      <c r="M82" s="128"/>
-      <c r="N82" s="128"/>
-      <c r="O82" s="128"/>
-      <c r="P82" s="128"/>
-      <c r="Q82" s="128" t="s">
+      <c r="G82" s="135"/>
+      <c r="H82" s="135"/>
+      <c r="I82" s="135"/>
+      <c r="J82" s="135"/>
+      <c r="K82" s="135"/>
+      <c r="L82" s="135"/>
+      <c r="M82" s="135"/>
+      <c r="N82" s="135"/>
+      <c r="O82" s="135"/>
+      <c r="P82" s="135"/>
+      <c r="Q82" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="128"/>
-      <c r="S82" s="128"/>
-      <c r="T82" s="128"/>
-      <c r="U82" s="128"/>
-      <c r="V82" s="128"/>
-      <c r="W82" s="128"/>
-      <c r="X82" s="128"/>
-      <c r="Y82" s="128"/>
-      <c r="Z82" s="128"/>
-      <c r="AA82" s="128"/>
+      <c r="R82" s="135"/>
+      <c r="S82" s="135"/>
+      <c r="T82" s="135"/>
+      <c r="U82" s="135"/>
+      <c r="V82" s="135"/>
+      <c r="W82" s="135"/>
+      <c r="X82" s="135"/>
+      <c r="Y82" s="135"/>
+      <c r="Z82" s="135"/>
+      <c r="AA82" s="135"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7627,24 +7627,24 @@
       <c r="B90" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="126" t="s">
+      <c r="C90" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="126"/>
-      <c r="E90" s="126"/>
-      <c r="F90" s="126"/>
-      <c r="G90" s="126"/>
-      <c r="H90" s="126" t="s">
+      <c r="D90" s="130"/>
+      <c r="E90" s="130"/>
+      <c r="F90" s="130"/>
+      <c r="G90" s="130"/>
+      <c r="H90" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="126"/>
-      <c r="J90" s="126"/>
-      <c r="K90" s="126"/>
-      <c r="L90" s="126"/>
-      <c r="M90" s="123" t="s">
+      <c r="I90" s="130"/>
+      <c r="J90" s="130"/>
+      <c r="K90" s="130"/>
+      <c r="L90" s="130"/>
+      <c r="M90" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="123"/>
+      <c r="N90" s="122"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>197</v>
@@ -7657,24 +7657,24 @@
       <c r="B91" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="116" t="s">
+      <c r="C91" s="117" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="116"/>
-      <c r="E91" s="116"/>
-      <c r="F91" s="116"/>
-      <c r="G91" s="116"/>
-      <c r="H91" s="116" t="s">
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="117"/>
+      <c r="G91" s="117"/>
+      <c r="H91" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="116"/>
-      <c r="J91" s="116"/>
-      <c r="K91" s="116"/>
-      <c r="L91" s="116"/>
-      <c r="M91" s="117" t="s">
+      <c r="I91" s="117"/>
+      <c r="J91" s="117"/>
+      <c r="K91" s="117"/>
+      <c r="L91" s="117"/>
+      <c r="M91" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="117"/>
+      <c r="N91" s="116"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7684,24 +7684,24 @@
       <c r="B92" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="116" t="s">
+      <c r="C92" s="117" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="116"/>
-      <c r="E92" s="116"/>
-      <c r="F92" s="116"/>
-      <c r="G92" s="116"/>
-      <c r="H92" s="116" t="s">
+      <c r="D92" s="117"/>
+      <c r="E92" s="117"/>
+      <c r="F92" s="117"/>
+      <c r="G92" s="117"/>
+      <c r="H92" s="117" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="116"/>
-      <c r="J92" s="116"/>
-      <c r="K92" s="116"/>
-      <c r="L92" s="116"/>
-      <c r="M92" s="117" t="s">
+      <c r="I92" s="117"/>
+      <c r="J92" s="117"/>
+      <c r="K92" s="117"/>
+      <c r="L92" s="117"/>
+      <c r="M92" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="117"/>
+      <c r="N92" s="116"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7711,24 +7711,24 @@
       <c r="B93" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="116" t="s">
+      <c r="C93" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="116"/>
-      <c r="E93" s="116"/>
-      <c r="F93" s="116"/>
-      <c r="G93" s="116"/>
-      <c r="H93" s="116" t="s">
+      <c r="D93" s="117"/>
+      <c r="E93" s="117"/>
+      <c r="F93" s="117"/>
+      <c r="G93" s="117"/>
+      <c r="H93" s="117" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="116"/>
-      <c r="J93" s="116"/>
-      <c r="K93" s="116"/>
-      <c r="L93" s="116"/>
-      <c r="M93" s="117" t="s">
+      <c r="I93" s="117"/>
+      <c r="J93" s="117"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="117"/>
+      <c r="M93" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="117"/>
+      <c r="N93" s="116"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7738,24 +7738,24 @@
       <c r="B94" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="116" t="s">
+      <c r="C94" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="116"/>
-      <c r="E94" s="116"/>
-      <c r="F94" s="116"/>
-      <c r="G94" s="116"/>
-      <c r="H94" s="116" t="s">
+      <c r="D94" s="117"/>
+      <c r="E94" s="117"/>
+      <c r="F94" s="117"/>
+      <c r="G94" s="117"/>
+      <c r="H94" s="117" t="s">
         <v>218</v>
       </c>
-      <c r="I94" s="116"/>
-      <c r="J94" s="116"/>
-      <c r="K94" s="116"/>
-      <c r="L94" s="116"/>
-      <c r="M94" s="117" t="s">
+      <c r="I94" s="117"/>
+      <c r="J94" s="117"/>
+      <c r="K94" s="117"/>
+      <c r="L94" s="117"/>
+      <c r="M94" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="117"/>
+      <c r="N94" s="116"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7765,24 +7765,24 @@
       <c r="B95" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C95" s="116" t="s">
+      <c r="C95" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="116"/>
-      <c r="E95" s="116"/>
-      <c r="F95" s="116"/>
-      <c r="G95" s="116"/>
-      <c r="H95" s="116" t="s">
+      <c r="D95" s="117"/>
+      <c r="E95" s="117"/>
+      <c r="F95" s="117"/>
+      <c r="G95" s="117"/>
+      <c r="H95" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="I95" s="116"/>
-      <c r="J95" s="116"/>
-      <c r="K95" s="116"/>
-      <c r="L95" s="116"/>
-      <c r="M95" s="117" t="s">
+      <c r="I95" s="117"/>
+      <c r="J95" s="117"/>
+      <c r="K95" s="117"/>
+      <c r="L95" s="117"/>
+      <c r="M95" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="117"/>
+      <c r="N95" s="116"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7792,24 +7792,24 @@
       <c r="B96" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="116" t="s">
+      <c r="C96" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="116"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="116"/>
-      <c r="G96" s="116"/>
-      <c r="H96" s="116" t="s">
+      <c r="D96" s="117"/>
+      <c r="E96" s="117"/>
+      <c r="F96" s="117"/>
+      <c r="G96" s="117"/>
+      <c r="H96" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="I96" s="116"/>
-      <c r="J96" s="116"/>
-      <c r="K96" s="116"/>
-      <c r="L96" s="116"/>
-      <c r="M96" s="117" t="s">
+      <c r="I96" s="117"/>
+      <c r="J96" s="117"/>
+      <c r="K96" s="117"/>
+      <c r="L96" s="117"/>
+      <c r="M96" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="117"/>
+      <c r="N96" s="116"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7819,24 +7819,24 @@
       <c r="B97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="116" t="s">
+      <c r="C97" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="116"/>
-      <c r="E97" s="116"/>
-      <c r="F97" s="116"/>
-      <c r="G97" s="116"/>
-      <c r="H97" s="116" t="s">
+      <c r="D97" s="117"/>
+      <c r="E97" s="117"/>
+      <c r="F97" s="117"/>
+      <c r="G97" s="117"/>
+      <c r="H97" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="I97" s="116"/>
-      <c r="J97" s="116"/>
-      <c r="K97" s="116"/>
-      <c r="L97" s="116"/>
-      <c r="M97" s="117" t="s">
+      <c r="I97" s="117"/>
+      <c r="J97" s="117"/>
+      <c r="K97" s="117"/>
+      <c r="L97" s="117"/>
+      <c r="M97" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="117"/>
+      <c r="N97" s="116"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7846,24 +7846,24 @@
       <c r="B98" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="116" t="s">
+      <c r="C98" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="116"/>
-      <c r="E98" s="116"/>
-      <c r="F98" s="116"/>
-      <c r="G98" s="116"/>
-      <c r="H98" s="116" t="s">
+      <c r="D98" s="117"/>
+      <c r="E98" s="117"/>
+      <c r="F98" s="117"/>
+      <c r="G98" s="117"/>
+      <c r="H98" s="117" t="s">
         <v>222</v>
       </c>
-      <c r="I98" s="116"/>
-      <c r="J98" s="116"/>
-      <c r="K98" s="116"/>
-      <c r="L98" s="116"/>
-      <c r="M98" s="117" t="s">
+      <c r="I98" s="117"/>
+      <c r="J98" s="117"/>
+      <c r="K98" s="117"/>
+      <c r="L98" s="117"/>
+      <c r="M98" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="117"/>
+      <c r="N98" s="116"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7873,24 +7873,24 @@
       <c r="B99" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C99" s="116" t="s">
+      <c r="C99" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="116"/>
-      <c r="E99" s="116"/>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116" t="s">
+      <c r="D99" s="117"/>
+      <c r="E99" s="117"/>
+      <c r="F99" s="117"/>
+      <c r="G99" s="117"/>
+      <c r="H99" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="I99" s="116"/>
-      <c r="J99" s="116"/>
-      <c r="K99" s="116"/>
-      <c r="L99" s="116"/>
-      <c r="M99" s="117" t="s">
+      <c r="I99" s="117"/>
+      <c r="J99" s="117"/>
+      <c r="K99" s="117"/>
+      <c r="L99" s="117"/>
+      <c r="M99" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="117"/>
+      <c r="N99" s="116"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7900,329 +7900,478 @@
       <c r="B100" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C100" s="116" t="s">
+      <c r="C100" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="116"/>
-      <c r="E100" s="116"/>
-      <c r="F100" s="116"/>
-      <c r="G100" s="116"/>
-      <c r="H100" s="116" t="s">
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="116"/>
-      <c r="J100" s="116"/>
-      <c r="K100" s="116"/>
-      <c r="L100" s="116"/>
-      <c r="M100" s="117" t="s">
+      <c r="I100" s="117"/>
+      <c r="J100" s="117"/>
+      <c r="K100" s="117"/>
+      <c r="L100" s="117"/>
+      <c r="M100" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="117"/>
+      <c r="N100" s="116"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="116"/>
-      <c r="D101" s="116"/>
-      <c r="E101" s="116"/>
-      <c r="F101" s="116"/>
-      <c r="G101" s="116"/>
-      <c r="H101" s="116"/>
-      <c r="I101" s="116"/>
-      <c r="J101" s="116"/>
-      <c r="K101" s="116"/>
-      <c r="L101" s="116"/>
-      <c r="M101" s="117"/>
-      <c r="N101" s="117"/>
+      <c r="C101" s="117"/>
+      <c r="D101" s="117"/>
+      <c r="E101" s="117"/>
+      <c r="F101" s="117"/>
+      <c r="G101" s="117"/>
+      <c r="H101" s="117"/>
+      <c r="I101" s="117"/>
+      <c r="J101" s="117"/>
+      <c r="K101" s="117"/>
+      <c r="L101" s="117"/>
+      <c r="M101" s="116"/>
+      <c r="N101" s="116"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="116"/>
-      <c r="I102" s="116"/>
-      <c r="J102" s="116"/>
-      <c r="K102" s="116"/>
-      <c r="L102" s="116"/>
-      <c r="M102" s="117"/>
-      <c r="N102" s="117"/>
+      <c r="H102" s="117"/>
+      <c r="I102" s="117"/>
+      <c r="J102" s="117"/>
+      <c r="K102" s="117"/>
+      <c r="L102" s="117"/>
+      <c r="M102" s="116"/>
+      <c r="N102" s="116"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="116"/>
-      <c r="D103" s="116"/>
-      <c r="E103" s="116"/>
-      <c r="F103" s="116"/>
-      <c r="G103" s="116"/>
-      <c r="H103" s="116"/>
-      <c r="I103" s="116"/>
-      <c r="J103" s="116"/>
-      <c r="K103" s="116"/>
-      <c r="L103" s="116"/>
-      <c r="M103" s="117"/>
-      <c r="N103" s="117"/>
+      <c r="C103" s="117"/>
+      <c r="D103" s="117"/>
+      <c r="E103" s="117"/>
+      <c r="F103" s="117"/>
+      <c r="G103" s="117"/>
+      <c r="H103" s="117"/>
+      <c r="I103" s="117"/>
+      <c r="J103" s="117"/>
+      <c r="K103" s="117"/>
+      <c r="L103" s="117"/>
+      <c r="M103" s="116"/>
+      <c r="N103" s="116"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="116"/>
-      <c r="D104" s="116"/>
-      <c r="E104" s="116"/>
-      <c r="F104" s="116"/>
-      <c r="G104" s="116"/>
-      <c r="H104" s="116"/>
-      <c r="I104" s="116"/>
-      <c r="J104" s="116"/>
-      <c r="K104" s="116"/>
-      <c r="L104" s="116"/>
-      <c r="M104" s="117"/>
-      <c r="N104" s="117"/>
+      <c r="C104" s="117"/>
+      <c r="D104" s="117"/>
+      <c r="E104" s="117"/>
+      <c r="F104" s="117"/>
+      <c r="G104" s="117"/>
+      <c r="H104" s="117"/>
+      <c r="I104" s="117"/>
+      <c r="J104" s="117"/>
+      <c r="K104" s="117"/>
+      <c r="L104" s="117"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="116"/>
-      <c r="D105" s="116"/>
-      <c r="E105" s="116"/>
-      <c r="F105" s="116"/>
-      <c r="G105" s="116"/>
-      <c r="H105" s="116"/>
-      <c r="I105" s="116"/>
-      <c r="J105" s="116"/>
-      <c r="K105" s="116"/>
-      <c r="L105" s="116"/>
-      <c r="M105" s="117"/>
-      <c r="N105" s="117"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
+      <c r="M105" s="116"/>
+      <c r="N105" s="116"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="116"/>
-      <c r="D106" s="116"/>
-      <c r="E106" s="116"/>
-      <c r="F106" s="116"/>
-      <c r="G106" s="116"/>
-      <c r="H106" s="116"/>
-      <c r="I106" s="116"/>
-      <c r="J106" s="116"/>
-      <c r="K106" s="116"/>
-      <c r="L106" s="116"/>
-      <c r="M106" s="117"/>
-      <c r="N106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
+      <c r="M106" s="116"/>
+      <c r="N106" s="116"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="116"/>
-      <c r="D107" s="116"/>
-      <c r="E107" s="116"/>
-      <c r="F107" s="116"/>
-      <c r="G107" s="116"/>
-      <c r="H107" s="116"/>
-      <c r="I107" s="116"/>
-      <c r="J107" s="116"/>
-      <c r="K107" s="116"/>
-      <c r="L107" s="116"/>
-      <c r="M107" s="117"/>
-      <c r="N107" s="117"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="117"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="117"/>
+      <c r="J107" s="117"/>
+      <c r="K107" s="117"/>
+      <c r="L107" s="117"/>
+      <c r="M107" s="116"/>
+      <c r="N107" s="116"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="116"/>
-      <c r="D108" s="116"/>
-      <c r="E108" s="116"/>
-      <c r="F108" s="116"/>
-      <c r="G108" s="116"/>
-      <c r="H108" s="116"/>
-      <c r="I108" s="116"/>
-      <c r="J108" s="116"/>
-      <c r="K108" s="116"/>
-      <c r="L108" s="116"/>
-      <c r="M108" s="117"/>
-      <c r="N108" s="117"/>
+      <c r="C108" s="117"/>
+      <c r="D108" s="117"/>
+      <c r="E108" s="117"/>
+      <c r="F108" s="117"/>
+      <c r="G108" s="117"/>
+      <c r="H108" s="117"/>
+      <c r="I108" s="117"/>
+      <c r="J108" s="117"/>
+      <c r="K108" s="117"/>
+      <c r="L108" s="117"/>
+      <c r="M108" s="116"/>
+      <c r="N108" s="116"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="116"/>
-      <c r="D109" s="116"/>
-      <c r="E109" s="116"/>
-      <c r="F109" s="116"/>
-      <c r="G109" s="116"/>
-      <c r="H109" s="116"/>
-      <c r="I109" s="116"/>
-      <c r="J109" s="116"/>
-      <c r="K109" s="116"/>
-      <c r="L109" s="116"/>
-      <c r="M109" s="117"/>
-      <c r="N109" s="117"/>
+      <c r="C109" s="117"/>
+      <c r="D109" s="117"/>
+      <c r="E109" s="117"/>
+      <c r="F109" s="117"/>
+      <c r="G109" s="117"/>
+      <c r="H109" s="117"/>
+      <c r="I109" s="117"/>
+      <c r="J109" s="117"/>
+      <c r="K109" s="117"/>
+      <c r="L109" s="117"/>
+      <c r="M109" s="116"/>
+      <c r="N109" s="116"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="116"/>
-      <c r="D110" s="116"/>
-      <c r="E110" s="116"/>
-      <c r="F110" s="116"/>
-      <c r="G110" s="116"/>
-      <c r="H110" s="116"/>
-      <c r="I110" s="116"/>
-      <c r="J110" s="116"/>
-      <c r="K110" s="116"/>
-      <c r="L110" s="116"/>
-      <c r="M110" s="117"/>
-      <c r="N110" s="117"/>
+      <c r="C110" s="117"/>
+      <c r="D110" s="117"/>
+      <c r="E110" s="117"/>
+      <c r="F110" s="117"/>
+      <c r="G110" s="117"/>
+      <c r="H110" s="117"/>
+      <c r="I110" s="117"/>
+      <c r="J110" s="117"/>
+      <c r="K110" s="117"/>
+      <c r="L110" s="117"/>
+      <c r="M110" s="116"/>
+      <c r="N110" s="116"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="116"/>
-      <c r="E111" s="116"/>
-      <c r="F111" s="116"/>
-      <c r="G111" s="116"/>
-      <c r="H111" s="116"/>
-      <c r="I111" s="116"/>
-      <c r="J111" s="116"/>
-      <c r="K111" s="116"/>
-      <c r="L111" s="116"/>
-      <c r="M111" s="117"/>
-      <c r="N111" s="117"/>
+      <c r="C111" s="117"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="117"/>
+      <c r="F111" s="117"/>
+      <c r="G111" s="117"/>
+      <c r="H111" s="117"/>
+      <c r="I111" s="117"/>
+      <c r="J111" s="117"/>
+      <c r="K111" s="117"/>
+      <c r="L111" s="117"/>
+      <c r="M111" s="116"/>
+      <c r="N111" s="116"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="116"/>
-      <c r="D112" s="116"/>
-      <c r="E112" s="116"/>
-      <c r="F112" s="116"/>
-      <c r="G112" s="116"/>
-      <c r="H112" s="116"/>
-      <c r="I112" s="116"/>
-      <c r="J112" s="116"/>
-      <c r="K112" s="116"/>
-      <c r="L112" s="116"/>
-      <c r="M112" s="117"/>
-      <c r="N112" s="117"/>
+      <c r="C112" s="117"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="117"/>
+      <c r="F112" s="117"/>
+      <c r="G112" s="117"/>
+      <c r="H112" s="117"/>
+      <c r="I112" s="117"/>
+      <c r="J112" s="117"/>
+      <c r="K112" s="117"/>
+      <c r="L112" s="117"/>
+      <c r="M112" s="116"/>
+      <c r="N112" s="116"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="116"/>
-      <c r="D113" s="116"/>
-      <c r="E113" s="116"/>
-      <c r="F113" s="116"/>
-      <c r="G113" s="116"/>
-      <c r="H113" s="116"/>
-      <c r="I113" s="116"/>
-      <c r="J113" s="116"/>
-      <c r="K113" s="116"/>
-      <c r="L113" s="116"/>
-      <c r="M113" s="117"/>
-      <c r="N113" s="117"/>
+      <c r="C113" s="117"/>
+      <c r="D113" s="117"/>
+      <c r="E113" s="117"/>
+      <c r="F113" s="117"/>
+      <c r="G113" s="117"/>
+      <c r="H113" s="117"/>
+      <c r="I113" s="117"/>
+      <c r="J113" s="117"/>
+      <c r="K113" s="117"/>
+      <c r="L113" s="117"/>
+      <c r="M113" s="116"/>
+      <c r="N113" s="116"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="116"/>
-      <c r="D114" s="116"/>
-      <c r="E114" s="116"/>
-      <c r="F114" s="116"/>
-      <c r="G114" s="116"/>
-      <c r="H114" s="116"/>
-      <c r="I114" s="116"/>
-      <c r="J114" s="116"/>
-      <c r="K114" s="116"/>
-      <c r="L114" s="116"/>
-      <c r="M114" s="117"/>
-      <c r="N114" s="117"/>
+      <c r="C114" s="117"/>
+      <c r="D114" s="117"/>
+      <c r="E114" s="117"/>
+      <c r="F114" s="117"/>
+      <c r="G114" s="117"/>
+      <c r="H114" s="117"/>
+      <c r="I114" s="117"/>
+      <c r="J114" s="117"/>
+      <c r="K114" s="117"/>
+      <c r="L114" s="117"/>
+      <c r="M114" s="116"/>
+      <c r="N114" s="116"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="116"/>
-      <c r="D115" s="116"/>
-      <c r="E115" s="116"/>
-      <c r="F115" s="116"/>
-      <c r="G115" s="116"/>
-      <c r="H115" s="116"/>
-      <c r="I115" s="116"/>
-      <c r="J115" s="116"/>
-      <c r="K115" s="116"/>
-      <c r="L115" s="116"/>
-      <c r="M115" s="117"/>
-      <c r="N115" s="117"/>
+      <c r="C115" s="117"/>
+      <c r="D115" s="117"/>
+      <c r="E115" s="117"/>
+      <c r="F115" s="117"/>
+      <c r="G115" s="117"/>
+      <c r="H115" s="117"/>
+      <c r="I115" s="117"/>
+      <c r="J115" s="117"/>
+      <c r="K115" s="117"/>
+      <c r="L115" s="117"/>
+      <c r="M115" s="116"/>
+      <c r="N115" s="116"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="116"/>
-      <c r="D116" s="116"/>
-      <c r="E116" s="116"/>
-      <c r="F116" s="116"/>
-      <c r="G116" s="116"/>
-      <c r="H116" s="116"/>
-      <c r="I116" s="116"/>
-      <c r="J116" s="116"/>
-      <c r="K116" s="116"/>
-      <c r="L116" s="116"/>
-      <c r="M116" s="117"/>
-      <c r="N116" s="117"/>
+      <c r="C116" s="117"/>
+      <c r="D116" s="117"/>
+      <c r="E116" s="117"/>
+      <c r="F116" s="117"/>
+      <c r="G116" s="117"/>
+      <c r="H116" s="117"/>
+      <c r="I116" s="117"/>
+      <c r="J116" s="117"/>
+      <c r="K116" s="117"/>
+      <c r="L116" s="117"/>
+      <c r="M116" s="116"/>
+      <c r="N116" s="116"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="116"/>
-      <c r="D117" s="116"/>
-      <c r="E117" s="116"/>
-      <c r="F117" s="116"/>
-      <c r="G117" s="116"/>
-      <c r="H117" s="116"/>
-      <c r="I117" s="116"/>
-      <c r="J117" s="116"/>
-      <c r="K117" s="116"/>
-      <c r="L117" s="116"/>
-      <c r="M117" s="117"/>
-      <c r="N117" s="117"/>
+      <c r="C117" s="117"/>
+      <c r="D117" s="117"/>
+      <c r="E117" s="117"/>
+      <c r="F117" s="117"/>
+      <c r="G117" s="117"/>
+      <c r="H117" s="117"/>
+      <c r="I117" s="117"/>
+      <c r="J117" s="117"/>
+      <c r="K117" s="117"/>
+      <c r="L117" s="117"/>
+      <c r="M117" s="116"/>
+      <c r="N117" s="116"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="116"/>
-      <c r="D118" s="116"/>
-      <c r="E118" s="116"/>
-      <c r="F118" s="116"/>
-      <c r="G118" s="116"/>
-      <c r="H118" s="116"/>
-      <c r="I118" s="116"/>
-      <c r="J118" s="116"/>
-      <c r="K118" s="116"/>
-      <c r="L118" s="116"/>
-      <c r="M118" s="117"/>
-      <c r="N118" s="117"/>
+      <c r="C118" s="117"/>
+      <c r="D118" s="117"/>
+      <c r="E118" s="117"/>
+      <c r="F118" s="117"/>
+      <c r="G118" s="117"/>
+      <c r="H118" s="117"/>
+      <c r="I118" s="117"/>
+      <c r="J118" s="117"/>
+      <c r="K118" s="117"/>
+      <c r="L118" s="117"/>
+      <c r="M118" s="116"/>
+      <c r="N118" s="116"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
     <mergeCell ref="M96:N96"/>
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="Q83:AA83"/>
@@ -8247,155 +8396,6 @@
     <mergeCell ref="J65:K65"/>
     <mergeCell ref="J66:K66"/>
     <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ump balance patch: shake 2 -> 1
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFB0ED7-6E21-4724-AD85-7FF2E3061D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FEC62D-ADC7-4B86-B215-C2F7130FE1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="225" windowWidth="14243" windowHeight="12112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2370,69 +2370,69 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3587,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3606,10 +3606,10 @@
       <c r="B1" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="132" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="126"/>
+      <c r="D1" s="132"/>
       <c r="G1" s="56" t="s">
         <v>159</v>
       </c>
@@ -3705,10 +3705,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="131" t="s">
+      <c r="Z2" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="131"/>
+      <c r="AA2" s="124"/>
       <c r="AG2" s="43" t="s">
         <v>84</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>700</v>
       </c>
       <c r="D28" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="19">
         <v>1</v>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="R28" s="19">
         <f>ROUND(D28/H28,3)</f>
-        <v>0.125</v>
+        <v>6.3E-2</v>
       </c>
       <c r="S28" s="28" t="s">
         <v>29</v>
@@ -6110,28 +6110,28 @@
       <c r="B40" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="119" t="s">
+      <c r="C40" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119" t="s">
+      <c r="D40" s="130"/>
+      <c r="E40" s="130"/>
+      <c r="F40" s="130"/>
+      <c r="G40" s="130"/>
+      <c r="H40" s="130"/>
+      <c r="I40" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="119"/>
-      <c r="K40" s="119"/>
-      <c r="L40" s="119"/>
+      <c r="J40" s="130"/>
+      <c r="K40" s="130"/>
+      <c r="L40" s="130"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="132" t="s">
+      <c r="S40" s="129" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="132"/>
+      <c r="T40" s="129"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6141,30 +6141,30 @@
       <c r="B41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="120" t="s">
+      <c r="C41" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120" t="s">
+      <c r="D41" s="131"/>
+      <c r="E41" s="131"/>
+      <c r="F41" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120" t="s">
+      <c r="G41" s="131"/>
+      <c r="H41" s="131"/>
+      <c r="I41" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="120"/>
-      <c r="K41" s="120"/>
-      <c r="L41" s="120"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="131"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="132" t="s">
+      <c r="S41" s="129" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="132"/>
+      <c r="T41" s="129"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -6177,30 +6177,30 @@
       <c r="B42" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="120" t="s">
+      <c r="C42" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="120" t="s">
+      <c r="D42" s="131"/>
+      <c r="E42" s="131"/>
+      <c r="F42" s="131" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="120"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="120" t="s">
+      <c r="G42" s="131"/>
+      <c r="H42" s="131"/>
+      <c r="I42" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="120"/>
-      <c r="K42" s="120"/>
-      <c r="L42" s="120"/>
+      <c r="J42" s="131"/>
+      <c r="K42" s="131"/>
+      <c r="L42" s="131"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="132" t="s">
+      <c r="S42" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="132"/>
+      <c r="T42" s="129"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6213,30 +6213,30 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="121" t="s">
+      <c r="C43" s="127" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
-      <c r="F43" s="121" t="s">
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="121"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="121" t="s">
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
+      <c r="I43" s="127" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="121"/>
-      <c r="K43" s="121"/>
-      <c r="L43" s="121"/>
+      <c r="J43" s="127"/>
+      <c r="K43" s="127"/>
+      <c r="L43" s="127"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="132" t="s">
+      <c r="S43" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="132"/>
+      <c r="T43" s="129"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6251,20 +6251,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="121" t="s">
+      <c r="C44" s="127" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121" t="s">
+      <c r="D44" s="127"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="127"/>
+      <c r="I44" s="127" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="121"/>
+      <c r="J44" s="127"/>
+      <c r="K44" s="127"/>
+      <c r="L44" s="127"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6280,16 +6280,16 @@
       <c r="B47" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="119" t="s">
+      <c r="C47" s="130" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="119"/>
-      <c r="E47" s="119" t="s">
+      <c r="D47" s="130"/>
+      <c r="E47" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
+      <c r="F47" s="130"/>
+      <c r="G47" s="130"/>
+      <c r="H47" s="130"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -6300,16 +6300,16 @@
       <c r="B48" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="120">
+      <c r="C48" s="131">
         <v>2</v>
       </c>
-      <c r="D48" s="120"/>
-      <c r="E48" s="120" t="s">
+      <c r="D48" s="131"/>
+      <c r="E48" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="120"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="120"/>
+      <c r="F48" s="131"/>
+      <c r="G48" s="131"/>
+      <c r="H48" s="131"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
@@ -6320,28 +6320,28 @@
       <c r="B49" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="120" t="s">
+      <c r="C49" s="131" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="120" t="s">
+      <c r="D49" s="131"/>
+      <c r="E49" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="120"/>
-      <c r="G49" s="120"/>
-      <c r="H49" s="120"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="121"/>
-      <c r="D50" s="121"/>
-      <c r="E50" s="121"/>
-      <c r="F50" s="121"/>
-      <c r="G50" s="121"/>
-      <c r="H50" s="121"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="127"/>
+      <c r="E50" s="127"/>
+      <c r="F50" s="127"/>
+      <c r="G50" s="127"/>
+      <c r="H50" s="127"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6359,14 +6359,14 @@
       <c r="D54" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="124" t="s">
+      <c r="H54" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="124"/>
-      <c r="J54" s="124"/>
-      <c r="K54" s="124"/>
-      <c r="L54" s="124"/>
-      <c r="M54" s="124"/>
+      <c r="I54" s="136"/>
+      <c r="J54" s="136"/>
+      <c r="K54" s="136"/>
+      <c r="L54" s="136"/>
+      <c r="M54" s="136"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6517,14 +6517,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="125" t="s">
+      <c r="H58" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="125"/>
-      <c r="J58" s="125"/>
-      <c r="K58" s="125"/>
-      <c r="L58" s="125"/>
-      <c r="M58" s="125"/>
+      <c r="I58" s="137"/>
+      <c r="J58" s="137"/>
+      <c r="K58" s="137"/>
+      <c r="L58" s="137"/>
+      <c r="M58" s="137"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6573,10 +6573,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="128" t="s">
+      <c r="J62" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="128"/>
+      <c r="K62" s="134"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -6584,13 +6584,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="127" t="s">
+      <c r="O62" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="127"/>
-      <c r="Q62" s="127"/>
-      <c r="R62" s="127"/>
-      <c r="S62" s="127"/>
+      <c r="P62" s="133"/>
+      <c r="Q62" s="133"/>
+      <c r="R62" s="133"/>
+      <c r="S62" s="133"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6612,20 +6612,20 @@
       <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="133" t="s">
+      <c r="F63" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="133"/>
+      <c r="G63" s="119"/>
       <c r="H63" s="86" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="133" t="s">
+      <c r="J63" s="119" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="133"/>
+      <c r="K63" s="119"/>
       <c r="L63" s="86" t="s">
         <v>102</v>
       </c>
@@ -6649,10 +6649,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="133" t="s">
+      <c r="U63" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="133"/>
+      <c r="V63" s="119"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6680,21 +6680,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="134" t="s">
+      <c r="F64" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="134"/>
+      <c r="G64" s="135"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="123">
+      <c r="J64" s="122">
         <f t="shared" ref="J64:J69" si="31">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="123"/>
+      <c r="K64" s="122"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -6725,11 +6725,11 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="136">
+      <c r="U64" s="120">
         <f>R64+O64+P64</f>
         <v>3.8</v>
       </c>
-      <c r="V64" s="136"/>
+      <c r="V64" s="120"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6757,21 +6757,21 @@
       <c r="E65" s="54">
         <v>4</v>
       </c>
-      <c r="F65" s="116" t="s">
+      <c r="F65" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="116"/>
+      <c r="G65" s="117"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="123">
+      <c r="J65" s="122">
         <f t="shared" si="31"/>
         <v>32</v>
       </c>
-      <c r="K65" s="123"/>
+      <c r="K65" s="122"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6802,11 +6802,11 @@
         <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="137">
+      <c r="U65" s="121">
         <f t="shared" ref="U65:U70" si="38">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="137"/>
+      <c r="V65" s="121"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6834,21 +6834,21 @@
       <c r="E66" s="54">
         <v>3</v>
       </c>
-      <c r="F66" s="116" t="s">
+      <c r="F66" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="116"/>
+      <c r="G66" s="117"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="123">
+      <c r="J66" s="122">
         <f t="shared" si="31"/>
         <v>28</v>
       </c>
-      <c r="K66" s="123"/>
+      <c r="K66" s="122"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6879,11 +6879,11 @@
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="137">
+      <c r="U66" s="121">
         <f t="shared" si="38"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="137"/>
+      <c r="V66" s="121"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6911,21 +6911,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="116" t="s">
+      <c r="F67" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="116"/>
+      <c r="G67" s="117"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="123">
+      <c r="J67" s="122">
         <f t="shared" si="31"/>
         <v>48</v>
       </c>
-      <c r="K67" s="123"/>
+      <c r="K67" s="122"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6956,11 +6956,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="137">
+      <c r="U67" s="121">
         <f t="shared" si="38"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="137"/>
+      <c r="V67" s="121"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6984,21 +6984,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="116" t="s">
+      <c r="F68" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="116"/>
+      <c r="G68" s="117"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="123">
+      <c r="J68" s="122">
         <f t="shared" si="31"/>
         <v>72</v>
       </c>
-      <c r="K68" s="123"/>
+      <c r="K68" s="122"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7029,11 +7029,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="137">
+      <c r="U68" s="121">
         <f t="shared" si="38"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="137"/>
+      <c r="V68" s="121"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7057,21 +7057,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="116" t="s">
+      <c r="F69" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="116"/>
+      <c r="G69" s="117"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="123">
+      <c r="J69" s="122">
         <f t="shared" si="31"/>
         <v>20</v>
       </c>
-      <c r="K69" s="123"/>
+      <c r="K69" s="122"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7102,11 +7102,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="137">
+      <c r="U69" s="121">
         <f t="shared" si="38"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="137"/>
+      <c r="V69" s="121"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7130,21 +7130,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="116" t="s">
+      <c r="F70" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="116"/>
+      <c r="G70" s="117"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="123">
+      <c r="J70" s="122">
         <f t="shared" ref="J70" si="39">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="123"/>
+      <c r="K70" s="122"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7175,11 +7175,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="137">
+      <c r="U70" s="121">
         <f t="shared" si="38"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="137"/>
+      <c r="V70" s="121"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7192,12 +7192,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="131" t="s">
+      <c r="O73" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="131"/>
-      <c r="Q73" s="131"/>
-      <c r="R73" s="131"/>
+      <c r="P73" s="124"/>
+      <c r="Q73" s="124"/>
+      <c r="R73" s="124"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7213,31 +7213,31 @@
       <c r="E74" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="122" t="s">
+      <c r="F74" s="123" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="122"/>
-      <c r="H74" s="122" t="s">
+      <c r="G74" s="123"/>
+      <c r="H74" s="123" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="122"/>
-      <c r="J74" s="122" t="s">
+      <c r="I74" s="123"/>
+      <c r="J74" s="123" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="122"/>
-      <c r="L74" s="122"/>
-      <c r="M74" s="122"/>
+      <c r="K74" s="123"/>
+      <c r="L74" s="123"/>
+      <c r="M74" s="123"/>
       <c r="N74" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="122" t="s">
+      <c r="O74" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="122"/>
-      <c r="Q74" s="122" t="s">
+      <c r="P74" s="123"/>
+      <c r="Q74" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="122"/>
+      <c r="R74" s="123"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="29">
@@ -7255,21 +7255,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="123" t="s">
+      <c r="F75" s="122" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="123"/>
-      <c r="H75" s="123">
+      <c r="G75" s="122"/>
+      <c r="H75" s="122">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="123"/>
-      <c r="J75" s="123" t="s">
+      <c r="I75" s="122"/>
+      <c r="J75" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="123"/>
-      <c r="L75" s="123"/>
-      <c r="M75" s="123"/>
+      <c r="K75" s="122"/>
+      <c r="L75" s="122"/>
+      <c r="M75" s="122"/>
       <c r="N75" s="78" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7298,21 +7298,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="123" t="s">
+      <c r="F76" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="123"/>
-      <c r="H76" s="123">
+      <c r="G76" s="122"/>
+      <c r="H76" s="122">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="123"/>
-      <c r="J76" s="123" t="s">
+      <c r="I76" s="122"/>
+      <c r="J76" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="123"/>
-      <c r="L76" s="123"/>
-      <c r="M76" s="123"/>
+      <c r="K76" s="122"/>
+      <c r="L76" s="122"/>
+      <c r="M76" s="122"/>
       <c r="N76" s="78" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7331,19 +7331,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="121"/>
-      <c r="G77" s="121"/>
-      <c r="H77" s="121"/>
-      <c r="I77" s="121"/>
-      <c r="J77" s="121"/>
-      <c r="K77" s="121"/>
-      <c r="L77" s="121"/>
-      <c r="M77" s="121"/>
+      <c r="F77" s="127"/>
+      <c r="G77" s="127"/>
+      <c r="H77" s="127"/>
+      <c r="I77" s="127"/>
+      <c r="J77" s="127"/>
+      <c r="K77" s="127"/>
+      <c r="L77" s="127"/>
+      <c r="M77" s="127"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="129"/>
-      <c r="P77" s="129"/>
-      <c r="Q77" s="129"/>
-      <c r="R77" s="129"/>
+      <c r="O77" s="125"/>
+      <c r="P77" s="125"/>
+      <c r="Q77" s="125"/>
+      <c r="R77" s="125"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7371,32 +7371,32 @@
       <c r="E81" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="122" t="s">
+      <c r="F81" s="123" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="122"/>
-      <c r="H81" s="122"/>
-      <c r="I81" s="122"/>
-      <c r="J81" s="122"/>
-      <c r="K81" s="122"/>
-      <c r="L81" s="122"/>
-      <c r="M81" s="122"/>
-      <c r="N81" s="122"/>
-      <c r="O81" s="122"/>
-      <c r="P81" s="122"/>
-      <c r="Q81" s="122" t="s">
+      <c r="G81" s="123"/>
+      <c r="H81" s="123"/>
+      <c r="I81" s="123"/>
+      <c r="J81" s="123"/>
+      <c r="K81" s="123"/>
+      <c r="L81" s="123"/>
+      <c r="M81" s="123"/>
+      <c r="N81" s="123"/>
+      <c r="O81" s="123"/>
+      <c r="P81" s="123"/>
+      <c r="Q81" s="123" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="122"/>
-      <c r="S81" s="122"/>
-      <c r="T81" s="122"/>
-      <c r="U81" s="122"/>
-      <c r="V81" s="122"/>
-      <c r="W81" s="122"/>
-      <c r="X81" s="122"/>
-      <c r="Y81" s="122"/>
-      <c r="Z81" s="122"/>
-      <c r="AA81" s="122"/>
+      <c r="R81" s="123"/>
+      <c r="S81" s="123"/>
+      <c r="T81" s="123"/>
+      <c r="U81" s="123"/>
+      <c r="V81" s="123"/>
+      <c r="W81" s="123"/>
+      <c r="X81" s="123"/>
+      <c r="Y81" s="123"/>
+      <c r="Z81" s="123"/>
+      <c r="AA81" s="123"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7412,32 +7412,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="135" t="s">
+      <c r="F82" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="135"/>
-      <c r="H82" s="135"/>
-      <c r="I82" s="135"/>
-      <c r="J82" s="135"/>
-      <c r="K82" s="135"/>
-      <c r="L82" s="135"/>
-      <c r="M82" s="135"/>
-      <c r="N82" s="135"/>
-      <c r="O82" s="135"/>
-      <c r="P82" s="135"/>
-      <c r="Q82" s="135" t="s">
+      <c r="G82" s="128"/>
+      <c r="H82" s="128"/>
+      <c r="I82" s="128"/>
+      <c r="J82" s="128"/>
+      <c r="K82" s="128"/>
+      <c r="L82" s="128"/>
+      <c r="M82" s="128"/>
+      <c r="N82" s="128"/>
+      <c r="O82" s="128"/>
+      <c r="P82" s="128"/>
+      <c r="Q82" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="135"/>
-      <c r="S82" s="135"/>
-      <c r="T82" s="135"/>
-      <c r="U82" s="135"/>
-      <c r="V82" s="135"/>
-      <c r="W82" s="135"/>
-      <c r="X82" s="135"/>
-      <c r="Y82" s="135"/>
-      <c r="Z82" s="135"/>
-      <c r="AA82" s="135"/>
+      <c r="R82" s="128"/>
+      <c r="S82" s="128"/>
+      <c r="T82" s="128"/>
+      <c r="U82" s="128"/>
+      <c r="V82" s="128"/>
+      <c r="W82" s="128"/>
+      <c r="X82" s="128"/>
+      <c r="Y82" s="128"/>
+      <c r="Z82" s="128"/>
+      <c r="AA82" s="128"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7627,24 +7627,24 @@
       <c r="B90" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="130" t="s">
+      <c r="C90" s="126" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="130"/>
-      <c r="E90" s="130"/>
-      <c r="F90" s="130"/>
-      <c r="G90" s="130"/>
-      <c r="H90" s="130" t="s">
+      <c r="D90" s="126"/>
+      <c r="E90" s="126"/>
+      <c r="F90" s="126"/>
+      <c r="G90" s="126"/>
+      <c r="H90" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="130"/>
-      <c r="J90" s="130"/>
-      <c r="K90" s="130"/>
-      <c r="L90" s="130"/>
-      <c r="M90" s="122" t="s">
+      <c r="I90" s="126"/>
+      <c r="J90" s="126"/>
+      <c r="K90" s="126"/>
+      <c r="L90" s="126"/>
+      <c r="M90" s="123" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="122"/>
+      <c r="N90" s="123"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>197</v>
@@ -7657,24 +7657,24 @@
       <c r="B91" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="117" t="s">
+      <c r="C91" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="117"/>
-      <c r="E91" s="117"/>
-      <c r="F91" s="117"/>
-      <c r="G91" s="117"/>
-      <c r="H91" s="117" t="s">
+      <c r="D91" s="116"/>
+      <c r="E91" s="116"/>
+      <c r="F91" s="116"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="117"/>
-      <c r="J91" s="117"/>
-      <c r="K91" s="117"/>
-      <c r="L91" s="117"/>
-      <c r="M91" s="116" t="s">
+      <c r="I91" s="116"/>
+      <c r="J91" s="116"/>
+      <c r="K91" s="116"/>
+      <c r="L91" s="116"/>
+      <c r="M91" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="116"/>
+      <c r="N91" s="117"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7684,24 +7684,24 @@
       <c r="B92" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="117" t="s">
+      <c r="C92" s="116" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="117"/>
-      <c r="E92" s="117"/>
-      <c r="F92" s="117"/>
-      <c r="G92" s="117"/>
-      <c r="H92" s="117" t="s">
+      <c r="D92" s="116"/>
+      <c r="E92" s="116"/>
+      <c r="F92" s="116"/>
+      <c r="G92" s="116"/>
+      <c r="H92" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="117"/>
-      <c r="J92" s="117"/>
-      <c r="K92" s="117"/>
-      <c r="L92" s="117"/>
-      <c r="M92" s="116" t="s">
+      <c r="I92" s="116"/>
+      <c r="J92" s="116"/>
+      <c r="K92" s="116"/>
+      <c r="L92" s="116"/>
+      <c r="M92" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="116"/>
+      <c r="N92" s="117"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7711,24 +7711,24 @@
       <c r="B93" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="117" t="s">
+      <c r="C93" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="117"/>
-      <c r="E93" s="117"/>
-      <c r="F93" s="117"/>
-      <c r="G93" s="117"/>
-      <c r="H93" s="117" t="s">
+      <c r="D93" s="116"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="116"/>
+      <c r="G93" s="116"/>
+      <c r="H93" s="116" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="117"/>
-      <c r="J93" s="117"/>
-      <c r="K93" s="117"/>
-      <c r="L93" s="117"/>
-      <c r="M93" s="116" t="s">
+      <c r="I93" s="116"/>
+      <c r="J93" s="116"/>
+      <c r="K93" s="116"/>
+      <c r="L93" s="116"/>
+      <c r="M93" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="116"/>
+      <c r="N93" s="117"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7738,24 +7738,24 @@
       <c r="B94" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="117" t="s">
+      <c r="C94" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="117"/>
-      <c r="E94" s="117"/>
-      <c r="F94" s="117"/>
-      <c r="G94" s="117"/>
-      <c r="H94" s="117" t="s">
+      <c r="D94" s="116"/>
+      <c r="E94" s="116"/>
+      <c r="F94" s="116"/>
+      <c r="G94" s="116"/>
+      <c r="H94" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="I94" s="117"/>
-      <c r="J94" s="117"/>
-      <c r="K94" s="117"/>
-      <c r="L94" s="117"/>
-      <c r="M94" s="116" t="s">
+      <c r="I94" s="116"/>
+      <c r="J94" s="116"/>
+      <c r="K94" s="116"/>
+      <c r="L94" s="116"/>
+      <c r="M94" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="116"/>
+      <c r="N94" s="117"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7765,24 +7765,24 @@
       <c r="B95" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C95" s="117" t="s">
+      <c r="C95" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="117"/>
-      <c r="E95" s="117"/>
-      <c r="F95" s="117"/>
-      <c r="G95" s="117"/>
-      <c r="H95" s="117" t="s">
+      <c r="D95" s="116"/>
+      <c r="E95" s="116"/>
+      <c r="F95" s="116"/>
+      <c r="G95" s="116"/>
+      <c r="H95" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="I95" s="117"/>
-      <c r="J95" s="117"/>
-      <c r="K95" s="117"/>
-      <c r="L95" s="117"/>
-      <c r="M95" s="116" t="s">
+      <c r="I95" s="116"/>
+      <c r="J95" s="116"/>
+      <c r="K95" s="116"/>
+      <c r="L95" s="116"/>
+      <c r="M95" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="116"/>
+      <c r="N95" s="117"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7792,24 +7792,24 @@
       <c r="B96" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="117" t="s">
+      <c r="C96" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="117"/>
-      <c r="E96" s="117"/>
-      <c r="F96" s="117"/>
-      <c r="G96" s="117"/>
-      <c r="H96" s="117" t="s">
+      <c r="D96" s="116"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="116"/>
+      <c r="G96" s="116"/>
+      <c r="H96" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="I96" s="117"/>
-      <c r="J96" s="117"/>
-      <c r="K96" s="117"/>
-      <c r="L96" s="117"/>
-      <c r="M96" s="116" t="s">
+      <c r="I96" s="116"/>
+      <c r="J96" s="116"/>
+      <c r="K96" s="116"/>
+      <c r="L96" s="116"/>
+      <c r="M96" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="116"/>
+      <c r="N96" s="117"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7819,24 +7819,24 @@
       <c r="B97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="117" t="s">
+      <c r="C97" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="117"/>
-      <c r="E97" s="117"/>
-      <c r="F97" s="117"/>
-      <c r="G97" s="117"/>
-      <c r="H97" s="117" t="s">
+      <c r="D97" s="116"/>
+      <c r="E97" s="116"/>
+      <c r="F97" s="116"/>
+      <c r="G97" s="116"/>
+      <c r="H97" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="I97" s="117"/>
-      <c r="J97" s="117"/>
-      <c r="K97" s="117"/>
-      <c r="L97" s="117"/>
-      <c r="M97" s="116" t="s">
+      <c r="I97" s="116"/>
+      <c r="J97" s="116"/>
+      <c r="K97" s="116"/>
+      <c r="L97" s="116"/>
+      <c r="M97" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="116"/>
+      <c r="N97" s="117"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7846,24 +7846,24 @@
       <c r="B98" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="117" t="s">
+      <c r="C98" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="117"/>
-      <c r="E98" s="117"/>
-      <c r="F98" s="117"/>
-      <c r="G98" s="117"/>
-      <c r="H98" s="117" t="s">
+      <c r="D98" s="116"/>
+      <c r="E98" s="116"/>
+      <c r="F98" s="116"/>
+      <c r="G98" s="116"/>
+      <c r="H98" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="I98" s="117"/>
-      <c r="J98" s="117"/>
-      <c r="K98" s="117"/>
-      <c r="L98" s="117"/>
-      <c r="M98" s="116" t="s">
+      <c r="I98" s="116"/>
+      <c r="J98" s="116"/>
+      <c r="K98" s="116"/>
+      <c r="L98" s="116"/>
+      <c r="M98" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="116"/>
+      <c r="N98" s="117"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7873,24 +7873,24 @@
       <c r="B99" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C99" s="117" t="s">
+      <c r="C99" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="117"/>
-      <c r="E99" s="117"/>
-      <c r="F99" s="117"/>
-      <c r="G99" s="117"/>
-      <c r="H99" s="117" t="s">
+      <c r="D99" s="116"/>
+      <c r="E99" s="116"/>
+      <c r="F99" s="116"/>
+      <c r="G99" s="116"/>
+      <c r="H99" s="116" t="s">
         <v>223</v>
       </c>
-      <c r="I99" s="117"/>
-      <c r="J99" s="117"/>
-      <c r="K99" s="117"/>
-      <c r="L99" s="117"/>
-      <c r="M99" s="116" t="s">
+      <c r="I99" s="116"/>
+      <c r="J99" s="116"/>
+      <c r="K99" s="116"/>
+      <c r="L99" s="116"/>
+      <c r="M99" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="116"/>
+      <c r="N99" s="117"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7900,411 +7900,396 @@
       <c r="B100" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C100" s="117" t="s">
+      <c r="C100" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="117"/>
-      <c r="E100" s="117"/>
-      <c r="F100" s="117"/>
-      <c r="G100" s="117"/>
-      <c r="H100" s="117" t="s">
+      <c r="D100" s="116"/>
+      <c r="E100" s="116"/>
+      <c r="F100" s="116"/>
+      <c r="G100" s="116"/>
+      <c r="H100" s="116" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="117"/>
-      <c r="J100" s="117"/>
-      <c r="K100" s="117"/>
-      <c r="L100" s="117"/>
-      <c r="M100" s="116" t="s">
+      <c r="I100" s="116"/>
+      <c r="J100" s="116"/>
+      <c r="K100" s="116"/>
+      <c r="L100" s="116"/>
+      <c r="M100" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="116"/>
+      <c r="N100" s="117"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="117"/>
-      <c r="D101" s="117"/>
-      <c r="E101" s="117"/>
-      <c r="F101" s="117"/>
-      <c r="G101" s="117"/>
-      <c r="H101" s="117"/>
-      <c r="I101" s="117"/>
-      <c r="J101" s="117"/>
-      <c r="K101" s="117"/>
-      <c r="L101" s="117"/>
-      <c r="M101" s="116"/>
-      <c r="N101" s="116"/>
+      <c r="C101" s="116"/>
+      <c r="D101" s="116"/>
+      <c r="E101" s="116"/>
+      <c r="F101" s="116"/>
+      <c r="G101" s="116"/>
+      <c r="H101" s="116"/>
+      <c r="I101" s="116"/>
+      <c r="J101" s="116"/>
+      <c r="K101" s="116"/>
+      <c r="L101" s="116"/>
+      <c r="M101" s="117"/>
+      <c r="N101" s="117"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="117"/>
-      <c r="I102" s="117"/>
-      <c r="J102" s="117"/>
-      <c r="K102" s="117"/>
-      <c r="L102" s="117"/>
-      <c r="M102" s="116"/>
-      <c r="N102" s="116"/>
+      <c r="H102" s="116"/>
+      <c r="I102" s="116"/>
+      <c r="J102" s="116"/>
+      <c r="K102" s="116"/>
+      <c r="L102" s="116"/>
+      <c r="M102" s="117"/>
+      <c r="N102" s="117"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="117"/>
-      <c r="D103" s="117"/>
-      <c r="E103" s="117"/>
-      <c r="F103" s="117"/>
-      <c r="G103" s="117"/>
-      <c r="H103" s="117"/>
-      <c r="I103" s="117"/>
-      <c r="J103" s="117"/>
-      <c r="K103" s="117"/>
-      <c r="L103" s="117"/>
-      <c r="M103" s="116"/>
-      <c r="N103" s="116"/>
+      <c r="C103" s="116"/>
+      <c r="D103" s="116"/>
+      <c r="E103" s="116"/>
+      <c r="F103" s="116"/>
+      <c r="G103" s="116"/>
+      <c r="H103" s="116"/>
+      <c r="I103" s="116"/>
+      <c r="J103" s="116"/>
+      <c r="K103" s="116"/>
+      <c r="L103" s="116"/>
+      <c r="M103" s="117"/>
+      <c r="N103" s="117"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="117"/>
-      <c r="D104" s="117"/>
-      <c r="E104" s="117"/>
-      <c r="F104" s="117"/>
-      <c r="G104" s="117"/>
-      <c r="H104" s="117"/>
-      <c r="I104" s="117"/>
-      <c r="J104" s="117"/>
-      <c r="K104" s="117"/>
-      <c r="L104" s="117"/>
-      <c r="M104" s="116"/>
-      <c r="N104" s="116"/>
+      <c r="C104" s="116"/>
+      <c r="D104" s="116"/>
+      <c r="E104" s="116"/>
+      <c r="F104" s="116"/>
+      <c r="G104" s="116"/>
+      <c r="H104" s="116"/>
+      <c r="I104" s="116"/>
+      <c r="J104" s="116"/>
+      <c r="K104" s="116"/>
+      <c r="L104" s="116"/>
+      <c r="M104" s="117"/>
+      <c r="N104" s="117"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="117"/>
-      <c r="D105" s="117"/>
-      <c r="E105" s="117"/>
-      <c r="F105" s="117"/>
-      <c r="G105" s="117"/>
-      <c r="H105" s="117"/>
-      <c r="I105" s="117"/>
-      <c r="J105" s="117"/>
-      <c r="K105" s="117"/>
-      <c r="L105" s="117"/>
-      <c r="M105" s="116"/>
-      <c r="N105" s="116"/>
+      <c r="C105" s="116"/>
+      <c r="D105" s="116"/>
+      <c r="E105" s="116"/>
+      <c r="F105" s="116"/>
+      <c r="G105" s="116"/>
+      <c r="H105" s="116"/>
+      <c r="I105" s="116"/>
+      <c r="J105" s="116"/>
+      <c r="K105" s="116"/>
+      <c r="L105" s="116"/>
+      <c r="M105" s="117"/>
+      <c r="N105" s="117"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="117"/>
-      <c r="D106" s="117"/>
-      <c r="E106" s="117"/>
-      <c r="F106" s="117"/>
-      <c r="G106" s="117"/>
-      <c r="H106" s="117"/>
-      <c r="I106" s="117"/>
-      <c r="J106" s="117"/>
-      <c r="K106" s="117"/>
-      <c r="L106" s="117"/>
-      <c r="M106" s="116"/>
-      <c r="N106" s="116"/>
+      <c r="C106" s="116"/>
+      <c r="D106" s="116"/>
+      <c r="E106" s="116"/>
+      <c r="F106" s="116"/>
+      <c r="G106" s="116"/>
+      <c r="H106" s="116"/>
+      <c r="I106" s="116"/>
+      <c r="J106" s="116"/>
+      <c r="K106" s="116"/>
+      <c r="L106" s="116"/>
+      <c r="M106" s="117"/>
+      <c r="N106" s="117"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="117"/>
-      <c r="D107" s="117"/>
-      <c r="E107" s="117"/>
-      <c r="F107" s="117"/>
-      <c r="G107" s="117"/>
-      <c r="H107" s="117"/>
-      <c r="I107" s="117"/>
-      <c r="J107" s="117"/>
-      <c r="K107" s="117"/>
-      <c r="L107" s="117"/>
-      <c r="M107" s="116"/>
-      <c r="N107" s="116"/>
+      <c r="C107" s="116"/>
+      <c r="D107" s="116"/>
+      <c r="E107" s="116"/>
+      <c r="F107" s="116"/>
+      <c r="G107" s="116"/>
+      <c r="H107" s="116"/>
+      <c r="I107" s="116"/>
+      <c r="J107" s="116"/>
+      <c r="K107" s="116"/>
+      <c r="L107" s="116"/>
+      <c r="M107" s="117"/>
+      <c r="N107" s="117"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="117"/>
-      <c r="D108" s="117"/>
-      <c r="E108" s="117"/>
-      <c r="F108" s="117"/>
-      <c r="G108" s="117"/>
-      <c r="H108" s="117"/>
-      <c r="I108" s="117"/>
-      <c r="J108" s="117"/>
-      <c r="K108" s="117"/>
-      <c r="L108" s="117"/>
-      <c r="M108" s="116"/>
-      <c r="N108" s="116"/>
+      <c r="C108" s="116"/>
+      <c r="D108" s="116"/>
+      <c r="E108" s="116"/>
+      <c r="F108" s="116"/>
+      <c r="G108" s="116"/>
+      <c r="H108" s="116"/>
+      <c r="I108" s="116"/>
+      <c r="J108" s="116"/>
+      <c r="K108" s="116"/>
+      <c r="L108" s="116"/>
+      <c r="M108" s="117"/>
+      <c r="N108" s="117"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="117"/>
-      <c r="D109" s="117"/>
-      <c r="E109" s="117"/>
-      <c r="F109" s="117"/>
-      <c r="G109" s="117"/>
-      <c r="H109" s="117"/>
-      <c r="I109" s="117"/>
-      <c r="J109" s="117"/>
-      <c r="K109" s="117"/>
-      <c r="L109" s="117"/>
-      <c r="M109" s="116"/>
-      <c r="N109" s="116"/>
+      <c r="C109" s="116"/>
+      <c r="D109" s="116"/>
+      <c r="E109" s="116"/>
+      <c r="F109" s="116"/>
+      <c r="G109" s="116"/>
+      <c r="H109" s="116"/>
+      <c r="I109" s="116"/>
+      <c r="J109" s="116"/>
+      <c r="K109" s="116"/>
+      <c r="L109" s="116"/>
+      <c r="M109" s="117"/>
+      <c r="N109" s="117"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="117"/>
-      <c r="D110" s="117"/>
-      <c r="E110" s="117"/>
-      <c r="F110" s="117"/>
-      <c r="G110" s="117"/>
-      <c r="H110" s="117"/>
-      <c r="I110" s="117"/>
-      <c r="J110" s="117"/>
-      <c r="K110" s="117"/>
-      <c r="L110" s="117"/>
-      <c r="M110" s="116"/>
-      <c r="N110" s="116"/>
+      <c r="C110" s="116"/>
+      <c r="D110" s="116"/>
+      <c r="E110" s="116"/>
+      <c r="F110" s="116"/>
+      <c r="G110" s="116"/>
+      <c r="H110" s="116"/>
+      <c r="I110" s="116"/>
+      <c r="J110" s="116"/>
+      <c r="K110" s="116"/>
+      <c r="L110" s="116"/>
+      <c r="M110" s="117"/>
+      <c r="N110" s="117"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="117"/>
-      <c r="D111" s="117"/>
-      <c r="E111" s="117"/>
-      <c r="F111" s="117"/>
-      <c r="G111" s="117"/>
-      <c r="H111" s="117"/>
-      <c r="I111" s="117"/>
-      <c r="J111" s="117"/>
-      <c r="K111" s="117"/>
-      <c r="L111" s="117"/>
-      <c r="M111" s="116"/>
-      <c r="N111" s="116"/>
+      <c r="C111" s="116"/>
+      <c r="D111" s="116"/>
+      <c r="E111" s="116"/>
+      <c r="F111" s="116"/>
+      <c r="G111" s="116"/>
+      <c r="H111" s="116"/>
+      <c r="I111" s="116"/>
+      <c r="J111" s="116"/>
+      <c r="K111" s="116"/>
+      <c r="L111" s="116"/>
+      <c r="M111" s="117"/>
+      <c r="N111" s="117"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="117"/>
-      <c r="D112" s="117"/>
-      <c r="E112" s="117"/>
-      <c r="F112" s="117"/>
-      <c r="G112" s="117"/>
-      <c r="H112" s="117"/>
-      <c r="I112" s="117"/>
-      <c r="J112" s="117"/>
-      <c r="K112" s="117"/>
-      <c r="L112" s="117"/>
-      <c r="M112" s="116"/>
-      <c r="N112" s="116"/>
+      <c r="C112" s="116"/>
+      <c r="D112" s="116"/>
+      <c r="E112" s="116"/>
+      <c r="F112" s="116"/>
+      <c r="G112" s="116"/>
+      <c r="H112" s="116"/>
+      <c r="I112" s="116"/>
+      <c r="J112" s="116"/>
+      <c r="K112" s="116"/>
+      <c r="L112" s="116"/>
+      <c r="M112" s="117"/>
+      <c r="N112" s="117"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="117"/>
-      <c r="D113" s="117"/>
-      <c r="E113" s="117"/>
-      <c r="F113" s="117"/>
-      <c r="G113" s="117"/>
-      <c r="H113" s="117"/>
-      <c r="I113" s="117"/>
-      <c r="J113" s="117"/>
-      <c r="K113" s="117"/>
-      <c r="L113" s="117"/>
-      <c r="M113" s="116"/>
-      <c r="N113" s="116"/>
+      <c r="C113" s="116"/>
+      <c r="D113" s="116"/>
+      <c r="E113" s="116"/>
+      <c r="F113" s="116"/>
+      <c r="G113" s="116"/>
+      <c r="H113" s="116"/>
+      <c r="I113" s="116"/>
+      <c r="J113" s="116"/>
+      <c r="K113" s="116"/>
+      <c r="L113" s="116"/>
+      <c r="M113" s="117"/>
+      <c r="N113" s="117"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="117"/>
-      <c r="D114" s="117"/>
-      <c r="E114" s="117"/>
-      <c r="F114" s="117"/>
-      <c r="G114" s="117"/>
-      <c r="H114" s="117"/>
-      <c r="I114" s="117"/>
-      <c r="J114" s="117"/>
-      <c r="K114" s="117"/>
-      <c r="L114" s="117"/>
-      <c r="M114" s="116"/>
-      <c r="N114" s="116"/>
+      <c r="C114" s="116"/>
+      <c r="D114" s="116"/>
+      <c r="E114" s="116"/>
+      <c r="F114" s="116"/>
+      <c r="G114" s="116"/>
+      <c r="H114" s="116"/>
+      <c r="I114" s="116"/>
+      <c r="J114" s="116"/>
+      <c r="K114" s="116"/>
+      <c r="L114" s="116"/>
+      <c r="M114" s="117"/>
+      <c r="N114" s="117"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="117"/>
-      <c r="D115" s="117"/>
-      <c r="E115" s="117"/>
-      <c r="F115" s="117"/>
-      <c r="G115" s="117"/>
-      <c r="H115" s="117"/>
-      <c r="I115" s="117"/>
-      <c r="J115" s="117"/>
-      <c r="K115" s="117"/>
-      <c r="L115" s="117"/>
-      <c r="M115" s="116"/>
-      <c r="N115" s="116"/>
+      <c r="C115" s="116"/>
+      <c r="D115" s="116"/>
+      <c r="E115" s="116"/>
+      <c r="F115" s="116"/>
+      <c r="G115" s="116"/>
+      <c r="H115" s="116"/>
+      <c r="I115" s="116"/>
+      <c r="J115" s="116"/>
+      <c r="K115" s="116"/>
+      <c r="L115" s="116"/>
+      <c r="M115" s="117"/>
+      <c r="N115" s="117"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="117"/>
-      <c r="D116" s="117"/>
-      <c r="E116" s="117"/>
-      <c r="F116" s="117"/>
-      <c r="G116" s="117"/>
-      <c r="H116" s="117"/>
-      <c r="I116" s="117"/>
-      <c r="J116" s="117"/>
-      <c r="K116" s="117"/>
-      <c r="L116" s="117"/>
-      <c r="M116" s="116"/>
-      <c r="N116" s="116"/>
+      <c r="C116" s="116"/>
+      <c r="D116" s="116"/>
+      <c r="E116" s="116"/>
+      <c r="F116" s="116"/>
+      <c r="G116" s="116"/>
+      <c r="H116" s="116"/>
+      <c r="I116" s="116"/>
+      <c r="J116" s="116"/>
+      <c r="K116" s="116"/>
+      <c r="L116" s="116"/>
+      <c r="M116" s="117"/>
+      <c r="N116" s="117"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="117"/>
-      <c r="D117" s="117"/>
-      <c r="E117" s="117"/>
-      <c r="F117" s="117"/>
-      <c r="G117" s="117"/>
-      <c r="H117" s="117"/>
-      <c r="I117" s="117"/>
-      <c r="J117" s="117"/>
-      <c r="K117" s="117"/>
-      <c r="L117" s="117"/>
-      <c r="M117" s="116"/>
-      <c r="N117" s="116"/>
+      <c r="C117" s="116"/>
+      <c r="D117" s="116"/>
+      <c r="E117" s="116"/>
+      <c r="F117" s="116"/>
+      <c r="G117" s="116"/>
+      <c r="H117" s="116"/>
+      <c r="I117" s="116"/>
+      <c r="J117" s="116"/>
+      <c r="K117" s="116"/>
+      <c r="L117" s="116"/>
+      <c r="M117" s="117"/>
+      <c r="N117" s="117"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="117"/>
-      <c r="D118" s="117"/>
-      <c r="E118" s="117"/>
-      <c r="F118" s="117"/>
-      <c r="G118" s="117"/>
-      <c r="H118" s="117"/>
-      <c r="I118" s="117"/>
-      <c r="J118" s="117"/>
-      <c r="K118" s="117"/>
-      <c r="L118" s="117"/>
-      <c r="M118" s="116"/>
-      <c r="N118" s="116"/>
+      <c r="C118" s="116"/>
+      <c r="D118" s="116"/>
+      <c r="E118" s="116"/>
+      <c r="F118" s="116"/>
+      <c r="G118" s="116"/>
+      <c r="H118" s="116"/>
+      <c r="I118" s="116"/>
+      <c r="J118" s="116"/>
+      <c r="K118" s="116"/>
+      <c r="L118" s="116"/>
+      <c r="M118" s="117"/>
+      <c r="N118" s="117"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="H54:M54"/>
+    <mergeCell ref="H58:M58"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
     <mergeCell ref="C92:G92"/>
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="Q77:R77"/>
@@ -8329,73 +8314,88 @@
     <mergeCell ref="M93:N93"/>
     <mergeCell ref="Q81:AA81"/>
     <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="H54:M54"/>
-    <mergeCell ref="H58:M58"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nerfed vector & mp5 range
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FEC62D-ADC7-4B86-B215-C2F7130FE1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEB1416-973A-4A02-B214-05787EA59878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2370,69 +2370,69 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2986,45 +2986,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="304816" cy="298920"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C046836F-8785-4B25-BC2D-DB9ADCFB8881}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38100" y="721179"/>
-          <a:ext cx="304816" cy="298920"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3587,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3606,10 +3567,10 @@
       <c r="B1" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="132"/>
+      <c r="D1" s="126"/>
       <c r="G1" s="56" t="s">
         <v>159</v>
       </c>
@@ -3705,10 +3666,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="124" t="s">
+      <c r="Z2" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="124"/>
+      <c r="AA2" s="131"/>
       <c r="AG2" s="43" t="s">
         <v>84</v>
       </c>
@@ -5606,7 +5567,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="42">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="D29" s="19">
         <v>1</v>
@@ -5691,7 +5652,7 @@
         <v>48</v>
       </c>
       <c r="C30" s="42">
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="D30" s="19">
         <v>1</v>
@@ -6110,28 +6071,28 @@
       <c r="B40" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="130" t="s">
+      <c r="C40" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="130"/>
-      <c r="E40" s="130"/>
-      <c r="F40" s="130"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="130"/>
-      <c r="I40" s="130" t="s">
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="130"/>
-      <c r="K40" s="130"/>
-      <c r="L40" s="130"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="129" t="s">
+      <c r="S40" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="129"/>
+      <c r="T40" s="132"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6141,30 +6102,30 @@
       <c r="B41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="131" t="s">
+      <c r="C41" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="131"/>
-      <c r="E41" s="131"/>
-      <c r="F41" s="131" t="s">
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="131"/>
-      <c r="H41" s="131"/>
-      <c r="I41" s="131" t="s">
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="131"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="131"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
       <c r="M41" s="109"/>
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="129" t="s">
+      <c r="S41" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="129"/>
+      <c r="T41" s="132"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -6177,30 +6138,30 @@
       <c r="B42" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="131" t="s">
+      <c r="C42" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131"/>
-      <c r="F42" s="131" t="s">
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="131"/>
-      <c r="H42" s="131"/>
-      <c r="I42" s="131" t="s">
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="131"/>
-      <c r="K42" s="131"/>
-      <c r="L42" s="131"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
       <c r="M42" s="109"/>
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="129" t="s">
+      <c r="S42" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="129"/>
+      <c r="T42" s="132"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -6213,30 +6174,30 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="127" t="s">
+      <c r="C43" s="121" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="127"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127" t="s">
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="127"/>
-      <c r="H43" s="127"/>
-      <c r="I43" s="127" t="s">
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="I43" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="127"/>
-      <c r="K43" s="127"/>
-      <c r="L43" s="127"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="121"/>
+      <c r="L43" s="121"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="129" t="s">
+      <c r="S43" s="132" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="129"/>
+      <c r="T43" s="132"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -6251,20 +6212,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="127" t="s">
+      <c r="C44" s="121" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="127"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="127" t="s">
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="121" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="127"/>
-      <c r="K44" s="127"/>
-      <c r="L44" s="127"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="121"/>
+      <c r="L44" s="121"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
       <c r="O44" s="109"/>
@@ -6280,16 +6241,16 @@
       <c r="B47" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="130" t="s">
+      <c r="C47" s="119" t="s">
         <v>192</v>
       </c>
-      <c r="D47" s="130"/>
-      <c r="E47" s="130" t="s">
+      <c r="D47" s="119"/>
+      <c r="E47" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="130"/>
-      <c r="G47" s="130"/>
-      <c r="H47" s="130"/>
+      <c r="F47" s="119"/>
+      <c r="G47" s="119"/>
+      <c r="H47" s="119"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -6300,16 +6261,16 @@
       <c r="B48" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="131">
+      <c r="C48" s="120">
         <v>2</v>
       </c>
-      <c r="D48" s="131"/>
-      <c r="E48" s="131" t="s">
+      <c r="D48" s="120"/>
+      <c r="E48" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
       <c r="I48" s="110"/>
       <c r="J48" s="110"/>
     </row>
@@ -6320,28 +6281,28 @@
       <c r="B49" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="131" t="s">
+      <c r="C49" s="120" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="131"/>
-      <c r="E49" s="131" t="s">
+      <c r="D49" s="120"/>
+      <c r="E49" s="120" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="131"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="120"/>
       <c r="I49" s="110"/>
       <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="127"/>
-      <c r="D50" s="127"/>
-      <c r="E50" s="127"/>
-      <c r="F50" s="127"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="127"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="121"/>
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
@@ -6359,14 +6320,14 @@
       <c r="D54" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="136" t="s">
+      <c r="H54" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="136"/>
-      <c r="J54" s="136"/>
-      <c r="K54" s="136"/>
-      <c r="L54" s="136"/>
-      <c r="M54" s="136"/>
+      <c r="I54" s="124"/>
+      <c r="J54" s="124"/>
+      <c r="K54" s="124"/>
+      <c r="L54" s="124"/>
+      <c r="M54" s="124"/>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="91"/>
@@ -6517,14 +6478,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="137" t="s">
+      <c r="H58" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="137"/>
-      <c r="J58" s="137"/>
-      <c r="K58" s="137"/>
-      <c r="L58" s="137"/>
-      <c r="M58" s="137"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="125"/>
+      <c r="L58" s="125"/>
+      <c r="M58" s="125"/>
     </row>
     <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6573,10 +6534,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="134" t="s">
+      <c r="J62" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="134"/>
+      <c r="K62" s="128"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -6584,13 +6545,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="133" t="s">
+      <c r="O62" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="133"/>
-      <c r="Q62" s="133"/>
-      <c r="R62" s="133"/>
-      <c r="S62" s="133"/>
+      <c r="P62" s="127"/>
+      <c r="Q62" s="127"/>
+      <c r="R62" s="127"/>
+      <c r="S62" s="127"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6612,20 +6573,20 @@
       <c r="E63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="119" t="s">
+      <c r="F63" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="119"/>
+      <c r="G63" s="133"/>
       <c r="H63" s="86" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="119" t="s">
+      <c r="J63" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="119"/>
+      <c r="K63" s="133"/>
       <c r="L63" s="86" t="s">
         <v>102</v>
       </c>
@@ -6649,10 +6610,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="119" t="s">
+      <c r="U63" s="133" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="119"/>
+      <c r="V63" s="133"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6680,21 +6641,21 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="135" t="s">
+      <c r="F64" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="135"/>
+      <c r="G64" s="134"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="122">
+      <c r="J64" s="123">
         <f t="shared" ref="J64:J69" si="31">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="122"/>
+      <c r="K64" s="123"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -6725,11 +6686,11 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="120">
+      <c r="U64" s="136">
         <f>R64+O64+P64</f>
         <v>3.8</v>
       </c>
-      <c r="V64" s="120"/>
+      <c r="V64" s="136"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6757,21 +6718,21 @@
       <c r="E65" s="54">
         <v>4</v>
       </c>
-      <c r="F65" s="117" t="s">
+      <c r="F65" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="117"/>
+      <c r="G65" s="116"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="122">
+      <c r="J65" s="123">
         <f t="shared" si="31"/>
         <v>32</v>
       </c>
-      <c r="K65" s="122"/>
+      <c r="K65" s="123"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6802,11 +6763,11 @@
         <v>13.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="121">
+      <c r="U65" s="137">
         <f t="shared" ref="U65:U70" si="38">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="121"/>
+      <c r="V65" s="137"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6834,21 +6795,21 @@
       <c r="E66" s="54">
         <v>3</v>
       </c>
-      <c r="F66" s="117" t="s">
+      <c r="F66" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="117"/>
+      <c r="G66" s="116"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="122">
+      <c r="J66" s="123">
         <f t="shared" si="31"/>
         <v>28</v>
       </c>
-      <c r="K66" s="122"/>
+      <c r="K66" s="123"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6879,11 +6840,11 @@
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="121">
+      <c r="U66" s="137">
         <f t="shared" si="38"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="121"/>
+      <c r="V66" s="137"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6911,21 +6872,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="117" t="s">
+      <c r="F67" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="117"/>
+      <c r="G67" s="116"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="122">
+      <c r="J67" s="123">
         <f t="shared" si="31"/>
         <v>48</v>
       </c>
-      <c r="K67" s="122"/>
+      <c r="K67" s="123"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6956,11 +6917,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="121">
+      <c r="U67" s="137">
         <f t="shared" si="38"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="121"/>
+      <c r="V67" s="137"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6984,21 +6945,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="117" t="s">
+      <c r="F68" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="117"/>
+      <c r="G68" s="116"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="122">
+      <c r="J68" s="123">
         <f t="shared" si="31"/>
         <v>72</v>
       </c>
-      <c r="K68" s="122"/>
+      <c r="K68" s="123"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7029,11 +6990,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="121">
+      <c r="U68" s="137">
         <f t="shared" si="38"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="121"/>
+      <c r="V68" s="137"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7057,21 +7018,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="117" t="s">
+      <c r="F69" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="117"/>
+      <c r="G69" s="116"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="122">
+      <c r="J69" s="123">
         <f t="shared" si="31"/>
         <v>20</v>
       </c>
-      <c r="K69" s="122"/>
+      <c r="K69" s="123"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7102,11 +7063,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="121">
+      <c r="U69" s="137">
         <f t="shared" si="38"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="121"/>
+      <c r="V69" s="137"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7130,21 +7091,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="117"/>
+      <c r="G70" s="116"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="122">
+      <c r="J70" s="123">
         <f t="shared" ref="J70" si="39">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="122"/>
+      <c r="K70" s="123"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7175,11 +7136,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="121">
+      <c r="U70" s="137">
         <f t="shared" si="38"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="121"/>
+      <c r="V70" s="137"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7192,12 +7153,12 @@
     <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="O73" s="124" t="s">
+      <c r="O73" s="131" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="124"/>
-      <c r="Q73" s="124"/>
-      <c r="R73" s="124"/>
+      <c r="P73" s="131"/>
+      <c r="Q73" s="131"/>
+      <c r="R73" s="131"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="35"/>
@@ -7213,31 +7174,31 @@
       <c r="E74" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="123" t="s">
+      <c r="F74" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="123"/>
-      <c r="H74" s="123" t="s">
+      <c r="G74" s="122"/>
+      <c r="H74" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="123"/>
-      <c r="J74" s="123" t="s">
+      <c r="I74" s="122"/>
+      <c r="J74" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="123"/>
-      <c r="L74" s="123"/>
-      <c r="M74" s="123"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="122"/>
+      <c r="M74" s="122"/>
       <c r="N74" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="123" t="s">
+      <c r="O74" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="123"/>
-      <c r="Q74" s="123" t="s">
+      <c r="P74" s="122"/>
+      <c r="Q74" s="122" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="123"/>
+      <c r="R74" s="122"/>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="38" t="e" vm="29">
@@ -7255,21 +7216,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="122" t="s">
+      <c r="F75" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122">
+      <c r="G75" s="123"/>
+      <c r="H75" s="123">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="122"/>
-      <c r="J75" s="122" t="s">
+      <c r="I75" s="123"/>
+      <c r="J75" s="123" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="122"/>
-      <c r="L75" s="122"/>
-      <c r="M75" s="122"/>
+      <c r="K75" s="123"/>
+      <c r="L75" s="123"/>
+      <c r="M75" s="123"/>
       <c r="N75" s="78" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7298,21 +7259,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="122" t="s">
+      <c r="F76" s="123" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="122"/>
-      <c r="H76" s="122">
+      <c r="G76" s="123"/>
+      <c r="H76" s="123">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="122"/>
-      <c r="J76" s="122" t="s">
+      <c r="I76" s="123"/>
+      <c r="J76" s="123" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="122"/>
-      <c r="L76" s="122"/>
-      <c r="M76" s="122"/>
+      <c r="K76" s="123"/>
+      <c r="L76" s="123"/>
+      <c r="M76" s="123"/>
       <c r="N76" s="78" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7331,19 +7292,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="127"/>
-      <c r="G77" s="127"/>
-      <c r="H77" s="127"/>
-      <c r="I77" s="127"/>
-      <c r="J77" s="127"/>
-      <c r="K77" s="127"/>
-      <c r="L77" s="127"/>
-      <c r="M77" s="127"/>
+      <c r="F77" s="121"/>
+      <c r="G77" s="121"/>
+      <c r="H77" s="121"/>
+      <c r="I77" s="121"/>
+      <c r="J77" s="121"/>
+      <c r="K77" s="121"/>
+      <c r="L77" s="121"/>
+      <c r="M77" s="121"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="125"/>
-      <c r="P77" s="125"/>
-      <c r="Q77" s="125"/>
-      <c r="R77" s="125"/>
+      <c r="O77" s="129"/>
+      <c r="P77" s="129"/>
+      <c r="Q77" s="129"/>
+      <c r="R77" s="129"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="112" t="s">
@@ -7371,32 +7332,32 @@
       <c r="E81" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="123" t="s">
+      <c r="F81" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="123"/>
-      <c r="H81" s="123"/>
-      <c r="I81" s="123"/>
-      <c r="J81" s="123"/>
-      <c r="K81" s="123"/>
-      <c r="L81" s="123"/>
-      <c r="M81" s="123"/>
-      <c r="N81" s="123"/>
-      <c r="O81" s="123"/>
-      <c r="P81" s="123"/>
-      <c r="Q81" s="123" t="s">
+      <c r="G81" s="122"/>
+      <c r="H81" s="122"/>
+      <c r="I81" s="122"/>
+      <c r="J81" s="122"/>
+      <c r="K81" s="122"/>
+      <c r="L81" s="122"/>
+      <c r="M81" s="122"/>
+      <c r="N81" s="122"/>
+      <c r="O81" s="122"/>
+      <c r="P81" s="122"/>
+      <c r="Q81" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="123"/>
-      <c r="S81" s="123"/>
-      <c r="T81" s="123"/>
-      <c r="U81" s="123"/>
-      <c r="V81" s="123"/>
-      <c r="W81" s="123"/>
-      <c r="X81" s="123"/>
-      <c r="Y81" s="123"/>
-      <c r="Z81" s="123"/>
-      <c r="AA81" s="123"/>
+      <c r="R81" s="122"/>
+      <c r="S81" s="122"/>
+      <c r="T81" s="122"/>
+      <c r="U81" s="122"/>
+      <c r="V81" s="122"/>
+      <c r="W81" s="122"/>
+      <c r="X81" s="122"/>
+      <c r="Y81" s="122"/>
+      <c r="Z81" s="122"/>
+      <c r="AA81" s="122"/>
     </row>
     <row r="82" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="38"/>
@@ -7412,32 +7373,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="128" t="s">
+      <c r="F82" s="135" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="128"/>
-      <c r="H82" s="128"/>
-      <c r="I82" s="128"/>
-      <c r="J82" s="128"/>
-      <c r="K82" s="128"/>
-      <c r="L82" s="128"/>
-      <c r="M82" s="128"/>
-      <c r="N82" s="128"/>
-      <c r="O82" s="128"/>
-      <c r="P82" s="128"/>
-      <c r="Q82" s="128" t="s">
+      <c r="G82" s="135"/>
+      <c r="H82" s="135"/>
+      <c r="I82" s="135"/>
+      <c r="J82" s="135"/>
+      <c r="K82" s="135"/>
+      <c r="L82" s="135"/>
+      <c r="M82" s="135"/>
+      <c r="N82" s="135"/>
+      <c r="O82" s="135"/>
+      <c r="P82" s="135"/>
+      <c r="Q82" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="128"/>
-      <c r="S82" s="128"/>
-      <c r="T82" s="128"/>
-      <c r="U82" s="128"/>
-      <c r="V82" s="128"/>
-      <c r="W82" s="128"/>
-      <c r="X82" s="128"/>
-      <c r="Y82" s="128"/>
-      <c r="Z82" s="128"/>
-      <c r="AA82" s="128"/>
+      <c r="R82" s="135"/>
+      <c r="S82" s="135"/>
+      <c r="T82" s="135"/>
+      <c r="U82" s="135"/>
+      <c r="V82" s="135"/>
+      <c r="W82" s="135"/>
+      <c r="X82" s="135"/>
+      <c r="Y82" s="135"/>
+      <c r="Z82" s="135"/>
+      <c r="AA82" s="135"/>
     </row>
     <row r="83" spans="1:27" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="38"/>
@@ -7627,24 +7588,24 @@
       <c r="B90" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="126" t="s">
+      <c r="C90" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="126"/>
-      <c r="E90" s="126"/>
-      <c r="F90" s="126"/>
-      <c r="G90" s="126"/>
-      <c r="H90" s="126" t="s">
+      <c r="D90" s="130"/>
+      <c r="E90" s="130"/>
+      <c r="F90" s="130"/>
+      <c r="G90" s="130"/>
+      <c r="H90" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="126"/>
-      <c r="J90" s="126"/>
-      <c r="K90" s="126"/>
-      <c r="L90" s="126"/>
-      <c r="M90" s="123" t="s">
+      <c r="I90" s="130"/>
+      <c r="J90" s="130"/>
+      <c r="K90" s="130"/>
+      <c r="L90" s="130"/>
+      <c r="M90" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="123"/>
+      <c r="N90" s="122"/>
       <c r="O90" s="107"/>
       <c r="T90" s="58" t="s">
         <v>197</v>
@@ -7657,24 +7618,24 @@
       <c r="B91" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="116" t="s">
+      <c r="C91" s="117" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="116"/>
-      <c r="E91" s="116"/>
-      <c r="F91" s="116"/>
-      <c r="G91" s="116"/>
-      <c r="H91" s="116" t="s">
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="117"/>
+      <c r="G91" s="117"/>
+      <c r="H91" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="116"/>
-      <c r="J91" s="116"/>
-      <c r="K91" s="116"/>
-      <c r="L91" s="116"/>
-      <c r="M91" s="117" t="s">
+      <c r="I91" s="117"/>
+      <c r="J91" s="117"/>
+      <c r="K91" s="117"/>
+      <c r="L91" s="117"/>
+      <c r="M91" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="117"/>
+      <c r="N91" s="116"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7684,24 +7645,24 @@
       <c r="B92" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="116" t="s">
+      <c r="C92" s="117" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="116"/>
-      <c r="E92" s="116"/>
-      <c r="F92" s="116"/>
-      <c r="G92" s="116"/>
-      <c r="H92" s="116" t="s">
+      <c r="D92" s="117"/>
+      <c r="E92" s="117"/>
+      <c r="F92" s="117"/>
+      <c r="G92" s="117"/>
+      <c r="H92" s="117" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="116"/>
-      <c r="J92" s="116"/>
-      <c r="K92" s="116"/>
-      <c r="L92" s="116"/>
-      <c r="M92" s="117" t="s">
+      <c r="I92" s="117"/>
+      <c r="J92" s="117"/>
+      <c r="K92" s="117"/>
+      <c r="L92" s="117"/>
+      <c r="M92" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="117"/>
+      <c r="N92" s="116"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7711,24 +7672,24 @@
       <c r="B93" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="116" t="s">
+      <c r="C93" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D93" s="116"/>
-      <c r="E93" s="116"/>
-      <c r="F93" s="116"/>
-      <c r="G93" s="116"/>
-      <c r="H93" s="116" t="s">
+      <c r="D93" s="117"/>
+      <c r="E93" s="117"/>
+      <c r="F93" s="117"/>
+      <c r="G93" s="117"/>
+      <c r="H93" s="117" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="116"/>
-      <c r="J93" s="116"/>
-      <c r="K93" s="116"/>
-      <c r="L93" s="116"/>
-      <c r="M93" s="117" t="s">
+      <c r="I93" s="117"/>
+      <c r="J93" s="117"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="117"/>
+      <c r="M93" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="117"/>
+      <c r="N93" s="116"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7738,24 +7699,24 @@
       <c r="B94" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="116" t="s">
+      <c r="C94" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="116"/>
-      <c r="E94" s="116"/>
-      <c r="F94" s="116"/>
-      <c r="G94" s="116"/>
-      <c r="H94" s="116" t="s">
+      <c r="D94" s="117"/>
+      <c r="E94" s="117"/>
+      <c r="F94" s="117"/>
+      <c r="G94" s="117"/>
+      <c r="H94" s="117" t="s">
         <v>218</v>
       </c>
-      <c r="I94" s="116"/>
-      <c r="J94" s="116"/>
-      <c r="K94" s="116"/>
-      <c r="L94" s="116"/>
-      <c r="M94" s="117" t="s">
+      <c r="I94" s="117"/>
+      <c r="J94" s="117"/>
+      <c r="K94" s="117"/>
+      <c r="L94" s="117"/>
+      <c r="M94" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="117"/>
+      <c r="N94" s="116"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7765,24 +7726,24 @@
       <c r="B95" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C95" s="116" t="s">
+      <c r="C95" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D95" s="116"/>
-      <c r="E95" s="116"/>
-      <c r="F95" s="116"/>
-      <c r="G95" s="116"/>
-      <c r="H95" s="116" t="s">
+      <c r="D95" s="117"/>
+      <c r="E95" s="117"/>
+      <c r="F95" s="117"/>
+      <c r="G95" s="117"/>
+      <c r="H95" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="I95" s="116"/>
-      <c r="J95" s="116"/>
-      <c r="K95" s="116"/>
-      <c r="L95" s="116"/>
-      <c r="M95" s="117" t="s">
+      <c r="I95" s="117"/>
+      <c r="J95" s="117"/>
+      <c r="K95" s="117"/>
+      <c r="L95" s="117"/>
+      <c r="M95" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="117"/>
+      <c r="N95" s="116"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7792,24 +7753,24 @@
       <c r="B96" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="116" t="s">
+      <c r="C96" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D96" s="116"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="116"/>
-      <c r="G96" s="116"/>
-      <c r="H96" s="116" t="s">
+      <c r="D96" s="117"/>
+      <c r="E96" s="117"/>
+      <c r="F96" s="117"/>
+      <c r="G96" s="117"/>
+      <c r="H96" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="I96" s="116"/>
-      <c r="J96" s="116"/>
-      <c r="K96" s="116"/>
-      <c r="L96" s="116"/>
-      <c r="M96" s="117" t="s">
+      <c r="I96" s="117"/>
+      <c r="J96" s="117"/>
+      <c r="K96" s="117"/>
+      <c r="L96" s="117"/>
+      <c r="M96" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="117"/>
+      <c r="N96" s="116"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7819,24 +7780,24 @@
       <c r="B97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="116" t="s">
+      <c r="C97" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D97" s="116"/>
-      <c r="E97" s="116"/>
-      <c r="F97" s="116"/>
-      <c r="G97" s="116"/>
-      <c r="H97" s="116" t="s">
+      <c r="D97" s="117"/>
+      <c r="E97" s="117"/>
+      <c r="F97" s="117"/>
+      <c r="G97" s="117"/>
+      <c r="H97" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="I97" s="116"/>
-      <c r="J97" s="116"/>
-      <c r="K97" s="116"/>
-      <c r="L97" s="116"/>
-      <c r="M97" s="117" t="s">
+      <c r="I97" s="117"/>
+      <c r="J97" s="117"/>
+      <c r="K97" s="117"/>
+      <c r="L97" s="117"/>
+      <c r="M97" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="117"/>
+      <c r="N97" s="116"/>
       <c r="O97" s="65"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -7846,24 +7807,24 @@
       <c r="B98" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="116" t="s">
+      <c r="C98" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="116"/>
-      <c r="E98" s="116"/>
-      <c r="F98" s="116"/>
-      <c r="G98" s="116"/>
-      <c r="H98" s="116" t="s">
+      <c r="D98" s="117"/>
+      <c r="E98" s="117"/>
+      <c r="F98" s="117"/>
+      <c r="G98" s="117"/>
+      <c r="H98" s="117" t="s">
         <v>222</v>
       </c>
-      <c r="I98" s="116"/>
-      <c r="J98" s="116"/>
-      <c r="K98" s="116"/>
-      <c r="L98" s="116"/>
-      <c r="M98" s="117" t="s">
+      <c r="I98" s="117"/>
+      <c r="J98" s="117"/>
+      <c r="K98" s="117"/>
+      <c r="L98" s="117"/>
+      <c r="M98" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="117"/>
+      <c r="N98" s="116"/>
       <c r="O98" s="65"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7873,24 +7834,24 @@
       <c r="B99" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C99" s="116" t="s">
+      <c r="C99" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="116"/>
-      <c r="E99" s="116"/>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116" t="s">
+      <c r="D99" s="117"/>
+      <c r="E99" s="117"/>
+      <c r="F99" s="117"/>
+      <c r="G99" s="117"/>
+      <c r="H99" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="I99" s="116"/>
-      <c r="J99" s="116"/>
-      <c r="K99" s="116"/>
-      <c r="L99" s="116"/>
-      <c r="M99" s="117" t="s">
+      <c r="I99" s="117"/>
+      <c r="J99" s="117"/>
+      <c r="K99" s="117"/>
+      <c r="L99" s="117"/>
+      <c r="M99" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="117"/>
+      <c r="N99" s="116"/>
       <c r="O99" s="65"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -7900,329 +7861,478 @@
       <c r="B100" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C100" s="116" t="s">
+      <c r="C100" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="116"/>
-      <c r="E100" s="116"/>
-      <c r="F100" s="116"/>
-      <c r="G100" s="116"/>
-      <c r="H100" s="116" t="s">
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="116"/>
-      <c r="J100" s="116"/>
-      <c r="K100" s="116"/>
-      <c r="L100" s="116"/>
-      <c r="M100" s="117" t="s">
+      <c r="I100" s="117"/>
+      <c r="J100" s="117"/>
+      <c r="K100" s="117"/>
+      <c r="L100" s="117"/>
+      <c r="M100" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="117"/>
+      <c r="N100" s="116"/>
       <c r="O100" s="65"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
-      <c r="C101" s="116"/>
-      <c r="D101" s="116"/>
-      <c r="E101" s="116"/>
-      <c r="F101" s="116"/>
-      <c r="G101" s="116"/>
-      <c r="H101" s="116"/>
-      <c r="I101" s="116"/>
-      <c r="J101" s="116"/>
-      <c r="K101" s="116"/>
-      <c r="L101" s="116"/>
-      <c r="M101" s="117"/>
-      <c r="N101" s="117"/>
+      <c r="C101" s="117"/>
+      <c r="D101" s="117"/>
+      <c r="E101" s="117"/>
+      <c r="F101" s="117"/>
+      <c r="G101" s="117"/>
+      <c r="H101" s="117"/>
+      <c r="I101" s="117"/>
+      <c r="J101" s="117"/>
+      <c r="K101" s="117"/>
+      <c r="L101" s="117"/>
+      <c r="M101" s="116"/>
+      <c r="N101" s="116"/>
       <c r="O101" s="65"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
-      <c r="H102" s="116"/>
-      <c r="I102" s="116"/>
-      <c r="J102" s="116"/>
-      <c r="K102" s="116"/>
-      <c r="L102" s="116"/>
-      <c r="M102" s="117"/>
-      <c r="N102" s="117"/>
+      <c r="H102" s="117"/>
+      <c r="I102" s="117"/>
+      <c r="J102" s="117"/>
+      <c r="K102" s="117"/>
+      <c r="L102" s="117"/>
+      <c r="M102" s="116"/>
+      <c r="N102" s="116"/>
       <c r="O102" s="65"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
-      <c r="C103" s="116"/>
-      <c r="D103" s="116"/>
-      <c r="E103" s="116"/>
-      <c r="F103" s="116"/>
-      <c r="G103" s="116"/>
-      <c r="H103" s="116"/>
-      <c r="I103" s="116"/>
-      <c r="J103" s="116"/>
-      <c r="K103" s="116"/>
-      <c r="L103" s="116"/>
-      <c r="M103" s="117"/>
-      <c r="N103" s="117"/>
+      <c r="C103" s="117"/>
+      <c r="D103" s="117"/>
+      <c r="E103" s="117"/>
+      <c r="F103" s="117"/>
+      <c r="G103" s="117"/>
+      <c r="H103" s="117"/>
+      <c r="I103" s="117"/>
+      <c r="J103" s="117"/>
+      <c r="K103" s="117"/>
+      <c r="L103" s="117"/>
+      <c r="M103" s="116"/>
+      <c r="N103" s="116"/>
       <c r="O103" s="65"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="38"/>
       <c r="B104" s="38"/>
-      <c r="C104" s="116"/>
-      <c r="D104" s="116"/>
-      <c r="E104" s="116"/>
-      <c r="F104" s="116"/>
-      <c r="G104" s="116"/>
-      <c r="H104" s="116"/>
-      <c r="I104" s="116"/>
-      <c r="J104" s="116"/>
-      <c r="K104" s="116"/>
-      <c r="L104" s="116"/>
-      <c r="M104" s="117"/>
-      <c r="N104" s="117"/>
+      <c r="C104" s="117"/>
+      <c r="D104" s="117"/>
+      <c r="E104" s="117"/>
+      <c r="F104" s="117"/>
+      <c r="G104" s="117"/>
+      <c r="H104" s="117"/>
+      <c r="I104" s="117"/>
+      <c r="J104" s="117"/>
+      <c r="K104" s="117"/>
+      <c r="L104" s="117"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
       <c r="O104" s="65"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="38"/>
       <c r="B105" s="38"/>
-      <c r="C105" s="116"/>
-      <c r="D105" s="116"/>
-      <c r="E105" s="116"/>
-      <c r="F105" s="116"/>
-      <c r="G105" s="116"/>
-      <c r="H105" s="116"/>
-      <c r="I105" s="116"/>
-      <c r="J105" s="116"/>
-      <c r="K105" s="116"/>
-      <c r="L105" s="116"/>
-      <c r="M105" s="117"/>
-      <c r="N105" s="117"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
+      <c r="M105" s="116"/>
+      <c r="N105" s="116"/>
       <c r="O105" s="65"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="38"/>
       <c r="B106" s="38"/>
-      <c r="C106" s="116"/>
-      <c r="D106" s="116"/>
-      <c r="E106" s="116"/>
-      <c r="F106" s="116"/>
-      <c r="G106" s="116"/>
-      <c r="H106" s="116"/>
-      <c r="I106" s="116"/>
-      <c r="J106" s="116"/>
-      <c r="K106" s="116"/>
-      <c r="L106" s="116"/>
-      <c r="M106" s="117"/>
-      <c r="N106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
+      <c r="M106" s="116"/>
+      <c r="N106" s="116"/>
       <c r="O106" s="65"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
-      <c r="C107" s="116"/>
-      <c r="D107" s="116"/>
-      <c r="E107" s="116"/>
-      <c r="F107" s="116"/>
-      <c r="G107" s="116"/>
-      <c r="H107" s="116"/>
-      <c r="I107" s="116"/>
-      <c r="J107" s="116"/>
-      <c r="K107" s="116"/>
-      <c r="L107" s="116"/>
-      <c r="M107" s="117"/>
-      <c r="N107" s="117"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="117"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="117"/>
+      <c r="J107" s="117"/>
+      <c r="K107" s="117"/>
+      <c r="L107" s="117"/>
+      <c r="M107" s="116"/>
+      <c r="N107" s="116"/>
       <c r="O107" s="65"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
-      <c r="C108" s="116"/>
-      <c r="D108" s="116"/>
-      <c r="E108" s="116"/>
-      <c r="F108" s="116"/>
-      <c r="G108" s="116"/>
-      <c r="H108" s="116"/>
-      <c r="I108" s="116"/>
-      <c r="J108" s="116"/>
-      <c r="K108" s="116"/>
-      <c r="L108" s="116"/>
-      <c r="M108" s="117"/>
-      <c r="N108" s="117"/>
+      <c r="C108" s="117"/>
+      <c r="D108" s="117"/>
+      <c r="E108" s="117"/>
+      <c r="F108" s="117"/>
+      <c r="G108" s="117"/>
+      <c r="H108" s="117"/>
+      <c r="I108" s="117"/>
+      <c r="J108" s="117"/>
+      <c r="K108" s="117"/>
+      <c r="L108" s="117"/>
+      <c r="M108" s="116"/>
+      <c r="N108" s="116"/>
       <c r="O108" s="65"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="38"/>
       <c r="B109" s="38"/>
-      <c r="C109" s="116"/>
-      <c r="D109" s="116"/>
-      <c r="E109" s="116"/>
-      <c r="F109" s="116"/>
-      <c r="G109" s="116"/>
-      <c r="H109" s="116"/>
-      <c r="I109" s="116"/>
-      <c r="J109" s="116"/>
-      <c r="K109" s="116"/>
-      <c r="L109" s="116"/>
-      <c r="M109" s="117"/>
-      <c r="N109" s="117"/>
+      <c r="C109" s="117"/>
+      <c r="D109" s="117"/>
+      <c r="E109" s="117"/>
+      <c r="F109" s="117"/>
+      <c r="G109" s="117"/>
+      <c r="H109" s="117"/>
+      <c r="I109" s="117"/>
+      <c r="J109" s="117"/>
+      <c r="K109" s="117"/>
+      <c r="L109" s="117"/>
+      <c r="M109" s="116"/>
+      <c r="N109" s="116"/>
       <c r="O109" s="65"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="38"/>
       <c r="B110" s="38"/>
-      <c r="C110" s="116"/>
-      <c r="D110" s="116"/>
-      <c r="E110" s="116"/>
-      <c r="F110" s="116"/>
-      <c r="G110" s="116"/>
-      <c r="H110" s="116"/>
-      <c r="I110" s="116"/>
-      <c r="J110" s="116"/>
-      <c r="K110" s="116"/>
-      <c r="L110" s="116"/>
-      <c r="M110" s="117"/>
-      <c r="N110" s="117"/>
+      <c r="C110" s="117"/>
+      <c r="D110" s="117"/>
+      <c r="E110" s="117"/>
+      <c r="F110" s="117"/>
+      <c r="G110" s="117"/>
+      <c r="H110" s="117"/>
+      <c r="I110" s="117"/>
+      <c r="J110" s="117"/>
+      <c r="K110" s="117"/>
+      <c r="L110" s="117"/>
+      <c r="M110" s="116"/>
+      <c r="N110" s="116"/>
       <c r="O110" s="65"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="38"/>
       <c r="B111" s="38"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="116"/>
-      <c r="E111" s="116"/>
-      <c r="F111" s="116"/>
-      <c r="G111" s="116"/>
-      <c r="H111" s="116"/>
-      <c r="I111" s="116"/>
-      <c r="J111" s="116"/>
-      <c r="K111" s="116"/>
-      <c r="L111" s="116"/>
-      <c r="M111" s="117"/>
-      <c r="N111" s="117"/>
+      <c r="C111" s="117"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="117"/>
+      <c r="F111" s="117"/>
+      <c r="G111" s="117"/>
+      <c r="H111" s="117"/>
+      <c r="I111" s="117"/>
+      <c r="J111" s="117"/>
+      <c r="K111" s="117"/>
+      <c r="L111" s="117"/>
+      <c r="M111" s="116"/>
+      <c r="N111" s="116"/>
       <c r="O111" s="65"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="38"/>
       <c r="B112" s="38"/>
-      <c r="C112" s="116"/>
-      <c r="D112" s="116"/>
-      <c r="E112" s="116"/>
-      <c r="F112" s="116"/>
-      <c r="G112" s="116"/>
-      <c r="H112" s="116"/>
-      <c r="I112" s="116"/>
-      <c r="J112" s="116"/>
-      <c r="K112" s="116"/>
-      <c r="L112" s="116"/>
-      <c r="M112" s="117"/>
-      <c r="N112" s="117"/>
+      <c r="C112" s="117"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="117"/>
+      <c r="F112" s="117"/>
+      <c r="G112" s="117"/>
+      <c r="H112" s="117"/>
+      <c r="I112" s="117"/>
+      <c r="J112" s="117"/>
+      <c r="K112" s="117"/>
+      <c r="L112" s="117"/>
+      <c r="M112" s="116"/>
+      <c r="N112" s="116"/>
       <c r="O112" s="65"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="38"/>
       <c r="B113" s="38"/>
-      <c r="C113" s="116"/>
-      <c r="D113" s="116"/>
-      <c r="E113" s="116"/>
-      <c r="F113" s="116"/>
-      <c r="G113" s="116"/>
-      <c r="H113" s="116"/>
-      <c r="I113" s="116"/>
-      <c r="J113" s="116"/>
-      <c r="K113" s="116"/>
-      <c r="L113" s="116"/>
-      <c r="M113" s="117"/>
-      <c r="N113" s="117"/>
+      <c r="C113" s="117"/>
+      <c r="D113" s="117"/>
+      <c r="E113" s="117"/>
+      <c r="F113" s="117"/>
+      <c r="G113" s="117"/>
+      <c r="H113" s="117"/>
+      <c r="I113" s="117"/>
+      <c r="J113" s="117"/>
+      <c r="K113" s="117"/>
+      <c r="L113" s="117"/>
+      <c r="M113" s="116"/>
+      <c r="N113" s="116"/>
       <c r="O113" s="65"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
-      <c r="C114" s="116"/>
-      <c r="D114" s="116"/>
-      <c r="E114" s="116"/>
-      <c r="F114" s="116"/>
-      <c r="G114" s="116"/>
-      <c r="H114" s="116"/>
-      <c r="I114" s="116"/>
-      <c r="J114" s="116"/>
-      <c r="K114" s="116"/>
-      <c r="L114" s="116"/>
-      <c r="M114" s="117"/>
-      <c r="N114" s="117"/>
+      <c r="C114" s="117"/>
+      <c r="D114" s="117"/>
+      <c r="E114" s="117"/>
+      <c r="F114" s="117"/>
+      <c r="G114" s="117"/>
+      <c r="H114" s="117"/>
+      <c r="I114" s="117"/>
+      <c r="J114" s="117"/>
+      <c r="K114" s="117"/>
+      <c r="L114" s="117"/>
+      <c r="M114" s="116"/>
+      <c r="N114" s="116"/>
       <c r="O114" s="65"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
-      <c r="C115" s="116"/>
-      <c r="D115" s="116"/>
-      <c r="E115" s="116"/>
-      <c r="F115" s="116"/>
-      <c r="G115" s="116"/>
-      <c r="H115" s="116"/>
-      <c r="I115" s="116"/>
-      <c r="J115" s="116"/>
-      <c r="K115" s="116"/>
-      <c r="L115" s="116"/>
-      <c r="M115" s="117"/>
-      <c r="N115" s="117"/>
+      <c r="C115" s="117"/>
+      <c r="D115" s="117"/>
+      <c r="E115" s="117"/>
+      <c r="F115" s="117"/>
+      <c r="G115" s="117"/>
+      <c r="H115" s="117"/>
+      <c r="I115" s="117"/>
+      <c r="J115" s="117"/>
+      <c r="K115" s="117"/>
+      <c r="L115" s="117"/>
+      <c r="M115" s="116"/>
+      <c r="N115" s="116"/>
       <c r="O115" s="65"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="38"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="116"/>
-      <c r="D116" s="116"/>
-      <c r="E116" s="116"/>
-      <c r="F116" s="116"/>
-      <c r="G116" s="116"/>
-      <c r="H116" s="116"/>
-      <c r="I116" s="116"/>
-      <c r="J116" s="116"/>
-      <c r="K116" s="116"/>
-      <c r="L116" s="116"/>
-      <c r="M116" s="117"/>
-      <c r="N116" s="117"/>
+      <c r="C116" s="117"/>
+      <c r="D116" s="117"/>
+      <c r="E116" s="117"/>
+      <c r="F116" s="117"/>
+      <c r="G116" s="117"/>
+      <c r="H116" s="117"/>
+      <c r="I116" s="117"/>
+      <c r="J116" s="117"/>
+      <c r="K116" s="117"/>
+      <c r="L116" s="117"/>
+      <c r="M116" s="116"/>
+      <c r="N116" s="116"/>
       <c r="O116" s="65"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="38"/>
       <c r="B117" s="38"/>
-      <c r="C117" s="116"/>
-      <c r="D117" s="116"/>
-      <c r="E117" s="116"/>
-      <c r="F117" s="116"/>
-      <c r="G117" s="116"/>
-      <c r="H117" s="116"/>
-      <c r="I117" s="116"/>
-      <c r="J117" s="116"/>
-      <c r="K117" s="116"/>
-      <c r="L117" s="116"/>
-      <c r="M117" s="117"/>
-      <c r="N117" s="117"/>
+      <c r="C117" s="117"/>
+      <c r="D117" s="117"/>
+      <c r="E117" s="117"/>
+      <c r="F117" s="117"/>
+      <c r="G117" s="117"/>
+      <c r="H117" s="117"/>
+      <c r="I117" s="117"/>
+      <c r="J117" s="117"/>
+      <c r="K117" s="117"/>
+      <c r="L117" s="117"/>
+      <c r="M117" s="116"/>
+      <c r="N117" s="116"/>
       <c r="O117" s="65"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="116"/>
-      <c r="D118" s="116"/>
-      <c r="E118" s="116"/>
-      <c r="F118" s="116"/>
-      <c r="G118" s="116"/>
-      <c r="H118" s="116"/>
-      <c r="I118" s="116"/>
-      <c r="J118" s="116"/>
-      <c r="K118" s="116"/>
-      <c r="L118" s="116"/>
-      <c r="M118" s="117"/>
-      <c r="N118" s="117"/>
+      <c r="C118" s="117"/>
+      <c r="D118" s="117"/>
+      <c r="E118" s="117"/>
+      <c r="F118" s="117"/>
+      <c r="G118" s="117"/>
+      <c r="H118" s="117"/>
+      <c r="I118" s="117"/>
+      <c r="J118" s="117"/>
+      <c r="K118" s="117"/>
+      <c r="L118" s="117"/>
+      <c r="M118" s="116"/>
+      <c r="N118" s="116"/>
       <c r="O118" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="173">
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
     <mergeCell ref="M96:N96"/>
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="Q83:AA83"/>
@@ -8247,155 +8357,6 @@
     <mergeCell ref="J65:K65"/>
     <mergeCell ref="J66:K66"/>
     <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Vehicle health increased - tank radius increased - Bufed FAMAS bullet speed 17 -> 20 - Buffed M1 fire rate 1600 -> 1400 reload 4000 -> 3600 GUN dist of AWM M1 increased
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DEEB79-DEBB-466D-B6FF-81D50775F90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F78C66F-9D49-4410-82E5-79139561452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -2584,74 +2584,74 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3898,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P130" sqref="P130"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3917,10 +3917,10 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="140" t="s">
+      <c r="C1" s="134" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="140"/>
+      <c r="D1" s="134"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4016,10 +4016,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="132" t="s">
+      <c r="Z2" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="132"/>
+      <c r="AA2" s="139"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -4559,8 +4559,8 @@
       <c r="B10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="44">
-        <v>1472</v>
+      <c r="C10" s="41">
+        <v>1600</v>
       </c>
       <c r="D10" s="19">
         <v>0</v>
@@ -4572,7 +4572,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="19">
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="H10" s="19">
         <v>42</v>
@@ -4581,7 +4581,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="19">
-        <v>4000</v>
+        <v>3600</v>
       </c>
       <c r="K10" s="19">
         <v>7</v>
@@ -4589,11 +4589,11 @@
       <c r="L10" s="19"/>
       <c r="M10" s="19">
         <f>ROUND(E10*F10/G10*1000,2)</f>
-        <v>3.75</v>
+        <v>4.29</v>
       </c>
       <c r="N10" s="19">
         <f>ROUND(E10*F10/(G10+J10/I10)*1000,2)</f>
-        <v>2.5</v>
+        <v>2.83</v>
       </c>
       <c r="O10" s="19">
         <f>E10*F10*I10</f>
@@ -4769,7 +4769,7 @@
         <f>E12*F12*I12</f>
         <v>25</v>
       </c>
-      <c r="P12" s="145">
+      <c r="P12" s="124">
         <f>ROUND(playerHealth/(E12*F12),1)</f>
         <v>3.2</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="41">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
@@ -5384,7 +5384,7 @@
         <v>90</v>
       </c>
       <c r="H20" s="19">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I20" s="19">
         <v>30</v>
@@ -5414,11 +5414,11 @@
       </c>
       <c r="Q20" s="19">
         <f t="shared" si="17"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="R20" s="19">
         <f t="shared" si="18"/>
-        <v>5.8999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="S20" s="28" t="s">
         <v>29</v>
@@ -5567,8 +5567,8 @@
         <f>ROUND(D23/H23,3)</f>
         <v>0.4</v>
       </c>
-      <c r="S23" s="28" t="s">
-        <v>29</v>
+      <c r="S23" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="T23" s="19"/>
       <c r="U23" s="19">
@@ -5654,8 +5654,8 @@
         <f>ROUND(D24/H24,3)</f>
         <v>0.154</v>
       </c>
-      <c r="S24" s="21" t="s">
-        <v>28</v>
+      <c r="S24" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="T24" s="19"/>
       <c r="U24" s="19">
@@ -5920,7 +5920,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="41">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="D29" s="19">
         <v>1</v>
@@ -6005,7 +6005,7 @@
         <v>48</v>
       </c>
       <c r="C30" s="41">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="D30" s="19">
         <v>1</v>
@@ -6201,7 +6201,7 @@
         <v>17.78</v>
       </c>
       <c r="W33" s="19">
-        <f t="shared" ref="W33:W34" si="26">E33*(F33-0.2)</f>
+        <f t="shared" ref="W33" si="26">E33*(F33-0.2)</f>
         <v>0.3</v>
       </c>
       <c r="X33" s="33">
@@ -6413,7 +6413,7 @@
         <v>3.27</v>
       </c>
       <c r="W36" s="19">
-        <f t="shared" ref="W36:W37" si="28">E36*(F36-0.4)</f>
+        <f t="shared" ref="W36" si="28">E36*(F36-0.4)</f>
         <v>3.1</v>
       </c>
       <c r="X36" s="29">
@@ -6468,7 +6468,7 @@
         <v>5</v>
       </c>
       <c r="O37" s="73"/>
-      <c r="P37" s="146">
+      <c r="P37" s="125">
         <f>ROUND(8/(E37*F37),1)</f>
         <v>5.3</v>
       </c>
@@ -6512,20 +6512,20 @@
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="138" t="s">
+      <c r="C40" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138" t="s">
+      <c r="D40" s="128"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="128"/>
+      <c r="G40" s="128"/>
+      <c r="H40" s="128"/>
+      <c r="I40" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="138"/>
-      <c r="K40" s="138"/>
-      <c r="L40" s="138"/>
+      <c r="J40" s="128"/>
+      <c r="K40" s="128"/>
+      <c r="L40" s="128"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -6533,10 +6533,10 @@
       <c r="Q40" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="S40" s="137" t="s">
+      <c r="S40" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="137"/>
+      <c r="T40" s="140"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6546,22 +6546,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="139" t="s">
+      <c r="C41" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="139"/>
-      <c r="E41" s="139"/>
-      <c r="F41" s="139" t="s">
+      <c r="D41" s="143"/>
+      <c r="E41" s="143"/>
+      <c r="F41" s="143" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="139"/>
-      <c r="H41" s="139"/>
-      <c r="I41" s="139" t="s">
+      <c r="G41" s="143"/>
+      <c r="H41" s="143"/>
+      <c r="I41" s="143" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="139"/>
-      <c r="K41" s="139"/>
-      <c r="L41" s="139"/>
+      <c r="J41" s="143"/>
+      <c r="K41" s="143"/>
+      <c r="L41" s="143"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6569,10 +6569,10 @@
       <c r="Q41" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S41" s="137" t="s">
+      <c r="S41" s="140" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="137"/>
+      <c r="T41" s="140"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6585,22 +6585,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="139" t="s">
+      <c r="C42" s="143" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="139"/>
-      <c r="E42" s="139"/>
-      <c r="F42" s="139" t="s">
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="139"/>
-      <c r="H42" s="139"/>
-      <c r="I42" s="139" t="s">
+      <c r="G42" s="143"/>
+      <c r="H42" s="143"/>
+      <c r="I42" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="139"/>
-      <c r="K42" s="139"/>
-      <c r="L42" s="139"/>
+      <c r="J42" s="143"/>
+      <c r="K42" s="143"/>
+      <c r="L42" s="143"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6608,10 +6608,10 @@
       <c r="Q42" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S42" s="137" t="s">
+      <c r="S42" s="140" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="137"/>
+      <c r="T42" s="140"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6624,22 +6624,22 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="135" t="s">
+      <c r="C43" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="135" t="s">
+      <c r="D43" s="131"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="131" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="135"/>
-      <c r="H43" s="135"/>
-      <c r="I43" s="135" t="s">
+      <c r="G43" s="131"/>
+      <c r="H43" s="131"/>
+      <c r="I43" s="131" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="135"/>
-      <c r="K43" s="135"/>
-      <c r="L43" s="135"/>
+      <c r="J43" s="131"/>
+      <c r="K43" s="131"/>
+      <c r="L43" s="131"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -6647,10 +6647,10 @@
       <c r="Q43" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="S43" s="137" t="s">
+      <c r="S43" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="137"/>
+      <c r="T43" s="140"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6665,20 +6665,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="135" t="s">
+      <c r="C44" s="131" t="s">
         <v>269</v>
       </c>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="135"/>
-      <c r="H44" s="135"/>
-      <c r="I44" s="135" t="s">
+      <c r="D44" s="131"/>
+      <c r="E44" s="131"/>
+      <c r="F44" s="131"/>
+      <c r="G44" s="131"/>
+      <c r="H44" s="131"/>
+      <c r="I44" s="131" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="135"/>
-      <c r="K44" s="135"/>
-      <c r="L44" s="135"/>
+      <c r="J44" s="131"/>
+      <c r="K44" s="131"/>
+      <c r="L44" s="131"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -6761,12 +6761,12 @@
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="135"/>
-      <c r="G49" s="135"/>
-      <c r="H49" s="135"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="131"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
@@ -6777,18 +6777,18 @@
       <c r="B51" s="76" t="s">
         <v>265</v>
       </c>
-      <c r="C51" s="138" t="s">
+      <c r="C51" s="128" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="138"/>
-      <c r="E51" s="138" t="s">
+      <c r="D51" s="128"/>
+      <c r="E51" s="128" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="138"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="138"/>
-      <c r="I51" s="138"/>
-      <c r="J51" s="138"/>
+      <c r="F51" s="128"/>
+      <c r="G51" s="128"/>
+      <c r="H51" s="128"/>
+      <c r="I51" s="128"/>
+      <c r="J51" s="128"/>
       <c r="K51" s="120" t="s">
         <v>259</v>
       </c>
@@ -6800,18 +6800,18 @@
       <c r="B52" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="C52" s="130" t="s">
+      <c r="C52" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="D52" s="130"/>
-      <c r="E52" s="126" t="s">
+      <c r="D52" s="126"/>
+      <c r="E52" s="127" t="s">
         <v>270</v>
       </c>
-      <c r="F52" s="126"/>
-      <c r="G52" s="126"/>
-      <c r="H52" s="126"/>
-      <c r="I52" s="126"/>
-      <c r="J52" s="126"/>
+      <c r="F52" s="127"/>
+      <c r="G52" s="127"/>
+      <c r="H52" s="127"/>
+      <c r="I52" s="127"/>
+      <c r="J52" s="127"/>
       <c r="K52" s="64" t="s">
         <v>261</v>
       </c>
@@ -6823,18 +6823,18 @@
       <c r="B53" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="C53" s="130" t="s">
+      <c r="C53" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="D53" s="130"/>
-      <c r="E53" s="126" t="s">
+      <c r="D53" s="126"/>
+      <c r="E53" s="127" t="s">
         <v>271</v>
       </c>
-      <c r="F53" s="126"/>
-      <c r="G53" s="126"/>
-      <c r="H53" s="126"/>
-      <c r="I53" s="126"/>
-      <c r="J53" s="126"/>
+      <c r="F53" s="127"/>
+      <c r="G53" s="127"/>
+      <c r="H53" s="127"/>
+      <c r="I53" s="127"/>
+      <c r="J53" s="127"/>
       <c r="K53" s="64" t="s">
         <v>261</v>
       </c>
@@ -6846,18 +6846,18 @@
       <c r="B54" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="C54" s="130" t="s">
+      <c r="C54" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="D54" s="130"/>
-      <c r="E54" s="126" t="s">
+      <c r="D54" s="126"/>
+      <c r="E54" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="F54" s="126"/>
-      <c r="G54" s="126"/>
-      <c r="H54" s="126"/>
-      <c r="I54" s="126"/>
-      <c r="J54" s="126"/>
+      <c r="F54" s="127"/>
+      <c r="G54" s="127"/>
+      <c r="H54" s="127"/>
+      <c r="I54" s="127"/>
+      <c r="J54" s="127"/>
       <c r="K54" s="64" t="s">
         <v>261</v>
       </c>
@@ -6874,14 +6874,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="144" t="s">
+      <c r="H56" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="144"/>
-      <c r="J56" s="144"/>
-      <c r="K56" s="144"/>
-      <c r="L56" s="144"/>
-      <c r="M56" s="144"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="133"/>
+      <c r="L56" s="133"/>
+      <c r="M56" s="133"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
@@ -7085,10 +7085,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="142" t="s">
+      <c r="J62" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="142"/>
+      <c r="K62" s="136"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7096,13 +7096,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="141" t="s">
+      <c r="O62" s="135" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="141"/>
-      <c r="Q62" s="141"/>
-      <c r="R62" s="141"/>
-      <c r="S62" s="141"/>
+      <c r="P62" s="135"/>
+      <c r="Q62" s="135"/>
+      <c r="R62" s="135"/>
+      <c r="S62" s="135"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
@@ -7124,20 +7124,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="127" t="s">
+      <c r="F63" s="141" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="127"/>
+      <c r="G63" s="141"/>
       <c r="H63" s="85" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="127" t="s">
+      <c r="J63" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="127"/>
+      <c r="K63" s="141"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7161,10 +7161,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="127" t="s">
+      <c r="U63" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="127"/>
+      <c r="V63" s="141"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7187,26 +7187,26 @@
         <v>24</v>
       </c>
       <c r="D64" s="96">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="143" t="s">
+      <c r="F64" s="142" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="142"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="130">
+      <c r="J64" s="126">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="130"/>
+      <c r="K64" s="126"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7218,7 +7218,7 @@
       <c r="N64" s="96"/>
       <c r="O64" s="98">
         <f t="shared" ref="O64:O70" si="33">ROUND(D64/health_cap,2)*10</f>
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="P64" s="99">
         <f t="shared" ref="P64:P70" si="34">ROUND(M64/guns_cap,2)*10</f>
@@ -7234,14 +7234,14 @@
       </c>
       <c r="S64" s="102">
         <f>SUM(O64:R64)</f>
-        <v>9.8000000000000007</v>
+        <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="128">
+      <c r="U64" s="145">
         <f>R64+O64+P64</f>
-        <v>3.8</v>
-      </c>
-      <c r="V64" s="128"/>
+        <v>4.5</v>
+      </c>
+      <c r="V64" s="145"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7264,26 +7264,26 @@
         <v>32</v>
       </c>
       <c r="D65" s="53">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="125" t="s">
+      <c r="F65" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="125"/>
+      <c r="G65" s="129"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="130">
+      <c r="J65" s="126">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="130"/>
+      <c r="K65" s="126"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -7295,7 +7295,7 @@
       <c r="N65" s="53"/>
       <c r="O65" s="65">
         <f t="shared" si="33"/>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="P65" s="66">
         <f t="shared" si="34"/>
@@ -7311,14 +7311,14 @@
       </c>
       <c r="S65" s="69">
         <f t="shared" ref="S65:S69" si="38">SUM(O65:R65)</f>
-        <v>13.3</v>
+        <v>14.8</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="129">
+      <c r="U65" s="146">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="V65" s="129"/>
+        <v>10.8</v>
+      </c>
+      <c r="V65" s="146"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7341,26 +7341,26 @@
         <v>30</v>
       </c>
       <c r="D66" s="53">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="125" t="s">
+      <c r="F66" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="125"/>
+      <c r="G66" s="129"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="130">
+      <c r="J66" s="126">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="130"/>
+      <c r="K66" s="126"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -7372,7 +7372,7 @@
       <c r="N66" s="53"/>
       <c r="O66" s="65">
         <f t="shared" si="33"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="P66" s="66">
         <f t="shared" si="34"/>
@@ -7388,14 +7388,14 @@
       </c>
       <c r="S66" s="69">
         <f t="shared" si="38"/>
-        <v>13.399999999999999</v>
+        <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="129">
+      <c r="U66" s="146">
         <f t="shared" si="39"/>
-        <v>10.399999999999999</v>
-      </c>
-      <c r="V66" s="129"/>
+        <v>10.899999999999999</v>
+      </c>
+      <c r="V66" s="146"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>88</v>
       </c>
       <c r="C67" s="53">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D67" s="53">
         <v>192</v>
@@ -7423,21 +7423,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="125" t="s">
+      <c r="F67" s="129" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="125"/>
+      <c r="G67" s="129"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="130">
+      <c r="J67" s="126">
         <f t="shared" si="32"/>
-        <v>48</v>
-      </c>
-      <c r="K67" s="130"/>
+        <v>58</v>
+      </c>
+      <c r="K67" s="126"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -7468,11 +7468,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="129">
+      <c r="U67" s="146">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="129"/>
+      <c r="V67" s="146"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7496,21 +7496,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="125" t="s">
+      <c r="F68" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="125"/>
+      <c r="G68" s="129"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="130">
+      <c r="J68" s="126">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="130"/>
+      <c r="K68" s="126"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7541,11 +7541,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="129">
+      <c r="U68" s="146">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="129"/>
+      <c r="V68" s="146"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7569,21 +7569,21 @@
       <c r="E69" s="53">
         <v>10</v>
       </c>
-      <c r="F69" s="125" t="s">
+      <c r="F69" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="125"/>
+      <c r="G69" s="129"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="130">
+      <c r="J69" s="126">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="130"/>
+      <c r="K69" s="126"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7614,11 +7614,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="129">
+      <c r="U69" s="146">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="129"/>
+      <c r="V69" s="146"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7642,21 +7642,21 @@
       <c r="E70" s="53">
         <v>8</v>
       </c>
-      <c r="F70" s="125" t="s">
+      <c r="F70" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="125"/>
+      <c r="G70" s="129"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="130">
+      <c r="J70" s="126">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="130"/>
+      <c r="K70" s="126"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7687,11 +7687,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="129">
+      <c r="U70" s="146">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="129"/>
+      <c r="V70" s="146"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7707,12 +7707,12 @@
       <c r="B73" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="O73" s="132" t="s">
+      <c r="O73" s="139" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="132"/>
-      <c r="Q73" s="132"/>
-      <c r="R73" s="132"/>
+      <c r="P73" s="139"/>
+      <c r="Q73" s="139"/>
+      <c r="R73" s="139"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7728,31 +7728,31 @@
       <c r="E74" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="131" t="s">
+      <c r="F74" s="132" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="131"/>
-      <c r="H74" s="131" t="s">
+      <c r="G74" s="132"/>
+      <c r="H74" s="132" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="131"/>
-      <c r="J74" s="131" t="s">
+      <c r="I74" s="132"/>
+      <c r="J74" s="132" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="131"/>
-      <c r="L74" s="131"/>
-      <c r="M74" s="131"/>
+      <c r="K74" s="132"/>
+      <c r="L74" s="132"/>
+      <c r="M74" s="132"/>
       <c r="N74" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="131" t="s">
+      <c r="O74" s="132" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="131"/>
-      <c r="Q74" s="131" t="s">
+      <c r="P74" s="132"/>
+      <c r="Q74" s="132" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="131"/>
+      <c r="R74" s="132"/>
       <c r="S74" s="120" t="s">
         <v>259</v>
       </c>
@@ -7773,21 +7773,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="130" t="s">
+      <c r="F75" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="130"/>
-      <c r="H75" s="130">
+      <c r="G75" s="126"/>
+      <c r="H75" s="126">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="130"/>
-      <c r="J75" s="130" t="s">
+      <c r="I75" s="126"/>
+      <c r="J75" s="126" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="130"/>
-      <c r="L75" s="130"/>
-      <c r="M75" s="130"/>
+      <c r="K75" s="126"/>
+      <c r="L75" s="126"/>
+      <c r="M75" s="126"/>
       <c r="N75" s="77" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7819,21 +7819,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="130" t="s">
+      <c r="F76" s="126" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="130"/>
-      <c r="H76" s="130">
+      <c r="G76" s="126"/>
+      <c r="H76" s="126">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="130"/>
-      <c r="J76" s="130" t="s">
+      <c r="I76" s="126"/>
+      <c r="J76" s="126" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="130"/>
-      <c r="L76" s="130"/>
-      <c r="M76" s="130"/>
+      <c r="K76" s="126"/>
+      <c r="L76" s="126"/>
+      <c r="M76" s="126"/>
       <c r="N76" s="77" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7855,19 +7855,19 @@
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="135"/>
-      <c r="G77" s="135"/>
-      <c r="H77" s="135"/>
-      <c r="I77" s="135"/>
-      <c r="J77" s="135"/>
-      <c r="K77" s="135"/>
-      <c r="L77" s="135"/>
-      <c r="M77" s="135"/>
+      <c r="F77" s="131"/>
+      <c r="G77" s="131"/>
+      <c r="H77" s="131"/>
+      <c r="I77" s="131"/>
+      <c r="J77" s="131"/>
+      <c r="K77" s="131"/>
+      <c r="L77" s="131"/>
+      <c r="M77" s="131"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="133"/>
-      <c r="P77" s="133"/>
-      <c r="Q77" s="133"/>
-      <c r="R77" s="133"/>
+      <c r="O77" s="137"/>
+      <c r="P77" s="137"/>
+      <c r="Q77" s="137"/>
+      <c r="R77" s="137"/>
       <c r="S77" s="64"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7896,32 +7896,32 @@
       <c r="E81" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="131" t="s">
+      <c r="F81" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="131"/>
-      <c r="H81" s="131"/>
-      <c r="I81" s="131"/>
-      <c r="J81" s="131"/>
-      <c r="K81" s="131"/>
-      <c r="L81" s="131"/>
-      <c r="M81" s="131"/>
-      <c r="N81" s="131"/>
-      <c r="O81" s="131"/>
-      <c r="P81" s="131"/>
-      <c r="Q81" s="131" t="s">
+      <c r="G81" s="132"/>
+      <c r="H81" s="132"/>
+      <c r="I81" s="132"/>
+      <c r="J81" s="132"/>
+      <c r="K81" s="132"/>
+      <c r="L81" s="132"/>
+      <c r="M81" s="132"/>
+      <c r="N81" s="132"/>
+      <c r="O81" s="132"/>
+      <c r="P81" s="132"/>
+      <c r="Q81" s="132" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="131"/>
-      <c r="S81" s="131"/>
-      <c r="T81" s="131"/>
-      <c r="U81" s="131"/>
-      <c r="V81" s="131"/>
-      <c r="W81" s="131"/>
-      <c r="X81" s="131"/>
-      <c r="Y81" s="131"/>
-      <c r="Z81" s="131"/>
-      <c r="AA81" s="131"/>
+      <c r="R81" s="132"/>
+      <c r="S81" s="132"/>
+      <c r="T81" s="132"/>
+      <c r="U81" s="132"/>
+      <c r="V81" s="132"/>
+      <c r="W81" s="132"/>
+      <c r="X81" s="132"/>
+      <c r="Y81" s="132"/>
+      <c r="Z81" s="132"/>
+      <c r="AA81" s="132"/>
       <c r="AB81" s="120" t="s">
         <v>259</v>
       </c>
@@ -7940,32 +7940,32 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="136" t="s">
+      <c r="F82" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="136"/>
-      <c r="H82" s="136"/>
-      <c r="I82" s="136"/>
-      <c r="J82" s="136"/>
-      <c r="K82" s="136"/>
-      <c r="L82" s="136"/>
-      <c r="M82" s="136"/>
-      <c r="N82" s="136"/>
-      <c r="O82" s="136"/>
-      <c r="P82" s="136"/>
-      <c r="Q82" s="136" t="s">
+      <c r="G82" s="144"/>
+      <c r="H82" s="144"/>
+      <c r="I82" s="144"/>
+      <c r="J82" s="144"/>
+      <c r="K82" s="144"/>
+      <c r="L82" s="144"/>
+      <c r="M82" s="144"/>
+      <c r="N82" s="144"/>
+      <c r="O82" s="144"/>
+      <c r="P82" s="144"/>
+      <c r="Q82" s="144" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="136"/>
-      <c r="S82" s="136"/>
-      <c r="T82" s="136"/>
-      <c r="U82" s="136"/>
-      <c r="V82" s="136"/>
-      <c r="W82" s="136"/>
-      <c r="X82" s="136"/>
-      <c r="Y82" s="136"/>
-      <c r="Z82" s="136"/>
-      <c r="AA82" s="136"/>
+      <c r="R82" s="144"/>
+      <c r="S82" s="144"/>
+      <c r="T82" s="144"/>
+      <c r="U82" s="144"/>
+      <c r="V82" s="144"/>
+      <c r="W82" s="144"/>
+      <c r="X82" s="144"/>
+      <c r="Y82" s="144"/>
+      <c r="Z82" s="144"/>
+      <c r="AA82" s="144"/>
       <c r="AB82" s="64" t="s">
         <v>260</v>
       </c>
@@ -7984,30 +7984,30 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="126" t="s">
+      <c r="F83" s="127" t="s">
         <v>225</v>
       </c>
-      <c r="G83" s="126"/>
-      <c r="H83" s="126"/>
-      <c r="I83" s="126"/>
-      <c r="J83" s="126"/>
-      <c r="K83" s="126"/>
-      <c r="L83" s="126"/>
-      <c r="M83" s="126"/>
-      <c r="N83" s="126"/>
-      <c r="O83" s="126"/>
-      <c r="P83" s="126"/>
-      <c r="Q83" s="126"/>
-      <c r="R83" s="126"/>
-      <c r="S83" s="126"/>
-      <c r="T83" s="126"/>
-      <c r="U83" s="126"/>
-      <c r="V83" s="126"/>
-      <c r="W83" s="126"/>
-      <c r="X83" s="126"/>
-      <c r="Y83" s="126"/>
-      <c r="Z83" s="126"/>
-      <c r="AA83" s="126"/>
+      <c r="G83" s="127"/>
+      <c r="H83" s="127"/>
+      <c r="I83" s="127"/>
+      <c r="J83" s="127"/>
+      <c r="K83" s="127"/>
+      <c r="L83" s="127"/>
+      <c r="M83" s="127"/>
+      <c r="N83" s="127"/>
+      <c r="O83" s="127"/>
+      <c r="P83" s="127"/>
+      <c r="Q83" s="127"/>
+      <c r="R83" s="127"/>
+      <c r="S83" s="127"/>
+      <c r="T83" s="127"/>
+      <c r="U83" s="127"/>
+      <c r="V83" s="127"/>
+      <c r="W83" s="127"/>
+      <c r="X83" s="127"/>
+      <c r="Y83" s="127"/>
+      <c r="Z83" s="127"/>
+      <c r="AA83" s="127"/>
       <c r="AB83" s="64" t="s">
         <v>260</v>
       </c>
@@ -8026,30 +8026,30 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="126" t="s">
+      <c r="F84" s="127" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="126"/>
-      <c r="H84" s="126"/>
-      <c r="I84" s="126"/>
-      <c r="J84" s="126"/>
-      <c r="K84" s="126"/>
-      <c r="L84" s="126"/>
-      <c r="M84" s="126"/>
-      <c r="N84" s="126"/>
-      <c r="O84" s="126"/>
-      <c r="P84" s="126"/>
-      <c r="Q84" s="126"/>
-      <c r="R84" s="126"/>
-      <c r="S84" s="126"/>
-      <c r="T84" s="126"/>
-      <c r="U84" s="126"/>
-      <c r="V84" s="126"/>
-      <c r="W84" s="126"/>
-      <c r="X84" s="126"/>
-      <c r="Y84" s="126"/>
-      <c r="Z84" s="126"/>
-      <c r="AA84" s="126"/>
+      <c r="G84" s="127"/>
+      <c r="H84" s="127"/>
+      <c r="I84" s="127"/>
+      <c r="J84" s="127"/>
+      <c r="K84" s="127"/>
+      <c r="L84" s="127"/>
+      <c r="M84" s="127"/>
+      <c r="N84" s="127"/>
+      <c r="O84" s="127"/>
+      <c r="P84" s="127"/>
+      <c r="Q84" s="127"/>
+      <c r="R84" s="127"/>
+      <c r="S84" s="127"/>
+      <c r="T84" s="127"/>
+      <c r="U84" s="127"/>
+      <c r="V84" s="127"/>
+      <c r="W84" s="127"/>
+      <c r="X84" s="127"/>
+      <c r="Y84" s="127"/>
+      <c r="Z84" s="127"/>
+      <c r="AA84" s="127"/>
       <c r="AB84" s="64" t="s">
         <v>260</v>
       </c>
@@ -8068,32 +8068,32 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="126" t="s">
+      <c r="F85" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="126"/>
-      <c r="H85" s="126"/>
-      <c r="I85" s="126"/>
-      <c r="J85" s="126"/>
-      <c r="K85" s="126"/>
-      <c r="L85" s="126"/>
-      <c r="M85" s="126"/>
-      <c r="N85" s="126"/>
-      <c r="O85" s="126"/>
-      <c r="P85" s="126"/>
-      <c r="Q85" s="126" t="s">
+      <c r="G85" s="127"/>
+      <c r="H85" s="127"/>
+      <c r="I85" s="127"/>
+      <c r="J85" s="127"/>
+      <c r="K85" s="127"/>
+      <c r="L85" s="127"/>
+      <c r="M85" s="127"/>
+      <c r="N85" s="127"/>
+      <c r="O85" s="127"/>
+      <c r="P85" s="127"/>
+      <c r="Q85" s="127" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="126"/>
-      <c r="S85" s="126"/>
-      <c r="T85" s="126"/>
-      <c r="U85" s="126"/>
-      <c r="V85" s="126"/>
-      <c r="W85" s="126"/>
-      <c r="X85" s="126"/>
-      <c r="Y85" s="126"/>
-      <c r="Z85" s="126"/>
-      <c r="AA85" s="126"/>
+      <c r="R85" s="127"/>
+      <c r="S85" s="127"/>
+      <c r="T85" s="127"/>
+      <c r="U85" s="127"/>
+      <c r="V85" s="127"/>
+      <c r="W85" s="127"/>
+      <c r="X85" s="127"/>
+      <c r="Y85" s="127"/>
+      <c r="Z85" s="127"/>
+      <c r="AA85" s="127"/>
       <c r="AB85" s="64" t="s">
         <v>260</v>
       </c>
@@ -8112,32 +8112,32 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="126" t="s">
+      <c r="F86" s="127" t="s">
         <v>257</v>
       </c>
-      <c r="G86" s="126"/>
-      <c r="H86" s="126"/>
-      <c r="I86" s="126"/>
-      <c r="J86" s="126"/>
-      <c r="K86" s="126"/>
-      <c r="L86" s="126"/>
-      <c r="M86" s="126"/>
-      <c r="N86" s="126"/>
-      <c r="O86" s="126"/>
-      <c r="P86" s="126"/>
-      <c r="Q86" s="126" t="s">
+      <c r="G86" s="127"/>
+      <c r="H86" s="127"/>
+      <c r="I86" s="127"/>
+      <c r="J86" s="127"/>
+      <c r="K86" s="127"/>
+      <c r="L86" s="127"/>
+      <c r="M86" s="127"/>
+      <c r="N86" s="127"/>
+      <c r="O86" s="127"/>
+      <c r="P86" s="127"/>
+      <c r="Q86" s="127" t="s">
         <v>258</v>
       </c>
-      <c r="R86" s="126"/>
-      <c r="S86" s="126"/>
-      <c r="T86" s="126"/>
-      <c r="U86" s="126"/>
-      <c r="V86" s="126"/>
-      <c r="W86" s="126"/>
-      <c r="X86" s="126"/>
-      <c r="Y86" s="126"/>
-      <c r="Z86" s="126"/>
-      <c r="AA86" s="126"/>
+      <c r="R86" s="127"/>
+      <c r="S86" s="127"/>
+      <c r="T86" s="127"/>
+      <c r="U86" s="127"/>
+      <c r="V86" s="127"/>
+      <c r="W86" s="127"/>
+      <c r="X86" s="127"/>
+      <c r="Y86" s="127"/>
+      <c r="Z86" s="127"/>
+      <c r="AA86" s="127"/>
       <c r="AB86" s="64" t="s">
         <v>261</v>
       </c>
@@ -8152,28 +8152,28 @@
       </c>
       <c r="D87" s="53"/>
       <c r="E87" s="53"/>
-      <c r="F87" s="126"/>
-      <c r="G87" s="126"/>
-      <c r="H87" s="126"/>
-      <c r="I87" s="126"/>
-      <c r="J87" s="126"/>
-      <c r="K87" s="126"/>
-      <c r="L87" s="126"/>
-      <c r="M87" s="126"/>
-      <c r="N87" s="126"/>
-      <c r="O87" s="126"/>
-      <c r="P87" s="126"/>
-      <c r="Q87" s="126"/>
-      <c r="R87" s="126"/>
-      <c r="S87" s="126"/>
-      <c r="T87" s="126"/>
-      <c r="U87" s="126"/>
-      <c r="V87" s="126"/>
-      <c r="W87" s="126"/>
-      <c r="X87" s="126"/>
-      <c r="Y87" s="126"/>
-      <c r="Z87" s="126"/>
-      <c r="AA87" s="126"/>
+      <c r="F87" s="127"/>
+      <c r="G87" s="127"/>
+      <c r="H87" s="127"/>
+      <c r="I87" s="127"/>
+      <c r="J87" s="127"/>
+      <c r="K87" s="127"/>
+      <c r="L87" s="127"/>
+      <c r="M87" s="127"/>
+      <c r="N87" s="127"/>
+      <c r="O87" s="127"/>
+      <c r="P87" s="127"/>
+      <c r="Q87" s="127"/>
+      <c r="R87" s="127"/>
+      <c r="S87" s="127"/>
+      <c r="T87" s="127"/>
+      <c r="U87" s="127"/>
+      <c r="V87" s="127"/>
+      <c r="W87" s="127"/>
+      <c r="X87" s="127"/>
+      <c r="Y87" s="127"/>
+      <c r="Z87" s="127"/>
+      <c r="AA87" s="127"/>
       <c r="AB87" s="64" t="s">
         <v>261</v>
       </c>
@@ -8185,24 +8185,24 @@
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="134" t="s">
+      <c r="C90" s="138" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="134"/>
-      <c r="E90" s="134"/>
-      <c r="F90" s="134"/>
-      <c r="G90" s="134"/>
-      <c r="H90" s="134" t="s">
+      <c r="D90" s="138"/>
+      <c r="E90" s="138"/>
+      <c r="F90" s="138"/>
+      <c r="G90" s="138"/>
+      <c r="H90" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="134"/>
-      <c r="J90" s="134"/>
-      <c r="K90" s="134"/>
-      <c r="L90" s="134"/>
-      <c r="M90" s="131" t="s">
+      <c r="I90" s="138"/>
+      <c r="J90" s="138"/>
+      <c r="K90" s="138"/>
+      <c r="L90" s="138"/>
+      <c r="M90" s="132" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="131"/>
+      <c r="N90" s="132"/>
       <c r="O90" s="106"/>
       <c r="T90" s="57" t="s">
         <v>197</v>
@@ -8215,24 +8215,24 @@
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="124" t="s">
+      <c r="C91" s="130" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="124"/>
-      <c r="E91" s="124"/>
-      <c r="F91" s="124"/>
-      <c r="G91" s="124"/>
-      <c r="H91" s="124" t="s">
+      <c r="D91" s="130"/>
+      <c r="E91" s="130"/>
+      <c r="F91" s="130"/>
+      <c r="G91" s="130"/>
+      <c r="H91" s="130" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="124"/>
-      <c r="J91" s="124"/>
-      <c r="K91" s="124"/>
-      <c r="L91" s="124"/>
-      <c r="M91" s="125" t="s">
+      <c r="I91" s="130"/>
+      <c r="J91" s="130"/>
+      <c r="K91" s="130"/>
+      <c r="L91" s="130"/>
+      <c r="M91" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="125"/>
+      <c r="N91" s="129"/>
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8242,24 +8242,24 @@
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="124" t="s">
+      <c r="C92" s="130" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="124"/>
-      <c r="E92" s="124"/>
-      <c r="F92" s="124"/>
-      <c r="G92" s="124"/>
-      <c r="H92" s="124" t="s">
+      <c r="D92" s="130"/>
+      <c r="E92" s="130"/>
+      <c r="F92" s="130"/>
+      <c r="G92" s="130"/>
+      <c r="H92" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="124"/>
-      <c r="J92" s="124"/>
-      <c r="K92" s="124"/>
-      <c r="L92" s="124"/>
-      <c r="M92" s="125" t="s">
+      <c r="I92" s="130"/>
+      <c r="J92" s="130"/>
+      <c r="K92" s="130"/>
+      <c r="L92" s="130"/>
+      <c r="M92" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="125"/>
+      <c r="N92" s="129"/>
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8269,24 +8269,24 @@
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="124" t="s">
+      <c r="C93" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="124"/>
-      <c r="E93" s="124"/>
-      <c r="F93" s="124"/>
-      <c r="G93" s="124"/>
-      <c r="H93" s="124" t="s">
+      <c r="D93" s="130"/>
+      <c r="E93" s="130"/>
+      <c r="F93" s="130"/>
+      <c r="G93" s="130"/>
+      <c r="H93" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="124"/>
-      <c r="J93" s="124"/>
-      <c r="K93" s="124"/>
-      <c r="L93" s="124"/>
-      <c r="M93" s="125" t="s">
+      <c r="I93" s="130"/>
+      <c r="J93" s="130"/>
+      <c r="K93" s="130"/>
+      <c r="L93" s="130"/>
+      <c r="M93" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="125"/>
+      <c r="N93" s="129"/>
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8296,24 +8296,24 @@
       <c r="B94" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C94" s="124" t="s">
+      <c r="C94" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="124"/>
-      <c r="E94" s="124"/>
-      <c r="F94" s="124"/>
-      <c r="G94" s="124"/>
-      <c r="H94" s="124" t="s">
+      <c r="D94" s="130"/>
+      <c r="E94" s="130"/>
+      <c r="F94" s="130"/>
+      <c r="G94" s="130"/>
+      <c r="H94" s="130" t="s">
         <v>217</v>
       </c>
-      <c r="I94" s="124"/>
-      <c r="J94" s="124"/>
-      <c r="K94" s="124"/>
-      <c r="L94" s="124"/>
-      <c r="M94" s="125" t="s">
+      <c r="I94" s="130"/>
+      <c r="J94" s="130"/>
+      <c r="K94" s="130"/>
+      <c r="L94" s="130"/>
+      <c r="M94" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="125"/>
+      <c r="N94" s="129"/>
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8323,24 +8323,24 @@
       <c r="B95" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C95" s="124" t="s">
+      <c r="C95" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="124"/>
-      <c r="E95" s="124"/>
-      <c r="F95" s="124"/>
-      <c r="G95" s="124"/>
-      <c r="H95" s="124" t="s">
+      <c r="D95" s="130"/>
+      <c r="E95" s="130"/>
+      <c r="F95" s="130"/>
+      <c r="G95" s="130"/>
+      <c r="H95" s="130" t="s">
         <v>218</v>
       </c>
-      <c r="I95" s="124"/>
-      <c r="J95" s="124"/>
-      <c r="K95" s="124"/>
-      <c r="L95" s="124"/>
-      <c r="M95" s="125" t="s">
+      <c r="I95" s="130"/>
+      <c r="J95" s="130"/>
+      <c r="K95" s="130"/>
+      <c r="L95" s="130"/>
+      <c r="M95" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="125"/>
+      <c r="N95" s="129"/>
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8350,24 +8350,24 @@
       <c r="B96" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="124" t="s">
+      <c r="C96" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="124"/>
-      <c r="E96" s="124"/>
-      <c r="F96" s="124"/>
-      <c r="G96" s="124"/>
-      <c r="H96" s="124" t="s">
+      <c r="D96" s="130"/>
+      <c r="E96" s="130"/>
+      <c r="F96" s="130"/>
+      <c r="G96" s="130"/>
+      <c r="H96" s="130" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="124"/>
-      <c r="J96" s="124"/>
-      <c r="K96" s="124"/>
-      <c r="L96" s="124"/>
-      <c r="M96" s="125" t="s">
+      <c r="I96" s="130"/>
+      <c r="J96" s="130"/>
+      <c r="K96" s="130"/>
+      <c r="L96" s="130"/>
+      <c r="M96" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="125"/>
+      <c r="N96" s="129"/>
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8377,24 +8377,24 @@
       <c r="B97" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="124" t="s">
+      <c r="C97" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="124"/>
-      <c r="E97" s="124"/>
-      <c r="F97" s="124"/>
-      <c r="G97" s="124"/>
-      <c r="H97" s="124" t="s">
+      <c r="D97" s="130"/>
+      <c r="E97" s="130"/>
+      <c r="F97" s="130"/>
+      <c r="G97" s="130"/>
+      <c r="H97" s="130" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="124"/>
-      <c r="J97" s="124"/>
-      <c r="K97" s="124"/>
-      <c r="L97" s="124"/>
-      <c r="M97" s="125" t="s">
+      <c r="I97" s="130"/>
+      <c r="J97" s="130"/>
+      <c r="K97" s="130"/>
+      <c r="L97" s="130"/>
+      <c r="M97" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="125"/>
+      <c r="N97" s="129"/>
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8404,24 +8404,24 @@
       <c r="B98" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C98" s="124" t="s">
+      <c r="C98" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="124"/>
-      <c r="E98" s="124"/>
-      <c r="F98" s="124"/>
-      <c r="G98" s="124"/>
-      <c r="H98" s="124" t="s">
+      <c r="D98" s="130"/>
+      <c r="E98" s="130"/>
+      <c r="F98" s="130"/>
+      <c r="G98" s="130"/>
+      <c r="H98" s="130" t="s">
         <v>221</v>
       </c>
-      <c r="I98" s="124"/>
-      <c r="J98" s="124"/>
-      <c r="K98" s="124"/>
-      <c r="L98" s="124"/>
-      <c r="M98" s="125" t="s">
+      <c r="I98" s="130"/>
+      <c r="J98" s="130"/>
+      <c r="K98" s="130"/>
+      <c r="L98" s="130"/>
+      <c r="M98" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="125"/>
+      <c r="N98" s="129"/>
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8431,24 +8431,24 @@
       <c r="B99" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="124" t="s">
+      <c r="C99" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="124"/>
-      <c r="E99" s="124"/>
-      <c r="F99" s="124"/>
-      <c r="G99" s="124"/>
-      <c r="H99" s="124" t="s">
+      <c r="D99" s="130"/>
+      <c r="E99" s="130"/>
+      <c r="F99" s="130"/>
+      <c r="G99" s="130"/>
+      <c r="H99" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="I99" s="124"/>
-      <c r="J99" s="124"/>
-      <c r="K99" s="124"/>
-      <c r="L99" s="124"/>
-      <c r="M99" s="125" t="s">
+      <c r="I99" s="130"/>
+      <c r="J99" s="130"/>
+      <c r="K99" s="130"/>
+      <c r="L99" s="130"/>
+      <c r="M99" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="125"/>
+      <c r="N99" s="129"/>
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8458,325 +8458,325 @@
       <c r="B100" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="124" t="s">
+      <c r="C100" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="D100" s="124"/>
-      <c r="E100" s="124"/>
-      <c r="F100" s="124"/>
-      <c r="G100" s="124"/>
-      <c r="H100" s="124" t="s">
+      <c r="D100" s="130"/>
+      <c r="E100" s="130"/>
+      <c r="F100" s="130"/>
+      <c r="G100" s="130"/>
+      <c r="H100" s="130" t="s">
         <v>223</v>
       </c>
-      <c r="I100" s="124"/>
-      <c r="J100" s="124"/>
-      <c r="K100" s="124"/>
-      <c r="L100" s="124"/>
-      <c r="M100" s="125" t="s">
+      <c r="I100" s="130"/>
+      <c r="J100" s="130"/>
+      <c r="K100" s="130"/>
+      <c r="L100" s="130"/>
+      <c r="M100" s="129" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="125"/>
+      <c r="N100" s="129"/>
       <c r="O100" s="64"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="124"/>
-      <c r="D101" s="124"/>
-      <c r="E101" s="124"/>
-      <c r="F101" s="124"/>
-      <c r="G101" s="124"/>
-      <c r="H101" s="124"/>
-      <c r="I101" s="124"/>
-      <c r="J101" s="124"/>
-      <c r="K101" s="124"/>
-      <c r="L101" s="124"/>
-      <c r="M101" s="125"/>
-      <c r="N101" s="125"/>
+      <c r="C101" s="130"/>
+      <c r="D101" s="130"/>
+      <c r="E101" s="130"/>
+      <c r="F101" s="130"/>
+      <c r="G101" s="130"/>
+      <c r="H101" s="130"/>
+      <c r="I101" s="130"/>
+      <c r="J101" s="130"/>
+      <c r="K101" s="130"/>
+      <c r="L101" s="130"/>
+      <c r="M101" s="129"/>
+      <c r="N101" s="129"/>
       <c r="O101" s="64"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="124"/>
-      <c r="I102" s="124"/>
-      <c r="J102" s="124"/>
-      <c r="K102" s="124"/>
-      <c r="L102" s="124"/>
-      <c r="M102" s="125"/>
-      <c r="N102" s="125"/>
+      <c r="H102" s="130"/>
+      <c r="I102" s="130"/>
+      <c r="J102" s="130"/>
+      <c r="K102" s="130"/>
+      <c r="L102" s="130"/>
+      <c r="M102" s="129"/>
+      <c r="N102" s="129"/>
       <c r="O102" s="64"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="124"/>
-      <c r="D103" s="124"/>
-      <c r="E103" s="124"/>
-      <c r="F103" s="124"/>
-      <c r="G103" s="124"/>
-      <c r="H103" s="124"/>
-      <c r="I103" s="124"/>
-      <c r="J103" s="124"/>
-      <c r="K103" s="124"/>
-      <c r="L103" s="124"/>
-      <c r="M103" s="125"/>
-      <c r="N103" s="125"/>
+      <c r="C103" s="130"/>
+      <c r="D103" s="130"/>
+      <c r="E103" s="130"/>
+      <c r="F103" s="130"/>
+      <c r="G103" s="130"/>
+      <c r="H103" s="130"/>
+      <c r="I103" s="130"/>
+      <c r="J103" s="130"/>
+      <c r="K103" s="130"/>
+      <c r="L103" s="130"/>
+      <c r="M103" s="129"/>
+      <c r="N103" s="129"/>
       <c r="O103" s="64"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="124"/>
-      <c r="D104" s="124"/>
-      <c r="E104" s="124"/>
-      <c r="F104" s="124"/>
-      <c r="G104" s="124"/>
-      <c r="H104" s="124"/>
-      <c r="I104" s="124"/>
-      <c r="J104" s="124"/>
-      <c r="K104" s="124"/>
-      <c r="L104" s="124"/>
-      <c r="M104" s="125"/>
-      <c r="N104" s="125"/>
+      <c r="C104" s="130"/>
+      <c r="D104" s="130"/>
+      <c r="E104" s="130"/>
+      <c r="F104" s="130"/>
+      <c r="G104" s="130"/>
+      <c r="H104" s="130"/>
+      <c r="I104" s="130"/>
+      <c r="J104" s="130"/>
+      <c r="K104" s="130"/>
+      <c r="L104" s="130"/>
+      <c r="M104" s="129"/>
+      <c r="N104" s="129"/>
       <c r="O104" s="64"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="124"/>
-      <c r="D105" s="124"/>
-      <c r="E105" s="124"/>
-      <c r="F105" s="124"/>
-      <c r="G105" s="124"/>
-      <c r="H105" s="124"/>
-      <c r="I105" s="124"/>
-      <c r="J105" s="124"/>
-      <c r="K105" s="124"/>
-      <c r="L105" s="124"/>
-      <c r="M105" s="125"/>
-      <c r="N105" s="125"/>
+      <c r="C105" s="130"/>
+      <c r="D105" s="130"/>
+      <c r="E105" s="130"/>
+      <c r="F105" s="130"/>
+      <c r="G105" s="130"/>
+      <c r="H105" s="130"/>
+      <c r="I105" s="130"/>
+      <c r="J105" s="130"/>
+      <c r="K105" s="130"/>
+      <c r="L105" s="130"/>
+      <c r="M105" s="129"/>
+      <c r="N105" s="129"/>
       <c r="O105" s="64"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="124"/>
-      <c r="D106" s="124"/>
-      <c r="E106" s="124"/>
-      <c r="F106" s="124"/>
-      <c r="G106" s="124"/>
-      <c r="H106" s="124"/>
-      <c r="I106" s="124"/>
-      <c r="J106" s="124"/>
-      <c r="K106" s="124"/>
-      <c r="L106" s="124"/>
-      <c r="M106" s="125"/>
-      <c r="N106" s="125"/>
+      <c r="C106" s="130"/>
+      <c r="D106" s="130"/>
+      <c r="E106" s="130"/>
+      <c r="F106" s="130"/>
+      <c r="G106" s="130"/>
+      <c r="H106" s="130"/>
+      <c r="I106" s="130"/>
+      <c r="J106" s="130"/>
+      <c r="K106" s="130"/>
+      <c r="L106" s="130"/>
+      <c r="M106" s="129"/>
+      <c r="N106" s="129"/>
       <c r="O106" s="64"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="37"/>
       <c r="B107" s="37"/>
-      <c r="C107" s="124"/>
-      <c r="D107" s="124"/>
-      <c r="E107" s="124"/>
-      <c r="F107" s="124"/>
-      <c r="G107" s="124"/>
-      <c r="H107" s="124"/>
-      <c r="I107" s="124"/>
-      <c r="J107" s="124"/>
-      <c r="K107" s="124"/>
-      <c r="L107" s="124"/>
-      <c r="M107" s="125"/>
-      <c r="N107" s="125"/>
+      <c r="C107" s="130"/>
+      <c r="D107" s="130"/>
+      <c r="E107" s="130"/>
+      <c r="F107" s="130"/>
+      <c r="G107" s="130"/>
+      <c r="H107" s="130"/>
+      <c r="I107" s="130"/>
+      <c r="J107" s="130"/>
+      <c r="K107" s="130"/>
+      <c r="L107" s="130"/>
+      <c r="M107" s="129"/>
+      <c r="N107" s="129"/>
       <c r="O107" s="64"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="37"/>
       <c r="B108" s="37"/>
-      <c r="C108" s="124"/>
-      <c r="D108" s="124"/>
-      <c r="E108" s="124"/>
-      <c r="F108" s="124"/>
-      <c r="G108" s="124"/>
-      <c r="H108" s="124"/>
-      <c r="I108" s="124"/>
-      <c r="J108" s="124"/>
-      <c r="K108" s="124"/>
-      <c r="L108" s="124"/>
-      <c r="M108" s="125"/>
-      <c r="N108" s="125"/>
+      <c r="C108" s="130"/>
+      <c r="D108" s="130"/>
+      <c r="E108" s="130"/>
+      <c r="F108" s="130"/>
+      <c r="G108" s="130"/>
+      <c r="H108" s="130"/>
+      <c r="I108" s="130"/>
+      <c r="J108" s="130"/>
+      <c r="K108" s="130"/>
+      <c r="L108" s="130"/>
+      <c r="M108" s="129"/>
+      <c r="N108" s="129"/>
       <c r="O108" s="64"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="37"/>
       <c r="B109" s="37"/>
-      <c r="C109" s="124"/>
-      <c r="D109" s="124"/>
-      <c r="E109" s="124"/>
-      <c r="F109" s="124"/>
-      <c r="G109" s="124"/>
-      <c r="H109" s="124"/>
-      <c r="I109" s="124"/>
-      <c r="J109" s="124"/>
-      <c r="K109" s="124"/>
-      <c r="L109" s="124"/>
-      <c r="M109" s="125"/>
-      <c r="N109" s="125"/>
+      <c r="C109" s="130"/>
+      <c r="D109" s="130"/>
+      <c r="E109" s="130"/>
+      <c r="F109" s="130"/>
+      <c r="G109" s="130"/>
+      <c r="H109" s="130"/>
+      <c r="I109" s="130"/>
+      <c r="J109" s="130"/>
+      <c r="K109" s="130"/>
+      <c r="L109" s="130"/>
+      <c r="M109" s="129"/>
+      <c r="N109" s="129"/>
       <c r="O109" s="64"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="37"/>
       <c r="B110" s="37"/>
-      <c r="C110" s="124"/>
-      <c r="D110" s="124"/>
-      <c r="E110" s="124"/>
-      <c r="F110" s="124"/>
-      <c r="G110" s="124"/>
-      <c r="H110" s="124"/>
-      <c r="I110" s="124"/>
-      <c r="J110" s="124"/>
-      <c r="K110" s="124"/>
-      <c r="L110" s="124"/>
-      <c r="M110" s="125"/>
-      <c r="N110" s="125"/>
+      <c r="C110" s="130"/>
+      <c r="D110" s="130"/>
+      <c r="E110" s="130"/>
+      <c r="F110" s="130"/>
+      <c r="G110" s="130"/>
+      <c r="H110" s="130"/>
+      <c r="I110" s="130"/>
+      <c r="J110" s="130"/>
+      <c r="K110" s="130"/>
+      <c r="L110" s="130"/>
+      <c r="M110" s="129"/>
+      <c r="N110" s="129"/>
       <c r="O110" s="64"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="37"/>
       <c r="B111" s="37"/>
-      <c r="C111" s="124"/>
-      <c r="D111" s="124"/>
-      <c r="E111" s="124"/>
-      <c r="F111" s="124"/>
-      <c r="G111" s="124"/>
-      <c r="H111" s="124"/>
-      <c r="I111" s="124"/>
-      <c r="J111" s="124"/>
-      <c r="K111" s="124"/>
-      <c r="L111" s="124"/>
-      <c r="M111" s="125"/>
-      <c r="N111" s="125"/>
+      <c r="C111" s="130"/>
+      <c r="D111" s="130"/>
+      <c r="E111" s="130"/>
+      <c r="F111" s="130"/>
+      <c r="G111" s="130"/>
+      <c r="H111" s="130"/>
+      <c r="I111" s="130"/>
+      <c r="J111" s="130"/>
+      <c r="K111" s="130"/>
+      <c r="L111" s="130"/>
+      <c r="M111" s="129"/>
+      <c r="N111" s="129"/>
       <c r="O111" s="64"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="37"/>
       <c r="B112" s="37"/>
-      <c r="C112" s="124"/>
-      <c r="D112" s="124"/>
-      <c r="E112" s="124"/>
-      <c r="F112" s="124"/>
-      <c r="G112" s="124"/>
-      <c r="H112" s="124"/>
-      <c r="I112" s="124"/>
-      <c r="J112" s="124"/>
-      <c r="K112" s="124"/>
-      <c r="L112" s="124"/>
-      <c r="M112" s="125"/>
-      <c r="N112" s="125"/>
+      <c r="C112" s="130"/>
+      <c r="D112" s="130"/>
+      <c r="E112" s="130"/>
+      <c r="F112" s="130"/>
+      <c r="G112" s="130"/>
+      <c r="H112" s="130"/>
+      <c r="I112" s="130"/>
+      <c r="J112" s="130"/>
+      <c r="K112" s="130"/>
+      <c r="L112" s="130"/>
+      <c r="M112" s="129"/>
+      <c r="N112" s="129"/>
       <c r="O112" s="64"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="37"/>
       <c r="B113" s="37"/>
-      <c r="C113" s="124"/>
-      <c r="D113" s="124"/>
-      <c r="E113" s="124"/>
-      <c r="F113" s="124"/>
-      <c r="G113" s="124"/>
-      <c r="H113" s="124"/>
-      <c r="I113" s="124"/>
-      <c r="J113" s="124"/>
-      <c r="K113" s="124"/>
-      <c r="L113" s="124"/>
-      <c r="M113" s="125"/>
-      <c r="N113" s="125"/>
+      <c r="C113" s="130"/>
+      <c r="D113" s="130"/>
+      <c r="E113" s="130"/>
+      <c r="F113" s="130"/>
+      <c r="G113" s="130"/>
+      <c r="H113" s="130"/>
+      <c r="I113" s="130"/>
+      <c r="J113" s="130"/>
+      <c r="K113" s="130"/>
+      <c r="L113" s="130"/>
+      <c r="M113" s="129"/>
+      <c r="N113" s="129"/>
       <c r="O113" s="64"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="37"/>
       <c r="B114" s="37"/>
-      <c r="C114" s="124"/>
-      <c r="D114" s="124"/>
-      <c r="E114" s="124"/>
-      <c r="F114" s="124"/>
-      <c r="G114" s="124"/>
-      <c r="H114" s="124"/>
-      <c r="I114" s="124"/>
-      <c r="J114" s="124"/>
-      <c r="K114" s="124"/>
-      <c r="L114" s="124"/>
-      <c r="M114" s="125"/>
-      <c r="N114" s="125"/>
+      <c r="C114" s="130"/>
+      <c r="D114" s="130"/>
+      <c r="E114" s="130"/>
+      <c r="F114" s="130"/>
+      <c r="G114" s="130"/>
+      <c r="H114" s="130"/>
+      <c r="I114" s="130"/>
+      <c r="J114" s="130"/>
+      <c r="K114" s="130"/>
+      <c r="L114" s="130"/>
+      <c r="M114" s="129"/>
+      <c r="N114" s="129"/>
       <c r="O114" s="64"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="37"/>
       <c r="B115" s="37"/>
-      <c r="C115" s="124"/>
-      <c r="D115" s="124"/>
-      <c r="E115" s="124"/>
-      <c r="F115" s="124"/>
-      <c r="G115" s="124"/>
-      <c r="H115" s="124"/>
-      <c r="I115" s="124"/>
-      <c r="J115" s="124"/>
-      <c r="K115" s="124"/>
-      <c r="L115" s="124"/>
-      <c r="M115" s="125"/>
-      <c r="N115" s="125"/>
+      <c r="C115" s="130"/>
+      <c r="D115" s="130"/>
+      <c r="E115" s="130"/>
+      <c r="F115" s="130"/>
+      <c r="G115" s="130"/>
+      <c r="H115" s="130"/>
+      <c r="I115" s="130"/>
+      <c r="J115" s="130"/>
+      <c r="K115" s="130"/>
+      <c r="L115" s="130"/>
+      <c r="M115" s="129"/>
+      <c r="N115" s="129"/>
       <c r="O115" s="64"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="37"/>
       <c r="B116" s="37"/>
-      <c r="C116" s="124"/>
-      <c r="D116" s="124"/>
-      <c r="E116" s="124"/>
-      <c r="F116" s="124"/>
-      <c r="G116" s="124"/>
-      <c r="H116" s="124"/>
-      <c r="I116" s="124"/>
-      <c r="J116" s="124"/>
-      <c r="K116" s="124"/>
-      <c r="L116" s="124"/>
-      <c r="M116" s="125"/>
-      <c r="N116" s="125"/>
+      <c r="C116" s="130"/>
+      <c r="D116" s="130"/>
+      <c r="E116" s="130"/>
+      <c r="F116" s="130"/>
+      <c r="G116" s="130"/>
+      <c r="H116" s="130"/>
+      <c r="I116" s="130"/>
+      <c r="J116" s="130"/>
+      <c r="K116" s="130"/>
+      <c r="L116" s="130"/>
+      <c r="M116" s="129"/>
+      <c r="N116" s="129"/>
       <c r="O116" s="64"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="37"/>
       <c r="B117" s="37"/>
-      <c r="C117" s="124"/>
-      <c r="D117" s="124"/>
-      <c r="E117" s="124"/>
-      <c r="F117" s="124"/>
-      <c r="G117" s="124"/>
-      <c r="H117" s="124"/>
-      <c r="I117" s="124"/>
-      <c r="J117" s="124"/>
-      <c r="K117" s="124"/>
-      <c r="L117" s="124"/>
-      <c r="M117" s="125"/>
-      <c r="N117" s="125"/>
+      <c r="C117" s="130"/>
+      <c r="D117" s="130"/>
+      <c r="E117" s="130"/>
+      <c r="F117" s="130"/>
+      <c r="G117" s="130"/>
+      <c r="H117" s="130"/>
+      <c r="I117" s="130"/>
+      <c r="J117" s="130"/>
+      <c r="K117" s="130"/>
+      <c r="L117" s="130"/>
+      <c r="M117" s="129"/>
+      <c r="N117" s="129"/>
       <c r="O117" s="64"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="37"/>
       <c r="B118" s="37"/>
-      <c r="C118" s="124"/>
-      <c r="D118" s="124"/>
-      <c r="E118" s="124"/>
-      <c r="F118" s="124"/>
-      <c r="G118" s="124"/>
-      <c r="H118" s="124"/>
-      <c r="I118" s="124"/>
-      <c r="J118" s="124"/>
-      <c r="K118" s="124"/>
-      <c r="L118" s="124"/>
-      <c r="M118" s="125"/>
-      <c r="N118" s="125"/>
+      <c r="C118" s="130"/>
+      <c r="D118" s="130"/>
+      <c r="E118" s="130"/>
+      <c r="F118" s="130"/>
+      <c r="G118" s="130"/>
+      <c r="H118" s="130"/>
+      <c r="I118" s="130"/>
+      <c r="J118" s="130"/>
+      <c r="K118" s="130"/>
+      <c r="L118" s="130"/>
+      <c r="M118" s="129"/>
+      <c r="N118" s="129"/>
       <c r="O118" s="64"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.6">
@@ -9107,28 +9107,119 @@
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="174">
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="M90:N90"/>
     <mergeCell ref="F83:P83"/>
@@ -9153,28 +9244,28 @@
     <mergeCell ref="F65:G65"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
     <mergeCell ref="C92:G92"/>
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="Q77:R77"/>
@@ -9190,97 +9281,6 @@
     <mergeCell ref="H95:L95"/>
     <mergeCell ref="H96:L96"/>
     <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
AWM range: 1800 -> 2000
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F78C66F-9D49-4410-82E5-79139561452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6628ABE-0AAD-418F-AFA5-813EA1B07EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7358" yWindow="495" windowWidth="14242" windowHeight="12112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2590,28 +2590,46 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2629,28 +2647,10 @@
     <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3899,7 +3899,7 @@
   <dimension ref="A1:AL143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3917,10 +3917,10 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="134" t="s">
+      <c r="C1" s="140" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="134"/>
+      <c r="D1" s="140"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4016,10 +4016,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="139" t="s">
+      <c r="Z2" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="139"/>
+      <c r="AA2" s="133"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="41">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
@@ -6512,20 +6512,20 @@
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="128" t="s">
+      <c r="C40" s="138" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="128"/>
-      <c r="E40" s="128"/>
-      <c r="F40" s="128"/>
-      <c r="G40" s="128"/>
-      <c r="H40" s="128"/>
-      <c r="I40" s="128" t="s">
+      <c r="D40" s="138"/>
+      <c r="E40" s="138"/>
+      <c r="F40" s="138"/>
+      <c r="G40" s="138"/>
+      <c r="H40" s="138"/>
+      <c r="I40" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="128"/>
-      <c r="K40" s="128"/>
-      <c r="L40" s="128"/>
+      <c r="J40" s="138"/>
+      <c r="K40" s="138"/>
+      <c r="L40" s="138"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -6533,10 +6533,10 @@
       <c r="Q40" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="S40" s="140" t="s">
+      <c r="S40" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="140"/>
+      <c r="T40" s="137"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6546,22 +6546,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="143" t="s">
+      <c r="C41" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="143"/>
-      <c r="E41" s="143"/>
-      <c r="F41" s="143" t="s">
+      <c r="D41" s="139"/>
+      <c r="E41" s="139"/>
+      <c r="F41" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="143"/>
-      <c r="H41" s="143"/>
-      <c r="I41" s="143" t="s">
+      <c r="G41" s="139"/>
+      <c r="H41" s="139"/>
+      <c r="I41" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="143"/>
-      <c r="K41" s="143"/>
-      <c r="L41" s="143"/>
+      <c r="J41" s="139"/>
+      <c r="K41" s="139"/>
+      <c r="L41" s="139"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6569,10 +6569,10 @@
       <c r="Q41" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S41" s="140" t="s">
+      <c r="S41" s="137" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="140"/>
+      <c r="T41" s="137"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6585,22 +6585,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="143" t="s">
+      <c r="C42" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="143"/>
-      <c r="E42" s="143"/>
-      <c r="F42" s="143" t="s">
+      <c r="D42" s="139"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="139" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="143"/>
-      <c r="H42" s="143"/>
-      <c r="I42" s="143" t="s">
+      <c r="G42" s="139"/>
+      <c r="H42" s="139"/>
+      <c r="I42" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="143"/>
-      <c r="K42" s="143"/>
-      <c r="L42" s="143"/>
+      <c r="J42" s="139"/>
+      <c r="K42" s="139"/>
+      <c r="L42" s="139"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6608,10 +6608,10 @@
       <c r="Q42" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S42" s="140" t="s">
+      <c r="S42" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="140"/>
+      <c r="T42" s="137"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6624,22 +6624,22 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="131" t="s">
+      <c r="C43" s="134" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="131"/>
-      <c r="E43" s="131"/>
-      <c r="F43" s="131" t="s">
+      <c r="D43" s="134"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="134" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="131"/>
-      <c r="H43" s="131"/>
-      <c r="I43" s="131" t="s">
+      <c r="G43" s="134"/>
+      <c r="H43" s="134"/>
+      <c r="I43" s="134" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="131"/>
-      <c r="K43" s="131"/>
-      <c r="L43" s="131"/>
+      <c r="J43" s="134"/>
+      <c r="K43" s="134"/>
+      <c r="L43" s="134"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -6647,10 +6647,10 @@
       <c r="Q43" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="S43" s="140" t="s">
+      <c r="S43" s="137" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="140"/>
+      <c r="T43" s="137"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6665,20 +6665,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="131" t="s">
+      <c r="C44" s="134" t="s">
         <v>269</v>
       </c>
-      <c r="D44" s="131"/>
-      <c r="E44" s="131"/>
-      <c r="F44" s="131"/>
-      <c r="G44" s="131"/>
-      <c r="H44" s="131"/>
-      <c r="I44" s="131" t="s">
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
+      <c r="H44" s="134"/>
+      <c r="I44" s="134" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="131"/>
-      <c r="K44" s="131"/>
-      <c r="L44" s="131"/>
+      <c r="J44" s="134"/>
+      <c r="K44" s="134"/>
+      <c r="L44" s="134"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -6761,12 +6761,12 @@
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="131"/>
-      <c r="D49" s="131"/>
-      <c r="E49" s="131"/>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="131"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134"/>
+      <c r="G49" s="134"/>
+      <c r="H49" s="134"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
@@ -6777,18 +6777,18 @@
       <c r="B51" s="76" t="s">
         <v>265</v>
       </c>
-      <c r="C51" s="128" t="s">
+      <c r="C51" s="138" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="128"/>
-      <c r="E51" s="128" t="s">
+      <c r="D51" s="138"/>
+      <c r="E51" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="128"/>
-      <c r="G51" s="128"/>
-      <c r="H51" s="128"/>
-      <c r="I51" s="128"/>
-      <c r="J51" s="128"/>
+      <c r="F51" s="138"/>
+      <c r="G51" s="138"/>
+      <c r="H51" s="138"/>
+      <c r="I51" s="138"/>
+      <c r="J51" s="138"/>
       <c r="K51" s="120" t="s">
         <v>259</v>
       </c>
@@ -6800,18 +6800,18 @@
       <c r="B52" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="C52" s="126" t="s">
+      <c r="C52" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="D52" s="126"/>
-      <c r="E52" s="127" t="s">
+      <c r="D52" s="131"/>
+      <c r="E52" s="136" t="s">
         <v>270</v>
       </c>
-      <c r="F52" s="127"/>
-      <c r="G52" s="127"/>
-      <c r="H52" s="127"/>
-      <c r="I52" s="127"/>
-      <c r="J52" s="127"/>
+      <c r="F52" s="136"/>
+      <c r="G52" s="136"/>
+      <c r="H52" s="136"/>
+      <c r="I52" s="136"/>
+      <c r="J52" s="136"/>
       <c r="K52" s="64" t="s">
         <v>261</v>
       </c>
@@ -6823,18 +6823,18 @@
       <c r="B53" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="C53" s="126" t="s">
+      <c r="C53" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="D53" s="126"/>
-      <c r="E53" s="127" t="s">
+      <c r="D53" s="131"/>
+      <c r="E53" s="136" t="s">
         <v>271</v>
       </c>
-      <c r="F53" s="127"/>
-      <c r="G53" s="127"/>
-      <c r="H53" s="127"/>
-      <c r="I53" s="127"/>
-      <c r="J53" s="127"/>
+      <c r="F53" s="136"/>
+      <c r="G53" s="136"/>
+      <c r="H53" s="136"/>
+      <c r="I53" s="136"/>
+      <c r="J53" s="136"/>
       <c r="K53" s="64" t="s">
         <v>261</v>
       </c>
@@ -6846,18 +6846,18 @@
       <c r="B54" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="C54" s="126" t="s">
+      <c r="C54" s="131" t="s">
         <v>274</v>
       </c>
-      <c r="D54" s="126"/>
-      <c r="E54" s="127" t="s">
+      <c r="D54" s="131"/>
+      <c r="E54" s="136" t="s">
         <v>272</v>
       </c>
-      <c r="F54" s="127"/>
-      <c r="G54" s="127"/>
-      <c r="H54" s="127"/>
-      <c r="I54" s="127"/>
-      <c r="J54" s="127"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="136"/>
+      <c r="H54" s="136"/>
+      <c r="I54" s="136"/>
+      <c r="J54" s="136"/>
       <c r="K54" s="64" t="s">
         <v>261</v>
       </c>
@@ -6874,14 +6874,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="133" t="s">
+      <c r="H56" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="133"/>
-      <c r="J56" s="133"/>
-      <c r="K56" s="133"/>
-      <c r="L56" s="133"/>
-      <c r="M56" s="133"/>
+      <c r="I56" s="146"/>
+      <c r="J56" s="146"/>
+      <c r="K56" s="146"/>
+      <c r="L56" s="146"/>
+      <c r="M56" s="146"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
@@ -7085,10 +7085,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="136" t="s">
+      <c r="J62" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="136"/>
+      <c r="K62" s="142"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7096,13 +7096,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="135" t="s">
+      <c r="O62" s="141" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="135"/>
-      <c r="Q62" s="135"/>
-      <c r="R62" s="135"/>
-      <c r="S62" s="135"/>
+      <c r="P62" s="141"/>
+      <c r="Q62" s="141"/>
+      <c r="R62" s="141"/>
+      <c r="S62" s="141"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
@@ -7124,20 +7124,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="141" t="s">
+      <c r="F63" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="141"/>
+      <c r="G63" s="128"/>
       <c r="H63" s="85" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="141" t="s">
+      <c r="J63" s="128" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="141"/>
+      <c r="K63" s="128"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7161,10 +7161,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="141" t="s">
+      <c r="U63" s="128" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="141"/>
+      <c r="V63" s="128"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7192,21 +7192,21 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="142" t="s">
+      <c r="F64" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="142"/>
+      <c r="G64" s="145"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="126">
+      <c r="J64" s="131">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="126"/>
+      <c r="K64" s="131"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7237,11 +7237,11 @@
         <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="145">
+      <c r="U64" s="129">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="145"/>
+      <c r="V64" s="129"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7269,21 +7269,21 @@
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="129" t="s">
+      <c r="F65" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="129"/>
+      <c r="G65" s="127"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="126">
+      <c r="J65" s="131">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="126"/>
+      <c r="K65" s="131"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -7314,11 +7314,11 @@
         <v>14.8</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="146">
+      <c r="U65" s="130">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
         <v>10.8</v>
       </c>
-      <c r="V65" s="146"/>
+      <c r="V65" s="130"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7346,21 +7346,21 @@
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="129" t="s">
+      <c r="F66" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="129"/>
+      <c r="G66" s="127"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="126">
+      <c r="J66" s="131">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="126"/>
+      <c r="K66" s="131"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -7391,11 +7391,11 @@
         <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="146">
+      <c r="U66" s="130">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="146"/>
+      <c r="V66" s="130"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7423,21 +7423,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="129" t="s">
+      <c r="F67" s="127" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="129"/>
+      <c r="G67" s="127"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="126">
+      <c r="J67" s="131">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="126"/>
+      <c r="K67" s="131"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -7468,11 +7468,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="146">
+      <c r="U67" s="130">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="146"/>
+      <c r="V67" s="130"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7496,21 +7496,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="129" t="s">
+      <c r="F68" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="129"/>
+      <c r="G68" s="127"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="126">
+      <c r="J68" s="131">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="126"/>
+      <c r="K68" s="131"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7541,11 +7541,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="146">
+      <c r="U68" s="130">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="146"/>
+      <c r="V68" s="130"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7569,21 +7569,21 @@
       <c r="E69" s="53">
         <v>10</v>
       </c>
-      <c r="F69" s="129" t="s">
+      <c r="F69" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="129"/>
+      <c r="G69" s="127"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="126">
+      <c r="J69" s="131">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="126"/>
+      <c r="K69" s="131"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7614,11 +7614,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="146">
+      <c r="U69" s="130">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="146"/>
+      <c r="V69" s="130"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7642,21 +7642,21 @@
       <c r="E70" s="53">
         <v>8</v>
       </c>
-      <c r="F70" s="129" t="s">
+      <c r="F70" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="129"/>
+      <c r="G70" s="127"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="126">
+      <c r="J70" s="131">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="126"/>
+      <c r="K70" s="131"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7687,11 +7687,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="146">
+      <c r="U70" s="130">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="146"/>
+      <c r="V70" s="130"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7707,12 +7707,12 @@
       <c r="B73" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="O73" s="139" t="s">
+      <c r="O73" s="133" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="139"/>
-      <c r="Q73" s="139"/>
-      <c r="R73" s="139"/>
+      <c r="P73" s="133"/>
+      <c r="Q73" s="133"/>
+      <c r="R73" s="133"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7773,21 +7773,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="126" t="s">
+      <c r="F75" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="126"/>
-      <c r="H75" s="126">
+      <c r="G75" s="131"/>
+      <c r="H75" s="131">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="126"/>
-      <c r="J75" s="126" t="s">
+      <c r="I75" s="131"/>
+      <c r="J75" s="131" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="126"/>
-      <c r="L75" s="126"/>
-      <c r="M75" s="126"/>
+      <c r="K75" s="131"/>
+      <c r="L75" s="131"/>
+      <c r="M75" s="131"/>
       <c r="N75" s="77" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7819,21 +7819,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="126" t="s">
+      <c r="F76" s="131" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="126"/>
-      <c r="H76" s="126">
+      <c r="G76" s="131"/>
+      <c r="H76" s="131">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="126"/>
-      <c r="J76" s="126" t="s">
+      <c r="I76" s="131"/>
+      <c r="J76" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="126"/>
-      <c r="L76" s="126"/>
-      <c r="M76" s="126"/>
+      <c r="K76" s="131"/>
+      <c r="L76" s="131"/>
+      <c r="M76" s="131"/>
       <c r="N76" s="77" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7855,19 +7855,19 @@
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="131"/>
-      <c r="G77" s="131"/>
-      <c r="H77" s="131"/>
-      <c r="I77" s="131"/>
-      <c r="J77" s="131"/>
-      <c r="K77" s="131"/>
-      <c r="L77" s="131"/>
-      <c r="M77" s="131"/>
+      <c r="F77" s="134"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="134"/>
+      <c r="I77" s="134"/>
+      <c r="J77" s="134"/>
+      <c r="K77" s="134"/>
+      <c r="L77" s="134"/>
+      <c r="M77" s="134"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="137"/>
-      <c r="P77" s="137"/>
-      <c r="Q77" s="137"/>
-      <c r="R77" s="137"/>
+      <c r="O77" s="143"/>
+      <c r="P77" s="143"/>
+      <c r="Q77" s="143"/>
+      <c r="R77" s="143"/>
       <c r="S77" s="64"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7940,32 +7940,32 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="144" t="s">
+      <c r="F82" s="135" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="144"/>
-      <c r="H82" s="144"/>
-      <c r="I82" s="144"/>
-      <c r="J82" s="144"/>
-      <c r="K82" s="144"/>
-      <c r="L82" s="144"/>
-      <c r="M82" s="144"/>
-      <c r="N82" s="144"/>
-      <c r="O82" s="144"/>
-      <c r="P82" s="144"/>
-      <c r="Q82" s="144" t="s">
+      <c r="G82" s="135"/>
+      <c r="H82" s="135"/>
+      <c r="I82" s="135"/>
+      <c r="J82" s="135"/>
+      <c r="K82" s="135"/>
+      <c r="L82" s="135"/>
+      <c r="M82" s="135"/>
+      <c r="N82" s="135"/>
+      <c r="O82" s="135"/>
+      <c r="P82" s="135"/>
+      <c r="Q82" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="144"/>
-      <c r="S82" s="144"/>
-      <c r="T82" s="144"/>
-      <c r="U82" s="144"/>
-      <c r="V82" s="144"/>
-      <c r="W82" s="144"/>
-      <c r="X82" s="144"/>
-      <c r="Y82" s="144"/>
-      <c r="Z82" s="144"/>
-      <c r="AA82" s="144"/>
+      <c r="R82" s="135"/>
+      <c r="S82" s="135"/>
+      <c r="T82" s="135"/>
+      <c r="U82" s="135"/>
+      <c r="V82" s="135"/>
+      <c r="W82" s="135"/>
+      <c r="X82" s="135"/>
+      <c r="Y82" s="135"/>
+      <c r="Z82" s="135"/>
+      <c r="AA82" s="135"/>
       <c r="AB82" s="64" t="s">
         <v>260</v>
       </c>
@@ -7984,30 +7984,30 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="127" t="s">
+      <c r="F83" s="136" t="s">
         <v>225</v>
       </c>
-      <c r="G83" s="127"/>
-      <c r="H83" s="127"/>
-      <c r="I83" s="127"/>
-      <c r="J83" s="127"/>
-      <c r="K83" s="127"/>
-      <c r="L83" s="127"/>
-      <c r="M83" s="127"/>
-      <c r="N83" s="127"/>
-      <c r="O83" s="127"/>
-      <c r="P83" s="127"/>
-      <c r="Q83" s="127"/>
-      <c r="R83" s="127"/>
-      <c r="S83" s="127"/>
-      <c r="T83" s="127"/>
-      <c r="U83" s="127"/>
-      <c r="V83" s="127"/>
-      <c r="W83" s="127"/>
-      <c r="X83" s="127"/>
-      <c r="Y83" s="127"/>
-      <c r="Z83" s="127"/>
-      <c r="AA83" s="127"/>
+      <c r="G83" s="136"/>
+      <c r="H83" s="136"/>
+      <c r="I83" s="136"/>
+      <c r="J83" s="136"/>
+      <c r="K83" s="136"/>
+      <c r="L83" s="136"/>
+      <c r="M83" s="136"/>
+      <c r="N83" s="136"/>
+      <c r="O83" s="136"/>
+      <c r="P83" s="136"/>
+      <c r="Q83" s="136"/>
+      <c r="R83" s="136"/>
+      <c r="S83" s="136"/>
+      <c r="T83" s="136"/>
+      <c r="U83" s="136"/>
+      <c r="V83" s="136"/>
+      <c r="W83" s="136"/>
+      <c r="X83" s="136"/>
+      <c r="Y83" s="136"/>
+      <c r="Z83" s="136"/>
+      <c r="AA83" s="136"/>
       <c r="AB83" s="64" t="s">
         <v>260</v>
       </c>
@@ -8026,30 +8026,30 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="127" t="s">
+      <c r="F84" s="136" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="127"/>
-      <c r="H84" s="127"/>
-      <c r="I84" s="127"/>
-      <c r="J84" s="127"/>
-      <c r="K84" s="127"/>
-      <c r="L84" s="127"/>
-      <c r="M84" s="127"/>
-      <c r="N84" s="127"/>
-      <c r="O84" s="127"/>
-      <c r="P84" s="127"/>
-      <c r="Q84" s="127"/>
-      <c r="R84" s="127"/>
-      <c r="S84" s="127"/>
-      <c r="T84" s="127"/>
-      <c r="U84" s="127"/>
-      <c r="V84" s="127"/>
-      <c r="W84" s="127"/>
-      <c r="X84" s="127"/>
-      <c r="Y84" s="127"/>
-      <c r="Z84" s="127"/>
-      <c r="AA84" s="127"/>
+      <c r="G84" s="136"/>
+      <c r="H84" s="136"/>
+      <c r="I84" s="136"/>
+      <c r="J84" s="136"/>
+      <c r="K84" s="136"/>
+      <c r="L84" s="136"/>
+      <c r="M84" s="136"/>
+      <c r="N84" s="136"/>
+      <c r="O84" s="136"/>
+      <c r="P84" s="136"/>
+      <c r="Q84" s="136"/>
+      <c r="R84" s="136"/>
+      <c r="S84" s="136"/>
+      <c r="T84" s="136"/>
+      <c r="U84" s="136"/>
+      <c r="V84" s="136"/>
+      <c r="W84" s="136"/>
+      <c r="X84" s="136"/>
+      <c r="Y84" s="136"/>
+      <c r="Z84" s="136"/>
+      <c r="AA84" s="136"/>
       <c r="AB84" s="64" t="s">
         <v>260</v>
       </c>
@@ -8068,32 +8068,32 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="127" t="s">
+      <c r="F85" s="136" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="127"/>
-      <c r="H85" s="127"/>
-      <c r="I85" s="127"/>
-      <c r="J85" s="127"/>
-      <c r="K85" s="127"/>
-      <c r="L85" s="127"/>
-      <c r="M85" s="127"/>
-      <c r="N85" s="127"/>
-      <c r="O85" s="127"/>
-      <c r="P85" s="127"/>
-      <c r="Q85" s="127" t="s">
+      <c r="G85" s="136"/>
+      <c r="H85" s="136"/>
+      <c r="I85" s="136"/>
+      <c r="J85" s="136"/>
+      <c r="K85" s="136"/>
+      <c r="L85" s="136"/>
+      <c r="M85" s="136"/>
+      <c r="N85" s="136"/>
+      <c r="O85" s="136"/>
+      <c r="P85" s="136"/>
+      <c r="Q85" s="136" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="127"/>
-      <c r="S85" s="127"/>
-      <c r="T85" s="127"/>
-      <c r="U85" s="127"/>
-      <c r="V85" s="127"/>
-      <c r="W85" s="127"/>
-      <c r="X85" s="127"/>
-      <c r="Y85" s="127"/>
-      <c r="Z85" s="127"/>
-      <c r="AA85" s="127"/>
+      <c r="R85" s="136"/>
+      <c r="S85" s="136"/>
+      <c r="T85" s="136"/>
+      <c r="U85" s="136"/>
+      <c r="V85" s="136"/>
+      <c r="W85" s="136"/>
+      <c r="X85" s="136"/>
+      <c r="Y85" s="136"/>
+      <c r="Z85" s="136"/>
+      <c r="AA85" s="136"/>
       <c r="AB85" s="64" t="s">
         <v>260</v>
       </c>
@@ -8112,32 +8112,32 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="127" t="s">
+      <c r="F86" s="136" t="s">
         <v>257</v>
       </c>
-      <c r="G86" s="127"/>
-      <c r="H86" s="127"/>
-      <c r="I86" s="127"/>
-      <c r="J86" s="127"/>
-      <c r="K86" s="127"/>
-      <c r="L86" s="127"/>
-      <c r="M86" s="127"/>
-      <c r="N86" s="127"/>
-      <c r="O86" s="127"/>
-      <c r="P86" s="127"/>
-      <c r="Q86" s="127" t="s">
+      <c r="G86" s="136"/>
+      <c r="H86" s="136"/>
+      <c r="I86" s="136"/>
+      <c r="J86" s="136"/>
+      <c r="K86" s="136"/>
+      <c r="L86" s="136"/>
+      <c r="M86" s="136"/>
+      <c r="N86" s="136"/>
+      <c r="O86" s="136"/>
+      <c r="P86" s="136"/>
+      <c r="Q86" s="136" t="s">
         <v>258</v>
       </c>
-      <c r="R86" s="127"/>
-      <c r="S86" s="127"/>
-      <c r="T86" s="127"/>
-      <c r="U86" s="127"/>
-      <c r="V86" s="127"/>
-      <c r="W86" s="127"/>
-      <c r="X86" s="127"/>
-      <c r="Y86" s="127"/>
-      <c r="Z86" s="127"/>
-      <c r="AA86" s="127"/>
+      <c r="R86" s="136"/>
+      <c r="S86" s="136"/>
+      <c r="T86" s="136"/>
+      <c r="U86" s="136"/>
+      <c r="V86" s="136"/>
+      <c r="W86" s="136"/>
+      <c r="X86" s="136"/>
+      <c r="Y86" s="136"/>
+      <c r="Z86" s="136"/>
+      <c r="AA86" s="136"/>
       <c r="AB86" s="64" t="s">
         <v>261</v>
       </c>
@@ -8152,28 +8152,28 @@
       </c>
       <c r="D87" s="53"/>
       <c r="E87" s="53"/>
-      <c r="F87" s="127"/>
-      <c r="G87" s="127"/>
-      <c r="H87" s="127"/>
-      <c r="I87" s="127"/>
-      <c r="J87" s="127"/>
-      <c r="K87" s="127"/>
-      <c r="L87" s="127"/>
-      <c r="M87" s="127"/>
-      <c r="N87" s="127"/>
-      <c r="O87" s="127"/>
-      <c r="P87" s="127"/>
-      <c r="Q87" s="127"/>
-      <c r="R87" s="127"/>
-      <c r="S87" s="127"/>
-      <c r="T87" s="127"/>
-      <c r="U87" s="127"/>
-      <c r="V87" s="127"/>
-      <c r="W87" s="127"/>
-      <c r="X87" s="127"/>
-      <c r="Y87" s="127"/>
-      <c r="Z87" s="127"/>
-      <c r="AA87" s="127"/>
+      <c r="F87" s="136"/>
+      <c r="G87" s="136"/>
+      <c r="H87" s="136"/>
+      <c r="I87" s="136"/>
+      <c r="J87" s="136"/>
+      <c r="K87" s="136"/>
+      <c r="L87" s="136"/>
+      <c r="M87" s="136"/>
+      <c r="N87" s="136"/>
+      <c r="O87" s="136"/>
+      <c r="P87" s="136"/>
+      <c r="Q87" s="136"/>
+      <c r="R87" s="136"/>
+      <c r="S87" s="136"/>
+      <c r="T87" s="136"/>
+      <c r="U87" s="136"/>
+      <c r="V87" s="136"/>
+      <c r="W87" s="136"/>
+      <c r="X87" s="136"/>
+      <c r="Y87" s="136"/>
+      <c r="Z87" s="136"/>
+      <c r="AA87" s="136"/>
       <c r="AB87" s="64" t="s">
         <v>261</v>
       </c>
@@ -8185,20 +8185,20 @@
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="138" t="s">
+      <c r="C90" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="138"/>
-      <c r="E90" s="138"/>
-      <c r="F90" s="138"/>
-      <c r="G90" s="138"/>
-      <c r="H90" s="138" t="s">
+      <c r="D90" s="144"/>
+      <c r="E90" s="144"/>
+      <c r="F90" s="144"/>
+      <c r="G90" s="144"/>
+      <c r="H90" s="144" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="138"/>
-      <c r="J90" s="138"/>
-      <c r="K90" s="138"/>
-      <c r="L90" s="138"/>
+      <c r="I90" s="144"/>
+      <c r="J90" s="144"/>
+      <c r="K90" s="144"/>
+      <c r="L90" s="144"/>
       <c r="M90" s="132" t="s">
         <v>186</v>
       </c>
@@ -8215,24 +8215,24 @@
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="130" t="s">
+      <c r="C91" s="126" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="130"/>
-      <c r="E91" s="130"/>
-      <c r="F91" s="130"/>
-      <c r="G91" s="130"/>
-      <c r="H91" s="130" t="s">
+      <c r="D91" s="126"/>
+      <c r="E91" s="126"/>
+      <c r="F91" s="126"/>
+      <c r="G91" s="126"/>
+      <c r="H91" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="130"/>
-      <c r="J91" s="130"/>
-      <c r="K91" s="130"/>
-      <c r="L91" s="130"/>
-      <c r="M91" s="129" t="s">
+      <c r="I91" s="126"/>
+      <c r="J91" s="126"/>
+      <c r="K91" s="126"/>
+      <c r="L91" s="126"/>
+      <c r="M91" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="129"/>
+      <c r="N91" s="127"/>
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8242,24 +8242,24 @@
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="130" t="s">
+      <c r="C92" s="126" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="130"/>
-      <c r="E92" s="130"/>
-      <c r="F92" s="130"/>
-      <c r="G92" s="130"/>
-      <c r="H92" s="130" t="s">
+      <c r="D92" s="126"/>
+      <c r="E92" s="126"/>
+      <c r="F92" s="126"/>
+      <c r="G92" s="126"/>
+      <c r="H92" s="126" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="130"/>
-      <c r="J92" s="130"/>
-      <c r="K92" s="130"/>
-      <c r="L92" s="130"/>
-      <c r="M92" s="129" t="s">
+      <c r="I92" s="126"/>
+      <c r="J92" s="126"/>
+      <c r="K92" s="126"/>
+      <c r="L92" s="126"/>
+      <c r="M92" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="129"/>
+      <c r="N92" s="127"/>
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8269,24 +8269,24 @@
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="130" t="s">
+      <c r="C93" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="130"/>
-      <c r="E93" s="130"/>
-      <c r="F93" s="130"/>
-      <c r="G93" s="130"/>
-      <c r="H93" s="130" t="s">
+      <c r="D93" s="126"/>
+      <c r="E93" s="126"/>
+      <c r="F93" s="126"/>
+      <c r="G93" s="126"/>
+      <c r="H93" s="126" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="130"/>
-      <c r="J93" s="130"/>
-      <c r="K93" s="130"/>
-      <c r="L93" s="130"/>
-      <c r="M93" s="129" t="s">
+      <c r="I93" s="126"/>
+      <c r="J93" s="126"/>
+      <c r="K93" s="126"/>
+      <c r="L93" s="126"/>
+      <c r="M93" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="129"/>
+      <c r="N93" s="127"/>
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8296,24 +8296,24 @@
       <c r="B94" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C94" s="130" t="s">
+      <c r="C94" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="130"/>
-      <c r="E94" s="130"/>
-      <c r="F94" s="130"/>
-      <c r="G94" s="130"/>
-      <c r="H94" s="130" t="s">
+      <c r="D94" s="126"/>
+      <c r="E94" s="126"/>
+      <c r="F94" s="126"/>
+      <c r="G94" s="126"/>
+      <c r="H94" s="126" t="s">
         <v>217</v>
       </c>
-      <c r="I94" s="130"/>
-      <c r="J94" s="130"/>
-      <c r="K94" s="130"/>
-      <c r="L94" s="130"/>
-      <c r="M94" s="129" t="s">
+      <c r="I94" s="126"/>
+      <c r="J94" s="126"/>
+      <c r="K94" s="126"/>
+      <c r="L94" s="126"/>
+      <c r="M94" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="129"/>
+      <c r="N94" s="127"/>
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8323,24 +8323,24 @@
       <c r="B95" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C95" s="130" t="s">
+      <c r="C95" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="130"/>
-      <c r="E95" s="130"/>
-      <c r="F95" s="130"/>
-      <c r="G95" s="130"/>
-      <c r="H95" s="130" t="s">
+      <c r="D95" s="126"/>
+      <c r="E95" s="126"/>
+      <c r="F95" s="126"/>
+      <c r="G95" s="126"/>
+      <c r="H95" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="I95" s="130"/>
-      <c r="J95" s="130"/>
-      <c r="K95" s="130"/>
-      <c r="L95" s="130"/>
-      <c r="M95" s="129" t="s">
+      <c r="I95" s="126"/>
+      <c r="J95" s="126"/>
+      <c r="K95" s="126"/>
+      <c r="L95" s="126"/>
+      <c r="M95" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="129"/>
+      <c r="N95" s="127"/>
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8350,24 +8350,24 @@
       <c r="B96" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="130" t="s">
+      <c r="C96" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="130"/>
-      <c r="E96" s="130"/>
-      <c r="F96" s="130"/>
-      <c r="G96" s="130"/>
-      <c r="H96" s="130" t="s">
+      <c r="D96" s="126"/>
+      <c r="E96" s="126"/>
+      <c r="F96" s="126"/>
+      <c r="G96" s="126"/>
+      <c r="H96" s="126" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="130"/>
-      <c r="J96" s="130"/>
-      <c r="K96" s="130"/>
-      <c r="L96" s="130"/>
-      <c r="M96" s="129" t="s">
+      <c r="I96" s="126"/>
+      <c r="J96" s="126"/>
+      <c r="K96" s="126"/>
+      <c r="L96" s="126"/>
+      <c r="M96" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="129"/>
+      <c r="N96" s="127"/>
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8377,24 +8377,24 @@
       <c r="B97" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="130" t="s">
+      <c r="C97" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="130"/>
-      <c r="E97" s="130"/>
-      <c r="F97" s="130"/>
-      <c r="G97" s="130"/>
-      <c r="H97" s="130" t="s">
+      <c r="D97" s="126"/>
+      <c r="E97" s="126"/>
+      <c r="F97" s="126"/>
+      <c r="G97" s="126"/>
+      <c r="H97" s="126" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="130"/>
-      <c r="J97" s="130"/>
-      <c r="K97" s="130"/>
-      <c r="L97" s="130"/>
-      <c r="M97" s="129" t="s">
+      <c r="I97" s="126"/>
+      <c r="J97" s="126"/>
+      <c r="K97" s="126"/>
+      <c r="L97" s="126"/>
+      <c r="M97" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="129"/>
+      <c r="N97" s="127"/>
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8404,24 +8404,24 @@
       <c r="B98" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C98" s="130" t="s">
+      <c r="C98" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="130"/>
-      <c r="E98" s="130"/>
-      <c r="F98" s="130"/>
-      <c r="G98" s="130"/>
-      <c r="H98" s="130" t="s">
+      <c r="D98" s="126"/>
+      <c r="E98" s="126"/>
+      <c r="F98" s="126"/>
+      <c r="G98" s="126"/>
+      <c r="H98" s="126" t="s">
         <v>221</v>
       </c>
-      <c r="I98" s="130"/>
-      <c r="J98" s="130"/>
-      <c r="K98" s="130"/>
-      <c r="L98" s="130"/>
-      <c r="M98" s="129" t="s">
+      <c r="I98" s="126"/>
+      <c r="J98" s="126"/>
+      <c r="K98" s="126"/>
+      <c r="L98" s="126"/>
+      <c r="M98" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="129"/>
+      <c r="N98" s="127"/>
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8431,24 +8431,24 @@
       <c r="B99" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="130" t="s">
+      <c r="C99" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="130"/>
-      <c r="E99" s="130"/>
-      <c r="F99" s="130"/>
-      <c r="G99" s="130"/>
-      <c r="H99" s="130" t="s">
+      <c r="D99" s="126"/>
+      <c r="E99" s="126"/>
+      <c r="F99" s="126"/>
+      <c r="G99" s="126"/>
+      <c r="H99" s="126" t="s">
         <v>222</v>
       </c>
-      <c r="I99" s="130"/>
-      <c r="J99" s="130"/>
-      <c r="K99" s="130"/>
-      <c r="L99" s="130"/>
-      <c r="M99" s="129" t="s">
+      <c r="I99" s="126"/>
+      <c r="J99" s="126"/>
+      <c r="K99" s="126"/>
+      <c r="L99" s="126"/>
+      <c r="M99" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="129"/>
+      <c r="N99" s="127"/>
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8458,325 +8458,325 @@
       <c r="B100" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="130" t="s">
+      <c r="C100" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D100" s="130"/>
-      <c r="E100" s="130"/>
-      <c r="F100" s="130"/>
-      <c r="G100" s="130"/>
-      <c r="H100" s="130" t="s">
+      <c r="D100" s="126"/>
+      <c r="E100" s="126"/>
+      <c r="F100" s="126"/>
+      <c r="G100" s="126"/>
+      <c r="H100" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="I100" s="130"/>
-      <c r="J100" s="130"/>
-      <c r="K100" s="130"/>
-      <c r="L100" s="130"/>
-      <c r="M100" s="129" t="s">
+      <c r="I100" s="126"/>
+      <c r="J100" s="126"/>
+      <c r="K100" s="126"/>
+      <c r="L100" s="126"/>
+      <c r="M100" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="129"/>
+      <c r="N100" s="127"/>
       <c r="O100" s="64"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="130"/>
-      <c r="D101" s="130"/>
-      <c r="E101" s="130"/>
-      <c r="F101" s="130"/>
-      <c r="G101" s="130"/>
-      <c r="H101" s="130"/>
-      <c r="I101" s="130"/>
-      <c r="J101" s="130"/>
-      <c r="K101" s="130"/>
-      <c r="L101" s="130"/>
-      <c r="M101" s="129"/>
-      <c r="N101" s="129"/>
+      <c r="C101" s="126"/>
+      <c r="D101" s="126"/>
+      <c r="E101" s="126"/>
+      <c r="F101" s="126"/>
+      <c r="G101" s="126"/>
+      <c r="H101" s="126"/>
+      <c r="I101" s="126"/>
+      <c r="J101" s="126"/>
+      <c r="K101" s="126"/>
+      <c r="L101" s="126"/>
+      <c r="M101" s="127"/>
+      <c r="N101" s="127"/>
       <c r="O101" s="64"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="130"/>
-      <c r="I102" s="130"/>
-      <c r="J102" s="130"/>
-      <c r="K102" s="130"/>
-      <c r="L102" s="130"/>
-      <c r="M102" s="129"/>
-      <c r="N102" s="129"/>
+      <c r="H102" s="126"/>
+      <c r="I102" s="126"/>
+      <c r="J102" s="126"/>
+      <c r="K102" s="126"/>
+      <c r="L102" s="126"/>
+      <c r="M102" s="127"/>
+      <c r="N102" s="127"/>
       <c r="O102" s="64"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="130"/>
-      <c r="D103" s="130"/>
-      <c r="E103" s="130"/>
-      <c r="F103" s="130"/>
-      <c r="G103" s="130"/>
-      <c r="H103" s="130"/>
-      <c r="I103" s="130"/>
-      <c r="J103" s="130"/>
-      <c r="K103" s="130"/>
-      <c r="L103" s="130"/>
-      <c r="M103" s="129"/>
-      <c r="N103" s="129"/>
+      <c r="C103" s="126"/>
+      <c r="D103" s="126"/>
+      <c r="E103" s="126"/>
+      <c r="F103" s="126"/>
+      <c r="G103" s="126"/>
+      <c r="H103" s="126"/>
+      <c r="I103" s="126"/>
+      <c r="J103" s="126"/>
+      <c r="K103" s="126"/>
+      <c r="L103" s="126"/>
+      <c r="M103" s="127"/>
+      <c r="N103" s="127"/>
       <c r="O103" s="64"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="130"/>
-      <c r="D104" s="130"/>
-      <c r="E104" s="130"/>
-      <c r="F104" s="130"/>
-      <c r="G104" s="130"/>
-      <c r="H104" s="130"/>
-      <c r="I104" s="130"/>
-      <c r="J104" s="130"/>
-      <c r="K104" s="130"/>
-      <c r="L104" s="130"/>
-      <c r="M104" s="129"/>
-      <c r="N104" s="129"/>
+      <c r="C104" s="126"/>
+      <c r="D104" s="126"/>
+      <c r="E104" s="126"/>
+      <c r="F104" s="126"/>
+      <c r="G104" s="126"/>
+      <c r="H104" s="126"/>
+      <c r="I104" s="126"/>
+      <c r="J104" s="126"/>
+      <c r="K104" s="126"/>
+      <c r="L104" s="126"/>
+      <c r="M104" s="127"/>
+      <c r="N104" s="127"/>
       <c r="O104" s="64"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="130"/>
-      <c r="D105" s="130"/>
-      <c r="E105" s="130"/>
-      <c r="F105" s="130"/>
-      <c r="G105" s="130"/>
-      <c r="H105" s="130"/>
-      <c r="I105" s="130"/>
-      <c r="J105" s="130"/>
-      <c r="K105" s="130"/>
-      <c r="L105" s="130"/>
-      <c r="M105" s="129"/>
-      <c r="N105" s="129"/>
+      <c r="C105" s="126"/>
+      <c r="D105" s="126"/>
+      <c r="E105" s="126"/>
+      <c r="F105" s="126"/>
+      <c r="G105" s="126"/>
+      <c r="H105" s="126"/>
+      <c r="I105" s="126"/>
+      <c r="J105" s="126"/>
+      <c r="K105" s="126"/>
+      <c r="L105" s="126"/>
+      <c r="M105" s="127"/>
+      <c r="N105" s="127"/>
       <c r="O105" s="64"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="130"/>
-      <c r="D106" s="130"/>
-      <c r="E106" s="130"/>
-      <c r="F106" s="130"/>
-      <c r="G106" s="130"/>
-      <c r="H106" s="130"/>
-      <c r="I106" s="130"/>
-      <c r="J106" s="130"/>
-      <c r="K106" s="130"/>
-      <c r="L106" s="130"/>
-      <c r="M106" s="129"/>
-      <c r="N106" s="129"/>
+      <c r="C106" s="126"/>
+      <c r="D106" s="126"/>
+      <c r="E106" s="126"/>
+      <c r="F106" s="126"/>
+      <c r="G106" s="126"/>
+      <c r="H106" s="126"/>
+      <c r="I106" s="126"/>
+      <c r="J106" s="126"/>
+      <c r="K106" s="126"/>
+      <c r="L106" s="126"/>
+      <c r="M106" s="127"/>
+      <c r="N106" s="127"/>
       <c r="O106" s="64"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="37"/>
       <c r="B107" s="37"/>
-      <c r="C107" s="130"/>
-      <c r="D107" s="130"/>
-      <c r="E107" s="130"/>
-      <c r="F107" s="130"/>
-      <c r="G107" s="130"/>
-      <c r="H107" s="130"/>
-      <c r="I107" s="130"/>
-      <c r="J107" s="130"/>
-      <c r="K107" s="130"/>
-      <c r="L107" s="130"/>
-      <c r="M107" s="129"/>
-      <c r="N107" s="129"/>
+      <c r="C107" s="126"/>
+      <c r="D107" s="126"/>
+      <c r="E107" s="126"/>
+      <c r="F107" s="126"/>
+      <c r="G107" s="126"/>
+      <c r="H107" s="126"/>
+      <c r="I107" s="126"/>
+      <c r="J107" s="126"/>
+      <c r="K107" s="126"/>
+      <c r="L107" s="126"/>
+      <c r="M107" s="127"/>
+      <c r="N107" s="127"/>
       <c r="O107" s="64"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="37"/>
       <c r="B108" s="37"/>
-      <c r="C108" s="130"/>
-      <c r="D108" s="130"/>
-      <c r="E108" s="130"/>
-      <c r="F108" s="130"/>
-      <c r="G108" s="130"/>
-      <c r="H108" s="130"/>
-      <c r="I108" s="130"/>
-      <c r="J108" s="130"/>
-      <c r="K108" s="130"/>
-      <c r="L108" s="130"/>
-      <c r="M108" s="129"/>
-      <c r="N108" s="129"/>
+      <c r="C108" s="126"/>
+      <c r="D108" s="126"/>
+      <c r="E108" s="126"/>
+      <c r="F108" s="126"/>
+      <c r="G108" s="126"/>
+      <c r="H108" s="126"/>
+      <c r="I108" s="126"/>
+      <c r="J108" s="126"/>
+      <c r="K108" s="126"/>
+      <c r="L108" s="126"/>
+      <c r="M108" s="127"/>
+      <c r="N108" s="127"/>
       <c r="O108" s="64"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="37"/>
       <c r="B109" s="37"/>
-      <c r="C109" s="130"/>
-      <c r="D109" s="130"/>
-      <c r="E109" s="130"/>
-      <c r="F109" s="130"/>
-      <c r="G109" s="130"/>
-      <c r="H109" s="130"/>
-      <c r="I109" s="130"/>
-      <c r="J109" s="130"/>
-      <c r="K109" s="130"/>
-      <c r="L109" s="130"/>
-      <c r="M109" s="129"/>
-      <c r="N109" s="129"/>
+      <c r="C109" s="126"/>
+      <c r="D109" s="126"/>
+      <c r="E109" s="126"/>
+      <c r="F109" s="126"/>
+      <c r="G109" s="126"/>
+      <c r="H109" s="126"/>
+      <c r="I109" s="126"/>
+      <c r="J109" s="126"/>
+      <c r="K109" s="126"/>
+      <c r="L109" s="126"/>
+      <c r="M109" s="127"/>
+      <c r="N109" s="127"/>
       <c r="O109" s="64"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="37"/>
       <c r="B110" s="37"/>
-      <c r="C110" s="130"/>
-      <c r="D110" s="130"/>
-      <c r="E110" s="130"/>
-      <c r="F110" s="130"/>
-      <c r="G110" s="130"/>
-      <c r="H110" s="130"/>
-      <c r="I110" s="130"/>
-      <c r="J110" s="130"/>
-      <c r="K110" s="130"/>
-      <c r="L110" s="130"/>
-      <c r="M110" s="129"/>
-      <c r="N110" s="129"/>
+      <c r="C110" s="126"/>
+      <c r="D110" s="126"/>
+      <c r="E110" s="126"/>
+      <c r="F110" s="126"/>
+      <c r="G110" s="126"/>
+      <c r="H110" s="126"/>
+      <c r="I110" s="126"/>
+      <c r="J110" s="126"/>
+      <c r="K110" s="126"/>
+      <c r="L110" s="126"/>
+      <c r="M110" s="127"/>
+      <c r="N110" s="127"/>
       <c r="O110" s="64"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="37"/>
       <c r="B111" s="37"/>
-      <c r="C111" s="130"/>
-      <c r="D111" s="130"/>
-      <c r="E111" s="130"/>
-      <c r="F111" s="130"/>
-      <c r="G111" s="130"/>
-      <c r="H111" s="130"/>
-      <c r="I111" s="130"/>
-      <c r="J111" s="130"/>
-      <c r="K111" s="130"/>
-      <c r="L111" s="130"/>
-      <c r="M111" s="129"/>
-      <c r="N111" s="129"/>
+      <c r="C111" s="126"/>
+      <c r="D111" s="126"/>
+      <c r="E111" s="126"/>
+      <c r="F111" s="126"/>
+      <c r="G111" s="126"/>
+      <c r="H111" s="126"/>
+      <c r="I111" s="126"/>
+      <c r="J111" s="126"/>
+      <c r="K111" s="126"/>
+      <c r="L111" s="126"/>
+      <c r="M111" s="127"/>
+      <c r="N111" s="127"/>
       <c r="O111" s="64"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="37"/>
       <c r="B112" s="37"/>
-      <c r="C112" s="130"/>
-      <c r="D112" s="130"/>
-      <c r="E112" s="130"/>
-      <c r="F112" s="130"/>
-      <c r="G112" s="130"/>
-      <c r="H112" s="130"/>
-      <c r="I112" s="130"/>
-      <c r="J112" s="130"/>
-      <c r="K112" s="130"/>
-      <c r="L112" s="130"/>
-      <c r="M112" s="129"/>
-      <c r="N112" s="129"/>
+      <c r="C112" s="126"/>
+      <c r="D112" s="126"/>
+      <c r="E112" s="126"/>
+      <c r="F112" s="126"/>
+      <c r="G112" s="126"/>
+      <c r="H112" s="126"/>
+      <c r="I112" s="126"/>
+      <c r="J112" s="126"/>
+      <c r="K112" s="126"/>
+      <c r="L112" s="126"/>
+      <c r="M112" s="127"/>
+      <c r="N112" s="127"/>
       <c r="O112" s="64"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="37"/>
       <c r="B113" s="37"/>
-      <c r="C113" s="130"/>
-      <c r="D113" s="130"/>
-      <c r="E113" s="130"/>
-      <c r="F113" s="130"/>
-      <c r="G113" s="130"/>
-      <c r="H113" s="130"/>
-      <c r="I113" s="130"/>
-      <c r="J113" s="130"/>
-      <c r="K113" s="130"/>
-      <c r="L113" s="130"/>
-      <c r="M113" s="129"/>
-      <c r="N113" s="129"/>
+      <c r="C113" s="126"/>
+      <c r="D113" s="126"/>
+      <c r="E113" s="126"/>
+      <c r="F113" s="126"/>
+      <c r="G113" s="126"/>
+      <c r="H113" s="126"/>
+      <c r="I113" s="126"/>
+      <c r="J113" s="126"/>
+      <c r="K113" s="126"/>
+      <c r="L113" s="126"/>
+      <c r="M113" s="127"/>
+      <c r="N113" s="127"/>
       <c r="O113" s="64"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="37"/>
       <c r="B114" s="37"/>
-      <c r="C114" s="130"/>
-      <c r="D114" s="130"/>
-      <c r="E114" s="130"/>
-      <c r="F114" s="130"/>
-      <c r="G114" s="130"/>
-      <c r="H114" s="130"/>
-      <c r="I114" s="130"/>
-      <c r="J114" s="130"/>
-      <c r="K114" s="130"/>
-      <c r="L114" s="130"/>
-      <c r="M114" s="129"/>
-      <c r="N114" s="129"/>
+      <c r="C114" s="126"/>
+      <c r="D114" s="126"/>
+      <c r="E114" s="126"/>
+      <c r="F114" s="126"/>
+      <c r="G114" s="126"/>
+      <c r="H114" s="126"/>
+      <c r="I114" s="126"/>
+      <c r="J114" s="126"/>
+      <c r="K114" s="126"/>
+      <c r="L114" s="126"/>
+      <c r="M114" s="127"/>
+      <c r="N114" s="127"/>
       <c r="O114" s="64"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="37"/>
       <c r="B115" s="37"/>
-      <c r="C115" s="130"/>
-      <c r="D115" s="130"/>
-      <c r="E115" s="130"/>
-      <c r="F115" s="130"/>
-      <c r="G115" s="130"/>
-      <c r="H115" s="130"/>
-      <c r="I115" s="130"/>
-      <c r="J115" s="130"/>
-      <c r="K115" s="130"/>
-      <c r="L115" s="130"/>
-      <c r="M115" s="129"/>
-      <c r="N115" s="129"/>
+      <c r="C115" s="126"/>
+      <c r="D115" s="126"/>
+      <c r="E115" s="126"/>
+      <c r="F115" s="126"/>
+      <c r="G115" s="126"/>
+      <c r="H115" s="126"/>
+      <c r="I115" s="126"/>
+      <c r="J115" s="126"/>
+      <c r="K115" s="126"/>
+      <c r="L115" s="126"/>
+      <c r="M115" s="127"/>
+      <c r="N115" s="127"/>
       <c r="O115" s="64"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="37"/>
       <c r="B116" s="37"/>
-      <c r="C116" s="130"/>
-      <c r="D116" s="130"/>
-      <c r="E116" s="130"/>
-      <c r="F116" s="130"/>
-      <c r="G116" s="130"/>
-      <c r="H116" s="130"/>
-      <c r="I116" s="130"/>
-      <c r="J116" s="130"/>
-      <c r="K116" s="130"/>
-      <c r="L116" s="130"/>
-      <c r="M116" s="129"/>
-      <c r="N116" s="129"/>
+      <c r="C116" s="126"/>
+      <c r="D116" s="126"/>
+      <c r="E116" s="126"/>
+      <c r="F116" s="126"/>
+      <c r="G116" s="126"/>
+      <c r="H116" s="126"/>
+      <c r="I116" s="126"/>
+      <c r="J116" s="126"/>
+      <c r="K116" s="126"/>
+      <c r="L116" s="126"/>
+      <c r="M116" s="127"/>
+      <c r="N116" s="127"/>
       <c r="O116" s="64"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="37"/>
       <c r="B117" s="37"/>
-      <c r="C117" s="130"/>
-      <c r="D117" s="130"/>
-      <c r="E117" s="130"/>
-      <c r="F117" s="130"/>
-      <c r="G117" s="130"/>
-      <c r="H117" s="130"/>
-      <c r="I117" s="130"/>
-      <c r="J117" s="130"/>
-      <c r="K117" s="130"/>
-      <c r="L117" s="130"/>
-      <c r="M117" s="129"/>
-      <c r="N117" s="129"/>
+      <c r="C117" s="126"/>
+      <c r="D117" s="126"/>
+      <c r="E117" s="126"/>
+      <c r="F117" s="126"/>
+      <c r="G117" s="126"/>
+      <c r="H117" s="126"/>
+      <c r="I117" s="126"/>
+      <c r="J117" s="126"/>
+      <c r="K117" s="126"/>
+      <c r="L117" s="126"/>
+      <c r="M117" s="127"/>
+      <c r="N117" s="127"/>
       <c r="O117" s="64"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="37"/>
       <c r="B118" s="37"/>
-      <c r="C118" s="130"/>
-      <c r="D118" s="130"/>
-      <c r="E118" s="130"/>
-      <c r="F118" s="130"/>
-      <c r="G118" s="130"/>
-      <c r="H118" s="130"/>
-      <c r="I118" s="130"/>
-      <c r="J118" s="130"/>
-      <c r="K118" s="130"/>
-      <c r="L118" s="130"/>
-      <c r="M118" s="129"/>
-      <c r="N118" s="129"/>
+      <c r="C118" s="126"/>
+      <c r="D118" s="126"/>
+      <c r="E118" s="126"/>
+      <c r="F118" s="126"/>
+      <c r="G118" s="126"/>
+      <c r="H118" s="126"/>
+      <c r="I118" s="126"/>
+      <c r="J118" s="126"/>
+      <c r="K118" s="126"/>
+      <c r="L118" s="126"/>
+      <c r="M118" s="127"/>
+      <c r="N118" s="127"/>
       <c r="O118" s="64"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.6">
@@ -9107,119 +9107,34 @@
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="174">
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="M90:N90"/>
     <mergeCell ref="F83:P83"/>
@@ -9244,8 +9159,56 @@
     <mergeCell ref="F65:G65"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="F67:G67"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:H49"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
     <mergeCell ref="F74:G74"/>
     <mergeCell ref="F75:G75"/>
     <mergeCell ref="F70:G70"/>
@@ -9253,34 +9216,71 @@
     <mergeCell ref="J69:K69"/>
     <mergeCell ref="J70:K70"/>
     <mergeCell ref="J74:M74"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added ping (WARNING: this may slow down performance)
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6628ABE-0AAD-418F-AFA5-813EA1B07EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5507632F-B728-4001-803A-E965D58AD2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7358" yWindow="495" windowWidth="14242" windowHeight="12112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="284">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1595,10 +1595,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>???</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(sky) blue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1668,6 +1664,22 @@
   </si>
   <si>
     <t>damage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TORNADO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Projectiles will be directed towards the center constantly with wind speed of maximum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Spawns tornado attracting wind into the strike center </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* after wind update: added wind that blows projectiles/throwables (wind direction changes every minute)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2233,7 +2245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2591,67 +2603,70 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3898,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3917,10 +3932,10 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="140" t="s">
+      <c r="C1" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="140"/>
+      <c r="D1" s="135"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4016,10 +4031,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="133" t="s">
+      <c r="Z2" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="133"/>
+      <c r="AA2" s="139"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -6359,10 +6374,10 @@
         <v>202</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D36" s="73">
         <v>0</v>
@@ -6377,7 +6392,7 @@
         <v>800</v>
       </c>
       <c r="H36" s="64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>51</v>
@@ -6422,7 +6437,7 @@
       </c>
       <c r="Y36" s="19"/>
       <c r="Z36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AL36" s="35"/>
     </row>
@@ -6431,7 +6446,7 @@
         <v>202</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" s="75">
         <v>90</v>
@@ -6512,20 +6527,20 @@
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="138" t="s">
+      <c r="C40" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138" t="s">
+      <c r="D40" s="134"/>
+      <c r="E40" s="134"/>
+      <c r="F40" s="134"/>
+      <c r="G40" s="134"/>
+      <c r="H40" s="134"/>
+      <c r="I40" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="138"/>
-      <c r="K40" s="138"/>
-      <c r="L40" s="138"/>
+      <c r="J40" s="134"/>
+      <c r="K40" s="134"/>
+      <c r="L40" s="134"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -6533,10 +6548,10 @@
       <c r="Q40" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="S40" s="137" t="s">
+      <c r="S40" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="137"/>
+      <c r="T40" s="140"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6546,22 +6561,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="139" t="s">
+      <c r="C41" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="139"/>
-      <c r="E41" s="139"/>
-      <c r="F41" s="139" t="s">
+      <c r="D41" s="143"/>
+      <c r="E41" s="143"/>
+      <c r="F41" s="143" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="139"/>
-      <c r="H41" s="139"/>
-      <c r="I41" s="139" t="s">
+      <c r="G41" s="143"/>
+      <c r="H41" s="143"/>
+      <c r="I41" s="143" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="139"/>
-      <c r="K41" s="139"/>
-      <c r="L41" s="139"/>
+      <c r="J41" s="143"/>
+      <c r="K41" s="143"/>
+      <c r="L41" s="143"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6569,10 +6584,10 @@
       <c r="Q41" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S41" s="137" t="s">
+      <c r="S41" s="140" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="137"/>
+      <c r="T41" s="140"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6585,22 +6600,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="139" t="s">
+      <c r="C42" s="143" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="139"/>
-      <c r="E42" s="139"/>
-      <c r="F42" s="139" t="s">
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="139"/>
-      <c r="H42" s="139"/>
-      <c r="I42" s="139" t="s">
+      <c r="G42" s="143"/>
+      <c r="H42" s="143"/>
+      <c r="I42" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="139"/>
-      <c r="K42" s="139"/>
-      <c r="L42" s="139"/>
+      <c r="J42" s="143"/>
+      <c r="K42" s="143"/>
+      <c r="L42" s="143"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6608,10 +6623,10 @@
       <c r="Q42" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S42" s="137" t="s">
+      <c r="S42" s="140" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="137"/>
+      <c r="T42" s="140"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6624,22 +6639,22 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="134" t="s">
+      <c r="C43" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="134"/>
-      <c r="E43" s="134"/>
-      <c r="F43" s="134" t="s">
+      <c r="D43" s="131"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="131" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="134"/>
-      <c r="H43" s="134"/>
-      <c r="I43" s="134" t="s">
+      <c r="G43" s="131"/>
+      <c r="H43" s="131"/>
+      <c r="I43" s="131" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="134"/>
-      <c r="K43" s="134"/>
-      <c r="L43" s="134"/>
+      <c r="J43" s="131"/>
+      <c r="K43" s="131"/>
+      <c r="L43" s="131"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -6647,10 +6662,10 @@
       <c r="Q43" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="S43" s="137" t="s">
+      <c r="S43" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="137"/>
+      <c r="T43" s="140"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6665,20 +6680,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="134" t="s">
-        <v>269</v>
-      </c>
-      <c r="D44" s="134"/>
-      <c r="E44" s="134"/>
-      <c r="F44" s="134"/>
-      <c r="G44" s="134"/>
-      <c r="H44" s="134"/>
-      <c r="I44" s="134" t="s">
+      <c r="C44" s="131" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" s="131"/>
+      <c r="E44" s="131"/>
+      <c r="F44" s="131"/>
+      <c r="G44" s="131"/>
+      <c r="H44" s="131"/>
+      <c r="I44" s="131" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="134"/>
-      <c r="K44" s="134"/>
-      <c r="L44" s="134"/>
+      <c r="J44" s="131"/>
+      <c r="K44" s="131"/>
+      <c r="L44" s="131"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -6761,12 +6776,12 @@
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="134"/>
-      <c r="D49" s="134"/>
-      <c r="E49" s="134"/>
-      <c r="F49" s="134"/>
-      <c r="G49" s="134"/>
-      <c r="H49" s="134"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="131"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
@@ -6775,20 +6790,20 @@
     <row r="51" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="34"/>
       <c r="B51" s="76" t="s">
-        <v>265</v>
-      </c>
-      <c r="C51" s="138" t="s">
-        <v>273</v>
-      </c>
-      <c r="D51" s="138"/>
-      <c r="E51" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="C51" s="134" t="s">
+        <v>272</v>
+      </c>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="138"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="138"/>
-      <c r="I51" s="138"/>
-      <c r="J51" s="138"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="134"/>
+      <c r="H51" s="134"/>
+      <c r="I51" s="134"/>
+      <c r="J51" s="134"/>
       <c r="K51" s="120" t="s">
         <v>259</v>
       </c>
@@ -6798,20 +6813,20 @@
         <v>202</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="C52" s="131" t="s">
-        <v>275</v>
-      </c>
-      <c r="D52" s="131"/>
-      <c r="E52" s="136" t="s">
-        <v>270</v>
-      </c>
-      <c r="F52" s="136"/>
-      <c r="G52" s="136"/>
-      <c r="H52" s="136"/>
-      <c r="I52" s="136"/>
-      <c r="J52" s="136"/>
+        <v>265</v>
+      </c>
+      <c r="C52" s="133" t="s">
+        <v>274</v>
+      </c>
+      <c r="D52" s="133"/>
+      <c r="E52" s="128" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
+      <c r="H52" s="128"/>
+      <c r="I52" s="128"/>
+      <c r="J52" s="128"/>
       <c r="K52" s="64" t="s">
         <v>261</v>
       </c>
@@ -6821,20 +6836,20 @@
         <v>202</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="C53" s="131" t="s">
-        <v>275</v>
-      </c>
-      <c r="D53" s="131"/>
-      <c r="E53" s="136" t="s">
-        <v>271</v>
-      </c>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="136"/>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
+        <v>266</v>
+      </c>
+      <c r="C53" s="133" t="s">
+        <v>274</v>
+      </c>
+      <c r="D53" s="133"/>
+      <c r="E53" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="F53" s="128"/>
+      <c r="G53" s="128"/>
+      <c r="H53" s="128"/>
+      <c r="I53" s="128"/>
+      <c r="J53" s="128"/>
       <c r="K53" s="64" t="s">
         <v>261</v>
       </c>
@@ -6844,20 +6859,20 @@
         <v>202</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="C54" s="131" t="s">
-        <v>274</v>
-      </c>
-      <c r="D54" s="131"/>
-      <c r="E54" s="136" t="s">
-        <v>272</v>
-      </c>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="H54" s="136"/>
-      <c r="I54" s="136"/>
-      <c r="J54" s="136"/>
+        <v>267</v>
+      </c>
+      <c r="C54" s="133" t="s">
+        <v>273</v>
+      </c>
+      <c r="D54" s="133"/>
+      <c r="E54" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="F54" s="128"/>
+      <c r="G54" s="128"/>
+      <c r="H54" s="128"/>
+      <c r="I54" s="128"/>
+      <c r="J54" s="128"/>
       <c r="K54" s="64" t="s">
         <v>261</v>
       </c>
@@ -6874,14 +6889,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="146" t="s">
+      <c r="H56" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="146"/>
-      <c r="J56" s="146"/>
-      <c r="K56" s="146"/>
-      <c r="L56" s="146"/>
-      <c r="M56" s="146"/>
+      <c r="I56" s="132"/>
+      <c r="J56" s="132"/>
+      <c r="K56" s="132"/>
+      <c r="L56" s="132"/>
+      <c r="M56" s="132"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
@@ -7085,10 +7100,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="142" t="s">
+      <c r="J62" s="138" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="142"/>
+      <c r="K62" s="138"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7096,13 +7111,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="141" t="s">
+      <c r="O62" s="137" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="141"/>
-      <c r="Q62" s="141"/>
-      <c r="R62" s="141"/>
-      <c r="S62" s="141"/>
+      <c r="P62" s="137"/>
+      <c r="Q62" s="137"/>
+      <c r="R62" s="137"/>
+      <c r="S62" s="137"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
@@ -7124,20 +7139,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="128" t="s">
+      <c r="F63" s="141" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="128"/>
+      <c r="G63" s="141"/>
       <c r="H63" s="85" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="128" t="s">
+      <c r="J63" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="128"/>
+      <c r="K63" s="141"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7161,10 +7176,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="128" t="s">
+      <c r="U63" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="128"/>
+      <c r="V63" s="141"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7192,21 +7207,21 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="145" t="s">
+      <c r="F64" s="142" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="145"/>
+      <c r="G64" s="142"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="131">
+      <c r="J64" s="133">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="131"/>
+      <c r="K64" s="133"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7237,11 +7252,11 @@
         <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="129">
+      <c r="U64" s="145">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="129"/>
+      <c r="V64" s="145"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7269,21 +7284,21 @@
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="127" t="s">
+      <c r="F65" s="126" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="127"/>
+      <c r="G65" s="126"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="131">
+      <c r="J65" s="133">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="131"/>
+      <c r="K65" s="133"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -7314,11 +7329,11 @@
         <v>14.8</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="130">
+      <c r="U65" s="146">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
         <v>10.8</v>
       </c>
-      <c r="V65" s="130"/>
+      <c r="V65" s="146"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7346,21 +7361,21 @@
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="127" t="s">
+      <c r="F66" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="127"/>
+      <c r="G66" s="126"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="131">
+      <c r="J66" s="133">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="131"/>
+      <c r="K66" s="133"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -7391,11 +7406,11 @@
         <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="130">
+      <c r="U66" s="146">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="130"/>
+      <c r="V66" s="146"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7423,21 +7438,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="127" t="s">
+      <c r="F67" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="127"/>
+      <c r="G67" s="126"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="131">
+      <c r="J67" s="133">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="131"/>
+      <c r="K67" s="133"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -7468,11 +7483,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="130">
+      <c r="U67" s="146">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="130"/>
+      <c r="V67" s="146"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7496,21 +7511,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="127" t="s">
+      <c r="F68" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="127"/>
+      <c r="G68" s="126"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="131">
+      <c r="J68" s="133">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="131"/>
+      <c r="K68" s="133"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7541,11 +7556,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="130">
+      <c r="U68" s="146">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="130"/>
+      <c r="V68" s="146"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7569,21 +7584,21 @@
       <c r="E69" s="53">
         <v>10</v>
       </c>
-      <c r="F69" s="127" t="s">
+      <c r="F69" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="127"/>
+      <c r="G69" s="126"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="131">
+      <c r="J69" s="133">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="131"/>
+      <c r="K69" s="133"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7614,11 +7629,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="130">
+      <c r="U69" s="146">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="130"/>
+      <c r="V69" s="146"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7642,21 +7657,21 @@
       <c r="E70" s="53">
         <v>8</v>
       </c>
-      <c r="F70" s="127" t="s">
+      <c r="F70" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="127"/>
+      <c r="G70" s="126"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="131">
+      <c r="J70" s="133">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="131"/>
+      <c r="K70" s="133"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7687,11 +7702,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="130">
+      <c r="U70" s="146">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="130"/>
+      <c r="V70" s="146"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7707,12 +7722,12 @@
       <c r="B73" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="O73" s="133" t="s">
+      <c r="O73" s="139" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="133"/>
-      <c r="Q73" s="133"/>
-      <c r="R73" s="133"/>
+      <c r="P73" s="139"/>
+      <c r="Q73" s="139"/>
+      <c r="R73" s="139"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7728,31 +7743,31 @@
       <c r="E74" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="132" t="s">
+      <c r="F74" s="136" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="132"/>
-      <c r="H74" s="132" t="s">
+      <c r="G74" s="136"/>
+      <c r="H74" s="136" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="132"/>
-      <c r="J74" s="132" t="s">
+      <c r="I74" s="136"/>
+      <c r="J74" s="136" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="132"/>
-      <c r="L74" s="132"/>
-      <c r="M74" s="132"/>
+      <c r="K74" s="136"/>
+      <c r="L74" s="136"/>
+      <c r="M74" s="136"/>
       <c r="N74" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="132" t="s">
+      <c r="O74" s="136" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="132"/>
-      <c r="Q74" s="132" t="s">
+      <c r="P74" s="136"/>
+      <c r="Q74" s="136" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="132"/>
+      <c r="R74" s="136"/>
       <c r="S74" s="120" t="s">
         <v>259</v>
       </c>
@@ -7773,21 +7788,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="131" t="s">
+      <c r="F75" s="133" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="131"/>
-      <c r="H75" s="131">
+      <c r="G75" s="133"/>
+      <c r="H75" s="133">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="131"/>
-      <c r="J75" s="131" t="s">
+      <c r="I75" s="133"/>
+      <c r="J75" s="133" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="131"/>
-      <c r="L75" s="131"/>
-      <c r="M75" s="131"/>
+      <c r="K75" s="133"/>
+      <c r="L75" s="133"/>
+      <c r="M75" s="133"/>
       <c r="N75" s="77" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7819,21 +7834,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="131" t="s">
+      <c r="F76" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="131"/>
-      <c r="H76" s="131">
+      <c r="G76" s="133"/>
+      <c r="H76" s="133">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="131"/>
-      <c r="J76" s="131" t="s">
+      <c r="I76" s="133"/>
+      <c r="J76" s="133" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="131"/>
-      <c r="L76" s="131"/>
-      <c r="M76" s="131"/>
+      <c r="K76" s="133"/>
+      <c r="L76" s="133"/>
+      <c r="M76" s="133"/>
       <c r="N76" s="77" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7855,19 +7870,19 @@
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="134"/>
-      <c r="G77" s="134"/>
-      <c r="H77" s="134"/>
-      <c r="I77" s="134"/>
-      <c r="J77" s="134"/>
-      <c r="K77" s="134"/>
-      <c r="L77" s="134"/>
-      <c r="M77" s="134"/>
+      <c r="F77" s="131"/>
+      <c r="G77" s="131"/>
+      <c r="H77" s="131"/>
+      <c r="I77" s="131"/>
+      <c r="J77" s="131"/>
+      <c r="K77" s="131"/>
+      <c r="L77" s="131"/>
+      <c r="M77" s="131"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="143"/>
-      <c r="P77" s="143"/>
-      <c r="Q77" s="143"/>
-      <c r="R77" s="143"/>
+      <c r="O77" s="129"/>
+      <c r="P77" s="129"/>
+      <c r="Q77" s="129"/>
+      <c r="R77" s="129"/>
       <c r="S77" s="64"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7896,32 +7911,32 @@
       <c r="E81" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="132" t="s">
+      <c r="F81" s="136" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="132"/>
-      <c r="H81" s="132"/>
-      <c r="I81" s="132"/>
-      <c r="J81" s="132"/>
-      <c r="K81" s="132"/>
-      <c r="L81" s="132"/>
-      <c r="M81" s="132"/>
-      <c r="N81" s="132"/>
-      <c r="O81" s="132"/>
-      <c r="P81" s="132"/>
-      <c r="Q81" s="132" t="s">
+      <c r="G81" s="136"/>
+      <c r="H81" s="136"/>
+      <c r="I81" s="136"/>
+      <c r="J81" s="136"/>
+      <c r="K81" s="136"/>
+      <c r="L81" s="136"/>
+      <c r="M81" s="136"/>
+      <c r="N81" s="136"/>
+      <c r="O81" s="136"/>
+      <c r="P81" s="136"/>
+      <c r="Q81" s="136" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="132"/>
-      <c r="S81" s="132"/>
-      <c r="T81" s="132"/>
-      <c r="U81" s="132"/>
-      <c r="V81" s="132"/>
-      <c r="W81" s="132"/>
-      <c r="X81" s="132"/>
-      <c r="Y81" s="132"/>
-      <c r="Z81" s="132"/>
-      <c r="AA81" s="132"/>
+      <c r="R81" s="136"/>
+      <c r="S81" s="136"/>
+      <c r="T81" s="136"/>
+      <c r="U81" s="136"/>
+      <c r="V81" s="136"/>
+      <c r="W81" s="136"/>
+      <c r="X81" s="136"/>
+      <c r="Y81" s="136"/>
+      <c r="Z81" s="136"/>
+      <c r="AA81" s="136"/>
       <c r="AB81" s="120" t="s">
         <v>259</v>
       </c>
@@ -7940,32 +7955,32 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="135" t="s">
+      <c r="F82" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="135"/>
-      <c r="H82" s="135"/>
-      <c r="I82" s="135"/>
-      <c r="J82" s="135"/>
-      <c r="K82" s="135"/>
-      <c r="L82" s="135"/>
-      <c r="M82" s="135"/>
-      <c r="N82" s="135"/>
-      <c r="O82" s="135"/>
-      <c r="P82" s="135"/>
-      <c r="Q82" s="135" t="s">
+      <c r="G82" s="144"/>
+      <c r="H82" s="144"/>
+      <c r="I82" s="144"/>
+      <c r="J82" s="144"/>
+      <c r="K82" s="144"/>
+      <c r="L82" s="144"/>
+      <c r="M82" s="144"/>
+      <c r="N82" s="144"/>
+      <c r="O82" s="144"/>
+      <c r="P82" s="144"/>
+      <c r="Q82" s="144" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="135"/>
-      <c r="S82" s="135"/>
-      <c r="T82" s="135"/>
-      <c r="U82" s="135"/>
-      <c r="V82" s="135"/>
-      <c r="W82" s="135"/>
-      <c r="X82" s="135"/>
-      <c r="Y82" s="135"/>
-      <c r="Z82" s="135"/>
-      <c r="AA82" s="135"/>
+      <c r="R82" s="144"/>
+      <c r="S82" s="144"/>
+      <c r="T82" s="144"/>
+      <c r="U82" s="144"/>
+      <c r="V82" s="144"/>
+      <c r="W82" s="144"/>
+      <c r="X82" s="144"/>
+      <c r="Y82" s="144"/>
+      <c r="Z82" s="144"/>
+      <c r="AA82" s="144"/>
       <c r="AB82" s="64" t="s">
         <v>260</v>
       </c>
@@ -7984,30 +7999,30 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="136" t="s">
+      <c r="F83" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="G83" s="136"/>
-      <c r="H83" s="136"/>
-      <c r="I83" s="136"/>
-      <c r="J83" s="136"/>
-      <c r="K83" s="136"/>
-      <c r="L83" s="136"/>
-      <c r="M83" s="136"/>
-      <c r="N83" s="136"/>
-      <c r="O83" s="136"/>
-      <c r="P83" s="136"/>
-      <c r="Q83" s="136"/>
-      <c r="R83" s="136"/>
-      <c r="S83" s="136"/>
-      <c r="T83" s="136"/>
-      <c r="U83" s="136"/>
-      <c r="V83" s="136"/>
-      <c r="W83" s="136"/>
-      <c r="X83" s="136"/>
-      <c r="Y83" s="136"/>
-      <c r="Z83" s="136"/>
-      <c r="AA83" s="136"/>
+      <c r="G83" s="128"/>
+      <c r="H83" s="128"/>
+      <c r="I83" s="128"/>
+      <c r="J83" s="128"/>
+      <c r="K83" s="128"/>
+      <c r="L83" s="128"/>
+      <c r="M83" s="128"/>
+      <c r="N83" s="128"/>
+      <c r="O83" s="128"/>
+      <c r="P83" s="128"/>
+      <c r="Q83" s="128"/>
+      <c r="R83" s="128"/>
+      <c r="S83" s="128"/>
+      <c r="T83" s="128"/>
+      <c r="U83" s="128"/>
+      <c r="V83" s="128"/>
+      <c r="W83" s="128"/>
+      <c r="X83" s="128"/>
+      <c r="Y83" s="128"/>
+      <c r="Z83" s="128"/>
+      <c r="AA83" s="128"/>
       <c r="AB83" s="64" t="s">
         <v>260</v>
       </c>
@@ -8026,30 +8041,30 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="136" t="s">
+      <c r="F84" s="128" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="136"/>
-      <c r="H84" s="136"/>
-      <c r="I84" s="136"/>
-      <c r="J84" s="136"/>
-      <c r="K84" s="136"/>
-      <c r="L84" s="136"/>
-      <c r="M84" s="136"/>
-      <c r="N84" s="136"/>
-      <c r="O84" s="136"/>
-      <c r="P84" s="136"/>
-      <c r="Q84" s="136"/>
-      <c r="R84" s="136"/>
-      <c r="S84" s="136"/>
-      <c r="T84" s="136"/>
-      <c r="U84" s="136"/>
-      <c r="V84" s="136"/>
-      <c r="W84" s="136"/>
-      <c r="X84" s="136"/>
-      <c r="Y84" s="136"/>
-      <c r="Z84" s="136"/>
-      <c r="AA84" s="136"/>
+      <c r="G84" s="128"/>
+      <c r="H84" s="128"/>
+      <c r="I84" s="128"/>
+      <c r="J84" s="128"/>
+      <c r="K84" s="128"/>
+      <c r="L84" s="128"/>
+      <c r="M84" s="128"/>
+      <c r="N84" s="128"/>
+      <c r="O84" s="128"/>
+      <c r="P84" s="128"/>
+      <c r="Q84" s="128"/>
+      <c r="R84" s="128"/>
+      <c r="S84" s="128"/>
+      <c r="T84" s="128"/>
+      <c r="U84" s="128"/>
+      <c r="V84" s="128"/>
+      <c r="W84" s="128"/>
+      <c r="X84" s="128"/>
+      <c r="Y84" s="128"/>
+      <c r="Z84" s="128"/>
+      <c r="AA84" s="128"/>
       <c r="AB84" s="64" t="s">
         <v>260</v>
       </c>
@@ -8068,32 +8083,32 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="136" t="s">
+      <c r="F85" s="128" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="136"/>
-      <c r="H85" s="136"/>
-      <c r="I85" s="136"/>
-      <c r="J85" s="136"/>
-      <c r="K85" s="136"/>
-      <c r="L85" s="136"/>
-      <c r="M85" s="136"/>
-      <c r="N85" s="136"/>
-      <c r="O85" s="136"/>
-      <c r="P85" s="136"/>
-      <c r="Q85" s="136" t="s">
+      <c r="G85" s="128"/>
+      <c r="H85" s="128"/>
+      <c r="I85" s="128"/>
+      <c r="J85" s="128"/>
+      <c r="K85" s="128"/>
+      <c r="L85" s="128"/>
+      <c r="M85" s="128"/>
+      <c r="N85" s="128"/>
+      <c r="O85" s="128"/>
+      <c r="P85" s="128"/>
+      <c r="Q85" s="128" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="136"/>
-      <c r="S85" s="136"/>
-      <c r="T85" s="136"/>
-      <c r="U85" s="136"/>
-      <c r="V85" s="136"/>
-      <c r="W85" s="136"/>
-      <c r="X85" s="136"/>
-      <c r="Y85" s="136"/>
-      <c r="Z85" s="136"/>
-      <c r="AA85" s="136"/>
+      <c r="R85" s="128"/>
+      <c r="S85" s="128"/>
+      <c r="T85" s="128"/>
+      <c r="U85" s="128"/>
+      <c r="V85" s="128"/>
+      <c r="W85" s="128"/>
+      <c r="X85" s="128"/>
+      <c r="Y85" s="128"/>
+      <c r="Z85" s="128"/>
+      <c r="AA85" s="128"/>
       <c r="AB85" s="64" t="s">
         <v>260</v>
       </c>
@@ -8112,32 +8127,32 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="136" t="s">
+      <c r="F86" s="128" t="s">
         <v>257</v>
       </c>
-      <c r="G86" s="136"/>
-      <c r="H86" s="136"/>
-      <c r="I86" s="136"/>
-      <c r="J86" s="136"/>
-      <c r="K86" s="136"/>
-      <c r="L86" s="136"/>
-      <c r="M86" s="136"/>
-      <c r="N86" s="136"/>
-      <c r="O86" s="136"/>
-      <c r="P86" s="136"/>
-      <c r="Q86" s="136" t="s">
+      <c r="G86" s="128"/>
+      <c r="H86" s="128"/>
+      <c r="I86" s="128"/>
+      <c r="J86" s="128"/>
+      <c r="K86" s="128"/>
+      <c r="L86" s="128"/>
+      <c r="M86" s="128"/>
+      <c r="N86" s="128"/>
+      <c r="O86" s="128"/>
+      <c r="P86" s="128"/>
+      <c r="Q86" s="128" t="s">
         <v>258</v>
       </c>
-      <c r="R86" s="136"/>
-      <c r="S86" s="136"/>
-      <c r="T86" s="136"/>
-      <c r="U86" s="136"/>
-      <c r="V86" s="136"/>
-      <c r="W86" s="136"/>
-      <c r="X86" s="136"/>
-      <c r="Y86" s="136"/>
-      <c r="Z86" s="136"/>
-      <c r="AA86" s="136"/>
+      <c r="R86" s="128"/>
+      <c r="S86" s="128"/>
+      <c r="T86" s="128"/>
+      <c r="U86" s="128"/>
+      <c r="V86" s="128"/>
+      <c r="W86" s="128"/>
+      <c r="X86" s="128"/>
+      <c r="Y86" s="128"/>
+      <c r="Z86" s="128"/>
+      <c r="AA86" s="128"/>
       <c r="AB86" s="64" t="s">
         <v>261</v>
       </c>
@@ -8145,64 +8160,76 @@
     <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="37"/>
       <c r="B87" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="C87" s="64" t="s">
         <v>262</v>
       </c>
-      <c r="C87" s="64" t="s">
-        <v>263</v>
-      </c>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="136"/>
-      <c r="G87" s="136"/>
-      <c r="H87" s="136"/>
-      <c r="I87" s="136"/>
-      <c r="J87" s="136"/>
-      <c r="K87" s="136"/>
-      <c r="L87" s="136"/>
-      <c r="M87" s="136"/>
-      <c r="N87" s="136"/>
-      <c r="O87" s="136"/>
-      <c r="P87" s="136"/>
-      <c r="Q87" s="136"/>
-      <c r="R87" s="136"/>
-      <c r="S87" s="136"/>
-      <c r="T87" s="136"/>
-      <c r="U87" s="136"/>
-      <c r="V87" s="136"/>
-      <c r="W87" s="136"/>
-      <c r="X87" s="136"/>
-      <c r="Y87" s="136"/>
-      <c r="Z87" s="136"/>
-      <c r="AA87" s="136"/>
+      <c r="D87" s="53">
+        <v>0</v>
+      </c>
+      <c r="E87" s="53">
+        <v>1</v>
+      </c>
+      <c r="F87" s="128" t="s">
+        <v>282</v>
+      </c>
+      <c r="G87" s="128"/>
+      <c r="H87" s="128"/>
+      <c r="I87" s="128"/>
+      <c r="J87" s="128"/>
+      <c r="K87" s="128"/>
+      <c r="L87" s="128"/>
+      <c r="M87" s="128"/>
+      <c r="N87" s="128"/>
+      <c r="O87" s="128"/>
+      <c r="P87" s="128"/>
+      <c r="Q87" s="128" t="s">
+        <v>281</v>
+      </c>
+      <c r="R87" s="128"/>
+      <c r="S87" s="128"/>
+      <c r="T87" s="128"/>
+      <c r="U87" s="128"/>
+      <c r="V87" s="128"/>
+      <c r="W87" s="128"/>
+      <c r="X87" s="128"/>
+      <c r="Y87" s="128"/>
+      <c r="Z87" s="128"/>
+      <c r="AA87" s="128"/>
       <c r="AB87" s="64" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B88" s="147" t="s">
+        <v>283</v>
+      </c>
+    </row>
     <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="90" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="34"/>
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="144" t="s">
+      <c r="C90" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="144"/>
-      <c r="E90" s="144"/>
-      <c r="F90" s="144"/>
-      <c r="G90" s="144"/>
-      <c r="H90" s="144" t="s">
+      <c r="D90" s="130"/>
+      <c r="E90" s="130"/>
+      <c r="F90" s="130"/>
+      <c r="G90" s="130"/>
+      <c r="H90" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="144"/>
-      <c r="J90" s="144"/>
-      <c r="K90" s="144"/>
-      <c r="L90" s="144"/>
-      <c r="M90" s="132" t="s">
+      <c r="I90" s="130"/>
+      <c r="J90" s="130"/>
+      <c r="K90" s="130"/>
+      <c r="L90" s="130"/>
+      <c r="M90" s="136" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="132"/>
+      <c r="N90" s="136"/>
       <c r="O90" s="106"/>
       <c r="T90" s="57" t="s">
         <v>197</v>
@@ -8215,24 +8242,24 @@
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="126" t="s">
+      <c r="C91" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="126"/>
-      <c r="E91" s="126"/>
-      <c r="F91" s="126"/>
-      <c r="G91" s="126"/>
-      <c r="H91" s="126" t="s">
+      <c r="D91" s="127"/>
+      <c r="E91" s="127"/>
+      <c r="F91" s="127"/>
+      <c r="G91" s="127"/>
+      <c r="H91" s="127" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="126"/>
-      <c r="J91" s="126"/>
-      <c r="K91" s="126"/>
-      <c r="L91" s="126"/>
-      <c r="M91" s="127" t="s">
+      <c r="I91" s="127"/>
+      <c r="J91" s="127"/>
+      <c r="K91" s="127"/>
+      <c r="L91" s="127"/>
+      <c r="M91" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="127"/>
+      <c r="N91" s="126"/>
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8242,24 +8269,24 @@
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="126" t="s">
+      <c r="C92" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="126"/>
-      <c r="E92" s="126"/>
-      <c r="F92" s="126"/>
-      <c r="G92" s="126"/>
-      <c r="H92" s="126" t="s">
+      <c r="D92" s="127"/>
+      <c r="E92" s="127"/>
+      <c r="F92" s="127"/>
+      <c r="G92" s="127"/>
+      <c r="H92" s="127" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="126"/>
-      <c r="J92" s="126"/>
-      <c r="K92" s="126"/>
-      <c r="L92" s="126"/>
-      <c r="M92" s="127" t="s">
+      <c r="I92" s="127"/>
+      <c r="J92" s="127"/>
+      <c r="K92" s="127"/>
+      <c r="L92" s="127"/>
+      <c r="M92" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="127"/>
+      <c r="N92" s="126"/>
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8269,24 +8296,24 @@
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="126" t="s">
+      <c r="C93" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="126"/>
-      <c r="E93" s="126"/>
-      <c r="F93" s="126"/>
-      <c r="G93" s="126"/>
-      <c r="H93" s="126" t="s">
+      <c r="D93" s="127"/>
+      <c r="E93" s="127"/>
+      <c r="F93" s="127"/>
+      <c r="G93" s="127"/>
+      <c r="H93" s="127" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="126"/>
-      <c r="J93" s="126"/>
-      <c r="K93" s="126"/>
-      <c r="L93" s="126"/>
-      <c r="M93" s="127" t="s">
+      <c r="I93" s="127"/>
+      <c r="J93" s="127"/>
+      <c r="K93" s="127"/>
+      <c r="L93" s="127"/>
+      <c r="M93" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="127"/>
+      <c r="N93" s="126"/>
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8296,24 +8323,24 @@
       <c r="B94" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C94" s="126" t="s">
+      <c r="C94" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="126"/>
-      <c r="E94" s="126"/>
-      <c r="F94" s="126"/>
-      <c r="G94" s="126"/>
-      <c r="H94" s="126" t="s">
+      <c r="D94" s="127"/>
+      <c r="E94" s="127"/>
+      <c r="F94" s="127"/>
+      <c r="G94" s="127"/>
+      <c r="H94" s="127" t="s">
         <v>217</v>
       </c>
-      <c r="I94" s="126"/>
-      <c r="J94" s="126"/>
-      <c r="K94" s="126"/>
-      <c r="L94" s="126"/>
-      <c r="M94" s="127" t="s">
+      <c r="I94" s="127"/>
+      <c r="J94" s="127"/>
+      <c r="K94" s="127"/>
+      <c r="L94" s="127"/>
+      <c r="M94" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="127"/>
+      <c r="N94" s="126"/>
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8323,24 +8350,24 @@
       <c r="B95" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C95" s="126" t="s">
+      <c r="C95" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="126"/>
-      <c r="E95" s="126"/>
-      <c r="F95" s="126"/>
-      <c r="G95" s="126"/>
-      <c r="H95" s="126" t="s">
+      <c r="D95" s="127"/>
+      <c r="E95" s="127"/>
+      <c r="F95" s="127"/>
+      <c r="G95" s="127"/>
+      <c r="H95" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="I95" s="126"/>
-      <c r="J95" s="126"/>
-      <c r="K95" s="126"/>
-      <c r="L95" s="126"/>
-      <c r="M95" s="127" t="s">
+      <c r="I95" s="127"/>
+      <c r="J95" s="127"/>
+      <c r="K95" s="127"/>
+      <c r="L95" s="127"/>
+      <c r="M95" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="127"/>
+      <c r="N95" s="126"/>
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8350,24 +8377,24 @@
       <c r="B96" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="126" t="s">
+      <c r="C96" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="126"/>
-      <c r="E96" s="126"/>
-      <c r="F96" s="126"/>
-      <c r="G96" s="126"/>
-      <c r="H96" s="126" t="s">
+      <c r="D96" s="127"/>
+      <c r="E96" s="127"/>
+      <c r="F96" s="127"/>
+      <c r="G96" s="127"/>
+      <c r="H96" s="127" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="126"/>
-      <c r="J96" s="126"/>
-      <c r="K96" s="126"/>
-      <c r="L96" s="126"/>
-      <c r="M96" s="127" t="s">
+      <c r="I96" s="127"/>
+      <c r="J96" s="127"/>
+      <c r="K96" s="127"/>
+      <c r="L96" s="127"/>
+      <c r="M96" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="127"/>
+      <c r="N96" s="126"/>
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8377,24 +8404,24 @@
       <c r="B97" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="126" t="s">
+      <c r="C97" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="126"/>
-      <c r="E97" s="126"/>
-      <c r="F97" s="126"/>
-      <c r="G97" s="126"/>
-      <c r="H97" s="126" t="s">
+      <c r="D97" s="127"/>
+      <c r="E97" s="127"/>
+      <c r="F97" s="127"/>
+      <c r="G97" s="127"/>
+      <c r="H97" s="127" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="126"/>
-      <c r="J97" s="126"/>
-      <c r="K97" s="126"/>
-      <c r="L97" s="126"/>
-      <c r="M97" s="127" t="s">
+      <c r="I97" s="127"/>
+      <c r="J97" s="127"/>
+      <c r="K97" s="127"/>
+      <c r="L97" s="127"/>
+      <c r="M97" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="127"/>
+      <c r="N97" s="126"/>
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8404,24 +8431,24 @@
       <c r="B98" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C98" s="126" t="s">
+      <c r="C98" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="126"/>
-      <c r="E98" s="126"/>
-      <c r="F98" s="126"/>
-      <c r="G98" s="126"/>
-      <c r="H98" s="126" t="s">
+      <c r="D98" s="127"/>
+      <c r="E98" s="127"/>
+      <c r="F98" s="127"/>
+      <c r="G98" s="127"/>
+      <c r="H98" s="127" t="s">
         <v>221</v>
       </c>
-      <c r="I98" s="126"/>
-      <c r="J98" s="126"/>
-      <c r="K98" s="126"/>
-      <c r="L98" s="126"/>
-      <c r="M98" s="127" t="s">
+      <c r="I98" s="127"/>
+      <c r="J98" s="127"/>
+      <c r="K98" s="127"/>
+      <c r="L98" s="127"/>
+      <c r="M98" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="127"/>
+      <c r="N98" s="126"/>
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8431,24 +8458,24 @@
       <c r="B99" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="126" t="s">
+      <c r="C99" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="126"/>
-      <c r="E99" s="126"/>
-      <c r="F99" s="126"/>
-      <c r="G99" s="126"/>
-      <c r="H99" s="126" t="s">
+      <c r="D99" s="127"/>
+      <c r="E99" s="127"/>
+      <c r="F99" s="127"/>
+      <c r="G99" s="127"/>
+      <c r="H99" s="127" t="s">
         <v>222</v>
       </c>
-      <c r="I99" s="126"/>
-      <c r="J99" s="126"/>
-      <c r="K99" s="126"/>
-      <c r="L99" s="126"/>
-      <c r="M99" s="127" t="s">
+      <c r="I99" s="127"/>
+      <c r="J99" s="127"/>
+      <c r="K99" s="127"/>
+      <c r="L99" s="127"/>
+      <c r="M99" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="127"/>
+      <c r="N99" s="126"/>
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8458,325 +8485,325 @@
       <c r="B100" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="126" t="s">
+      <c r="C100" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D100" s="126"/>
-      <c r="E100" s="126"/>
-      <c r="F100" s="126"/>
-      <c r="G100" s="126"/>
-      <c r="H100" s="126" t="s">
+      <c r="D100" s="127"/>
+      <c r="E100" s="127"/>
+      <c r="F100" s="127"/>
+      <c r="G100" s="127"/>
+      <c r="H100" s="127" t="s">
         <v>223</v>
       </c>
-      <c r="I100" s="126"/>
-      <c r="J100" s="126"/>
-      <c r="K100" s="126"/>
-      <c r="L100" s="126"/>
-      <c r="M100" s="127" t="s">
+      <c r="I100" s="127"/>
+      <c r="J100" s="127"/>
+      <c r="K100" s="127"/>
+      <c r="L100" s="127"/>
+      <c r="M100" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="127"/>
+      <c r="N100" s="126"/>
       <c r="O100" s="64"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="126"/>
-      <c r="D101" s="126"/>
-      <c r="E101" s="126"/>
-      <c r="F101" s="126"/>
-      <c r="G101" s="126"/>
-      <c r="H101" s="126"/>
-      <c r="I101" s="126"/>
-      <c r="J101" s="126"/>
-      <c r="K101" s="126"/>
-      <c r="L101" s="126"/>
-      <c r="M101" s="127"/>
-      <c r="N101" s="127"/>
+      <c r="C101" s="127"/>
+      <c r="D101" s="127"/>
+      <c r="E101" s="127"/>
+      <c r="F101" s="127"/>
+      <c r="G101" s="127"/>
+      <c r="H101" s="127"/>
+      <c r="I101" s="127"/>
+      <c r="J101" s="127"/>
+      <c r="K101" s="127"/>
+      <c r="L101" s="127"/>
+      <c r="M101" s="126"/>
+      <c r="N101" s="126"/>
       <c r="O101" s="64"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="126"/>
-      <c r="I102" s="126"/>
-      <c r="J102" s="126"/>
-      <c r="K102" s="126"/>
-      <c r="L102" s="126"/>
-      <c r="M102" s="127"/>
-      <c r="N102" s="127"/>
+      <c r="H102" s="127"/>
+      <c r="I102" s="127"/>
+      <c r="J102" s="127"/>
+      <c r="K102" s="127"/>
+      <c r="L102" s="127"/>
+      <c r="M102" s="126"/>
+      <c r="N102" s="126"/>
       <c r="O102" s="64"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="126"/>
-      <c r="D103" s="126"/>
-      <c r="E103" s="126"/>
-      <c r="F103" s="126"/>
-      <c r="G103" s="126"/>
-      <c r="H103" s="126"/>
-      <c r="I103" s="126"/>
-      <c r="J103" s="126"/>
-      <c r="K103" s="126"/>
-      <c r="L103" s="126"/>
-      <c r="M103" s="127"/>
-      <c r="N103" s="127"/>
+      <c r="C103" s="127"/>
+      <c r="D103" s="127"/>
+      <c r="E103" s="127"/>
+      <c r="F103" s="127"/>
+      <c r="G103" s="127"/>
+      <c r="H103" s="127"/>
+      <c r="I103" s="127"/>
+      <c r="J103" s="127"/>
+      <c r="K103" s="127"/>
+      <c r="L103" s="127"/>
+      <c r="M103" s="126"/>
+      <c r="N103" s="126"/>
       <c r="O103" s="64"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="126"/>
-      <c r="D104" s="126"/>
-      <c r="E104" s="126"/>
-      <c r="F104" s="126"/>
-      <c r="G104" s="126"/>
-      <c r="H104" s="126"/>
-      <c r="I104" s="126"/>
-      <c r="J104" s="126"/>
-      <c r="K104" s="126"/>
-      <c r="L104" s="126"/>
-      <c r="M104" s="127"/>
-      <c r="N104" s="127"/>
+      <c r="C104" s="127"/>
+      <c r="D104" s="127"/>
+      <c r="E104" s="127"/>
+      <c r="F104" s="127"/>
+      <c r="G104" s="127"/>
+      <c r="H104" s="127"/>
+      <c r="I104" s="127"/>
+      <c r="J104" s="127"/>
+      <c r="K104" s="127"/>
+      <c r="L104" s="127"/>
+      <c r="M104" s="126"/>
+      <c r="N104" s="126"/>
       <c r="O104" s="64"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="126"/>
-      <c r="D105" s="126"/>
-      <c r="E105" s="126"/>
-      <c r="F105" s="126"/>
-      <c r="G105" s="126"/>
-      <c r="H105" s="126"/>
-      <c r="I105" s="126"/>
-      <c r="J105" s="126"/>
-      <c r="K105" s="126"/>
-      <c r="L105" s="126"/>
-      <c r="M105" s="127"/>
-      <c r="N105" s="127"/>
+      <c r="C105" s="127"/>
+      <c r="D105" s="127"/>
+      <c r="E105" s="127"/>
+      <c r="F105" s="127"/>
+      <c r="G105" s="127"/>
+      <c r="H105" s="127"/>
+      <c r="I105" s="127"/>
+      <c r="J105" s="127"/>
+      <c r="K105" s="127"/>
+      <c r="L105" s="127"/>
+      <c r="M105" s="126"/>
+      <c r="N105" s="126"/>
       <c r="O105" s="64"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="126"/>
-      <c r="D106" s="126"/>
-      <c r="E106" s="126"/>
-      <c r="F106" s="126"/>
-      <c r="G106" s="126"/>
-      <c r="H106" s="126"/>
-      <c r="I106" s="126"/>
-      <c r="J106" s="126"/>
-      <c r="K106" s="126"/>
-      <c r="L106" s="126"/>
-      <c r="M106" s="127"/>
-      <c r="N106" s="127"/>
+      <c r="C106" s="127"/>
+      <c r="D106" s="127"/>
+      <c r="E106" s="127"/>
+      <c r="F106" s="127"/>
+      <c r="G106" s="127"/>
+      <c r="H106" s="127"/>
+      <c r="I106" s="127"/>
+      <c r="J106" s="127"/>
+      <c r="K106" s="127"/>
+      <c r="L106" s="127"/>
+      <c r="M106" s="126"/>
+      <c r="N106" s="126"/>
       <c r="O106" s="64"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="37"/>
       <c r="B107" s="37"/>
-      <c r="C107" s="126"/>
-      <c r="D107" s="126"/>
-      <c r="E107" s="126"/>
-      <c r="F107" s="126"/>
-      <c r="G107" s="126"/>
-      <c r="H107" s="126"/>
-      <c r="I107" s="126"/>
-      <c r="J107" s="126"/>
-      <c r="K107" s="126"/>
-      <c r="L107" s="126"/>
-      <c r="M107" s="127"/>
-      <c r="N107" s="127"/>
+      <c r="C107" s="127"/>
+      <c r="D107" s="127"/>
+      <c r="E107" s="127"/>
+      <c r="F107" s="127"/>
+      <c r="G107" s="127"/>
+      <c r="H107" s="127"/>
+      <c r="I107" s="127"/>
+      <c r="J107" s="127"/>
+      <c r="K107" s="127"/>
+      <c r="L107" s="127"/>
+      <c r="M107" s="126"/>
+      <c r="N107" s="126"/>
       <c r="O107" s="64"/>
     </row>
     <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="37"/>
       <c r="B108" s="37"/>
-      <c r="C108" s="126"/>
-      <c r="D108" s="126"/>
-      <c r="E108" s="126"/>
-      <c r="F108" s="126"/>
-      <c r="G108" s="126"/>
-      <c r="H108" s="126"/>
-      <c r="I108" s="126"/>
-      <c r="J108" s="126"/>
-      <c r="K108" s="126"/>
-      <c r="L108" s="126"/>
-      <c r="M108" s="127"/>
-      <c r="N108" s="127"/>
+      <c r="C108" s="127"/>
+      <c r="D108" s="127"/>
+      <c r="E108" s="127"/>
+      <c r="F108" s="127"/>
+      <c r="G108" s="127"/>
+      <c r="H108" s="127"/>
+      <c r="I108" s="127"/>
+      <c r="J108" s="127"/>
+      <c r="K108" s="127"/>
+      <c r="L108" s="127"/>
+      <c r="M108" s="126"/>
+      <c r="N108" s="126"/>
       <c r="O108" s="64"/>
     </row>
     <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="37"/>
       <c r="B109" s="37"/>
-      <c r="C109" s="126"/>
-      <c r="D109" s="126"/>
-      <c r="E109" s="126"/>
-      <c r="F109" s="126"/>
-      <c r="G109" s="126"/>
-      <c r="H109" s="126"/>
-      <c r="I109" s="126"/>
-      <c r="J109" s="126"/>
-      <c r="K109" s="126"/>
-      <c r="L109" s="126"/>
-      <c r="M109" s="127"/>
-      <c r="N109" s="127"/>
+      <c r="C109" s="127"/>
+      <c r="D109" s="127"/>
+      <c r="E109" s="127"/>
+      <c r="F109" s="127"/>
+      <c r="G109" s="127"/>
+      <c r="H109" s="127"/>
+      <c r="I109" s="127"/>
+      <c r="J109" s="127"/>
+      <c r="K109" s="127"/>
+      <c r="L109" s="127"/>
+      <c r="M109" s="126"/>
+      <c r="N109" s="126"/>
       <c r="O109" s="64"/>
     </row>
     <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="37"/>
       <c r="B110" s="37"/>
-      <c r="C110" s="126"/>
-      <c r="D110" s="126"/>
-      <c r="E110" s="126"/>
-      <c r="F110" s="126"/>
-      <c r="G110" s="126"/>
-      <c r="H110" s="126"/>
-      <c r="I110" s="126"/>
-      <c r="J110" s="126"/>
-      <c r="K110" s="126"/>
-      <c r="L110" s="126"/>
-      <c r="M110" s="127"/>
-      <c r="N110" s="127"/>
+      <c r="C110" s="127"/>
+      <c r="D110" s="127"/>
+      <c r="E110" s="127"/>
+      <c r="F110" s="127"/>
+      <c r="G110" s="127"/>
+      <c r="H110" s="127"/>
+      <c r="I110" s="127"/>
+      <c r="J110" s="127"/>
+      <c r="K110" s="127"/>
+      <c r="L110" s="127"/>
+      <c r="M110" s="126"/>
+      <c r="N110" s="126"/>
       <c r="O110" s="64"/>
     </row>
     <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="37"/>
       <c r="B111" s="37"/>
-      <c r="C111" s="126"/>
-      <c r="D111" s="126"/>
-      <c r="E111" s="126"/>
-      <c r="F111" s="126"/>
-      <c r="G111" s="126"/>
-      <c r="H111" s="126"/>
-      <c r="I111" s="126"/>
-      <c r="J111" s="126"/>
-      <c r="K111" s="126"/>
-      <c r="L111" s="126"/>
-      <c r="M111" s="127"/>
-      <c r="N111" s="127"/>
+      <c r="C111" s="127"/>
+      <c r="D111" s="127"/>
+      <c r="E111" s="127"/>
+      <c r="F111" s="127"/>
+      <c r="G111" s="127"/>
+      <c r="H111" s="127"/>
+      <c r="I111" s="127"/>
+      <c r="J111" s="127"/>
+      <c r="K111" s="127"/>
+      <c r="L111" s="127"/>
+      <c r="M111" s="126"/>
+      <c r="N111" s="126"/>
       <c r="O111" s="64"/>
     </row>
     <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="37"/>
       <c r="B112" s="37"/>
-      <c r="C112" s="126"/>
-      <c r="D112" s="126"/>
-      <c r="E112" s="126"/>
-      <c r="F112" s="126"/>
-      <c r="G112" s="126"/>
-      <c r="H112" s="126"/>
-      <c r="I112" s="126"/>
-      <c r="J112" s="126"/>
-      <c r="K112" s="126"/>
-      <c r="L112" s="126"/>
-      <c r="M112" s="127"/>
-      <c r="N112" s="127"/>
+      <c r="C112" s="127"/>
+      <c r="D112" s="127"/>
+      <c r="E112" s="127"/>
+      <c r="F112" s="127"/>
+      <c r="G112" s="127"/>
+      <c r="H112" s="127"/>
+      <c r="I112" s="127"/>
+      <c r="J112" s="127"/>
+      <c r="K112" s="127"/>
+      <c r="L112" s="127"/>
+      <c r="M112" s="126"/>
+      <c r="N112" s="126"/>
       <c r="O112" s="64"/>
     </row>
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="37"/>
       <c r="B113" s="37"/>
-      <c r="C113" s="126"/>
-      <c r="D113" s="126"/>
-      <c r="E113" s="126"/>
-      <c r="F113" s="126"/>
-      <c r="G113" s="126"/>
-      <c r="H113" s="126"/>
-      <c r="I113" s="126"/>
-      <c r="J113" s="126"/>
-      <c r="K113" s="126"/>
-      <c r="L113" s="126"/>
-      <c r="M113" s="127"/>
-      <c r="N113" s="127"/>
+      <c r="C113" s="127"/>
+      <c r="D113" s="127"/>
+      <c r="E113" s="127"/>
+      <c r="F113" s="127"/>
+      <c r="G113" s="127"/>
+      <c r="H113" s="127"/>
+      <c r="I113" s="127"/>
+      <c r="J113" s="127"/>
+      <c r="K113" s="127"/>
+      <c r="L113" s="127"/>
+      <c r="M113" s="126"/>
+      <c r="N113" s="126"/>
       <c r="O113" s="64"/>
     </row>
     <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="37"/>
       <c r="B114" s="37"/>
-      <c r="C114" s="126"/>
-      <c r="D114" s="126"/>
-      <c r="E114" s="126"/>
-      <c r="F114" s="126"/>
-      <c r="G114" s="126"/>
-      <c r="H114" s="126"/>
-      <c r="I114" s="126"/>
-      <c r="J114" s="126"/>
-      <c r="K114" s="126"/>
-      <c r="L114" s="126"/>
-      <c r="M114" s="127"/>
-      <c r="N114" s="127"/>
+      <c r="C114" s="127"/>
+      <c r="D114" s="127"/>
+      <c r="E114" s="127"/>
+      <c r="F114" s="127"/>
+      <c r="G114" s="127"/>
+      <c r="H114" s="127"/>
+      <c r="I114" s="127"/>
+      <c r="J114" s="127"/>
+      <c r="K114" s="127"/>
+      <c r="L114" s="127"/>
+      <c r="M114" s="126"/>
+      <c r="N114" s="126"/>
       <c r="O114" s="64"/>
     </row>
     <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="37"/>
       <c r="B115" s="37"/>
-      <c r="C115" s="126"/>
-      <c r="D115" s="126"/>
-      <c r="E115" s="126"/>
-      <c r="F115" s="126"/>
-      <c r="G115" s="126"/>
-      <c r="H115" s="126"/>
-      <c r="I115" s="126"/>
-      <c r="J115" s="126"/>
-      <c r="K115" s="126"/>
-      <c r="L115" s="126"/>
-      <c r="M115" s="127"/>
-      <c r="N115" s="127"/>
+      <c r="C115" s="127"/>
+      <c r="D115" s="127"/>
+      <c r="E115" s="127"/>
+      <c r="F115" s="127"/>
+      <c r="G115" s="127"/>
+      <c r="H115" s="127"/>
+      <c r="I115" s="127"/>
+      <c r="J115" s="127"/>
+      <c r="K115" s="127"/>
+      <c r="L115" s="127"/>
+      <c r="M115" s="126"/>
+      <c r="N115" s="126"/>
       <c r="O115" s="64"/>
     </row>
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="37"/>
       <c r="B116" s="37"/>
-      <c r="C116" s="126"/>
-      <c r="D116" s="126"/>
-      <c r="E116" s="126"/>
-      <c r="F116" s="126"/>
-      <c r="G116" s="126"/>
-      <c r="H116" s="126"/>
-      <c r="I116" s="126"/>
-      <c r="J116" s="126"/>
-      <c r="K116" s="126"/>
-      <c r="L116" s="126"/>
-      <c r="M116" s="127"/>
-      <c r="N116" s="127"/>
+      <c r="C116" s="127"/>
+      <c r="D116" s="127"/>
+      <c r="E116" s="127"/>
+      <c r="F116" s="127"/>
+      <c r="G116" s="127"/>
+      <c r="H116" s="127"/>
+      <c r="I116" s="127"/>
+      <c r="J116" s="127"/>
+      <c r="K116" s="127"/>
+      <c r="L116" s="127"/>
+      <c r="M116" s="126"/>
+      <c r="N116" s="126"/>
       <c r="O116" s="64"/>
     </row>
     <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="37"/>
       <c r="B117" s="37"/>
-      <c r="C117" s="126"/>
-      <c r="D117" s="126"/>
-      <c r="E117" s="126"/>
-      <c r="F117" s="126"/>
-      <c r="G117" s="126"/>
-      <c r="H117" s="126"/>
-      <c r="I117" s="126"/>
-      <c r="J117" s="126"/>
-      <c r="K117" s="126"/>
-      <c r="L117" s="126"/>
-      <c r="M117" s="127"/>
-      <c r="N117" s="127"/>
+      <c r="C117" s="127"/>
+      <c r="D117" s="127"/>
+      <c r="E117" s="127"/>
+      <c r="F117" s="127"/>
+      <c r="G117" s="127"/>
+      <c r="H117" s="127"/>
+      <c r="I117" s="127"/>
+      <c r="J117" s="127"/>
+      <c r="K117" s="127"/>
+      <c r="L117" s="127"/>
+      <c r="M117" s="126"/>
+      <c r="N117" s="126"/>
       <c r="O117" s="64"/>
     </row>
     <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="37"/>
       <c r="B118" s="37"/>
-      <c r="C118" s="126"/>
-      <c r="D118" s="126"/>
-      <c r="E118" s="126"/>
-      <c r="F118" s="126"/>
-      <c r="G118" s="126"/>
-      <c r="H118" s="126"/>
-      <c r="I118" s="126"/>
-      <c r="J118" s="126"/>
-      <c r="K118" s="126"/>
-      <c r="L118" s="126"/>
-      <c r="M118" s="127"/>
-      <c r="N118" s="127"/>
+      <c r="C118" s="127"/>
+      <c r="D118" s="127"/>
+      <c r="E118" s="127"/>
+      <c r="F118" s="127"/>
+      <c r="G118" s="127"/>
+      <c r="H118" s="127"/>
+      <c r="I118" s="127"/>
+      <c r="J118" s="127"/>
+      <c r="K118" s="127"/>
+      <c r="L118" s="127"/>
+      <c r="M118" s="126"/>
+      <c r="N118" s="126"/>
       <c r="O118" s="64"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.6">
@@ -8966,7 +8993,7 @@
         <v>245</v>
       </c>
       <c r="G131" s="117" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H131" s="115" t="s">
         <v>255</v>
@@ -9107,34 +9134,123 @@
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="174">
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:H49"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="M90:N90"/>
     <mergeCell ref="F83:P83"/>
@@ -9159,128 +9275,39 @@
     <mergeCell ref="F65:G65"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="J77:M77"/>
     <mergeCell ref="F81:P81"/>
     <mergeCell ref="F82:P82"/>
     <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="H107:L107"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:L108"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="H109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:L110"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H111:L111"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="H112:L112"/>
-    <mergeCell ref="M112:N112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H113:L113"/>
-    <mergeCell ref="M113:N113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="H114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="H118:L118"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="H115:L115"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="H116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="H117:L117"/>
-    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added blood particle effect!
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4E8E86-6233-4619-B9CC-EA4A21D59934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED3B68D-0382-4611-9A5A-49E26597807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2632,67 +2632,67 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3945,8 +3945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3964,10 +3964,10 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="140" t="s">
+      <c r="C1" s="137" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="140"/>
+      <c r="D1" s="137"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4063,10 +4063,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="135" t="s">
+      <c r="Z2" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="135"/>
+      <c r="AA2" s="140"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="19">
-        <v>1400</v>
+        <v>1300</v>
       </c>
       <c r="H10" s="19">
         <v>42</v>
@@ -4636,11 +4636,11 @@
       <c r="L10" s="19"/>
       <c r="M10" s="19">
         <f>ROUND(E10*F10/G10*1000,2)</f>
-        <v>4.29</v>
+        <v>4.62</v>
       </c>
       <c r="N10" s="19">
         <f>ROUND(E10*F10/(G10+J10/I10)*1000,2)</f>
-        <v>2.83</v>
+        <v>2.97</v>
       </c>
       <c r="O10" s="19">
         <f>E10*F10*I10</f>
@@ -4707,7 +4707,7 @@
         <v>650</v>
       </c>
       <c r="H11" s="19">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I11" s="19">
         <v>14</v>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="R11" s="19">
         <f>ROUND(D11/H11,3)</f>
-        <v>3.1E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="S11" s="28" t="s">
         <v>29</v>
@@ -4877,7 +4877,7 @@
         <v>2000</v>
       </c>
       <c r="H13" s="19">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="19">
         <v>7</v>
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="G17" s="19">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H17" s="19">
         <v>23</v>
       </c>
       <c r="I17" s="19">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="J17" s="19">
-        <v>7400</v>
+        <v>7200</v>
       </c>
       <c r="K17" s="19">
         <v>5</v>
@@ -5180,15 +5180,15 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19">
         <f t="shared" si="14"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="N17" s="19">
         <f>ROUND(E17*F17/(G17+J17/I17)*1000,2)</f>
-        <v>7.73</v>
+        <v>5.81</v>
       </c>
       <c r="O17" s="19">
         <f t="shared" si="15"/>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P17" s="32">
         <f t="shared" si="16"/>
@@ -6559,20 +6559,20 @@
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="137" t="s">
+      <c r="C40" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="137"/>
-      <c r="E40" s="137"/>
-      <c r="F40" s="137"/>
-      <c r="G40" s="137"/>
-      <c r="H40" s="137"/>
-      <c r="I40" s="137" t="s">
+      <c r="D40" s="136"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="136"/>
+      <c r="G40" s="136"/>
+      <c r="H40" s="136"/>
+      <c r="I40" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="137"/>
-      <c r="K40" s="137"/>
-      <c r="L40" s="137"/>
+      <c r="J40" s="136"/>
+      <c r="K40" s="136"/>
+      <c r="L40" s="136"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -6580,10 +6580,10 @@
       <c r="Q40" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="S40" s="136" t="s">
+      <c r="S40" s="141" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="136"/>
+      <c r="T40" s="141"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6593,22 +6593,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="138" t="s">
+      <c r="C41" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="138"/>
-      <c r="E41" s="138"/>
-      <c r="F41" s="138" t="s">
+      <c r="D41" s="144"/>
+      <c r="E41" s="144"/>
+      <c r="F41" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="138"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138" t="s">
+      <c r="G41" s="144"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="138"/>
-      <c r="K41" s="138"/>
-      <c r="L41" s="138"/>
+      <c r="J41" s="144"/>
+      <c r="K41" s="144"/>
+      <c r="L41" s="144"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6616,10 +6616,10 @@
       <c r="Q41" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S41" s="136" t="s">
+      <c r="S41" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="136"/>
+      <c r="T41" s="141"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6632,22 +6632,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="138" t="s">
+      <c r="C42" s="144" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="138"/>
-      <c r="E42" s="138"/>
-      <c r="F42" s="138" t="s">
+      <c r="D42" s="144"/>
+      <c r="E42" s="144"/>
+      <c r="F42" s="144" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="138"/>
-      <c r="H42" s="138"/>
-      <c r="I42" s="138" t="s">
+      <c r="G42" s="144"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="138"/>
-      <c r="K42" s="138"/>
-      <c r="L42" s="138"/>
+      <c r="J42" s="144"/>
+      <c r="K42" s="144"/>
+      <c r="L42" s="144"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6655,10 +6655,10 @@
       <c r="Q42" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S42" s="136" t="s">
+      <c r="S42" s="141" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="136"/>
+      <c r="T42" s="141"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6671,22 +6671,22 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="139" t="s">
+      <c r="C43" s="130" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="139"/>
-      <c r="E43" s="139"/>
-      <c r="F43" s="139" t="s">
+      <c r="D43" s="130"/>
+      <c r="E43" s="130"/>
+      <c r="F43" s="130" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="139"/>
-      <c r="H43" s="139"/>
-      <c r="I43" s="139" t="s">
+      <c r="G43" s="130"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="139"/>
-      <c r="K43" s="139"/>
-      <c r="L43" s="139"/>
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -6694,10 +6694,10 @@
       <c r="Q43" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="S43" s="136" t="s">
+      <c r="S43" s="141" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="136"/>
+      <c r="T43" s="141"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6712,20 +6712,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="139" t="s">
+      <c r="C44" s="130" t="s">
         <v>268</v>
       </c>
-      <c r="D44" s="139"/>
-      <c r="E44" s="139"/>
-      <c r="F44" s="139"/>
-      <c r="G44" s="139"/>
-      <c r="H44" s="139"/>
-      <c r="I44" s="139" t="s">
+      <c r="D44" s="130"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="130"/>
+      <c r="G44" s="130"/>
+      <c r="H44" s="130"/>
+      <c r="I44" s="130" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="139"/>
-      <c r="K44" s="139"/>
-      <c r="L44" s="139"/>
+      <c r="J44" s="130"/>
+      <c r="K44" s="130"/>
+      <c r="L44" s="130"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -6808,12 +6808,12 @@
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="139"/>
-      <c r="E49" s="139"/>
-      <c r="F49" s="139"/>
-      <c r="G49" s="139"/>
-      <c r="H49" s="139"/>
+      <c r="C49" s="130"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="130"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
@@ -6824,18 +6824,18 @@
       <c r="B51" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="C51" s="137" t="s">
+      <c r="C51" s="136" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="137"/>
-      <c r="E51" s="137" t="s">
+      <c r="D51" s="136"/>
+      <c r="E51" s="136" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="137"/>
-      <c r="G51" s="137"/>
-      <c r="H51" s="137"/>
-      <c r="I51" s="137"/>
-      <c r="J51" s="137"/>
+      <c r="F51" s="136"/>
+      <c r="G51" s="136"/>
+      <c r="H51" s="136"/>
+      <c r="I51" s="136"/>
+      <c r="J51" s="136"/>
       <c r="K51" s="120" t="s">
         <v>259</v>
       </c>
@@ -6847,18 +6847,18 @@
       <c r="B52" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="C52" s="128" t="s">
+      <c r="C52" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="D52" s="128"/>
-      <c r="E52" s="131" t="s">
+      <c r="D52" s="134"/>
+      <c r="E52" s="135" t="s">
         <v>269</v>
       </c>
-      <c r="F52" s="131"/>
-      <c r="G52" s="131"/>
-      <c r="H52" s="131"/>
-      <c r="I52" s="131"/>
-      <c r="J52" s="131"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
+      <c r="H52" s="135"/>
+      <c r="I52" s="135"/>
+      <c r="J52" s="135"/>
       <c r="K52" s="64" t="s">
         <v>261</v>
       </c>
@@ -6870,18 +6870,18 @@
       <c r="B53" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="C53" s="128" t="s">
+      <c r="C53" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="D53" s="128"/>
-      <c r="E53" s="131" t="s">
+      <c r="D53" s="134"/>
+      <c r="E53" s="135" t="s">
         <v>270</v>
       </c>
-      <c r="F53" s="131"/>
-      <c r="G53" s="131"/>
-      <c r="H53" s="131"/>
-      <c r="I53" s="131"/>
-      <c r="J53" s="131"/>
+      <c r="F53" s="135"/>
+      <c r="G53" s="135"/>
+      <c r="H53" s="135"/>
+      <c r="I53" s="135"/>
+      <c r="J53" s="135"/>
       <c r="K53" s="64" t="s">
         <v>261</v>
       </c>
@@ -6893,18 +6893,18 @@
       <c r="B54" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C54" s="128" t="s">
+      <c r="C54" s="134" t="s">
         <v>273</v>
       </c>
-      <c r="D54" s="128"/>
-      <c r="E54" s="131" t="s">
+      <c r="D54" s="134"/>
+      <c r="E54" s="135" t="s">
         <v>271</v>
       </c>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="131"/>
-      <c r="I54" s="131"/>
-      <c r="J54" s="131"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="135"/>
+      <c r="J54" s="135"/>
       <c r="K54" s="64" t="s">
         <v>261</v>
       </c>
@@ -6921,14 +6921,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="146" t="s">
+      <c r="H56" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="146"/>
-      <c r="J56" s="146"/>
-      <c r="K56" s="146"/>
-      <c r="L56" s="146"/>
-      <c r="M56" s="146"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="133"/>
+      <c r="L56" s="133"/>
+      <c r="M56" s="133"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
@@ -7132,10 +7132,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="142" t="s">
+      <c r="J62" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="142"/>
+      <c r="K62" s="139"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7143,13 +7143,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="141" t="s">
+      <c r="O62" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="141"/>
-      <c r="Q62" s="141"/>
-      <c r="R62" s="141"/>
-      <c r="S62" s="141"/>
+      <c r="P62" s="138"/>
+      <c r="Q62" s="138"/>
+      <c r="R62" s="138"/>
+      <c r="S62" s="138"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
@@ -7171,20 +7171,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="132" t="s">
+      <c r="F63" s="142" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="132"/>
+      <c r="G63" s="142"/>
       <c r="H63" s="85" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="132" t="s">
+      <c r="J63" s="142" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="132"/>
+      <c r="K63" s="142"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7208,10 +7208,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="132" t="s">
+      <c r="U63" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="132"/>
+      <c r="V63" s="142"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7239,21 +7239,21 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="145" t="s">
+      <c r="F64" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="145"/>
+      <c r="G64" s="143"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="128">
+      <c r="J64" s="134">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="128"/>
+      <c r="K64" s="134"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7284,11 +7284,11 @@
         <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="133">
+      <c r="U64" s="145">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="133"/>
+      <c r="V64" s="145"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7316,28 +7316,28 @@
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="127" t="s">
+      <c r="F65" s="128" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="127"/>
+      <c r="G65" s="128"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="128">
+      <c r="J65" s="134">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="128"/>
+      <c r="K65" s="134"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M65" s="53">
         <f t="shared" ref="M65:M68" si="37">21-L65</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N65" s="53"/>
       <c r="O65" s="65">
@@ -7346,7 +7346,7 @@
       </c>
       <c r="P65" s="66">
         <f t="shared" si="34"/>
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="Q65" s="67">
         <f t="shared" si="35"/>
@@ -7358,14 +7358,14 @@
       </c>
       <c r="S65" s="69">
         <f t="shared" ref="S65:S69" si="38">SUM(O65:R65)</f>
-        <v>14.8</v>
+        <v>14.5</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="134">
+      <c r="U65" s="146">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
-        <v>10.8</v>
-      </c>
-      <c r="V65" s="134"/>
+        <v>10.5</v>
+      </c>
+      <c r="V65" s="146"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7393,21 +7393,21 @@
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="127" t="s">
+      <c r="F66" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="127"/>
+      <c r="G66" s="128"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="128">
+      <c r="J66" s="134">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="128"/>
+      <c r="K66" s="134"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -7438,11 +7438,11 @@
         <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="134">
+      <c r="U66" s="146">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="134"/>
+      <c r="V66" s="146"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7470,21 +7470,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="127" t="s">
+      <c r="F67" s="128" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="127"/>
+      <c r="G67" s="128"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="128">
+      <c r="J67" s="134">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="128"/>
+      <c r="K67" s="134"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -7515,11 +7515,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="134">
+      <c r="U67" s="146">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="134"/>
+      <c r="V67" s="146"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7543,21 +7543,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="127" t="s">
+      <c r="F68" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="127"/>
+      <c r="G68" s="128"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="128">
+      <c r="J68" s="134">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="128"/>
+      <c r="K68" s="134"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7588,11 +7588,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="134">
+      <c r="U68" s="146">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="134"/>
+      <c r="V68" s="146"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7616,21 +7616,21 @@
       <c r="E69" s="53">
         <v>10</v>
       </c>
-      <c r="F69" s="127" t="s">
+      <c r="F69" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="127"/>
+      <c r="G69" s="128"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="128">
+      <c r="J69" s="134">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="128"/>
+      <c r="K69" s="134"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7661,11 +7661,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="134">
+      <c r="U69" s="146">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="134"/>
+      <c r="V69" s="146"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7689,21 +7689,21 @@
       <c r="E70" s="53">
         <v>8</v>
       </c>
-      <c r="F70" s="127" t="s">
+      <c r="F70" s="128" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="127"/>
+      <c r="G70" s="128"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="128">
+      <c r="J70" s="134">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="128"/>
+      <c r="K70" s="134"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7734,11 +7734,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="134">
+      <c r="U70" s="146">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="134"/>
+      <c r="V70" s="146"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7754,12 +7754,12 @@
       <c r="B73" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="O73" s="135" t="s">
+      <c r="O73" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="135"/>
-      <c r="Q73" s="135"/>
-      <c r="R73" s="135"/>
+      <c r="P73" s="140"/>
+      <c r="Q73" s="140"/>
+      <c r="R73" s="140"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7775,31 +7775,31 @@
       <c r="E74" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="129" t="s">
+      <c r="F74" s="131" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="129"/>
-      <c r="H74" s="129" t="s">
+      <c r="G74" s="131"/>
+      <c r="H74" s="131" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="129"/>
-      <c r="J74" s="129" t="s">
+      <c r="I74" s="131"/>
+      <c r="J74" s="131" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="129"/>
-      <c r="L74" s="129"/>
-      <c r="M74" s="129"/>
+      <c r="K74" s="131"/>
+      <c r="L74" s="131"/>
+      <c r="M74" s="131"/>
       <c r="N74" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="129" t="s">
+      <c r="O74" s="131" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="129"/>
-      <c r="Q74" s="129" t="s">
+      <c r="P74" s="131"/>
+      <c r="Q74" s="131" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="129"/>
+      <c r="R74" s="131"/>
       <c r="S74" s="120" t="s">
         <v>259</v>
       </c>
@@ -7820,21 +7820,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="128" t="s">
+      <c r="F75" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="128"/>
-      <c r="H75" s="128">
+      <c r="G75" s="134"/>
+      <c r="H75" s="134">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="128"/>
-      <c r="J75" s="128" t="s">
+      <c r="I75" s="134"/>
+      <c r="J75" s="134" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="128"/>
-      <c r="L75" s="128"/>
-      <c r="M75" s="128"/>
+      <c r="K75" s="134"/>
+      <c r="L75" s="134"/>
+      <c r="M75" s="134"/>
       <c r="N75" s="77" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7866,21 +7866,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="128" t="s">
+      <c r="F76" s="134" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="128"/>
-      <c r="H76" s="128">
+      <c r="G76" s="134"/>
+      <c r="H76" s="134">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="128"/>
-      <c r="J76" s="128" t="s">
+      <c r="I76" s="134"/>
+      <c r="J76" s="134" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="128"/>
-      <c r="L76" s="128"/>
-      <c r="M76" s="128"/>
+      <c r="K76" s="134"/>
+      <c r="L76" s="134"/>
+      <c r="M76" s="134"/>
       <c r="N76" s="77" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7902,19 +7902,19 @@
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="139"/>
-      <c r="G77" s="139"/>
-      <c r="H77" s="139"/>
-      <c r="I77" s="139"/>
-      <c r="J77" s="139"/>
-      <c r="K77" s="139"/>
-      <c r="L77" s="139"/>
-      <c r="M77" s="139"/>
+      <c r="F77" s="130"/>
+      <c r="G77" s="130"/>
+      <c r="H77" s="130"/>
+      <c r="I77" s="130"/>
+      <c r="J77" s="130"/>
+      <c r="K77" s="130"/>
+      <c r="L77" s="130"/>
+      <c r="M77" s="130"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="143"/>
-      <c r="P77" s="143"/>
-      <c r="Q77" s="143"/>
-      <c r="R77" s="143"/>
+      <c r="O77" s="126"/>
+      <c r="P77" s="126"/>
+      <c r="Q77" s="126"/>
+      <c r="R77" s="126"/>
       <c r="S77" s="64"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7943,32 +7943,32 @@
       <c r="E81" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="129" t="s">
+      <c r="F81" s="131" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="129"/>
-      <c r="H81" s="129"/>
-      <c r="I81" s="129"/>
-      <c r="J81" s="129"/>
-      <c r="K81" s="129"/>
-      <c r="L81" s="129"/>
-      <c r="M81" s="129"/>
-      <c r="N81" s="129"/>
-      <c r="O81" s="129"/>
-      <c r="P81" s="129"/>
-      <c r="Q81" s="129" t="s">
+      <c r="G81" s="131"/>
+      <c r="H81" s="131"/>
+      <c r="I81" s="131"/>
+      <c r="J81" s="131"/>
+      <c r="K81" s="131"/>
+      <c r="L81" s="131"/>
+      <c r="M81" s="131"/>
+      <c r="N81" s="131"/>
+      <c r="O81" s="131"/>
+      <c r="P81" s="131"/>
+      <c r="Q81" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="129"/>
-      <c r="S81" s="129"/>
-      <c r="T81" s="129"/>
-      <c r="U81" s="129"/>
-      <c r="V81" s="129"/>
-      <c r="W81" s="129"/>
-      <c r="X81" s="129"/>
-      <c r="Y81" s="129"/>
-      <c r="Z81" s="129"/>
-      <c r="AA81" s="129"/>
+      <c r="R81" s="131"/>
+      <c r="S81" s="131"/>
+      <c r="T81" s="131"/>
+      <c r="U81" s="131"/>
+      <c r="V81" s="131"/>
+      <c r="W81" s="131"/>
+      <c r="X81" s="131"/>
+      <c r="Y81" s="131"/>
+      <c r="Z81" s="131"/>
+      <c r="AA81" s="131"/>
       <c r="AB81" s="120" t="s">
         <v>259</v>
       </c>
@@ -7987,32 +7987,32 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="130" t="s">
+      <c r="F82" s="132" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="130"/>
-      <c r="H82" s="130"/>
-      <c r="I82" s="130"/>
-      <c r="J82" s="130"/>
-      <c r="K82" s="130"/>
-      <c r="L82" s="130"/>
-      <c r="M82" s="130"/>
-      <c r="N82" s="130"/>
-      <c r="O82" s="130"/>
-      <c r="P82" s="130"/>
-      <c r="Q82" s="130" t="s">
+      <c r="G82" s="132"/>
+      <c r="H82" s="132"/>
+      <c r="I82" s="132"/>
+      <c r="J82" s="132"/>
+      <c r="K82" s="132"/>
+      <c r="L82" s="132"/>
+      <c r="M82" s="132"/>
+      <c r="N82" s="132"/>
+      <c r="O82" s="132"/>
+      <c r="P82" s="132"/>
+      <c r="Q82" s="132" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="130"/>
-      <c r="S82" s="130"/>
-      <c r="T82" s="130"/>
-      <c r="U82" s="130"/>
-      <c r="V82" s="130"/>
-      <c r="W82" s="130"/>
-      <c r="X82" s="130"/>
-      <c r="Y82" s="130"/>
-      <c r="Z82" s="130"/>
-      <c r="AA82" s="130"/>
+      <c r="R82" s="132"/>
+      <c r="S82" s="132"/>
+      <c r="T82" s="132"/>
+      <c r="U82" s="132"/>
+      <c r="V82" s="132"/>
+      <c r="W82" s="132"/>
+      <c r="X82" s="132"/>
+      <c r="Y82" s="132"/>
+      <c r="Z82" s="132"/>
+      <c r="AA82" s="132"/>
       <c r="AB82" s="64" t="s">
         <v>260</v>
       </c>
@@ -8031,30 +8031,30 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="131" t="s">
+      <c r="F83" s="135" t="s">
         <v>225</v>
       </c>
-      <c r="G83" s="131"/>
-      <c r="H83" s="131"/>
-      <c r="I83" s="131"/>
-      <c r="J83" s="131"/>
-      <c r="K83" s="131"/>
-      <c r="L83" s="131"/>
-      <c r="M83" s="131"/>
-      <c r="N83" s="131"/>
-      <c r="O83" s="131"/>
-      <c r="P83" s="131"/>
-      <c r="Q83" s="131"/>
-      <c r="R83" s="131"/>
-      <c r="S83" s="131"/>
-      <c r="T83" s="131"/>
-      <c r="U83" s="131"/>
-      <c r="V83" s="131"/>
-      <c r="W83" s="131"/>
-      <c r="X83" s="131"/>
-      <c r="Y83" s="131"/>
-      <c r="Z83" s="131"/>
-      <c r="AA83" s="131"/>
+      <c r="G83" s="135"/>
+      <c r="H83" s="135"/>
+      <c r="I83" s="135"/>
+      <c r="J83" s="135"/>
+      <c r="K83" s="135"/>
+      <c r="L83" s="135"/>
+      <c r="M83" s="135"/>
+      <c r="N83" s="135"/>
+      <c r="O83" s="135"/>
+      <c r="P83" s="135"/>
+      <c r="Q83" s="135"/>
+      <c r="R83" s="135"/>
+      <c r="S83" s="135"/>
+      <c r="T83" s="135"/>
+      <c r="U83" s="135"/>
+      <c r="V83" s="135"/>
+      <c r="W83" s="135"/>
+      <c r="X83" s="135"/>
+      <c r="Y83" s="135"/>
+      <c r="Z83" s="135"/>
+      <c r="AA83" s="135"/>
       <c r="AB83" s="64" t="s">
         <v>260</v>
       </c>
@@ -8073,30 +8073,30 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="131" t="s">
+      <c r="F84" s="135" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="131"/>
-      <c r="H84" s="131"/>
-      <c r="I84" s="131"/>
-      <c r="J84" s="131"/>
-      <c r="K84" s="131"/>
-      <c r="L84" s="131"/>
-      <c r="M84" s="131"/>
-      <c r="N84" s="131"/>
-      <c r="O84" s="131"/>
-      <c r="P84" s="131"/>
-      <c r="Q84" s="131"/>
-      <c r="R84" s="131"/>
-      <c r="S84" s="131"/>
-      <c r="T84" s="131"/>
-      <c r="U84" s="131"/>
-      <c r="V84" s="131"/>
-      <c r="W84" s="131"/>
-      <c r="X84" s="131"/>
-      <c r="Y84" s="131"/>
-      <c r="Z84" s="131"/>
-      <c r="AA84" s="131"/>
+      <c r="G84" s="135"/>
+      <c r="H84" s="135"/>
+      <c r="I84" s="135"/>
+      <c r="J84" s="135"/>
+      <c r="K84" s="135"/>
+      <c r="L84" s="135"/>
+      <c r="M84" s="135"/>
+      <c r="N84" s="135"/>
+      <c r="O84" s="135"/>
+      <c r="P84" s="135"/>
+      <c r="Q84" s="135"/>
+      <c r="R84" s="135"/>
+      <c r="S84" s="135"/>
+      <c r="T84" s="135"/>
+      <c r="U84" s="135"/>
+      <c r="V84" s="135"/>
+      <c r="W84" s="135"/>
+      <c r="X84" s="135"/>
+      <c r="Y84" s="135"/>
+      <c r="Z84" s="135"/>
+      <c r="AA84" s="135"/>
       <c r="AB84" s="64" t="s">
         <v>260</v>
       </c>
@@ -8115,32 +8115,32 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="131" t="s">
+      <c r="F85" s="135" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="131"/>
-      <c r="H85" s="131"/>
-      <c r="I85" s="131"/>
-      <c r="J85" s="131"/>
-      <c r="K85" s="131"/>
-      <c r="L85" s="131"/>
-      <c r="M85" s="131"/>
-      <c r="N85" s="131"/>
-      <c r="O85" s="131"/>
-      <c r="P85" s="131"/>
-      <c r="Q85" s="131" t="s">
+      <c r="G85" s="135"/>
+      <c r="H85" s="135"/>
+      <c r="I85" s="135"/>
+      <c r="J85" s="135"/>
+      <c r="K85" s="135"/>
+      <c r="L85" s="135"/>
+      <c r="M85" s="135"/>
+      <c r="N85" s="135"/>
+      <c r="O85" s="135"/>
+      <c r="P85" s="135"/>
+      <c r="Q85" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="131"/>
-      <c r="S85" s="131"/>
-      <c r="T85" s="131"/>
-      <c r="U85" s="131"/>
-      <c r="V85" s="131"/>
-      <c r="W85" s="131"/>
-      <c r="X85" s="131"/>
-      <c r="Y85" s="131"/>
-      <c r="Z85" s="131"/>
-      <c r="AA85" s="131"/>
+      <c r="R85" s="135"/>
+      <c r="S85" s="135"/>
+      <c r="T85" s="135"/>
+      <c r="U85" s="135"/>
+      <c r="V85" s="135"/>
+      <c r="W85" s="135"/>
+      <c r="X85" s="135"/>
+      <c r="Y85" s="135"/>
+      <c r="Z85" s="135"/>
+      <c r="AA85" s="135"/>
       <c r="AB85" s="64" t="s">
         <v>260</v>
       </c>
@@ -8159,32 +8159,32 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="131" t="s">
+      <c r="F86" s="135" t="s">
         <v>257</v>
       </c>
-      <c r="G86" s="131"/>
-      <c r="H86" s="131"/>
-      <c r="I86" s="131"/>
-      <c r="J86" s="131"/>
-      <c r="K86" s="131"/>
-      <c r="L86" s="131"/>
-      <c r="M86" s="131"/>
-      <c r="N86" s="131"/>
-      <c r="O86" s="131"/>
-      <c r="P86" s="131"/>
-      <c r="Q86" s="131" t="s">
+      <c r="G86" s="135"/>
+      <c r="H86" s="135"/>
+      <c r="I86" s="135"/>
+      <c r="J86" s="135"/>
+      <c r="K86" s="135"/>
+      <c r="L86" s="135"/>
+      <c r="M86" s="135"/>
+      <c r="N86" s="135"/>
+      <c r="O86" s="135"/>
+      <c r="P86" s="135"/>
+      <c r="Q86" s="135" t="s">
         <v>258</v>
       </c>
-      <c r="R86" s="131"/>
-      <c r="S86" s="131"/>
-      <c r="T86" s="131"/>
-      <c r="U86" s="131"/>
-      <c r="V86" s="131"/>
-      <c r="W86" s="131"/>
-      <c r="X86" s="131"/>
-      <c r="Y86" s="131"/>
-      <c r="Z86" s="131"/>
-      <c r="AA86" s="131"/>
+      <c r="R86" s="135"/>
+      <c r="S86" s="135"/>
+      <c r="T86" s="135"/>
+      <c r="U86" s="135"/>
+      <c r="V86" s="135"/>
+      <c r="W86" s="135"/>
+      <c r="X86" s="135"/>
+      <c r="Y86" s="135"/>
+      <c r="Z86" s="135"/>
+      <c r="AA86" s="135"/>
       <c r="AB86" s="64" t="s">
         <v>261</v>
       </c>
@@ -8203,32 +8203,32 @@
       <c r="E87" s="53">
         <v>1</v>
       </c>
-      <c r="F87" s="131" t="s">
+      <c r="F87" s="135" t="s">
         <v>282</v>
       </c>
-      <c r="G87" s="131"/>
-      <c r="H87" s="131"/>
-      <c r="I87" s="131"/>
-      <c r="J87" s="131"/>
-      <c r="K87" s="131"/>
-      <c r="L87" s="131"/>
-      <c r="M87" s="131"/>
-      <c r="N87" s="131"/>
-      <c r="O87" s="131"/>
-      <c r="P87" s="131"/>
-      <c r="Q87" s="131" t="s">
+      <c r="G87" s="135"/>
+      <c r="H87" s="135"/>
+      <c r="I87" s="135"/>
+      <c r="J87" s="135"/>
+      <c r="K87" s="135"/>
+      <c r="L87" s="135"/>
+      <c r="M87" s="135"/>
+      <c r="N87" s="135"/>
+      <c r="O87" s="135"/>
+      <c r="P87" s="135"/>
+      <c r="Q87" s="135" t="s">
         <v>281</v>
       </c>
-      <c r="R87" s="131"/>
-      <c r="S87" s="131"/>
-      <c r="T87" s="131"/>
-      <c r="U87" s="131"/>
-      <c r="V87" s="131"/>
-      <c r="W87" s="131"/>
-      <c r="X87" s="131"/>
-      <c r="Y87" s="131"/>
-      <c r="Z87" s="131"/>
-      <c r="AA87" s="131"/>
+      <c r="R87" s="135"/>
+      <c r="S87" s="135"/>
+      <c r="T87" s="135"/>
+      <c r="U87" s="135"/>
+      <c r="V87" s="135"/>
+      <c r="W87" s="135"/>
+      <c r="X87" s="135"/>
+      <c r="Y87" s="135"/>
+      <c r="Z87" s="135"/>
+      <c r="AA87" s="135"/>
       <c r="AB87" s="64" t="s">
         <v>261</v>
       </c>
@@ -8244,24 +8244,24 @@
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="144" t="s">
+      <c r="C90" s="129" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="144"/>
-      <c r="E90" s="144"/>
-      <c r="F90" s="144"/>
-      <c r="G90" s="144"/>
-      <c r="H90" s="144" t="s">
+      <c r="D90" s="129"/>
+      <c r="E90" s="129"/>
+      <c r="F90" s="129"/>
+      <c r="G90" s="129"/>
+      <c r="H90" s="129" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="144"/>
-      <c r="J90" s="144"/>
-      <c r="K90" s="144"/>
-      <c r="L90" s="144"/>
-      <c r="M90" s="129" t="s">
+      <c r="I90" s="129"/>
+      <c r="J90" s="129"/>
+      <c r="K90" s="129"/>
+      <c r="L90" s="129"/>
+      <c r="M90" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="129"/>
+      <c r="N90" s="131"/>
       <c r="O90" s="106"/>
       <c r="T90" s="57" t="s">
         <v>197</v>
@@ -8274,24 +8274,24 @@
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="126" t="s">
+      <c r="C91" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="126"/>
-      <c r="E91" s="126"/>
-      <c r="F91" s="126"/>
-      <c r="G91" s="126"/>
-      <c r="H91" s="126" t="s">
+      <c r="D91" s="127"/>
+      <c r="E91" s="127"/>
+      <c r="F91" s="127"/>
+      <c r="G91" s="127"/>
+      <c r="H91" s="127" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="126"/>
-      <c r="J91" s="126"/>
-      <c r="K91" s="126"/>
-      <c r="L91" s="126"/>
-      <c r="M91" s="127" t="s">
+      <c r="I91" s="127"/>
+      <c r="J91" s="127"/>
+      <c r="K91" s="127"/>
+      <c r="L91" s="127"/>
+      <c r="M91" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="127"/>
+      <c r="N91" s="128"/>
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8301,24 +8301,24 @@
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="126" t="s">
+      <c r="C92" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="126"/>
-      <c r="E92" s="126"/>
-      <c r="F92" s="126"/>
-      <c r="G92" s="126"/>
-      <c r="H92" s="126" t="s">
+      <c r="D92" s="127"/>
+      <c r="E92" s="127"/>
+      <c r="F92" s="127"/>
+      <c r="G92" s="127"/>
+      <c r="H92" s="127" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="126"/>
-      <c r="J92" s="126"/>
-      <c r="K92" s="126"/>
-      <c r="L92" s="126"/>
-      <c r="M92" s="127" t="s">
+      <c r="I92" s="127"/>
+      <c r="J92" s="127"/>
+      <c r="K92" s="127"/>
+      <c r="L92" s="127"/>
+      <c r="M92" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="127"/>
+      <c r="N92" s="128"/>
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8328,24 +8328,24 @@
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="126" t="s">
+      <c r="C93" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="126"/>
-      <c r="E93" s="126"/>
-      <c r="F93" s="126"/>
-      <c r="G93" s="126"/>
-      <c r="H93" s="126" t="s">
+      <c r="D93" s="127"/>
+      <c r="E93" s="127"/>
+      <c r="F93" s="127"/>
+      <c r="G93" s="127"/>
+      <c r="H93" s="127" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="126"/>
-      <c r="J93" s="126"/>
-      <c r="K93" s="126"/>
-      <c r="L93" s="126"/>
-      <c r="M93" s="127" t="s">
+      <c r="I93" s="127"/>
+      <c r="J93" s="127"/>
+      <c r="K93" s="127"/>
+      <c r="L93" s="127"/>
+      <c r="M93" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="127"/>
+      <c r="N93" s="128"/>
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8355,24 +8355,24 @@
       <c r="B94" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C94" s="126" t="s">
+      <c r="C94" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="126"/>
-      <c r="E94" s="126"/>
-      <c r="F94" s="126"/>
-      <c r="G94" s="126"/>
-      <c r="H94" s="126" t="s">
+      <c r="D94" s="127"/>
+      <c r="E94" s="127"/>
+      <c r="F94" s="127"/>
+      <c r="G94" s="127"/>
+      <c r="H94" s="127" t="s">
         <v>217</v>
       </c>
-      <c r="I94" s="126"/>
-      <c r="J94" s="126"/>
-      <c r="K94" s="126"/>
-      <c r="L94" s="126"/>
-      <c r="M94" s="127" t="s">
+      <c r="I94" s="127"/>
+      <c r="J94" s="127"/>
+      <c r="K94" s="127"/>
+      <c r="L94" s="127"/>
+      <c r="M94" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="127"/>
+      <c r="N94" s="128"/>
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8382,24 +8382,24 @@
       <c r="B95" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C95" s="126" t="s">
+      <c r="C95" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="126"/>
-      <c r="E95" s="126"/>
-      <c r="F95" s="126"/>
-      <c r="G95" s="126"/>
-      <c r="H95" s="126" t="s">
+      <c r="D95" s="127"/>
+      <c r="E95" s="127"/>
+      <c r="F95" s="127"/>
+      <c r="G95" s="127"/>
+      <c r="H95" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="I95" s="126"/>
-      <c r="J95" s="126"/>
-      <c r="K95" s="126"/>
-      <c r="L95" s="126"/>
-      <c r="M95" s="127" t="s">
+      <c r="I95" s="127"/>
+      <c r="J95" s="127"/>
+      <c r="K95" s="127"/>
+      <c r="L95" s="127"/>
+      <c r="M95" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="127"/>
+      <c r="N95" s="128"/>
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8409,24 +8409,24 @@
       <c r="B96" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="126" t="s">
+      <c r="C96" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="126"/>
-      <c r="E96" s="126"/>
-      <c r="F96" s="126"/>
-      <c r="G96" s="126"/>
-      <c r="H96" s="126" t="s">
+      <c r="D96" s="127"/>
+      <c r="E96" s="127"/>
+      <c r="F96" s="127"/>
+      <c r="G96" s="127"/>
+      <c r="H96" s="127" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="126"/>
-      <c r="J96" s="126"/>
-      <c r="K96" s="126"/>
-      <c r="L96" s="126"/>
-      <c r="M96" s="127" t="s">
+      <c r="I96" s="127"/>
+      <c r="J96" s="127"/>
+      <c r="K96" s="127"/>
+      <c r="L96" s="127"/>
+      <c r="M96" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="127"/>
+      <c r="N96" s="128"/>
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8436,24 +8436,24 @@
       <c r="B97" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="126" t="s">
+      <c r="C97" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="126"/>
-      <c r="E97" s="126"/>
-      <c r="F97" s="126"/>
-      <c r="G97" s="126"/>
-      <c r="H97" s="126" t="s">
+      <c r="D97" s="127"/>
+      <c r="E97" s="127"/>
+      <c r="F97" s="127"/>
+      <c r="G97" s="127"/>
+      <c r="H97" s="127" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="126"/>
-      <c r="J97" s="126"/>
-      <c r="K97" s="126"/>
-      <c r="L97" s="126"/>
-      <c r="M97" s="127" t="s">
+      <c r="I97" s="127"/>
+      <c r="J97" s="127"/>
+      <c r="K97" s="127"/>
+      <c r="L97" s="127"/>
+      <c r="M97" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="127"/>
+      <c r="N97" s="128"/>
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8463,24 +8463,24 @@
       <c r="B98" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C98" s="126" t="s">
+      <c r="C98" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="126"/>
-      <c r="E98" s="126"/>
-      <c r="F98" s="126"/>
-      <c r="G98" s="126"/>
-      <c r="H98" s="126" t="s">
+      <c r="D98" s="127"/>
+      <c r="E98" s="127"/>
+      <c r="F98" s="127"/>
+      <c r="G98" s="127"/>
+      <c r="H98" s="127" t="s">
         <v>221</v>
       </c>
-      <c r="I98" s="126"/>
-      <c r="J98" s="126"/>
-      <c r="K98" s="126"/>
-      <c r="L98" s="126"/>
-      <c r="M98" s="127" t="s">
+      <c r="I98" s="127"/>
+      <c r="J98" s="127"/>
+      <c r="K98" s="127"/>
+      <c r="L98" s="127"/>
+      <c r="M98" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="127"/>
+      <c r="N98" s="128"/>
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8490,24 +8490,24 @@
       <c r="B99" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="126" t="s">
+      <c r="C99" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="126"/>
-      <c r="E99" s="126"/>
-      <c r="F99" s="126"/>
-      <c r="G99" s="126"/>
-      <c r="H99" s="126" t="s">
+      <c r="D99" s="127"/>
+      <c r="E99" s="127"/>
+      <c r="F99" s="127"/>
+      <c r="G99" s="127"/>
+      <c r="H99" s="127" t="s">
         <v>222</v>
       </c>
-      <c r="I99" s="126"/>
-      <c r="J99" s="126"/>
-      <c r="K99" s="126"/>
-      <c r="L99" s="126"/>
-      <c r="M99" s="127" t="s">
+      <c r="I99" s="127"/>
+      <c r="J99" s="127"/>
+      <c r="K99" s="127"/>
+      <c r="L99" s="127"/>
+      <c r="M99" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="127"/>
+      <c r="N99" s="128"/>
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8517,121 +8517,121 @@
       <c r="B100" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="126" t="s">
+      <c r="C100" s="127" t="s">
         <v>216</v>
       </c>
-      <c r="D100" s="126"/>
-      <c r="E100" s="126"/>
-      <c r="F100" s="126"/>
-      <c r="G100" s="126"/>
-      <c r="H100" s="126" t="s">
+      <c r="D100" s="127"/>
+      <c r="E100" s="127"/>
+      <c r="F100" s="127"/>
+      <c r="G100" s="127"/>
+      <c r="H100" s="127" t="s">
         <v>223</v>
       </c>
-      <c r="I100" s="126"/>
-      <c r="J100" s="126"/>
-      <c r="K100" s="126"/>
-      <c r="L100" s="126"/>
-      <c r="M100" s="127" t="s">
+      <c r="I100" s="127"/>
+      <c r="J100" s="127"/>
+      <c r="K100" s="127"/>
+      <c r="L100" s="127"/>
+      <c r="M100" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="127"/>
+      <c r="N100" s="128"/>
       <c r="O100" s="64"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="126"/>
-      <c r="D101" s="126"/>
-      <c r="E101" s="126"/>
-      <c r="F101" s="126"/>
-      <c r="G101" s="126"/>
-      <c r="H101" s="126"/>
-      <c r="I101" s="126"/>
-      <c r="J101" s="126"/>
-      <c r="K101" s="126"/>
-      <c r="L101" s="126"/>
-      <c r="M101" s="127"/>
-      <c r="N101" s="127"/>
+      <c r="C101" s="127"/>
+      <c r="D101" s="127"/>
+      <c r="E101" s="127"/>
+      <c r="F101" s="127"/>
+      <c r="G101" s="127"/>
+      <c r="H101" s="127"/>
+      <c r="I101" s="127"/>
+      <c r="J101" s="127"/>
+      <c r="K101" s="127"/>
+      <c r="L101" s="127"/>
+      <c r="M101" s="128"/>
+      <c r="N101" s="128"/>
       <c r="O101" s="64"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="126"/>
-      <c r="I102" s="126"/>
-      <c r="J102" s="126"/>
-      <c r="K102" s="126"/>
-      <c r="L102" s="126"/>
-      <c r="M102" s="127"/>
-      <c r="N102" s="127"/>
+      <c r="H102" s="127"/>
+      <c r="I102" s="127"/>
+      <c r="J102" s="127"/>
+      <c r="K102" s="127"/>
+      <c r="L102" s="127"/>
+      <c r="M102" s="128"/>
+      <c r="N102" s="128"/>
       <c r="O102" s="64"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="126"/>
-      <c r="D103" s="126"/>
-      <c r="E103" s="126"/>
-      <c r="F103" s="126"/>
-      <c r="G103" s="126"/>
-      <c r="H103" s="126"/>
-      <c r="I103" s="126"/>
-      <c r="J103" s="126"/>
-      <c r="K103" s="126"/>
-      <c r="L103" s="126"/>
-      <c r="M103" s="127"/>
-      <c r="N103" s="127"/>
+      <c r="C103" s="127"/>
+      <c r="D103" s="127"/>
+      <c r="E103" s="127"/>
+      <c r="F103" s="127"/>
+      <c r="G103" s="127"/>
+      <c r="H103" s="127"/>
+      <c r="I103" s="127"/>
+      <c r="J103" s="127"/>
+      <c r="K103" s="127"/>
+      <c r="L103" s="127"/>
+      <c r="M103" s="128"/>
+      <c r="N103" s="128"/>
       <c r="O103" s="64"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="126"/>
-      <c r="D104" s="126"/>
-      <c r="E104" s="126"/>
-      <c r="F104" s="126"/>
-      <c r="G104" s="126"/>
-      <c r="H104" s="126"/>
-      <c r="I104" s="126"/>
-      <c r="J104" s="126"/>
-      <c r="K104" s="126"/>
-      <c r="L104" s="126"/>
-      <c r="M104" s="127"/>
-      <c r="N104" s="127"/>
+      <c r="C104" s="127"/>
+      <c r="D104" s="127"/>
+      <c r="E104" s="127"/>
+      <c r="F104" s="127"/>
+      <c r="G104" s="127"/>
+      <c r="H104" s="127"/>
+      <c r="I104" s="127"/>
+      <c r="J104" s="127"/>
+      <c r="K104" s="127"/>
+      <c r="L104" s="127"/>
+      <c r="M104" s="128"/>
+      <c r="N104" s="128"/>
       <c r="O104" s="64"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="126"/>
-      <c r="D105" s="126"/>
-      <c r="E105" s="126"/>
-      <c r="F105" s="126"/>
-      <c r="G105" s="126"/>
-      <c r="H105" s="126"/>
-      <c r="I105" s="126"/>
-      <c r="J105" s="126"/>
-      <c r="K105" s="126"/>
-      <c r="L105" s="126"/>
-      <c r="M105" s="127"/>
-      <c r="N105" s="127"/>
+      <c r="C105" s="127"/>
+      <c r="D105" s="127"/>
+      <c r="E105" s="127"/>
+      <c r="F105" s="127"/>
+      <c r="G105" s="127"/>
+      <c r="H105" s="127"/>
+      <c r="I105" s="127"/>
+      <c r="J105" s="127"/>
+      <c r="K105" s="127"/>
+      <c r="L105" s="127"/>
+      <c r="M105" s="128"/>
+      <c r="N105" s="128"/>
       <c r="O105" s="64"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="126"/>
-      <c r="D106" s="126"/>
-      <c r="E106" s="126"/>
-      <c r="F106" s="126"/>
-      <c r="G106" s="126"/>
-      <c r="H106" s="126"/>
-      <c r="I106" s="126"/>
-      <c r="J106" s="126"/>
-      <c r="K106" s="126"/>
-      <c r="L106" s="126"/>
-      <c r="M106" s="127"/>
-      <c r="N106" s="127"/>
+      <c r="C106" s="127"/>
+      <c r="D106" s="127"/>
+      <c r="E106" s="127"/>
+      <c r="F106" s="127"/>
+      <c r="G106" s="127"/>
+      <c r="H106" s="127"/>
+      <c r="I106" s="127"/>
+      <c r="J106" s="127"/>
+      <c r="K106" s="127"/>
+      <c r="L106" s="127"/>
+      <c r="M106" s="128"/>
+      <c r="N106" s="128"/>
       <c r="O106" s="64"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -9229,33 +9229,87 @@
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:H49"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="M90:N90"/>
     <mergeCell ref="F83:P83"/>
@@ -9280,93 +9334,39 @@
     <mergeCell ref="F65:G65"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="F67:G67"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
     <mergeCell ref="Q81:AA81"/>
     <mergeCell ref="Q82:AA82"/>
     <mergeCell ref="Q85:AA85"/>
     <mergeCell ref="C91:G91"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
     <mergeCell ref="Q83:AA83"/>
     <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
balance patch s686 range increased
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED3B68D-0382-4611-9A5A-49E26597807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F05EB4-E181-4C9C-804B-DB5DC936862C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2632,68 +2632,68 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3945,8 +3945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3964,10 +3964,10 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="138" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="137"/>
+      <c r="D1" s="138"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4063,10 +4063,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="140" t="s">
+      <c r="Z2" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="140"/>
+      <c r="AA2" s="133"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="50">
-        <v>180</v>
+        <v>256</v>
       </c>
       <c r="D23" s="19">
         <v>4</v>
@@ -6559,20 +6559,20 @@
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="136" t="s">
+      <c r="C40" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="136"/>
-      <c r="E40" s="136"/>
-      <c r="F40" s="136"/>
-      <c r="G40" s="136"/>
-      <c r="H40" s="136"/>
-      <c r="I40" s="136" t="s">
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="135"/>
+      <c r="G40" s="135"/>
+      <c r="H40" s="135"/>
+      <c r="I40" s="135" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="136"/>
-      <c r="K40" s="136"/>
-      <c r="L40" s="136"/>
+      <c r="J40" s="135"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="135"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -6580,10 +6580,10 @@
       <c r="Q40" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="S40" s="141" t="s">
+      <c r="S40" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="141"/>
+      <c r="T40" s="134"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6593,22 +6593,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="144" t="s">
+      <c r="C41" s="136" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="144"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="144" t="s">
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144" t="s">
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+      <c r="I41" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="144"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="144"/>
+      <c r="J41" s="136"/>
+      <c r="K41" s="136"/>
+      <c r="L41" s="136"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6616,10 +6616,10 @@
       <c r="Q41" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S41" s="141" t="s">
+      <c r="S41" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="141"/>
+      <c r="T41" s="134"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6632,22 +6632,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="144" t="s">
+      <c r="C42" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144" t="s">
+      <c r="D42" s="136"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144" t="s">
+      <c r="G42" s="136"/>
+      <c r="H42" s="136"/>
+      <c r="I42" s="136" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="144"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="144"/>
+      <c r="J42" s="136"/>
+      <c r="K42" s="136"/>
+      <c r="L42" s="136"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6655,10 +6655,10 @@
       <c r="Q42" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S42" s="141" t="s">
+      <c r="S42" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="141"/>
+      <c r="T42" s="134"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6671,22 +6671,22 @@
       <c r="B43" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="137" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130" t="s">
+      <c r="D43" s="137"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130" t="s">
+      <c r="G43" s="137"/>
+      <c r="H43" s="137"/>
+      <c r="I43" s="137" t="s">
         <v>205</v>
       </c>
-      <c r="J43" s="130"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="130"/>
+      <c r="J43" s="137"/>
+      <c r="K43" s="137"/>
+      <c r="L43" s="137"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -6694,10 +6694,10 @@
       <c r="Q43" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="S43" s="141" t="s">
+      <c r="S43" s="134" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="141"/>
+      <c r="T43" s="134"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6712,20 +6712,20 @@
       <c r="B44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="130" t="s">
+      <c r="C44" s="137" t="s">
         <v>268</v>
       </c>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="130"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="130"/>
-      <c r="I44" s="130" t="s">
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="137" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="130"/>
-      <c r="K44" s="130"/>
-      <c r="L44" s="130"/>
+      <c r="J44" s="137"/>
+      <c r="K44" s="137"/>
+      <c r="L44" s="137"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -6808,12 +6808,12 @@
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="130"/>
-      <c r="D49" s="130"/>
-      <c r="E49" s="130"/>
-      <c r="F49" s="130"/>
-      <c r="G49" s="130"/>
-      <c r="H49" s="130"/>
+      <c r="C49" s="137"/>
+      <c r="D49" s="137"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="137"/>
+      <c r="G49" s="137"/>
+      <c r="H49" s="137"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
@@ -6824,18 +6824,18 @@
       <c r="B51" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="C51" s="136" t="s">
+      <c r="C51" s="135" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136" t="s">
+      <c r="D51" s="135"/>
+      <c r="E51" s="135" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="136"/>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
+      <c r="F51" s="135"/>
+      <c r="G51" s="135"/>
+      <c r="H51" s="135"/>
+      <c r="I51" s="135"/>
+      <c r="J51" s="135"/>
       <c r="K51" s="120" t="s">
         <v>259</v>
       </c>
@@ -6847,18 +6847,18 @@
       <c r="B52" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="C52" s="134" t="s">
+      <c r="C52" s="131" t="s">
         <v>274</v>
       </c>
-      <c r="D52" s="134"/>
-      <c r="E52" s="135" t="s">
+      <c r="D52" s="131"/>
+      <c r="E52" s="139" t="s">
         <v>269</v>
       </c>
-      <c r="F52" s="135"/>
-      <c r="G52" s="135"/>
-      <c r="H52" s="135"/>
-      <c r="I52" s="135"/>
-      <c r="J52" s="135"/>
+      <c r="F52" s="139"/>
+      <c r="G52" s="139"/>
+      <c r="H52" s="139"/>
+      <c r="I52" s="139"/>
+      <c r="J52" s="139"/>
       <c r="K52" s="64" t="s">
         <v>261</v>
       </c>
@@ -6870,18 +6870,18 @@
       <c r="B53" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="C53" s="134" t="s">
+      <c r="C53" s="131" t="s">
         <v>274</v>
       </c>
-      <c r="D53" s="134"/>
-      <c r="E53" s="135" t="s">
+      <c r="D53" s="131"/>
+      <c r="E53" s="139" t="s">
         <v>270</v>
       </c>
-      <c r="F53" s="135"/>
-      <c r="G53" s="135"/>
-      <c r="H53" s="135"/>
-      <c r="I53" s="135"/>
-      <c r="J53" s="135"/>
+      <c r="F53" s="139"/>
+      <c r="G53" s="139"/>
+      <c r="H53" s="139"/>
+      <c r="I53" s="139"/>
+      <c r="J53" s="139"/>
       <c r="K53" s="64" t="s">
         <v>261</v>
       </c>
@@ -6893,18 +6893,18 @@
       <c r="B54" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C54" s="134" t="s">
+      <c r="C54" s="131" t="s">
         <v>273</v>
       </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="135" t="s">
+      <c r="D54" s="131"/>
+      <c r="E54" s="139" t="s">
         <v>271</v>
       </c>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="135"/>
-      <c r="I54" s="135"/>
-      <c r="J54" s="135"/>
+      <c r="F54" s="139"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="139"/>
+      <c r="I54" s="139"/>
+      <c r="J54" s="139"/>
       <c r="K54" s="64" t="s">
         <v>261</v>
       </c>
@@ -6921,14 +6921,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="133" t="s">
+      <c r="H56" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="133"/>
-      <c r="J56" s="133"/>
-      <c r="K56" s="133"/>
-      <c r="L56" s="133"/>
-      <c r="M56" s="133"/>
+      <c r="I56" s="145"/>
+      <c r="J56" s="145"/>
+      <c r="K56" s="145"/>
+      <c r="L56" s="145"/>
+      <c r="M56" s="145"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
@@ -7132,10 +7132,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="139" t="s">
+      <c r="J62" s="141" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="139"/>
+      <c r="K62" s="141"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7143,13 +7143,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="138" t="s">
+      <c r="O62" s="140" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="138"/>
-      <c r="Q62" s="138"/>
-      <c r="R62" s="138"/>
-      <c r="S62" s="138"/>
+      <c r="P62" s="140"/>
+      <c r="Q62" s="140"/>
+      <c r="R62" s="140"/>
+      <c r="S62" s="140"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
@@ -7171,20 +7171,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="142" t="s">
+      <c r="F63" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="142"/>
+      <c r="G63" s="128"/>
       <c r="H63" s="85" t="s">
         <v>188</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="142" t="s">
+      <c r="J63" s="128" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="142"/>
+      <c r="K63" s="128"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7208,10 +7208,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="142" t="s">
+      <c r="U63" s="128" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="142"/>
+      <c r="V63" s="128"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7239,21 +7239,21 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="143" t="s">
+      <c r="F64" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="144"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="134">
+      <c r="J64" s="131">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="134"/>
+      <c r="K64" s="131"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7284,11 +7284,11 @@
         <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="145">
+      <c r="U64" s="129">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="145"/>
+      <c r="V64" s="129"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7316,21 +7316,21 @@
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="128" t="s">
+      <c r="F65" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="128"/>
+      <c r="G65" s="127"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="134">
+      <c r="J65" s="131">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="134"/>
+      <c r="K65" s="131"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>3</v>
@@ -7361,11 +7361,11 @@
         <v>14.5</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="146">
+      <c r="U65" s="130">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
         <v>10.5</v>
       </c>
-      <c r="V65" s="146"/>
+      <c r="V65" s="130"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7393,21 +7393,21 @@
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="128" t="s">
+      <c r="F66" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="128"/>
+      <c r="G66" s="127"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="134">
+      <c r="J66" s="131">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="134"/>
+      <c r="K66" s="131"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -7438,11 +7438,11 @@
         <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="146">
+      <c r="U66" s="130">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="146"/>
+      <c r="V66" s="130"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7470,21 +7470,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="128" t="s">
+      <c r="F67" s="127" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="128"/>
+      <c r="G67" s="127"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="134">
+      <c r="J67" s="131">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="134"/>
+      <c r="K67" s="131"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -7515,11 +7515,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="146">
+      <c r="U67" s="130">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="146"/>
+      <c r="V67" s="130"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7543,21 +7543,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="128" t="s">
+      <c r="F68" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="128"/>
+      <c r="G68" s="127"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="134">
+      <c r="J68" s="131">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="134"/>
+      <c r="K68" s="131"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -7588,11 +7588,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="146">
+      <c r="U68" s="130">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="146"/>
+      <c r="V68" s="130"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7616,21 +7616,21 @@
       <c r="E69" s="53">
         <v>10</v>
       </c>
-      <c r="F69" s="128" t="s">
+      <c r="F69" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="128"/>
+      <c r="G69" s="127"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="134">
+      <c r="J69" s="131">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="134"/>
+      <c r="K69" s="131"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -7661,11 +7661,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="146">
+      <c r="U69" s="130">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="146"/>
+      <c r="V69" s="130"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7689,21 +7689,21 @@
       <c r="E70" s="53">
         <v>8</v>
       </c>
-      <c r="F70" s="128" t="s">
+      <c r="F70" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="128"/>
+      <c r="G70" s="127"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="134">
+      <c r="J70" s="131">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="134"/>
+      <c r="K70" s="131"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -7734,11 +7734,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="146">
+      <c r="U70" s="130">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="146"/>
+      <c r="V70" s="130"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7754,12 +7754,12 @@
       <c r="B73" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="O73" s="140" t="s">
+      <c r="O73" s="133" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="140"/>
-      <c r="Q73" s="140"/>
-      <c r="R73" s="140"/>
+      <c r="P73" s="133"/>
+      <c r="Q73" s="133"/>
+      <c r="R73" s="133"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7775,31 +7775,31 @@
       <c r="E74" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="131" t="s">
+      <c r="F74" s="132" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="131"/>
-      <c r="H74" s="131" t="s">
+      <c r="G74" s="132"/>
+      <c r="H74" s="132" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="131"/>
-      <c r="J74" s="131" t="s">
+      <c r="I74" s="132"/>
+      <c r="J74" s="132" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="131"/>
-      <c r="L74" s="131"/>
-      <c r="M74" s="131"/>
+      <c r="K74" s="132"/>
+      <c r="L74" s="132"/>
+      <c r="M74" s="132"/>
       <c r="N74" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="131" t="s">
+      <c r="O74" s="132" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="131"/>
-      <c r="Q74" s="131" t="s">
+      <c r="P74" s="132"/>
+      <c r="Q74" s="132" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="131"/>
+      <c r="R74" s="132"/>
       <c r="S74" s="120" t="s">
         <v>259</v>
       </c>
@@ -7820,21 +7820,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="134" t="s">
+      <c r="F75" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="134"/>
-      <c r="H75" s="134">
+      <c r="G75" s="131"/>
+      <c r="H75" s="131">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="134"/>
-      <c r="J75" s="134" t="s">
+      <c r="I75" s="131"/>
+      <c r="J75" s="131" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="134"/>
-      <c r="L75" s="134"/>
-      <c r="M75" s="134"/>
+      <c r="K75" s="131"/>
+      <c r="L75" s="131"/>
+      <c r="M75" s="131"/>
       <c r="N75" s="77" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7866,21 +7866,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="134" t="s">
+      <c r="F76" s="131" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="134"/>
-      <c r="H76" s="134">
+      <c r="G76" s="131"/>
+      <c r="H76" s="131">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="134"/>
-      <c r="J76" s="134" t="s">
+      <c r="I76" s="131"/>
+      <c r="J76" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="134"/>
-      <c r="L76" s="134"/>
-      <c r="M76" s="134"/>
+      <c r="K76" s="131"/>
+      <c r="L76" s="131"/>
+      <c r="M76" s="131"/>
       <c r="N76" s="77" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -7902,19 +7902,19 @@
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="130"/>
-      <c r="G77" s="130"/>
-      <c r="H77" s="130"/>
-      <c r="I77" s="130"/>
-      <c r="J77" s="130"/>
-      <c r="K77" s="130"/>
-      <c r="L77" s="130"/>
-      <c r="M77" s="130"/>
+      <c r="F77" s="137"/>
+      <c r="G77" s="137"/>
+      <c r="H77" s="137"/>
+      <c r="I77" s="137"/>
+      <c r="J77" s="137"/>
+      <c r="K77" s="137"/>
+      <c r="L77" s="137"/>
+      <c r="M77" s="137"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="126"/>
-      <c r="P77" s="126"/>
-      <c r="Q77" s="126"/>
-      <c r="R77" s="126"/>
+      <c r="O77" s="142"/>
+      <c r="P77" s="142"/>
+      <c r="Q77" s="142"/>
+      <c r="R77" s="142"/>
       <c r="S77" s="64"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7943,32 +7943,32 @@
       <c r="E81" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="131" t="s">
+      <c r="F81" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="131"/>
-      <c r="H81" s="131"/>
-      <c r="I81" s="131"/>
-      <c r="J81" s="131"/>
-      <c r="K81" s="131"/>
-      <c r="L81" s="131"/>
-      <c r="M81" s="131"/>
-      <c r="N81" s="131"/>
-      <c r="O81" s="131"/>
-      <c r="P81" s="131"/>
-      <c r="Q81" s="131" t="s">
+      <c r="G81" s="132"/>
+      <c r="H81" s="132"/>
+      <c r="I81" s="132"/>
+      <c r="J81" s="132"/>
+      <c r="K81" s="132"/>
+      <c r="L81" s="132"/>
+      <c r="M81" s="132"/>
+      <c r="N81" s="132"/>
+      <c r="O81" s="132"/>
+      <c r="P81" s="132"/>
+      <c r="Q81" s="132" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="131"/>
-      <c r="S81" s="131"/>
-      <c r="T81" s="131"/>
-      <c r="U81" s="131"/>
-      <c r="V81" s="131"/>
-      <c r="W81" s="131"/>
-      <c r="X81" s="131"/>
-      <c r="Y81" s="131"/>
-      <c r="Z81" s="131"/>
-      <c r="AA81" s="131"/>
+      <c r="R81" s="132"/>
+      <c r="S81" s="132"/>
+      <c r="T81" s="132"/>
+      <c r="U81" s="132"/>
+      <c r="V81" s="132"/>
+      <c r="W81" s="132"/>
+      <c r="X81" s="132"/>
+      <c r="Y81" s="132"/>
+      <c r="Z81" s="132"/>
+      <c r="AA81" s="132"/>
       <c r="AB81" s="120" t="s">
         <v>259</v>
       </c>
@@ -7987,32 +7987,32 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="132" t="s">
+      <c r="F82" s="146" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="132"/>
-      <c r="H82" s="132"/>
-      <c r="I82" s="132"/>
-      <c r="J82" s="132"/>
-      <c r="K82" s="132"/>
-      <c r="L82" s="132"/>
-      <c r="M82" s="132"/>
-      <c r="N82" s="132"/>
-      <c r="O82" s="132"/>
-      <c r="P82" s="132"/>
-      <c r="Q82" s="132" t="s">
+      <c r="G82" s="146"/>
+      <c r="H82" s="146"/>
+      <c r="I82" s="146"/>
+      <c r="J82" s="146"/>
+      <c r="K82" s="146"/>
+      <c r="L82" s="146"/>
+      <c r="M82" s="146"/>
+      <c r="N82" s="146"/>
+      <c r="O82" s="146"/>
+      <c r="P82" s="146"/>
+      <c r="Q82" s="146" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="132"/>
-      <c r="S82" s="132"/>
-      <c r="T82" s="132"/>
-      <c r="U82" s="132"/>
-      <c r="V82" s="132"/>
-      <c r="W82" s="132"/>
-      <c r="X82" s="132"/>
-      <c r="Y82" s="132"/>
-      <c r="Z82" s="132"/>
-      <c r="AA82" s="132"/>
+      <c r="R82" s="146"/>
+      <c r="S82" s="146"/>
+      <c r="T82" s="146"/>
+      <c r="U82" s="146"/>
+      <c r="V82" s="146"/>
+      <c r="W82" s="146"/>
+      <c r="X82" s="146"/>
+      <c r="Y82" s="146"/>
+      <c r="Z82" s="146"/>
+      <c r="AA82" s="146"/>
       <c r="AB82" s="64" t="s">
         <v>260</v>
       </c>
@@ -8031,30 +8031,30 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="135" t="s">
+      <c r="F83" s="139" t="s">
         <v>225</v>
       </c>
-      <c r="G83" s="135"/>
-      <c r="H83" s="135"/>
-      <c r="I83" s="135"/>
-      <c r="J83" s="135"/>
-      <c r="K83" s="135"/>
-      <c r="L83" s="135"/>
-      <c r="M83" s="135"/>
-      <c r="N83" s="135"/>
-      <c r="O83" s="135"/>
-      <c r="P83" s="135"/>
-      <c r="Q83" s="135"/>
-      <c r="R83" s="135"/>
-      <c r="S83" s="135"/>
-      <c r="T83" s="135"/>
-      <c r="U83" s="135"/>
-      <c r="V83" s="135"/>
-      <c r="W83" s="135"/>
-      <c r="X83" s="135"/>
-      <c r="Y83" s="135"/>
-      <c r="Z83" s="135"/>
-      <c r="AA83" s="135"/>
+      <c r="G83" s="139"/>
+      <c r="H83" s="139"/>
+      <c r="I83" s="139"/>
+      <c r="J83" s="139"/>
+      <c r="K83" s="139"/>
+      <c r="L83" s="139"/>
+      <c r="M83" s="139"/>
+      <c r="N83" s="139"/>
+      <c r="O83" s="139"/>
+      <c r="P83" s="139"/>
+      <c r="Q83" s="139"/>
+      <c r="R83" s="139"/>
+      <c r="S83" s="139"/>
+      <c r="T83" s="139"/>
+      <c r="U83" s="139"/>
+      <c r="V83" s="139"/>
+      <c r="W83" s="139"/>
+      <c r="X83" s="139"/>
+      <c r="Y83" s="139"/>
+      <c r="Z83" s="139"/>
+      <c r="AA83" s="139"/>
       <c r="AB83" s="64" t="s">
         <v>260</v>
       </c>
@@ -8073,30 +8073,30 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="135" t="s">
+      <c r="F84" s="139" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="135"/>
-      <c r="H84" s="135"/>
-      <c r="I84" s="135"/>
-      <c r="J84" s="135"/>
-      <c r="K84" s="135"/>
-      <c r="L84" s="135"/>
-      <c r="M84" s="135"/>
-      <c r="N84" s="135"/>
-      <c r="O84" s="135"/>
-      <c r="P84" s="135"/>
-      <c r="Q84" s="135"/>
-      <c r="R84" s="135"/>
-      <c r="S84" s="135"/>
-      <c r="T84" s="135"/>
-      <c r="U84" s="135"/>
-      <c r="V84" s="135"/>
-      <c r="W84" s="135"/>
-      <c r="X84" s="135"/>
-      <c r="Y84" s="135"/>
-      <c r="Z84" s="135"/>
-      <c r="AA84" s="135"/>
+      <c r="G84" s="139"/>
+      <c r="H84" s="139"/>
+      <c r="I84" s="139"/>
+      <c r="J84" s="139"/>
+      <c r="K84" s="139"/>
+      <c r="L84" s="139"/>
+      <c r="M84" s="139"/>
+      <c r="N84" s="139"/>
+      <c r="O84" s="139"/>
+      <c r="P84" s="139"/>
+      <c r="Q84" s="139"/>
+      <c r="R84" s="139"/>
+      <c r="S84" s="139"/>
+      <c r="T84" s="139"/>
+      <c r="U84" s="139"/>
+      <c r="V84" s="139"/>
+      <c r="W84" s="139"/>
+      <c r="X84" s="139"/>
+      <c r="Y84" s="139"/>
+      <c r="Z84" s="139"/>
+      <c r="AA84" s="139"/>
       <c r="AB84" s="64" t="s">
         <v>260</v>
       </c>
@@ -8115,32 +8115,32 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="135" t="s">
+      <c r="F85" s="139" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="135"/>
-      <c r="H85" s="135"/>
-      <c r="I85" s="135"/>
-      <c r="J85" s="135"/>
-      <c r="K85" s="135"/>
-      <c r="L85" s="135"/>
-      <c r="M85" s="135"/>
-      <c r="N85" s="135"/>
-      <c r="O85" s="135"/>
-      <c r="P85" s="135"/>
-      <c r="Q85" s="135" t="s">
+      <c r="G85" s="139"/>
+      <c r="H85" s="139"/>
+      <c r="I85" s="139"/>
+      <c r="J85" s="139"/>
+      <c r="K85" s="139"/>
+      <c r="L85" s="139"/>
+      <c r="M85" s="139"/>
+      <c r="N85" s="139"/>
+      <c r="O85" s="139"/>
+      <c r="P85" s="139"/>
+      <c r="Q85" s="139" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="135"/>
-      <c r="S85" s="135"/>
-      <c r="T85" s="135"/>
-      <c r="U85" s="135"/>
-      <c r="V85" s="135"/>
-      <c r="W85" s="135"/>
-      <c r="X85" s="135"/>
-      <c r="Y85" s="135"/>
-      <c r="Z85" s="135"/>
-      <c r="AA85" s="135"/>
+      <c r="R85" s="139"/>
+      <c r="S85" s="139"/>
+      <c r="T85" s="139"/>
+      <c r="U85" s="139"/>
+      <c r="V85" s="139"/>
+      <c r="W85" s="139"/>
+      <c r="X85" s="139"/>
+      <c r="Y85" s="139"/>
+      <c r="Z85" s="139"/>
+      <c r="AA85" s="139"/>
       <c r="AB85" s="64" t="s">
         <v>260</v>
       </c>
@@ -8159,32 +8159,32 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="135" t="s">
+      <c r="F86" s="139" t="s">
         <v>257</v>
       </c>
-      <c r="G86" s="135"/>
-      <c r="H86" s="135"/>
-      <c r="I86" s="135"/>
-      <c r="J86" s="135"/>
-      <c r="K86" s="135"/>
-      <c r="L86" s="135"/>
-      <c r="M86" s="135"/>
-      <c r="N86" s="135"/>
-      <c r="O86" s="135"/>
-      <c r="P86" s="135"/>
-      <c r="Q86" s="135" t="s">
+      <c r="G86" s="139"/>
+      <c r="H86" s="139"/>
+      <c r="I86" s="139"/>
+      <c r="J86" s="139"/>
+      <c r="K86" s="139"/>
+      <c r="L86" s="139"/>
+      <c r="M86" s="139"/>
+      <c r="N86" s="139"/>
+      <c r="O86" s="139"/>
+      <c r="P86" s="139"/>
+      <c r="Q86" s="139" t="s">
         <v>258</v>
       </c>
-      <c r="R86" s="135"/>
-      <c r="S86" s="135"/>
-      <c r="T86" s="135"/>
-      <c r="U86" s="135"/>
-      <c r="V86" s="135"/>
-      <c r="W86" s="135"/>
-      <c r="X86" s="135"/>
-      <c r="Y86" s="135"/>
-      <c r="Z86" s="135"/>
-      <c r="AA86" s="135"/>
+      <c r="R86" s="139"/>
+      <c r="S86" s="139"/>
+      <c r="T86" s="139"/>
+      <c r="U86" s="139"/>
+      <c r="V86" s="139"/>
+      <c r="W86" s="139"/>
+      <c r="X86" s="139"/>
+      <c r="Y86" s="139"/>
+      <c r="Z86" s="139"/>
+      <c r="AA86" s="139"/>
       <c r="AB86" s="64" t="s">
         <v>261</v>
       </c>
@@ -8203,32 +8203,32 @@
       <c r="E87" s="53">
         <v>1</v>
       </c>
-      <c r="F87" s="135" t="s">
+      <c r="F87" s="139" t="s">
         <v>282</v>
       </c>
-      <c r="G87" s="135"/>
-      <c r="H87" s="135"/>
-      <c r="I87" s="135"/>
-      <c r="J87" s="135"/>
-      <c r="K87" s="135"/>
-      <c r="L87" s="135"/>
-      <c r="M87" s="135"/>
-      <c r="N87" s="135"/>
-      <c r="O87" s="135"/>
-      <c r="P87" s="135"/>
-      <c r="Q87" s="135" t="s">
+      <c r="G87" s="139"/>
+      <c r="H87" s="139"/>
+      <c r="I87" s="139"/>
+      <c r="J87" s="139"/>
+      <c r="K87" s="139"/>
+      <c r="L87" s="139"/>
+      <c r="M87" s="139"/>
+      <c r="N87" s="139"/>
+      <c r="O87" s="139"/>
+      <c r="P87" s="139"/>
+      <c r="Q87" s="139" t="s">
         <v>281</v>
       </c>
-      <c r="R87" s="135"/>
-      <c r="S87" s="135"/>
-      <c r="T87" s="135"/>
-      <c r="U87" s="135"/>
-      <c r="V87" s="135"/>
-      <c r="W87" s="135"/>
-      <c r="X87" s="135"/>
-      <c r="Y87" s="135"/>
-      <c r="Z87" s="135"/>
-      <c r="AA87" s="135"/>
+      <c r="R87" s="139"/>
+      <c r="S87" s="139"/>
+      <c r="T87" s="139"/>
+      <c r="U87" s="139"/>
+      <c r="V87" s="139"/>
+      <c r="W87" s="139"/>
+      <c r="X87" s="139"/>
+      <c r="Y87" s="139"/>
+      <c r="Z87" s="139"/>
+      <c r="AA87" s="139"/>
       <c r="AB87" s="64" t="s">
         <v>261</v>
       </c>
@@ -8244,24 +8244,24 @@
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="129" t="s">
+      <c r="C90" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="129"/>
-      <c r="E90" s="129"/>
-      <c r="F90" s="129"/>
-      <c r="G90" s="129"/>
-      <c r="H90" s="129" t="s">
+      <c r="D90" s="143"/>
+      <c r="E90" s="143"/>
+      <c r="F90" s="143"/>
+      <c r="G90" s="143"/>
+      <c r="H90" s="143" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="129"/>
-      <c r="J90" s="129"/>
-      <c r="K90" s="129"/>
-      <c r="L90" s="129"/>
-      <c r="M90" s="131" t="s">
+      <c r="I90" s="143"/>
+      <c r="J90" s="143"/>
+      <c r="K90" s="143"/>
+      <c r="L90" s="143"/>
+      <c r="M90" s="132" t="s">
         <v>186</v>
       </c>
-      <c r="N90" s="131"/>
+      <c r="N90" s="132"/>
       <c r="O90" s="106"/>
       <c r="T90" s="57" t="s">
         <v>197</v>
@@ -8274,24 +8274,24 @@
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="127" t="s">
+      <c r="C91" s="126" t="s">
         <v>181</v>
       </c>
-      <c r="D91" s="127"/>
-      <c r="E91" s="127"/>
-      <c r="F91" s="127"/>
-      <c r="G91" s="127"/>
-      <c r="H91" s="127" t="s">
+      <c r="D91" s="126"/>
+      <c r="E91" s="126"/>
+      <c r="F91" s="126"/>
+      <c r="G91" s="126"/>
+      <c r="H91" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="I91" s="127"/>
-      <c r="J91" s="127"/>
-      <c r="K91" s="127"/>
-      <c r="L91" s="127"/>
-      <c r="M91" s="128" t="s">
+      <c r="I91" s="126"/>
+      <c r="J91" s="126"/>
+      <c r="K91" s="126"/>
+      <c r="L91" s="126"/>
+      <c r="M91" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N91" s="128"/>
+      <c r="N91" s="127"/>
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8301,24 +8301,24 @@
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="127" t="s">
+      <c r="C92" s="126" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="127"/>
-      <c r="E92" s="127"/>
-      <c r="F92" s="127"/>
-      <c r="G92" s="127"/>
-      <c r="H92" s="127" t="s">
+      <c r="D92" s="126"/>
+      <c r="E92" s="126"/>
+      <c r="F92" s="126"/>
+      <c r="G92" s="126"/>
+      <c r="H92" s="126" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="127"/>
-      <c r="J92" s="127"/>
-      <c r="K92" s="127"/>
-      <c r="L92" s="127"/>
-      <c r="M92" s="128" t="s">
+      <c r="I92" s="126"/>
+      <c r="J92" s="126"/>
+      <c r="K92" s="126"/>
+      <c r="L92" s="126"/>
+      <c r="M92" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N92" s="128"/>
+      <c r="N92" s="127"/>
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8328,24 +8328,24 @@
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="127" t="s">
+      <c r="C93" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="127"/>
-      <c r="E93" s="127"/>
-      <c r="F93" s="127"/>
-      <c r="G93" s="127"/>
-      <c r="H93" s="127" t="s">
+      <c r="D93" s="126"/>
+      <c r="E93" s="126"/>
+      <c r="F93" s="126"/>
+      <c r="G93" s="126"/>
+      <c r="H93" s="126" t="s">
         <v>182</v>
       </c>
-      <c r="I93" s="127"/>
-      <c r="J93" s="127"/>
-      <c r="K93" s="127"/>
-      <c r="L93" s="127"/>
-      <c r="M93" s="128" t="s">
+      <c r="I93" s="126"/>
+      <c r="J93" s="126"/>
+      <c r="K93" s="126"/>
+      <c r="L93" s="126"/>
+      <c r="M93" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N93" s="128"/>
+      <c r="N93" s="127"/>
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8355,24 +8355,24 @@
       <c r="B94" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C94" s="127" t="s">
+      <c r="C94" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="127"/>
-      <c r="E94" s="127"/>
-      <c r="F94" s="127"/>
-      <c r="G94" s="127"/>
-      <c r="H94" s="127" t="s">
+      <c r="D94" s="126"/>
+      <c r="E94" s="126"/>
+      <c r="F94" s="126"/>
+      <c r="G94" s="126"/>
+      <c r="H94" s="126" t="s">
         <v>217</v>
       </c>
-      <c r="I94" s="127"/>
-      <c r="J94" s="127"/>
-      <c r="K94" s="127"/>
-      <c r="L94" s="127"/>
-      <c r="M94" s="128" t="s">
+      <c r="I94" s="126"/>
+      <c r="J94" s="126"/>
+      <c r="K94" s="126"/>
+      <c r="L94" s="126"/>
+      <c r="M94" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N94" s="128"/>
+      <c r="N94" s="127"/>
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8382,24 +8382,24 @@
       <c r="B95" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C95" s="127" t="s">
+      <c r="C95" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="127"/>
-      <c r="E95" s="127"/>
-      <c r="F95" s="127"/>
-      <c r="G95" s="127"/>
-      <c r="H95" s="127" t="s">
+      <c r="D95" s="126"/>
+      <c r="E95" s="126"/>
+      <c r="F95" s="126"/>
+      <c r="G95" s="126"/>
+      <c r="H95" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="I95" s="127"/>
-      <c r="J95" s="127"/>
-      <c r="K95" s="127"/>
-      <c r="L95" s="127"/>
-      <c r="M95" s="128" t="s">
+      <c r="I95" s="126"/>
+      <c r="J95" s="126"/>
+      <c r="K95" s="126"/>
+      <c r="L95" s="126"/>
+      <c r="M95" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N95" s="128"/>
+      <c r="N95" s="127"/>
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8409,24 +8409,24 @@
       <c r="B96" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="127" t="s">
+      <c r="C96" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="127"/>
-      <c r="E96" s="127"/>
-      <c r="F96" s="127"/>
-      <c r="G96" s="127"/>
-      <c r="H96" s="127" t="s">
+      <c r="D96" s="126"/>
+      <c r="E96" s="126"/>
+      <c r="F96" s="126"/>
+      <c r="G96" s="126"/>
+      <c r="H96" s="126" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="127"/>
-      <c r="J96" s="127"/>
-      <c r="K96" s="127"/>
-      <c r="L96" s="127"/>
-      <c r="M96" s="128" t="s">
+      <c r="I96" s="126"/>
+      <c r="J96" s="126"/>
+      <c r="K96" s="126"/>
+      <c r="L96" s="126"/>
+      <c r="M96" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N96" s="128"/>
+      <c r="N96" s="127"/>
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8436,24 +8436,24 @@
       <c r="B97" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="127" t="s">
+      <c r="C97" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="127"/>
-      <c r="E97" s="127"/>
-      <c r="F97" s="127"/>
-      <c r="G97" s="127"/>
-      <c r="H97" s="127" t="s">
+      <c r="D97" s="126"/>
+      <c r="E97" s="126"/>
+      <c r="F97" s="126"/>
+      <c r="G97" s="126"/>
+      <c r="H97" s="126" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="127"/>
-      <c r="J97" s="127"/>
-      <c r="K97" s="127"/>
-      <c r="L97" s="127"/>
-      <c r="M97" s="128" t="s">
+      <c r="I97" s="126"/>
+      <c r="J97" s="126"/>
+      <c r="K97" s="126"/>
+      <c r="L97" s="126"/>
+      <c r="M97" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N97" s="128"/>
+      <c r="N97" s="127"/>
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -8463,24 +8463,24 @@
       <c r="B98" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C98" s="127" t="s">
+      <c r="C98" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="127"/>
-      <c r="E98" s="127"/>
-      <c r="F98" s="127"/>
-      <c r="G98" s="127"/>
-      <c r="H98" s="127" t="s">
+      <c r="D98" s="126"/>
+      <c r="E98" s="126"/>
+      <c r="F98" s="126"/>
+      <c r="G98" s="126"/>
+      <c r="H98" s="126" t="s">
         <v>221</v>
       </c>
-      <c r="I98" s="127"/>
-      <c r="J98" s="127"/>
-      <c r="K98" s="127"/>
-      <c r="L98" s="127"/>
-      <c r="M98" s="128" t="s">
+      <c r="I98" s="126"/>
+      <c r="J98" s="126"/>
+      <c r="K98" s="126"/>
+      <c r="L98" s="126"/>
+      <c r="M98" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N98" s="128"/>
+      <c r="N98" s="127"/>
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8490,24 +8490,24 @@
       <c r="B99" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="127" t="s">
+      <c r="C99" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="127"/>
-      <c r="E99" s="127"/>
-      <c r="F99" s="127"/>
-      <c r="G99" s="127"/>
-      <c r="H99" s="127" t="s">
+      <c r="D99" s="126"/>
+      <c r="E99" s="126"/>
+      <c r="F99" s="126"/>
+      <c r="G99" s="126"/>
+      <c r="H99" s="126" t="s">
         <v>222</v>
       </c>
-      <c r="I99" s="127"/>
-      <c r="J99" s="127"/>
-      <c r="K99" s="127"/>
-      <c r="L99" s="127"/>
-      <c r="M99" s="128" t="s">
+      <c r="I99" s="126"/>
+      <c r="J99" s="126"/>
+      <c r="K99" s="126"/>
+      <c r="L99" s="126"/>
+      <c r="M99" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N99" s="128"/>
+      <c r="N99" s="127"/>
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -8517,121 +8517,121 @@
       <c r="B100" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C100" s="127" t="s">
+      <c r="C100" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="D100" s="127"/>
-      <c r="E100" s="127"/>
-      <c r="F100" s="127"/>
-      <c r="G100" s="127"/>
-      <c r="H100" s="127" t="s">
+      <c r="D100" s="126"/>
+      <c r="E100" s="126"/>
+      <c r="F100" s="126"/>
+      <c r="G100" s="126"/>
+      <c r="H100" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="I100" s="127"/>
-      <c r="J100" s="127"/>
-      <c r="K100" s="127"/>
-      <c r="L100" s="127"/>
-      <c r="M100" s="128" t="s">
+      <c r="I100" s="126"/>
+      <c r="J100" s="126"/>
+      <c r="K100" s="126"/>
+      <c r="L100" s="126"/>
+      <c r="M100" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="N100" s="128"/>
+      <c r="N100" s="127"/>
       <c r="O100" s="64"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="127"/>
-      <c r="D101" s="127"/>
-      <c r="E101" s="127"/>
-      <c r="F101" s="127"/>
-      <c r="G101" s="127"/>
-      <c r="H101" s="127"/>
-      <c r="I101" s="127"/>
-      <c r="J101" s="127"/>
-      <c r="K101" s="127"/>
-      <c r="L101" s="127"/>
-      <c r="M101" s="128"/>
-      <c r="N101" s="128"/>
+      <c r="C101" s="126"/>
+      <c r="D101" s="126"/>
+      <c r="E101" s="126"/>
+      <c r="F101" s="126"/>
+      <c r="G101" s="126"/>
+      <c r="H101" s="126"/>
+      <c r="I101" s="126"/>
+      <c r="J101" s="126"/>
+      <c r="K101" s="126"/>
+      <c r="L101" s="126"/>
+      <c r="M101" s="127"/>
+      <c r="N101" s="127"/>
       <c r="O101" s="64"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="127"/>
-      <c r="I102" s="127"/>
-      <c r="J102" s="127"/>
-      <c r="K102" s="127"/>
-      <c r="L102" s="127"/>
-      <c r="M102" s="128"/>
-      <c r="N102" s="128"/>
+      <c r="H102" s="126"/>
+      <c r="I102" s="126"/>
+      <c r="J102" s="126"/>
+      <c r="K102" s="126"/>
+      <c r="L102" s="126"/>
+      <c r="M102" s="127"/>
+      <c r="N102" s="127"/>
       <c r="O102" s="64"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="127"/>
-      <c r="D103" s="127"/>
-      <c r="E103" s="127"/>
-      <c r="F103" s="127"/>
-      <c r="G103" s="127"/>
-      <c r="H103" s="127"/>
-      <c r="I103" s="127"/>
-      <c r="J103" s="127"/>
-      <c r="K103" s="127"/>
-      <c r="L103" s="127"/>
-      <c r="M103" s="128"/>
-      <c r="N103" s="128"/>
+      <c r="C103" s="126"/>
+      <c r="D103" s="126"/>
+      <c r="E103" s="126"/>
+      <c r="F103" s="126"/>
+      <c r="G103" s="126"/>
+      <c r="H103" s="126"/>
+      <c r="I103" s="126"/>
+      <c r="J103" s="126"/>
+      <c r="K103" s="126"/>
+      <c r="L103" s="126"/>
+      <c r="M103" s="127"/>
+      <c r="N103" s="127"/>
       <c r="O103" s="64"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="127"/>
-      <c r="D104" s="127"/>
-      <c r="E104" s="127"/>
-      <c r="F104" s="127"/>
-      <c r="G104" s="127"/>
-      <c r="H104" s="127"/>
-      <c r="I104" s="127"/>
-      <c r="J104" s="127"/>
-      <c r="K104" s="127"/>
-      <c r="L104" s="127"/>
-      <c r="M104" s="128"/>
-      <c r="N104" s="128"/>
+      <c r="C104" s="126"/>
+      <c r="D104" s="126"/>
+      <c r="E104" s="126"/>
+      <c r="F104" s="126"/>
+      <c r="G104" s="126"/>
+      <c r="H104" s="126"/>
+      <c r="I104" s="126"/>
+      <c r="J104" s="126"/>
+      <c r="K104" s="126"/>
+      <c r="L104" s="126"/>
+      <c r="M104" s="127"/>
+      <c r="N104" s="127"/>
       <c r="O104" s="64"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="127"/>
-      <c r="D105" s="127"/>
-      <c r="E105" s="127"/>
-      <c r="F105" s="127"/>
-      <c r="G105" s="127"/>
-      <c r="H105" s="127"/>
-      <c r="I105" s="127"/>
-      <c r="J105" s="127"/>
-      <c r="K105" s="127"/>
-      <c r="L105" s="127"/>
-      <c r="M105" s="128"/>
-      <c r="N105" s="128"/>
+      <c r="C105" s="126"/>
+      <c r="D105" s="126"/>
+      <c r="E105" s="126"/>
+      <c r="F105" s="126"/>
+      <c r="G105" s="126"/>
+      <c r="H105" s="126"/>
+      <c r="I105" s="126"/>
+      <c r="J105" s="126"/>
+      <c r="K105" s="126"/>
+      <c r="L105" s="126"/>
+      <c r="M105" s="127"/>
+      <c r="N105" s="127"/>
       <c r="O105" s="64"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="127"/>
-      <c r="D106" s="127"/>
-      <c r="E106" s="127"/>
-      <c r="F106" s="127"/>
-      <c r="G106" s="127"/>
-      <c r="H106" s="127"/>
-      <c r="I106" s="127"/>
-      <c r="J106" s="127"/>
-      <c r="K106" s="127"/>
-      <c r="L106" s="127"/>
-      <c r="M106" s="128"/>
-      <c r="N106" s="128"/>
+      <c r="C106" s="126"/>
+      <c r="D106" s="126"/>
+      <c r="E106" s="126"/>
+      <c r="F106" s="126"/>
+      <c r="G106" s="126"/>
+      <c r="H106" s="126"/>
+      <c r="I106" s="126"/>
+      <c r="J106" s="126"/>
+      <c r="K106" s="126"/>
+      <c r="L106" s="126"/>
+      <c r="M106" s="127"/>
+      <c r="N106" s="127"/>
       <c r="O106" s="64"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -9229,63 +9229,63 @@
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="M102:N102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="H99:L99"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="S41:T41"/>
     <mergeCell ref="S43:T43"/>
@@ -9310,63 +9310,63 @@
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:H49"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
holding item now displayed properly
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C848F1-0797-465E-8EC6-5E53939095F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC05CA9-3B1E-4E72-AB87-09CBD5361996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="48">
+  <futureMetadata name="XLRICHVALUE" count="51">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -391,8 +391,29 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="48"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="49"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="50"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="48">
+  <valueMetadata count="51">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -536,13 +557,22 @@
     </bk>
     <bk>
       <rc t="1" v="47"/>
+    </bk>
+    <bk>
+      <rc t="1" v="48"/>
+    </bk>
+    <bk>
+      <rc t="1" v="49"/>
+    </bk>
+    <bk>
+      <rc t="1" v="50"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="290">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1629,27 +1659,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Explodes after some time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Summons smoke that last some seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If explodes on sight, cannot see anything for some seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Distance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 ~ 400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 ~ 320</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1715,7 +1725,27 @@
   </si>
   <si>
     <t>last update
-2024 4 20</t>
+2024 6 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 ~ 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 ~ 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summons smoke that last approximately 3000 ticks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If explodes on sight, cannot see anything for 100 ticks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explodes after speed &lt;= 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2672,6 +2702,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2700,9 +2733,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3431,7 +3461,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="48">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="51">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -3624,6 +3654,18 @@
     <v>47</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>48</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>49</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>50</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -3686,6 +3728,9 @@
   <rel r:id="rId46"/>
   <rel r:id="rId47"/>
   <rel r:id="rId48"/>
+  <rel r:id="rId49"/>
+  <rel r:id="rId50"/>
+  <rel r:id="rId51"/>
 </richValueRels>
 </file>
 
@@ -3954,8 +3999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -3973,14 +4018,14 @@
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="147" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1" s="137"/>
-      <c r="E1" s="147" t="s">
-        <v>289</v>
-      </c>
-      <c r="F1" s="137"/>
+      <c r="C1" s="137" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="138"/>
+      <c r="E1" s="137" t="s">
+        <v>284</v>
+      </c>
+      <c r="F1" s="138"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4076,10 +4121,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="140" t="s">
+      <c r="Z2" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="140"/>
+      <c r="AA2" s="141"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -6419,10 +6464,10 @@
         <v>201</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D36" s="73">
         <v>0</v>
@@ -6437,7 +6482,7 @@
         <v>800</v>
       </c>
       <c r="H36" s="64" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>51</v>
@@ -6482,7 +6527,7 @@
       </c>
       <c r="Y36" s="19"/>
       <c r="Z36" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AL36" s="35"/>
     </row>
@@ -6593,10 +6638,10 @@
       <c r="Q40" s="120" t="s">
         <v>258</v>
       </c>
-      <c r="S40" s="141" t="s">
+      <c r="S40" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="141"/>
+      <c r="T40" s="142"/>
       <c r="U40" s="56"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -6606,22 +6651,22 @@
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="144" t="s">
+      <c r="C41" s="145" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="144"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="144" t="s">
+      <c r="D41" s="145"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144" t="s">
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="144"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="144"/>
+      <c r="J41" s="145"/>
+      <c r="K41" s="145"/>
+      <c r="L41" s="145"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -6629,10 +6674,10 @@
       <c r="Q41" s="64" t="s">
         <v>259</v>
       </c>
-      <c r="S41" s="141" t="s">
+      <c r="S41" s="142" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="141"/>
+      <c r="T41" s="142"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
@@ -6645,22 +6690,22 @@
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="144" t="s">
+      <c r="C42" s="145" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144" t="s">
+      <c r="D42" s="145"/>
+      <c r="E42" s="145"/>
+      <c r="F42" s="145" t="s">
         <v>199</v>
       </c>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144" t="s">
+      <c r="G42" s="145"/>
+      <c r="H42" s="145"/>
+      <c r="I42" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="144"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="144"/>
+      <c r="J42" s="145"/>
+      <c r="K42" s="145"/>
+      <c r="L42" s="145"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -6668,10 +6713,10 @@
       <c r="Q42" s="64" t="s">
         <v>259</v>
       </c>
-      <c r="S42" s="141" t="s">
+      <c r="S42" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="141"/>
+      <c r="T42" s="142"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
@@ -6707,10 +6752,10 @@
       <c r="Q43" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S43" s="141" t="s">
+      <c r="S43" s="142" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="141"/>
+      <c r="T43" s="142"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -6838,7 +6883,7 @@
         <v>263</v>
       </c>
       <c r="C51" s="136" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D51" s="136"/>
       <c r="E51" s="136" t="s">
@@ -6854,18 +6899,18 @@
       </c>
     </row>
     <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A52" s="37" t="s">
-        <v>201</v>
+      <c r="A52" s="37" t="e" vm="28">
+        <v>#VALUE!</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>264</v>
       </c>
       <c r="C52" s="135" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="D52" s="135"/>
       <c r="E52" s="133" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
       <c r="F52" s="133"/>
       <c r="G52" s="133"/>
@@ -6873,22 +6918,22 @@
       <c r="I52" s="133"/>
       <c r="J52" s="133"/>
       <c r="K52" s="64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A53" s="37" t="s">
-        <v>201</v>
+      <c r="A53" s="37" t="e" vm="29">
+        <v>#VALUE!</v>
       </c>
       <c r="B53" s="37" t="s">
         <v>265</v>
       </c>
       <c r="C53" s="135" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="D53" s="135"/>
       <c r="E53" s="133" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="F53" s="133"/>
       <c r="G53" s="133"/>
@@ -6896,22 +6941,22 @@
       <c r="I53" s="133"/>
       <c r="J53" s="133"/>
       <c r="K53" s="64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A54" s="18" t="s">
-        <v>201</v>
+      <c r="A54" s="18" t="e" vm="30">
+        <v>#VALUE!</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>266</v>
       </c>
       <c r="C54" s="135" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="D54" s="135"/>
       <c r="E54" s="133" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="F54" s="133"/>
       <c r="G54" s="133"/>
@@ -6919,7 +6964,7 @@
       <c r="I54" s="133"/>
       <c r="J54" s="133"/>
       <c r="K54" s="64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7145,10 +7190,10 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="139" t="s">
+      <c r="J62" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="139"/>
+      <c r="K62" s="140"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7156,20 +7201,20 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="138" t="s">
+      <c r="O62" s="139" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="138"/>
-      <c r="Q62" s="138"/>
-      <c r="R62" s="138"/>
-      <c r="S62" s="138"/>
+      <c r="P62" s="139"/>
+      <c r="Q62" s="139"/>
+      <c r="R62" s="139"/>
+      <c r="S62" s="139"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
       <c r="AJ62" s="80"/>
     </row>
     <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="90" t="e" vm="28">
+      <c r="A63" s="90" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="84" t="s">
@@ -7184,20 +7229,20 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="142" t="s">
+      <c r="F63" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="142"/>
+      <c r="G63" s="143"/>
       <c r="H63" s="85" t="s">
         <v>187</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="142" t="s">
+      <c r="J63" s="143" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="142"/>
+      <c r="K63" s="143"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
@@ -7221,10 +7266,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="142" t="s">
+      <c r="U63" s="143" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="142"/>
+      <c r="V63" s="143"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7252,10 +7297,10 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="143" t="s">
+      <c r="F64" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="144"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
@@ -7297,11 +7342,11 @@
         <v>10.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="145">
+      <c r="U64" s="146">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="145"/>
+      <c r="V64" s="146"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7374,11 +7419,11 @@
         <v>14.5</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="146">
+      <c r="U65" s="147">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
         <v>10.5</v>
       </c>
-      <c r="V65" s="146"/>
+      <c r="V65" s="147"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7451,11 +7496,11 @@
         <v>13.899999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="146">
+      <c r="U66" s="147">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="146"/>
+      <c r="V66" s="147"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -7528,11 +7573,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="146">
+      <c r="U67" s="147">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="146"/>
+      <c r="V67" s="147"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -7601,11 +7646,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="146">
+      <c r="U68" s="147">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="146"/>
+      <c r="V68" s="147"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7674,11 +7719,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="146">
+      <c r="U69" s="147">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="146"/>
+      <c r="V69" s="147"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -7747,11 +7792,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="146">
+      <c r="U70" s="147">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="146"/>
+      <c r="V70" s="147"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -7767,12 +7812,12 @@
       <c r="B73" s="116" t="s">
         <v>238</v>
       </c>
-      <c r="O73" s="140" t="s">
+      <c r="O73" s="141" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="140"/>
-      <c r="Q73" s="140"/>
-      <c r="R73" s="140"/>
+      <c r="P73" s="141"/>
+      <c r="Q73" s="141"/>
+      <c r="R73" s="141"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -7818,7 +7863,7 @@
       </c>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A75" s="37" t="e" vm="29">
+      <c r="A75" s="37" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
       <c r="B75" s="37" t="s">
@@ -7848,13 +7893,13 @@
       <c r="K75" s="135"/>
       <c r="L75" s="135"/>
       <c r="M75" s="135"/>
-      <c r="N75" s="77" t="e" vm="30">
+      <c r="N75" s="77" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
-      <c r="O75" s="69" t="e" vm="31">
+      <c r="O75" s="69" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
-      <c r="P75" s="69" t="e" vm="32">
+      <c r="P75" s="69" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
       <c r="Q75" s="78"/>
@@ -7864,7 +7909,7 @@
       </c>
     </row>
     <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A76" s="37" t="e" vm="33">
+      <c r="A76" s="37" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="37" t="s">
@@ -7894,13 +7939,13 @@
       <c r="K76" s="135"/>
       <c r="L76" s="135"/>
       <c r="M76" s="135"/>
-      <c r="N76" s="77" t="e" vm="34">
+      <c r="N76" s="77" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
-      <c r="O76" s="69" t="e" vm="35">
+      <c r="O76" s="69" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
-      <c r="P76" s="69" t="e" vm="36">
+      <c r="P76" s="69" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
       <c r="Q76" s="78"/>
@@ -7941,7 +7986,7 @@
     <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="81" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A81" s="34" t="e" vm="37">
+      <c r="A81" s="34" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
       <c r="B81" s="76" t="s">
@@ -8205,7 +8250,7 @@
     <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="37"/>
       <c r="B87" s="37" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C87" s="64" t="s">
         <v>261</v>
@@ -8217,7 +8262,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="133" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G87" s="133"/>
       <c r="H87" s="133"/>
@@ -8230,7 +8275,7 @@
       <c r="O87" s="133"/>
       <c r="P87" s="133"/>
       <c r="Q87" s="133" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="R87" s="133"/>
       <c r="S87" s="133"/>
@@ -8248,7 +8293,7 @@
     </row>
     <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B88" s="57" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -8281,7 +8326,7 @@
       </c>
     </row>
     <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A91" s="37" t="e" vm="38">
+      <c r="A91" s="37" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="37" t="s">
@@ -8308,7 +8353,7 @@
       <c r="O91" s="64"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A92" s="37" t="e" vm="39">
+      <c r="A92" s="37" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="37" t="s">
@@ -8335,7 +8380,7 @@
       <c r="O92" s="64"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A93" s="37" t="e" vm="40">
+      <c r="A93" s="37" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="37" t="s">
@@ -8362,7 +8407,7 @@
       <c r="O93" s="64"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A94" s="37" t="e" vm="41">
+      <c r="A94" s="37" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="37" t="s">
@@ -8389,7 +8434,7 @@
       <c r="O94" s="64"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A95" s="37" t="e" vm="42">
+      <c r="A95" s="37" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="37" t="s">
@@ -8416,7 +8461,7 @@
       <c r="O95" s="64"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A96" s="37" t="e" vm="43">
+      <c r="A96" s="37" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="37" t="s">
@@ -8443,7 +8488,7 @@
       <c r="O96" s="64"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A97" s="37" t="e" vm="44">
+      <c r="A97" s="37" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="37" t="s">
@@ -8470,7 +8515,7 @@
       <c r="O97" s="64"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A98" s="37" t="e" vm="45">
+      <c r="A98" s="37" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="37" t="s">
@@ -8497,7 +8542,7 @@
       <c r="O98" s="64"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A99" s="37" t="e" vm="46">
+      <c r="A99" s="37" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="37" t="s">
@@ -8524,7 +8569,7 @@
       <c r="O99" s="64"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A100" s="37" t="e" vm="47">
+      <c r="A100" s="37" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="37" t="s">
@@ -8729,7 +8774,7 @@
       <c r="A111" s="37"/>
       <c r="B111" s="118"/>
       <c r="C111" s="115" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D111" s="115"/>
       <c r="E111" s="115"/>
@@ -8836,7 +8881,7 @@
         <v>244</v>
       </c>
       <c r="G116" s="117" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H116" s="115" t="s">
         <v>254</v>
@@ -8987,14 +9032,14 @@
       <c r="O123" s="64"/>
     </row>
     <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A124" s="37" t="e" vm="48">
+      <c r="A124" s="37" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="B124" s="118" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C124" s="115" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D124" s="115"/>
       <c r="E124" s="115"/>
@@ -9013,7 +9058,7 @@
       <c r="A125" s="37"/>
       <c r="B125" s="118"/>
       <c r="C125" s="115" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D125" s="115"/>
       <c r="E125" s="115"/>
@@ -9032,7 +9077,7 @@
       <c r="A126" s="37"/>
       <c r="B126" s="118"/>
       <c r="C126" s="115" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D126" s="115"/>
       <c r="E126" s="115"/>

</xml_diff>

<commit_message>
Military base update: In progress (added map, but without complete structures & items)
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC05CA9-3B1E-4E72-AB87-09CBD5361996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D518D706-EFBF-41AA-989C-7E78756B74FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="51">
+  <futureMetadata name="XLRICHVALUE" count="55">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -412,8 +412,36 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="51"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="52"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="53"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="54"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="51">
+  <valueMetadata count="55">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -566,13 +594,25 @@
     </bk>
     <bk>
       <rc t="1" v="50"/>
+    </bk>
+    <bk>
+      <rc t="1" v="51"/>
+    </bk>
+    <bk>
+      <rc t="1" v="52"/>
+    </bk>
+    <bk>
+      <rc t="1" v="53"/>
+    </bk>
+    <bk>
+      <rc t="1" v="54"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="292">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1746,6 +1786,14 @@
   </si>
   <si>
     <t>Explodes after speed &lt;= 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO TIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move busy - we also have peeker's advantage, so the player peeking first will see first</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2740,6 +2788,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB2B2B2"/>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FF958A5B"/>
+      <color rgb="FF0DDEE3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3417,6 +3473,472 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>84044</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>39220</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>299944</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>255120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="타원 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EECC1C5-B675-47B3-8E07-5ED485CE802A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="84044" y="18881912"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0DDEE3"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>79562</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>34738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295462</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>250638</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="타원 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62790101-E110-406B-94AE-E58C0EB08D21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="79562" y="19768297"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="958A5B"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91889</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>47064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>307789</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>262964</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="타원 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1A7FD1-685C-415D-A36A-09AEA5820EEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91889" y="19483668"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>87406</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>48187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>303306</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>264087</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="타원 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EF0844C-B62F-4EB6-8B07-4C9E4653A78F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="87406" y="19187834"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91889</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>30255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>307789</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>246155</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="타원 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8564820E-1D8B-49D8-BEBA-348E083B7770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91889" y="20060770"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>93009</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>42581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>308909</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>258481</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="타원 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{370F7771-E95A-491E-9AA6-3CB9064920E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="93009" y="20370052"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="66FFFF"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>99732</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>49304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>315632</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>265204</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="타원 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CDABA8-F493-4D2D-97A2-6F61A2FFD9F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="99732" y="20673731"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="B2B2B2"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3461,7 +3983,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="51">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="55">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -3666,6 +4188,22 @@
     <v>50</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>51</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>52</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>53</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>54</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -3731,6 +4269,10 @@
   <rel r:id="rId49"/>
   <rel r:id="rId50"/>
   <rel r:id="rId51"/>
+  <rel r:id="rId52"/>
+  <rel r:id="rId53"/>
+  <rel r:id="rId54"/>
+  <rel r:id="rId55"/>
 </richValueRels>
 </file>
 
@@ -3999,21 +4541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U76" sqref="U76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.0625" customWidth="1"/>
-    <col min="2" max="2" width="20.9375" customWidth="1"/>
-    <col min="10" max="10" width="10.6875" customWidth="1"/>
-    <col min="12" max="12" width="10.0625" customWidth="1"/>
-    <col min="15" max="15" width="9.3125" customWidth="1"/>
-    <col min="38" max="38" width="20.0625" customWidth="1"/>
+    <col min="1" max="1" width="5.08203125" customWidth="1"/>
+    <col min="2" max="2" width="20.9140625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.08203125" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1"/>
+    <col min="38" max="38" width="20.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:38" ht="34" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="81"/>
       <c r="B1" s="82" t="s">
         <v>175</v>
@@ -4051,7 +4593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="34"/>
       <c r="B2" s="76" t="s">
         <v>174</v>
@@ -4134,7 +4676,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="58"/>
       <c r="B3" s="18" t="s">
         <v>65</v>
@@ -4227,7 +4769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -4312,7 +4854,7 @@
       </c>
       <c r="AL4" s="35"/>
     </row>
-    <row r="5" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -4401,7 +4943,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -4486,7 +5028,7 @@
       </c>
       <c r="AL6" s="35"/>
     </row>
-    <row r="7" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="22" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -4547,7 +5089,7 @@
       </c>
       <c r="AL7" s="35"/>
     </row>
-    <row r="8" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -4628,7 +5170,7 @@
       <c r="Z8" s="56"/>
       <c r="AL8" s="35"/>
     </row>
-    <row r="9" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="75"/>
@@ -4657,7 +5199,7 @@
       <c r="Z9" s="56"/>
       <c r="AL9" s="35"/>
     </row>
-    <row r="10" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -4742,7 +5284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="18" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -4827,7 +5369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -4912,7 +5454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="18" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -4999,7 +5541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -5086,7 +5628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="75"/>
@@ -5114,7 +5656,7 @@
       <c r="Y15" s="73"/>
       <c r="Z15" s="56"/>
     </row>
-    <row r="16" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -5201,7 +5743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -5294,7 +5836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -5381,7 +5923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -5466,7 +6008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -5557,7 +6099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="75"/>
@@ -5584,7 +6126,7 @@
       <c r="X21" s="73"/>
       <c r="Y21" s="73"/>
     </row>
-    <row r="22" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="75"/>
@@ -5613,7 +6155,7 @@
       <c r="Z22" s="56"/>
       <c r="AL22" s="35"/>
     </row>
-    <row r="23" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -5700,7 +6242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="18" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
@@ -5785,7 +6327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -5874,7 +6416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="41"/>
@@ -5903,7 +6445,7 @@
       <c r="Z26" s="56"/>
       <c r="AL26" s="35"/>
     </row>
-    <row r="27" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="75"/>
@@ -5932,7 +6474,7 @@
       <c r="Z27" s="56"/>
       <c r="AL27" s="35"/>
     </row>
-    <row r="28" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -6017,7 +6559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="18" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
@@ -6102,7 +6644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="18" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
@@ -6187,7 +6729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="41"/>
@@ -6216,7 +6758,7 @@
       <c r="Z31" s="56"/>
       <c r="AL31" s="35"/>
     </row>
-    <row r="32" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="34"/>
       <c r="B32" s="76" t="s">
         <v>49</v>
@@ -6247,7 +6789,7 @@
       <c r="Z32" s="56"/>
       <c r="AL32" s="35"/>
     </row>
-    <row r="33" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
@@ -6319,7 +6861,7 @@
       </c>
       <c r="AL33" s="35"/>
     </row>
-    <row r="34" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
@@ -6389,7 +6931,7 @@
       <c r="Z34" s="56"/>
       <c r="AL34" s="35"/>
     </row>
-    <row r="35" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="18" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
@@ -6459,7 +7001,7 @@
       <c r="Z35" s="56"/>
       <c r="AL35" s="35"/>
     </row>
-    <row r="36" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="18" t="s">
         <v>201</v>
       </c>
@@ -6531,7 +7073,7 @@
       </c>
       <c r="AL36" s="35"/>
     </row>
-    <row r="37" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="18" t="s">
         <v>201</v>
       </c>
@@ -6600,8 +7142,8 @@
       <c r="Y37" s="19"/>
       <c r="AL37" s="35"/>
     </row>
-    <row r="38" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="39" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="35"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
@@ -6612,7 +7154,7 @@
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
     </row>
-    <row r="40" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="34"/>
       <c r="B40" s="76" t="s">
         <v>172</v>
@@ -6644,7 +7186,7 @@
       <c r="T40" s="142"/>
       <c r="U40" s="56"/>
     </row>
-    <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="37" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
@@ -6683,7 +7225,7 @@
       </c>
       <c r="V41" s="56"/>
     </row>
-    <row r="42" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="37" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
@@ -6722,7 +7264,7 @@
       </c>
       <c r="V42" s="56"/>
     </row>
-    <row r="43" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
         <v>201</v>
       </c>
@@ -6763,7 +7305,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
         <v>201</v>
       </c>
@@ -6795,8 +7337,8 @@
       <c r="T44" s="56"/>
       <c r="U44" s="56"/>
     </row>
-    <row r="45" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="46" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="34"/>
       <c r="B46" s="76" t="s">
         <v>189</v>
@@ -6817,7 +7359,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="37" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
@@ -6840,7 +7382,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="37" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -6863,7 +7405,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="130"/>
@@ -6876,8 +7418,8 @@
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
     </row>
-    <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="51" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="34"/>
       <c r="B51" s="76" t="s">
         <v>263</v>
@@ -6898,7 +7440,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="37" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
@@ -6921,7 +7463,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="37" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -6944,7 +7486,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="18" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -6967,12 +7509,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="57" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C56" s="62" t="s">
         <v>164</v>
       </c>
@@ -6988,7 +7530,7 @@
       <c r="L56" s="134"/>
       <c r="M56" s="134"/>
     </row>
-    <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="90"/>
       <c r="B57" s="86" t="s">
         <v>171</v>
@@ -7027,7 +7569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="89"/>
       <c r="B58" s="58" t="s">
         <v>69</v>
@@ -7077,7 +7619,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="89"/>
       <c r="B59" s="58" t="s">
         <v>70</v>
@@ -7127,7 +7669,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C60" s="63" t="s">
         <v>165</v>
       </c>
@@ -7165,7 +7707,7 @@
       <c r="AI60" s="79"/>
       <c r="AJ60" s="79"/>
     </row>
-    <row r="61" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="O61">
         <v>200</v>
       </c>
@@ -7186,7 +7728,7 @@
       <c r="AI61" s="80"/>
       <c r="AJ61" s="80"/>
     </row>
-    <row r="62" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I62" t="s">
         <v>96</v>
       </c>
@@ -7213,7 +7755,7 @@
       <c r="AI62" s="80"/>
       <c r="AJ62" s="80"/>
     </row>
-    <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="90" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
@@ -7283,7 +7825,7 @@
       <c r="AI63" s="80"/>
       <c r="AJ63" s="80"/>
     </row>
-    <row r="64" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="37"/>
       <c r="B64" s="37" t="s">
         <v>85</v>
@@ -7360,7 +7902,7 @@
       <c r="AI64" s="80"/>
       <c r="AJ64" s="80"/>
     </row>
-    <row r="65" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
         <v>86</v>
@@ -7437,7 +7979,7 @@
       <c r="AI65" s="80"/>
       <c r="AJ65" s="80"/>
     </row>
-    <row r="66" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
         <v>87</v>
@@ -7514,7 +8056,7 @@
       <c r="AI66" s="80"/>
       <c r="AJ66" s="80"/>
     </row>
-    <row r="67" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="18"/>
       <c r="B67" s="18" t="s">
         <v>88</v>
@@ -7587,7 +8129,7 @@
       <c r="Y67" s="56"/>
       <c r="Z67" s="56"/>
     </row>
-    <row r="68" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="18"/>
       <c r="B68" s="18" t="s">
         <v>93</v>
@@ -7660,7 +8202,7 @@
       <c r="Y68" s="56"/>
       <c r="Z68" s="56"/>
     </row>
-    <row r="69" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="18"/>
       <c r="B69" s="18" t="s">
         <v>104</v>
@@ -7733,7 +8275,7 @@
       <c r="Y69" s="56"/>
       <c r="Z69" s="56"/>
     </row>
-    <row r="70" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="18"/>
       <c r="B70" s="18" t="s">
         <v>115</v>
@@ -7806,9 +8348,9 @@
       <c r="Y70" s="56"/>
       <c r="Z70" s="56"/>
     </row>
-    <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B73" s="116" t="s">
         <v>238</v>
       </c>
@@ -7819,7 +8361,7 @@
       <c r="Q73" s="141"/>
       <c r="R73" s="141"/>
     </row>
-    <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="34"/>
       <c r="B74" s="76" t="s">
         <v>129</v>
@@ -7862,7 +8404,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="37" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
@@ -7902,14 +8444,18 @@
       <c r="P75" s="69" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
-      <c r="Q75" s="78"/>
-      <c r="R75" s="94"/>
+      <c r="Q75" s="78" t="e" vm="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R75" s="94" t="e" vm="37">
+        <v>#VALUE!</v>
+      </c>
       <c r="S75" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A76" s="37" t="e" vm="36">
+    <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="37" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="37" t="s">
@@ -7939,22 +8485,26 @@
       <c r="K76" s="135"/>
       <c r="L76" s="135"/>
       <c r="M76" s="135"/>
-      <c r="N76" s="77" t="e" vm="37">
+      <c r="N76" s="77" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
-      <c r="O76" s="69" t="e" vm="38">
+      <c r="O76" s="69" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
-      <c r="P76" s="69" t="e" vm="39">
+      <c r="P76" s="69" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
-      <c r="Q76" s="78"/>
-      <c r="R76" s="94"/>
+      <c r="Q76" s="78" t="e" vm="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R76" s="94" t="e" vm="43">
+        <v>#VALUE!</v>
+      </c>
       <c r="S76" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="18"/>
       <c r="B77" s="18"/>
       <c r="C77" s="43"/>
@@ -7975,7 +8525,7 @@
       <c r="R77" s="126"/>
       <c r="S77" s="64"/>
     </row>
-    <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="111" t="s">
         <v>198</v>
       </c>
@@ -7983,10 +8533,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="81" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A81" s="34" t="e" vm="40">
+    <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="34" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="B81" s="76" t="s">
@@ -8031,7 +8581,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="37"/>
       <c r="B82" s="37" t="s">
         <v>146</v>
@@ -8075,7 +8625,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="37"/>
       <c r="B83" s="37" t="s">
         <v>147</v>
@@ -8117,7 +8667,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="37"/>
       <c r="B84" s="37" t="s">
         <v>148</v>
@@ -8159,7 +8709,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="37"/>
       <c r="B85" s="37" t="s">
         <v>149</v>
@@ -8203,7 +8753,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="37"/>
       <c r="B86" s="37" t="s">
         <v>200</v>
@@ -8247,7 +8797,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="37"/>
       <c r="B87" s="37" t="s">
         <v>274</v>
@@ -8291,13 +8841,13 @@
         <v>260</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="57" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="90" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="34"/>
       <c r="B90" s="76" t="s">
         <v>173</v>
@@ -8325,8 +8875,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A91" s="37" t="e" vm="41">
+    <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="37" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="37" t="s">
@@ -8352,8 +8902,8 @@
       <c r="N91" s="128"/>
       <c r="O91" s="64"/>
     </row>
-    <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A92" s="37" t="e" vm="42">
+    <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="37" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="37" t="s">
@@ -8379,8 +8929,8 @@
       <c r="N92" s="128"/>
       <c r="O92" s="64"/>
     </row>
-    <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A93" s="37" t="e" vm="43">
+    <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="37" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="37" t="s">
@@ -8406,8 +8956,8 @@
       <c r="N93" s="128"/>
       <c r="O93" s="64"/>
     </row>
-    <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A94" s="37" t="e" vm="44">
+    <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="37" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="37" t="s">
@@ -8433,8 +8983,8 @@
       <c r="N94" s="128"/>
       <c r="O94" s="64"/>
     </row>
-    <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A95" s="37" t="e" vm="45">
+    <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="37" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="37" t="s">
@@ -8460,8 +9010,8 @@
       <c r="N95" s="128"/>
       <c r="O95" s="64"/>
     </row>
-    <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A96" s="37" t="e" vm="46">
+    <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="37" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="37" t="s">
@@ -8487,8 +9037,8 @@
       <c r="N96" s="128"/>
       <c r="O96" s="64"/>
     </row>
-    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A97" s="37" t="e" vm="47">
+    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="37" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="37" t="s">
@@ -8514,8 +9064,8 @@
       <c r="N97" s="128"/>
       <c r="O97" s="64"/>
     </row>
-    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A98" s="37" t="e" vm="48">
+    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="37" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="37" t="s">
@@ -8541,8 +9091,8 @@
       <c r="N98" s="128"/>
       <c r="O98" s="64"/>
     </row>
-    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A99" s="37" t="e" vm="49">
+    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="37" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="37" t="s">
@@ -8568,8 +9118,8 @@
       <c r="N99" s="128"/>
       <c r="O99" s="64"/>
     </row>
-    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A100" s="37" t="e" vm="50">
+    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="37" t="e" vm="54">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="37" t="s">
@@ -8595,7 +9145,7 @@
       <c r="N100" s="128"/>
       <c r="O100" s="64"/>
     </row>
-    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
       <c r="C101" s="127"/>
@@ -8612,7 +9162,7 @@
       <c r="N101" s="128"/>
       <c r="O101" s="64"/>
     </row>
-    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="H102" s="127"/>
@@ -8624,7 +9174,7 @@
       <c r="N102" s="128"/>
       <c r="O102" s="64"/>
     </row>
-    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
       <c r="C103" s="127"/>
@@ -8641,7 +9191,7 @@
       <c r="N103" s="128"/>
       <c r="O103" s="64"/>
     </row>
-    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
       <c r="C104" s="127"/>
@@ -8658,7 +9208,7 @@
       <c r="N104" s="128"/>
       <c r="O104" s="64"/>
     </row>
-    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
       <c r="C105" s="127"/>
@@ -8675,7 +9225,7 @@
       <c r="N105" s="128"/>
       <c r="O105" s="64"/>
     </row>
-    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
       <c r="C106" s="127"/>
@@ -8692,7 +9242,7 @@
       <c r="N106" s="128"/>
       <c r="O106" s="64"/>
     </row>
-    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="81"/>
       <c r="B107" s="113" t="s">
         <v>233</v>
@@ -8711,7 +9261,7 @@
       <c r="N107" s="81"/>
       <c r="O107" s="81"/>
     </row>
-    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="37"/>
       <c r="B108" s="118" t="s">
         <v>234</v>
@@ -8732,7 +9282,7 @@
       <c r="N108" s="64"/>
       <c r="O108" s="64"/>
     </row>
-    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="37"/>
       <c r="B109" s="118"/>
       <c r="C109" s="115" t="s">
@@ -8751,7 +9301,7 @@
       <c r="N109" s="64"/>
       <c r="O109" s="64"/>
     </row>
-    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="37"/>
       <c r="B110" s="118"/>
       <c r="C110" s="115" t="s">
@@ -8770,7 +9320,7 @@
       <c r="N110" s="64"/>
       <c r="O110" s="64"/>
     </row>
-    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="37"/>
       <c r="B111" s="118"/>
       <c r="C111" s="115" t="s">
@@ -8789,7 +9339,7 @@
       <c r="N111" s="64"/>
       <c r="O111" s="64"/>
     </row>
-    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="37"/>
       <c r="B112" s="118"/>
       <c r="C112" s="115"/>
@@ -8806,7 +9356,7 @@
       <c r="N112" s="64"/>
       <c r="O112" s="64"/>
     </row>
-    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="37"/>
       <c r="B113" s="118" t="s">
         <v>237</v>
@@ -8827,7 +9377,7 @@
       <c r="N113" s="64"/>
       <c r="O113" s="64"/>
     </row>
-    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="37"/>
       <c r="B114" s="118"/>
       <c r="C114" s="115" t="s">
@@ -8846,7 +9396,7 @@
       <c r="N114" s="64"/>
       <c r="O114" s="64"/>
     </row>
-    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="37"/>
       <c r="B115" s="118"/>
       <c r="C115" s="115"/>
@@ -8863,7 +9413,7 @@
       <c r="N115" s="64"/>
       <c r="O115" s="64"/>
     </row>
-    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="37"/>
       <c r="B116" s="118" t="s">
         <v>252</v>
@@ -8894,7 +9444,7 @@
       <c r="N116" s="64"/>
       <c r="O116" s="64"/>
     </row>
-    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="37"/>
       <c r="B117" s="118"/>
       <c r="C117" s="119" t="s">
@@ -8921,7 +9471,7 @@
       <c r="N117" s="64"/>
       <c r="O117" s="64"/>
     </row>
-    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="37"/>
       <c r="B118" s="118"/>
       <c r="C118" s="115"/>
@@ -8938,7 +9488,7 @@
       <c r="N118" s="64"/>
       <c r="O118" s="64"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A119" s="37"/>
       <c r="B119" s="118"/>
       <c r="C119" s="115" t="s">
@@ -8957,7 +9507,7 @@
       <c r="N119" s="64"/>
       <c r="O119" s="64"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A120" s="37"/>
       <c r="B120" s="118"/>
       <c r="C120" s="115" t="s">
@@ -8976,7 +9526,7 @@
       <c r="N120" s="64"/>
       <c r="O120" s="64"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A121" s="37"/>
       <c r="B121" s="118"/>
       <c r="C121" s="115" t="s">
@@ -8995,7 +9545,7 @@
       <c r="N121" s="64"/>
       <c r="O121" s="64"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A122" s="37"/>
       <c r="B122" s="118"/>
       <c r="C122" s="115" t="s">
@@ -9014,7 +9564,7 @@
       <c r="N122" s="64"/>
       <c r="O122" s="64"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A123" s="37"/>
       <c r="B123" s="118"/>
       <c r="C123" s="115"/>
@@ -9031,8 +9581,8 @@
       <c r="N123" s="64"/>
       <c r="O123" s="64"/>
     </row>
-    <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A124" s="37" t="e" vm="51">
+    <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A124" s="37" t="e" vm="55">
         <v>#VALUE!</v>
       </c>
       <c r="B124" s="118" t="s">
@@ -9054,7 +9604,7 @@
       <c r="N124" s="64"/>
       <c r="O124" s="64"/>
     </row>
-    <row r="125" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="37"/>
       <c r="B125" s="118"/>
       <c r="C125" s="115" t="s">
@@ -9073,7 +9623,7 @@
       <c r="N125" s="64"/>
       <c r="O125" s="64"/>
     </row>
-    <row r="126" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="126" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="37"/>
       <c r="B126" s="118"/>
       <c r="C126" s="115" t="s">
@@ -9092,7 +9642,7 @@
       <c r="N126" s="64"/>
       <c r="O126" s="64"/>
     </row>
-    <row r="127" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="127" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="37"/>
       <c r="B127" s="118"/>
       <c r="C127" s="115"/>
@@ -9109,10 +9659,14 @@
       <c r="N127" s="64"/>
       <c r="O127" s="64"/>
     </row>
-    <row r="128" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="128" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="37"/>
-      <c r="B128" s="118"/>
-      <c r="C128" s="115"/>
+      <c r="B128" s="118" t="s">
+        <v>290</v>
+      </c>
+      <c r="C128" s="115" t="s">
+        <v>291</v>
+      </c>
       <c r="D128" s="115"/>
       <c r="E128" s="115"/>
       <c r="F128" s="115"/>
@@ -9126,7 +9680,7 @@
       <c r="N128" s="64"/>
       <c r="O128" s="64"/>
     </row>
-    <row r="129" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="129" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129" s="37"/>
       <c r="B129" s="118"/>
       <c r="C129" s="115"/>
@@ -9143,7 +9697,7 @@
       <c r="N129" s="64"/>
       <c r="O129" s="64"/>
     </row>
-    <row r="130" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="130" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130" s="37"/>
       <c r="B130" s="118"/>
       <c r="C130" s="115"/>
@@ -9160,7 +9714,7 @@
       <c r="N130" s="64"/>
       <c r="O130" s="64"/>
     </row>
-    <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="37"/>
       <c r="B131" s="118"/>
       <c r="C131" s="115"/>
@@ -9177,7 +9731,7 @@
       <c r="N131" s="64"/>
       <c r="O131" s="64"/>
     </row>
-    <row r="132" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="132" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="37"/>
       <c r="B132" s="118"/>
       <c r="C132" s="115"/>
@@ -9194,7 +9748,7 @@
       <c r="N132" s="64"/>
       <c r="O132" s="64"/>
     </row>
-    <row r="133" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="133" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="37"/>
       <c r="B133" s="118"/>
       <c r="C133" s="115"/>
@@ -9211,7 +9765,7 @@
       <c r="N133" s="64"/>
       <c r="O133" s="64"/>
     </row>
-    <row r="134" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="134" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="37"/>
       <c r="B134" s="118"/>
       <c r="C134" s="115"/>
@@ -9228,7 +9782,7 @@
       <c r="N134" s="64"/>
       <c r="O134" s="64"/>
     </row>
-    <row r="135" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="135" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="37"/>
       <c r="B135" s="118"/>
       <c r="C135" s="115"/>
@@ -9245,7 +9799,7 @@
       <c r="N135" s="64"/>
       <c r="O135" s="64"/>
     </row>
-    <row r="136" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="136" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="37"/>
       <c r="B136" s="118"/>
       <c r="C136" s="115"/>
@@ -9262,7 +9816,7 @@
       <c r="N136" s="64"/>
       <c r="O136" s="64"/>
     </row>
-    <row r="137" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="137" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="37"/>
       <c r="B137" s="118"/>
       <c r="C137" s="115"/>
@@ -9279,12 +9833,12 @@
       <c r="N137" s="64"/>
       <c r="O137" s="64"/>
     </row>
-    <row r="138" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="139" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="140" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="141" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="142" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="138" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="139" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="140" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="141" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="142" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="139">
     <mergeCell ref="E1:F1"/>

</xml_diff>

<commit_message>
enhanced speed of flying vehicles
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D518D706-EFBF-41AA-989C-7E78756B74FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E178BCEF-AE74-4225-AF0D-F43A76CEEAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="293">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1794,6 +1794,10 @@
   </si>
   <si>
     <t>Move busy - we also have peeker's advantage, so the player peeking first will see first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 ~ 500</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4541,8 +4545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U76" sqref="U76"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V56" sqref="V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -7471,7 +7475,7 @@
         <v>265</v>
       </c>
       <c r="C53" s="135" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D53" s="135"/>
       <c r="E53" s="133" t="s">
@@ -7715,7 +7719,7 @@
         <v>30</v>
       </c>
       <c r="Q61">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R61">
         <v>50</v>
@@ -7873,7 +7877,7 @@
       </c>
       <c r="Q64" s="100">
         <f t="shared" ref="Q64:Q70" si="35">ROUND(E64/speed_cap,2)*10</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R64" s="101">
         <f t="shared" ref="R64:R70" si="36">ROUND(I64/DPS_cap,2)*10</f>
@@ -7881,7 +7885,7 @@
       </c>
       <c r="S64" s="102">
         <f>SUM(O64:R64)</f>
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="T64" s="96"/>
       <c r="U64" s="146">
@@ -7950,7 +7954,7 @@
       </c>
       <c r="Q65" s="67">
         <f t="shared" si="35"/>
-        <v>4</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="R65" s="68">
         <f t="shared" si="36"/>
@@ -7958,7 +7962,7 @@
       </c>
       <c r="S65" s="69">
         <f t="shared" ref="S65:S69" si="38">SUM(O65:R65)</f>
-        <v>14.5</v>
+        <v>13.8</v>
       </c>
       <c r="T65" s="53"/>
       <c r="U65" s="147">
@@ -8027,7 +8031,7 @@
       </c>
       <c r="Q66" s="67">
         <f t="shared" si="35"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="R66" s="68">
         <f t="shared" si="36"/>
@@ -8035,7 +8039,7 @@
       </c>
       <c r="S66" s="69">
         <f t="shared" si="38"/>
-        <v>13.899999999999999</v>
+        <v>13.399999999999999</v>
       </c>
       <c r="T66" s="53"/>
       <c r="U66" s="147">
@@ -8104,7 +8108,7 @@
       </c>
       <c r="Q67" s="67">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="R67" s="68">
         <f t="shared" si="36"/>
@@ -8112,7 +8116,7 @@
       </c>
       <c r="S67" s="69">
         <f t="shared" si="38"/>
-        <v>18.700000000000003</v>
+        <v>18.500000000000004</v>
       </c>
       <c r="T67" s="53"/>
       <c r="U67" s="147">
@@ -8214,7 +8218,7 @@
         <v>40</v>
       </c>
       <c r="E69" s="53">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F69" s="128" t="s">
         <v>39</v>
@@ -8249,7 +8253,7 @@
         <v>5</v>
       </c>
       <c r="Q69" s="67">
-        <f t="shared" si="35"/>
+        <f>ROUND(E69/speed_cap,2)*10</f>
         <v>10</v>
       </c>
       <c r="R69" s="68">
@@ -8287,7 +8291,7 @@
         <v>50</v>
       </c>
       <c r="E70" s="53">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F70" s="128" t="s">
         <v>116</v>
@@ -8323,7 +8327,7 @@
       </c>
       <c r="Q70" s="67">
         <f t="shared" si="35"/>
-        <v>8</v>
+        <v>8.2999999999999989</v>
       </c>
       <c r="R70" s="68">
         <f t="shared" si="36"/>
@@ -8331,7 +8335,7 @@
       </c>
       <c r="S70" s="69">
         <f t="shared" ref="S70" si="41">SUM(O70:R70)</f>
-        <v>25.799999999999997</v>
+        <v>26.1</v>
       </c>
       <c r="T70" s="53"/>
       <c r="U70" s="147">

</xml_diff>

<commit_message>
vehicle-cehicle collision not implemented
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E178BCEF-AE74-4225-AF0D-F43A76CEEAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96250E0-5950-41F3-86E2-CE4EABF19F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="294">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1798,6 +1798,10 @@
   </si>
   <si>
     <t>0 ~ 500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acceleration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2720,71 +2724,71 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4545,33 +4549,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V56" sqref="V56"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="5.08203125" customWidth="1"/>
-    <col min="2" max="2" width="20.9140625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.08203125" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" customWidth="1"/>
-    <col min="38" max="38" width="20.08203125" customWidth="1"/>
+    <col min="1" max="1" width="5.0625" customWidth="1"/>
+    <col min="2" max="2" width="20.9375" customWidth="1"/>
+    <col min="10" max="10" width="10.6875" customWidth="1"/>
+    <col min="12" max="12" width="10.0625" customWidth="1"/>
+    <col min="14" max="14" width="10.9375" customWidth="1"/>
+    <col min="15" max="15" width="9.3125" customWidth="1"/>
+    <col min="38" max="38" width="20.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:38" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="81"/>
       <c r="B1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="126" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="138"/>
-      <c r="E1" s="137" t="s">
+      <c r="D1" s="127"/>
+      <c r="E1" s="126" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="138"/>
+      <c r="F1" s="127"/>
       <c r="G1" s="55" t="s">
         <v>159</v>
       </c>
@@ -4597,7 +4602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="34"/>
       <c r="B2" s="76" t="s">
         <v>174</v>
@@ -4667,10 +4672,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="56"/>
-      <c r="Z2" s="141" t="s">
+      <c r="Z2" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="141"/>
+      <c r="AA2" s="135"/>
       <c r="AG2" s="42" t="s">
         <v>84</v>
       </c>
@@ -4680,7 +4685,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="58"/>
       <c r="B3" s="18" t="s">
         <v>65</v>
@@ -4773,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -4858,7 +4863,7 @@
       </c>
       <c r="AL4" s="35"/>
     </row>
-    <row r="5" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="22" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -4881,7 +4886,7 @@
         <v>4000</v>
       </c>
       <c r="H5" s="23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I5" s="23">
         <v>1</v>
@@ -4947,7 +4952,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="22" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -5032,7 +5037,7 @@
       </c>
       <c r="AL6" s="35"/>
     </row>
-    <row r="7" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="22" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -5093,7 +5098,7 @@
       </c>
       <c r="AL7" s="35"/>
     </row>
-    <row r="8" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -5174,7 +5179,7 @@
       <c r="Z8" s="56"/>
       <c r="AL8" s="35"/>
     </row>
-    <row r="9" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="75"/>
@@ -5203,7 +5208,7 @@
       <c r="Z9" s="56"/>
       <c r="AL9" s="35"/>
     </row>
-    <row r="10" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="18" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -5288,7 +5293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="18" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -5373,7 +5378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="18" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -5458,7 +5463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="18" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -5545,7 +5550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="18" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -5632,7 +5637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="75"/>
@@ -5660,7 +5665,7 @@
       <c r="Y15" s="73"/>
       <c r="Z15" s="56"/>
     </row>
-    <row r="16" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="18" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -5747,7 +5752,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="18" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -5840,7 +5845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="18" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -5927,7 +5932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="18" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -6012,7 +6017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="18" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -6103,7 +6108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="75"/>
@@ -6130,7 +6135,7 @@
       <c r="X21" s="73"/>
       <c r="Y21" s="73"/>
     </row>
-    <row r="22" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="75"/>
@@ -6159,7 +6164,7 @@
       <c r="Z22" s="56"/>
       <c r="AL22" s="35"/>
     </row>
-    <row r="23" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="18" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -6246,7 +6251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="18" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
@@ -6331,7 +6336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -6420,7 +6425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="41"/>
@@ -6449,7 +6454,7 @@
       <c r="Z26" s="56"/>
       <c r="AL26" s="35"/>
     </row>
-    <row r="27" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="75"/>
@@ -6478,7 +6483,7 @@
       <c r="Z27" s="56"/>
       <c r="AL27" s="35"/>
     </row>
-    <row r="28" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="18" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -6563,7 +6568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="18" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
@@ -6648,7 +6653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="18" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
@@ -6733,7 +6738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="41"/>
@@ -6762,7 +6767,7 @@
       <c r="Z31" s="56"/>
       <c r="AL31" s="35"/>
     </row>
-    <row r="32" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="34"/>
       <c r="B32" s="76" t="s">
         <v>49</v>
@@ -6793,7 +6798,7 @@
       <c r="Z32" s="56"/>
       <c r="AL32" s="35"/>
     </row>
-    <row r="33" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="18" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
@@ -6865,7 +6870,7 @@
       </c>
       <c r="AL33" s="35"/>
     </row>
-    <row r="34" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="18" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
@@ -6935,7 +6940,7 @@
       <c r="Z34" s="56"/>
       <c r="AL34" s="35"/>
     </row>
-    <row r="35" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="18" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
@@ -7005,7 +7010,7 @@
       <c r="Z35" s="56"/>
       <c r="AL35" s="35"/>
     </row>
-    <row r="36" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="18" t="s">
         <v>201</v>
       </c>
@@ -7077,7 +7082,7 @@
       </c>
       <c r="AL36" s="35"/>
     </row>
-    <row r="37" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="18" t="s">
         <v>201</v>
       </c>
@@ -7146,8 +7151,8 @@
       <c r="Y37" s="19"/>
       <c r="AL37" s="35"/>
     </row>
-    <row r="38" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="39" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="35"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
@@ -7158,25 +7163,25 @@
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
     </row>
-    <row r="40" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="34"/>
       <c r="B40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="136" t="s">
+      <c r="C40" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="136"/>
-      <c r="E40" s="136"/>
-      <c r="F40" s="136"/>
-      <c r="G40" s="136"/>
-      <c r="H40" s="136"/>
-      <c r="I40" s="136" t="s">
+      <c r="D40" s="137"/>
+      <c r="E40" s="137"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="137"/>
+      <c r="I40" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="136"/>
-      <c r="K40" s="136"/>
-      <c r="L40" s="136"/>
+      <c r="J40" s="137"/>
+      <c r="K40" s="137"/>
+      <c r="L40" s="137"/>
       <c r="M40" s="107"/>
       <c r="N40" s="107"/>
       <c r="O40" s="107"/>
@@ -7184,35 +7189,35 @@
       <c r="Q40" s="120" t="s">
         <v>258</v>
       </c>
-      <c r="S40" s="142" t="s">
+      <c r="S40" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="142"/>
+      <c r="T40" s="136"/>
       <c r="U40" s="56"/>
     </row>
-    <row r="41" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="37" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="145" t="s">
+      <c r="C41" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="145"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="145" t="s">
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="145"/>
-      <c r="H41" s="145"/>
-      <c r="I41" s="145" t="s">
+      <c r="G41" s="138"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="145"/>
-      <c r="K41" s="145"/>
-      <c r="L41" s="145"/>
+      <c r="J41" s="138"/>
+      <c r="K41" s="138"/>
+      <c r="L41" s="138"/>
       <c r="M41" s="108"/>
       <c r="N41" s="108"/>
       <c r="O41" s="108"/>
@@ -7220,38 +7225,38 @@
       <c r="Q41" s="64" t="s">
         <v>259</v>
       </c>
-      <c r="S41" s="142" t="s">
+      <c r="S41" s="136" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="142"/>
+      <c r="T41" s="136"/>
       <c r="U41" s="56">
         <v>8</v>
       </c>
       <c r="V41" s="56"/>
     </row>
-    <row r="42" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="37" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="145" t="s">
+      <c r="C42" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="145"/>
-      <c r="E42" s="145"/>
-      <c r="F42" s="145" t="s">
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138" t="s">
         <v>199</v>
       </c>
-      <c r="G42" s="145"/>
-      <c r="H42" s="145"/>
-      <c r="I42" s="145" t="s">
+      <c r="G42" s="138"/>
+      <c r="H42" s="138"/>
+      <c r="I42" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="145"/>
-      <c r="K42" s="145"/>
-      <c r="L42" s="145"/>
+      <c r="J42" s="138"/>
+      <c r="K42" s="138"/>
+      <c r="L42" s="138"/>
       <c r="M42" s="108"/>
       <c r="N42" s="108"/>
       <c r="O42" s="108"/>
@@ -7259,38 +7264,38 @@
       <c r="Q42" s="64" t="s">
         <v>259</v>
       </c>
-      <c r="S42" s="142" t="s">
+      <c r="S42" s="136" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="142"/>
+      <c r="T42" s="136"/>
       <c r="U42" s="56">
         <v>128</v>
       </c>
       <c r="V42" s="56"/>
     </row>
-    <row r="43" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="139" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130" t="s">
+      <c r="D43" s="139"/>
+      <c r="E43" s="139"/>
+      <c r="F43" s="139" t="s">
         <v>207</v>
       </c>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130" t="s">
+      <c r="G43" s="139"/>
+      <c r="H43" s="139"/>
+      <c r="I43" s="139" t="s">
         <v>204</v>
       </c>
-      <c r="J43" s="130"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="130"/>
+      <c r="J43" s="139"/>
+      <c r="K43" s="139"/>
+      <c r="L43" s="139"/>
       <c r="M43" s="43"/>
       <c r="N43" s="43"/>
       <c r="O43" s="108"/>
@@ -7298,10 +7303,10 @@
       <c r="Q43" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="S43" s="142" t="s">
+      <c r="S43" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="142"/>
+      <c r="T43" s="136"/>
       <c r="U43" s="56">
         <v>16</v>
       </c>
@@ -7309,27 +7314,27 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="130" t="s">
+      <c r="C44" s="139" t="s">
         <v>267</v>
       </c>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="130"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="130"/>
-      <c r="I44" s="130" t="s">
+      <c r="D44" s="139"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="139"/>
+      <c r="I44" s="139" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="130"/>
-      <c r="K44" s="130"/>
-      <c r="L44" s="130"/>
+      <c r="J44" s="139"/>
+      <c r="K44" s="139"/>
+      <c r="L44" s="139"/>
       <c r="M44" s="43"/>
       <c r="N44" s="43"/>
       <c r="O44" s="108"/>
@@ -7341,8 +7346,8 @@
       <c r="T44" s="56"/>
       <c r="U44" s="56"/>
     </row>
-    <row r="45" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="46" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A46" s="34"/>
       <c r="B46" s="76" t="s">
         <v>189</v>
@@ -7363,7 +7368,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="37" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
@@ -7386,7 +7391,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A48" s="37" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -7409,132 +7414,132 @@
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="130"/>
-      <c r="D49" s="130"/>
-      <c r="E49" s="130"/>
-      <c r="F49" s="130"/>
-      <c r="G49" s="130"/>
-      <c r="H49" s="130"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="139"/>
+      <c r="F49" s="139"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="139"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
       <c r="K49" s="64"/>
     </row>
-    <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="51" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="34"/>
       <c r="B51" s="76" t="s">
         <v>263</v>
       </c>
-      <c r="C51" s="136" t="s">
+      <c r="C51" s="137" t="s">
         <v>268</v>
       </c>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136" t="s">
+      <c r="D51" s="137"/>
+      <c r="E51" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="136"/>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
+      <c r="F51" s="137"/>
+      <c r="G51" s="137"/>
+      <c r="H51" s="137"/>
+      <c r="I51" s="137"/>
+      <c r="J51" s="137"/>
       <c r="K51" s="120" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A52" s="37" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="135" t="s">
+      <c r="C52" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D52" s="135"/>
-      <c r="E52" s="133" t="s">
+      <c r="D52" s="133"/>
+      <c r="E52" s="140" t="s">
         <v>289</v>
       </c>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="133"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="140"/>
+      <c r="I52" s="140"/>
+      <c r="J52" s="140"/>
       <c r="K52" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A53" s="37" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
       <c r="B53" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="C53" s="135" t="s">
+      <c r="C53" s="133" t="s">
         <v>292</v>
       </c>
-      <c r="D53" s="135"/>
-      <c r="E53" s="133" t="s">
+      <c r="D53" s="133"/>
+      <c r="E53" s="140" t="s">
         <v>287</v>
       </c>
-      <c r="F53" s="133"/>
-      <c r="G53" s="133"/>
-      <c r="H53" s="133"/>
-      <c r="I53" s="133"/>
-      <c r="J53" s="133"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="140"/>
+      <c r="H53" s="140"/>
+      <c r="I53" s="140"/>
+      <c r="J53" s="140"/>
       <c r="K53" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A54" s="18" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C54" s="135" t="s">
+      <c r="C54" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="D54" s="135"/>
-      <c r="E54" s="133" t="s">
+      <c r="D54" s="133"/>
+      <c r="E54" s="140" t="s">
         <v>288</v>
       </c>
-      <c r="F54" s="133"/>
-      <c r="G54" s="133"/>
-      <c r="H54" s="133"/>
-      <c r="I54" s="133"/>
-      <c r="J54" s="133"/>
+      <c r="F54" s="140"/>
+      <c r="G54" s="140"/>
+      <c r="H54" s="140"/>
+      <c r="I54" s="140"/>
+      <c r="J54" s="140"/>
       <c r="K54" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A55" s="57" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C56" s="62" t="s">
         <v>164</v>
       </c>
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="134" t="s">
+      <c r="H56" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="134"/>
-      <c r="J56" s="134"/>
-      <c r="K56" s="134"/>
-      <c r="L56" s="134"/>
-      <c r="M56" s="134"/>
-    </row>
-    <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I56" s="146"/>
+      <c r="J56" s="146"/>
+      <c r="K56" s="146"/>
+      <c r="L56" s="146"/>
+      <c r="M56" s="146"/>
+    </row>
+    <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="90"/>
       <c r="B57" s="86" t="s">
         <v>171</v>
@@ -7573,7 +7578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A58" s="89"/>
       <c r="B58" s="58" t="s">
         <v>69</v>
@@ -7623,7 +7628,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A59" s="89"/>
       <c r="B59" s="58" t="s">
         <v>70</v>
@@ -7673,7 +7678,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C60" s="63" t="s">
         <v>165</v>
       </c>
@@ -7711,7 +7716,7 @@
       <c r="AI60" s="79"/>
       <c r="AJ60" s="79"/>
     </row>
-    <row r="61" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="O61">
         <v>200</v>
       </c>
@@ -7732,14 +7737,14 @@
       <c r="AI61" s="80"/>
       <c r="AJ61" s="80"/>
     </row>
-    <row r="62" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="140" t="s">
+      <c r="J62" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="140"/>
+      <c r="K62" s="142"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
@@ -7747,19 +7752,19 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>25</v>
       </c>
-      <c r="O62" s="139" t="s">
+      <c r="O62" s="141" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="139"/>
-      <c r="Q62" s="139"/>
-      <c r="R62" s="139"/>
-      <c r="S62" s="139"/>
+      <c r="P62" s="141"/>
+      <c r="Q62" s="141"/>
+      <c r="R62" s="141"/>
+      <c r="S62" s="141"/>
       <c r="AG62" s="80"/>
       <c r="AH62" s="80"/>
       <c r="AI62" s="80"/>
       <c r="AJ62" s="80"/>
     </row>
-    <row r="63" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A63" s="90" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
@@ -7775,27 +7780,29 @@
       <c r="E63" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="143" t="s">
+      <c r="F63" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="143"/>
+      <c r="G63" s="130"/>
       <c r="H63" s="85" t="s">
         <v>187</v>
       </c>
       <c r="I63" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="143" t="s">
+      <c r="J63" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="143"/>
+      <c r="K63" s="130"/>
       <c r="L63" s="85" t="s">
         <v>102</v>
       </c>
       <c r="M63" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="N63" s="85"/>
+      <c r="N63" s="85" t="s">
+        <v>293</v>
+      </c>
       <c r="O63" s="104" t="s">
         <v>108</v>
       </c>
@@ -7812,10 +7819,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="85"/>
-      <c r="U63" s="143" t="s">
+      <c r="U63" s="130" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="143"/>
+      <c r="V63" s="130"/>
       <c r="W63" s="85" t="s">
         <v>22</v>
       </c>
@@ -7829,7 +7836,7 @@
       <c r="AI63" s="80"/>
       <c r="AJ63" s="80"/>
     </row>
-    <row r="64" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A64" s="37"/>
       <c r="B64" s="37" t="s">
         <v>85</v>
@@ -7843,21 +7850,21 @@
       <c r="E64" s="96">
         <v>6</v>
       </c>
-      <c r="F64" s="144" t="s">
+      <c r="F64" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="144"/>
+      <c r="G64" s="145"/>
       <c r="H64" s="96">
         <v>1</v>
       </c>
       <c r="I64" s="96">
         <v>0</v>
       </c>
-      <c r="J64" s="135">
+      <c r="J64" s="133">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="135"/>
+      <c r="K64" s="133"/>
       <c r="L64" s="96">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>12</v>
@@ -7866,7 +7873,9 @@
         <f>21-L64</f>
         <v>9</v>
       </c>
-      <c r="N64" s="96"/>
+      <c r="N64" s="96">
+        <v>0.12</v>
+      </c>
       <c r="O64" s="98">
         <f t="shared" ref="O64:O70" si="33">ROUND(D64/health_cap,2)*10</f>
         <v>1.5</v>
@@ -7888,11 +7897,11 @@
         <v>9.5</v>
       </c>
       <c r="T64" s="96"/>
-      <c r="U64" s="146">
+      <c r="U64" s="131">
         <f>R64+O64+P64</f>
         <v>4.5</v>
       </c>
-      <c r="V64" s="146"/>
+      <c r="V64" s="131"/>
       <c r="W64" s="103" t="s">
         <v>29</v>
       </c>
@@ -7906,7 +7915,7 @@
       <c r="AI64" s="80"/>
       <c r="AJ64" s="80"/>
     </row>
-    <row r="65" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
         <v>86</v>
@@ -7920,21 +7929,21 @@
       <c r="E65" s="53">
         <v>4</v>
       </c>
-      <c r="F65" s="128" t="s">
+      <c r="F65" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="128"/>
+      <c r="G65" s="129"/>
       <c r="H65" s="53">
         <v>1</v>
       </c>
       <c r="I65" s="53">
         <v>0</v>
       </c>
-      <c r="J65" s="135">
+      <c r="J65" s="133">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="135"/>
+      <c r="K65" s="133"/>
       <c r="L65" s="53">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>3</v>
@@ -7943,7 +7952,9 @@
         <f t="shared" ref="M65:M68" si="37">21-L65</f>
         <v>18</v>
       </c>
-      <c r="N65" s="53"/>
+      <c r="N65" s="53">
+        <v>0.08</v>
+      </c>
       <c r="O65" s="65">
         <f t="shared" si="33"/>
         <v>4.5</v>
@@ -7965,11 +7976,11 @@
         <v>13.8</v>
       </c>
       <c r="T65" s="53"/>
-      <c r="U65" s="147">
+      <c r="U65" s="132">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
         <v>10.5</v>
       </c>
-      <c r="V65" s="147"/>
+      <c r="V65" s="132"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -7983,7 +7994,7 @@
       <c r="AI65" s="80"/>
       <c r="AJ65" s="80"/>
     </row>
-    <row r="66" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
         <v>87</v>
@@ -7997,21 +8008,21 @@
       <c r="E66" s="53">
         <v>3</v>
       </c>
-      <c r="F66" s="128" t="s">
+      <c r="F66" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="128"/>
+      <c r="G66" s="129"/>
       <c r="H66" s="53">
         <v>1</v>
       </c>
       <c r="I66" s="53">
         <v>11.11</v>
       </c>
-      <c r="J66" s="135">
+      <c r="J66" s="133">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="135"/>
+      <c r="K66" s="133"/>
       <c r="L66" s="53">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -8020,7 +8031,9 @@
         <f t="shared" si="37"/>
         <v>17</v>
       </c>
-      <c r="N66" s="53"/>
+      <c r="N66" s="53">
+        <v>0.1</v>
+      </c>
       <c r="O66" s="65">
         <f t="shared" si="33"/>
         <v>3</v>
@@ -8042,11 +8055,11 @@
         <v>13.399999999999999</v>
       </c>
       <c r="T66" s="53"/>
-      <c r="U66" s="147">
+      <c r="U66" s="132">
         <f t="shared" si="39"/>
         <v>10.899999999999999</v>
       </c>
-      <c r="V66" s="147"/>
+      <c r="V66" s="132"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -8060,7 +8073,7 @@
       <c r="AI66" s="80"/>
       <c r="AJ66" s="80"/>
     </row>
-    <row r="67" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A67" s="18"/>
       <c r="B67" s="18" t="s">
         <v>88</v>
@@ -8074,21 +8087,21 @@
       <c r="E67" s="53">
         <v>1</v>
       </c>
-      <c r="F67" s="128" t="s">
+      <c r="F67" s="129" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="128"/>
+      <c r="G67" s="129"/>
       <c r="H67" s="53">
         <v>1</v>
       </c>
       <c r="I67" s="53">
         <v>5.63</v>
       </c>
-      <c r="J67" s="135">
+      <c r="J67" s="133">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="135"/>
+      <c r="K67" s="133"/>
       <c r="L67" s="53">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -8097,7 +8110,9 @@
         <f t="shared" si="37"/>
         <v>21</v>
       </c>
-      <c r="N67" s="53"/>
+      <c r="N67" s="53">
+        <v>0.05</v>
+      </c>
       <c r="O67" s="65">
         <f t="shared" si="33"/>
         <v>9.6</v>
@@ -8119,11 +8134,11 @@
         <v>18.500000000000004</v>
       </c>
       <c r="T67" s="53"/>
-      <c r="U67" s="147">
+      <c r="U67" s="132">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="147"/>
+      <c r="V67" s="132"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -8133,7 +8148,7 @@
       <c r="Y67" s="56"/>
       <c r="Z67" s="56"/>
     </row>
-    <row r="68" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A68" s="18"/>
       <c r="B68" s="18" t="s">
         <v>93</v>
@@ -8147,21 +8162,21 @@
       <c r="E68" s="53">
         <v>0</v>
       </c>
-      <c r="F68" s="128" t="s">
+      <c r="F68" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="128"/>
+      <c r="G68" s="129"/>
       <c r="H68" s="53">
         <v>1</v>
       </c>
       <c r="I68" s="53">
         <v>13.33</v>
       </c>
-      <c r="J68" s="135">
+      <c r="J68" s="133">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="135"/>
+      <c r="K68" s="133"/>
       <c r="L68" s="53">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -8170,7 +8185,9 @@
         <f t="shared" si="37"/>
         <v>21</v>
       </c>
-      <c r="N68" s="53"/>
+      <c r="N68" s="53">
+        <v>0</v>
+      </c>
       <c r="O68" s="65">
         <f t="shared" si="33"/>
         <v>7.4</v>
@@ -8192,11 +8209,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="53"/>
-      <c r="U68" s="147">
+      <c r="U68" s="132">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="147"/>
+      <c r="V68" s="132"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -8206,7 +8223,7 @@
       <c r="Y68" s="56"/>
       <c r="Z68" s="56"/>
     </row>
-    <row r="69" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A69" s="18"/>
       <c r="B69" s="18" t="s">
         <v>104</v>
@@ -8220,21 +8237,21 @@
       <c r="E69" s="53">
         <v>12</v>
       </c>
-      <c r="F69" s="128" t="s">
+      <c r="F69" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="128"/>
+      <c r="G69" s="129"/>
       <c r="H69" s="53">
         <v>1</v>
       </c>
       <c r="I69" s="53">
         <v>9.09</v>
       </c>
-      <c r="J69" s="135">
+      <c r="J69" s="133">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="135"/>
+      <c r="K69" s="133"/>
       <c r="L69" s="53">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -8243,7 +8260,9 @@
         <f>21-L69</f>
         <v>15</v>
       </c>
-      <c r="N69" s="53"/>
+      <c r="N69" s="53">
+        <v>0.18</v>
+      </c>
       <c r="O69" s="65">
         <f t="shared" si="33"/>
         <v>2</v>
@@ -8265,11 +8284,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="53"/>
-      <c r="U69" s="147">
+      <c r="U69" s="132">
         <f t="shared" si="39"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="147"/>
+      <c r="V69" s="132"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -8279,7 +8298,7 @@
       <c r="Y69" s="56"/>
       <c r="Z69" s="56"/>
     </row>
-    <row r="70" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A70" s="18"/>
       <c r="B70" s="18" t="s">
         <v>115</v>
@@ -8293,21 +8312,21 @@
       <c r="E70" s="53">
         <v>10</v>
       </c>
-      <c r="F70" s="128" t="s">
+      <c r="F70" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="128"/>
+      <c r="G70" s="129"/>
       <c r="H70" s="53">
         <v>1</v>
       </c>
       <c r="I70" s="53">
         <v>48</v>
       </c>
-      <c r="J70" s="135">
+      <c r="J70" s="133">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="135"/>
+      <c r="K70" s="133"/>
       <c r="L70" s="53">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -8316,7 +8335,9 @@
         <f>21-L70</f>
         <v>17</v>
       </c>
-      <c r="N70" s="53"/>
+      <c r="N70" s="53">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="O70" s="65">
         <f t="shared" si="33"/>
         <v>2.5</v>
@@ -8338,11 +8359,11 @@
         <v>26.1</v>
       </c>
       <c r="T70" s="53"/>
-      <c r="U70" s="147">
+      <c r="U70" s="132">
         <f t="shared" si="39"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="147"/>
+      <c r="V70" s="132"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -8352,20 +8373,20 @@
       <c r="Y70" s="56"/>
       <c r="Z70" s="56"/>
     </row>
-    <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="72" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="73" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B73" s="116" t="s">
         <v>238</v>
       </c>
-      <c r="O73" s="141" t="s">
+      <c r="O73" s="135" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="141"/>
-      <c r="Q73" s="141"/>
-      <c r="R73" s="141"/>
-    </row>
-    <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="P73" s="135"/>
+      <c r="Q73" s="135"/>
+      <c r="R73" s="135"/>
+    </row>
+    <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
       <c r="B74" s="76" t="s">
         <v>129</v>
@@ -8379,36 +8400,36 @@
       <c r="E74" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="131" t="s">
+      <c r="F74" s="134" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="131"/>
-      <c r="H74" s="131" t="s">
+      <c r="G74" s="134"/>
+      <c r="H74" s="134" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="131"/>
-      <c r="J74" s="131" t="s">
+      <c r="I74" s="134"/>
+      <c r="J74" s="134" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="131"/>
-      <c r="L74" s="131"/>
-      <c r="M74" s="131"/>
+      <c r="K74" s="134"/>
+      <c r="L74" s="134"/>
+      <c r="M74" s="134"/>
       <c r="N74" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="131" t="s">
+      <c r="O74" s="134" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="131"/>
-      <c r="Q74" s="131" t="s">
+      <c r="P74" s="134"/>
+      <c r="Q74" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="131"/>
+      <c r="R74" s="134"/>
       <c r="S74" s="120" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A75" s="37" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
@@ -8424,21 +8445,21 @@
       <c r="E75" s="53">
         <v>18</v>
       </c>
-      <c r="F75" s="135" t="s">
+      <c r="F75" s="133" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="135"/>
-      <c r="H75" s="135">
+      <c r="G75" s="133"/>
+      <c r="H75" s="133">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="135"/>
-      <c r="J75" s="135" t="s">
+      <c r="I75" s="133"/>
+      <c r="J75" s="133" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="135"/>
-      <c r="L75" s="135"/>
-      <c r="M75" s="135"/>
+      <c r="K75" s="133"/>
+      <c r="L75" s="133"/>
+      <c r="M75" s="133"/>
       <c r="N75" s="77" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -8458,7 +8479,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A76" s="37" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
@@ -8474,21 +8495,21 @@
       <c r="E76" s="53">
         <v>12</v>
       </c>
-      <c r="F76" s="135" t="s">
+      <c r="F76" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="135"/>
-      <c r="H76" s="135">
+      <c r="G76" s="133"/>
+      <c r="H76" s="133">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="135"/>
-      <c r="J76" s="135" t="s">
+      <c r="I76" s="133"/>
+      <c r="J76" s="133" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="135"/>
-      <c r="L76" s="135"/>
-      <c r="M76" s="135"/>
+      <c r="K76" s="133"/>
+      <c r="L76" s="133"/>
+      <c r="M76" s="133"/>
       <c r="N76" s="77" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
@@ -8508,28 +8529,28 @@
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A77" s="18"/>
       <c r="B77" s="18"/>
       <c r="C77" s="43"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
-      <c r="F77" s="130"/>
-      <c r="G77" s="130"/>
-      <c r="H77" s="130"/>
-      <c r="I77" s="130"/>
-      <c r="J77" s="130"/>
-      <c r="K77" s="130"/>
-      <c r="L77" s="130"/>
-      <c r="M77" s="130"/>
+      <c r="F77" s="139"/>
+      <c r="G77" s="139"/>
+      <c r="H77" s="139"/>
+      <c r="I77" s="139"/>
+      <c r="J77" s="139"/>
+      <c r="K77" s="139"/>
+      <c r="L77" s="139"/>
+      <c r="M77" s="139"/>
       <c r="N77" s="93"/>
-      <c r="O77" s="126"/>
-      <c r="P77" s="126"/>
-      <c r="Q77" s="126"/>
-      <c r="R77" s="126"/>
+      <c r="O77" s="143"/>
+      <c r="P77" s="143"/>
+      <c r="Q77" s="143"/>
+      <c r="R77" s="143"/>
       <c r="S77" s="64"/>
     </row>
-    <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="111" t="s">
         <v>198</v>
       </c>
@@ -8537,9 +8558,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="81" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A81" s="34" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
@@ -8555,37 +8576,37 @@
       <c r="E81" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="131" t="s">
+      <c r="F81" s="134" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="131"/>
-      <c r="H81" s="131"/>
-      <c r="I81" s="131"/>
-      <c r="J81" s="131"/>
-      <c r="K81" s="131"/>
-      <c r="L81" s="131"/>
-      <c r="M81" s="131"/>
-      <c r="N81" s="131"/>
-      <c r="O81" s="131"/>
-      <c r="P81" s="131"/>
-      <c r="Q81" s="131" t="s">
+      <c r="G81" s="134"/>
+      <c r="H81" s="134"/>
+      <c r="I81" s="134"/>
+      <c r="J81" s="134"/>
+      <c r="K81" s="134"/>
+      <c r="L81" s="134"/>
+      <c r="M81" s="134"/>
+      <c r="N81" s="134"/>
+      <c r="O81" s="134"/>
+      <c r="P81" s="134"/>
+      <c r="Q81" s="134" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="131"/>
-      <c r="S81" s="131"/>
-      <c r="T81" s="131"/>
-      <c r="U81" s="131"/>
-      <c r="V81" s="131"/>
-      <c r="W81" s="131"/>
-      <c r="X81" s="131"/>
-      <c r="Y81" s="131"/>
-      <c r="Z81" s="131"/>
-      <c r="AA81" s="131"/>
+      <c r="R81" s="134"/>
+      <c r="S81" s="134"/>
+      <c r="T81" s="134"/>
+      <c r="U81" s="134"/>
+      <c r="V81" s="134"/>
+      <c r="W81" s="134"/>
+      <c r="X81" s="134"/>
+      <c r="Y81" s="134"/>
+      <c r="Z81" s="134"/>
+      <c r="AA81" s="134"/>
       <c r="AB81" s="120" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="37"/>
       <c r="B82" s="37" t="s">
         <v>146</v>
@@ -8599,37 +8620,37 @@
       <c r="E82" s="96">
         <v>16</v>
       </c>
-      <c r="F82" s="132" t="s">
+      <c r="F82" s="147" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="132"/>
-      <c r="H82" s="132"/>
-      <c r="I82" s="132"/>
-      <c r="J82" s="132"/>
-      <c r="K82" s="132"/>
-      <c r="L82" s="132"/>
-      <c r="M82" s="132"/>
-      <c r="N82" s="132"/>
-      <c r="O82" s="132"/>
-      <c r="P82" s="132"/>
-      <c r="Q82" s="132" t="s">
+      <c r="G82" s="147"/>
+      <c r="H82" s="147"/>
+      <c r="I82" s="147"/>
+      <c r="J82" s="147"/>
+      <c r="K82" s="147"/>
+      <c r="L82" s="147"/>
+      <c r="M82" s="147"/>
+      <c r="N82" s="147"/>
+      <c r="O82" s="147"/>
+      <c r="P82" s="147"/>
+      <c r="Q82" s="147" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="132"/>
-      <c r="S82" s="132"/>
-      <c r="T82" s="132"/>
-      <c r="U82" s="132"/>
-      <c r="V82" s="132"/>
-      <c r="W82" s="132"/>
-      <c r="X82" s="132"/>
-      <c r="Y82" s="132"/>
-      <c r="Z82" s="132"/>
-      <c r="AA82" s="132"/>
+      <c r="R82" s="147"/>
+      <c r="S82" s="147"/>
+      <c r="T82" s="147"/>
+      <c r="U82" s="147"/>
+      <c r="V82" s="147"/>
+      <c r="W82" s="147"/>
+      <c r="X82" s="147"/>
+      <c r="Y82" s="147"/>
+      <c r="Z82" s="147"/>
+      <c r="AA82" s="147"/>
       <c r="AB82" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="37"/>
       <c r="B83" s="37" t="s">
         <v>147</v>
@@ -8643,35 +8664,35 @@
       <c r="E83" s="53">
         <v>1</v>
       </c>
-      <c r="F83" s="133" t="s">
+      <c r="F83" s="140" t="s">
         <v>224</v>
       </c>
-      <c r="G83" s="133"/>
-      <c r="H83" s="133"/>
-      <c r="I83" s="133"/>
-      <c r="J83" s="133"/>
-      <c r="K83" s="133"/>
-      <c r="L83" s="133"/>
-      <c r="M83" s="133"/>
-      <c r="N83" s="133"/>
-      <c r="O83" s="133"/>
-      <c r="P83" s="133"/>
-      <c r="Q83" s="133"/>
-      <c r="R83" s="133"/>
-      <c r="S83" s="133"/>
-      <c r="T83" s="133"/>
-      <c r="U83" s="133"/>
-      <c r="V83" s="133"/>
-      <c r="W83" s="133"/>
-      <c r="X83" s="133"/>
-      <c r="Y83" s="133"/>
-      <c r="Z83" s="133"/>
-      <c r="AA83" s="133"/>
+      <c r="G83" s="140"/>
+      <c r="H83" s="140"/>
+      <c r="I83" s="140"/>
+      <c r="J83" s="140"/>
+      <c r="K83" s="140"/>
+      <c r="L83" s="140"/>
+      <c r="M83" s="140"/>
+      <c r="N83" s="140"/>
+      <c r="O83" s="140"/>
+      <c r="P83" s="140"/>
+      <c r="Q83" s="140"/>
+      <c r="R83" s="140"/>
+      <c r="S83" s="140"/>
+      <c r="T83" s="140"/>
+      <c r="U83" s="140"/>
+      <c r="V83" s="140"/>
+      <c r="W83" s="140"/>
+      <c r="X83" s="140"/>
+      <c r="Y83" s="140"/>
+      <c r="Z83" s="140"/>
+      <c r="AA83" s="140"/>
       <c r="AB83" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A84" s="37"/>
       <c r="B84" s="37" t="s">
         <v>148</v>
@@ -8685,35 +8706,35 @@
       <c r="E84" s="53">
         <v>1</v>
       </c>
-      <c r="F84" s="133" t="s">
+      <c r="F84" s="140" t="s">
         <v>225</v>
       </c>
-      <c r="G84" s="133"/>
-      <c r="H84" s="133"/>
-      <c r="I84" s="133"/>
-      <c r="J84" s="133"/>
-      <c r="K84" s="133"/>
-      <c r="L84" s="133"/>
-      <c r="M84" s="133"/>
-      <c r="N84" s="133"/>
-      <c r="O84" s="133"/>
-      <c r="P84" s="133"/>
-      <c r="Q84" s="133"/>
-      <c r="R84" s="133"/>
-      <c r="S84" s="133"/>
-      <c r="T84" s="133"/>
-      <c r="U84" s="133"/>
-      <c r="V84" s="133"/>
-      <c r="W84" s="133"/>
-      <c r="X84" s="133"/>
-      <c r="Y84" s="133"/>
-      <c r="Z84" s="133"/>
-      <c r="AA84" s="133"/>
+      <c r="G84" s="140"/>
+      <c r="H84" s="140"/>
+      <c r="I84" s="140"/>
+      <c r="J84" s="140"/>
+      <c r="K84" s="140"/>
+      <c r="L84" s="140"/>
+      <c r="M84" s="140"/>
+      <c r="N84" s="140"/>
+      <c r="O84" s="140"/>
+      <c r="P84" s="140"/>
+      <c r="Q84" s="140"/>
+      <c r="R84" s="140"/>
+      <c r="S84" s="140"/>
+      <c r="T84" s="140"/>
+      <c r="U84" s="140"/>
+      <c r="V84" s="140"/>
+      <c r="W84" s="140"/>
+      <c r="X84" s="140"/>
+      <c r="Y84" s="140"/>
+      <c r="Z84" s="140"/>
+      <c r="AA84" s="140"/>
       <c r="AB84" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A85" s="37"/>
       <c r="B85" s="37" t="s">
         <v>149</v>
@@ -8727,37 +8748,37 @@
       <c r="E85" s="53">
         <v>1</v>
       </c>
-      <c r="F85" s="133" t="s">
+      <c r="F85" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="133"/>
-      <c r="H85" s="133"/>
-      <c r="I85" s="133"/>
-      <c r="J85" s="133"/>
-      <c r="K85" s="133"/>
-      <c r="L85" s="133"/>
-      <c r="M85" s="133"/>
-      <c r="N85" s="133"/>
-      <c r="O85" s="133"/>
-      <c r="P85" s="133"/>
-      <c r="Q85" s="133" t="s">
+      <c r="G85" s="140"/>
+      <c r="H85" s="140"/>
+      <c r="I85" s="140"/>
+      <c r="J85" s="140"/>
+      <c r="K85" s="140"/>
+      <c r="L85" s="140"/>
+      <c r="M85" s="140"/>
+      <c r="N85" s="140"/>
+      <c r="O85" s="140"/>
+      <c r="P85" s="140"/>
+      <c r="Q85" s="140" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="133"/>
-      <c r="S85" s="133"/>
-      <c r="T85" s="133"/>
-      <c r="U85" s="133"/>
-      <c r="V85" s="133"/>
-      <c r="W85" s="133"/>
-      <c r="X85" s="133"/>
-      <c r="Y85" s="133"/>
-      <c r="Z85" s="133"/>
-      <c r="AA85" s="133"/>
+      <c r="R85" s="140"/>
+      <c r="S85" s="140"/>
+      <c r="T85" s="140"/>
+      <c r="U85" s="140"/>
+      <c r="V85" s="140"/>
+      <c r="W85" s="140"/>
+      <c r="X85" s="140"/>
+      <c r="Y85" s="140"/>
+      <c r="Z85" s="140"/>
+      <c r="AA85" s="140"/>
       <c r="AB85" s="64" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="37"/>
       <c r="B86" s="37" t="s">
         <v>200</v>
@@ -8771,37 +8792,37 @@
       <c r="E86" s="53">
         <v>5</v>
       </c>
-      <c r="F86" s="133" t="s">
+      <c r="F86" s="140" t="s">
         <v>256</v>
       </c>
-      <c r="G86" s="133"/>
-      <c r="H86" s="133"/>
-      <c r="I86" s="133"/>
-      <c r="J86" s="133"/>
-      <c r="K86" s="133"/>
-      <c r="L86" s="133"/>
-      <c r="M86" s="133"/>
-      <c r="N86" s="133"/>
-      <c r="O86" s="133"/>
-      <c r="P86" s="133"/>
-      <c r="Q86" s="133" t="s">
+      <c r="G86" s="140"/>
+      <c r="H86" s="140"/>
+      <c r="I86" s="140"/>
+      <c r="J86" s="140"/>
+      <c r="K86" s="140"/>
+      <c r="L86" s="140"/>
+      <c r="M86" s="140"/>
+      <c r="N86" s="140"/>
+      <c r="O86" s="140"/>
+      <c r="P86" s="140"/>
+      <c r="Q86" s="140" t="s">
         <v>257</v>
       </c>
-      <c r="R86" s="133"/>
-      <c r="S86" s="133"/>
-      <c r="T86" s="133"/>
-      <c r="U86" s="133"/>
-      <c r="V86" s="133"/>
-      <c r="W86" s="133"/>
-      <c r="X86" s="133"/>
-      <c r="Y86" s="133"/>
-      <c r="Z86" s="133"/>
-      <c r="AA86" s="133"/>
+      <c r="R86" s="140"/>
+      <c r="S86" s="140"/>
+      <c r="T86" s="140"/>
+      <c r="U86" s="140"/>
+      <c r="V86" s="140"/>
+      <c r="W86" s="140"/>
+      <c r="X86" s="140"/>
+      <c r="Y86" s="140"/>
+      <c r="Z86" s="140"/>
+      <c r="AA86" s="140"/>
       <c r="AB86" s="64" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="37"/>
       <c r="B87" s="37" t="s">
         <v>274</v>
@@ -8815,438 +8836,438 @@
       <c r="E87" s="53">
         <v>1</v>
       </c>
-      <c r="F87" s="133" t="s">
+      <c r="F87" s="140" t="s">
         <v>276</v>
       </c>
-      <c r="G87" s="133"/>
-      <c r="H87" s="133"/>
-      <c r="I87" s="133"/>
-      <c r="J87" s="133"/>
-      <c r="K87" s="133"/>
-      <c r="L87" s="133"/>
-      <c r="M87" s="133"/>
-      <c r="N87" s="133"/>
-      <c r="O87" s="133"/>
-      <c r="P87" s="133"/>
-      <c r="Q87" s="133" t="s">
+      <c r="G87" s="140"/>
+      <c r="H87" s="140"/>
+      <c r="I87" s="140"/>
+      <c r="J87" s="140"/>
+      <c r="K87" s="140"/>
+      <c r="L87" s="140"/>
+      <c r="M87" s="140"/>
+      <c r="N87" s="140"/>
+      <c r="O87" s="140"/>
+      <c r="P87" s="140"/>
+      <c r="Q87" s="140" t="s">
         <v>275</v>
       </c>
-      <c r="R87" s="133"/>
-      <c r="S87" s="133"/>
-      <c r="T87" s="133"/>
-      <c r="U87" s="133"/>
-      <c r="V87" s="133"/>
-      <c r="W87" s="133"/>
-      <c r="X87" s="133"/>
-      <c r="Y87" s="133"/>
-      <c r="Z87" s="133"/>
-      <c r="AA87" s="133"/>
+      <c r="R87" s="140"/>
+      <c r="S87" s="140"/>
+      <c r="T87" s="140"/>
+      <c r="U87" s="140"/>
+      <c r="V87" s="140"/>
+      <c r="W87" s="140"/>
+      <c r="X87" s="140"/>
+      <c r="Y87" s="140"/>
+      <c r="Z87" s="140"/>
+      <c r="AA87" s="140"/>
       <c r="AB87" s="64" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B88" s="57" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="90" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="34"/>
       <c r="B90" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="129" t="s">
+      <c r="C90" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="129"/>
-      <c r="E90" s="129"/>
-      <c r="F90" s="129"/>
-      <c r="G90" s="129"/>
-      <c r="H90" s="129" t="s">
+      <c r="D90" s="144"/>
+      <c r="E90" s="144"/>
+      <c r="F90" s="144"/>
+      <c r="G90" s="144"/>
+      <c r="H90" s="144" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="129"/>
-      <c r="J90" s="129"/>
-      <c r="K90" s="129"/>
-      <c r="L90" s="129"/>
-      <c r="M90" s="131" t="s">
+      <c r="I90" s="144"/>
+      <c r="J90" s="144"/>
+      <c r="K90" s="144"/>
+      <c r="L90" s="144"/>
+      <c r="M90" s="134" t="s">
         <v>185</v>
       </c>
-      <c r="N90" s="131"/>
+      <c r="N90" s="134"/>
       <c r="O90" s="106"/>
       <c r="T90" s="57" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A91" s="37" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="127" t="s">
+      <c r="C91" s="128" t="s">
         <v>180</v>
       </c>
-      <c r="D91" s="127"/>
-      <c r="E91" s="127"/>
-      <c r="F91" s="127"/>
-      <c r="G91" s="127"/>
-      <c r="H91" s="127" t="s">
+      <c r="D91" s="128"/>
+      <c r="E91" s="128"/>
+      <c r="F91" s="128"/>
+      <c r="G91" s="128"/>
+      <c r="H91" s="128" t="s">
         <v>182</v>
       </c>
-      <c r="I91" s="127"/>
-      <c r="J91" s="127"/>
-      <c r="K91" s="127"/>
-      <c r="L91" s="127"/>
-      <c r="M91" s="128" t="s">
+      <c r="I91" s="128"/>
+      <c r="J91" s="128"/>
+      <c r="K91" s="128"/>
+      <c r="L91" s="128"/>
+      <c r="M91" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N91" s="128"/>
+      <c r="N91" s="129"/>
       <c r="O91" s="64"/>
     </row>
-    <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A92" s="37" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="127" t="s">
+      <c r="C92" s="128" t="s">
         <v>183</v>
       </c>
-      <c r="D92" s="127"/>
-      <c r="E92" s="127"/>
-      <c r="F92" s="127"/>
-      <c r="G92" s="127"/>
-      <c r="H92" s="127" t="s">
+      <c r="D92" s="128"/>
+      <c r="E92" s="128"/>
+      <c r="F92" s="128"/>
+      <c r="G92" s="128"/>
+      <c r="H92" s="128" t="s">
         <v>184</v>
       </c>
-      <c r="I92" s="127"/>
-      <c r="J92" s="127"/>
-      <c r="K92" s="127"/>
-      <c r="L92" s="127"/>
-      <c r="M92" s="128" t="s">
+      <c r="I92" s="128"/>
+      <c r="J92" s="128"/>
+      <c r="K92" s="128"/>
+      <c r="L92" s="128"/>
+      <c r="M92" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N92" s="128"/>
+      <c r="N92" s="129"/>
       <c r="O92" s="64"/>
     </row>
-    <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A93" s="37" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="127" t="s">
+      <c r="C93" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D93" s="127"/>
-      <c r="E93" s="127"/>
-      <c r="F93" s="127"/>
-      <c r="G93" s="127"/>
-      <c r="H93" s="127" t="s">
+      <c r="D93" s="128"/>
+      <c r="E93" s="128"/>
+      <c r="F93" s="128"/>
+      <c r="G93" s="128"/>
+      <c r="H93" s="128" t="s">
         <v>181</v>
       </c>
-      <c r="I93" s="127"/>
-      <c r="J93" s="127"/>
-      <c r="K93" s="127"/>
-      <c r="L93" s="127"/>
-      <c r="M93" s="128" t="s">
+      <c r="I93" s="128"/>
+      <c r="J93" s="128"/>
+      <c r="K93" s="128"/>
+      <c r="L93" s="128"/>
+      <c r="M93" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N93" s="128"/>
+      <c r="N93" s="129"/>
       <c r="O93" s="64"/>
     </row>
-    <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A94" s="37" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="C94" s="127" t="s">
+      <c r="C94" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D94" s="127"/>
-      <c r="E94" s="127"/>
-      <c r="F94" s="127"/>
-      <c r="G94" s="127"/>
-      <c r="H94" s="127" t="s">
+      <c r="D94" s="128"/>
+      <c r="E94" s="128"/>
+      <c r="F94" s="128"/>
+      <c r="G94" s="128"/>
+      <c r="H94" s="128" t="s">
         <v>216</v>
       </c>
-      <c r="I94" s="127"/>
-      <c r="J94" s="127"/>
-      <c r="K94" s="127"/>
-      <c r="L94" s="127"/>
-      <c r="M94" s="128" t="s">
+      <c r="I94" s="128"/>
+      <c r="J94" s="128"/>
+      <c r="K94" s="128"/>
+      <c r="L94" s="128"/>
+      <c r="M94" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N94" s="128"/>
+      <c r="N94" s="129"/>
       <c r="O94" s="64"/>
     </row>
-    <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A95" s="37" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C95" s="127" t="s">
+      <c r="C95" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D95" s="127"/>
-      <c r="E95" s="127"/>
-      <c r="F95" s="127"/>
-      <c r="G95" s="127"/>
-      <c r="H95" s="127" t="s">
+      <c r="D95" s="128"/>
+      <c r="E95" s="128"/>
+      <c r="F95" s="128"/>
+      <c r="G95" s="128"/>
+      <c r="H95" s="128" t="s">
         <v>217</v>
       </c>
-      <c r="I95" s="127"/>
-      <c r="J95" s="127"/>
-      <c r="K95" s="127"/>
-      <c r="L95" s="127"/>
-      <c r="M95" s="128" t="s">
+      <c r="I95" s="128"/>
+      <c r="J95" s="128"/>
+      <c r="K95" s="128"/>
+      <c r="L95" s="128"/>
+      <c r="M95" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N95" s="128"/>
+      <c r="N95" s="129"/>
       <c r="O95" s="64"/>
     </row>
-    <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A96" s="37" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C96" s="127" t="s">
+      <c r="C96" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D96" s="127"/>
-      <c r="E96" s="127"/>
-      <c r="F96" s="127"/>
-      <c r="G96" s="127"/>
-      <c r="H96" s="127" t="s">
+      <c r="D96" s="128"/>
+      <c r="E96" s="128"/>
+      <c r="F96" s="128"/>
+      <c r="G96" s="128"/>
+      <c r="H96" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="I96" s="127"/>
-      <c r="J96" s="127"/>
-      <c r="K96" s="127"/>
-      <c r="L96" s="127"/>
-      <c r="M96" s="128" t="s">
+      <c r="I96" s="128"/>
+      <c r="J96" s="128"/>
+      <c r="K96" s="128"/>
+      <c r="L96" s="128"/>
+      <c r="M96" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N96" s="128"/>
+      <c r="N96" s="129"/>
       <c r="O96" s="64"/>
     </row>
-    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A97" s="37" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C97" s="127" t="s">
+      <c r="C97" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D97" s="127"/>
-      <c r="E97" s="127"/>
-      <c r="F97" s="127"/>
-      <c r="G97" s="127"/>
-      <c r="H97" s="127" t="s">
+      <c r="D97" s="128"/>
+      <c r="E97" s="128"/>
+      <c r="F97" s="128"/>
+      <c r="G97" s="128"/>
+      <c r="H97" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="I97" s="127"/>
-      <c r="J97" s="127"/>
-      <c r="K97" s="127"/>
-      <c r="L97" s="127"/>
-      <c r="M97" s="128" t="s">
+      <c r="I97" s="128"/>
+      <c r="J97" s="128"/>
+      <c r="K97" s="128"/>
+      <c r="L97" s="128"/>
+      <c r="M97" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N97" s="128"/>
+      <c r="N97" s="129"/>
       <c r="O97" s="64"/>
     </row>
-    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A98" s="37" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C98" s="127" t="s">
+      <c r="C98" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D98" s="127"/>
-      <c r="E98" s="127"/>
-      <c r="F98" s="127"/>
-      <c r="G98" s="127"/>
-      <c r="H98" s="127" t="s">
+      <c r="D98" s="128"/>
+      <c r="E98" s="128"/>
+      <c r="F98" s="128"/>
+      <c r="G98" s="128"/>
+      <c r="H98" s="128" t="s">
         <v>220</v>
       </c>
-      <c r="I98" s="127"/>
-      <c r="J98" s="127"/>
-      <c r="K98" s="127"/>
-      <c r="L98" s="127"/>
-      <c r="M98" s="128" t="s">
+      <c r="I98" s="128"/>
+      <c r="J98" s="128"/>
+      <c r="K98" s="128"/>
+      <c r="L98" s="128"/>
+      <c r="M98" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N98" s="128"/>
+      <c r="N98" s="129"/>
       <c r="O98" s="64"/>
     </row>
-    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A99" s="37" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C99" s="127" t="s">
+      <c r="C99" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D99" s="127"/>
-      <c r="E99" s="127"/>
-      <c r="F99" s="127"/>
-      <c r="G99" s="127"/>
-      <c r="H99" s="127" t="s">
+      <c r="D99" s="128"/>
+      <c r="E99" s="128"/>
+      <c r="F99" s="128"/>
+      <c r="G99" s="128"/>
+      <c r="H99" s="128" t="s">
         <v>221</v>
       </c>
-      <c r="I99" s="127"/>
-      <c r="J99" s="127"/>
-      <c r="K99" s="127"/>
-      <c r="L99" s="127"/>
-      <c r="M99" s="128" t="s">
+      <c r="I99" s="128"/>
+      <c r="J99" s="128"/>
+      <c r="K99" s="128"/>
+      <c r="L99" s="128"/>
+      <c r="M99" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N99" s="128"/>
+      <c r="N99" s="129"/>
       <c r="O99" s="64"/>
     </row>
-    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A100" s="37" t="e" vm="54">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C100" s="127" t="s">
+      <c r="C100" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D100" s="127"/>
-      <c r="E100" s="127"/>
-      <c r="F100" s="127"/>
-      <c r="G100" s="127"/>
-      <c r="H100" s="127" t="s">
+      <c r="D100" s="128"/>
+      <c r="E100" s="128"/>
+      <c r="F100" s="128"/>
+      <c r="G100" s="128"/>
+      <c r="H100" s="128" t="s">
         <v>222</v>
       </c>
-      <c r="I100" s="127"/>
-      <c r="J100" s="127"/>
-      <c r="K100" s="127"/>
-      <c r="L100" s="127"/>
-      <c r="M100" s="128" t="s">
+      <c r="I100" s="128"/>
+      <c r="J100" s="128"/>
+      <c r="K100" s="128"/>
+      <c r="L100" s="128"/>
+      <c r="M100" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="N100" s="128"/>
+      <c r="N100" s="129"/>
       <c r="O100" s="64"/>
     </row>
-    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="127"/>
-      <c r="D101" s="127"/>
-      <c r="E101" s="127"/>
-      <c r="F101" s="127"/>
-      <c r="G101" s="127"/>
-      <c r="H101" s="127"/>
-      <c r="I101" s="127"/>
-      <c r="J101" s="127"/>
-      <c r="K101" s="127"/>
-      <c r="L101" s="127"/>
-      <c r="M101" s="128"/>
-      <c r="N101" s="128"/>
+      <c r="C101" s="128"/>
+      <c r="D101" s="128"/>
+      <c r="E101" s="128"/>
+      <c r="F101" s="128"/>
+      <c r="G101" s="128"/>
+      <c r="H101" s="128"/>
+      <c r="I101" s="128"/>
+      <c r="J101" s="128"/>
+      <c r="K101" s="128"/>
+      <c r="L101" s="128"/>
+      <c r="M101" s="129"/>
+      <c r="N101" s="129"/>
       <c r="O101" s="64"/>
     </row>
-    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="127"/>
-      <c r="I102" s="127"/>
-      <c r="J102" s="127"/>
-      <c r="K102" s="127"/>
-      <c r="L102" s="127"/>
-      <c r="M102" s="128"/>
-      <c r="N102" s="128"/>
+      <c r="H102" s="128"/>
+      <c r="I102" s="128"/>
+      <c r="J102" s="128"/>
+      <c r="K102" s="128"/>
+      <c r="L102" s="128"/>
+      <c r="M102" s="129"/>
+      <c r="N102" s="129"/>
       <c r="O102" s="64"/>
     </row>
-    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="127"/>
-      <c r="D103" s="127"/>
-      <c r="E103" s="127"/>
-      <c r="F103" s="127"/>
-      <c r="G103" s="127"/>
-      <c r="H103" s="127"/>
-      <c r="I103" s="127"/>
-      <c r="J103" s="127"/>
-      <c r="K103" s="127"/>
-      <c r="L103" s="127"/>
-      <c r="M103" s="128"/>
-      <c r="N103" s="128"/>
+      <c r="C103" s="128"/>
+      <c r="D103" s="128"/>
+      <c r="E103" s="128"/>
+      <c r="F103" s="128"/>
+      <c r="G103" s="128"/>
+      <c r="H103" s="128"/>
+      <c r="I103" s="128"/>
+      <c r="J103" s="128"/>
+      <c r="K103" s="128"/>
+      <c r="L103" s="128"/>
+      <c r="M103" s="129"/>
+      <c r="N103" s="129"/>
       <c r="O103" s="64"/>
     </row>
-    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="127"/>
-      <c r="D104" s="127"/>
-      <c r="E104" s="127"/>
-      <c r="F104" s="127"/>
-      <c r="G104" s="127"/>
-      <c r="H104" s="127"/>
-      <c r="I104" s="127"/>
-      <c r="J104" s="127"/>
-      <c r="K104" s="127"/>
-      <c r="L104" s="127"/>
-      <c r="M104" s="128"/>
-      <c r="N104" s="128"/>
+      <c r="C104" s="128"/>
+      <c r="D104" s="128"/>
+      <c r="E104" s="128"/>
+      <c r="F104" s="128"/>
+      <c r="G104" s="128"/>
+      <c r="H104" s="128"/>
+      <c r="I104" s="128"/>
+      <c r="J104" s="128"/>
+      <c r="K104" s="128"/>
+      <c r="L104" s="128"/>
+      <c r="M104" s="129"/>
+      <c r="N104" s="129"/>
       <c r="O104" s="64"/>
     </row>
-    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="127"/>
-      <c r="D105" s="127"/>
-      <c r="E105" s="127"/>
-      <c r="F105" s="127"/>
-      <c r="G105" s="127"/>
-      <c r="H105" s="127"/>
-      <c r="I105" s="127"/>
-      <c r="J105" s="127"/>
-      <c r="K105" s="127"/>
-      <c r="L105" s="127"/>
-      <c r="M105" s="128"/>
-      <c r="N105" s="128"/>
+      <c r="C105" s="128"/>
+      <c r="D105" s="128"/>
+      <c r="E105" s="128"/>
+      <c r="F105" s="128"/>
+      <c r="G105" s="128"/>
+      <c r="H105" s="128"/>
+      <c r="I105" s="128"/>
+      <c r="J105" s="128"/>
+      <c r="K105" s="128"/>
+      <c r="L105" s="128"/>
+      <c r="M105" s="129"/>
+      <c r="N105" s="129"/>
       <c r="O105" s="64"/>
     </row>
-    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="127"/>
-      <c r="D106" s="127"/>
-      <c r="E106" s="127"/>
-      <c r="F106" s="127"/>
-      <c r="G106" s="127"/>
-      <c r="H106" s="127"/>
-      <c r="I106" s="127"/>
-      <c r="J106" s="127"/>
-      <c r="K106" s="127"/>
-      <c r="L106" s="127"/>
-      <c r="M106" s="128"/>
-      <c r="N106" s="128"/>
+      <c r="C106" s="128"/>
+      <c r="D106" s="128"/>
+      <c r="E106" s="128"/>
+      <c r="F106" s="128"/>
+      <c r="G106" s="128"/>
+      <c r="H106" s="128"/>
+      <c r="I106" s="128"/>
+      <c r="J106" s="128"/>
+      <c r="K106" s="128"/>
+      <c r="L106" s="128"/>
+      <c r="M106" s="129"/>
+      <c r="N106" s="129"/>
       <c r="O106" s="64"/>
     </row>
-    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A107" s="81"/>
       <c r="B107" s="113" t="s">
         <v>233</v>
@@ -9265,7 +9286,7 @@
       <c r="N107" s="81"/>
       <c r="O107" s="81"/>
     </row>
-    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A108" s="37"/>
       <c r="B108" s="118" t="s">
         <v>234</v>
@@ -9286,7 +9307,7 @@
       <c r="N108" s="64"/>
       <c r="O108" s="64"/>
     </row>
-    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A109" s="37"/>
       <c r="B109" s="118"/>
       <c r="C109" s="115" t="s">
@@ -9305,7 +9326,7 @@
       <c r="N109" s="64"/>
       <c r="O109" s="64"/>
     </row>
-    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A110" s="37"/>
       <c r="B110" s="118"/>
       <c r="C110" s="115" t="s">
@@ -9324,7 +9345,7 @@
       <c r="N110" s="64"/>
       <c r="O110" s="64"/>
     </row>
-    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A111" s="37"/>
       <c r="B111" s="118"/>
       <c r="C111" s="115" t="s">
@@ -9343,7 +9364,7 @@
       <c r="N111" s="64"/>
       <c r="O111" s="64"/>
     </row>
-    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A112" s="37"/>
       <c r="B112" s="118"/>
       <c r="C112" s="115"/>
@@ -9360,7 +9381,7 @@
       <c r="N112" s="64"/>
       <c r="O112" s="64"/>
     </row>
-    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="37"/>
       <c r="B113" s="118" t="s">
         <v>237</v>
@@ -9381,7 +9402,7 @@
       <c r="N113" s="64"/>
       <c r="O113" s="64"/>
     </row>
-    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="37"/>
       <c r="B114" s="118"/>
       <c r="C114" s="115" t="s">
@@ -9400,7 +9421,7 @@
       <c r="N114" s="64"/>
       <c r="O114" s="64"/>
     </row>
-    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="37"/>
       <c r="B115" s="118"/>
       <c r="C115" s="115"/>
@@ -9417,7 +9438,7 @@
       <c r="N115" s="64"/>
       <c r="O115" s="64"/>
     </row>
-    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="37"/>
       <c r="B116" s="118" t="s">
         <v>252</v>
@@ -9448,7 +9469,7 @@
       <c r="N116" s="64"/>
       <c r="O116" s="64"/>
     </row>
-    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="37"/>
       <c r="B117" s="118"/>
       <c r="C117" s="119" t="s">
@@ -9475,7 +9496,7 @@
       <c r="N117" s="64"/>
       <c r="O117" s="64"/>
     </row>
-    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="37"/>
       <c r="B118" s="118"/>
       <c r="C118" s="115"/>
@@ -9492,7 +9513,7 @@
       <c r="N118" s="64"/>
       <c r="O118" s="64"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A119" s="37"/>
       <c r="B119" s="118"/>
       <c r="C119" s="115" t="s">
@@ -9511,7 +9532,7 @@
       <c r="N119" s="64"/>
       <c r="O119" s="64"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A120" s="37"/>
       <c r="B120" s="118"/>
       <c r="C120" s="115" t="s">
@@ -9530,7 +9551,7 @@
       <c r="N120" s="64"/>
       <c r="O120" s="64"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A121" s="37"/>
       <c r="B121" s="118"/>
       <c r="C121" s="115" t="s">
@@ -9549,7 +9570,7 @@
       <c r="N121" s="64"/>
       <c r="O121" s="64"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A122" s="37"/>
       <c r="B122" s="118"/>
       <c r="C122" s="115" t="s">
@@ -9568,7 +9589,7 @@
       <c r="N122" s="64"/>
       <c r="O122" s="64"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A123" s="37"/>
       <c r="B123" s="118"/>
       <c r="C123" s="115"/>
@@ -9585,7 +9606,7 @@
       <c r="N123" s="64"/>
       <c r="O123" s="64"/>
     </row>
-    <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A124" s="37" t="e" vm="55">
         <v>#VALUE!</v>
       </c>
@@ -9608,7 +9629,7 @@
       <c r="N124" s="64"/>
       <c r="O124" s="64"/>
     </row>
-    <row r="125" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A125" s="37"/>
       <c r="B125" s="118"/>
       <c r="C125" s="115" t="s">
@@ -9627,7 +9648,7 @@
       <c r="N125" s="64"/>
       <c r="O125" s="64"/>
     </row>
-    <row r="126" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A126" s="37"/>
       <c r="B126" s="118"/>
       <c r="C126" s="115" t="s">
@@ -9646,7 +9667,7 @@
       <c r="N126" s="64"/>
       <c r="O126" s="64"/>
     </row>
-    <row r="127" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A127" s="37"/>
       <c r="B127" s="118"/>
       <c r="C127" s="115"/>
@@ -9663,7 +9684,7 @@
       <c r="N127" s="64"/>
       <c r="O127" s="64"/>
     </row>
-    <row r="128" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A128" s="37"/>
       <c r="B128" s="118" t="s">
         <v>290</v>
@@ -9684,7 +9705,7 @@
       <c r="N128" s="64"/>
       <c r="O128" s="64"/>
     </row>
-    <row r="129" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A129" s="37"/>
       <c r="B129" s="118"/>
       <c r="C129" s="115"/>
@@ -9701,7 +9722,7 @@
       <c r="N129" s="64"/>
       <c r="O129" s="64"/>
     </row>
-    <row r="130" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A130" s="37"/>
       <c r="B130" s="118"/>
       <c r="C130" s="115"/>
@@ -9718,7 +9739,7 @@
       <c r="N130" s="64"/>
       <c r="O130" s="64"/>
     </row>
-    <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A131" s="37"/>
       <c r="B131" s="118"/>
       <c r="C131" s="115"/>
@@ -9735,7 +9756,7 @@
       <c r="N131" s="64"/>
       <c r="O131" s="64"/>
     </row>
-    <row r="132" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A132" s="37"/>
       <c r="B132" s="118"/>
       <c r="C132" s="115"/>
@@ -9752,7 +9773,7 @@
       <c r="N132" s="64"/>
       <c r="O132" s="64"/>
     </row>
-    <row r="133" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A133" s="37"/>
       <c r="B133" s="118"/>
       <c r="C133" s="115"/>
@@ -9769,7 +9790,7 @@
       <c r="N133" s="64"/>
       <c r="O133" s="64"/>
     </row>
-    <row r="134" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A134" s="37"/>
       <c r="B134" s="118"/>
       <c r="C134" s="115"/>
@@ -9786,7 +9807,7 @@
       <c r="N134" s="64"/>
       <c r="O134" s="64"/>
     </row>
-    <row r="135" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A135" s="37"/>
       <c r="B135" s="118"/>
       <c r="C135" s="115"/>
@@ -9803,7 +9824,7 @@
       <c r="N135" s="64"/>
       <c r="O135" s="64"/>
     </row>
-    <row r="136" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A136" s="37"/>
       <c r="B136" s="118"/>
       <c r="C136" s="115"/>
@@ -9820,7 +9841,7 @@
       <c r="N136" s="64"/>
       <c r="O136" s="64"/>
     </row>
-    <row r="137" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A137" s="37"/>
       <c r="B137" s="118"/>
       <c r="C137" s="115"/>
@@ -9837,14 +9858,129 @@
       <c r="N137" s="64"/>
       <c r="O137" s="64"/>
     </row>
-    <row r="138" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="139" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="140" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="141" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="142" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="138" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="139" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="140" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="141" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="142" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="139">
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C106:G106"/>
     <mergeCell ref="H106:L106"/>
@@ -9869,121 +10005,6 @@
     <mergeCell ref="H101:L101"/>
     <mergeCell ref="M101:N101"/>
     <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
New airdrop gun: Lynx added
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CBA6A2-7567-46D3-B126-10CF69E4A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D356880-5AE7-46BA-AC1E-7516C6647DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="55">
+  <futureMetadata name="XLRICHVALUE" count="56">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -440,8 +440,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="55"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="55">
+  <valueMetadata count="56">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -606,13 +613,16 @@
     </bk>
     <bk>
       <rc t="1" v="54"/>
+    </bk>
+    <bk>
+      <rc t="1" v="55"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="301">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1764,44 +1774,72 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0 ~ 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 ~ 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summons smoke that last approximately 3000 ticks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If explodes on sight, cannot see anything for 100 ticks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explodes after speed &lt;= 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO TIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move busy - we also have peeker's advantage, so the player peeking first will see first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 ~ 500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acceleration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>last update
-2024 6 17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 ~ 1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 ~ 1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Summons smoke that last approximately 3000 ticks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If explodes on sight, cannot see anything for 100 ticks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Explodes after speed &lt;= 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO TIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Move busy - we also have peeker's advantage, so the player peeking first will see first</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 ~ 500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>acceleration</t>
+2024 6 19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 (will become 4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>health will be gradually resored</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adrenaline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lynx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Penetration: penetrates through enemies and players / ammo is restricted (unreloadable)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2721,6 +2759,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2733,9 +2783,6 @@
     <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2751,9 +2798,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2778,17 +2822,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3991,7 +4029,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="55">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="56">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -4212,6 +4250,10 @@
     <v>54</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>55</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -4281,6 +4323,7 @@
   <rel r:id="rId53"/>
   <rel r:id="rId54"/>
   <rel r:id="rId55"/>
+  <rel r:id="rId56"/>
 </richValueRels>
 </file>
 
@@ -4549,8 +4592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -4569,14 +4612,14 @@
       <c r="B1" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="138" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="137"/>
-      <c r="E1" s="136" t="s">
-        <v>284</v>
-      </c>
-      <c r="F1" s="137"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="138" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="139"/>
       <c r="G1" s="54" t="s">
         <v>159</v>
       </c>
@@ -4672,10 +4715,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="55"/>
-      <c r="Z2" s="140" t="s">
+      <c r="Z2" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="140"/>
+      <c r="AA2" s="142"/>
       <c r="AG2" s="41" t="s">
         <v>84</v>
       </c>
@@ -4870,7 +4913,7 @@
       <c r="B5" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="147">
+      <c r="C5" s="125">
         <v>704</v>
       </c>
       <c r="D5" s="23">
@@ -5180,43 +5223,99 @@
       <c r="AL8" s="35"/>
     </row>
     <row r="9" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="55"/>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
+      <c r="A9" s="18" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" s="40">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1</v>
+      </c>
+      <c r="F9" s="19">
+        <v>50</v>
+      </c>
+      <c r="G9" s="19">
+        <v>2200</v>
+      </c>
+      <c r="H9" s="19">
+        <v>40</v>
+      </c>
+      <c r="I9" s="19">
+        <v>5</v>
+      </c>
+      <c r="J9" s="19">
+        <v>4000</v>
+      </c>
+      <c r="K9" s="19">
+        <v>7</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19">
+        <f>ROUND(E9*F9/G9*1000,2)</f>
+        <v>22.73</v>
+      </c>
+      <c r="N9" s="19">
+        <f>ROUND(E9*F9/(G9+J9/I9)*1000,2)</f>
+        <v>16.670000000000002</v>
+      </c>
+      <c r="O9" s="19">
+        <f>E9*F9*I9</f>
+        <v>250</v>
+      </c>
+      <c r="P9" s="24">
+        <f>ROUND(playerHealth/(E9*F9),1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q9" s="19">
+        <f>-(FLOOR(H9/6,1)-1)</f>
+        <v>-5</v>
+      </c>
+      <c r="R9" s="19">
+        <f>ROUND(D9/H9,3)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19">
+        <f xml:space="preserve"> E9*F9*7/10</f>
+        <v>35</v>
+      </c>
+      <c r="V9" s="27">
+        <f>ROUND(playerHealth/(U9),2)</f>
+        <v>0.23</v>
+      </c>
+      <c r="W9" s="19">
+        <f>E9*(F9-0.4)</f>
+        <v>49.6</v>
+      </c>
+      <c r="X9" s="27">
+        <f>ROUND(playerHealth/(W9),2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="Y9" s="72"/>
+      <c r="Z9" s="55" t="s">
+        <v>300</v>
+      </c>
       <c r="AL9" s="35"/>
     </row>
     <row r="10" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="18" t="e" vm="5">
+      <c r="A10" s="18" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="40">
-        <v>1600</v>
+        <v>2000</v>
       </c>
       <c r="D10" s="19">
         <v>0</v>
@@ -5294,7 +5393,7 @@
       </c>
     </row>
     <row r="11" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="18" t="e" vm="6">
+      <c r="A11" s="18" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="B11" s="18" t="s">
@@ -5379,7 +5478,7 @@
       </c>
     </row>
     <row r="12" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="18" t="e" vm="7">
+      <c r="A12" s="18" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -5464,14 +5563,14 @@
       </c>
     </row>
     <row r="13" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="18" t="e" vm="8">
+      <c r="A13" s="18" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="40">
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
@@ -5492,7 +5591,7 @@
         <v>7</v>
       </c>
       <c r="J13" s="19">
-        <v>4500</v>
+        <v>4000</v>
       </c>
       <c r="K13" s="19">
         <v>7</v>
@@ -5504,7 +5603,7 @@
       </c>
       <c r="N13" s="19">
         <f t="shared" si="12"/>
-        <v>4.16</v>
+        <v>4.28</v>
       </c>
       <c r="O13" s="19">
         <f>E13*F13*I13</f>
@@ -5551,7 +5650,7 @@
       </c>
     </row>
     <row r="14" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="18" t="e" vm="9">
+      <c r="A14" s="18" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -5590,7 +5689,7 @@
         <v>8.57</v>
       </c>
       <c r="N14" s="19">
-        <f t="shared" ref="N14" si="13">ROUND(E14*F14/(G14+J14/I14)*1000,2)</f>
+        <f t="shared" ref="N14:N15" si="13">ROUND(E14*F14/(G14+J14/I14)*1000,2)</f>
         <v>3.65</v>
       </c>
       <c r="O14" s="19">
@@ -5642,31 +5741,30 @@
       <c r="B15" s="18"/>
       <c r="C15" s="74"/>
       <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="72"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
       <c r="U15" s="72"/>
       <c r="V15" s="72"/>
       <c r="W15" s="72"/>
       <c r="X15" s="72"/>
       <c r="Y15" s="72"/>
-      <c r="Z15" s="55"/>
     </row>
     <row r="16" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="18" t="e" vm="10">
+      <c r="A16" s="18" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -5753,7 +5851,7 @@
       </c>
     </row>
     <row r="17" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="18" t="e" vm="11">
+      <c r="A17" s="18" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -5846,7 +5944,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="18" t="e" vm="12">
+      <c r="A18" s="18" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="B18" s="18" t="s">
@@ -5933,7 +6031,7 @@
       </c>
     </row>
     <row r="19" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="18" t="e" vm="13">
+      <c r="A19" s="18" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -6018,7 +6116,7 @@
       </c>
     </row>
     <row r="20" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="18" t="e" vm="14">
+      <c r="A20" s="18" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -6165,7 +6263,7 @@
       <c r="AL22" s="35"/>
     </row>
     <row r="23" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="18" t="e" vm="15">
+      <c r="A23" s="18" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -6252,7 +6350,7 @@
       </c>
     </row>
     <row r="24" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="18" t="e" vm="16">
+      <c r="A24" s="18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -6337,7 +6435,7 @@
       </c>
     </row>
     <row r="25" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="18" t="e" vm="17">
+      <c r="A25" s="18" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -6484,7 +6582,7 @@
       <c r="AL27" s="35"/>
     </row>
     <row r="28" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="18" t="e" vm="18">
+      <c r="A28" s="18" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -6569,7 +6667,7 @@
       </c>
     </row>
     <row r="29" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="18" t="e" vm="19">
+      <c r="A29" s="18" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -6654,7 +6752,7 @@
       </c>
     </row>
     <row r="30" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="18" t="e" vm="20">
+      <c r="A30" s="18" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -6799,7 +6897,7 @@
       <c r="AL32" s="35"/>
     </row>
     <row r="33" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A33" s="18" t="e" vm="21">
+      <c r="A33" s="18" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -6871,7 +6969,7 @@
       <c r="AL33" s="35"/>
     </row>
     <row r="34" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="18" t="e" vm="22">
+      <c r="A34" s="18" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="B34" s="18" t="s">
@@ -6941,7 +7039,7 @@
       <c r="AL34" s="35"/>
     </row>
     <row r="35" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="18" t="e" vm="23">
+      <c r="A35" s="18" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="B35" s="18" t="s">
@@ -7168,20 +7266,20 @@
       <c r="B40" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="135" t="s">
+      <c r="C40" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135" t="s">
+      <c r="D40" s="126"/>
+      <c r="E40" s="126"/>
+      <c r="F40" s="126"/>
+      <c r="G40" s="126"/>
+      <c r="H40" s="126"/>
+      <c r="I40" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="135"/>
-      <c r="K40" s="135"/>
-      <c r="L40" s="135"/>
+      <c r="J40" s="126"/>
+      <c r="K40" s="126"/>
+      <c r="L40" s="126"/>
       <c r="M40" s="106"/>
       <c r="N40" s="106"/>
       <c r="O40" s="106"/>
@@ -7189,35 +7287,35 @@
       <c r="Q40" s="119" t="s">
         <v>258</v>
       </c>
-      <c r="S40" s="141" t="s">
+      <c r="S40" s="143" t="s">
         <v>77</v>
       </c>
-      <c r="T40" s="141"/>
+      <c r="T40" s="143"/>
       <c r="U40" s="55"/>
     </row>
     <row r="41" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A41" s="37" t="e" vm="24">
+      <c r="A41" s="37" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
       <c r="B41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="144" t="s">
+      <c r="C41" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="144"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="144" t="s">
+      <c r="D41" s="127"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144" t="s">
+      <c r="G41" s="127"/>
+      <c r="H41" s="127"/>
+      <c r="I41" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="144"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="144"/>
+      <c r="J41" s="127"/>
+      <c r="K41" s="127"/>
+      <c r="L41" s="127"/>
       <c r="M41" s="107"/>
       <c r="N41" s="107"/>
       <c r="O41" s="107"/>
@@ -7225,38 +7323,38 @@
       <c r="Q41" s="63" t="s">
         <v>259</v>
       </c>
-      <c r="S41" s="141" t="s">
+      <c r="S41" s="143" t="s">
         <v>75</v>
       </c>
-      <c r="T41" s="141"/>
+      <c r="T41" s="143"/>
       <c r="U41" s="55">
         <v>8</v>
       </c>
       <c r="V41" s="55"/>
     </row>
     <row r="42" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="37" t="e" vm="25">
+      <c r="A42" s="37" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="144" t="s">
+      <c r="C42" s="127" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144" t="s">
+      <c r="D42" s="127"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127" t="s">
         <v>199</v>
       </c>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144" t="s">
+      <c r="G42" s="127"/>
+      <c r="H42" s="127"/>
+      <c r="I42" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="144"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="144"/>
+      <c r="J42" s="127"/>
+      <c r="K42" s="127"/>
+      <c r="L42" s="127"/>
       <c r="M42" s="107"/>
       <c r="N42" s="107"/>
       <c r="O42" s="107"/>
@@ -7264,10 +7362,10 @@
       <c r="Q42" s="63" t="s">
         <v>259</v>
       </c>
-      <c r="S42" s="141" t="s">
+      <c r="S42" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="T42" s="141"/>
+      <c r="T42" s="143"/>
       <c r="U42" s="55">
         <v>128</v>
       </c>
@@ -7280,22 +7378,22 @@
       <c r="B43" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C43" s="129" t="s">
+      <c r="C43" s="128" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="129"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129" t="s">
+      <c r="D43" s="128"/>
+      <c r="E43" s="128"/>
+      <c r="F43" s="128" t="s">
         <v>207</v>
       </c>
-      <c r="G43" s="129"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="129" t="s">
+      <c r="G43" s="128"/>
+      <c r="H43" s="128"/>
+      <c r="I43" s="128" t="s">
         <v>204</v>
       </c>
-      <c r="J43" s="129"/>
-      <c r="K43" s="129"/>
-      <c r="L43" s="129"/>
+      <c r="J43" s="128"/>
+      <c r="K43" s="128"/>
+      <c r="L43" s="128"/>
       <c r="M43" s="42"/>
       <c r="N43" s="42"/>
       <c r="O43" s="107"/>
@@ -7303,10 +7401,10 @@
       <c r="Q43" s="63" t="s">
         <v>260</v>
       </c>
-      <c r="S43" s="141" t="s">
+      <c r="S43" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="T43" s="141"/>
+      <c r="T43" s="143"/>
       <c r="U43" s="55">
         <v>16</v>
       </c>
@@ -7321,20 +7419,20 @@
       <c r="B44" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="129" t="s">
+      <c r="C44" s="128" t="s">
         <v>267</v>
       </c>
-      <c r="D44" s="129"/>
-      <c r="E44" s="129"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="129"/>
-      <c r="H44" s="129"/>
-      <c r="I44" s="129" t="s">
+      <c r="D44" s="128"/>
+      <c r="E44" s="128"/>
+      <c r="F44" s="128"/>
+      <c r="G44" s="128"/>
+      <c r="H44" s="128"/>
+      <c r="I44" s="128" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="129"/>
-      <c r="K44" s="129"/>
-      <c r="L44" s="129"/>
+      <c r="J44" s="128"/>
+      <c r="K44" s="128"/>
+      <c r="L44" s="128"/>
       <c r="M44" s="42"/>
       <c r="N44" s="42"/>
       <c r="O44" s="107"/>
@@ -7360,8 +7458,10 @@
         <v>190</v>
       </c>
       <c r="F46" s="120"/>
-      <c r="G46" s="120"/>
-      <c r="H46" s="120"/>
+      <c r="G46" s="126" t="s">
+        <v>294</v>
+      </c>
+      <c r="H46" s="126"/>
       <c r="I46" s="109"/>
       <c r="J46" s="109"/>
       <c r="K46" s="119" t="s">
@@ -7369,7 +7469,7 @@
       </c>
     </row>
     <row r="47" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A47" s="37" t="e" vm="26">
+      <c r="A47" s="37" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
       <c r="B47" s="37" t="s">
@@ -7383,8 +7483,10 @@
         <v>195</v>
       </c>
       <c r="F47" s="121"/>
-      <c r="G47" s="121"/>
-      <c r="H47" s="121"/>
+      <c r="G47" s="127">
+        <v>1</v>
+      </c>
+      <c r="H47" s="127"/>
       <c r="I47" s="108"/>
       <c r="J47" s="108"/>
       <c r="K47" s="63" t="s">
@@ -7392,7 +7494,7 @@
       </c>
     </row>
     <row r="48" spans="1:38" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="37" t="e" vm="27">
+      <c r="A48" s="37" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="37" t="s">
@@ -7406,8 +7508,10 @@
         <v>95</v>
       </c>
       <c r="F48" s="121"/>
-      <c r="G48" s="121"/>
-      <c r="H48" s="121"/>
+      <c r="G48" s="127" t="s">
+        <v>295</v>
+      </c>
+      <c r="H48" s="127"/>
       <c r="I48" s="108"/>
       <c r="J48" s="108"/>
       <c r="K48" s="63" t="s">
@@ -7416,16 +7520,26 @@
     </row>
     <row r="49" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="129"/>
-      <c r="E49" s="129"/>
-      <c r="F49" s="129"/>
-      <c r="G49" s="129"/>
-      <c r="H49" s="129"/>
+      <c r="B49" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C49" s="121">
+        <v>6</v>
+      </c>
+      <c r="D49" s="128" t="s">
+        <v>296</v>
+      </c>
+      <c r="E49" s="128"/>
+      <c r="F49" s="128"/>
+      <c r="G49" s="128">
+        <v>1</v>
+      </c>
+      <c r="H49" s="128"/>
       <c r="I49" s="42"/>
       <c r="J49" s="42"/>
-      <c r="K49" s="63"/>
+      <c r="K49" s="63" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="50" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="51" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7433,87 +7547,87 @@
       <c r="B51" s="75" t="s">
         <v>263</v>
       </c>
-      <c r="C51" s="135" t="s">
+      <c r="C51" s="126" t="s">
         <v>268</v>
       </c>
-      <c r="D51" s="135"/>
-      <c r="E51" s="135" t="s">
+      <c r="D51" s="126"/>
+      <c r="E51" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="135"/>
-      <c r="G51" s="135"/>
-      <c r="H51" s="135"/>
-      <c r="I51" s="135"/>
-      <c r="J51" s="135"/>
+      <c r="F51" s="126"/>
+      <c r="G51" s="126"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="126"/>
       <c r="K51" s="119" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A52" s="37" t="e" vm="28">
+      <c r="A52" s="37" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="134" t="s">
-        <v>285</v>
-      </c>
-      <c r="D52" s="134"/>
-      <c r="E52" s="132" t="s">
-        <v>289</v>
-      </c>
-      <c r="F52" s="132"/>
-      <c r="G52" s="132"/>
-      <c r="H52" s="132"/>
-      <c r="I52" s="132"/>
-      <c r="J52" s="132"/>
+      <c r="C52" s="137" t="s">
+        <v>284</v>
+      </c>
+      <c r="D52" s="137"/>
+      <c r="E52" s="135" t="s">
+        <v>288</v>
+      </c>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
+      <c r="H52" s="135"/>
+      <c r="I52" s="135"/>
+      <c r="J52" s="135"/>
       <c r="K52" s="63" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A53" s="37" t="e" vm="29">
+      <c r="A53" s="37" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
       <c r="B53" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="C53" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="D53" s="134"/>
-      <c r="E53" s="132" t="s">
-        <v>287</v>
-      </c>
-      <c r="F53" s="132"/>
-      <c r="G53" s="132"/>
-      <c r="H53" s="132"/>
-      <c r="I53" s="132"/>
-      <c r="J53" s="132"/>
+      <c r="C53" s="137" t="s">
+        <v>291</v>
+      </c>
+      <c r="D53" s="137"/>
+      <c r="E53" s="135" t="s">
+        <v>286</v>
+      </c>
+      <c r="F53" s="135"/>
+      <c r="G53" s="135"/>
+      <c r="H53" s="135"/>
+      <c r="I53" s="135"/>
+      <c r="J53" s="135"/>
       <c r="K53" s="63" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A54" s="18" t="e" vm="30">
+      <c r="A54" s="18" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C54" s="134" t="s">
-        <v>286</v>
-      </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="132" t="s">
-        <v>288</v>
-      </c>
-      <c r="F54" s="132"/>
-      <c r="G54" s="132"/>
-      <c r="H54" s="132"/>
-      <c r="I54" s="132"/>
-      <c r="J54" s="132"/>
+      <c r="C54" s="137" t="s">
+        <v>285</v>
+      </c>
+      <c r="D54" s="137"/>
+      <c r="E54" s="135" t="s">
+        <v>287</v>
+      </c>
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="135"/>
+      <c r="J54" s="135"/>
       <c r="K54" s="63" t="s">
         <v>259</v>
       </c>
@@ -7530,14 +7644,14 @@
       <c r="D56" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="H56" s="133" t="s">
+      <c r="H56" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="133"/>
-      <c r="J56" s="133"/>
-      <c r="K56" s="133"/>
-      <c r="L56" s="133"/>
-      <c r="M56" s="133"/>
+      <c r="I56" s="136"/>
+      <c r="J56" s="136"/>
+      <c r="K56" s="136"/>
+      <c r="L56" s="136"/>
+      <c r="M56" s="136"/>
     </row>
     <row r="57" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="89"/>
@@ -7741,31 +7855,31 @@
       <c r="I62" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="139" t="s">
+      <c r="J62" s="141" t="s">
         <v>100</v>
       </c>
-      <c r="K62" s="139"/>
+      <c r="K62" s="141"/>
       <c r="L62" t="s">
         <v>101</v>
       </c>
       <c r="M62" s="94">
         <f>COUNTIF(H3:H35,"&gt;0")</f>
-        <v>25</v>
-      </c>
-      <c r="O62" s="138" t="s">
+        <v>26</v>
+      </c>
+      <c r="O62" s="140" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="138"/>
-      <c r="Q62" s="138"/>
-      <c r="R62" s="138"/>
-      <c r="S62" s="138"/>
+      <c r="P62" s="140"/>
+      <c r="Q62" s="140"/>
+      <c r="R62" s="140"/>
+      <c r="S62" s="140"/>
       <c r="AG62" s="79"/>
       <c r="AH62" s="79"/>
       <c r="AI62" s="79"/>
       <c r="AJ62" s="79"/>
     </row>
     <row r="63" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="89" t="e" vm="31">
+      <c r="A63" s="89" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="83" t="s">
@@ -7780,20 +7894,20 @@
       <c r="E63" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="142" t="s">
+      <c r="F63" s="144" t="s">
         <v>92</v>
       </c>
-      <c r="G63" s="142"/>
+      <c r="G63" s="144"/>
       <c r="H63" s="84" t="s">
         <v>187</v>
       </c>
       <c r="I63" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="142" t="s">
+      <c r="J63" s="144" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="142"/>
+      <c r="K63" s="144"/>
       <c r="L63" s="84" t="s">
         <v>102</v>
       </c>
@@ -7801,7 +7915,7 @@
         <v>103</v>
       </c>
       <c r="N63" s="84" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O63" s="103" t="s">
         <v>108</v>
@@ -7819,10 +7933,10 @@
         <v>113</v>
       </c>
       <c r="T63" s="84"/>
-      <c r="U63" s="142" t="s">
+      <c r="U63" s="144" t="s">
         <v>117</v>
       </c>
-      <c r="V63" s="142"/>
+      <c r="V63" s="144"/>
       <c r="W63" s="84" t="s">
         <v>22</v>
       </c>
@@ -7850,28 +7964,28 @@
       <c r="E64" s="95">
         <v>6</v>
       </c>
-      <c r="F64" s="143" t="s">
+      <c r="F64" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="145"/>
       <c r="H64" s="95">
         <v>1</v>
       </c>
       <c r="I64" s="95">
         <v>0</v>
       </c>
-      <c r="J64" s="134">
+      <c r="J64" s="137">
         <f t="shared" ref="J64:J69" si="32">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="134"/>
+      <c r="K64" s="137"/>
       <c r="L64" s="95">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M64" s="95">
         <f>21-L64</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N64" s="95">
         <v>0.12</v>
@@ -7882,7 +7996,7 @@
       </c>
       <c r="P64" s="98">
         <f t="shared" ref="P64:P70" si="34">ROUND(M64/guns_cap,2)*10</f>
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="Q64" s="99">
         <f t="shared" ref="Q64:Q70" si="35">ROUND(E64/speed_cap,2)*10</f>
@@ -7894,14 +8008,14 @@
       </c>
       <c r="S64" s="101">
         <f>SUM(O64:R64)</f>
-        <v>9.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="T64" s="95"/>
-      <c r="U64" s="145">
+      <c r="U64" s="146">
         <f>R64+O64+P64</f>
-        <v>4.5</v>
-      </c>
-      <c r="V64" s="145"/>
+        <v>4.2</v>
+      </c>
+      <c r="V64" s="146"/>
       <c r="W64" s="102" t="s">
         <v>29</v>
       </c>
@@ -7929,28 +8043,28 @@
       <c r="E65" s="52">
         <v>4</v>
       </c>
-      <c r="F65" s="127" t="s">
+      <c r="F65" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="G65" s="127"/>
+      <c r="G65" s="131"/>
       <c r="H65" s="52">
         <v>1</v>
       </c>
       <c r="I65" s="52">
         <v>0</v>
       </c>
-      <c r="J65" s="134">
+      <c r="J65" s="137">
         <f t="shared" si="32"/>
         <v>32</v>
       </c>
-      <c r="K65" s="134"/>
+      <c r="K65" s="137"/>
       <c r="L65" s="52">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M65" s="52">
         <f t="shared" ref="M65:M68" si="37">21-L65</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N65" s="52">
         <v>0.08</v>
@@ -7961,7 +8075,7 @@
       </c>
       <c r="P65" s="65">
         <f t="shared" si="34"/>
-        <v>6</v>
+        <v>5.6999999999999993</v>
       </c>
       <c r="Q65" s="66">
         <f t="shared" si="35"/>
@@ -7973,14 +8087,14 @@
       </c>
       <c r="S65" s="68">
         <f t="shared" ref="S65:S69" si="38">SUM(O65:R65)</f>
-        <v>13.8</v>
+        <v>13.5</v>
       </c>
       <c r="T65" s="52"/>
-      <c r="U65" s="146">
+      <c r="U65" s="147">
         <f t="shared" ref="U65:U70" si="39">R65+O65+P65</f>
-        <v>10.5</v>
-      </c>
-      <c r="V65" s="146"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="V65" s="147"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -8008,28 +8122,28 @@
       <c r="E66" s="52">
         <v>3</v>
       </c>
-      <c r="F66" s="127" t="s">
+      <c r="F66" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="127"/>
+      <c r="G66" s="131"/>
       <c r="H66" s="52">
         <v>1</v>
       </c>
       <c r="I66" s="52">
         <v>11.11</v>
       </c>
-      <c r="J66" s="134">
+      <c r="J66" s="137">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K66" s="134"/>
+      <c r="K66" s="137"/>
       <c r="L66" s="52">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M66" s="52">
         <f t="shared" si="37"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N66" s="52">
         <v>0.1</v>
@@ -8040,7 +8154,7 @@
       </c>
       <c r="P66" s="65">
         <f t="shared" si="34"/>
-        <v>5.6999999999999993</v>
+        <v>5.3000000000000007</v>
       </c>
       <c r="Q66" s="66">
         <f t="shared" si="35"/>
@@ -8052,14 +8166,14 @@
       </c>
       <c r="S66" s="68">
         <f t="shared" si="38"/>
-        <v>13.399999999999999</v>
+        <v>13</v>
       </c>
       <c r="T66" s="52"/>
-      <c r="U66" s="146">
+      <c r="U66" s="147">
         <f t="shared" si="39"/>
-        <v>10.899999999999999</v>
-      </c>
-      <c r="V66" s="146"/>
+        <v>10.5</v>
+      </c>
+      <c r="V66" s="147"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -8087,21 +8201,21 @@
       <c r="E67" s="52">
         <v>1</v>
       </c>
-      <c r="F67" s="127" t="s">
+      <c r="F67" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="127"/>
+      <c r="G67" s="131"/>
       <c r="H67" s="52">
         <v>1</v>
       </c>
       <c r="I67" s="52">
         <v>5.63</v>
       </c>
-      <c r="J67" s="134">
+      <c r="J67" s="137">
         <f t="shared" si="32"/>
         <v>58</v>
       </c>
-      <c r="K67" s="134"/>
+      <c r="K67" s="137"/>
       <c r="L67" s="52">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -8134,11 +8248,11 @@
         <v>18.500000000000004</v>
       </c>
       <c r="T67" s="52"/>
-      <c r="U67" s="146">
+      <c r="U67" s="147">
         <f t="shared" si="39"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="146"/>
+      <c r="V67" s="147"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -8162,21 +8276,21 @@
       <c r="E68" s="52">
         <v>0</v>
       </c>
-      <c r="F68" s="127" t="s">
+      <c r="F68" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="127"/>
+      <c r="G68" s="131"/>
       <c r="H68" s="52">
         <v>1</v>
       </c>
       <c r="I68" s="52">
         <v>13.33</v>
       </c>
-      <c r="J68" s="134">
+      <c r="J68" s="137">
         <f t="shared" si="32"/>
         <v>72</v>
       </c>
-      <c r="K68" s="134"/>
+      <c r="K68" s="137"/>
       <c r="L68" s="52">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -8209,11 +8323,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="52"/>
-      <c r="U68" s="146">
+      <c r="U68" s="147">
         <f t="shared" si="39"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="146"/>
+      <c r="V68" s="147"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -8237,28 +8351,28 @@
       <c r="E69" s="52">
         <v>12</v>
       </c>
-      <c r="F69" s="127" t="s">
+      <c r="F69" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="127"/>
+      <c r="G69" s="131"/>
       <c r="H69" s="52">
         <v>1</v>
       </c>
       <c r="I69" s="52">
         <v>9.09</v>
       </c>
-      <c r="J69" s="134">
+      <c r="J69" s="137">
         <f t="shared" si="32"/>
         <v>20</v>
       </c>
-      <c r="K69" s="134"/>
+      <c r="K69" s="137"/>
       <c r="L69" s="52">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M69" s="52">
         <f>21-L69</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N69" s="52">
         <v>0.18</v>
@@ -8269,7 +8383,7 @@
       </c>
       <c r="P69" s="65">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>4.6999999999999993</v>
       </c>
       <c r="Q69" s="66">
         <f>ROUND(E69/speed_cap,2)*10</f>
@@ -8281,14 +8395,14 @@
       </c>
       <c r="S69" s="68">
         <f t="shared" si="38"/>
-        <v>18.8</v>
+        <v>18.5</v>
       </c>
       <c r="T69" s="52"/>
-      <c r="U69" s="146">
+      <c r="U69" s="147">
         <f t="shared" si="39"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="V69" s="146"/>
+        <v>8.5</v>
+      </c>
+      <c r="V69" s="147"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -8312,28 +8426,28 @@
       <c r="E70" s="52">
         <v>10</v>
       </c>
-      <c r="F70" s="127" t="s">
+      <c r="F70" s="131" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="127"/>
+      <c r="G70" s="131"/>
       <c r="H70" s="52">
         <v>1</v>
       </c>
       <c r="I70" s="52">
         <v>48</v>
       </c>
-      <c r="J70" s="134">
+      <c r="J70" s="137">
         <f t="shared" ref="J70" si="40">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="134"/>
+      <c r="K70" s="137"/>
       <c r="L70" s="52">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M70" s="52">
         <f>21-L70</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N70" s="52">
         <v>0.14000000000000001</v>
@@ -8344,7 +8458,7 @@
       </c>
       <c r="P70" s="65">
         <f t="shared" si="34"/>
-        <v>5.6999999999999993</v>
+        <v>5.3000000000000007</v>
       </c>
       <c r="Q70" s="66">
         <f t="shared" si="35"/>
@@ -8356,14 +8470,14 @@
       </c>
       <c r="S70" s="68">
         <f t="shared" ref="S70" si="41">SUM(O70:R70)</f>
-        <v>26.1</v>
+        <v>25.700000000000003</v>
       </c>
       <c r="T70" s="52"/>
-      <c r="U70" s="146">
+      <c r="U70" s="147">
         <f t="shared" si="39"/>
-        <v>17.799999999999997</v>
-      </c>
-      <c r="V70" s="146"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="V70" s="147"/>
       <c r="W70" s="25" t="s">
         <v>74</v>
       </c>
@@ -8379,12 +8493,12 @@
       <c r="B73" s="115" t="s">
         <v>238</v>
       </c>
-      <c r="O73" s="140" t="s">
+      <c r="O73" s="142" t="s">
         <v>166</v>
       </c>
-      <c r="P73" s="140"/>
-      <c r="Q73" s="140"/>
-      <c r="R73" s="140"/>
+      <c r="P73" s="142"/>
+      <c r="Q73" s="142"/>
+      <c r="R73" s="142"/>
     </row>
     <row r="74" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="34"/>
@@ -8400,37 +8514,37 @@
       <c r="E74" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="130" t="s">
+      <c r="F74" s="133" t="s">
         <v>136</v>
       </c>
-      <c r="G74" s="130"/>
-      <c r="H74" s="130" t="s">
+      <c r="G74" s="133"/>
+      <c r="H74" s="133" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="130"/>
-      <c r="J74" s="130" t="s">
+      <c r="I74" s="133"/>
+      <c r="J74" s="133" t="s">
         <v>134</v>
       </c>
-      <c r="K74" s="130"/>
-      <c r="L74" s="130"/>
-      <c r="M74" s="130"/>
+      <c r="K74" s="133"/>
+      <c r="L74" s="133"/>
+      <c r="M74" s="133"/>
       <c r="N74" s="105" t="s">
         <v>167</v>
       </c>
-      <c r="O74" s="130" t="s">
+      <c r="O74" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="P74" s="130"/>
-      <c r="Q74" s="130" t="s">
+      <c r="P74" s="133"/>
+      <c r="Q74" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="R74" s="130"/>
+      <c r="R74" s="133"/>
       <c r="S74" s="119" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A75" s="37" t="e" vm="32">
+      <c r="A75" s="37" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
       <c r="B75" s="37" t="s">
@@ -8445,34 +8559,34 @@
       <c r="E75" s="52">
         <v>18</v>
       </c>
-      <c r="F75" s="134" t="s">
+      <c r="F75" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="134"/>
-      <c r="H75" s="134">
+      <c r="G75" s="137"/>
+      <c r="H75" s="137">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="134"/>
-      <c r="J75" s="134" t="s">
+      <c r="I75" s="137"/>
+      <c r="J75" s="137" t="s">
         <v>133</v>
       </c>
-      <c r="K75" s="134"/>
-      <c r="L75" s="134"/>
-      <c r="M75" s="134"/>
-      <c r="N75" s="76" t="e" vm="33">
+      <c r="K75" s="137"/>
+      <c r="L75" s="137"/>
+      <c r="M75" s="137"/>
+      <c r="N75" s="76" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
-      <c r="O75" s="68" t="e" vm="34">
+      <c r="O75" s="68" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
-      <c r="P75" s="68" t="e" vm="35">
+      <c r="P75" s="68" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
-      <c r="Q75" s="77" t="e" vm="36">
+      <c r="Q75" s="77" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
-      <c r="R75" s="93" t="e" vm="37">
+      <c r="R75" s="93" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
       <c r="S75" s="63" t="s">
@@ -8480,7 +8594,7 @@
       </c>
     </row>
     <row r="76" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A76" s="37" t="e" vm="38">
+      <c r="A76" s="37" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="37" t="s">
@@ -8495,34 +8609,34 @@
       <c r="E76" s="52">
         <v>12</v>
       </c>
-      <c r="F76" s="134" t="s">
+      <c r="F76" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="134"/>
-      <c r="H76" s="134">
+      <c r="G76" s="137"/>
+      <c r="H76" s="137">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="134"/>
-      <c r="J76" s="134" t="s">
+      <c r="I76" s="137"/>
+      <c r="J76" s="137" t="s">
         <v>132</v>
       </c>
-      <c r="K76" s="134"/>
-      <c r="L76" s="134"/>
-      <c r="M76" s="134"/>
-      <c r="N76" s="76" t="e" vm="39">
+      <c r="K76" s="137"/>
+      <c r="L76" s="137"/>
+      <c r="M76" s="137"/>
+      <c r="N76" s="76" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
-      <c r="O76" s="68" t="e" vm="40">
+      <c r="O76" s="68" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
-      <c r="P76" s="68" t="e" vm="41">
+      <c r="P76" s="68" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
-      <c r="Q76" s="77" t="e" vm="42">
+      <c r="Q76" s="77" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
-      <c r="R76" s="93" t="e" vm="43">
+      <c r="R76" s="93" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
       <c r="S76" s="63" t="s">
@@ -8535,19 +8649,19 @@
       <c r="C77" s="42"/>
       <c r="D77" s="42"/>
       <c r="E77" s="42"/>
-      <c r="F77" s="129"/>
-      <c r="G77" s="129"/>
-      <c r="H77" s="129"/>
-      <c r="I77" s="129"/>
-      <c r="J77" s="129"/>
-      <c r="K77" s="129"/>
-      <c r="L77" s="129"/>
-      <c r="M77" s="129"/>
+      <c r="F77" s="128"/>
+      <c r="G77" s="128"/>
+      <c r="H77" s="128"/>
+      <c r="I77" s="128"/>
+      <c r="J77" s="128"/>
+      <c r="K77" s="128"/>
+      <c r="L77" s="128"/>
+      <c r="M77" s="128"/>
       <c r="N77" s="92"/>
-      <c r="O77" s="125"/>
-      <c r="P77" s="125"/>
-      <c r="Q77" s="125"/>
-      <c r="R77" s="125"/>
+      <c r="O77" s="129"/>
+      <c r="P77" s="129"/>
+      <c r="Q77" s="129"/>
+      <c r="R77" s="129"/>
       <c r="S77" s="63"/>
     </row>
     <row r="78" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -8561,7 +8675,7 @@
     <row r="79" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="80" spans="1:36" ht="23.55" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="81" spans="1:28" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A81" s="34" t="e" vm="44">
+      <c r="A81" s="34" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
       <c r="B81" s="75" t="s">
@@ -8576,32 +8690,32 @@
       <c r="E81" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="F81" s="130" t="s">
+      <c r="F81" s="133" t="s">
         <v>140</v>
       </c>
-      <c r="G81" s="130"/>
-      <c r="H81" s="130"/>
-      <c r="I81" s="130"/>
-      <c r="J81" s="130"/>
-      <c r="K81" s="130"/>
-      <c r="L81" s="130"/>
-      <c r="M81" s="130"/>
-      <c r="N81" s="130"/>
-      <c r="O81" s="130"/>
-      <c r="P81" s="130"/>
-      <c r="Q81" s="130" t="s">
+      <c r="G81" s="133"/>
+      <c r="H81" s="133"/>
+      <c r="I81" s="133"/>
+      <c r="J81" s="133"/>
+      <c r="K81" s="133"/>
+      <c r="L81" s="133"/>
+      <c r="M81" s="133"/>
+      <c r="N81" s="133"/>
+      <c r="O81" s="133"/>
+      <c r="P81" s="133"/>
+      <c r="Q81" s="133" t="s">
         <v>153</v>
       </c>
-      <c r="R81" s="130"/>
-      <c r="S81" s="130"/>
-      <c r="T81" s="130"/>
-      <c r="U81" s="130"/>
-      <c r="V81" s="130"/>
-      <c r="W81" s="130"/>
-      <c r="X81" s="130"/>
-      <c r="Y81" s="130"/>
-      <c r="Z81" s="130"/>
-      <c r="AA81" s="130"/>
+      <c r="R81" s="133"/>
+      <c r="S81" s="133"/>
+      <c r="T81" s="133"/>
+      <c r="U81" s="133"/>
+      <c r="V81" s="133"/>
+      <c r="W81" s="133"/>
+      <c r="X81" s="133"/>
+      <c r="Y81" s="133"/>
+      <c r="Z81" s="133"/>
+      <c r="AA81" s="133"/>
       <c r="AB81" s="119" t="s">
         <v>258</v>
       </c>
@@ -8620,32 +8734,32 @@
       <c r="E82" s="95">
         <v>16</v>
       </c>
-      <c r="F82" s="131" t="s">
+      <c r="F82" s="134" t="s">
         <v>151</v>
       </c>
-      <c r="G82" s="131"/>
-      <c r="H82" s="131"/>
-      <c r="I82" s="131"/>
-      <c r="J82" s="131"/>
-      <c r="K82" s="131"/>
-      <c r="L82" s="131"/>
-      <c r="M82" s="131"/>
-      <c r="N82" s="131"/>
-      <c r="O82" s="131"/>
-      <c r="P82" s="131"/>
-      <c r="Q82" s="131" t="s">
+      <c r="G82" s="134"/>
+      <c r="H82" s="134"/>
+      <c r="I82" s="134"/>
+      <c r="J82" s="134"/>
+      <c r="K82" s="134"/>
+      <c r="L82" s="134"/>
+      <c r="M82" s="134"/>
+      <c r="N82" s="134"/>
+      <c r="O82" s="134"/>
+      <c r="P82" s="134"/>
+      <c r="Q82" s="134" t="s">
         <v>154</v>
       </c>
-      <c r="R82" s="131"/>
-      <c r="S82" s="131"/>
-      <c r="T82" s="131"/>
-      <c r="U82" s="131"/>
-      <c r="V82" s="131"/>
-      <c r="W82" s="131"/>
-      <c r="X82" s="131"/>
-      <c r="Y82" s="131"/>
-      <c r="Z82" s="131"/>
-      <c r="AA82" s="131"/>
+      <c r="R82" s="134"/>
+      <c r="S82" s="134"/>
+      <c r="T82" s="134"/>
+      <c r="U82" s="134"/>
+      <c r="V82" s="134"/>
+      <c r="W82" s="134"/>
+      <c r="X82" s="134"/>
+      <c r="Y82" s="134"/>
+      <c r="Z82" s="134"/>
+      <c r="AA82" s="134"/>
       <c r="AB82" s="63" t="s">
         <v>259</v>
       </c>
@@ -8664,30 +8778,30 @@
       <c r="E83" s="52">
         <v>1</v>
       </c>
-      <c r="F83" s="132" t="s">
+      <c r="F83" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="G83" s="132"/>
-      <c r="H83" s="132"/>
-      <c r="I83" s="132"/>
-      <c r="J83" s="132"/>
-      <c r="K83" s="132"/>
-      <c r="L83" s="132"/>
-      <c r="M83" s="132"/>
-      <c r="N83" s="132"/>
-      <c r="O83" s="132"/>
-      <c r="P83" s="132"/>
-      <c r="Q83" s="132"/>
-      <c r="R83" s="132"/>
-      <c r="S83" s="132"/>
-      <c r="T83" s="132"/>
-      <c r="U83" s="132"/>
-      <c r="V83" s="132"/>
-      <c r="W83" s="132"/>
-      <c r="X83" s="132"/>
-      <c r="Y83" s="132"/>
-      <c r="Z83" s="132"/>
-      <c r="AA83" s="132"/>
+      <c r="G83" s="135"/>
+      <c r="H83" s="135"/>
+      <c r="I83" s="135"/>
+      <c r="J83" s="135"/>
+      <c r="K83" s="135"/>
+      <c r="L83" s="135"/>
+      <c r="M83" s="135"/>
+      <c r="N83" s="135"/>
+      <c r="O83" s="135"/>
+      <c r="P83" s="135"/>
+      <c r="Q83" s="135"/>
+      <c r="R83" s="135"/>
+      <c r="S83" s="135"/>
+      <c r="T83" s="135"/>
+      <c r="U83" s="135"/>
+      <c r="V83" s="135"/>
+      <c r="W83" s="135"/>
+      <c r="X83" s="135"/>
+      <c r="Y83" s="135"/>
+      <c r="Z83" s="135"/>
+      <c r="AA83" s="135"/>
       <c r="AB83" s="63" t="s">
         <v>259</v>
       </c>
@@ -8706,30 +8820,30 @@
       <c r="E84" s="52">
         <v>1</v>
       </c>
-      <c r="F84" s="132" t="s">
+      <c r="F84" s="135" t="s">
         <v>225</v>
       </c>
-      <c r="G84" s="132"/>
-      <c r="H84" s="132"/>
-      <c r="I84" s="132"/>
-      <c r="J84" s="132"/>
-      <c r="K84" s="132"/>
-      <c r="L84" s="132"/>
-      <c r="M84" s="132"/>
-      <c r="N84" s="132"/>
-      <c r="O84" s="132"/>
-      <c r="P84" s="132"/>
-      <c r="Q84" s="132"/>
-      <c r="R84" s="132"/>
-      <c r="S84" s="132"/>
-      <c r="T84" s="132"/>
-      <c r="U84" s="132"/>
-      <c r="V84" s="132"/>
-      <c r="W84" s="132"/>
-      <c r="X84" s="132"/>
-      <c r="Y84" s="132"/>
-      <c r="Z84" s="132"/>
-      <c r="AA84" s="132"/>
+      <c r="G84" s="135"/>
+      <c r="H84" s="135"/>
+      <c r="I84" s="135"/>
+      <c r="J84" s="135"/>
+      <c r="K84" s="135"/>
+      <c r="L84" s="135"/>
+      <c r="M84" s="135"/>
+      <c r="N84" s="135"/>
+      <c r="O84" s="135"/>
+      <c r="P84" s="135"/>
+      <c r="Q84" s="135"/>
+      <c r="R84" s="135"/>
+      <c r="S84" s="135"/>
+      <c r="T84" s="135"/>
+      <c r="U84" s="135"/>
+      <c r="V84" s="135"/>
+      <c r="W84" s="135"/>
+      <c r="X84" s="135"/>
+      <c r="Y84" s="135"/>
+      <c r="Z84" s="135"/>
+      <c r="AA84" s="135"/>
       <c r="AB84" s="63" t="s">
         <v>259</v>
       </c>
@@ -8748,32 +8862,32 @@
       <c r="E85" s="52">
         <v>1</v>
       </c>
-      <c r="F85" s="132" t="s">
+      <c r="F85" s="135" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="132"/>
-      <c r="H85" s="132"/>
-      <c r="I85" s="132"/>
-      <c r="J85" s="132"/>
-      <c r="K85" s="132"/>
-      <c r="L85" s="132"/>
-      <c r="M85" s="132"/>
-      <c r="N85" s="132"/>
-      <c r="O85" s="132"/>
-      <c r="P85" s="132"/>
-      <c r="Q85" s="132" t="s">
+      <c r="G85" s="135"/>
+      <c r="H85" s="135"/>
+      <c r="I85" s="135"/>
+      <c r="J85" s="135"/>
+      <c r="K85" s="135"/>
+      <c r="L85" s="135"/>
+      <c r="M85" s="135"/>
+      <c r="N85" s="135"/>
+      <c r="O85" s="135"/>
+      <c r="P85" s="135"/>
+      <c r="Q85" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="R85" s="132"/>
-      <c r="S85" s="132"/>
-      <c r="T85" s="132"/>
-      <c r="U85" s="132"/>
-      <c r="V85" s="132"/>
-      <c r="W85" s="132"/>
-      <c r="X85" s="132"/>
-      <c r="Y85" s="132"/>
-      <c r="Z85" s="132"/>
-      <c r="AA85" s="132"/>
+      <c r="R85" s="135"/>
+      <c r="S85" s="135"/>
+      <c r="T85" s="135"/>
+      <c r="U85" s="135"/>
+      <c r="V85" s="135"/>
+      <c r="W85" s="135"/>
+      <c r="X85" s="135"/>
+      <c r="Y85" s="135"/>
+      <c r="Z85" s="135"/>
+      <c r="AA85" s="135"/>
       <c r="AB85" s="63" t="s">
         <v>259</v>
       </c>
@@ -8792,32 +8906,32 @@
       <c r="E86" s="52">
         <v>5</v>
       </c>
-      <c r="F86" s="132" t="s">
+      <c r="F86" s="135" t="s">
         <v>256</v>
       </c>
-      <c r="G86" s="132"/>
-      <c r="H86" s="132"/>
-      <c r="I86" s="132"/>
-      <c r="J86" s="132"/>
-      <c r="K86" s="132"/>
-      <c r="L86" s="132"/>
-      <c r="M86" s="132"/>
-      <c r="N86" s="132"/>
-      <c r="O86" s="132"/>
-      <c r="P86" s="132"/>
-      <c r="Q86" s="132" t="s">
+      <c r="G86" s="135"/>
+      <c r="H86" s="135"/>
+      <c r="I86" s="135"/>
+      <c r="J86" s="135"/>
+      <c r="K86" s="135"/>
+      <c r="L86" s="135"/>
+      <c r="M86" s="135"/>
+      <c r="N86" s="135"/>
+      <c r="O86" s="135"/>
+      <c r="P86" s="135"/>
+      <c r="Q86" s="135" t="s">
         <v>257</v>
       </c>
-      <c r="R86" s="132"/>
-      <c r="S86" s="132"/>
-      <c r="T86" s="132"/>
-      <c r="U86" s="132"/>
-      <c r="V86" s="132"/>
-      <c r="W86" s="132"/>
-      <c r="X86" s="132"/>
-      <c r="Y86" s="132"/>
-      <c r="Z86" s="132"/>
-      <c r="AA86" s="132"/>
+      <c r="R86" s="135"/>
+      <c r="S86" s="135"/>
+      <c r="T86" s="135"/>
+      <c r="U86" s="135"/>
+      <c r="V86" s="135"/>
+      <c r="W86" s="135"/>
+      <c r="X86" s="135"/>
+      <c r="Y86" s="135"/>
+      <c r="Z86" s="135"/>
+      <c r="AA86" s="135"/>
       <c r="AB86" s="63" t="s">
         <v>260</v>
       </c>
@@ -8836,32 +8950,32 @@
       <c r="E87" s="52">
         <v>1</v>
       </c>
-      <c r="F87" s="132" t="s">
+      <c r="F87" s="135" t="s">
         <v>276</v>
       </c>
-      <c r="G87" s="132"/>
-      <c r="H87" s="132"/>
-      <c r="I87" s="132"/>
-      <c r="J87" s="132"/>
-      <c r="K87" s="132"/>
-      <c r="L87" s="132"/>
-      <c r="M87" s="132"/>
-      <c r="N87" s="132"/>
-      <c r="O87" s="132"/>
-      <c r="P87" s="132"/>
-      <c r="Q87" s="132" t="s">
+      <c r="G87" s="135"/>
+      <c r="H87" s="135"/>
+      <c r="I87" s="135"/>
+      <c r="J87" s="135"/>
+      <c r="K87" s="135"/>
+      <c r="L87" s="135"/>
+      <c r="M87" s="135"/>
+      <c r="N87" s="135"/>
+      <c r="O87" s="135"/>
+      <c r="P87" s="135"/>
+      <c r="Q87" s="135" t="s">
         <v>275</v>
       </c>
-      <c r="R87" s="132"/>
-      <c r="S87" s="132"/>
-      <c r="T87" s="132"/>
-      <c r="U87" s="132"/>
-      <c r="V87" s="132"/>
-      <c r="W87" s="132"/>
-      <c r="X87" s="132"/>
-      <c r="Y87" s="132"/>
-      <c r="Z87" s="132"/>
-      <c r="AA87" s="132"/>
+      <c r="R87" s="135"/>
+      <c r="S87" s="135"/>
+      <c r="T87" s="135"/>
+      <c r="U87" s="135"/>
+      <c r="V87" s="135"/>
+      <c r="W87" s="135"/>
+      <c r="X87" s="135"/>
+      <c r="Y87" s="135"/>
+      <c r="Z87" s="135"/>
+      <c r="AA87" s="135"/>
       <c r="AB87" s="63" t="s">
         <v>260</v>
       </c>
@@ -8877,394 +8991,394 @@
       <c r="B90" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="128" t="s">
+      <c r="C90" s="132" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="128"/>
-      <c r="E90" s="128"/>
-      <c r="F90" s="128"/>
-      <c r="G90" s="128"/>
-      <c r="H90" s="128" t="s">
+      <c r="D90" s="132"/>
+      <c r="E90" s="132"/>
+      <c r="F90" s="132"/>
+      <c r="G90" s="132"/>
+      <c r="H90" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="I90" s="128"/>
-      <c r="J90" s="128"/>
-      <c r="K90" s="128"/>
-      <c r="L90" s="128"/>
-      <c r="M90" s="130" t="s">
+      <c r="I90" s="132"/>
+      <c r="J90" s="132"/>
+      <c r="K90" s="132"/>
+      <c r="L90" s="132"/>
+      <c r="M90" s="133" t="s">
         <v>185</v>
       </c>
-      <c r="N90" s="130"/>
+      <c r="N90" s="133"/>
       <c r="O90" s="105"/>
       <c r="T90" s="56" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A91" s="37" t="e" vm="45">
+      <c r="A91" s="37" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="126" t="s">
+      <c r="C91" s="130" t="s">
         <v>180</v>
       </c>
-      <c r="D91" s="126"/>
-      <c r="E91" s="126"/>
-      <c r="F91" s="126"/>
-      <c r="G91" s="126"/>
-      <c r="H91" s="126" t="s">
+      <c r="D91" s="130"/>
+      <c r="E91" s="130"/>
+      <c r="F91" s="130"/>
+      <c r="G91" s="130"/>
+      <c r="H91" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="I91" s="126"/>
-      <c r="J91" s="126"/>
-      <c r="K91" s="126"/>
-      <c r="L91" s="126"/>
-      <c r="M91" s="127" t="s">
+      <c r="I91" s="130"/>
+      <c r="J91" s="130"/>
+      <c r="K91" s="130"/>
+      <c r="L91" s="130"/>
+      <c r="M91" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N91" s="127"/>
+      <c r="N91" s="131"/>
       <c r="O91" s="63"/>
     </row>
     <row r="92" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A92" s="37" t="e" vm="46">
+      <c r="A92" s="37" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="126" t="s">
+      <c r="C92" s="130" t="s">
         <v>183</v>
       </c>
-      <c r="D92" s="126"/>
-      <c r="E92" s="126"/>
-      <c r="F92" s="126"/>
-      <c r="G92" s="126"/>
-      <c r="H92" s="126" t="s">
+      <c r="D92" s="130"/>
+      <c r="E92" s="130"/>
+      <c r="F92" s="130"/>
+      <c r="G92" s="130"/>
+      <c r="H92" s="130" t="s">
         <v>184</v>
       </c>
-      <c r="I92" s="126"/>
-      <c r="J92" s="126"/>
-      <c r="K92" s="126"/>
-      <c r="L92" s="126"/>
-      <c r="M92" s="127" t="s">
+      <c r="I92" s="130"/>
+      <c r="J92" s="130"/>
+      <c r="K92" s="130"/>
+      <c r="L92" s="130"/>
+      <c r="M92" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N92" s="127"/>
+      <c r="N92" s="131"/>
       <c r="O92" s="63"/>
     </row>
     <row r="93" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A93" s="37" t="e" vm="47">
+      <c r="A93" s="37" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
       <c r="B93" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="126" t="s">
+      <c r="C93" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D93" s="126"/>
-      <c r="E93" s="126"/>
-      <c r="F93" s="126"/>
-      <c r="G93" s="126"/>
-      <c r="H93" s="126" t="s">
+      <c r="D93" s="130"/>
+      <c r="E93" s="130"/>
+      <c r="F93" s="130"/>
+      <c r="G93" s="130"/>
+      <c r="H93" s="130" t="s">
         <v>181</v>
       </c>
-      <c r="I93" s="126"/>
-      <c r="J93" s="126"/>
-      <c r="K93" s="126"/>
-      <c r="L93" s="126"/>
-      <c r="M93" s="127" t="s">
+      <c r="I93" s="130"/>
+      <c r="J93" s="130"/>
+      <c r="K93" s="130"/>
+      <c r="L93" s="130"/>
+      <c r="M93" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N93" s="127"/>
+      <c r="N93" s="131"/>
       <c r="O93" s="63"/>
     </row>
     <row r="94" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A94" s="37" t="e" vm="48">
+      <c r="A94" s="37" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="C94" s="126" t="s">
+      <c r="C94" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D94" s="126"/>
-      <c r="E94" s="126"/>
-      <c r="F94" s="126"/>
-      <c r="G94" s="126"/>
-      <c r="H94" s="126" t="s">
+      <c r="D94" s="130"/>
+      <c r="E94" s="130"/>
+      <c r="F94" s="130"/>
+      <c r="G94" s="130"/>
+      <c r="H94" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="I94" s="126"/>
-      <c r="J94" s="126"/>
-      <c r="K94" s="126"/>
-      <c r="L94" s="126"/>
-      <c r="M94" s="127" t="s">
+      <c r="I94" s="130"/>
+      <c r="J94" s="130"/>
+      <c r="K94" s="130"/>
+      <c r="L94" s="130"/>
+      <c r="M94" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N94" s="127"/>
+      <c r="N94" s="131"/>
       <c r="O94" s="63"/>
     </row>
     <row r="95" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A95" s="37" t="e" vm="49">
+      <c r="A95" s="37" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C95" s="126" t="s">
+      <c r="C95" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D95" s="126"/>
-      <c r="E95" s="126"/>
-      <c r="F95" s="126"/>
-      <c r="G95" s="126"/>
-      <c r="H95" s="126" t="s">
+      <c r="D95" s="130"/>
+      <c r="E95" s="130"/>
+      <c r="F95" s="130"/>
+      <c r="G95" s="130"/>
+      <c r="H95" s="130" t="s">
         <v>217</v>
       </c>
-      <c r="I95" s="126"/>
-      <c r="J95" s="126"/>
-      <c r="K95" s="126"/>
-      <c r="L95" s="126"/>
-      <c r="M95" s="127" t="s">
+      <c r="I95" s="130"/>
+      <c r="J95" s="130"/>
+      <c r="K95" s="130"/>
+      <c r="L95" s="130"/>
+      <c r="M95" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N95" s="127"/>
+      <c r="N95" s="131"/>
       <c r="O95" s="63"/>
     </row>
     <row r="96" spans="1:28" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A96" s="37" t="e" vm="50">
+      <c r="A96" s="37" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C96" s="126" t="s">
+      <c r="C96" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D96" s="126"/>
-      <c r="E96" s="126"/>
-      <c r="F96" s="126"/>
-      <c r="G96" s="126"/>
-      <c r="H96" s="126" t="s">
+      <c r="D96" s="130"/>
+      <c r="E96" s="130"/>
+      <c r="F96" s="130"/>
+      <c r="G96" s="130"/>
+      <c r="H96" s="130" t="s">
         <v>218</v>
       </c>
-      <c r="I96" s="126"/>
-      <c r="J96" s="126"/>
-      <c r="K96" s="126"/>
-      <c r="L96" s="126"/>
-      <c r="M96" s="127" t="s">
+      <c r="I96" s="130"/>
+      <c r="J96" s="130"/>
+      <c r="K96" s="130"/>
+      <c r="L96" s="130"/>
+      <c r="M96" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N96" s="127"/>
+      <c r="N96" s="131"/>
       <c r="O96" s="63"/>
     </row>
     <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A97" s="37" t="e" vm="51">
+      <c r="A97" s="37" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C97" s="126" t="s">
+      <c r="C97" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D97" s="126"/>
-      <c r="E97" s="126"/>
-      <c r="F97" s="126"/>
-      <c r="G97" s="126"/>
-      <c r="H97" s="126" t="s">
+      <c r="D97" s="130"/>
+      <c r="E97" s="130"/>
+      <c r="F97" s="130"/>
+      <c r="G97" s="130"/>
+      <c r="H97" s="130" t="s">
         <v>219</v>
       </c>
-      <c r="I97" s="126"/>
-      <c r="J97" s="126"/>
-      <c r="K97" s="126"/>
-      <c r="L97" s="126"/>
-      <c r="M97" s="127" t="s">
+      <c r="I97" s="130"/>
+      <c r="J97" s="130"/>
+      <c r="K97" s="130"/>
+      <c r="L97" s="130"/>
+      <c r="M97" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N97" s="127"/>
+      <c r="N97" s="131"/>
       <c r="O97" s="63"/>
     </row>
     <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A98" s="37" t="e" vm="52">
+      <c r="A98" s="37" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C98" s="126" t="s">
+      <c r="C98" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D98" s="126"/>
-      <c r="E98" s="126"/>
-      <c r="F98" s="126"/>
-      <c r="G98" s="126"/>
-      <c r="H98" s="126" t="s">
+      <c r="D98" s="130"/>
+      <c r="E98" s="130"/>
+      <c r="F98" s="130"/>
+      <c r="G98" s="130"/>
+      <c r="H98" s="130" t="s">
         <v>220</v>
       </c>
-      <c r="I98" s="126"/>
-      <c r="J98" s="126"/>
-      <c r="K98" s="126"/>
-      <c r="L98" s="126"/>
-      <c r="M98" s="127" t="s">
+      <c r="I98" s="130"/>
+      <c r="J98" s="130"/>
+      <c r="K98" s="130"/>
+      <c r="L98" s="130"/>
+      <c r="M98" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N98" s="127"/>
+      <c r="N98" s="131"/>
       <c r="O98" s="63"/>
     </row>
     <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A99" s="37" t="e" vm="53">
+      <c r="A99" s="37" t="e" vm="54">
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C99" s="126" t="s">
+      <c r="C99" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D99" s="126"/>
-      <c r="E99" s="126"/>
-      <c r="F99" s="126"/>
-      <c r="G99" s="126"/>
-      <c r="H99" s="126" t="s">
+      <c r="D99" s="130"/>
+      <c r="E99" s="130"/>
+      <c r="F99" s="130"/>
+      <c r="G99" s="130"/>
+      <c r="H99" s="130" t="s">
         <v>221</v>
       </c>
-      <c r="I99" s="126"/>
-      <c r="J99" s="126"/>
-      <c r="K99" s="126"/>
-      <c r="L99" s="126"/>
-      <c r="M99" s="127" t="s">
+      <c r="I99" s="130"/>
+      <c r="J99" s="130"/>
+      <c r="K99" s="130"/>
+      <c r="L99" s="130"/>
+      <c r="M99" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N99" s="127"/>
+      <c r="N99" s="131"/>
       <c r="O99" s="63"/>
     </row>
     <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A100" s="37" t="e" vm="54">
+      <c r="A100" s="37" t="e" vm="55">
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C100" s="126" t="s">
+      <c r="C100" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="D100" s="126"/>
-      <c r="E100" s="126"/>
-      <c r="F100" s="126"/>
-      <c r="G100" s="126"/>
-      <c r="H100" s="126" t="s">
+      <c r="D100" s="130"/>
+      <c r="E100" s="130"/>
+      <c r="F100" s="130"/>
+      <c r="G100" s="130"/>
+      <c r="H100" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="I100" s="126"/>
-      <c r="J100" s="126"/>
-      <c r="K100" s="126"/>
-      <c r="L100" s="126"/>
-      <c r="M100" s="127" t="s">
+      <c r="I100" s="130"/>
+      <c r="J100" s="130"/>
+      <c r="K100" s="130"/>
+      <c r="L100" s="130"/>
+      <c r="M100" s="131" t="s">
         <v>186</v>
       </c>
-      <c r="N100" s="127"/>
+      <c r="N100" s="131"/>
       <c r="O100" s="63"/>
     </row>
     <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A101" s="37"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="126"/>
-      <c r="D101" s="126"/>
-      <c r="E101" s="126"/>
-      <c r="F101" s="126"/>
-      <c r="G101" s="126"/>
-      <c r="H101" s="126"/>
-      <c r="I101" s="126"/>
-      <c r="J101" s="126"/>
-      <c r="K101" s="126"/>
-      <c r="L101" s="126"/>
-      <c r="M101" s="127"/>
-      <c r="N101" s="127"/>
+      <c r="C101" s="130"/>
+      <c r="D101" s="130"/>
+      <c r="E101" s="130"/>
+      <c r="F101" s="130"/>
+      <c r="G101" s="130"/>
+      <c r="H101" s="130"/>
+      <c r="I101" s="130"/>
+      <c r="J101" s="130"/>
+      <c r="K101" s="130"/>
+      <c r="L101" s="130"/>
+      <c r="M101" s="131"/>
+      <c r="N101" s="131"/>
       <c r="O101" s="63"/>
     </row>
     <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
-      <c r="H102" s="126"/>
-      <c r="I102" s="126"/>
-      <c r="J102" s="126"/>
-      <c r="K102" s="126"/>
-      <c r="L102" s="126"/>
-      <c r="M102" s="127"/>
-      <c r="N102" s="127"/>
+      <c r="H102" s="130"/>
+      <c r="I102" s="130"/>
+      <c r="J102" s="130"/>
+      <c r="K102" s="130"/>
+      <c r="L102" s="130"/>
+      <c r="M102" s="131"/>
+      <c r="N102" s="131"/>
       <c r="O102" s="63"/>
     </row>
     <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A103" s="37"/>
       <c r="B103" s="37"/>
-      <c r="C103" s="126"/>
-      <c r="D103" s="126"/>
-      <c r="E103" s="126"/>
-      <c r="F103" s="126"/>
-      <c r="G103" s="126"/>
-      <c r="H103" s="126"/>
-      <c r="I103" s="126"/>
-      <c r="J103" s="126"/>
-      <c r="K103" s="126"/>
-      <c r="L103" s="126"/>
-      <c r="M103" s="127"/>
-      <c r="N103" s="127"/>
+      <c r="C103" s="130"/>
+      <c r="D103" s="130"/>
+      <c r="E103" s="130"/>
+      <c r="F103" s="130"/>
+      <c r="G103" s="130"/>
+      <c r="H103" s="130"/>
+      <c r="I103" s="130"/>
+      <c r="J103" s="130"/>
+      <c r="K103" s="130"/>
+      <c r="L103" s="130"/>
+      <c r="M103" s="131"/>
+      <c r="N103" s="131"/>
       <c r="O103" s="63"/>
     </row>
     <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A104" s="37"/>
       <c r="B104" s="37"/>
-      <c r="C104" s="126"/>
-      <c r="D104" s="126"/>
-      <c r="E104" s="126"/>
-      <c r="F104" s="126"/>
-      <c r="G104" s="126"/>
-      <c r="H104" s="126"/>
-      <c r="I104" s="126"/>
-      <c r="J104" s="126"/>
-      <c r="K104" s="126"/>
-      <c r="L104" s="126"/>
-      <c r="M104" s="127"/>
-      <c r="N104" s="127"/>
+      <c r="C104" s="130"/>
+      <c r="D104" s="130"/>
+      <c r="E104" s="130"/>
+      <c r="F104" s="130"/>
+      <c r="G104" s="130"/>
+      <c r="H104" s="130"/>
+      <c r="I104" s="130"/>
+      <c r="J104" s="130"/>
+      <c r="K104" s="130"/>
+      <c r="L104" s="130"/>
+      <c r="M104" s="131"/>
+      <c r="N104" s="131"/>
       <c r="O104" s="63"/>
     </row>
     <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A105" s="37"/>
       <c r="B105" s="37"/>
-      <c r="C105" s="126"/>
-      <c r="D105" s="126"/>
-      <c r="E105" s="126"/>
-      <c r="F105" s="126"/>
-      <c r="G105" s="126"/>
-      <c r="H105" s="126"/>
-      <c r="I105" s="126"/>
-      <c r="J105" s="126"/>
-      <c r="K105" s="126"/>
-      <c r="L105" s="126"/>
-      <c r="M105" s="127"/>
-      <c r="N105" s="127"/>
+      <c r="C105" s="130"/>
+      <c r="D105" s="130"/>
+      <c r="E105" s="130"/>
+      <c r="F105" s="130"/>
+      <c r="G105" s="130"/>
+      <c r="H105" s="130"/>
+      <c r="I105" s="130"/>
+      <c r="J105" s="130"/>
+      <c r="K105" s="130"/>
+      <c r="L105" s="130"/>
+      <c r="M105" s="131"/>
+      <c r="N105" s="131"/>
       <c r="O105" s="63"/>
     </row>
     <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="126"/>
-      <c r="D106" s="126"/>
-      <c r="E106" s="126"/>
-      <c r="F106" s="126"/>
-      <c r="G106" s="126"/>
-      <c r="H106" s="126"/>
-      <c r="I106" s="126"/>
-      <c r="J106" s="126"/>
-      <c r="K106" s="126"/>
-      <c r="L106" s="126"/>
-      <c r="M106" s="127"/>
-      <c r="N106" s="127"/>
+      <c r="C106" s="130"/>
+      <c r="D106" s="130"/>
+      <c r="E106" s="130"/>
+      <c r="F106" s="130"/>
+      <c r="G106" s="130"/>
+      <c r="H106" s="130"/>
+      <c r="I106" s="130"/>
+      <c r="J106" s="130"/>
+      <c r="K106" s="130"/>
+      <c r="L106" s="130"/>
+      <c r="M106" s="131"/>
+      <c r="N106" s="131"/>
       <c r="O106" s="63"/>
     </row>
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.6">
@@ -9607,7 +9721,7 @@
       <c r="O123" s="63"/>
     </row>
     <row r="124" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A124" s="37" t="e" vm="55">
+      <c r="A124" s="37" t="e" vm="56">
         <v>#VALUE!</v>
       </c>
       <c r="B124" s="117" t="s">
@@ -9687,10 +9801,10 @@
     <row r="128" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A128" s="37"/>
       <c r="B128" s="117" t="s">
+        <v>289</v>
+      </c>
+      <c r="C128" s="114" t="s">
         <v>290</v>
-      </c>
-      <c r="C128" s="114" t="s">
-        <v>291</v>
       </c>
       <c r="D128" s="114"/>
       <c r="E128" s="114"/>
@@ -9865,7 +9979,7 @@
     <row r="142" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="143" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
-  <mergeCells count="139">
+  <mergeCells count="142">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C106:G106"/>
     <mergeCell ref="H106:L106"/>
@@ -9902,7 +10016,6 @@
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="C92:G92"/>
     <mergeCell ref="C93:G93"/>
-    <mergeCell ref="U63:V63"/>
     <mergeCell ref="U64:V64"/>
     <mergeCell ref="U65:V65"/>
     <mergeCell ref="U66:V66"/>
@@ -9946,8 +10059,6 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:H49"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="M90:N90"/>
     <mergeCell ref="F83:P83"/>
@@ -9972,19 +10083,6 @@
     <mergeCell ref="F65:G65"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E52:J52"/>
-    <mergeCell ref="E53:J53"/>
-    <mergeCell ref="E54:J54"/>
-    <mergeCell ref="E51:J51"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
     <mergeCell ref="C96:G96"/>
     <mergeCell ref="H90:L90"/>
     <mergeCell ref="H91:L91"/>
@@ -9999,12 +10097,31 @@
     <mergeCell ref="F81:P81"/>
     <mergeCell ref="F82:P82"/>
     <mergeCell ref="M91:N91"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
     <mergeCell ref="Q81:AA81"/>
     <mergeCell ref="Q82:AA82"/>
     <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
     <mergeCell ref="Q83:AA83"/>
     <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="U63:V63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
dash added. Press E to dash!
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25DF55A-7A26-44D2-A654-3DF601D165CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE160D2-1E9A-4759-A54A-479CD59A176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,7 +672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="309">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1832,88 +1832,96 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>adrenaline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lynx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(beta) Drops walls with random deviation from the center 5 times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop a cross-shaped wall with 120 hitpoints </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summons wall on the way</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not reloadable / Shoots upto player's cursor location with maximum distance fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not reloadable / Penetration: penetrates through enemies and players</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not reloadable / Designed to destroy a tank (too slow bullet for practical fights)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>health is gradually restored</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.50BMG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extreme friction applied / Mine &amp; TankBuster uses shockWave / Penetration: penetrates through enemies and players</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flare drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Airdrops are powerful - fire a green flare gun to get Lynx; a god-tier weapon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal amt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply time (s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 ~ 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 ~ 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DASH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>last update
-2024 6 19</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adrenaline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lynx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(beta) Drops walls with random deviation from the center 5 times</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop a cross-shaped wall with 120 hitpoints </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Summons wall on the way</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not reloadable / Shoots upto player's cursor location with maximum distance fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not reloadable / Penetration: penetrates through enemies and players</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not reloadable / Designed to destroy a tank (too slow bullet for practical fights)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>health is gradually restored</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>.50BMG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extreme friction applied / Mine &amp; TankBuster uses shockWave / Penetration: penetrates through enemies and players</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flare drop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Airdrops are powerful - fire a green flare gun to get Lynx; a god-tier weapon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drink</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heal amt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apply time (s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 ~ 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 ~ 5</t>
+2024 7 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Press 'E' to dash towards a mouse direction. Dash is recharged when you get a kill, charging upto one. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4942,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -4968,7 +4976,7 @@
       </c>
       <c r="D1" s="192"/>
       <c r="E1" s="191" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="F1" s="192"/>
       <c r="G1" s="43" t="s">
@@ -5079,7 +5087,7 @@
         <v>218</v>
       </c>
       <c r="AM2" s="96" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:39" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -5172,7 +5180,7 @@
       <c r="AI3" s="40"/>
       <c r="AJ3" s="40"/>
       <c r="AM3" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -5343,7 +5351,7 @@
       </c>
       <c r="Y5" s="9"/>
       <c r="Z5" s="44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AL5" s="25" t="s">
         <v>227</v>
@@ -5430,7 +5438,7 @@
       </c>
       <c r="Y6" s="58"/>
       <c r="Z6" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AL6" s="25"/>
     </row>
@@ -5491,7 +5499,7 @@
       <c r="X7" s="16"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AL7" s="25"/>
     </row>
@@ -5581,7 +5589,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B9" s="114" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" s="115">
         <v>3200</v>
@@ -5608,7 +5616,7 @@
         <v>4000</v>
       </c>
       <c r="K9" s="116" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L9" s="116"/>
       <c r="M9" s="116">
@@ -5657,11 +5665,11 @@
       </c>
       <c r="Y9" s="119"/>
       <c r="Z9" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AL9" s="25"/>
       <c r="AM9" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="23.55" customHeight="1" x14ac:dyDescent="0.6">
@@ -7630,7 +7638,7 @@
       <c r="N39" s="90"/>
       <c r="O39" s="90"/>
       <c r="P39" s="104" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q39" s="103" t="s">
         <v>251</v>
@@ -7773,7 +7781,7 @@
         <v>185</v>
       </c>
       <c r="C45" s="104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D45" s="104"/>
       <c r="E45" s="104" t="s">
@@ -7781,7 +7789,7 @@
       </c>
       <c r="F45" s="104"/>
       <c r="G45" s="188" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H45" s="188"/>
       <c r="I45" s="93"/>
@@ -7866,13 +7874,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C48" s="105">
         <v>6.4</v>
       </c>
       <c r="D48" s="183" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E48" s="181"/>
       <c r="F48" s="181"/>
@@ -7901,13 +7909,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="163" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C49" s="164">
         <v>3.2</v>
       </c>
       <c r="D49" s="189" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E49" s="189"/>
       <c r="F49" s="189"/>
@@ -9156,7 +9164,7 @@
         <v>140</v>
       </c>
       <c r="D83" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E83" s="41">
         <v>1</v>
@@ -9198,7 +9206,7 @@
         <v>141</v>
       </c>
       <c r="D84" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E84" s="41">
         <v>1</v>
@@ -9290,7 +9298,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="176" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G86" s="176"/>
       <c r="H86" s="176"/>
@@ -9303,7 +9311,7 @@
       <c r="O86" s="176"/>
       <c r="P86" s="176"/>
       <c r="Q86" s="176" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R86" s="176"/>
       <c r="S86" s="176"/>
@@ -9319,7 +9327,7 @@
         <v>252</v>
       </c>
       <c r="AC86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:29" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
@@ -10213,7 +10221,7 @@
       <c r="A129" s="27"/>
       <c r="B129" s="101"/>
       <c r="C129" s="98" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D129" s="98"/>
       <c r="E129" s="98"/>
@@ -10247,8 +10255,12 @@
     </row>
     <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A131" s="27"/>
-      <c r="B131" s="101"/>
-      <c r="C131" s="98"/>
+      <c r="B131" s="101" t="s">
+        <v>306</v>
+      </c>
+      <c r="C131" s="98" t="s">
+        <v>308</v>
+      </c>
       <c r="D131" s="98"/>
       <c r="E131" s="98"/>
       <c r="F131" s="98"/>

</xml_diff>

<commit_message>
tried to make MAXHP 100 but gave up
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout_deathmatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983E4A20-1279-41C8-A831-896622280984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB4E740-AAD3-458C-B4E2-F71702F623E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1443,10 +1443,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8 (max)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Player health must be blow 6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1942,6 +1938,10 @@
   </si>
   <si>
     <t>TBU: no spread, rapid fire gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 (max)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4968,7 +4968,7 @@
   <dimension ref="A1:AM143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D48" sqref="D48:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4989,11 +4989,11 @@
         <v>171</v>
       </c>
       <c r="C1" s="168" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D1" s="169"/>
       <c r="E1" s="168" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F1" s="169"/>
       <c r="G1" s="43" t="s">
@@ -5101,10 +5101,10 @@
       <c r="AH2" s="28"/>
       <c r="AI2" s="28"/>
       <c r="AL2" s="95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AM2" s="95" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5197,7 +5197,7 @@
       <c r="AI3" s="40"/>
       <c r="AJ3" s="40"/>
       <c r="AM3" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5368,10 +5368,10 @@
       </c>
       <c r="Y5" s="9"/>
       <c r="Z5" s="44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AL5" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="Y6" s="58"/>
       <c r="Z6" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AL6" s="25"/>
     </row>
@@ -5516,7 +5516,7 @@
       <c r="X7" s="16"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AL7" s="25"/>
     </row>
@@ -5525,7 +5525,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="29">
         <v>32</v>
@@ -5606,7 +5606,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B9" s="113" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C9" s="114">
         <v>3200</v>
@@ -5633,10 +5633,10 @@
         <v>4000</v>
       </c>
       <c r="K9" s="115" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L9" s="115" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M9" s="115">
         <f t="shared" si="10"/>
@@ -5684,11 +5684,11 @@
       </c>
       <c r="Y9" s="118"/>
       <c r="Z9" s="44" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AL9" s="25"/>
       <c r="AM9" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6038,7 +6038,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C14" s="119">
         <v>640</v>
@@ -6114,7 +6114,7 @@
       </c>
       <c r="Y14" s="9"/>
       <c r="Z14" s="44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AL14" s="94">
         <v>15</v>
@@ -6228,10 +6228,10 @@
       </c>
       <c r="Y16" s="109"/>
       <c r="Z16" s="44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AL16" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6408,7 +6408,7 @@
       </c>
       <c r="Y18" s="9"/>
       <c r="Z18" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AL18" s="93">
         <v>11</v>
@@ -6592,10 +6592,10 @@
     </row>
     <row r="21" spans="1:39" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C21" s="119">
         <v>640</v>
@@ -6671,10 +6671,10 @@
       </c>
       <c r="Y21" s="9"/>
       <c r="Z21" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AM21" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:39" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="Y25" s="9"/>
       <c r="Z25" s="44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL25" s="93">
         <v>7</v>
@@ -7554,13 +7554,13 @@
     </row>
     <row r="36" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D36" s="58">
         <v>0</v>
@@ -7575,7 +7575,7 @@
         <v>800</v>
       </c>
       <c r="H36" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>51</v>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="Y36" s="9"/>
       <c r="Z36" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AL36" s="25"/>
     </row>
@@ -7629,7 +7629,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B37" s="113" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" s="123">
         <v>90</v>
@@ -7717,10 +7717,10 @@
       <c r="N39" s="89"/>
       <c r="O39" s="89"/>
       <c r="P39" s="103" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q39" s="102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7736,7 +7736,7 @@
       <c r="D40" s="181"/>
       <c r="E40" s="181"/>
       <c r="F40" s="181" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G40" s="181"/>
       <c r="H40" s="181"/>
@@ -7753,7 +7753,7 @@
         <v>4</v>
       </c>
       <c r="Q40" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7786,7 +7786,7 @@
         <v>2</v>
       </c>
       <c r="Q41" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7794,20 +7794,20 @@
         <v>#VALUE!</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C42" s="182" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D42" s="182"/>
       <c r="E42" s="182"/>
       <c r="F42" s="182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G42" s="182"/>
       <c r="H42" s="182"/>
       <c r="I42" s="182" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J42" s="182"/>
       <c r="K42" s="182"/>
@@ -7819,7 +7819,7 @@
         <v>3</v>
       </c>
       <c r="Q42" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:38" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -7827,10 +7827,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B43" s="113" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C43" s="183" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D43" s="183"/>
       <c r="E43" s="183"/>
@@ -7838,7 +7838,7 @@
       <c r="G43" s="183"/>
       <c r="H43" s="183"/>
       <c r="I43" s="183" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J43" s="183"/>
       <c r="K43" s="183"/>
@@ -7850,7 +7850,7 @@
         <v>1</v>
       </c>
       <c r="Q43" s="151" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:38" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7860,7 +7860,7 @@
         <v>185</v>
       </c>
       <c r="C45" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D45" s="103"/>
       <c r="E45" s="103" t="s">
@@ -7868,13 +7868,13 @@
       </c>
       <c r="F45" s="103"/>
       <c r="G45" s="180" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H45" s="180"/>
       <c r="I45" s="92"/>
       <c r="J45" s="92"/>
       <c r="K45" s="102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N45" s="178" t="s">
         <v>77</v>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="D46" s="104"/>
       <c r="E46" s="104" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F46" s="104"/>
       <c r="G46" s="181">
@@ -7904,7 +7904,7 @@
       <c r="I46" s="91"/>
       <c r="J46" s="91"/>
       <c r="K46" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N46" s="178" t="s">
         <v>75</v>
@@ -7923,7 +7923,7 @@
         <v>187</v>
       </c>
       <c r="C47" s="104" t="s">
-        <v>189</v>
+        <v>313</v>
       </c>
       <c r="D47" s="104"/>
       <c r="E47" s="104" t="s">
@@ -7937,7 +7937,7 @@
       <c r="I47" s="91"/>
       <c r="J47" s="91"/>
       <c r="K47" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N47" s="178" t="s">
         <v>67</v>
@@ -7953,13 +7953,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C48" s="104">
         <v>6.4</v>
       </c>
       <c r="D48" s="191" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E48" s="181"/>
       <c r="F48" s="181"/>
@@ -7970,7 +7970,7 @@
       <c r="I48" s="31"/>
       <c r="J48" s="31"/>
       <c r="K48" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N48" s="178" t="s">
         <v>97</v>
@@ -7988,13 +7988,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="161" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C49" s="162">
         <v>3.2</v>
       </c>
       <c r="D49" s="193" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E49" s="193"/>
       <c r="F49" s="193"/>
@@ -8005,7 +8005,7 @@
       <c r="I49" s="163"/>
       <c r="J49" s="163"/>
       <c r="K49" s="164" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N49" s="44"/>
       <c r="O49" s="44"/>
@@ -8015,10 +8015,10 @@
     <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="24"/>
       <c r="B51" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C51" s="180" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D51" s="180"/>
       <c r="E51" s="180" t="s">
@@ -8030,7 +8030,7 @@
       <c r="I51" s="180"/>
       <c r="J51" s="180"/>
       <c r="K51" s="102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -8038,14 +8038,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C52" s="173" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D52" s="173"/>
       <c r="E52" s="184" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F52" s="184"/>
       <c r="G52" s="184"/>
@@ -8053,7 +8053,7 @@
       <c r="I52" s="184"/>
       <c r="J52" s="184"/>
       <c r="K52" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -8061,14 +8061,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C53" s="173" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D53" s="173"/>
       <c r="E53" s="184" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F53" s="184"/>
       <c r="G53" s="184"/>
@@ -8076,7 +8076,7 @@
       <c r="I53" s="184"/>
       <c r="J53" s="184"/>
       <c r="K53" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -8084,14 +8084,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B54" s="113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C54" s="177" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D54" s="177"/>
       <c r="E54" s="185" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F54" s="185"/>
       <c r="G54" s="185"/>
@@ -8099,7 +8099,7 @@
       <c r="I54" s="185"/>
       <c r="J54" s="185"/>
       <c r="K54" s="151" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -8385,7 +8385,7 @@
         <v>102</v>
       </c>
       <c r="N63" s="68" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O63" s="86" t="s">
         <v>107</v>
@@ -8961,7 +8961,7 @@
     <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B73" s="98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O73" s="175" t="s">
         <v>162</v>
@@ -9010,7 +9010,7 @@
       </c>
       <c r="R74" s="174"/>
       <c r="S74" s="102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9060,7 +9060,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="S75" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9110,7 +9110,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="S76" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:36" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -9136,10 +9136,10 @@
     </row>
     <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B78" s="93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9187,7 +9187,7 @@
       <c r="Z81" s="174"/>
       <c r="AA81" s="174"/>
       <c r="AB81" s="102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="82" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9231,7 +9231,7 @@
       <c r="Z82" s="195"/>
       <c r="AA82" s="195"/>
       <c r="AB82" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9243,13 +9243,13 @@
         <v>140</v>
       </c>
       <c r="D83" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E83" s="41">
         <v>1</v>
       </c>
       <c r="F83" s="184" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G83" s="184"/>
       <c r="H83" s="184"/>
@@ -9273,7 +9273,7 @@
       <c r="Z83" s="184"/>
       <c r="AA83" s="184"/>
       <c r="AB83" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9285,13 +9285,13 @@
         <v>141</v>
       </c>
       <c r="D84" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E84" s="41">
         <v>1</v>
       </c>
       <c r="F84" s="184" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G84" s="184"/>
       <c r="H84" s="184"/>
@@ -9315,7 +9315,7 @@
       <c r="Z84" s="184"/>
       <c r="AA84" s="184"/>
       <c r="AB84" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9359,16 +9359,16 @@
       <c r="Z85" s="184"/>
       <c r="AA85" s="184"/>
       <c r="AB85" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="27"/>
       <c r="B86" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D86" s="41">
         <v>6</v>
@@ -9377,7 +9377,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="184" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G86" s="184"/>
       <c r="H86" s="184"/>
@@ -9390,7 +9390,7 @@
       <c r="O86" s="184"/>
       <c r="P86" s="184"/>
       <c r="Q86" s="184" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R86" s="184"/>
       <c r="S86" s="184"/>
@@ -9403,19 +9403,19 @@
       <c r="Z86" s="184"/>
       <c r="AA86" s="184"/>
       <c r="AB86" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AC86" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:29" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A87" s="113"/>
       <c r="B87" s="113" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C87" s="151" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D87" s="152">
         <v>0</v>
@@ -9424,7 +9424,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="185" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G87" s="185"/>
       <c r="H87" s="185"/>
@@ -9437,7 +9437,7 @@
       <c r="O87" s="185"/>
       <c r="P87" s="185"/>
       <c r="Q87" s="185" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R87" s="185"/>
       <c r="S87" s="185"/>
@@ -9450,12 +9450,12 @@
       <c r="Z87" s="185"/>
       <c r="AA87" s="185"/>
       <c r="AB87" s="151" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="45" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:29" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9484,7 +9484,7 @@
       <c r="N90" s="174"/>
       <c r="O90" s="88"/>
       <c r="T90" s="45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:29" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -9549,7 +9549,7 @@
         <v>175</v>
       </c>
       <c r="C93" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D93" s="170"/>
       <c r="E93" s="170"/>
@@ -9573,17 +9573,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C94" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D94" s="170"/>
       <c r="E94" s="170"/>
       <c r="F94" s="170"/>
       <c r="G94" s="170"/>
       <c r="H94" s="170" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I94" s="170"/>
       <c r="J94" s="170"/>
@@ -9600,17 +9600,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C95" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D95" s="170"/>
       <c r="E95" s="170"/>
       <c r="F95" s="170"/>
       <c r="G95" s="170"/>
       <c r="H95" s="170" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I95" s="170"/>
       <c r="J95" s="170"/>
@@ -9627,17 +9627,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C96" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D96" s="170"/>
       <c r="E96" s="170"/>
       <c r="F96" s="170"/>
       <c r="G96" s="170"/>
       <c r="H96" s="170" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I96" s="170"/>
       <c r="J96" s="170"/>
@@ -9654,17 +9654,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C97" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D97" s="170"/>
       <c r="E97" s="170"/>
       <c r="F97" s="170"/>
       <c r="G97" s="170"/>
       <c r="H97" s="170" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I97" s="170"/>
       <c r="J97" s="170"/>
@@ -9681,17 +9681,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C98" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D98" s="170"/>
       <c r="E98" s="170"/>
       <c r="F98" s="170"/>
       <c r="G98" s="170"/>
       <c r="H98" s="170" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I98" s="170"/>
       <c r="J98" s="170"/>
@@ -9708,17 +9708,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C99" s="170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D99" s="170"/>
       <c r="E99" s="170"/>
       <c r="F99" s="170"/>
       <c r="G99" s="170"/>
       <c r="H99" s="170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I99" s="170"/>
       <c r="J99" s="170"/>
@@ -9735,17 +9735,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="B100" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C100" s="170" t="s">
         <v>209</v>
-      </c>
-      <c r="C100" s="170" t="s">
-        <v>210</v>
       </c>
       <c r="D100" s="170"/>
       <c r="E100" s="170"/>
       <c r="F100" s="170"/>
       <c r="G100" s="170"/>
       <c r="H100" s="170" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I100" s="170"/>
       <c r="J100" s="170"/>
@@ -9857,7 +9857,7 @@
     <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="65"/>
       <c r="B107" s="95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C107" s="65"/>
       <c r="D107" s="65"/>
@@ -9878,10 +9878,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B108" s="100" t="s">
+        <v>228</v>
+      </c>
+      <c r="C108" s="97" t="s">
         <v>229</v>
-      </c>
-      <c r="C108" s="97" t="s">
-        <v>230</v>
       </c>
       <c r="D108" s="97"/>
       <c r="E108" s="97"/>
@@ -9900,7 +9900,7 @@
       <c r="A109" s="27"/>
       <c r="B109" s="100"/>
       <c r="C109" s="97" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D109" s="97"/>
       <c r="E109" s="97"/>
@@ -9919,7 +9919,7 @@
       <c r="A110" s="27"/>
       <c r="B110" s="100"/>
       <c r="C110" s="97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D110" s="97"/>
       <c r="E110" s="97"/>
@@ -9938,7 +9938,7 @@
       <c r="A111" s="27"/>
       <c r="B111" s="100"/>
       <c r="C111" s="97" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D111" s="97"/>
       <c r="E111" s="97"/>
@@ -9973,10 +9973,10 @@
     <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="27"/>
       <c r="B113" s="100" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C113" s="97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D113" s="97"/>
       <c r="E113" s="97"/>
@@ -9995,7 +9995,7 @@
       <c r="A114" s="27"/>
       <c r="B114" s="100"/>
       <c r="C114" s="97" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D114" s="97"/>
       <c r="E114" s="97"/>
@@ -10030,25 +10030,25 @@
     <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="27"/>
       <c r="B116" s="100" t="s">
+        <v>244</v>
+      </c>
+      <c r="C116" s="99" t="s">
         <v>245</v>
       </c>
-      <c r="C116" s="99" t="s">
+      <c r="D116" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="E116" s="99" t="s">
+        <v>237</v>
+      </c>
+      <c r="F116" s="99" t="s">
+        <v>238</v>
+      </c>
+      <c r="G116" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="H116" s="97" t="s">
         <v>246</v>
-      </c>
-      <c r="D116" s="99" t="s">
-        <v>237</v>
-      </c>
-      <c r="E116" s="99" t="s">
-        <v>238</v>
-      </c>
-      <c r="F116" s="99" t="s">
-        <v>239</v>
-      </c>
-      <c r="G116" s="99" t="s">
-        <v>264</v>
-      </c>
-      <c r="H116" s="97" t="s">
-        <v>247</v>
       </c>
       <c r="I116" s="97"/>
       <c r="J116" s="97"/>
@@ -10062,22 +10062,22 @@
       <c r="A117" s="27"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D117" s="101" t="s">
+        <v>307</v>
+      </c>
+      <c r="E117" s="167" t="s">
+        <v>304</v>
+      </c>
+      <c r="F117" s="101" t="s">
         <v>308</v>
       </c>
-      <c r="E117" s="167" t="s">
+      <c r="G117" s="101" t="s">
+        <v>308</v>
+      </c>
+      <c r="H117" s="97" t="s">
         <v>305</v>
-      </c>
-      <c r="F117" s="101" t="s">
-        <v>309</v>
-      </c>
-      <c r="G117" s="101" t="s">
-        <v>309</v>
-      </c>
-      <c r="H117" s="97" t="s">
-        <v>306</v>
       </c>
       <c r="I117" s="97"/>
       <c r="J117" s="97"/>
@@ -10108,7 +10108,7 @@
       <c r="A119" s="27"/>
       <c r="B119" s="100"/>
       <c r="C119" s="97" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D119" s="97"/>
       <c r="E119" s="97"/>
@@ -10127,7 +10127,7 @@
       <c r="A120" s="27"/>
       <c r="B120" s="100"/>
       <c r="C120" s="97" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D120" s="97"/>
       <c r="E120" s="97"/>
@@ -10146,7 +10146,7 @@
       <c r="A121" s="27"/>
       <c r="B121" s="100"/>
       <c r="C121" s="97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D121" s="97"/>
       <c r="E121" s="97"/>
@@ -10165,7 +10165,7 @@
       <c r="A122" s="27"/>
       <c r="B122" s="100"/>
       <c r="C122" s="97" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D122" s="97"/>
       <c r="E122" s="97"/>
@@ -10202,10 +10202,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B124" s="100" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C124" s="97" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D124" s="97"/>
       <c r="E124" s="97"/>
@@ -10224,7 +10224,7 @@
       <c r="A125" s="27"/>
       <c r="B125" s="100"/>
       <c r="C125" s="97" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D125" s="97"/>
       <c r="E125" s="97"/>
@@ -10243,7 +10243,7 @@
       <c r="A126" s="27"/>
       <c r="B126" s="100"/>
       <c r="C126" s="97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D126" s="97"/>
       <c r="E126" s="97"/>
@@ -10280,10 +10280,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B128" s="100" t="s">
+        <v>279</v>
+      </c>
+      <c r="C128" s="97" t="s">
         <v>280</v>
-      </c>
-      <c r="C128" s="97" t="s">
-        <v>281</v>
       </c>
       <c r="D128" s="97"/>
       <c r="E128" s="97"/>
@@ -10302,7 +10302,7 @@
       <c r="A129" s="27"/>
       <c r="B129" s="100"/>
       <c r="C129" s="97" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D129" s="97"/>
       <c r="E129" s="97"/>
@@ -10337,10 +10337,10 @@
     <row r="131" spans="1:15" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="27"/>
       <c r="B131" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="C131" s="97" t="s">
         <v>303</v>
-      </c>
-      <c r="C131" s="97" t="s">
-        <v>304</v>
       </c>
       <c r="D131" s="97"/>
       <c r="E131" s="97"/>

</xml_diff>